<commit_message>
Add data for 2022-05-02
</commit_message>
<xml_diff>
--- a/output/index-crime-full-year.xlsx
+++ b/output/index-crime-full-year.xlsx
@@ -888,7 +888,7 @@
         <v>7238</v>
       </c>
       <c r="I2">
-        <v>1988</v>
+        <v>2011</v>
       </c>
     </row>
     <row r="3" spans="1:9">
@@ -917,7 +917,7 @@
         <v>8348</v>
       </c>
       <c r="I3">
-        <v>2116</v>
+        <v>2128</v>
       </c>
     </row>
     <row r="4" spans="1:9">
@@ -946,7 +946,7 @@
         <v>526</v>
       </c>
       <c r="I4">
-        <v>114</v>
+        <v>115</v>
       </c>
     </row>
     <row r="5" spans="1:9">
@@ -975,7 +975,7 @@
         <v>6656</v>
       </c>
       <c r="I5">
-        <v>2222</v>
+        <v>2240</v>
       </c>
     </row>
     <row r="6" spans="1:9">
@@ -998,13 +998,13 @@
         <v>1854</v>
       </c>
       <c r="G6">
-        <v>1426</v>
+        <v>1427</v>
       </c>
       <c r="H6">
         <v>1657</v>
       </c>
       <c r="I6">
-        <v>530</v>
+        <v>531</v>
       </c>
     </row>
     <row r="7" spans="1:9">
@@ -1033,7 +1033,7 @@
         <v>802</v>
       </c>
       <c r="I7">
-        <v>186</v>
+        <v>187</v>
       </c>
     </row>
     <row r="8" spans="1:9">
@@ -1059,10 +1059,10 @@
         <v>9952</v>
       </c>
       <c r="H8">
-        <v>10574</v>
+        <v>10575</v>
       </c>
       <c r="I8">
-        <v>4136</v>
+        <v>4167</v>
       </c>
     </row>
     <row r="9" spans="1:9">
@@ -1091,7 +1091,7 @@
         <v>7922</v>
       </c>
       <c r="I9">
-        <v>2517</v>
+        <v>2533</v>
       </c>
     </row>
     <row r="10" spans="1:9">
@@ -1117,10 +1117,10 @@
         <v>41279</v>
       </c>
       <c r="H10">
-        <v>40667</v>
+        <v>40669</v>
       </c>
       <c r="I10">
-        <v>14558</v>
+        <v>14662</v>
       </c>
     </row>
     <row r="11" spans="1:9">
@@ -1143,13 +1143,13 @@
         <v>105508</v>
       </c>
       <c r="G11">
-        <v>85218</v>
+        <v>85219</v>
       </c>
       <c r="H11">
-        <v>84390</v>
+        <v>84393</v>
       </c>
       <c r="I11">
-        <v>28367</v>
+        <v>28574</v>
       </c>
     </row>
   </sheetData>
@@ -1318,7 +1318,7 @@
         <v>220</v>
       </c>
       <c r="I5">
-        <v>86</v>
+        <v>88</v>
       </c>
     </row>
     <row r="6" spans="1:9">
@@ -1463,7 +1463,7 @@
         <v>856</v>
       </c>
       <c r="I10">
-        <v>312</v>
+        <v>314</v>
       </c>
     </row>
     <row r="11" spans="1:9">
@@ -1492,7 +1492,7 @@
         <v>2236</v>
       </c>
       <c r="I11">
-        <v>768</v>
+        <v>772</v>
       </c>
     </row>
   </sheetData>
@@ -1843,7 +1843,7 @@
         <v>43</v>
       </c>
       <c r="I3">
-        <v>28</v>
+        <v>29</v>
       </c>
     </row>
     <row r="4" spans="1:9">
@@ -2014,7 +2014,7 @@
         <v>95</v>
       </c>
       <c r="I9">
-        <v>37</v>
+        <v>38</v>
       </c>
     </row>
     <row r="10" spans="1:9">
@@ -2043,7 +2043,7 @@
         <v>691</v>
       </c>
       <c r="I10">
-        <v>221</v>
+        <v>223</v>
       </c>
     </row>
     <row r="11" spans="1:9">
@@ -2072,7 +2072,7 @@
         <v>1149</v>
       </c>
       <c r="I11">
-        <v>402</v>
+        <v>406</v>
       </c>
     </row>
   </sheetData>
@@ -2295,7 +2295,7 @@
         <v>60</v>
       </c>
       <c r="I8">
-        <v>37</v>
+        <v>38</v>
       </c>
     </row>
     <row r="9" spans="1:9">
@@ -2353,7 +2353,7 @@
         <v>371</v>
       </c>
       <c r="I10">
-        <v>137</v>
+        <v>140</v>
       </c>
     </row>
     <row r="11" spans="1:9">
@@ -2382,7 +2382,7 @@
         <v>500</v>
       </c>
       <c r="I11">
-        <v>190</v>
+        <v>194</v>
       </c>
     </row>
   </sheetData>
@@ -2623,7 +2623,7 @@
         <v>49</v>
       </c>
       <c r="I8">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="9" spans="1:9">
@@ -2681,7 +2681,7 @@
         <v>224</v>
       </c>
       <c r="I10">
-        <v>97</v>
+        <v>98</v>
       </c>
     </row>
     <row r="11" spans="1:9">
@@ -2710,7 +2710,7 @@
         <v>474</v>
       </c>
       <c r="I11">
-        <v>177</v>
+        <v>179</v>
       </c>
     </row>
   </sheetData>
@@ -2989,7 +2989,7 @@
         <v>22</v>
       </c>
       <c r="I9">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="10" spans="1:9">
@@ -3018,7 +3018,7 @@
         <v>61</v>
       </c>
       <c r="I10">
-        <v>41</v>
+        <v>43</v>
       </c>
     </row>
     <row r="11" spans="1:9">
@@ -3047,7 +3047,7 @@
         <v>200</v>
       </c>
       <c r="I11">
-        <v>92</v>
+        <v>95</v>
       </c>
     </row>
   </sheetData>
@@ -3303,7 +3303,7 @@
         <v>329</v>
       </c>
       <c r="I8">
-        <v>132</v>
+        <v>134</v>
       </c>
     </row>
     <row r="9" spans="1:9">
@@ -3361,7 +3361,7 @@
         <v>692</v>
       </c>
       <c r="I10">
-        <v>226</v>
+        <v>229</v>
       </c>
     </row>
     <row r="11" spans="1:9">
@@ -3390,7 +3390,7 @@
         <v>2161</v>
       </c>
       <c r="I11">
-        <v>644</v>
+        <v>649</v>
       </c>
     </row>
   </sheetData>
@@ -3501,7 +3501,7 @@
         <v>175</v>
       </c>
       <c r="I3">
-        <v>46</v>
+        <v>47</v>
       </c>
     </row>
     <row r="4" spans="1:9">
@@ -3646,7 +3646,7 @@
         <v>149</v>
       </c>
       <c r="I8">
-        <v>42</v>
+        <v>43</v>
       </c>
     </row>
     <row r="9" spans="1:9">
@@ -3675,7 +3675,7 @@
         <v>88</v>
       </c>
       <c r="I9">
-        <v>39</v>
+        <v>40</v>
       </c>
     </row>
     <row r="10" spans="1:9">
@@ -3704,7 +3704,7 @@
         <v>435</v>
       </c>
       <c r="I10">
-        <v>141</v>
+        <v>144</v>
       </c>
     </row>
     <row r="11" spans="1:9">
@@ -3733,7 +3733,7 @@
         <v>1119</v>
       </c>
       <c r="I11">
-        <v>347</v>
+        <v>353</v>
       </c>
     </row>
   </sheetData>
@@ -3815,7 +3815,7 @@
         <v>279</v>
       </c>
       <c r="I2">
-        <v>65</v>
+        <v>66</v>
       </c>
     </row>
     <row r="3" spans="1:9">
@@ -3844,7 +3844,7 @@
         <v>420</v>
       </c>
       <c r="I3">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="4" spans="1:9">
@@ -4018,7 +4018,7 @@
         <v>301</v>
       </c>
       <c r="I9">
-        <v>96</v>
+        <v>98</v>
       </c>
     </row>
     <row r="10" spans="1:9">
@@ -4047,7 +4047,7 @@
         <v>769</v>
       </c>
       <c r="I10">
-        <v>243</v>
+        <v>245</v>
       </c>
     </row>
     <row r="11" spans="1:9">
@@ -4076,7 +4076,7 @@
         <v>2309</v>
       </c>
       <c r="I11">
-        <v>651</v>
+        <v>655</v>
       </c>
     </row>
   </sheetData>
@@ -4158,7 +4158,7 @@
         <v>61</v>
       </c>
       <c r="I2">
-        <v>20</v>
+        <v>21</v>
       </c>
     </row>
     <row r="3" spans="1:9">
@@ -4187,7 +4187,7 @@
         <v>50</v>
       </c>
       <c r="I3">
-        <v>20</v>
+        <v>21</v>
       </c>
     </row>
     <row r="4" spans="1:9">
@@ -4358,7 +4358,7 @@
         <v>66</v>
       </c>
       <c r="I9">
-        <v>27</v>
+        <v>28</v>
       </c>
     </row>
     <row r="10" spans="1:9">
@@ -4387,7 +4387,7 @@
         <v>275</v>
       </c>
       <c r="I10">
-        <v>104</v>
+        <v>107</v>
       </c>
     </row>
     <row r="11" spans="1:9">
@@ -4416,7 +4416,7 @@
         <v>615</v>
       </c>
       <c r="I11">
-        <v>249</v>
+        <v>255</v>
       </c>
     </row>
   </sheetData>
@@ -4498,7 +4498,7 @@
         <v>76</v>
       </c>
       <c r="I2">
-        <v>19</v>
+        <v>20</v>
       </c>
     </row>
     <row r="3" spans="1:9">
@@ -4698,7 +4698,7 @@
         <v>43</v>
       </c>
       <c r="I9">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="10" spans="1:9">
@@ -4756,7 +4756,7 @@
         <v>587</v>
       </c>
       <c r="I11">
-        <v>155</v>
+        <v>157</v>
       </c>
     </row>
   </sheetData>
@@ -4838,7 +4838,7 @@
         <v>767</v>
       </c>
       <c r="I2">
-        <v>235</v>
+        <v>236</v>
       </c>
     </row>
     <row r="3" spans="1:9">
@@ -4896,7 +4896,7 @@
         <v>303</v>
       </c>
       <c r="I4">
-        <v>139</v>
+        <v>140</v>
       </c>
     </row>
     <row r="5" spans="1:9">
@@ -4954,7 +4954,7 @@
         <v>627</v>
       </c>
       <c r="I6">
-        <v>188</v>
+        <v>191</v>
       </c>
     </row>
     <row r="7" spans="1:9">
@@ -4983,7 +4983,7 @@
         <v>2236</v>
       </c>
       <c r="I7">
-        <v>768</v>
+        <v>772</v>
       </c>
     </row>
     <row r="8" spans="1:9">
@@ -5012,7 +5012,7 @@
         <v>3973</v>
       </c>
       <c r="I8">
-        <v>1198</v>
+        <v>1205</v>
       </c>
     </row>
     <row r="9" spans="1:9">
@@ -5070,7 +5070,7 @@
         <v>692</v>
       </c>
       <c r="I10">
-        <v>230</v>
+        <v>234</v>
       </c>
     </row>
     <row r="11" spans="1:9">
@@ -5099,7 +5099,7 @@
         <v>1312</v>
       </c>
       <c r="I11">
-        <v>463</v>
+        <v>464</v>
       </c>
     </row>
     <row r="12" spans="1:9">
@@ -5128,7 +5128,7 @@
         <v>265</v>
       </c>
       <c r="I12">
-        <v>95</v>
+        <v>96</v>
       </c>
     </row>
     <row r="13" spans="1:9">
@@ -5157,7 +5157,7 @@
         <v>173</v>
       </c>
       <c r="I13">
-        <v>56</v>
+        <v>57</v>
       </c>
     </row>
     <row r="14" spans="1:9">
@@ -5186,7 +5186,7 @@
         <v>474</v>
       </c>
       <c r="I14">
-        <v>177</v>
+        <v>179</v>
       </c>
     </row>
     <row r="15" spans="1:9">
@@ -5244,7 +5244,7 @@
         <v>435</v>
       </c>
       <c r="I16">
-        <v>161</v>
+        <v>163</v>
       </c>
     </row>
     <row r="17" spans="1:9">
@@ -5331,7 +5331,7 @@
         <v>1973</v>
       </c>
       <c r="I19">
-        <v>635</v>
+        <v>641</v>
       </c>
     </row>
     <row r="20" spans="1:9">
@@ -5354,13 +5354,13 @@
         <v>2076</v>
       </c>
       <c r="G20">
-        <v>1834</v>
+        <v>1835</v>
       </c>
       <c r="H20">
         <v>1676</v>
       </c>
       <c r="I20">
-        <v>608</v>
+        <v>612</v>
       </c>
     </row>
     <row r="21" spans="1:9">
@@ -5418,7 +5418,7 @@
         <v>275</v>
       </c>
       <c r="I22">
-        <v>113</v>
+        <v>117</v>
       </c>
     </row>
     <row r="23" spans="1:9">
@@ -5447,7 +5447,7 @@
         <v>944</v>
       </c>
       <c r="I23">
-        <v>308</v>
+        <v>307</v>
       </c>
     </row>
     <row r="24" spans="1:9">
@@ -5476,7 +5476,7 @@
         <v>531</v>
       </c>
       <c r="I24">
-        <v>128</v>
+        <v>129</v>
       </c>
     </row>
     <row r="25" spans="1:9">
@@ -5505,7 +5505,7 @@
         <v>325</v>
       </c>
       <c r="I25">
-        <v>98</v>
+        <v>99</v>
       </c>
     </row>
     <row r="26" spans="1:9">
@@ -5534,7 +5534,7 @@
         <v>180</v>
       </c>
       <c r="I26">
-        <v>54</v>
+        <v>55</v>
       </c>
     </row>
     <row r="27" spans="1:9">
@@ -5563,7 +5563,7 @@
         <v>969</v>
       </c>
       <c r="I27">
-        <v>307</v>
+        <v>314</v>
       </c>
     </row>
     <row r="28" spans="1:9">
@@ -5621,7 +5621,7 @@
         <v>3522</v>
       </c>
       <c r="I29">
-        <v>1068</v>
+        <v>1079</v>
       </c>
     </row>
     <row r="30" spans="1:9">
@@ -5650,7 +5650,7 @@
         <v>200</v>
       </c>
       <c r="I30">
-        <v>92</v>
+        <v>95</v>
       </c>
     </row>
     <row r="31" spans="1:9">
@@ -5679,7 +5679,7 @@
         <v>615</v>
       </c>
       <c r="I31">
-        <v>249</v>
+        <v>255</v>
       </c>
     </row>
     <row r="32" spans="1:9">
@@ -5737,7 +5737,7 @@
         <v>2688</v>
       </c>
       <c r="I33">
-        <v>788</v>
+        <v>795</v>
       </c>
     </row>
     <row r="34" spans="1:9">
@@ -5766,7 +5766,7 @@
         <v>565</v>
       </c>
       <c r="I34">
-        <v>201</v>
+        <v>202</v>
       </c>
     </row>
     <row r="35" spans="1:9">
@@ -5853,7 +5853,7 @@
         <v>2161</v>
       </c>
       <c r="I37">
-        <v>644</v>
+        <v>649</v>
       </c>
     </row>
     <row r="38" spans="1:9">
@@ -5882,7 +5882,7 @@
         <v>104</v>
       </c>
       <c r="I38">
-        <v>20</v>
+        <v>21</v>
       </c>
     </row>
     <row r="39" spans="1:9">
@@ -5911,7 +5911,7 @@
         <v>140</v>
       </c>
       <c r="I39">
-        <v>61</v>
+        <v>62</v>
       </c>
     </row>
     <row r="40" spans="1:9">
@@ -5998,7 +5998,7 @@
         <v>2425</v>
       </c>
       <c r="I42">
-        <v>695</v>
+        <v>698</v>
       </c>
     </row>
     <row r="43" spans="1:9">
@@ -6027,7 +6027,7 @@
         <v>841</v>
       </c>
       <c r="I43">
-        <v>282</v>
+        <v>283</v>
       </c>
     </row>
     <row r="44" spans="1:9">
@@ -6056,7 +6056,7 @@
         <v>967</v>
       </c>
       <c r="I44">
-        <v>281</v>
+        <v>283</v>
       </c>
     </row>
     <row r="45" spans="1:9">
@@ -6085,7 +6085,7 @@
         <v>141</v>
       </c>
       <c r="I45">
-        <v>60</v>
+        <v>61</v>
       </c>
     </row>
     <row r="46" spans="1:9">
@@ -6172,7 +6172,7 @@
         <v>1998</v>
       </c>
       <c r="I48">
-        <v>631</v>
+        <v>636</v>
       </c>
     </row>
     <row r="49" spans="1:9">
@@ -6201,7 +6201,7 @@
         <v>1162</v>
       </c>
       <c r="I49">
-        <v>398</v>
+        <v>401</v>
       </c>
     </row>
     <row r="50" spans="1:9">
@@ -6230,7 +6230,7 @@
         <v>760</v>
       </c>
       <c r="I50">
-        <v>210</v>
+        <v>211</v>
       </c>
     </row>
     <row r="51" spans="1:9">
@@ -6259,7 +6259,7 @@
         <v>1012</v>
       </c>
       <c r="I51">
-        <v>303</v>
+        <v>307</v>
       </c>
     </row>
     <row r="52" spans="1:9">
@@ -6288,7 +6288,7 @@
         <v>1246</v>
       </c>
       <c r="I52">
-        <v>403</v>
+        <v>405</v>
       </c>
     </row>
     <row r="53" spans="1:9">
@@ -6317,7 +6317,7 @@
         <v>1182</v>
       </c>
       <c r="I53">
-        <v>383</v>
+        <v>385</v>
       </c>
     </row>
     <row r="54" spans="1:9">
@@ -6346,7 +6346,7 @@
         <v>2196</v>
       </c>
       <c r="I54">
-        <v>1015</v>
+        <v>1026</v>
       </c>
     </row>
     <row r="55" spans="1:9">
@@ -6375,7 +6375,7 @@
         <v>908</v>
       </c>
       <c r="I55">
-        <v>328</v>
+        <v>329</v>
       </c>
     </row>
     <row r="56" spans="1:9">
@@ -6404,7 +6404,7 @@
         <v>482</v>
       </c>
       <c r="I56">
-        <v>158</v>
+        <v>159</v>
       </c>
     </row>
     <row r="57" spans="1:9">
@@ -6433,7 +6433,7 @@
         <v>296</v>
       </c>
       <c r="I57">
-        <v>105</v>
+        <v>106</v>
       </c>
     </row>
     <row r="58" spans="1:9">
@@ -6462,7 +6462,7 @@
         <v>338</v>
       </c>
       <c r="I58">
-        <v>28</v>
+        <v>29</v>
       </c>
     </row>
     <row r="59" spans="1:9">
@@ -6491,7 +6491,7 @@
         <v>177</v>
       </c>
       <c r="I59">
-        <v>67</v>
+        <v>68</v>
       </c>
     </row>
     <row r="60" spans="1:9">
@@ -6520,7 +6520,7 @@
         <v>618</v>
       </c>
       <c r="I60">
-        <v>201</v>
+        <v>202</v>
       </c>
     </row>
     <row r="61" spans="1:9">
@@ -6604,10 +6604,10 @@
         <v>1562</v>
       </c>
       <c r="H63">
-        <v>1931</v>
+        <v>1934</v>
       </c>
       <c r="I63">
-        <v>596</v>
+        <v>608</v>
       </c>
     </row>
     <row r="64" spans="1:9">
@@ -6636,7 +6636,7 @@
         <v>788</v>
       </c>
       <c r="I64">
-        <v>394</v>
+        <v>396</v>
       </c>
     </row>
     <row r="65" spans="1:9">
@@ -6665,7 +6665,7 @@
         <v>1208</v>
       </c>
       <c r="I65">
-        <v>422</v>
+        <v>426</v>
       </c>
     </row>
     <row r="66" spans="1:9">
@@ -6723,7 +6723,7 @@
         <v>2309</v>
       </c>
       <c r="I67">
-        <v>651</v>
+        <v>655</v>
       </c>
     </row>
     <row r="68" spans="1:9">
@@ -6781,7 +6781,7 @@
         <v>354</v>
       </c>
       <c r="I69">
-        <v>126</v>
+        <v>128</v>
       </c>
     </row>
     <row r="70" spans="1:9">
@@ -6810,7 +6810,7 @@
         <v>500</v>
       </c>
       <c r="I70">
-        <v>190</v>
+        <v>194</v>
       </c>
     </row>
     <row r="71" spans="1:9">
@@ -6839,7 +6839,7 @@
         <v>220</v>
       </c>
       <c r="I71">
-        <v>67</v>
+        <v>68</v>
       </c>
     </row>
     <row r="72" spans="1:9">
@@ -6868,7 +6868,7 @@
         <v>564</v>
       </c>
       <c r="I72">
-        <v>181</v>
+        <v>183</v>
       </c>
     </row>
     <row r="73" spans="1:9">
@@ -6897,7 +6897,7 @@
         <v>933</v>
       </c>
       <c r="I73">
-        <v>313</v>
+        <v>317</v>
       </c>
     </row>
     <row r="74" spans="1:9">
@@ -6984,7 +6984,7 @@
         <v>1998</v>
       </c>
       <c r="I76">
-        <v>837</v>
+        <v>840</v>
       </c>
     </row>
     <row r="77" spans="1:9">
@@ -7013,7 +7013,7 @@
         <v>377</v>
       </c>
       <c r="I77">
-        <v>114</v>
+        <v>115</v>
       </c>
     </row>
     <row r="78" spans="1:9">
@@ -7042,7 +7042,7 @@
         <v>1372</v>
       </c>
       <c r="I78">
-        <v>458</v>
+        <v>460</v>
       </c>
     </row>
     <row r="79" spans="1:9">
@@ -7071,7 +7071,7 @@
         <v>1893</v>
       </c>
       <c r="I79">
-        <v>580</v>
+        <v>583</v>
       </c>
     </row>
     <row r="80" spans="1:9">
@@ -7129,7 +7129,7 @@
         <v>156</v>
       </c>
       <c r="I81">
-        <v>56</v>
+        <v>57</v>
       </c>
     </row>
     <row r="82" spans="1:9">
@@ -7187,7 +7187,7 @@
         <v>1319</v>
       </c>
       <c r="I83">
-        <v>429</v>
+        <v>432</v>
       </c>
     </row>
     <row r="84" spans="1:9">
@@ -7216,7 +7216,7 @@
         <v>587</v>
       </c>
       <c r="I84">
-        <v>155</v>
+        <v>157</v>
       </c>
     </row>
     <row r="85" spans="1:9">
@@ -7245,7 +7245,7 @@
         <v>2851</v>
       </c>
       <c r="I85">
-        <v>987</v>
+        <v>991</v>
       </c>
     </row>
     <row r="86" spans="1:9">
@@ -7303,7 +7303,7 @@
         <v>250</v>
       </c>
       <c r="I87">
-        <v>78</v>
+        <v>79</v>
       </c>
     </row>
     <row r="88" spans="1:9">
@@ -7332,7 +7332,7 @@
         <v>690</v>
       </c>
       <c r="I88">
-        <v>252</v>
+        <v>253</v>
       </c>
     </row>
     <row r="89" spans="1:9">
@@ -7361,7 +7361,7 @@
         <v>1294</v>
       </c>
       <c r="I89">
-        <v>452</v>
+        <v>456</v>
       </c>
     </row>
     <row r="90" spans="1:9">
@@ -7390,7 +7390,7 @@
         <v>903</v>
       </c>
       <c r="I90">
-        <v>327</v>
+        <v>328</v>
       </c>
     </row>
     <row r="91" spans="1:9">
@@ -7419,7 +7419,7 @@
         <v>722</v>
       </c>
       <c r="I91">
-        <v>248</v>
+        <v>249</v>
       </c>
     </row>
     <row r="92" spans="1:9">
@@ -7477,7 +7477,7 @@
         <v>501</v>
       </c>
       <c r="I93">
-        <v>187</v>
+        <v>189</v>
       </c>
     </row>
     <row r="94" spans="1:9">
@@ -7506,7 +7506,7 @@
         <v>1595</v>
       </c>
       <c r="I94">
-        <v>751</v>
+        <v>752</v>
       </c>
     </row>
     <row r="95" spans="1:9">
@@ -7535,7 +7535,7 @@
         <v>1315</v>
       </c>
       <c r="I95">
-        <v>366</v>
+        <v>369</v>
       </c>
     </row>
     <row r="96" spans="1:9">
@@ -7564,7 +7564,7 @@
         <v>1149</v>
       </c>
       <c r="I96">
-        <v>402</v>
+        <v>406</v>
       </c>
     </row>
     <row r="97" spans="1:9">
@@ -7593,7 +7593,7 @@
         <v>1270</v>
       </c>
       <c r="I97">
-        <v>435</v>
+        <v>437</v>
       </c>
     </row>
     <row r="98" spans="1:9">
@@ -7622,7 +7622,7 @@
         <v>963</v>
       </c>
       <c r="I98">
-        <v>387</v>
+        <v>388</v>
       </c>
     </row>
     <row r="99" spans="1:9">
@@ -7651,7 +7651,7 @@
         <v>1119</v>
       </c>
       <c r="I99">
-        <v>347</v>
+        <v>353</v>
       </c>
     </row>
     <row r="100" spans="1:9">
@@ -7703,13 +7703,13 @@
         <v>105508</v>
       </c>
       <c r="G101">
-        <v>85218</v>
+        <v>85219</v>
       </c>
       <c r="H101">
-        <v>84390</v>
+        <v>84393</v>
       </c>
       <c r="I101">
-        <v>28367</v>
+        <v>28574</v>
       </c>
     </row>
   </sheetData>
@@ -7893,7 +7893,7 @@
         <v>188</v>
       </c>
       <c r="I2">
-        <v>46</v>
+        <v>48</v>
       </c>
     </row>
     <row r="3" spans="1:9">
@@ -7980,7 +7980,7 @@
         <v>92</v>
       </c>
       <c r="I5">
-        <v>32</v>
+        <v>33</v>
       </c>
     </row>
     <row r="6" spans="1:9">
@@ -8125,7 +8125,7 @@
         <v>418</v>
       </c>
       <c r="I10">
-        <v>158</v>
+        <v>159</v>
       </c>
     </row>
     <row r="11" spans="1:9">
@@ -8154,7 +8154,7 @@
         <v>1208</v>
       </c>
       <c r="I11">
-        <v>422</v>
+        <v>426</v>
       </c>
     </row>
   </sheetData>
@@ -8236,7 +8236,7 @@
         <v>40</v>
       </c>
       <c r="I2">
-        <v>14</v>
+        <v>15</v>
       </c>
     </row>
     <row r="3" spans="1:9">
@@ -8365,6 +8365,9 @@
       <c r="H7">
         <v>1</v>
       </c>
+      <c r="I7">
+        <v>1</v>
+      </c>
     </row>
     <row r="8" spans="1:9">
       <c r="A8" s="1" t="s">
@@ -8392,7 +8395,7 @@
         <v>76</v>
       </c>
       <c r="I8">
-        <v>42</v>
+        <v>44</v>
       </c>
     </row>
     <row r="9" spans="1:9">
@@ -8421,7 +8424,7 @@
         <v>69</v>
       </c>
       <c r="I9">
-        <v>32</v>
+        <v>33</v>
       </c>
     </row>
     <row r="10" spans="1:9">
@@ -8450,7 +8453,7 @@
         <v>622</v>
       </c>
       <c r="I10">
-        <v>180</v>
+        <v>182</v>
       </c>
     </row>
     <row r="11" spans="1:9">
@@ -8479,7 +8482,7 @@
         <v>969</v>
       </c>
       <c r="I11">
-        <v>307</v>
+        <v>314</v>
       </c>
     </row>
   </sheetData>
@@ -8561,7 +8564,7 @@
         <v>179</v>
       </c>
       <c r="I2">
-        <v>49</v>
+        <v>51</v>
       </c>
     </row>
     <row r="3" spans="1:9">
@@ -8793,7 +8796,7 @@
         <v>465</v>
       </c>
       <c r="I10">
-        <v>180</v>
+        <v>181</v>
       </c>
     </row>
     <row r="11" spans="1:9">
@@ -8822,7 +8825,7 @@
         <v>1319</v>
       </c>
       <c r="I11">
-        <v>429</v>
+        <v>432</v>
       </c>
     </row>
   </sheetData>
@@ -8904,7 +8907,7 @@
         <v>283</v>
       </c>
       <c r="I2">
-        <v>83</v>
+        <v>84</v>
       </c>
     </row>
     <row r="3" spans="1:9">
@@ -8991,7 +8994,7 @@
         <v>147</v>
       </c>
       <c r="I5">
-        <v>53</v>
+        <v>54</v>
       </c>
     </row>
     <row r="6" spans="1:9">
@@ -9020,7 +9023,7 @@
         <v>63</v>
       </c>
       <c r="I6">
-        <v>19</v>
+        <v>20</v>
       </c>
     </row>
     <row r="7" spans="1:9">
@@ -9078,7 +9081,7 @@
         <v>369</v>
       </c>
       <c r="I8">
-        <v>115</v>
+        <v>117</v>
       </c>
     </row>
     <row r="9" spans="1:9">
@@ -9136,7 +9139,7 @@
         <v>840</v>
       </c>
       <c r="I10">
-        <v>268</v>
+        <v>270</v>
       </c>
     </row>
     <row r="11" spans="1:9">
@@ -9165,7 +9168,7 @@
         <v>2688</v>
       </c>
       <c r="I11">
-        <v>788</v>
+        <v>795</v>
       </c>
     </row>
   </sheetData>
@@ -9421,7 +9424,7 @@
         <v>153</v>
       </c>
       <c r="I8">
-        <v>58</v>
+        <v>59</v>
       </c>
     </row>
     <row r="9" spans="1:9">
@@ -9479,7 +9482,7 @@
         <v>387</v>
       </c>
       <c r="I10">
-        <v>127</v>
+        <v>129</v>
       </c>
     </row>
     <row r="11" spans="1:9">
@@ -9508,7 +9511,7 @@
         <v>1315</v>
       </c>
       <c r="I11">
-        <v>366</v>
+        <v>369</v>
       </c>
     </row>
   </sheetData>
@@ -9918,7 +9921,7 @@
         <v>231</v>
       </c>
       <c r="I2">
-        <v>52</v>
+        <v>53</v>
       </c>
     </row>
     <row r="3" spans="1:9">
@@ -9947,7 +9950,7 @@
         <v>275</v>
       </c>
       <c r="I3">
-        <v>54</v>
+        <v>55</v>
       </c>
     </row>
     <row r="4" spans="1:9">
@@ -10121,7 +10124,7 @@
         <v>196</v>
       </c>
       <c r="I9">
-        <v>66</v>
+        <v>67</v>
       </c>
     </row>
     <row r="10" spans="1:9">
@@ -10179,7 +10182,7 @@
         <v>1893</v>
       </c>
       <c r="I11">
-        <v>580</v>
+        <v>583</v>
       </c>
     </row>
   </sheetData>
@@ -10478,7 +10481,7 @@
         <v>91</v>
       </c>
       <c r="I10">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="11" spans="1:9">
@@ -10507,7 +10510,7 @@
         <v>220</v>
       </c>
       <c r="I11">
-        <v>67</v>
+        <v>68</v>
       </c>
     </row>
   </sheetData>
@@ -11105,7 +11108,7 @@
         <v>32</v>
       </c>
       <c r="I9">
-        <v>14</v>
+        <v>15</v>
       </c>
     </row>
     <row r="10" spans="1:9">
@@ -11163,7 +11166,7 @@
         <v>618</v>
       </c>
       <c r="I11">
-        <v>201</v>
+        <v>202</v>
       </c>
     </row>
   </sheetData>
@@ -11245,7 +11248,7 @@
         <v>86</v>
       </c>
       <c r="I2">
-        <v>18</v>
+        <v>19</v>
       </c>
     </row>
     <row r="3" spans="1:9">
@@ -11474,7 +11477,7 @@
         <v>791</v>
       </c>
       <c r="I10">
-        <v>284</v>
+        <v>287</v>
       </c>
     </row>
     <row r="11" spans="1:9">
@@ -11503,7 +11506,7 @@
         <v>1294</v>
       </c>
       <c r="I11">
-        <v>452</v>
+        <v>456</v>
       </c>
     </row>
   </sheetData>
@@ -11585,7 +11588,7 @@
         <v>38</v>
       </c>
       <c r="I2">
-        <v>15</v>
+        <v>16</v>
       </c>
     </row>
     <row r="3" spans="1:9">
@@ -11750,7 +11753,7 @@
         <v>211</v>
       </c>
       <c r="I8">
-        <v>122</v>
+        <v>123</v>
       </c>
     </row>
     <row r="9" spans="1:9">
@@ -11837,7 +11840,7 @@
         <v>788</v>
       </c>
       <c r="I11">
-        <v>394</v>
+        <v>396</v>
       </c>
     </row>
   </sheetData>
@@ -12446,7 +12449,7 @@
         <v>1132</v>
       </c>
       <c r="I10">
-        <v>580</v>
+        <v>581</v>
       </c>
     </row>
     <row r="11" spans="1:9">
@@ -12475,7 +12478,7 @@
         <v>1595</v>
       </c>
       <c r="I11">
-        <v>751</v>
+        <v>752</v>
       </c>
     </row>
   </sheetData>
@@ -12728,7 +12731,7 @@
         <v>241</v>
       </c>
       <c r="I8">
-        <v>90</v>
+        <v>92</v>
       </c>
     </row>
     <row r="9" spans="1:9">
@@ -12786,7 +12789,7 @@
         <v>1314</v>
       </c>
       <c r="I10">
-        <v>605</v>
+        <v>606</v>
       </c>
     </row>
     <row r="11" spans="1:9">
@@ -12815,7 +12818,7 @@
         <v>1998</v>
       </c>
       <c r="I11">
-        <v>837</v>
+        <v>840</v>
       </c>
     </row>
   </sheetData>
@@ -13424,7 +13427,7 @@
         <v>133</v>
       </c>
       <c r="I10">
-        <v>51</v>
+        <v>52</v>
       </c>
     </row>
     <row r="11" spans="1:9">
@@ -13453,7 +13456,7 @@
         <v>250</v>
       </c>
       <c r="I11">
-        <v>78</v>
+        <v>79</v>
       </c>
     </row>
   </sheetData>
@@ -14051,7 +14054,7 @@
         <v>121</v>
       </c>
       <c r="I10">
-        <v>39</v>
+        <v>40</v>
       </c>
     </row>
     <row r="11" spans="1:9">
@@ -14080,7 +14083,7 @@
         <v>325</v>
       </c>
       <c r="I11">
-        <v>98</v>
+        <v>99</v>
       </c>
     </row>
   </sheetData>
@@ -14162,7 +14165,7 @@
         <v>9</v>
       </c>
       <c r="I2">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="3" spans="1:9">
@@ -14234,7 +14237,7 @@
         <v>41</v>
       </c>
       <c r="I5">
-        <v>20</v>
+        <v>21</v>
       </c>
     </row>
     <row r="6" spans="1:9">
@@ -14390,7 +14393,7 @@
         <v>435</v>
       </c>
       <c r="I11">
-        <v>161</v>
+        <v>163</v>
       </c>
     </row>
   </sheetData>
@@ -14631,7 +14634,7 @@
         <v>171</v>
       </c>
       <c r="I8">
-        <v>70</v>
+        <v>71</v>
       </c>
     </row>
     <row r="9" spans="1:9">
@@ -14689,7 +14692,7 @@
         <v>773</v>
       </c>
       <c r="I10">
-        <v>255</v>
+        <v>257</v>
       </c>
     </row>
     <row r="11" spans="1:9">
@@ -14718,7 +14721,7 @@
         <v>1162</v>
       </c>
       <c r="I11">
-        <v>398</v>
+        <v>401</v>
       </c>
     </row>
   </sheetData>
@@ -14829,7 +14832,7 @@
         <v>479</v>
       </c>
       <c r="I3">
-        <v>133</v>
+        <v>134</v>
       </c>
     </row>
     <row r="4" spans="1:9">
@@ -14887,7 +14890,7 @@
         <v>262</v>
       </c>
       <c r="I5">
-        <v>126</v>
+        <v>127</v>
       </c>
     </row>
     <row r="6" spans="1:9">
@@ -14974,7 +14977,7 @@
         <v>349</v>
       </c>
       <c r="I8">
-        <v>152</v>
+        <v>153</v>
       </c>
     </row>
     <row r="9" spans="1:9">
@@ -15003,7 +15006,7 @@
         <v>300</v>
       </c>
       <c r="I9">
-        <v>99</v>
+        <v>100</v>
       </c>
     </row>
     <row r="10" spans="1:9">
@@ -15061,7 +15064,7 @@
         <v>2851</v>
       </c>
       <c r="I11">
-        <v>987</v>
+        <v>991</v>
       </c>
     </row>
   </sheetData>
@@ -15369,7 +15372,7 @@
         <v>783</v>
       </c>
       <c r="I10">
-        <v>281</v>
+        <v>283</v>
       </c>
     </row>
     <row r="11" spans="1:9">
@@ -15398,7 +15401,7 @@
         <v>1270</v>
       </c>
       <c r="I11">
-        <v>435</v>
+        <v>437</v>
       </c>
     </row>
   </sheetData>
@@ -15712,7 +15715,7 @@
         <v>390</v>
       </c>
       <c r="I10">
-        <v>163</v>
+        <v>164</v>
       </c>
     </row>
     <row r="11" spans="1:9">
@@ -15741,7 +15744,7 @@
         <v>908</v>
       </c>
       <c r="I11">
-        <v>328</v>
+        <v>329</v>
       </c>
     </row>
   </sheetData>
@@ -15852,7 +15855,7 @@
         <v>116</v>
       </c>
       <c r="I3">
-        <v>34</v>
+        <v>35</v>
       </c>
     </row>
     <row r="4" spans="1:9">
@@ -15991,7 +15994,7 @@
         <v>239</v>
       </c>
       <c r="I8">
-        <v>128</v>
+        <v>130</v>
       </c>
     </row>
     <row r="9" spans="1:9">
@@ -16020,7 +16023,7 @@
         <v>205</v>
       </c>
       <c r="I9">
-        <v>79</v>
+        <v>80</v>
       </c>
     </row>
     <row r="10" spans="1:9">
@@ -16049,7 +16052,7 @@
         <v>1457</v>
       </c>
       <c r="I10">
-        <v>690</v>
+        <v>697</v>
       </c>
     </row>
     <row r="11" spans="1:9">
@@ -16078,7 +16081,7 @@
         <v>2196</v>
       </c>
       <c r="I11">
-        <v>1015</v>
+        <v>1026</v>
       </c>
     </row>
   </sheetData>
@@ -16247,7 +16250,7 @@
         <v>92</v>
       </c>
       <c r="I5">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="6" spans="1:9">
@@ -16389,7 +16392,7 @@
         <v>530</v>
       </c>
       <c r="I10">
-        <v>172</v>
+        <v>175</v>
       </c>
     </row>
     <row r="11" spans="1:9">
@@ -16418,7 +16421,7 @@
         <v>933</v>
       </c>
       <c r="I11">
-        <v>313</v>
+        <v>317</v>
       </c>
     </row>
   </sheetData>
@@ -16500,7 +16503,7 @@
         <v>543</v>
       </c>
       <c r="I2">
-        <v>142</v>
+        <v>144</v>
       </c>
     </row>
     <row r="3" spans="1:9">
@@ -16529,7 +16532,7 @@
         <v>675</v>
       </c>
       <c r="I3">
-        <v>156</v>
+        <v>159</v>
       </c>
     </row>
     <row r="4" spans="1:9">
@@ -16674,7 +16677,7 @@
         <v>436</v>
       </c>
       <c r="I8">
-        <v>170</v>
+        <v>172</v>
       </c>
     </row>
     <row r="9" spans="1:9">
@@ -16732,7 +16735,7 @@
         <v>1107</v>
       </c>
       <c r="I10">
-        <v>351</v>
+        <v>355</v>
       </c>
     </row>
     <row r="11" spans="1:9">
@@ -16761,7 +16764,7 @@
         <v>3522</v>
       </c>
       <c r="I11">
-        <v>1068</v>
+        <v>1079</v>
       </c>
     </row>
   </sheetData>
@@ -16930,7 +16933,7 @@
         <v>169</v>
       </c>
       <c r="I5">
-        <v>56</v>
+        <v>57</v>
       </c>
     </row>
     <row r="6" spans="1:9">
@@ -17075,7 +17078,7 @@
         <v>782</v>
       </c>
       <c r="I10">
-        <v>243</v>
+        <v>248</v>
       </c>
     </row>
     <row r="11" spans="1:9">
@@ -17104,7 +17107,7 @@
         <v>1973</v>
       </c>
       <c r="I11">
-        <v>635</v>
+        <v>641</v>
       </c>
     </row>
   </sheetData>
@@ -17403,7 +17406,7 @@
         <v>155</v>
       </c>
       <c r="I10">
-        <v>56</v>
+        <v>60</v>
       </c>
     </row>
     <row r="11" spans="1:9">
@@ -17432,7 +17435,7 @@
         <v>275</v>
       </c>
       <c r="I11">
-        <v>113</v>
+        <v>117</v>
       </c>
     </row>
   </sheetData>
@@ -17598,7 +17601,7 @@
         <v>94</v>
       </c>
       <c r="I5">
-        <v>27</v>
+        <v>28</v>
       </c>
     </row>
     <row r="6" spans="1:9">
@@ -17682,7 +17685,7 @@
         <v>101</v>
       </c>
       <c r="I8">
-        <v>41</v>
+        <v>42</v>
       </c>
     </row>
     <row r="9" spans="1:9">
@@ -17769,7 +17772,7 @@
         <v>967</v>
       </c>
       <c r="I11">
-        <v>281</v>
+        <v>283</v>
       </c>
     </row>
   </sheetData>
@@ -17880,7 +17883,7 @@
         <v>293</v>
       </c>
       <c r="I3">
-        <v>87</v>
+        <v>89</v>
       </c>
     </row>
     <row r="4" spans="1:9">
@@ -17938,7 +17941,7 @@
         <v>266</v>
       </c>
       <c r="I5">
-        <v>57</v>
+        <v>58</v>
       </c>
     </row>
     <row r="6" spans="1:9">
@@ -18025,7 +18028,7 @@
         <v>267</v>
       </c>
       <c r="I8">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="9" spans="1:9">
@@ -18083,7 +18086,7 @@
         <v>955</v>
       </c>
       <c r="I10">
-        <v>292</v>
+        <v>293</v>
       </c>
     </row>
     <row r="11" spans="1:9">
@@ -18112,7 +18115,7 @@
         <v>2425</v>
       </c>
       <c r="I11">
-        <v>695</v>
+        <v>698</v>
       </c>
     </row>
   </sheetData>
@@ -18362,7 +18365,7 @@
         <v>191</v>
       </c>
       <c r="I8">
-        <v>71</v>
+        <v>73</v>
       </c>
     </row>
     <row r="9" spans="1:9">
@@ -18420,7 +18423,7 @@
         <v>1303</v>
       </c>
       <c r="I10">
-        <v>435</v>
+        <v>438</v>
       </c>
     </row>
     <row r="11" spans="1:9">
@@ -18449,7 +18452,7 @@
         <v>1998</v>
       </c>
       <c r="I11">
-        <v>631</v>
+        <v>636</v>
       </c>
     </row>
   </sheetData>
@@ -18716,7 +18719,7 @@
         <v>16</v>
       </c>
       <c r="I9">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="10" spans="1:9">
@@ -18745,7 +18748,7 @@
         <v>221</v>
       </c>
       <c r="I10">
-        <v>76</v>
+        <v>77</v>
       </c>
     </row>
     <row r="11" spans="1:9">
@@ -18774,7 +18777,7 @@
         <v>354</v>
       </c>
       <c r="I11">
-        <v>126</v>
+        <v>128</v>
       </c>
     </row>
   </sheetData>
@@ -18856,7 +18859,7 @@
         <v>64</v>
       </c>
       <c r="I2">
-        <v>18</v>
+        <v>19</v>
       </c>
     </row>
     <row r="3" spans="1:9">
@@ -19079,7 +19082,7 @@
         <v>266</v>
       </c>
       <c r="I10">
-        <v>85</v>
+        <v>87</v>
       </c>
     </row>
     <row r="11" spans="1:9">
@@ -19108,7 +19111,7 @@
         <v>627</v>
       </c>
       <c r="I11">
-        <v>188</v>
+        <v>191</v>
       </c>
     </row>
   </sheetData>
@@ -20046,7 +20049,7 @@
         <v>133</v>
       </c>
       <c r="I9">
-        <v>38</v>
+        <v>39</v>
       </c>
     </row>
     <row r="10" spans="1:9">
@@ -20075,7 +20078,7 @@
         <v>173</v>
       </c>
       <c r="I10">
-        <v>56</v>
+        <v>57</v>
       </c>
     </row>
   </sheetData>
@@ -20157,7 +20160,7 @@
         <v>42</v>
       </c>
       <c r="I2">
-        <v>16</v>
+        <v>17</v>
       </c>
     </row>
     <row r="3" spans="1:9">
@@ -20325,7 +20328,7 @@
         <v>82</v>
       </c>
       <c r="I8">
-        <v>30</v>
+        <v>31</v>
       </c>
     </row>
     <row r="9" spans="1:9">
@@ -20383,7 +20386,7 @@
         <v>369</v>
       </c>
       <c r="I10">
-        <v>118</v>
+        <v>120</v>
       </c>
     </row>
     <row r="11" spans="1:9">
@@ -20412,7 +20415,7 @@
         <v>692</v>
       </c>
       <c r="I11">
-        <v>230</v>
+        <v>234</v>
       </c>
     </row>
   </sheetData>
@@ -20839,7 +20842,7 @@
         <v>93</v>
       </c>
       <c r="I3">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="4" spans="1:9">
@@ -21036,7 +21039,7 @@
         <v>804</v>
       </c>
       <c r="I10">
-        <v>270</v>
+        <v>271</v>
       </c>
     </row>
     <row r="11" spans="1:9">
@@ -21065,7 +21068,7 @@
         <v>1372</v>
       </c>
       <c r="I11">
-        <v>458</v>
+        <v>460</v>
       </c>
     </row>
   </sheetData>
@@ -21905,7 +21908,7 @@
         <v>60</v>
       </c>
       <c r="I5">
-        <v>18</v>
+        <v>19</v>
       </c>
     </row>
     <row r="6" spans="1:9">
@@ -22067,7 +22070,7 @@
         <v>531</v>
       </c>
       <c r="I11">
-        <v>128</v>
+        <v>129</v>
       </c>
     </row>
   </sheetData>
@@ -22323,7 +22326,7 @@
         <v>156</v>
       </c>
       <c r="I8">
-        <v>58</v>
+        <v>59</v>
       </c>
     </row>
     <row r="9" spans="1:9">
@@ -22381,7 +22384,7 @@
         <v>475</v>
       </c>
       <c r="I10">
-        <v>166</v>
+        <v>167</v>
       </c>
     </row>
     <row r="11" spans="1:9">
@@ -22410,7 +22413,7 @@
         <v>1246</v>
       </c>
       <c r="I11">
-        <v>403</v>
+        <v>405</v>
       </c>
     </row>
   </sheetData>
@@ -22686,7 +22689,7 @@
         <v>86</v>
       </c>
       <c r="I9">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="10" spans="1:9">
@@ -22744,7 +22747,7 @@
         <v>944</v>
       </c>
       <c r="I11">
-        <v>308</v>
+        <v>307</v>
       </c>
     </row>
   </sheetData>
@@ -22913,7 +22916,7 @@
         <v>185</v>
       </c>
       <c r="I5">
-        <v>74</v>
+        <v>75</v>
       </c>
     </row>
     <row r="6" spans="1:9">
@@ -22936,7 +22939,7 @@
         <v>47</v>
       </c>
       <c r="G6">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="H6">
         <v>38</v>
@@ -23000,7 +23003,7 @@
         <v>200</v>
       </c>
       <c r="I8">
-        <v>83</v>
+        <v>84</v>
       </c>
     </row>
     <row r="9" spans="1:9">
@@ -23058,7 +23061,7 @@
         <v>605</v>
       </c>
       <c r="I10">
-        <v>245</v>
+        <v>247</v>
       </c>
     </row>
     <row r="11" spans="1:9">
@@ -23081,13 +23084,13 @@
         <v>2076</v>
       </c>
       <c r="G11">
-        <v>1834</v>
+        <v>1835</v>
       </c>
       <c r="H11">
         <v>1676</v>
       </c>
       <c r="I11">
-        <v>608</v>
+        <v>612</v>
       </c>
     </row>
   </sheetData>
@@ -23334,7 +23337,7 @@
         <v>137</v>
       </c>
       <c r="I8">
-        <v>45</v>
+        <v>47</v>
       </c>
     </row>
     <row r="9" spans="1:9">
@@ -23363,7 +23366,7 @@
         <v>136</v>
       </c>
       <c r="I9">
-        <v>33</v>
+        <v>34</v>
       </c>
     </row>
     <row r="10" spans="1:9">
@@ -23392,7 +23395,7 @@
         <v>545</v>
       </c>
       <c r="I10">
-        <v>170</v>
+        <v>171</v>
       </c>
     </row>
     <row r="11" spans="1:9">
@@ -23421,7 +23424,7 @@
         <v>1012</v>
       </c>
       <c r="I11">
-        <v>303</v>
+        <v>307</v>
       </c>
     </row>
   </sheetData>
@@ -23590,7 +23593,7 @@
         <v>53</v>
       </c>
       <c r="I5">
-        <v>17</v>
+        <v>18</v>
       </c>
     </row>
     <row r="6" spans="1:9">
@@ -23761,7 +23764,7 @@
         <v>722</v>
       </c>
       <c r="I11">
-        <v>248</v>
+        <v>249</v>
       </c>
     </row>
   </sheetData>
@@ -24719,7 +24722,7 @@
         <v>366</v>
       </c>
       <c r="I10">
-        <v>147</v>
+        <v>148</v>
       </c>
     </row>
     <row r="11" spans="1:9">
@@ -24748,7 +24751,7 @@
         <v>903</v>
       </c>
       <c r="I11">
-        <v>327</v>
+        <v>328</v>
       </c>
     </row>
   </sheetData>
@@ -24989,7 +24992,7 @@
         <v>46</v>
       </c>
       <c r="I8">
-        <v>14</v>
+        <v>15</v>
       </c>
     </row>
     <row r="9" spans="1:9">
@@ -25076,7 +25079,7 @@
         <v>760</v>
       </c>
       <c r="I11">
-        <v>210</v>
+        <v>211</v>
       </c>
     </row>
   </sheetData>
@@ -25378,7 +25381,7 @@
         <v>248</v>
       </c>
       <c r="I10">
-        <v>101</v>
+        <v>103</v>
       </c>
     </row>
     <row r="11" spans="1:9">
@@ -25407,7 +25410,7 @@
         <v>501</v>
       </c>
       <c r="I11">
-        <v>187</v>
+        <v>189</v>
       </c>
     </row>
   </sheetData>
@@ -25887,7 +25890,7 @@
         <v>6</v>
       </c>
       <c r="I4">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="5" spans="1:9">
@@ -26090,7 +26093,7 @@
         <v>1312</v>
       </c>
       <c r="I11">
-        <v>463</v>
+        <v>464</v>
       </c>
     </row>
   </sheetData>
@@ -26172,7 +26175,7 @@
         <v>67</v>
       </c>
       <c r="I2">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="3" spans="1:9">
@@ -26427,7 +26430,7 @@
         <v>377</v>
       </c>
       <c r="I11">
-        <v>114</v>
+        <v>115</v>
       </c>
     </row>
   </sheetData>
@@ -26696,7 +26699,7 @@
         <v>431</v>
       </c>
       <c r="I10">
-        <v>140</v>
+        <v>141</v>
       </c>
     </row>
     <row r="11" spans="1:9">
@@ -26725,7 +26728,7 @@
         <v>482</v>
       </c>
       <c r="I11">
-        <v>158</v>
+        <v>159</v>
       </c>
     </row>
   </sheetData>
@@ -27294,7 +27297,7 @@
         <v>75</v>
       </c>
       <c r="I8">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="9" spans="1:9">
@@ -27381,7 +27384,7 @@
         <v>767</v>
       </c>
       <c r="I11">
-        <v>235</v>
+        <v>236</v>
       </c>
     </row>
   </sheetData>
@@ -27463,7 +27466,7 @@
         <v>19</v>
       </c>
       <c r="I2">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="3" spans="1:9">
@@ -27674,7 +27677,7 @@
         <v>353</v>
       </c>
       <c r="I10">
-        <v>127</v>
+        <v>128</v>
       </c>
     </row>
     <row r="11" spans="1:9">
@@ -27703,7 +27706,7 @@
         <v>564</v>
       </c>
       <c r="I11">
-        <v>181</v>
+        <v>183</v>
       </c>
     </row>
   </sheetData>
@@ -27785,7 +27788,7 @@
         <v>39</v>
       </c>
       <c r="I2">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="3" spans="1:9">
@@ -28022,7 +28025,7 @@
         <v>841</v>
       </c>
       <c r="I11">
-        <v>282</v>
+        <v>283</v>
       </c>
     </row>
   </sheetData>
@@ -28501,7 +28504,7 @@
         <v>22</v>
       </c>
       <c r="I5">
-        <v>12</v>
+        <v>13</v>
       </c>
     </row>
     <row r="6" spans="1:9">
@@ -28666,7 +28669,7 @@
         <v>303</v>
       </c>
       <c r="I11">
-        <v>139</v>
+        <v>140</v>
       </c>
     </row>
   </sheetData>
@@ -29229,7 +29232,7 @@
         <v>70</v>
       </c>
       <c r="I8">
-        <v>41</v>
+        <v>42</v>
       </c>
     </row>
     <row r="9" spans="1:9">
@@ -29316,7 +29319,7 @@
         <v>565</v>
       </c>
       <c r="I11">
-        <v>201</v>
+        <v>202</v>
       </c>
     </row>
   </sheetData>
@@ -29398,7 +29401,7 @@
         <v>452</v>
       </c>
       <c r="I2">
-        <v>142</v>
+        <v>144</v>
       </c>
     </row>
     <row r="3" spans="1:9">
@@ -29543,7 +29546,7 @@
         <v>69</v>
       </c>
       <c r="I7">
-        <v>15</v>
+        <v>16</v>
       </c>
     </row>
     <row r="8" spans="1:9">
@@ -29572,7 +29575,7 @@
         <v>560</v>
       </c>
       <c r="I8">
-        <v>179</v>
+        <v>180</v>
       </c>
     </row>
     <row r="9" spans="1:9">
@@ -29601,7 +29604,7 @@
         <v>506</v>
       </c>
       <c r="I9">
-        <v>155</v>
+        <v>156</v>
       </c>
     </row>
     <row r="10" spans="1:9">
@@ -29630,7 +29633,7 @@
         <v>1392</v>
       </c>
       <c r="I10">
-        <v>456</v>
+        <v>458</v>
       </c>
     </row>
     <row r="11" spans="1:9">
@@ -29659,7 +29662,7 @@
         <v>3973</v>
       </c>
       <c r="I11">
-        <v>1198</v>
+        <v>1205</v>
       </c>
     </row>
   </sheetData>
@@ -30358,7 +30361,7 @@
         <v>16</v>
       </c>
       <c r="I2">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="3" spans="1:9">
@@ -30572,7 +30575,7 @@
         <v>141</v>
       </c>
       <c r="I10">
-        <v>60</v>
+        <v>61</v>
       </c>
     </row>
   </sheetData>
@@ -30836,7 +30839,7 @@
         <v>109</v>
       </c>
       <c r="I9">
-        <v>32</v>
+        <v>33</v>
       </c>
     </row>
     <row r="10" spans="1:9">
@@ -30894,7 +30897,7 @@
         <v>963</v>
       </c>
       <c r="I11">
-        <v>387</v>
+        <v>388</v>
       </c>
     </row>
   </sheetData>
@@ -31139,7 +31142,7 @@
         <v>321</v>
       </c>
       <c r="I10">
-        <v>21</v>
+        <v>22</v>
       </c>
     </row>
     <row r="11" spans="1:9">
@@ -31168,7 +31171,7 @@
         <v>338</v>
       </c>
       <c r="I11">
-        <v>28</v>
+        <v>29</v>
       </c>
     </row>
   </sheetData>
@@ -31250,7 +31253,7 @@
         <v>4</v>
       </c>
       <c r="I2">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="3" spans="1:9">
@@ -31475,7 +31478,7 @@
         <v>180</v>
       </c>
       <c r="I11">
-        <v>54</v>
+        <v>55</v>
       </c>
     </row>
   </sheetData>
@@ -33063,7 +33066,7 @@
         <v>716</v>
       </c>
       <c r="I10">
-        <v>225</v>
+        <v>227</v>
       </c>
     </row>
     <row r="11" spans="1:9">
@@ -33092,7 +33095,7 @@
         <v>1182</v>
       </c>
       <c r="I11">
-        <v>383</v>
+        <v>385</v>
       </c>
     </row>
   </sheetData>
@@ -33255,7 +33258,7 @@
         <v>10</v>
       </c>
       <c r="I5">
-        <v>15</v>
+        <v>16</v>
       </c>
     </row>
     <row r="6" spans="1:9">
@@ -33414,7 +33417,7 @@
         <v>177</v>
       </c>
       <c r="I11">
-        <v>67</v>
+        <v>68</v>
       </c>
     </row>
   </sheetData>
@@ -33658,7 +33661,7 @@
         <v>98</v>
       </c>
       <c r="I8">
-        <v>47</v>
+        <v>48</v>
       </c>
     </row>
     <row r="9" spans="1:9">
@@ -33687,7 +33690,7 @@
         <v>140</v>
       </c>
       <c r="I9">
-        <v>61</v>
+        <v>62</v>
       </c>
     </row>
   </sheetData>
@@ -33992,7 +33995,7 @@
         <v>136</v>
       </c>
       <c r="I10">
-        <v>65</v>
+        <v>66</v>
       </c>
     </row>
     <row r="11" spans="1:9">
@@ -34021,7 +34024,7 @@
         <v>296</v>
       </c>
       <c r="I11">
-        <v>105</v>
+        <v>106</v>
       </c>
     </row>
   </sheetData>
@@ -34335,7 +34338,7 @@
         <v>329</v>
       </c>
       <c r="I10">
-        <v>136</v>
+        <v>137</v>
       </c>
     </row>
     <row r="11" spans="1:9">
@@ -34364,7 +34367,7 @@
         <v>690</v>
       </c>
       <c r="I11">
-        <v>252</v>
+        <v>253</v>
       </c>
     </row>
   </sheetData>
@@ -35192,7 +35195,7 @@
         <v>88</v>
       </c>
       <c r="I9">
-        <v>33</v>
+        <v>34</v>
       </c>
     </row>
     <row r="10" spans="1:9">
@@ -35221,7 +35224,7 @@
         <v>156</v>
       </c>
       <c r="I10">
-        <v>56</v>
+        <v>57</v>
       </c>
     </row>
   </sheetData>
@@ -35464,7 +35467,7 @@
         <v>77</v>
       </c>
       <c r="I9">
-        <v>15</v>
+        <v>16</v>
       </c>
     </row>
     <row r="10" spans="1:9">
@@ -35493,7 +35496,7 @@
         <v>104</v>
       </c>
       <c r="I10">
-        <v>20</v>
+        <v>21</v>
       </c>
     </row>
   </sheetData>
@@ -35780,7 +35783,7 @@
         <v>128</v>
       </c>
       <c r="I10">
-        <v>52</v>
+        <v>53</v>
       </c>
     </row>
     <row r="11" spans="1:9">
@@ -35809,7 +35812,7 @@
         <v>265</v>
       </c>
       <c r="I11">
-        <v>95</v>
+        <v>96</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add data for 2022-05-18
</commit_message>
<xml_diff>
--- a/output/index-crime-full-year.xlsx
+++ b/output/index-crime-full-year.xlsx
@@ -888,7 +888,7 @@
         <v>7238</v>
       </c>
       <c r="I2">
-        <v>2304</v>
+        <v>2331</v>
       </c>
     </row>
     <row r="3" spans="1:9">
@@ -917,7 +917,7 @@
         <v>8349</v>
       </c>
       <c r="I3">
-        <v>2468</v>
+        <v>2484</v>
       </c>
     </row>
     <row r="4" spans="1:9">
@@ -946,7 +946,7 @@
         <v>526</v>
       </c>
       <c r="I4">
-        <v>135</v>
+        <v>137</v>
       </c>
     </row>
     <row r="5" spans="1:9">
@@ -975,7 +975,7 @@
         <v>6657</v>
       </c>
       <c r="I5">
-        <v>2525</v>
+        <v>2558</v>
       </c>
     </row>
     <row r="6" spans="1:9">
@@ -1004,7 +1004,7 @@
         <v>1661</v>
       </c>
       <c r="I6">
-        <v>600</v>
+        <v>609</v>
       </c>
     </row>
     <row r="7" spans="1:9">
@@ -1030,10 +1030,10 @@
         <v>785</v>
       </c>
       <c r="H7">
-        <v>802</v>
+        <v>801</v>
       </c>
       <c r="I7">
-        <v>218</v>
+        <v>222</v>
       </c>
     </row>
     <row r="8" spans="1:9">
@@ -1062,7 +1062,7 @@
         <v>10580</v>
       </c>
       <c r="I8">
-        <v>4651</v>
+        <v>4687</v>
       </c>
     </row>
     <row r="9" spans="1:9">
@@ -1091,7 +1091,7 @@
         <v>7922</v>
       </c>
       <c r="I9">
-        <v>2846</v>
+        <v>2863</v>
       </c>
     </row>
     <row r="10" spans="1:9">
@@ -1120,7 +1120,7 @@
         <v>40684</v>
       </c>
       <c r="I10">
-        <v>16872</v>
+        <v>17052</v>
       </c>
     </row>
     <row r="11" spans="1:9">
@@ -1146,10 +1146,10 @@
         <v>85227</v>
       </c>
       <c r="H11">
-        <v>84419</v>
+        <v>84418</v>
       </c>
       <c r="I11">
-        <v>32619</v>
+        <v>32943</v>
       </c>
     </row>
   </sheetData>
@@ -1260,7 +1260,7 @@
         <v>270</v>
       </c>
       <c r="I3">
-        <v>85</v>
+        <v>86</v>
       </c>
     </row>
     <row r="4" spans="1:9">
@@ -1463,7 +1463,7 @@
         <v>856</v>
       </c>
       <c r="I10">
-        <v>365</v>
+        <v>368</v>
       </c>
     </row>
     <row r="11" spans="1:9">
@@ -1492,7 +1492,7 @@
         <v>2236</v>
       </c>
       <c r="I11">
-        <v>873</v>
+        <v>877</v>
       </c>
     </row>
   </sheetData>
@@ -1706,7 +1706,7 @@
         <v>12</v>
       </c>
       <c r="I8">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="9" spans="1:9">
@@ -1735,7 +1735,7 @@
         <v>27</v>
       </c>
       <c r="I9">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
   </sheetData>
@@ -1875,7 +1875,7 @@
         <v>6</v>
       </c>
       <c r="I4">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="5" spans="1:9">
@@ -1904,7 +1904,7 @@
         <v>117</v>
       </c>
       <c r="I5">
-        <v>34</v>
+        <v>35</v>
       </c>
     </row>
     <row r="6" spans="1:9">
@@ -1988,7 +1988,7 @@
         <v>113</v>
       </c>
       <c r="I8">
-        <v>68</v>
+        <v>69</v>
       </c>
     </row>
     <row r="9" spans="1:9">
@@ -2075,7 +2075,7 @@
         <v>1149</v>
       </c>
       <c r="I11">
-        <v>476</v>
+        <v>479</v>
       </c>
     </row>
   </sheetData>
@@ -2356,7 +2356,7 @@
         <v>371</v>
       </c>
       <c r="I10">
-        <v>156</v>
+        <v>157</v>
       </c>
     </row>
     <row r="11" spans="1:9">
@@ -2385,7 +2385,7 @@
         <v>500</v>
       </c>
       <c r="I11">
-        <v>213</v>
+        <v>214</v>
       </c>
     </row>
   </sheetData>
@@ -2963,7 +2963,7 @@
         <v>39</v>
       </c>
       <c r="I8">
-        <v>20</v>
+        <v>21</v>
       </c>
     </row>
     <row r="9" spans="1:9">
@@ -3050,7 +3050,7 @@
         <v>200</v>
       </c>
       <c r="I11">
-        <v>104</v>
+        <v>105</v>
       </c>
     </row>
   </sheetData>
@@ -3132,7 +3132,7 @@
         <v>292</v>
       </c>
       <c r="I2">
-        <v>85</v>
+        <v>87</v>
       </c>
     </row>
     <row r="3" spans="1:9">
@@ -3161,7 +3161,7 @@
         <v>336</v>
       </c>
       <c r="I3">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="4" spans="1:9">
@@ -3219,7 +3219,7 @@
         <v>186</v>
       </c>
       <c r="I5">
-        <v>54</v>
+        <v>56</v>
       </c>
     </row>
     <row r="6" spans="1:9">
@@ -3364,7 +3364,7 @@
         <v>692</v>
       </c>
       <c r="I10">
-        <v>257</v>
+        <v>259</v>
       </c>
     </row>
     <row r="11" spans="1:9">
@@ -3393,7 +3393,7 @@
         <v>2162</v>
       </c>
       <c r="I11">
-        <v>727</v>
+        <v>732</v>
       </c>
     </row>
   </sheetData>
@@ -3475,7 +3475,7 @@
         <v>131</v>
       </c>
       <c r="I2">
-        <v>42</v>
+        <v>43</v>
       </c>
     </row>
     <row r="3" spans="1:9">
@@ -3562,7 +3562,7 @@
         <v>93</v>
       </c>
       <c r="I5">
-        <v>36</v>
+        <v>37</v>
       </c>
     </row>
     <row r="6" spans="1:9">
@@ -3707,7 +3707,7 @@
         <v>435</v>
       </c>
       <c r="I10">
-        <v>169</v>
+        <v>172</v>
       </c>
     </row>
     <row r="11" spans="1:9">
@@ -3736,7 +3736,7 @@
         <v>1119</v>
       </c>
       <c r="I11">
-        <v>424</v>
+        <v>429</v>
       </c>
     </row>
   </sheetData>
@@ -3818,7 +3818,7 @@
         <v>279</v>
       </c>
       <c r="I2">
-        <v>74</v>
+        <v>75</v>
       </c>
     </row>
     <row r="3" spans="1:9">
@@ -3905,7 +3905,7 @@
         <v>134</v>
       </c>
       <c r="I5">
-        <v>35</v>
+        <v>36</v>
       </c>
     </row>
     <row r="6" spans="1:9">
@@ -3992,7 +3992,7 @@
         <v>286</v>
       </c>
       <c r="I8">
-        <v>106</v>
+        <v>107</v>
       </c>
     </row>
     <row r="9" spans="1:9">
@@ -4021,7 +4021,7 @@
         <v>301</v>
       </c>
       <c r="I9">
-        <v>112</v>
+        <v>113</v>
       </c>
     </row>
     <row r="10" spans="1:9">
@@ -4050,7 +4050,7 @@
         <v>769</v>
       </c>
       <c r="I10">
-        <v>278</v>
+        <v>280</v>
       </c>
     </row>
     <row r="11" spans="1:9">
@@ -4079,7 +4079,7 @@
         <v>2309</v>
       </c>
       <c r="I11">
-        <v>751</v>
+        <v>757</v>
       </c>
     </row>
   </sheetData>
@@ -4332,7 +4332,7 @@
         <v>89</v>
       </c>
       <c r="I8">
-        <v>43</v>
+        <v>44</v>
       </c>
     </row>
     <row r="9" spans="1:9">
@@ -4390,7 +4390,7 @@
         <v>275</v>
       </c>
       <c r="I10">
-        <v>120</v>
+        <v>122</v>
       </c>
     </row>
     <row r="11" spans="1:9">
@@ -4419,7 +4419,7 @@
         <v>615</v>
       </c>
       <c r="I11">
-        <v>279</v>
+        <v>282</v>
       </c>
     </row>
   </sheetData>
@@ -4501,7 +4501,7 @@
         <v>76</v>
       </c>
       <c r="I2">
-        <v>24</v>
+        <v>25</v>
       </c>
     </row>
     <row r="3" spans="1:9">
@@ -4730,7 +4730,7 @@
         <v>237</v>
       </c>
       <c r="I10">
-        <v>79</v>
+        <v>80</v>
       </c>
     </row>
     <row r="11" spans="1:9">
@@ -4759,7 +4759,7 @@
         <v>587</v>
       </c>
       <c r="I11">
-        <v>190</v>
+        <v>192</v>
       </c>
     </row>
   </sheetData>
@@ -4841,7 +4841,7 @@
         <v>767</v>
       </c>
       <c r="I2">
-        <v>272</v>
+        <v>274</v>
       </c>
     </row>
     <row r="3" spans="1:9">
@@ -4870,7 +4870,7 @@
         <v>123</v>
       </c>
       <c r="I3">
-        <v>34</v>
+        <v>35</v>
       </c>
     </row>
     <row r="4" spans="1:9">
@@ -4928,7 +4928,7 @@
         <v>193</v>
       </c>
       <c r="I5">
-        <v>69</v>
+        <v>70</v>
       </c>
     </row>
     <row r="6" spans="1:9">
@@ -4957,7 +4957,7 @@
         <v>627</v>
       </c>
       <c r="I6">
-        <v>229</v>
+        <v>231</v>
       </c>
     </row>
     <row r="7" spans="1:9">
@@ -4986,7 +4986,7 @@
         <v>2236</v>
       </c>
       <c r="I7">
-        <v>873</v>
+        <v>877</v>
       </c>
     </row>
     <row r="8" spans="1:9">
@@ -5015,7 +5015,7 @@
         <v>3973</v>
       </c>
       <c r="I8">
-        <v>1378</v>
+        <v>1390</v>
       </c>
     </row>
     <row r="9" spans="1:9">
@@ -5073,7 +5073,7 @@
         <v>692</v>
       </c>
       <c r="I10">
-        <v>258</v>
+        <v>263</v>
       </c>
     </row>
     <row r="11" spans="1:9">
@@ -5102,7 +5102,7 @@
         <v>1312</v>
       </c>
       <c r="I11">
-        <v>520</v>
+        <v>522</v>
       </c>
     </row>
     <row r="12" spans="1:9">
@@ -5218,7 +5218,7 @@
         <v>664</v>
       </c>
       <c r="I15">
-        <v>314</v>
+        <v>315</v>
       </c>
     </row>
     <row r="16" spans="1:9">
@@ -5247,7 +5247,7 @@
         <v>435</v>
       </c>
       <c r="I16">
-        <v>188</v>
+        <v>189</v>
       </c>
     </row>
     <row r="17" spans="1:9">
@@ -5276,7 +5276,7 @@
         <v>130</v>
       </c>
       <c r="I17">
-        <v>30</v>
+        <v>31</v>
       </c>
     </row>
     <row r="18" spans="1:9">
@@ -5305,7 +5305,7 @@
         <v>559</v>
       </c>
       <c r="I18">
-        <v>191</v>
+        <v>196</v>
       </c>
     </row>
     <row r="19" spans="1:9">
@@ -5334,7 +5334,7 @@
         <v>1973</v>
       </c>
       <c r="I19">
-        <v>733</v>
+        <v>736</v>
       </c>
     </row>
     <row r="20" spans="1:9">
@@ -5363,7 +5363,7 @@
         <v>1676</v>
       </c>
       <c r="I20">
-        <v>704</v>
+        <v>709</v>
       </c>
     </row>
     <row r="21" spans="1:9">
@@ -5392,7 +5392,7 @@
         <v>293</v>
       </c>
       <c r="I21">
-        <v>128</v>
+        <v>130</v>
       </c>
     </row>
     <row r="22" spans="1:9">
@@ -5421,7 +5421,7 @@
         <v>275</v>
       </c>
       <c r="I22">
-        <v>132</v>
+        <v>134</v>
       </c>
     </row>
     <row r="23" spans="1:9">
@@ -5450,7 +5450,7 @@
         <v>944</v>
       </c>
       <c r="I23">
-        <v>363</v>
+        <v>366</v>
       </c>
     </row>
     <row r="24" spans="1:9">
@@ -5479,7 +5479,7 @@
         <v>531</v>
       </c>
       <c r="I24">
-        <v>138</v>
+        <v>140</v>
       </c>
     </row>
     <row r="25" spans="1:9">
@@ -5508,7 +5508,7 @@
         <v>325</v>
       </c>
       <c r="I25">
-        <v>107</v>
+        <v>109</v>
       </c>
     </row>
     <row r="26" spans="1:9">
@@ -5537,7 +5537,7 @@
         <v>180</v>
       </c>
       <c r="I26">
-        <v>72</v>
+        <v>73</v>
       </c>
     </row>
     <row r="27" spans="1:9">
@@ -5624,7 +5624,7 @@
         <v>3521</v>
       </c>
       <c r="I29">
-        <v>1230</v>
+        <v>1243</v>
       </c>
     </row>
     <row r="30" spans="1:9">
@@ -5653,7 +5653,7 @@
         <v>200</v>
       </c>
       <c r="I30">
-        <v>104</v>
+        <v>105</v>
       </c>
     </row>
     <row r="31" spans="1:9">
@@ -5682,7 +5682,7 @@
         <v>615</v>
       </c>
       <c r="I31">
-        <v>279</v>
+        <v>282</v>
       </c>
     </row>
     <row r="32" spans="1:9">
@@ -5711,7 +5711,7 @@
         <v>170</v>
       </c>
       <c r="I32">
-        <v>61</v>
+        <v>62</v>
       </c>
     </row>
     <row r="33" spans="1:9">
@@ -5740,7 +5740,7 @@
         <v>2688</v>
       </c>
       <c r="I33">
-        <v>900</v>
+        <v>906</v>
       </c>
     </row>
     <row r="34" spans="1:9">
@@ -5769,7 +5769,7 @@
         <v>565</v>
       </c>
       <c r="I34">
-        <v>231</v>
+        <v>235</v>
       </c>
     </row>
     <row r="35" spans="1:9">
@@ -5827,7 +5827,7 @@
         <v>1019</v>
       </c>
       <c r="I36">
-        <v>422</v>
+        <v>427</v>
       </c>
     </row>
     <row r="37" spans="1:9">
@@ -5856,7 +5856,7 @@
         <v>2162</v>
       </c>
       <c r="I37">
-        <v>727</v>
+        <v>732</v>
       </c>
     </row>
     <row r="38" spans="1:9">
@@ -5943,7 +5943,7 @@
         <v>217</v>
       </c>
       <c r="I40">
-        <v>64</v>
+        <v>65</v>
       </c>
     </row>
     <row r="41" spans="1:9">
@@ -5972,7 +5972,7 @@
         <v>351</v>
       </c>
       <c r="I41">
-        <v>133</v>
+        <v>134</v>
       </c>
     </row>
     <row r="42" spans="1:9">
@@ -6001,7 +6001,7 @@
         <v>2425</v>
       </c>
       <c r="I42">
-        <v>804</v>
+        <v>809</v>
       </c>
     </row>
     <row r="43" spans="1:9">
@@ -6030,7 +6030,7 @@
         <v>841</v>
       </c>
       <c r="I43">
-        <v>308</v>
+        <v>312</v>
       </c>
     </row>
     <row r="44" spans="1:9">
@@ -6059,7 +6059,7 @@
         <v>967</v>
       </c>
       <c r="I44">
-        <v>315</v>
+        <v>322</v>
       </c>
     </row>
     <row r="45" spans="1:9">
@@ -6088,7 +6088,7 @@
         <v>141</v>
       </c>
       <c r="I45">
-        <v>65</v>
+        <v>67</v>
       </c>
     </row>
     <row r="46" spans="1:9">
@@ -6117,7 +6117,7 @@
         <v>308</v>
       </c>
       <c r="I46">
-        <v>123</v>
+        <v>125</v>
       </c>
     </row>
     <row r="47" spans="1:9">
@@ -6175,7 +6175,7 @@
         <v>1997</v>
       </c>
       <c r="I48">
-        <v>755</v>
+        <v>765</v>
       </c>
     </row>
     <row r="49" spans="1:9">
@@ -6204,7 +6204,7 @@
         <v>1162</v>
       </c>
       <c r="I49">
-        <v>477</v>
+        <v>483</v>
       </c>
     </row>
     <row r="50" spans="1:9">
@@ -6233,7 +6233,7 @@
         <v>760</v>
       </c>
       <c r="I50">
-        <v>249</v>
+        <v>250</v>
       </c>
     </row>
     <row r="51" spans="1:9">
@@ -6262,7 +6262,7 @@
         <v>1012</v>
       </c>
       <c r="I51">
-        <v>355</v>
+        <v>363</v>
       </c>
     </row>
     <row r="52" spans="1:9">
@@ -6291,7 +6291,7 @@
         <v>1246</v>
       </c>
       <c r="I52">
-        <v>458</v>
+        <v>462</v>
       </c>
     </row>
     <row r="53" spans="1:9">
@@ -6320,7 +6320,7 @@
         <v>1182</v>
       </c>
       <c r="I53">
-        <v>446</v>
+        <v>453</v>
       </c>
     </row>
     <row r="54" spans="1:9">
@@ -6349,7 +6349,7 @@
         <v>2196</v>
       </c>
       <c r="I54">
-        <v>1164</v>
+        <v>1171</v>
       </c>
     </row>
     <row r="55" spans="1:9">
@@ -6378,7 +6378,7 @@
         <v>908</v>
       </c>
       <c r="I55">
-        <v>384</v>
+        <v>386</v>
       </c>
     </row>
     <row r="56" spans="1:9">
@@ -6407,7 +6407,7 @@
         <v>482</v>
       </c>
       <c r="I56">
-        <v>181</v>
+        <v>182</v>
       </c>
     </row>
     <row r="57" spans="1:9">
@@ -6436,7 +6436,7 @@
         <v>296</v>
       </c>
       <c r="I57">
-        <v>123</v>
+        <v>126</v>
       </c>
     </row>
     <row r="58" spans="1:9">
@@ -6494,7 +6494,7 @@
         <v>177</v>
       </c>
       <c r="I59">
-        <v>77</v>
+        <v>78</v>
       </c>
     </row>
     <row r="60" spans="1:9">
@@ -6581,7 +6581,7 @@
         <v>27</v>
       </c>
       <c r="I62">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="63" spans="1:9">
@@ -6610,7 +6610,7 @@
         <v>1961</v>
       </c>
       <c r="I63">
-        <v>674</v>
+        <v>716</v>
       </c>
     </row>
     <row r="64" spans="1:9">
@@ -6639,7 +6639,7 @@
         <v>787</v>
       </c>
       <c r="I64">
-        <v>442</v>
+        <v>443</v>
       </c>
     </row>
     <row r="65" spans="1:9">
@@ -6668,7 +6668,7 @@
         <v>1208</v>
       </c>
       <c r="I65">
-        <v>487</v>
+        <v>492</v>
       </c>
     </row>
     <row r="66" spans="1:9">
@@ -6697,7 +6697,7 @@
         <v>455</v>
       </c>
       <c r="I66">
-        <v>177</v>
+        <v>181</v>
       </c>
     </row>
     <row r="67" spans="1:9">
@@ -6726,7 +6726,7 @@
         <v>2309</v>
       </c>
       <c r="I67">
-        <v>751</v>
+        <v>757</v>
       </c>
     </row>
     <row r="68" spans="1:9">
@@ -6755,7 +6755,7 @@
         <v>293</v>
       </c>
       <c r="I68">
-        <v>141</v>
+        <v>142</v>
       </c>
     </row>
     <row r="69" spans="1:9">
@@ -6784,7 +6784,7 @@
         <v>354</v>
       </c>
       <c r="I69">
-        <v>145</v>
+        <v>147</v>
       </c>
     </row>
     <row r="70" spans="1:9">
@@ -6813,7 +6813,7 @@
         <v>500</v>
       </c>
       <c r="I70">
-        <v>213</v>
+        <v>214</v>
       </c>
     </row>
     <row r="71" spans="1:9">
@@ -6842,7 +6842,7 @@
         <v>220</v>
       </c>
       <c r="I71">
-        <v>83</v>
+        <v>84</v>
       </c>
     </row>
     <row r="72" spans="1:9">
@@ -6871,7 +6871,7 @@
         <v>564</v>
       </c>
       <c r="I72">
-        <v>219</v>
+        <v>221</v>
       </c>
     </row>
     <row r="73" spans="1:9">
@@ -6900,7 +6900,7 @@
         <v>933</v>
       </c>
       <c r="I73">
-        <v>365</v>
+        <v>369</v>
       </c>
     </row>
     <row r="74" spans="1:9">
@@ -6929,7 +6929,7 @@
         <v>198</v>
       </c>
       <c r="I74">
-        <v>136</v>
+        <v>139</v>
       </c>
     </row>
     <row r="75" spans="1:9">
@@ -6987,7 +6987,7 @@
         <v>1998</v>
       </c>
       <c r="I76">
-        <v>961</v>
+        <v>969</v>
       </c>
     </row>
     <row r="77" spans="1:9">
@@ -7045,7 +7045,7 @@
         <v>1372</v>
       </c>
       <c r="I78">
-        <v>528</v>
+        <v>537</v>
       </c>
     </row>
     <row r="79" spans="1:9">
@@ -7074,7 +7074,7 @@
         <v>1893</v>
       </c>
       <c r="I79">
-        <v>671</v>
+        <v>675</v>
       </c>
     </row>
     <row r="80" spans="1:9">
@@ -7103,7 +7103,7 @@
         <v>314</v>
       </c>
       <c r="I80">
-        <v>138</v>
+        <v>139</v>
       </c>
     </row>
     <row r="81" spans="1:9">
@@ -7190,7 +7190,7 @@
         <v>1319</v>
       </c>
       <c r="I83">
-        <v>495</v>
+        <v>502</v>
       </c>
     </row>
     <row r="84" spans="1:9">
@@ -7219,7 +7219,7 @@
         <v>587</v>
       </c>
       <c r="I84">
-        <v>190</v>
+        <v>192</v>
       </c>
     </row>
     <row r="85" spans="1:9">
@@ -7248,7 +7248,7 @@
         <v>2851</v>
       </c>
       <c r="I85">
-        <v>1116</v>
+        <v>1125</v>
       </c>
     </row>
     <row r="86" spans="1:9">
@@ -7277,7 +7277,7 @@
         <v>691</v>
       </c>
       <c r="I86">
-        <v>311</v>
+        <v>314</v>
       </c>
     </row>
     <row r="87" spans="1:9">
@@ -7306,7 +7306,7 @@
         <v>250</v>
       </c>
       <c r="I87">
-        <v>101</v>
+        <v>102</v>
       </c>
     </row>
     <row r="88" spans="1:9">
@@ -7364,7 +7364,7 @@
         <v>1294</v>
       </c>
       <c r="I89">
-        <v>521</v>
+        <v>522</v>
       </c>
     </row>
     <row r="90" spans="1:9">
@@ -7390,10 +7390,10 @@
         <v>960</v>
       </c>
       <c r="H90">
-        <v>903</v>
+        <v>902</v>
       </c>
       <c r="I90">
-        <v>369</v>
+        <v>370</v>
       </c>
     </row>
     <row r="91" spans="1:9">
@@ -7422,7 +7422,7 @@
         <v>722</v>
       </c>
       <c r="I91">
-        <v>286</v>
+        <v>287</v>
       </c>
     </row>
     <row r="92" spans="1:9">
@@ -7451,7 +7451,7 @@
         <v>273</v>
       </c>
       <c r="I92">
-        <v>105</v>
+        <v>106</v>
       </c>
     </row>
     <row r="93" spans="1:9">
@@ -7480,7 +7480,7 @@
         <v>501</v>
       </c>
       <c r="I93">
-        <v>221</v>
+        <v>224</v>
       </c>
     </row>
     <row r="94" spans="1:9">
@@ -7509,7 +7509,7 @@
         <v>1595</v>
       </c>
       <c r="I94">
-        <v>838</v>
+        <v>846</v>
       </c>
     </row>
     <row r="95" spans="1:9">
@@ -7538,7 +7538,7 @@
         <v>1315</v>
       </c>
       <c r="I95">
-        <v>422</v>
+        <v>426</v>
       </c>
     </row>
     <row r="96" spans="1:9">
@@ -7567,7 +7567,7 @@
         <v>1149</v>
       </c>
       <c r="I96">
-        <v>476</v>
+        <v>479</v>
       </c>
     </row>
     <row r="97" spans="1:9">
@@ -7596,7 +7596,7 @@
         <v>1270</v>
       </c>
       <c r="I97">
-        <v>493</v>
+        <v>501</v>
       </c>
     </row>
     <row r="98" spans="1:9">
@@ -7625,7 +7625,7 @@
         <v>963</v>
       </c>
       <c r="I98">
-        <v>426</v>
+        <v>429</v>
       </c>
     </row>
     <row r="99" spans="1:9">
@@ -7654,7 +7654,7 @@
         <v>1119</v>
       </c>
       <c r="I99">
-        <v>424</v>
+        <v>429</v>
       </c>
     </row>
     <row r="100" spans="1:9">
@@ -7683,7 +7683,7 @@
         <v>179</v>
       </c>
       <c r="I100">
-        <v>61</v>
+        <v>63</v>
       </c>
     </row>
     <row r="101" spans="1:9">
@@ -7709,10 +7709,10 @@
         <v>85227</v>
       </c>
       <c r="H101">
-        <v>84419</v>
+        <v>84418</v>
       </c>
       <c r="I101">
-        <v>32619</v>
+        <v>32943</v>
       </c>
     </row>
   </sheetData>
@@ -8012,7 +8012,7 @@
         <v>23</v>
       </c>
       <c r="I6">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="7" spans="1:9">
@@ -8070,7 +8070,7 @@
         <v>146</v>
       </c>
       <c r="I8">
-        <v>62</v>
+        <v>63</v>
       </c>
     </row>
     <row r="9" spans="1:9">
@@ -8128,7 +8128,7 @@
         <v>418</v>
       </c>
       <c r="I10">
-        <v>190</v>
+        <v>193</v>
       </c>
     </row>
     <row r="11" spans="1:9">
@@ -8157,7 +8157,7 @@
         <v>1208</v>
       </c>
       <c r="I11">
-        <v>487</v>
+        <v>492</v>
       </c>
     </row>
   </sheetData>
@@ -8567,7 +8567,7 @@
         <v>179</v>
       </c>
       <c r="I2">
-        <v>57</v>
+        <v>58</v>
       </c>
     </row>
     <row r="3" spans="1:9">
@@ -8741,7 +8741,7 @@
         <v>180</v>
       </c>
       <c r="I8">
-        <v>73</v>
+        <v>75</v>
       </c>
     </row>
     <row r="9" spans="1:9">
@@ -8770,7 +8770,7 @@
         <v>108</v>
       </c>
       <c r="I9">
-        <v>27</v>
+        <v>28</v>
       </c>
     </row>
     <row r="10" spans="1:9">
@@ -8799,7 +8799,7 @@
         <v>465</v>
       </c>
       <c r="I10">
-        <v>208</v>
+        <v>211</v>
       </c>
     </row>
     <row r="11" spans="1:9">
@@ -8828,7 +8828,7 @@
         <v>1319</v>
       </c>
       <c r="I11">
-        <v>495</v>
+        <v>502</v>
       </c>
     </row>
   </sheetData>
@@ -8910,7 +8910,7 @@
         <v>283</v>
       </c>
       <c r="I2">
-        <v>92</v>
+        <v>95</v>
       </c>
     </row>
     <row r="3" spans="1:9">
@@ -8939,7 +8939,7 @@
         <v>532</v>
       </c>
       <c r="I3">
-        <v>134</v>
+        <v>135</v>
       </c>
     </row>
     <row r="4" spans="1:9">
@@ -9055,7 +9055,7 @@
         <v>69</v>
       </c>
       <c r="I7">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="8" spans="1:9">
@@ -9113,7 +9113,7 @@
         <v>356</v>
       </c>
       <c r="I9">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="10" spans="1:9">
@@ -9142,7 +9142,7 @@
         <v>840</v>
       </c>
       <c r="I10">
-        <v>311</v>
+        <v>313</v>
       </c>
     </row>
     <row r="11" spans="1:9">
@@ -9171,7 +9171,7 @@
         <v>2688</v>
       </c>
       <c r="I11">
-        <v>900</v>
+        <v>906</v>
       </c>
     </row>
   </sheetData>
@@ -9340,7 +9340,7 @@
         <v>246</v>
       </c>
       <c r="I5">
-        <v>63</v>
+        <v>66</v>
       </c>
     </row>
     <row r="6" spans="1:9">
@@ -9369,7 +9369,7 @@
         <v>20</v>
       </c>
       <c r="I6">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="7" spans="1:9">
@@ -9514,7 +9514,7 @@
         <v>1315</v>
       </c>
       <c r="I11">
-        <v>422</v>
+        <v>426</v>
       </c>
     </row>
   </sheetData>
@@ -10069,7 +10069,7 @@
         <v>26</v>
       </c>
       <c r="I7">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="8" spans="1:9">
@@ -10156,7 +10156,7 @@
         <v>635</v>
       </c>
       <c r="I10">
-        <v>266</v>
+        <v>269</v>
       </c>
     </row>
     <row r="11" spans="1:9">
@@ -10185,7 +10185,7 @@
         <v>1893</v>
       </c>
       <c r="I11">
-        <v>671</v>
+        <v>675</v>
       </c>
     </row>
   </sheetData>
@@ -10484,7 +10484,7 @@
         <v>91</v>
       </c>
       <c r="I10">
-        <v>35</v>
+        <v>36</v>
       </c>
     </row>
     <row r="11" spans="1:9">
@@ -10513,7 +10513,7 @@
         <v>220</v>
       </c>
       <c r="I11">
-        <v>83</v>
+        <v>84</v>
       </c>
     </row>
   </sheetData>
@@ -10670,7 +10670,7 @@
         <v>33</v>
       </c>
       <c r="I5">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="6" spans="1:9">
@@ -10745,7 +10745,7 @@
         <v>30</v>
       </c>
       <c r="I8">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="9" spans="1:9">
@@ -10832,7 +10832,7 @@
         <v>308</v>
       </c>
       <c r="I11">
-        <v>123</v>
+        <v>125</v>
       </c>
     </row>
   </sheetData>
@@ -11480,7 +11480,7 @@
         <v>791</v>
       </c>
       <c r="I10">
-        <v>330</v>
+        <v>331</v>
       </c>
     </row>
     <row r="11" spans="1:9">
@@ -11509,7 +11509,7 @@
         <v>1294</v>
       </c>
       <c r="I11">
-        <v>521</v>
+        <v>522</v>
       </c>
     </row>
   </sheetData>
@@ -11620,7 +11620,7 @@
         <v>48</v>
       </c>
       <c r="I3">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="4" spans="1:9">
@@ -11843,7 +11843,7 @@
         <v>787</v>
       </c>
       <c r="I11">
-        <v>442</v>
+        <v>443</v>
       </c>
     </row>
   </sheetData>
@@ -12130,7 +12130,7 @@
         <v>116</v>
       </c>
       <c r="I10">
-        <v>34</v>
+        <v>35</v>
       </c>
     </row>
     <row r="11" spans="1:9">
@@ -12159,7 +12159,7 @@
         <v>217</v>
       </c>
       <c r="I11">
-        <v>64</v>
+        <v>65</v>
       </c>
     </row>
   </sheetData>
@@ -12270,7 +12270,7 @@
         <v>43</v>
       </c>
       <c r="I3">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="4" spans="1:9">
@@ -12313,7 +12313,7 @@
         <v>54</v>
       </c>
       <c r="I5">
-        <v>22</v>
+        <v>23</v>
       </c>
     </row>
     <row r="6" spans="1:9">
@@ -12452,7 +12452,7 @@
         <v>1132</v>
       </c>
       <c r="I10">
-        <v>640</v>
+        <v>646</v>
       </c>
     </row>
     <row r="11" spans="1:9">
@@ -12481,7 +12481,7 @@
         <v>1595</v>
       </c>
       <c r="I11">
-        <v>838</v>
+        <v>846</v>
       </c>
     </row>
   </sheetData>
@@ -12592,7 +12592,7 @@
         <v>85</v>
       </c>
       <c r="I3">
-        <v>31</v>
+        <v>32</v>
       </c>
     </row>
     <row r="4" spans="1:9">
@@ -12647,7 +12647,7 @@
         <v>89</v>
       </c>
       <c r="I5">
-        <v>26</v>
+        <v>29</v>
       </c>
     </row>
     <row r="6" spans="1:9">
@@ -12734,7 +12734,7 @@
         <v>241</v>
       </c>
       <c r="I8">
-        <v>109</v>
+        <v>110</v>
       </c>
     </row>
     <row r="9" spans="1:9">
@@ -12792,7 +12792,7 @@
         <v>1314</v>
       </c>
       <c r="I10">
-        <v>696</v>
+        <v>699</v>
       </c>
     </row>
     <row r="11" spans="1:9">
@@ -12821,7 +12821,7 @@
         <v>1998</v>
       </c>
       <c r="I11">
-        <v>961</v>
+        <v>969</v>
       </c>
     </row>
   </sheetData>
@@ -12978,7 +12978,7 @@
         <v>60</v>
       </c>
       <c r="I5">
-        <v>20</v>
+        <v>21</v>
       </c>
     </row>
     <row r="6" spans="1:9">
@@ -13050,7 +13050,7 @@
         <v>33</v>
       </c>
       <c r="I8">
-        <v>20</v>
+        <v>22</v>
       </c>
     </row>
     <row r="9" spans="1:9">
@@ -13108,7 +13108,7 @@
         <v>308</v>
       </c>
       <c r="I10">
-        <v>119</v>
+        <v>120</v>
       </c>
     </row>
     <row r="11" spans="1:9">
@@ -13137,7 +13137,7 @@
         <v>455</v>
       </c>
       <c r="I11">
-        <v>177</v>
+        <v>181</v>
       </c>
     </row>
   </sheetData>
@@ -13433,7 +13433,7 @@
         <v>133</v>
       </c>
       <c r="I10">
-        <v>63</v>
+        <v>64</v>
       </c>
     </row>
     <row r="11" spans="1:9">
@@ -13462,7 +13462,7 @@
         <v>250</v>
       </c>
       <c r="I11">
-        <v>101</v>
+        <v>102</v>
       </c>
     </row>
   </sheetData>
@@ -13694,7 +13694,7 @@
         <v>14</v>
       </c>
       <c r="I8">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="9" spans="1:9">
@@ -13723,7 +13723,7 @@
         <v>112</v>
       </c>
       <c r="I9">
-        <v>39</v>
+        <v>40</v>
       </c>
     </row>
     <row r="10" spans="1:9">
@@ -13752,7 +13752,7 @@
         <v>179</v>
       </c>
       <c r="I10">
-        <v>61</v>
+        <v>63</v>
       </c>
     </row>
   </sheetData>
@@ -13834,7 +13834,7 @@
         <v>35</v>
       </c>
       <c r="I2">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="3" spans="1:9">
@@ -14063,7 +14063,7 @@
         <v>121</v>
       </c>
       <c r="I10">
-        <v>43</v>
+        <v>44</v>
       </c>
     </row>
     <row r="11" spans="1:9">
@@ -14092,7 +14092,7 @@
         <v>325</v>
       </c>
       <c r="I11">
-        <v>107</v>
+        <v>109</v>
       </c>
     </row>
   </sheetData>
@@ -14315,7 +14315,7 @@
         <v>41</v>
       </c>
       <c r="I8">
-        <v>18</v>
+        <v>19</v>
       </c>
     </row>
     <row r="9" spans="1:9">
@@ -14402,7 +14402,7 @@
         <v>435</v>
       </c>
       <c r="I11">
-        <v>188</v>
+        <v>189</v>
       </c>
     </row>
   </sheetData>
@@ -14568,7 +14568,7 @@
         <v>87</v>
       </c>
       <c r="I5">
-        <v>33</v>
+        <v>34</v>
       </c>
     </row>
     <row r="6" spans="1:9">
@@ -14643,7 +14643,7 @@
         <v>171</v>
       </c>
       <c r="I8">
-        <v>84</v>
+        <v>86</v>
       </c>
     </row>
     <row r="9" spans="1:9">
@@ -14701,7 +14701,7 @@
         <v>773</v>
       </c>
       <c r="I10">
-        <v>303</v>
+        <v>306</v>
       </c>
     </row>
     <row r="11" spans="1:9">
@@ -14730,7 +14730,7 @@
         <v>1162</v>
       </c>
       <c r="I11">
-        <v>477</v>
+        <v>483</v>
       </c>
     </row>
   </sheetData>
@@ -14812,7 +14812,7 @@
         <v>353</v>
       </c>
       <c r="I2">
-        <v>97</v>
+        <v>98</v>
       </c>
     </row>
     <row r="3" spans="1:9">
@@ -14841,7 +14841,7 @@
         <v>479</v>
       </c>
       <c r="I3">
-        <v>154</v>
+        <v>156</v>
       </c>
     </row>
     <row r="4" spans="1:9">
@@ -14928,7 +14928,7 @@
         <v>61</v>
       </c>
       <c r="I6">
-        <v>17</v>
+        <v>18</v>
       </c>
     </row>
     <row r="7" spans="1:9">
@@ -14986,7 +14986,7 @@
         <v>349</v>
       </c>
       <c r="I8">
-        <v>171</v>
+        <v>173</v>
       </c>
     </row>
     <row r="9" spans="1:9">
@@ -15044,7 +15044,7 @@
         <v>997</v>
       </c>
       <c r="I10">
-        <v>407</v>
+        <v>410</v>
       </c>
     </row>
     <row r="11" spans="1:9">
@@ -15073,7 +15073,7 @@
         <v>2851</v>
       </c>
       <c r="I11">
-        <v>1116</v>
+        <v>1125</v>
       </c>
     </row>
   </sheetData>
@@ -15184,7 +15184,7 @@
         <v>35</v>
       </c>
       <c r="I3">
-        <v>12</v>
+        <v>13</v>
       </c>
     </row>
     <row r="4" spans="1:9">
@@ -15236,7 +15236,7 @@
         <v>95</v>
       </c>
       <c r="I5">
-        <v>43</v>
+        <v>44</v>
       </c>
     </row>
     <row r="6" spans="1:9">
@@ -15352,7 +15352,7 @@
         <v>122</v>
       </c>
       <c r="I9">
-        <v>37</v>
+        <v>38</v>
       </c>
     </row>
     <row r="10" spans="1:9">
@@ -15381,7 +15381,7 @@
         <v>783</v>
       </c>
       <c r="I10">
-        <v>331</v>
+        <v>336</v>
       </c>
     </row>
     <row r="11" spans="1:9">
@@ -15410,7 +15410,7 @@
         <v>1270</v>
       </c>
       <c r="I11">
-        <v>493</v>
+        <v>501</v>
       </c>
     </row>
   </sheetData>
@@ -15492,7 +15492,7 @@
         <v>83</v>
       </c>
       <c r="I2">
-        <v>32</v>
+        <v>33</v>
       </c>
     </row>
     <row r="3" spans="1:9">
@@ -15724,7 +15724,7 @@
         <v>390</v>
       </c>
       <c r="I10">
-        <v>202</v>
+        <v>203</v>
       </c>
     </row>
     <row r="11" spans="1:9">
@@ -15753,7 +15753,7 @@
         <v>908</v>
       </c>
       <c r="I11">
-        <v>384</v>
+        <v>386</v>
       </c>
     </row>
   </sheetData>
@@ -15835,7 +15835,7 @@
         <v>78</v>
       </c>
       <c r="I2">
-        <v>43</v>
+        <v>44</v>
       </c>
     </row>
     <row r="3" spans="1:9">
@@ -16003,7 +16003,7 @@
         <v>239</v>
       </c>
       <c r="I8">
-        <v>142</v>
+        <v>143</v>
       </c>
     </row>
     <row r="9" spans="1:9">
@@ -16032,7 +16032,7 @@
         <v>205</v>
       </c>
       <c r="I9">
-        <v>93</v>
+        <v>94</v>
       </c>
     </row>
     <row r="10" spans="1:9">
@@ -16061,7 +16061,7 @@
         <v>1457</v>
       </c>
       <c r="I10">
-        <v>800</v>
+        <v>804</v>
       </c>
     </row>
     <row r="11" spans="1:9">
@@ -16090,7 +16090,7 @@
         <v>2196</v>
       </c>
       <c r="I11">
-        <v>1164</v>
+        <v>1171</v>
       </c>
     </row>
   </sheetData>
@@ -16259,7 +16259,7 @@
         <v>92</v>
       </c>
       <c r="I5">
-        <v>29</v>
+        <v>30</v>
       </c>
     </row>
     <row r="6" spans="1:9">
@@ -16401,7 +16401,7 @@
         <v>530</v>
       </c>
       <c r="I10">
-        <v>205</v>
+        <v>208</v>
       </c>
     </row>
     <row r="11" spans="1:9">
@@ -16430,7 +16430,7 @@
         <v>933</v>
       </c>
       <c r="I11">
-        <v>365</v>
+        <v>369</v>
       </c>
     </row>
   </sheetData>
@@ -16512,7 +16512,7 @@
         <v>543</v>
       </c>
       <c r="I2">
-        <v>170</v>
+        <v>171</v>
       </c>
     </row>
     <row r="3" spans="1:9">
@@ -16541,7 +16541,7 @@
         <v>674</v>
       </c>
       <c r="I3">
-        <v>187</v>
+        <v>192</v>
       </c>
     </row>
     <row r="4" spans="1:9">
@@ -16657,7 +16657,7 @@
         <v>54</v>
       </c>
       <c r="I7">
-        <v>17</v>
+        <v>18</v>
       </c>
     </row>
     <row r="8" spans="1:9">
@@ -16686,7 +16686,7 @@
         <v>436</v>
       </c>
       <c r="I8">
-        <v>190</v>
+        <v>191</v>
       </c>
     </row>
     <row r="9" spans="1:9">
@@ -16715,7 +16715,7 @@
         <v>322</v>
       </c>
       <c r="I9">
-        <v>153</v>
+        <v>154</v>
       </c>
     </row>
     <row r="10" spans="1:9">
@@ -16744,7 +16744,7 @@
         <v>1107</v>
       </c>
       <c r="I10">
-        <v>409</v>
+        <v>413</v>
       </c>
     </row>
     <row r="11" spans="1:9">
@@ -16773,7 +16773,7 @@
         <v>3521</v>
       </c>
       <c r="I11">
-        <v>1230</v>
+        <v>1243</v>
       </c>
     </row>
   </sheetData>
@@ -16855,7 +16855,7 @@
         <v>220</v>
       </c>
       <c r="I2">
-        <v>96</v>
+        <v>98</v>
       </c>
     </row>
     <row r="3" spans="1:9">
@@ -17029,7 +17029,7 @@
         <v>284</v>
       </c>
       <c r="I8">
-        <v>138</v>
+        <v>139</v>
       </c>
     </row>
     <row r="9" spans="1:9">
@@ -17116,7 +17116,7 @@
         <v>1973</v>
       </c>
       <c r="I11">
-        <v>733</v>
+        <v>736</v>
       </c>
     </row>
   </sheetData>
@@ -17282,7 +17282,7 @@
         <v>26</v>
       </c>
       <c r="I5">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="6" spans="1:9">
@@ -17415,7 +17415,7 @@
         <v>155</v>
       </c>
       <c r="I10">
-        <v>71</v>
+        <v>72</v>
       </c>
     </row>
     <row r="11" spans="1:9">
@@ -17444,7 +17444,7 @@
         <v>275</v>
       </c>
       <c r="I11">
-        <v>132</v>
+        <v>134</v>
       </c>
     </row>
   </sheetData>
@@ -17555,7 +17555,7 @@
         <v>56</v>
       </c>
       <c r="I3">
-        <v>15</v>
+        <v>16</v>
       </c>
     </row>
     <row r="4" spans="1:9">
@@ -17610,7 +17610,7 @@
         <v>94</v>
       </c>
       <c r="I5">
-        <v>31</v>
+        <v>32</v>
       </c>
     </row>
     <row r="6" spans="1:9">
@@ -17694,7 +17694,7 @@
         <v>101</v>
       </c>
       <c r="I8">
-        <v>44</v>
+        <v>45</v>
       </c>
     </row>
     <row r="9" spans="1:9">
@@ -17752,7 +17752,7 @@
         <v>552</v>
       </c>
       <c r="I10">
-        <v>173</v>
+        <v>177</v>
       </c>
     </row>
     <row r="11" spans="1:9">
@@ -17781,7 +17781,7 @@
         <v>967</v>
       </c>
       <c r="I11">
-        <v>315</v>
+        <v>322</v>
       </c>
     </row>
   </sheetData>
@@ -17950,7 +17950,7 @@
         <v>266</v>
       </c>
       <c r="I5">
-        <v>61</v>
+        <v>63</v>
       </c>
     </row>
     <row r="6" spans="1:9">
@@ -18037,7 +18037,7 @@
         <v>267</v>
       </c>
       <c r="I8">
-        <v>109</v>
+        <v>111</v>
       </c>
     </row>
     <row r="9" spans="1:9">
@@ -18095,7 +18095,7 @@
         <v>955</v>
       </c>
       <c r="I10">
-        <v>340</v>
+        <v>341</v>
       </c>
     </row>
     <row r="11" spans="1:9">
@@ -18124,7 +18124,7 @@
         <v>2425</v>
       </c>
       <c r="I11">
-        <v>804</v>
+        <v>809</v>
       </c>
     </row>
   </sheetData>
@@ -18293,7 +18293,7 @@
         <v>167</v>
       </c>
       <c r="I5">
-        <v>60</v>
+        <v>61</v>
       </c>
     </row>
     <row r="6" spans="1:9">
@@ -18374,7 +18374,7 @@
         <v>191</v>
       </c>
       <c r="I8">
-        <v>84</v>
+        <v>85</v>
       </c>
     </row>
     <row r="9" spans="1:9">
@@ -18432,7 +18432,7 @@
         <v>1303</v>
       </c>
       <c r="I10">
-        <v>518</v>
+        <v>526</v>
       </c>
     </row>
     <row r="11" spans="1:9">
@@ -18461,7 +18461,7 @@
         <v>1997</v>
       </c>
       <c r="I11">
-        <v>755</v>
+        <v>765</v>
       </c>
     </row>
   </sheetData>
@@ -18627,7 +18627,7 @@
         <v>47</v>
       </c>
       <c r="I5">
-        <v>23</v>
+        <v>25</v>
       </c>
     </row>
     <row r="6" spans="1:9">
@@ -18786,7 +18786,7 @@
         <v>354</v>
       </c>
       <c r="I11">
-        <v>145</v>
+        <v>147</v>
       </c>
     </row>
   </sheetData>
@@ -18868,7 +18868,7 @@
         <v>64</v>
       </c>
       <c r="I2">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="3" spans="1:9">
@@ -19091,7 +19091,7 @@
         <v>266</v>
       </c>
       <c r="I10">
-        <v>103</v>
+        <v>104</v>
       </c>
     </row>
     <row r="11" spans="1:9">
@@ -19120,7 +19120,7 @@
         <v>627</v>
       </c>
       <c r="I11">
-        <v>229</v>
+        <v>231</v>
       </c>
     </row>
   </sheetData>
@@ -19425,7 +19425,7 @@
         <v>155</v>
       </c>
       <c r="I10">
-        <v>61</v>
+        <v>62</v>
       </c>
     </row>
     <row r="11" spans="1:9">
@@ -19454,7 +19454,7 @@
         <v>351</v>
       </c>
       <c r="I11">
-        <v>133</v>
+        <v>134</v>
       </c>
     </row>
   </sheetData>
@@ -19536,7 +19536,7 @@
         <v>111</v>
       </c>
       <c r="I2">
-        <v>34</v>
+        <v>35</v>
       </c>
     </row>
     <row r="3" spans="1:9">
@@ -19652,7 +19652,7 @@
         <v>24</v>
       </c>
       <c r="I6">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="7" spans="1:9">
@@ -19739,7 +19739,7 @@
         <v>95</v>
       </c>
       <c r="I9">
-        <v>34</v>
+        <v>36</v>
       </c>
     </row>
     <row r="10" spans="1:9">
@@ -19768,7 +19768,7 @@
         <v>416</v>
       </c>
       <c r="I10">
-        <v>186</v>
+        <v>187</v>
       </c>
     </row>
     <row r="11" spans="1:9">
@@ -19797,7 +19797,7 @@
         <v>1019</v>
       </c>
       <c r="I11">
-        <v>422</v>
+        <v>427</v>
       </c>
     </row>
   </sheetData>
@@ -20337,7 +20337,7 @@
         <v>82</v>
       </c>
       <c r="I8">
-        <v>33</v>
+        <v>34</v>
       </c>
     </row>
     <row r="9" spans="1:9">
@@ -20395,7 +20395,7 @@
         <v>369</v>
       </c>
       <c r="I10">
-        <v>131</v>
+        <v>135</v>
       </c>
     </row>
     <row r="11" spans="1:9">
@@ -20424,7 +20424,7 @@
         <v>692</v>
       </c>
       <c r="I11">
-        <v>258</v>
+        <v>263</v>
       </c>
     </row>
   </sheetData>
@@ -20653,7 +20653,7 @@
         <v>110</v>
       </c>
       <c r="I8">
-        <v>51</v>
+        <v>52</v>
       </c>
     </row>
     <row r="9" spans="1:9">
@@ -20711,7 +20711,7 @@
         <v>414</v>
       </c>
       <c r="I10">
-        <v>202</v>
+        <v>204</v>
       </c>
     </row>
     <row r="11" spans="1:9">
@@ -20740,7 +20740,7 @@
         <v>691</v>
       </c>
       <c r="I11">
-        <v>311</v>
+        <v>314</v>
       </c>
     </row>
   </sheetData>
@@ -20822,7 +20822,7 @@
         <v>69</v>
       </c>
       <c r="I2">
-        <v>21</v>
+        <v>22</v>
       </c>
     </row>
     <row r="3" spans="1:9">
@@ -20906,7 +20906,7 @@
         <v>77</v>
       </c>
       <c r="I5">
-        <v>39</v>
+        <v>40</v>
       </c>
     </row>
     <row r="6" spans="1:9">
@@ -21022,7 +21022,7 @@
         <v>165</v>
       </c>
       <c r="I9">
-        <v>39</v>
+        <v>40</v>
       </c>
     </row>
     <row r="10" spans="1:9">
@@ -21051,7 +21051,7 @@
         <v>804</v>
       </c>
       <c r="I10">
-        <v>316</v>
+        <v>322</v>
       </c>
     </row>
     <row r="11" spans="1:9">
@@ -21080,7 +21080,7 @@
         <v>1372</v>
       </c>
       <c r="I11">
-        <v>528</v>
+        <v>537</v>
       </c>
     </row>
   </sheetData>
@@ -21246,7 +21246,7 @@
         <v>30</v>
       </c>
       <c r="I5">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="6" spans="1:9">
@@ -21411,7 +21411,7 @@
         <v>293</v>
       </c>
       <c r="I11">
-        <v>141</v>
+        <v>142</v>
       </c>
     </row>
   </sheetData>
@@ -21722,7 +21722,7 @@
         <v>259</v>
       </c>
       <c r="I10">
-        <v>128</v>
+        <v>129</v>
       </c>
     </row>
     <row r="11" spans="1:9">
@@ -21751,7 +21751,7 @@
         <v>664</v>
       </c>
       <c r="I11">
-        <v>314</v>
+        <v>315</v>
       </c>
     </row>
   </sheetData>
@@ -22053,7 +22053,7 @@
         <v>306</v>
       </c>
       <c r="I10">
-        <v>76</v>
+        <v>78</v>
       </c>
     </row>
     <row r="11" spans="1:9">
@@ -22082,7 +22082,7 @@
         <v>531</v>
       </c>
       <c r="I11">
-        <v>138</v>
+        <v>140</v>
       </c>
     </row>
   </sheetData>
@@ -22164,7 +22164,7 @@
         <v>142</v>
       </c>
       <c r="I2">
-        <v>42</v>
+        <v>43</v>
       </c>
     </row>
     <row r="3" spans="1:9">
@@ -22367,7 +22367,7 @@
         <v>153</v>
       </c>
       <c r="I9">
-        <v>32</v>
+        <v>33</v>
       </c>
     </row>
     <row r="10" spans="1:9">
@@ -22396,7 +22396,7 @@
         <v>475</v>
       </c>
       <c r="I10">
-        <v>192</v>
+        <v>194</v>
       </c>
     </row>
     <row r="11" spans="1:9">
@@ -22425,7 +22425,7 @@
         <v>1246</v>
       </c>
       <c r="I11">
-        <v>458</v>
+        <v>462</v>
       </c>
     </row>
   </sheetData>
@@ -22730,7 +22730,7 @@
         <v>465</v>
       </c>
       <c r="I10">
-        <v>196</v>
+        <v>199</v>
       </c>
     </row>
     <row r="11" spans="1:9">
@@ -22759,7 +22759,7 @@
         <v>944</v>
       </c>
       <c r="I11">
-        <v>363</v>
+        <v>366</v>
       </c>
     </row>
   </sheetData>
@@ -23073,7 +23073,7 @@
         <v>605</v>
       </c>
       <c r="I10">
-        <v>292</v>
+        <v>297</v>
       </c>
     </row>
     <row r="11" spans="1:9">
@@ -23102,7 +23102,7 @@
         <v>1676</v>
       </c>
       <c r="I11">
-        <v>704</v>
+        <v>709</v>
       </c>
     </row>
   </sheetData>
@@ -23349,7 +23349,7 @@
         <v>137</v>
       </c>
       <c r="I8">
-        <v>55</v>
+        <v>56</v>
       </c>
     </row>
     <row r="9" spans="1:9">
@@ -23407,7 +23407,7 @@
         <v>545</v>
       </c>
       <c r="I10">
-        <v>203</v>
+        <v>210</v>
       </c>
     </row>
     <row r="11" spans="1:9">
@@ -23436,7 +23436,7 @@
         <v>1012</v>
       </c>
       <c r="I11">
-        <v>355</v>
+        <v>363</v>
       </c>
     </row>
   </sheetData>
@@ -23750,7 +23750,7 @@
         <v>243</v>
       </c>
       <c r="I10">
-        <v>120</v>
+        <v>121</v>
       </c>
     </row>
     <row r="11" spans="1:9">
@@ -23779,7 +23779,7 @@
         <v>722</v>
       </c>
       <c r="I11">
-        <v>286</v>
+        <v>287</v>
       </c>
     </row>
   </sheetData>
@@ -24031,7 +24031,7 @@
         <v>77</v>
       </c>
       <c r="I9">
-        <v>42</v>
+        <v>43</v>
       </c>
     </row>
     <row r="10" spans="1:9">
@@ -24060,7 +24060,7 @@
         <v>101</v>
       </c>
       <c r="I10">
-        <v>56</v>
+        <v>57</v>
       </c>
     </row>
     <row r="11" spans="1:9">
@@ -24089,7 +24089,7 @@
         <v>293</v>
       </c>
       <c r="I11">
-        <v>128</v>
+        <v>130</v>
       </c>
     </row>
   </sheetData>
@@ -24647,7 +24647,7 @@
         <v>7</v>
       </c>
       <c r="H7">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="I7">
         <v>5</v>
@@ -24737,7 +24737,7 @@
         <v>366</v>
       </c>
       <c r="I10">
-        <v>167</v>
+        <v>168</v>
       </c>
     </row>
     <row r="11" spans="1:9">
@@ -24763,10 +24763,10 @@
         <v>960</v>
       </c>
       <c r="H11">
-        <v>903</v>
+        <v>902</v>
       </c>
       <c r="I11">
-        <v>369</v>
+        <v>370</v>
       </c>
     </row>
   </sheetData>
@@ -25068,7 +25068,7 @@
         <v>512</v>
       </c>
       <c r="I10">
-        <v>179</v>
+        <v>180</v>
       </c>
     </row>
     <row r="11" spans="1:9">
@@ -25097,7 +25097,7 @@
         <v>760</v>
       </c>
       <c r="I11">
-        <v>249</v>
+        <v>250</v>
       </c>
     </row>
   </sheetData>
@@ -25399,7 +25399,7 @@
         <v>248</v>
       </c>
       <c r="I10">
-        <v>118</v>
+        <v>121</v>
       </c>
     </row>
     <row r="11" spans="1:9">
@@ -25428,7 +25428,7 @@
         <v>501</v>
       </c>
       <c r="I11">
-        <v>221</v>
+        <v>224</v>
       </c>
     </row>
   </sheetData>
@@ -25510,7 +25510,7 @@
         <v>52</v>
       </c>
       <c r="I2">
-        <v>14</v>
+        <v>15</v>
       </c>
     </row>
     <row r="3" spans="1:9">
@@ -25684,7 +25684,7 @@
         <v>102</v>
       </c>
       <c r="I8">
-        <v>44</v>
+        <v>45</v>
       </c>
     </row>
     <row r="9" spans="1:9">
@@ -25713,7 +25713,7 @@
         <v>99</v>
       </c>
       <c r="I9">
-        <v>32</v>
+        <v>33</v>
       </c>
     </row>
     <row r="10" spans="1:9">
@@ -25742,7 +25742,7 @@
         <v>188</v>
       </c>
       <c r="I10">
-        <v>65</v>
+        <v>67</v>
       </c>
     </row>
     <row r="11" spans="1:9">
@@ -25771,7 +25771,7 @@
         <v>559</v>
       </c>
       <c r="I11">
-        <v>191</v>
+        <v>196</v>
       </c>
     </row>
   </sheetData>
@@ -25853,7 +25853,7 @@
         <v>115</v>
       </c>
       <c r="I2">
-        <v>59</v>
+        <v>60</v>
       </c>
     </row>
     <row r="3" spans="1:9">
@@ -26027,7 +26027,7 @@
         <v>194</v>
       </c>
       <c r="I8">
-        <v>64</v>
+        <v>65</v>
       </c>
     </row>
     <row r="9" spans="1:9">
@@ -26114,7 +26114,7 @@
         <v>1312</v>
       </c>
       <c r="I11">
-        <v>520</v>
+        <v>522</v>
       </c>
     </row>
   </sheetData>
@@ -26720,7 +26720,7 @@
         <v>431</v>
       </c>
       <c r="I10">
-        <v>163</v>
+        <v>164</v>
       </c>
     </row>
     <row r="11" spans="1:9">
@@ -26749,7 +26749,7 @@
         <v>482</v>
       </c>
       <c r="I11">
-        <v>181</v>
+        <v>182</v>
       </c>
     </row>
   </sheetData>
@@ -27007,7 +27007,7 @@
         <v>37</v>
       </c>
       <c r="I9">
-        <v>16</v>
+        <v>17</v>
       </c>
     </row>
     <row r="10" spans="1:9">
@@ -27065,7 +27065,7 @@
         <v>193</v>
       </c>
       <c r="I11">
-        <v>69</v>
+        <v>70</v>
       </c>
     </row>
   </sheetData>
@@ -27376,7 +27376,7 @@
         <v>405</v>
       </c>
       <c r="I10">
-        <v>140</v>
+        <v>142</v>
       </c>
     </row>
     <row r="11" spans="1:9">
@@ -27405,7 +27405,7 @@
         <v>767</v>
       </c>
       <c r="I11">
-        <v>272</v>
+        <v>274</v>
       </c>
     </row>
   </sheetData>
@@ -27643,7 +27643,7 @@
         <v>56</v>
       </c>
       <c r="I8">
-        <v>31</v>
+        <v>32</v>
       </c>
     </row>
     <row r="9" spans="1:9">
@@ -27701,7 +27701,7 @@
         <v>353</v>
       </c>
       <c r="I10">
-        <v>146</v>
+        <v>147</v>
       </c>
     </row>
     <row r="11" spans="1:9">
@@ -27730,7 +27730,7 @@
         <v>564</v>
       </c>
       <c r="I11">
-        <v>219</v>
+        <v>221</v>
       </c>
     </row>
   </sheetData>
@@ -27991,7 +27991,7 @@
         <v>96</v>
       </c>
       <c r="I9">
-        <v>41</v>
+        <v>43</v>
       </c>
     </row>
     <row r="10" spans="1:9">
@@ -28020,7 +28020,7 @@
         <v>485</v>
       </c>
       <c r="I10">
-        <v>155</v>
+        <v>157</v>
       </c>
     </row>
     <row r="11" spans="1:9">
@@ -28049,7 +28049,7 @@
         <v>841</v>
       </c>
       <c r="I11">
-        <v>308</v>
+        <v>312</v>
       </c>
     </row>
   </sheetData>
@@ -28336,7 +28336,7 @@
         <v>39</v>
       </c>
       <c r="I10">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="11" spans="1:9">
@@ -28365,7 +28365,7 @@
         <v>130</v>
       </c>
       <c r="I11">
-        <v>30</v>
+        <v>31</v>
       </c>
     </row>
   </sheetData>
@@ -28977,7 +28977,7 @@
         <v>185</v>
       </c>
       <c r="I10">
-        <v>91</v>
+        <v>92</v>
       </c>
     </row>
     <row r="11" spans="1:9">
@@ -29006,7 +29006,7 @@
         <v>314</v>
       </c>
       <c r="I11">
-        <v>138</v>
+        <v>139</v>
       </c>
     </row>
   </sheetData>
@@ -29145,6 +29145,9 @@
       <c r="H4">
         <v>2</v>
       </c>
+      <c r="I4">
+        <v>1</v>
+      </c>
     </row>
     <row r="5" spans="1:9">
       <c r="A5" s="1" t="s">
@@ -29172,7 +29175,7 @@
         <v>41</v>
       </c>
       <c r="I5">
-        <v>20</v>
+        <v>21</v>
       </c>
     </row>
     <row r="6" spans="1:9">
@@ -29314,7 +29317,7 @@
         <v>329</v>
       </c>
       <c r="I10">
-        <v>134</v>
+        <v>136</v>
       </c>
     </row>
     <row r="11" spans="1:9">
@@ -29343,7 +29346,7 @@
         <v>565</v>
       </c>
       <c r="I11">
-        <v>231</v>
+        <v>235</v>
       </c>
     </row>
   </sheetData>
@@ -29425,7 +29428,7 @@
         <v>452</v>
       </c>
       <c r="I2">
-        <v>165</v>
+        <v>169</v>
       </c>
     </row>
     <row r="3" spans="1:9">
@@ -29454,7 +29457,7 @@
         <v>587</v>
       </c>
       <c r="I3">
-        <v>143</v>
+        <v>146</v>
       </c>
     </row>
     <row r="4" spans="1:9">
@@ -29570,7 +29573,7 @@
         <v>69</v>
       </c>
       <c r="I7">
-        <v>17</v>
+        <v>18</v>
       </c>
     </row>
     <row r="8" spans="1:9">
@@ -29628,7 +29631,7 @@
         <v>506</v>
       </c>
       <c r="I9">
-        <v>171</v>
+        <v>173</v>
       </c>
     </row>
     <row r="10" spans="1:9">
@@ -29657,7 +29660,7 @@
         <v>1392</v>
       </c>
       <c r="I10">
-        <v>531</v>
+        <v>533</v>
       </c>
     </row>
     <row r="11" spans="1:9">
@@ -29686,7 +29689,7 @@
         <v>3973</v>
       </c>
       <c r="I11">
-        <v>1378</v>
+        <v>1390</v>
       </c>
     </row>
   </sheetData>
@@ -30274,7 +30277,7 @@
         <v>91</v>
       </c>
       <c r="I10">
-        <v>29</v>
+        <v>30</v>
       </c>
     </row>
     <row r="11" spans="1:9">
@@ -30303,7 +30306,7 @@
         <v>170</v>
       </c>
       <c r="I11">
-        <v>61</v>
+        <v>62</v>
       </c>
     </row>
   </sheetData>
@@ -30512,7 +30515,7 @@
         <v>17</v>
       </c>
       <c r="I7">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="8" spans="1:9">
@@ -30570,7 +30573,7 @@
         <v>80</v>
       </c>
       <c r="I9">
-        <v>43</v>
+        <v>44</v>
       </c>
     </row>
     <row r="10" spans="1:9">
@@ -30599,7 +30602,7 @@
         <v>141</v>
       </c>
       <c r="I10">
-        <v>65</v>
+        <v>67</v>
       </c>
     </row>
   </sheetData>
@@ -30756,7 +30759,7 @@
         <v>85</v>
       </c>
       <c r="I5">
-        <v>27</v>
+        <v>28</v>
       </c>
     </row>
     <row r="6" spans="1:9">
@@ -30892,7 +30895,7 @@
         <v>592</v>
       </c>
       <c r="I10">
-        <v>315</v>
+        <v>317</v>
       </c>
     </row>
     <row r="11" spans="1:9">
@@ -30921,7 +30924,7 @@
         <v>963</v>
       </c>
       <c r="I11">
-        <v>426</v>
+        <v>429</v>
       </c>
     </row>
   </sheetData>
@@ -31349,7 +31352,7 @@
         <v>22</v>
       </c>
       <c r="I5">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="6" spans="1:9">
@@ -31508,7 +31511,7 @@
         <v>180</v>
       </c>
       <c r="I11">
-        <v>72</v>
+        <v>73</v>
       </c>
     </row>
   </sheetData>
@@ -31674,7 +31677,7 @@
         <v>52</v>
       </c>
       <c r="I5">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="6" spans="1:9">
@@ -31845,7 +31848,7 @@
         <v>273</v>
       </c>
       <c r="I11">
-        <v>105</v>
+        <v>106</v>
       </c>
     </row>
   </sheetData>
@@ -33096,7 +33099,7 @@
         <v>716</v>
       </c>
       <c r="I10">
-        <v>263</v>
+        <v>270</v>
       </c>
     </row>
     <row r="11" spans="1:9">
@@ -33125,7 +33128,7 @@
         <v>1182</v>
       </c>
       <c r="I11">
-        <v>446</v>
+        <v>453</v>
       </c>
     </row>
   </sheetData>
@@ -33389,7 +33392,7 @@
         <v>7</v>
       </c>
       <c r="I9">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="10" spans="1:9">
@@ -33447,7 +33450,7 @@
         <v>177</v>
       </c>
       <c r="I11">
-        <v>77</v>
+        <v>78</v>
       </c>
     </row>
   </sheetData>
@@ -33802,7 +33805,7 @@
         <v>30</v>
       </c>
       <c r="I2">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="3" spans="1:9">
@@ -33967,7 +33970,7 @@
         <v>39</v>
       </c>
       <c r="I8">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="9" spans="1:9">
@@ -34025,7 +34028,7 @@
         <v>136</v>
       </c>
       <c r="I10">
-        <v>77</v>
+        <v>78</v>
       </c>
     </row>
     <row r="11" spans="1:9">
@@ -34054,7 +34057,7 @@
         <v>296</v>
       </c>
       <c r="I11">
-        <v>123</v>
+        <v>126</v>
       </c>
     </row>
   </sheetData>
@@ -34542,7 +34545,7 @@
         <v>1</v>
       </c>
       <c r="I5">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="6" spans="1:9">
@@ -34663,7 +34666,7 @@
         <v>158</v>
       </c>
       <c r="I10">
-        <v>102</v>
+        <v>104</v>
       </c>
     </row>
     <row r="11" spans="1:9">
@@ -34692,7 +34695,7 @@
         <v>198</v>
       </c>
       <c r="I11">
-        <v>136</v>
+        <v>139</v>
       </c>
     </row>
   </sheetData>
@@ -34773,6 +34776,9 @@
       <c r="H2">
         <v>9</v>
       </c>
+      <c r="I2">
+        <v>1</v>
+      </c>
     </row>
     <row r="3" spans="1:9">
       <c r="A3" s="1" t="s">
@@ -34967,7 +34973,7 @@
         <v>123</v>
       </c>
       <c r="I10">
-        <v>34</v>
+        <v>35</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add data for 2022-05-19
</commit_message>
<xml_diff>
--- a/output/index-crime-full-year.xlsx
+++ b/output/index-crime-full-year.xlsx
@@ -888,7 +888,7 @@
         <v>7238</v>
       </c>
       <c r="I2">
-        <v>2331</v>
+        <v>2356</v>
       </c>
     </row>
     <row r="3" spans="1:9">
@@ -917,7 +917,7 @@
         <v>8349</v>
       </c>
       <c r="I3">
-        <v>2484</v>
+        <v>2509</v>
       </c>
     </row>
     <row r="4" spans="1:9">
@@ -946,7 +946,7 @@
         <v>526</v>
       </c>
       <c r="I4">
-        <v>137</v>
+        <v>140</v>
       </c>
     </row>
     <row r="5" spans="1:9">
@@ -972,10 +972,10 @@
         <v>8753</v>
       </c>
       <c r="H5">
-        <v>6657</v>
+        <v>6656</v>
       </c>
       <c r="I5">
-        <v>2558</v>
+        <v>2572</v>
       </c>
     </row>
     <row r="6" spans="1:9">
@@ -1001,10 +1001,10 @@
         <v>1428</v>
       </c>
       <c r="H6">
-        <v>1661</v>
+        <v>1662</v>
       </c>
       <c r="I6">
-        <v>609</v>
+        <v>613</v>
       </c>
     </row>
     <row r="7" spans="1:9">
@@ -1033,7 +1033,7 @@
         <v>801</v>
       </c>
       <c r="I7">
-        <v>222</v>
+        <v>225</v>
       </c>
     </row>
     <row r="8" spans="1:9">
@@ -1062,7 +1062,7 @@
         <v>10580</v>
       </c>
       <c r="I8">
-        <v>4687</v>
+        <v>4709</v>
       </c>
     </row>
     <row r="9" spans="1:9">
@@ -1091,7 +1091,7 @@
         <v>7922</v>
       </c>
       <c r="I9">
-        <v>2863</v>
+        <v>2886</v>
       </c>
     </row>
     <row r="10" spans="1:9">
@@ -1117,10 +1117,10 @@
         <v>41281</v>
       </c>
       <c r="H10">
-        <v>40684</v>
+        <v>40689</v>
       </c>
       <c r="I10">
-        <v>17052</v>
+        <v>17218</v>
       </c>
     </row>
     <row r="11" spans="1:9">
@@ -1146,10 +1146,10 @@
         <v>85227</v>
       </c>
       <c r="H11">
-        <v>84418</v>
+        <v>84423</v>
       </c>
       <c r="I11">
-        <v>32943</v>
+        <v>33228</v>
       </c>
     </row>
   </sheetData>
@@ -1231,7 +1231,7 @@
         <v>295</v>
       </c>
       <c r="I2">
-        <v>94</v>
+        <v>96</v>
       </c>
     </row>
     <row r="3" spans="1:9">
@@ -1260,7 +1260,7 @@
         <v>270</v>
       </c>
       <c r="I3">
-        <v>86</v>
+        <v>89</v>
       </c>
     </row>
     <row r="4" spans="1:9">
@@ -1405,7 +1405,7 @@
         <v>332</v>
       </c>
       <c r="I8">
-        <v>124</v>
+        <v>125</v>
       </c>
     </row>
     <row r="9" spans="1:9">
@@ -1434,7 +1434,7 @@
         <v>175</v>
       </c>
       <c r="I9">
-        <v>73</v>
+        <v>75</v>
       </c>
     </row>
     <row r="10" spans="1:9">
@@ -1463,7 +1463,7 @@
         <v>856</v>
       </c>
       <c r="I10">
-        <v>368</v>
+        <v>371</v>
       </c>
     </row>
     <row r="11" spans="1:9">
@@ -1492,7 +1492,7 @@
         <v>2236</v>
       </c>
       <c r="I11">
-        <v>877</v>
+        <v>888</v>
       </c>
     </row>
   </sheetData>
@@ -1904,7 +1904,7 @@
         <v>117</v>
       </c>
       <c r="I5">
-        <v>35</v>
+        <v>36</v>
       </c>
     </row>
     <row r="6" spans="1:9">
@@ -2046,7 +2046,7 @@
         <v>691</v>
       </c>
       <c r="I10">
-        <v>269</v>
+        <v>277</v>
       </c>
     </row>
     <row r="11" spans="1:9">
@@ -2075,7 +2075,7 @@
         <v>1149</v>
       </c>
       <c r="I11">
-        <v>479</v>
+        <v>488</v>
       </c>
     </row>
   </sheetData>
@@ -2327,7 +2327,7 @@
         <v>5</v>
       </c>
       <c r="I9">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="10" spans="1:9">
@@ -2356,7 +2356,7 @@
         <v>371</v>
       </c>
       <c r="I10">
-        <v>157</v>
+        <v>159</v>
       </c>
     </row>
     <row r="11" spans="1:9">
@@ -2385,7 +2385,7 @@
         <v>500</v>
       </c>
       <c r="I11">
-        <v>214</v>
+        <v>217</v>
       </c>
     </row>
   </sheetData>
@@ -2684,7 +2684,7 @@
         <v>224</v>
       </c>
       <c r="I10">
-        <v>115</v>
+        <v>117</v>
       </c>
     </row>
     <row r="11" spans="1:9">
@@ -2713,7 +2713,7 @@
         <v>474</v>
       </c>
       <c r="I11">
-        <v>204</v>
+        <v>206</v>
       </c>
     </row>
   </sheetData>
@@ -2824,7 +2824,7 @@
         <v>32</v>
       </c>
       <c r="I3">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="4" spans="1:9">
@@ -2992,7 +2992,7 @@
         <v>22</v>
       </c>
       <c r="I9">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="10" spans="1:9">
@@ -3050,7 +3050,7 @@
         <v>200</v>
       </c>
       <c r="I11">
-        <v>105</v>
+        <v>107</v>
       </c>
     </row>
   </sheetData>
@@ -3132,7 +3132,7 @@
         <v>292</v>
       </c>
       <c r="I2">
-        <v>87</v>
+        <v>90</v>
       </c>
     </row>
     <row r="3" spans="1:9">
@@ -3161,7 +3161,7 @@
         <v>336</v>
       </c>
       <c r="I3">
-        <v>80</v>
+        <v>82</v>
       </c>
     </row>
     <row r="4" spans="1:9">
@@ -3306,7 +3306,7 @@
         <v>329</v>
       </c>
       <c r="I8">
-        <v>145</v>
+        <v>146</v>
       </c>
     </row>
     <row r="9" spans="1:9">
@@ -3335,7 +3335,7 @@
         <v>243</v>
       </c>
       <c r="I9">
-        <v>74</v>
+        <v>75</v>
       </c>
     </row>
     <row r="10" spans="1:9">
@@ -3364,7 +3364,7 @@
         <v>692</v>
       </c>
       <c r="I10">
-        <v>259</v>
+        <v>264</v>
       </c>
     </row>
     <row r="11" spans="1:9">
@@ -3393,7 +3393,7 @@
         <v>2162</v>
       </c>
       <c r="I11">
-        <v>732</v>
+        <v>744</v>
       </c>
     </row>
   </sheetData>
@@ -3562,7 +3562,7 @@
         <v>93</v>
       </c>
       <c r="I5">
-        <v>37</v>
+        <v>39</v>
       </c>
     </row>
     <row r="6" spans="1:9">
@@ -3678,7 +3678,7 @@
         <v>88</v>
       </c>
       <c r="I9">
-        <v>43</v>
+        <v>45</v>
       </c>
     </row>
     <row r="10" spans="1:9">
@@ -3707,7 +3707,7 @@
         <v>435</v>
       </c>
       <c r="I10">
-        <v>172</v>
+        <v>176</v>
       </c>
     </row>
     <row r="11" spans="1:9">
@@ -3736,7 +3736,7 @@
         <v>1119</v>
       </c>
       <c r="I11">
-        <v>429</v>
+        <v>437</v>
       </c>
     </row>
   </sheetData>
@@ -3818,7 +3818,7 @@
         <v>279</v>
       </c>
       <c r="I2">
-        <v>75</v>
+        <v>76</v>
       </c>
     </row>
     <row r="3" spans="1:9">
@@ -3905,7 +3905,7 @@
         <v>134</v>
       </c>
       <c r="I5">
-        <v>36</v>
+        <v>37</v>
       </c>
     </row>
     <row r="6" spans="1:9">
@@ -3931,10 +3931,10 @@
         <v>49</v>
       </c>
       <c r="H6">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="I6">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="7" spans="1:9">
@@ -4021,7 +4021,7 @@
         <v>301</v>
       </c>
       <c r="I9">
-        <v>113</v>
+        <v>114</v>
       </c>
     </row>
     <row r="10" spans="1:9">
@@ -4050,7 +4050,7 @@
         <v>769</v>
       </c>
       <c r="I10">
-        <v>280</v>
+        <v>285</v>
       </c>
     </row>
     <row r="11" spans="1:9">
@@ -4076,10 +4076,10 @@
         <v>2456</v>
       </c>
       <c r="H11">
-        <v>2309</v>
+        <v>2310</v>
       </c>
       <c r="I11">
-        <v>757</v>
+        <v>764</v>
       </c>
     </row>
   </sheetData>
@@ -4277,7 +4277,7 @@
         <v>13</v>
       </c>
       <c r="I6">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="7" spans="1:9">
@@ -4390,7 +4390,7 @@
         <v>275</v>
       </c>
       <c r="I10">
-        <v>122</v>
+        <v>125</v>
       </c>
     </row>
     <row r="11" spans="1:9">
@@ -4419,7 +4419,7 @@
         <v>615</v>
       </c>
       <c r="I11">
-        <v>282</v>
+        <v>286</v>
       </c>
     </row>
   </sheetData>
@@ -4841,7 +4841,7 @@
         <v>767</v>
       </c>
       <c r="I2">
-        <v>274</v>
+        <v>276</v>
       </c>
     </row>
     <row r="3" spans="1:9">
@@ -4870,7 +4870,7 @@
         <v>123</v>
       </c>
       <c r="I3">
-        <v>35</v>
+        <v>37</v>
       </c>
     </row>
     <row r="4" spans="1:9">
@@ -4899,7 +4899,7 @@
         <v>303</v>
       </c>
       <c r="I4">
-        <v>154</v>
+        <v>155</v>
       </c>
     </row>
     <row r="5" spans="1:9">
@@ -4957,7 +4957,7 @@
         <v>627</v>
       </c>
       <c r="I6">
-        <v>231</v>
+        <v>232</v>
       </c>
     </row>
     <row r="7" spans="1:9">
@@ -4986,7 +4986,7 @@
         <v>2236</v>
       </c>
       <c r="I7">
-        <v>877</v>
+        <v>888</v>
       </c>
     </row>
     <row r="8" spans="1:9">
@@ -5015,7 +5015,7 @@
         <v>3973</v>
       </c>
       <c r="I8">
-        <v>1390</v>
+        <v>1408</v>
       </c>
     </row>
     <row r="9" spans="1:9">
@@ -5044,7 +5044,7 @@
         <v>395</v>
       </c>
       <c r="I9">
-        <v>149</v>
+        <v>153</v>
       </c>
     </row>
     <row r="10" spans="1:9">
@@ -5073,7 +5073,7 @@
         <v>692</v>
       </c>
       <c r="I10">
-        <v>263</v>
+        <v>266</v>
       </c>
     </row>
     <row r="11" spans="1:9">
@@ -5102,7 +5102,7 @@
         <v>1312</v>
       </c>
       <c r="I11">
-        <v>522</v>
+        <v>524</v>
       </c>
     </row>
     <row r="12" spans="1:9">
@@ -5131,7 +5131,7 @@
         <v>265</v>
       </c>
       <c r="I12">
-        <v>108</v>
+        <v>110</v>
       </c>
     </row>
     <row r="13" spans="1:9">
@@ -5189,7 +5189,7 @@
         <v>474</v>
       </c>
       <c r="I14">
-        <v>204</v>
+        <v>206</v>
       </c>
     </row>
     <row r="15" spans="1:9">
@@ -5218,7 +5218,7 @@
         <v>664</v>
       </c>
       <c r="I15">
-        <v>315</v>
+        <v>317</v>
       </c>
     </row>
     <row r="16" spans="1:9">
@@ -5247,7 +5247,7 @@
         <v>435</v>
       </c>
       <c r="I16">
-        <v>189</v>
+        <v>191</v>
       </c>
     </row>
     <row r="17" spans="1:9">
@@ -5276,7 +5276,7 @@
         <v>130</v>
       </c>
       <c r="I17">
-        <v>31</v>
+        <v>32</v>
       </c>
     </row>
     <row r="18" spans="1:9">
@@ -5305,7 +5305,7 @@
         <v>559</v>
       </c>
       <c r="I18">
-        <v>196</v>
+        <v>198</v>
       </c>
     </row>
     <row r="19" spans="1:9">
@@ -5334,7 +5334,7 @@
         <v>1973</v>
       </c>
       <c r="I19">
-        <v>736</v>
+        <v>739</v>
       </c>
     </row>
     <row r="20" spans="1:9">
@@ -5363,7 +5363,7 @@
         <v>1676</v>
       </c>
       <c r="I20">
-        <v>709</v>
+        <v>714</v>
       </c>
     </row>
     <row r="21" spans="1:9">
@@ -5450,7 +5450,7 @@
         <v>944</v>
       </c>
       <c r="I23">
-        <v>366</v>
+        <v>372</v>
       </c>
     </row>
     <row r="24" spans="1:9">
@@ -5479,7 +5479,7 @@
         <v>531</v>
       </c>
       <c r="I24">
-        <v>140</v>
+        <v>142</v>
       </c>
     </row>
     <row r="25" spans="1:9">
@@ -5508,7 +5508,7 @@
         <v>325</v>
       </c>
       <c r="I25">
-        <v>109</v>
+        <v>111</v>
       </c>
     </row>
     <row r="26" spans="1:9">
@@ -5537,7 +5537,7 @@
         <v>180</v>
       </c>
       <c r="I26">
-        <v>73</v>
+        <v>74</v>
       </c>
     </row>
     <row r="27" spans="1:9">
@@ -5566,7 +5566,7 @@
         <v>969</v>
       </c>
       <c r="I27">
-        <v>374</v>
+        <v>377</v>
       </c>
     </row>
     <row r="28" spans="1:9">
@@ -5624,7 +5624,7 @@
         <v>3521</v>
       </c>
       <c r="I29">
-        <v>1243</v>
+        <v>1255</v>
       </c>
     </row>
     <row r="30" spans="1:9">
@@ -5653,7 +5653,7 @@
         <v>200</v>
       </c>
       <c r="I30">
-        <v>105</v>
+        <v>107</v>
       </c>
     </row>
     <row r="31" spans="1:9">
@@ -5682,7 +5682,7 @@
         <v>615</v>
       </c>
       <c r="I31">
-        <v>282</v>
+        <v>286</v>
       </c>
     </row>
     <row r="32" spans="1:9">
@@ -5711,7 +5711,7 @@
         <v>170</v>
       </c>
       <c r="I32">
-        <v>62</v>
+        <v>64</v>
       </c>
     </row>
     <row r="33" spans="1:9">
@@ -5740,7 +5740,7 @@
         <v>2688</v>
       </c>
       <c r="I33">
-        <v>906</v>
+        <v>916</v>
       </c>
     </row>
     <row r="34" spans="1:9">
@@ -5769,7 +5769,7 @@
         <v>565</v>
       </c>
       <c r="I34">
-        <v>235</v>
+        <v>239</v>
       </c>
     </row>
     <row r="35" spans="1:9">
@@ -5798,7 +5798,7 @@
         <v>233</v>
       </c>
       <c r="I35">
-        <v>67</v>
+        <v>68</v>
       </c>
     </row>
     <row r="36" spans="1:9">
@@ -5827,7 +5827,7 @@
         <v>1019</v>
       </c>
       <c r="I36">
-        <v>427</v>
+        <v>430</v>
       </c>
     </row>
     <row r="37" spans="1:9">
@@ -5856,7 +5856,7 @@
         <v>2162</v>
       </c>
       <c r="I37">
-        <v>732</v>
+        <v>744</v>
       </c>
     </row>
     <row r="38" spans="1:9">
@@ -5885,7 +5885,7 @@
         <v>104</v>
       </c>
       <c r="I38">
-        <v>26</v>
+        <v>27</v>
       </c>
     </row>
     <row r="39" spans="1:9">
@@ -5972,7 +5972,7 @@
         <v>351</v>
       </c>
       <c r="I41">
-        <v>134</v>
+        <v>136</v>
       </c>
     </row>
     <row r="42" spans="1:9">
@@ -6001,7 +6001,7 @@
         <v>2425</v>
       </c>
       <c r="I42">
-        <v>809</v>
+        <v>815</v>
       </c>
     </row>
     <row r="43" spans="1:9">
@@ -6030,7 +6030,7 @@
         <v>841</v>
       </c>
       <c r="I43">
-        <v>312</v>
+        <v>317</v>
       </c>
     </row>
     <row r="44" spans="1:9">
@@ -6059,7 +6059,7 @@
         <v>967</v>
       </c>
       <c r="I44">
-        <v>322</v>
+        <v>323</v>
       </c>
     </row>
     <row r="45" spans="1:9">
@@ -6117,7 +6117,7 @@
         <v>308</v>
       </c>
       <c r="I46">
-        <v>125</v>
+        <v>127</v>
       </c>
     </row>
     <row r="47" spans="1:9">
@@ -6146,7 +6146,7 @@
         <v>587</v>
       </c>
       <c r="I47">
-        <v>244</v>
+        <v>245</v>
       </c>
     </row>
     <row r="48" spans="1:9">
@@ -6175,7 +6175,7 @@
         <v>1997</v>
       </c>
       <c r="I48">
-        <v>765</v>
+        <v>774</v>
       </c>
     </row>
     <row r="49" spans="1:9">
@@ -6204,7 +6204,7 @@
         <v>1162</v>
       </c>
       <c r="I49">
-        <v>483</v>
+        <v>488</v>
       </c>
     </row>
     <row r="50" spans="1:9">
@@ -6233,7 +6233,7 @@
         <v>760</v>
       </c>
       <c r="I50">
-        <v>250</v>
+        <v>252</v>
       </c>
     </row>
     <row r="51" spans="1:9">
@@ -6262,7 +6262,7 @@
         <v>1012</v>
       </c>
       <c r="I51">
-        <v>363</v>
+        <v>366</v>
       </c>
     </row>
     <row r="52" spans="1:9">
@@ -6291,7 +6291,7 @@
         <v>1246</v>
       </c>
       <c r="I52">
-        <v>462</v>
+        <v>463</v>
       </c>
     </row>
     <row r="53" spans="1:9">
@@ -6320,7 +6320,7 @@
         <v>1182</v>
       </c>
       <c r="I53">
-        <v>453</v>
+        <v>458</v>
       </c>
     </row>
     <row r="54" spans="1:9">
@@ -6349,7 +6349,7 @@
         <v>2196</v>
       </c>
       <c r="I54">
-        <v>1171</v>
+        <v>1181</v>
       </c>
     </row>
     <row r="55" spans="1:9">
@@ -6378,7 +6378,7 @@
         <v>908</v>
       </c>
       <c r="I55">
-        <v>386</v>
+        <v>395</v>
       </c>
     </row>
     <row r="56" spans="1:9">
@@ -6407,7 +6407,7 @@
         <v>482</v>
       </c>
       <c r="I56">
-        <v>182</v>
+        <v>184</v>
       </c>
     </row>
     <row r="57" spans="1:9">
@@ -6436,7 +6436,7 @@
         <v>296</v>
       </c>
       <c r="I57">
-        <v>126</v>
+        <v>128</v>
       </c>
     </row>
     <row r="58" spans="1:9">
@@ -6523,7 +6523,7 @@
         <v>618</v>
       </c>
       <c r="I60">
-        <v>225</v>
+        <v>228</v>
       </c>
     </row>
     <row r="61" spans="1:9">
@@ -6607,10 +6607,10 @@
         <v>1572</v>
       </c>
       <c r="H63">
-        <v>1961</v>
+        <v>1965</v>
       </c>
       <c r="I63">
-        <v>716</v>
+        <v>659</v>
       </c>
     </row>
     <row r="64" spans="1:9">
@@ -6639,7 +6639,7 @@
         <v>787</v>
       </c>
       <c r="I64">
-        <v>443</v>
+        <v>446</v>
       </c>
     </row>
     <row r="65" spans="1:9">
@@ -6668,7 +6668,7 @@
         <v>1208</v>
       </c>
       <c r="I65">
-        <v>492</v>
+        <v>497</v>
       </c>
     </row>
     <row r="66" spans="1:9">
@@ -6697,7 +6697,7 @@
         <v>455</v>
       </c>
       <c r="I66">
-        <v>181</v>
+        <v>183</v>
       </c>
     </row>
     <row r="67" spans="1:9">
@@ -6723,10 +6723,10 @@
         <v>2456</v>
       </c>
       <c r="H67">
-        <v>2309</v>
+        <v>2310</v>
       </c>
       <c r="I67">
-        <v>757</v>
+        <v>764</v>
       </c>
     </row>
     <row r="68" spans="1:9">
@@ -6755,7 +6755,7 @@
         <v>293</v>
       </c>
       <c r="I68">
-        <v>142</v>
+        <v>143</v>
       </c>
     </row>
     <row r="69" spans="1:9">
@@ -6784,7 +6784,7 @@
         <v>354</v>
       </c>
       <c r="I69">
-        <v>147</v>
+        <v>149</v>
       </c>
     </row>
     <row r="70" spans="1:9">
@@ -6813,7 +6813,7 @@
         <v>500</v>
       </c>
       <c r="I70">
-        <v>214</v>
+        <v>217</v>
       </c>
     </row>
     <row r="71" spans="1:9">
@@ -6900,7 +6900,7 @@
         <v>933</v>
       </c>
       <c r="I73">
-        <v>369</v>
+        <v>372</v>
       </c>
     </row>
     <row r="74" spans="1:9">
@@ -6929,7 +6929,7 @@
         <v>198</v>
       </c>
       <c r="I74">
-        <v>139</v>
+        <v>141</v>
       </c>
     </row>
     <row r="75" spans="1:9">
@@ -6987,7 +6987,7 @@
         <v>1998</v>
       </c>
       <c r="I76">
-        <v>969</v>
+        <v>980</v>
       </c>
     </row>
     <row r="77" spans="1:9">
@@ -7016,7 +7016,7 @@
         <v>377</v>
       </c>
       <c r="I77">
-        <v>125</v>
+        <v>127</v>
       </c>
     </row>
     <row r="78" spans="1:9">
@@ -7045,7 +7045,7 @@
         <v>1372</v>
       </c>
       <c r="I78">
-        <v>537</v>
+        <v>549</v>
       </c>
     </row>
     <row r="79" spans="1:9">
@@ -7074,7 +7074,7 @@
         <v>1893</v>
       </c>
       <c r="I79">
-        <v>675</v>
+        <v>681</v>
       </c>
     </row>
     <row r="80" spans="1:9">
@@ -7103,7 +7103,7 @@
         <v>314</v>
       </c>
       <c r="I80">
-        <v>139</v>
+        <v>141</v>
       </c>
     </row>
     <row r="81" spans="1:9">
@@ -7190,7 +7190,7 @@
         <v>1319</v>
       </c>
       <c r="I83">
-        <v>502</v>
+        <v>503</v>
       </c>
     </row>
     <row r="84" spans="1:9">
@@ -7248,7 +7248,7 @@
         <v>2851</v>
       </c>
       <c r="I85">
-        <v>1125</v>
+        <v>1134</v>
       </c>
     </row>
     <row r="86" spans="1:9">
@@ -7277,7 +7277,7 @@
         <v>691</v>
       </c>
       <c r="I86">
-        <v>314</v>
+        <v>318</v>
       </c>
     </row>
     <row r="87" spans="1:9">
@@ -7306,7 +7306,7 @@
         <v>250</v>
       </c>
       <c r="I87">
-        <v>102</v>
+        <v>104</v>
       </c>
     </row>
     <row r="88" spans="1:9">
@@ -7335,7 +7335,7 @@
         <v>690</v>
       </c>
       <c r="I88">
-        <v>294</v>
+        <v>301</v>
       </c>
     </row>
     <row r="89" spans="1:9">
@@ -7364,7 +7364,7 @@
         <v>1294</v>
       </c>
       <c r="I89">
-        <v>522</v>
+        <v>530</v>
       </c>
     </row>
     <row r="90" spans="1:9">
@@ -7393,7 +7393,7 @@
         <v>902</v>
       </c>
       <c r="I90">
-        <v>370</v>
+        <v>373</v>
       </c>
     </row>
     <row r="91" spans="1:9">
@@ -7422,7 +7422,7 @@
         <v>722</v>
       </c>
       <c r="I91">
-        <v>287</v>
+        <v>291</v>
       </c>
     </row>
     <row r="92" spans="1:9">
@@ -7451,7 +7451,7 @@
         <v>273</v>
       </c>
       <c r="I92">
-        <v>106</v>
+        <v>108</v>
       </c>
     </row>
     <row r="93" spans="1:9">
@@ -7480,7 +7480,7 @@
         <v>501</v>
       </c>
       <c r="I93">
-        <v>224</v>
+        <v>225</v>
       </c>
     </row>
     <row r="94" spans="1:9">
@@ -7509,7 +7509,7 @@
         <v>1595</v>
       </c>
       <c r="I94">
-        <v>846</v>
+        <v>852</v>
       </c>
     </row>
     <row r="95" spans="1:9">
@@ -7538,7 +7538,7 @@
         <v>1315</v>
       </c>
       <c r="I95">
-        <v>426</v>
+        <v>430</v>
       </c>
     </row>
     <row r="96" spans="1:9">
@@ -7567,7 +7567,7 @@
         <v>1149</v>
       </c>
       <c r="I96">
-        <v>479</v>
+        <v>488</v>
       </c>
     </row>
     <row r="97" spans="1:9">
@@ -7596,7 +7596,7 @@
         <v>1270</v>
       </c>
       <c r="I97">
-        <v>501</v>
+        <v>511</v>
       </c>
     </row>
     <row r="98" spans="1:9">
@@ -7625,7 +7625,7 @@
         <v>963</v>
       </c>
       <c r="I98">
-        <v>429</v>
+        <v>435</v>
       </c>
     </row>
     <row r="99" spans="1:9">
@@ -7654,7 +7654,7 @@
         <v>1119</v>
       </c>
       <c r="I99">
-        <v>429</v>
+        <v>437</v>
       </c>
     </row>
     <row r="100" spans="1:9">
@@ -7683,7 +7683,7 @@
         <v>179</v>
       </c>
       <c r="I100">
-        <v>63</v>
+        <v>64</v>
       </c>
     </row>
     <row r="101" spans="1:9">
@@ -7709,10 +7709,10 @@
         <v>85227</v>
       </c>
       <c r="H101">
-        <v>84418</v>
+        <v>84423</v>
       </c>
       <c r="I101">
-        <v>32943</v>
+        <v>33228</v>
       </c>
     </row>
   </sheetData>
@@ -7983,7 +7983,7 @@
         <v>92</v>
       </c>
       <c r="I5">
-        <v>34</v>
+        <v>35</v>
       </c>
     </row>
     <row r="6" spans="1:9">
@@ -8099,7 +8099,7 @@
         <v>113</v>
       </c>
       <c r="I9">
-        <v>65</v>
+        <v>66</v>
       </c>
     </row>
     <row r="10" spans="1:9">
@@ -8128,7 +8128,7 @@
         <v>418</v>
       </c>
       <c r="I10">
-        <v>193</v>
+        <v>196</v>
       </c>
     </row>
     <row r="11" spans="1:9">
@@ -8157,7 +8157,7 @@
         <v>1208</v>
       </c>
       <c r="I11">
-        <v>492</v>
+        <v>497</v>
       </c>
     </row>
   </sheetData>
@@ -8398,7 +8398,7 @@
         <v>76</v>
       </c>
       <c r="I8">
-        <v>50</v>
+        <v>51</v>
       </c>
     </row>
     <row r="9" spans="1:9">
@@ -8456,7 +8456,7 @@
         <v>622</v>
       </c>
       <c r="I10">
-        <v>215</v>
+        <v>217</v>
       </c>
     </row>
     <row r="11" spans="1:9">
@@ -8485,7 +8485,7 @@
         <v>969</v>
       </c>
       <c r="I11">
-        <v>374</v>
+        <v>377</v>
       </c>
     </row>
   </sheetData>
@@ -8596,7 +8596,7 @@
         <v>208</v>
       </c>
       <c r="I3">
-        <v>66</v>
+        <v>67</v>
       </c>
     </row>
     <row r="4" spans="1:9">
@@ -8828,7 +8828,7 @@
         <v>1319</v>
       </c>
       <c r="I11">
-        <v>502</v>
+        <v>503</v>
       </c>
     </row>
   </sheetData>
@@ -8910,7 +8910,7 @@
         <v>283</v>
       </c>
       <c r="I2">
-        <v>95</v>
+        <v>96</v>
       </c>
     </row>
     <row r="3" spans="1:9">
@@ -8939,7 +8939,7 @@
         <v>532</v>
       </c>
       <c r="I3">
-        <v>135</v>
+        <v>137</v>
       </c>
     </row>
     <row r="4" spans="1:9">
@@ -8997,7 +8997,7 @@
         <v>147</v>
       </c>
       <c r="I5">
-        <v>61</v>
+        <v>62</v>
       </c>
     </row>
     <row r="6" spans="1:9">
@@ -9084,7 +9084,7 @@
         <v>369</v>
       </c>
       <c r="I8">
-        <v>137</v>
+        <v>138</v>
       </c>
     </row>
     <row r="9" spans="1:9">
@@ -9113,7 +9113,7 @@
         <v>356</v>
       </c>
       <c r="I9">
-        <v>130</v>
+        <v>131</v>
       </c>
     </row>
     <row r="10" spans="1:9">
@@ -9142,7 +9142,7 @@
         <v>840</v>
       </c>
       <c r="I10">
-        <v>313</v>
+        <v>317</v>
       </c>
     </row>
     <row r="11" spans="1:9">
@@ -9171,7 +9171,7 @@
         <v>2688</v>
       </c>
       <c r="I11">
-        <v>906</v>
+        <v>916</v>
       </c>
     </row>
   </sheetData>
@@ -9398,7 +9398,7 @@
         <v>37</v>
       </c>
       <c r="I7">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="8" spans="1:9">
@@ -9485,7 +9485,7 @@
         <v>387</v>
       </c>
       <c r="I10">
-        <v>151</v>
+        <v>154</v>
       </c>
     </row>
     <row r="11" spans="1:9">
@@ -9514,7 +9514,7 @@
         <v>1315</v>
       </c>
       <c r="I11">
-        <v>426</v>
+        <v>430</v>
       </c>
     </row>
   </sheetData>
@@ -9924,7 +9924,7 @@
         <v>231</v>
       </c>
       <c r="I2">
-        <v>61</v>
+        <v>62</v>
       </c>
     </row>
     <row r="3" spans="1:9">
@@ -9982,7 +9982,7 @@
         <v>11</v>
       </c>
       <c r="I4">
-        <v>3</v>
+        <v>5</v>
       </c>
     </row>
     <row r="5" spans="1:9">
@@ -10156,7 +10156,7 @@
         <v>635</v>
       </c>
       <c r="I10">
-        <v>269</v>
+        <v>272</v>
       </c>
     </row>
     <row r="11" spans="1:9">
@@ -10185,7 +10185,7 @@
         <v>1893</v>
       </c>
       <c r="I11">
-        <v>675</v>
+        <v>681</v>
       </c>
     </row>
   </sheetData>
@@ -10803,7 +10803,7 @@
         <v>179</v>
       </c>
       <c r="I10">
-        <v>81</v>
+        <v>83</v>
       </c>
     </row>
     <row r="11" spans="1:9">
@@ -10832,7 +10832,7 @@
         <v>308</v>
       </c>
       <c r="I11">
-        <v>125</v>
+        <v>127</v>
       </c>
     </row>
   </sheetData>
@@ -11140,7 +11140,7 @@
         <v>341</v>
       </c>
       <c r="I10">
-        <v>130</v>
+        <v>133</v>
       </c>
     </row>
     <row r="11" spans="1:9">
@@ -11169,7 +11169,7 @@
         <v>618</v>
       </c>
       <c r="I11">
-        <v>225</v>
+        <v>228</v>
       </c>
     </row>
   </sheetData>
@@ -11280,7 +11280,7 @@
         <v>75</v>
       </c>
       <c r="I3">
-        <v>18</v>
+        <v>19</v>
       </c>
     </row>
     <row r="4" spans="1:9">
@@ -11338,7 +11338,7 @@
         <v>95</v>
       </c>
       <c r="I5">
-        <v>55</v>
+        <v>56</v>
       </c>
     </row>
     <row r="6" spans="1:9">
@@ -11367,7 +11367,7 @@
         <v>36</v>
       </c>
       <c r="I6">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="7" spans="1:9">
@@ -11480,7 +11480,7 @@
         <v>791</v>
       </c>
       <c r="I10">
-        <v>331</v>
+        <v>336</v>
       </c>
     </row>
     <row r="11" spans="1:9">
@@ -11509,7 +11509,7 @@
         <v>1294</v>
       </c>
       <c r="I11">
-        <v>522</v>
+        <v>530</v>
       </c>
     </row>
   </sheetData>
@@ -11591,7 +11591,7 @@
         <v>38</v>
       </c>
       <c r="I2">
-        <v>18</v>
+        <v>19</v>
       </c>
     </row>
     <row r="3" spans="1:9">
@@ -11814,7 +11814,7 @@
         <v>375</v>
       </c>
       <c r="I10">
-        <v>203</v>
+        <v>205</v>
       </c>
     </row>
     <row r="11" spans="1:9">
@@ -11843,7 +11843,7 @@
         <v>787</v>
       </c>
       <c r="I11">
-        <v>443</v>
+        <v>446</v>
       </c>
     </row>
   </sheetData>
@@ -12241,7 +12241,7 @@
         <v>36</v>
       </c>
       <c r="I2">
-        <v>15</v>
+        <v>16</v>
       </c>
     </row>
     <row r="3" spans="1:9">
@@ -12452,7 +12452,7 @@
         <v>1132</v>
       </c>
       <c r="I10">
-        <v>646</v>
+        <v>651</v>
       </c>
     </row>
     <row r="11" spans="1:9">
@@ -12481,7 +12481,7 @@
         <v>1595</v>
       </c>
       <c r="I11">
-        <v>846</v>
+        <v>852</v>
       </c>
     </row>
   </sheetData>
@@ -12592,7 +12592,7 @@
         <v>85</v>
       </c>
       <c r="I3">
-        <v>32</v>
+        <v>33</v>
       </c>
     </row>
     <row r="4" spans="1:9">
@@ -12792,7 +12792,7 @@
         <v>1314</v>
       </c>
       <c r="I10">
-        <v>699</v>
+        <v>709</v>
       </c>
     </row>
     <row r="11" spans="1:9">
@@ -12821,7 +12821,7 @@
         <v>1998</v>
       </c>
       <c r="I11">
-        <v>969</v>
+        <v>980</v>
       </c>
     </row>
   </sheetData>
@@ -13108,7 +13108,7 @@
         <v>308</v>
       </c>
       <c r="I10">
-        <v>120</v>
+        <v>122</v>
       </c>
     </row>
     <row r="11" spans="1:9">
@@ -13137,7 +13137,7 @@
         <v>455</v>
       </c>
       <c r="I11">
-        <v>181</v>
+        <v>183</v>
       </c>
     </row>
   </sheetData>
@@ -13219,7 +13219,7 @@
         <v>17</v>
       </c>
       <c r="I2">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="3" spans="1:9">
@@ -13433,7 +13433,7 @@
         <v>133</v>
       </c>
       <c r="I10">
-        <v>64</v>
+        <v>65</v>
       </c>
     </row>
     <row r="11" spans="1:9">
@@ -13462,7 +13462,7 @@
         <v>250</v>
       </c>
       <c r="I11">
-        <v>102</v>
+        <v>104</v>
       </c>
     </row>
   </sheetData>
@@ -13723,7 +13723,7 @@
         <v>112</v>
       </c>
       <c r="I9">
-        <v>40</v>
+        <v>41</v>
       </c>
     </row>
     <row r="10" spans="1:9">
@@ -13752,7 +13752,7 @@
         <v>179</v>
       </c>
       <c r="I10">
-        <v>63</v>
+        <v>64</v>
       </c>
     </row>
   </sheetData>
@@ -14063,7 +14063,7 @@
         <v>121</v>
       </c>
       <c r="I10">
-        <v>44</v>
+        <v>46</v>
       </c>
     </row>
     <row r="11" spans="1:9">
@@ -14092,7 +14092,7 @@
         <v>325</v>
       </c>
       <c r="I11">
-        <v>109</v>
+        <v>111</v>
       </c>
     </row>
   </sheetData>
@@ -14315,7 +14315,7 @@
         <v>41</v>
       </c>
       <c r="I8">
-        <v>19</v>
+        <v>20</v>
       </c>
     </row>
     <row r="9" spans="1:9">
@@ -14373,7 +14373,7 @@
         <v>276</v>
       </c>
       <c r="I10">
-        <v>121</v>
+        <v>122</v>
       </c>
     </row>
     <row r="11" spans="1:9">
@@ -14402,7 +14402,7 @@
         <v>435</v>
       </c>
       <c r="I11">
-        <v>189</v>
+        <v>191</v>
       </c>
     </row>
   </sheetData>
@@ -14484,7 +14484,7 @@
         <v>21</v>
       </c>
       <c r="I2">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="3" spans="1:9">
@@ -14643,7 +14643,7 @@
         <v>171</v>
       </c>
       <c r="I8">
-        <v>86</v>
+        <v>87</v>
       </c>
     </row>
     <row r="9" spans="1:9">
@@ -14701,7 +14701,7 @@
         <v>773</v>
       </c>
       <c r="I10">
-        <v>306</v>
+        <v>309</v>
       </c>
     </row>
     <row r="11" spans="1:9">
@@ -14730,7 +14730,7 @@
         <v>1162</v>
       </c>
       <c r="I11">
-        <v>483</v>
+        <v>488</v>
       </c>
     </row>
   </sheetData>
@@ -14841,7 +14841,7 @@
         <v>479</v>
       </c>
       <c r="I3">
-        <v>156</v>
+        <v>158</v>
       </c>
     </row>
     <row r="4" spans="1:9">
@@ -14899,7 +14899,7 @@
         <v>262</v>
       </c>
       <c r="I5">
-        <v>141</v>
+        <v>142</v>
       </c>
     </row>
     <row r="6" spans="1:9">
@@ -14986,7 +14986,7 @@
         <v>349</v>
       </c>
       <c r="I8">
-        <v>173</v>
+        <v>176</v>
       </c>
     </row>
     <row r="9" spans="1:9">
@@ -15044,7 +15044,7 @@
         <v>997</v>
       </c>
       <c r="I10">
-        <v>410</v>
+        <v>413</v>
       </c>
     </row>
     <row r="11" spans="1:9">
@@ -15073,7 +15073,7 @@
         <v>2851</v>
       </c>
       <c r="I11">
-        <v>1125</v>
+        <v>1134</v>
       </c>
     </row>
   </sheetData>
@@ -15323,7 +15323,7 @@
         <v>178</v>
       </c>
       <c r="I8">
-        <v>55</v>
+        <v>56</v>
       </c>
     </row>
     <row r="9" spans="1:9">
@@ -15381,7 +15381,7 @@
         <v>783</v>
       </c>
       <c r="I10">
-        <v>336</v>
+        <v>345</v>
       </c>
     </row>
     <row r="11" spans="1:9">
@@ -15410,7 +15410,7 @@
         <v>1270</v>
       </c>
       <c r="I11">
-        <v>501</v>
+        <v>511</v>
       </c>
     </row>
   </sheetData>
@@ -15521,7 +15521,7 @@
         <v>92</v>
       </c>
       <c r="I3">
-        <v>24</v>
+        <v>25</v>
       </c>
     </row>
     <row r="4" spans="1:9">
@@ -15666,7 +15666,7 @@
         <v>121</v>
       </c>
       <c r="I8">
-        <v>53</v>
+        <v>54</v>
       </c>
     </row>
     <row r="9" spans="1:9">
@@ -15724,7 +15724,7 @@
         <v>390</v>
       </c>
       <c r="I10">
-        <v>203</v>
+        <v>210</v>
       </c>
     </row>
     <row r="11" spans="1:9">
@@ -15753,7 +15753,7 @@
         <v>908</v>
       </c>
       <c r="I11">
-        <v>386</v>
+        <v>395</v>
       </c>
     </row>
   </sheetData>
@@ -15919,7 +15919,7 @@
         <v>239</v>
       </c>
       <c r="H5">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="I5">
         <v>31</v>
@@ -16003,7 +16003,7 @@
         <v>239</v>
       </c>
       <c r="I8">
-        <v>143</v>
+        <v>144</v>
       </c>
     </row>
     <row r="9" spans="1:9">
@@ -16032,7 +16032,7 @@
         <v>205</v>
       </c>
       <c r="I9">
-        <v>94</v>
+        <v>95</v>
       </c>
     </row>
     <row r="10" spans="1:9">
@@ -16058,10 +16058,10 @@
         <v>1579</v>
       </c>
       <c r="H10">
-        <v>1457</v>
+        <v>1458</v>
       </c>
       <c r="I10">
-        <v>804</v>
+        <v>812</v>
       </c>
     </row>
     <row r="11" spans="1:9">
@@ -16090,7 +16090,7 @@
         <v>2196</v>
       </c>
       <c r="I11">
-        <v>1171</v>
+        <v>1181</v>
       </c>
     </row>
   </sheetData>
@@ -16288,7 +16288,7 @@
         <v>12</v>
       </c>
       <c r="I6">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="7" spans="1:9">
@@ -16372,7 +16372,7 @@
         <v>55</v>
       </c>
       <c r="I9">
-        <v>20</v>
+        <v>21</v>
       </c>
     </row>
     <row r="10" spans="1:9">
@@ -16401,7 +16401,7 @@
         <v>530</v>
       </c>
       <c r="I10">
-        <v>208</v>
+        <v>209</v>
       </c>
     </row>
     <row r="11" spans="1:9">
@@ -16430,7 +16430,7 @@
         <v>933</v>
       </c>
       <c r="I11">
-        <v>369</v>
+        <v>372</v>
       </c>
     </row>
   </sheetData>
@@ -16512,7 +16512,7 @@
         <v>543</v>
       </c>
       <c r="I2">
-        <v>171</v>
+        <v>175</v>
       </c>
     </row>
     <row r="3" spans="1:9">
@@ -16599,7 +16599,7 @@
         <v>272</v>
       </c>
       <c r="I5">
-        <v>76</v>
+        <v>77</v>
       </c>
     </row>
     <row r="6" spans="1:9">
@@ -16628,7 +16628,7 @@
         <v>69</v>
       </c>
       <c r="I6">
-        <v>17</v>
+        <v>18</v>
       </c>
     </row>
     <row r="7" spans="1:9">
@@ -16686,7 +16686,7 @@
         <v>436</v>
       </c>
       <c r="I8">
-        <v>191</v>
+        <v>193</v>
       </c>
     </row>
     <row r="9" spans="1:9">
@@ -16744,7 +16744,7 @@
         <v>1107</v>
       </c>
       <c r="I10">
-        <v>413</v>
+        <v>417</v>
       </c>
     </row>
     <row r="11" spans="1:9">
@@ -16773,7 +16773,7 @@
         <v>3521</v>
       </c>
       <c r="I11">
-        <v>1243</v>
+        <v>1255</v>
       </c>
     </row>
   </sheetData>
@@ -16855,7 +16855,7 @@
         <v>220</v>
       </c>
       <c r="I2">
-        <v>98</v>
+        <v>99</v>
       </c>
     </row>
     <row r="3" spans="1:9">
@@ -17029,7 +17029,7 @@
         <v>284</v>
       </c>
       <c r="I8">
-        <v>139</v>
+        <v>140</v>
       </c>
     </row>
     <row r="9" spans="1:9">
@@ -17087,7 +17087,7 @@
         <v>782</v>
       </c>
       <c r="I10">
-        <v>285</v>
+        <v>286</v>
       </c>
     </row>
     <row r="11" spans="1:9">
@@ -17116,7 +17116,7 @@
         <v>1973</v>
       </c>
       <c r="I11">
-        <v>736</v>
+        <v>739</v>
       </c>
     </row>
   </sheetData>
@@ -17752,7 +17752,7 @@
         <v>552</v>
       </c>
       <c r="I10">
-        <v>177</v>
+        <v>178</v>
       </c>
     </row>
     <row r="11" spans="1:9">
@@ -17781,7 +17781,7 @@
         <v>967</v>
       </c>
       <c r="I11">
-        <v>322</v>
+        <v>323</v>
       </c>
     </row>
   </sheetData>
@@ -17892,7 +17892,7 @@
         <v>293</v>
       </c>
       <c r="I3">
-        <v>102</v>
+        <v>104</v>
       </c>
     </row>
     <row r="4" spans="1:9">
@@ -18037,7 +18037,7 @@
         <v>267</v>
       </c>
       <c r="I8">
-        <v>111</v>
+        <v>112</v>
       </c>
     </row>
     <row r="9" spans="1:9">
@@ -18095,7 +18095,7 @@
         <v>955</v>
       </c>
       <c r="I10">
-        <v>341</v>
+        <v>344</v>
       </c>
     </row>
     <row r="11" spans="1:9">
@@ -18124,7 +18124,7 @@
         <v>2425</v>
       </c>
       <c r="I11">
-        <v>809</v>
+        <v>815</v>
       </c>
     </row>
   </sheetData>
@@ -18374,7 +18374,7 @@
         <v>191</v>
       </c>
       <c r="I8">
-        <v>85</v>
+        <v>89</v>
       </c>
     </row>
     <row r="9" spans="1:9">
@@ -18403,7 +18403,7 @@
         <v>182</v>
       </c>
       <c r="I9">
-        <v>53</v>
+        <v>54</v>
       </c>
     </row>
     <row r="10" spans="1:9">
@@ -18432,7 +18432,7 @@
         <v>1303</v>
       </c>
       <c r="I10">
-        <v>526</v>
+        <v>530</v>
       </c>
     </row>
     <row r="11" spans="1:9">
@@ -18461,7 +18461,7 @@
         <v>1997</v>
       </c>
       <c r="I11">
-        <v>765</v>
+        <v>774</v>
       </c>
     </row>
   </sheetData>
@@ -18757,7 +18757,7 @@
         <v>221</v>
       </c>
       <c r="I10">
-        <v>86</v>
+        <v>88</v>
       </c>
     </row>
     <row r="11" spans="1:9">
@@ -18786,7 +18786,7 @@
         <v>354</v>
       </c>
       <c r="I11">
-        <v>147</v>
+        <v>149</v>
       </c>
     </row>
   </sheetData>
@@ -18897,7 +18897,7 @@
         <v>45</v>
       </c>
       <c r="I3">
-        <v>19</v>
+        <v>20</v>
       </c>
     </row>
     <row r="4" spans="1:9">
@@ -19120,7 +19120,7 @@
         <v>627</v>
       </c>
       <c r="I11">
-        <v>231</v>
+        <v>232</v>
       </c>
     </row>
   </sheetData>
@@ -19396,7 +19396,7 @@
         <v>39</v>
       </c>
       <c r="I9">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="10" spans="1:9">
@@ -19425,7 +19425,7 @@
         <v>155</v>
       </c>
       <c r="I10">
-        <v>62</v>
+        <v>63</v>
       </c>
     </row>
     <row r="11" spans="1:9">
@@ -19454,7 +19454,7 @@
         <v>351</v>
       </c>
       <c r="I11">
-        <v>134</v>
+        <v>136</v>
       </c>
     </row>
   </sheetData>
@@ -19768,7 +19768,7 @@
         <v>416</v>
       </c>
       <c r="I10">
-        <v>187</v>
+        <v>190</v>
       </c>
     </row>
     <row r="11" spans="1:9">
@@ -19797,7 +19797,7 @@
         <v>1019</v>
       </c>
       <c r="I11">
-        <v>427</v>
+        <v>430</v>
       </c>
     </row>
   </sheetData>
@@ -20395,7 +20395,7 @@
         <v>369</v>
       </c>
       <c r="I10">
-        <v>135</v>
+        <v>138</v>
       </c>
     </row>
     <row r="11" spans="1:9">
@@ -20424,7 +20424,7 @@
         <v>692</v>
       </c>
       <c r="I11">
-        <v>263</v>
+        <v>266</v>
       </c>
     </row>
   </sheetData>
@@ -20711,7 +20711,7 @@
         <v>414</v>
       </c>
       <c r="I10">
-        <v>204</v>
+        <v>208</v>
       </c>
     </row>
     <row r="11" spans="1:9">
@@ -20740,7 +20740,7 @@
         <v>691</v>
       </c>
       <c r="I11">
-        <v>314</v>
+        <v>318</v>
       </c>
     </row>
   </sheetData>
@@ -20822,7 +20822,7 @@
         <v>69</v>
       </c>
       <c r="I2">
-        <v>22</v>
+        <v>23</v>
       </c>
     </row>
     <row r="3" spans="1:9">
@@ -20906,7 +20906,7 @@
         <v>77</v>
       </c>
       <c r="I5">
-        <v>40</v>
+        <v>41</v>
       </c>
     </row>
     <row r="6" spans="1:9">
@@ -21022,7 +21022,7 @@
         <v>165</v>
       </c>
       <c r="I9">
-        <v>40</v>
+        <v>41</v>
       </c>
     </row>
     <row r="10" spans="1:9">
@@ -21051,7 +21051,7 @@
         <v>804</v>
       </c>
       <c r="I10">
-        <v>322</v>
+        <v>331</v>
       </c>
     </row>
     <row r="11" spans="1:9">
@@ -21080,7 +21080,7 @@
         <v>1372</v>
       </c>
       <c r="I11">
-        <v>537</v>
+        <v>549</v>
       </c>
     </row>
   </sheetData>
@@ -21353,7 +21353,7 @@
         <v>11</v>
       </c>
       <c r="I9">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="10" spans="1:9">
@@ -21411,7 +21411,7 @@
         <v>293</v>
       </c>
       <c r="I11">
-        <v>142</v>
+        <v>143</v>
       </c>
     </row>
   </sheetData>
@@ -21693,7 +21693,7 @@
         <v>65</v>
       </c>
       <c r="I9">
-        <v>43</v>
+        <v>44</v>
       </c>
     </row>
     <row r="10" spans="1:9">
@@ -21722,7 +21722,7 @@
         <v>259</v>
       </c>
       <c r="I10">
-        <v>129</v>
+        <v>130</v>
       </c>
     </row>
     <row r="11" spans="1:9">
@@ -21751,7 +21751,7 @@
         <v>664</v>
       </c>
       <c r="I11">
-        <v>315</v>
+        <v>317</v>
       </c>
     </row>
   </sheetData>
@@ -22053,7 +22053,7 @@
         <v>306</v>
       </c>
       <c r="I10">
-        <v>78</v>
+        <v>80</v>
       </c>
     </row>
     <row r="11" spans="1:9">
@@ -22082,7 +22082,7 @@
         <v>531</v>
       </c>
       <c r="I11">
-        <v>140</v>
+        <v>142</v>
       </c>
     </row>
   </sheetData>
@@ -22338,7 +22338,7 @@
         <v>156</v>
       </c>
       <c r="I8">
-        <v>64</v>
+        <v>65</v>
       </c>
     </row>
     <row r="9" spans="1:9">
@@ -22425,7 +22425,7 @@
         <v>1246</v>
       </c>
       <c r="I11">
-        <v>462</v>
+        <v>463</v>
       </c>
     </row>
   </sheetData>
@@ -22536,7 +22536,7 @@
         <v>81</v>
       </c>
       <c r="I3">
-        <v>27</v>
+        <v>28</v>
       </c>
     </row>
     <row r="4" spans="1:9">
@@ -22672,7 +22672,7 @@
         <v>177</v>
       </c>
       <c r="I8">
-        <v>78</v>
+        <v>79</v>
       </c>
     </row>
     <row r="9" spans="1:9">
@@ -22730,7 +22730,7 @@
         <v>465</v>
       </c>
       <c r="I10">
-        <v>199</v>
+        <v>203</v>
       </c>
     </row>
     <row r="11" spans="1:9">
@@ -22759,7 +22759,7 @@
         <v>944</v>
       </c>
       <c r="I11">
-        <v>366</v>
+        <v>372</v>
       </c>
     </row>
   </sheetData>
@@ -22870,7 +22870,7 @@
         <v>211</v>
       </c>
       <c r="I3">
-        <v>66</v>
+        <v>67</v>
       </c>
     </row>
     <row r="4" spans="1:9">
@@ -23015,7 +23015,7 @@
         <v>200</v>
       </c>
       <c r="I8">
-        <v>96</v>
+        <v>97</v>
       </c>
     </row>
     <row r="9" spans="1:9">
@@ -23073,7 +23073,7 @@
         <v>605</v>
       </c>
       <c r="I10">
-        <v>297</v>
+        <v>300</v>
       </c>
     </row>
     <row r="11" spans="1:9">
@@ -23102,7 +23102,7 @@
         <v>1676</v>
       </c>
       <c r="I11">
-        <v>709</v>
+        <v>714</v>
       </c>
     </row>
   </sheetData>
@@ -23213,7 +23213,7 @@
         <v>77</v>
       </c>
       <c r="I3">
-        <v>19</v>
+        <v>20</v>
       </c>
     </row>
     <row r="4" spans="1:9">
@@ -23238,6 +23238,9 @@
       <c r="H4">
         <v>3</v>
       </c>
+      <c r="I4">
+        <v>1</v>
+      </c>
     </row>
     <row r="5" spans="1:9">
       <c r="A5" s="1" t="s">
@@ -23407,7 +23410,7 @@
         <v>545</v>
       </c>
       <c r="I10">
-        <v>210</v>
+        <v>211</v>
       </c>
     </row>
     <row r="11" spans="1:9">
@@ -23436,7 +23439,7 @@
         <v>1012</v>
       </c>
       <c r="I11">
-        <v>363</v>
+        <v>366</v>
       </c>
     </row>
   </sheetData>
@@ -23518,7 +23521,7 @@
         <v>98</v>
       </c>
       <c r="I2">
-        <v>32</v>
+        <v>34</v>
       </c>
     </row>
     <row r="3" spans="1:9">
@@ -23750,7 +23753,7 @@
         <v>243</v>
       </c>
       <c r="I10">
-        <v>121</v>
+        <v>123</v>
       </c>
     </row>
     <row r="11" spans="1:9">
@@ -23779,7 +23782,7 @@
         <v>722</v>
       </c>
       <c r="I11">
-        <v>287</v>
+        <v>291</v>
       </c>
     </row>
   </sheetData>
@@ -24336,7 +24339,7 @@
         <v>90</v>
       </c>
       <c r="I8">
-        <v>40</v>
+        <v>41</v>
       </c>
     </row>
     <row r="9" spans="1:9">
@@ -24423,7 +24426,7 @@
         <v>587</v>
       </c>
       <c r="I11">
-        <v>244</v>
+        <v>245</v>
       </c>
     </row>
   </sheetData>
@@ -24505,7 +24508,7 @@
         <v>101</v>
       </c>
       <c r="I2">
-        <v>31</v>
+        <v>32</v>
       </c>
     </row>
     <row r="3" spans="1:9">
@@ -24621,7 +24624,7 @@
         <v>14</v>
       </c>
       <c r="I6">
-        <v>9</v>
+        <v>11</v>
       </c>
     </row>
     <row r="7" spans="1:9">
@@ -24766,7 +24769,7 @@
         <v>902</v>
       </c>
       <c r="I11">
-        <v>370</v>
+        <v>373</v>
       </c>
     </row>
   </sheetData>
@@ -25068,7 +25071,7 @@
         <v>512</v>
       </c>
       <c r="I10">
-        <v>180</v>
+        <v>182</v>
       </c>
     </row>
     <row r="11" spans="1:9">
@@ -25097,7 +25100,7 @@
         <v>760</v>
       </c>
       <c r="I11">
-        <v>250</v>
+        <v>252</v>
       </c>
     </row>
   </sheetData>
@@ -25208,7 +25211,7 @@
         <v>34</v>
       </c>
       <c r="I3">
-        <v>15</v>
+        <v>16</v>
       </c>
     </row>
     <row r="4" spans="1:9">
@@ -25428,7 +25431,7 @@
         <v>501</v>
       </c>
       <c r="I11">
-        <v>224</v>
+        <v>225</v>
       </c>
     </row>
   </sheetData>
@@ -25713,7 +25716,7 @@
         <v>99</v>
       </c>
       <c r="I9">
-        <v>33</v>
+        <v>34</v>
       </c>
     </row>
     <row r="10" spans="1:9">
@@ -25742,7 +25745,7 @@
         <v>188</v>
       </c>
       <c r="I10">
-        <v>67</v>
+        <v>68</v>
       </c>
     </row>
     <row r="11" spans="1:9">
@@ -25771,7 +25774,7 @@
         <v>559</v>
       </c>
       <c r="I11">
-        <v>196</v>
+        <v>198</v>
       </c>
     </row>
   </sheetData>
@@ -25853,7 +25856,7 @@
         <v>115</v>
       </c>
       <c r="I2">
-        <v>60</v>
+        <v>61</v>
       </c>
     </row>
     <row r="3" spans="1:9">
@@ -26085,7 +26088,7 @@
         <v>678</v>
       </c>
       <c r="I10">
-        <v>271</v>
+        <v>272</v>
       </c>
     </row>
     <row r="11" spans="1:9">
@@ -26114,7 +26117,7 @@
         <v>1312</v>
       </c>
       <c r="I11">
-        <v>522</v>
+        <v>524</v>
       </c>
     </row>
   </sheetData>
@@ -26196,7 +26199,7 @@
         <v>67</v>
       </c>
       <c r="I2">
-        <v>12</v>
+        <v>13</v>
       </c>
     </row>
     <row r="3" spans="1:9">
@@ -26422,7 +26425,7 @@
         <v>127</v>
       </c>
       <c r="I10">
-        <v>45</v>
+        <v>46</v>
       </c>
     </row>
     <row r="11" spans="1:9">
@@ -26451,7 +26454,7 @@
         <v>377</v>
       </c>
       <c r="I11">
-        <v>125</v>
+        <v>127</v>
       </c>
     </row>
   </sheetData>
@@ -26720,7 +26723,7 @@
         <v>431</v>
       </c>
       <c r="I10">
-        <v>164</v>
+        <v>166</v>
       </c>
     </row>
     <row r="11" spans="1:9">
@@ -26749,7 +26752,7 @@
         <v>482</v>
       </c>
       <c r="I11">
-        <v>182</v>
+        <v>184</v>
       </c>
     </row>
   </sheetData>
@@ -27231,7 +27234,7 @@
         <v>81</v>
       </c>
       <c r="I5">
-        <v>16</v>
+        <v>17</v>
       </c>
     </row>
     <row r="6" spans="1:9">
@@ -27376,7 +27379,7 @@
         <v>405</v>
       </c>
       <c r="I10">
-        <v>142</v>
+        <v>143</v>
       </c>
     </row>
     <row r="11" spans="1:9">
@@ -27405,7 +27408,7 @@
         <v>767</v>
       </c>
       <c r="I11">
-        <v>274</v>
+        <v>276</v>
       </c>
     </row>
   </sheetData>
@@ -27643,7 +27646,7 @@
         <v>56</v>
       </c>
       <c r="I8">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="9" spans="1:9">
@@ -27672,7 +27675,7 @@
         <v>66</v>
       </c>
       <c r="I9">
-        <v>16</v>
+        <v>17</v>
       </c>
     </row>
     <row r="10" spans="1:9">
@@ -27916,7 +27919,7 @@
         <v>19</v>
       </c>
       <c r="I6">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="7" spans="1:9">
@@ -27991,7 +27994,7 @@
         <v>96</v>
       </c>
       <c r="I9">
-        <v>43</v>
+        <v>45</v>
       </c>
     </row>
     <row r="10" spans="1:9">
@@ -28020,7 +28023,7 @@
         <v>485</v>
       </c>
       <c r="I10">
-        <v>157</v>
+        <v>159</v>
       </c>
     </row>
     <row r="11" spans="1:9">
@@ -28049,7 +28052,7 @@
         <v>841</v>
       </c>
       <c r="I11">
-        <v>312</v>
+        <v>317</v>
       </c>
     </row>
   </sheetData>
@@ -28206,7 +28209,7 @@
         <v>10</v>
       </c>
       <c r="I5">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="6" spans="1:9">
@@ -28365,7 +28368,7 @@
         <v>130</v>
       </c>
       <c r="I11">
-        <v>31</v>
+        <v>32</v>
       </c>
     </row>
   </sheetData>
@@ -28609,7 +28612,7 @@
         <v>42</v>
       </c>
       <c r="I8">
-        <v>20</v>
+        <v>21</v>
       </c>
     </row>
     <row r="9" spans="1:9">
@@ -28696,7 +28699,7 @@
         <v>303</v>
       </c>
       <c r="I11">
-        <v>154</v>
+        <v>155</v>
       </c>
     </row>
   </sheetData>
@@ -28892,6 +28895,9 @@
       <c r="E7">
         <v>1</v>
       </c>
+      <c r="I7">
+        <v>2</v>
+      </c>
     </row>
     <row r="8" spans="1:9">
       <c r="A8" s="1" t="s">
@@ -29006,7 +29012,7 @@
         <v>314</v>
       </c>
       <c r="I11">
-        <v>139</v>
+        <v>141</v>
       </c>
     </row>
   </sheetData>
@@ -29175,7 +29181,7 @@
         <v>41</v>
       </c>
       <c r="I5">
-        <v>21</v>
+        <v>22</v>
       </c>
     </row>
     <row r="6" spans="1:9">
@@ -29317,7 +29323,7 @@
         <v>329</v>
       </c>
       <c r="I10">
-        <v>136</v>
+        <v>139</v>
       </c>
     </row>
     <row r="11" spans="1:9">
@@ -29346,7 +29352,7 @@
         <v>565</v>
       </c>
       <c r="I11">
-        <v>235</v>
+        <v>239</v>
       </c>
     </row>
   </sheetData>
@@ -29428,7 +29434,7 @@
         <v>452</v>
       </c>
       <c r="I2">
-        <v>169</v>
+        <v>170</v>
       </c>
     </row>
     <row r="3" spans="1:9">
@@ -29457,7 +29463,7 @@
         <v>587</v>
       </c>
       <c r="I3">
-        <v>146</v>
+        <v>147</v>
       </c>
     </row>
     <row r="4" spans="1:9">
@@ -29515,7 +29521,7 @@
         <v>280</v>
       </c>
       <c r="I5">
-        <v>96</v>
+        <v>97</v>
       </c>
     </row>
     <row r="6" spans="1:9">
@@ -29544,7 +29550,7 @@
         <v>84</v>
       </c>
       <c r="I6">
-        <v>33</v>
+        <v>34</v>
       </c>
     </row>
     <row r="7" spans="1:9">
@@ -29602,7 +29608,7 @@
         <v>560</v>
       </c>
       <c r="I8">
-        <v>209</v>
+        <v>210</v>
       </c>
     </row>
     <row r="9" spans="1:9">
@@ -29631,7 +29637,7 @@
         <v>506</v>
       </c>
       <c r="I9">
-        <v>173</v>
+        <v>174</v>
       </c>
     </row>
     <row r="10" spans="1:9">
@@ -29660,7 +29666,7 @@
         <v>1392</v>
       </c>
       <c r="I10">
-        <v>533</v>
+        <v>545</v>
       </c>
     </row>
     <row r="11" spans="1:9">
@@ -29689,7 +29695,7 @@
         <v>3973</v>
       </c>
       <c r="I11">
-        <v>1390</v>
+        <v>1408</v>
       </c>
     </row>
   </sheetData>
@@ -29935,7 +29941,7 @@
         <v>17</v>
       </c>
       <c r="I9">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="10" spans="1:9">
@@ -29993,7 +29999,7 @@
         <v>233</v>
       </c>
       <c r="I11">
-        <v>67</v>
+        <v>68</v>
       </c>
     </row>
   </sheetData>
@@ -30277,7 +30283,7 @@
         <v>91</v>
       </c>
       <c r="I10">
-        <v>30</v>
+        <v>32</v>
       </c>
     </row>
     <row r="11" spans="1:9">
@@ -30306,7 +30312,7 @@
         <v>170</v>
       </c>
       <c r="I11">
-        <v>62</v>
+        <v>64</v>
       </c>
     </row>
   </sheetData>
@@ -30713,7 +30719,7 @@
         <v>21</v>
       </c>
       <c r="I3">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="4" spans="1:9">
@@ -30759,7 +30765,7 @@
         <v>85</v>
       </c>
       <c r="I5">
-        <v>28</v>
+        <v>29</v>
       </c>
     </row>
     <row r="6" spans="1:9">
@@ -30895,7 +30901,7 @@
         <v>592</v>
       </c>
       <c r="I10">
-        <v>317</v>
+        <v>321</v>
       </c>
     </row>
     <row r="11" spans="1:9">
@@ -30924,7 +30930,7 @@
         <v>963</v>
       </c>
       <c r="I11">
-        <v>429</v>
+        <v>435</v>
       </c>
     </row>
   </sheetData>
@@ -31352,7 +31358,7 @@
         <v>22</v>
       </c>
       <c r="I5">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="6" spans="1:9">
@@ -31511,7 +31517,7 @@
         <v>180</v>
       </c>
       <c r="I11">
-        <v>73</v>
+        <v>74</v>
       </c>
     </row>
   </sheetData>
@@ -31593,7 +31599,7 @@
         <v>19</v>
       </c>
       <c r="I2">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="3" spans="1:9">
@@ -31819,7 +31825,7 @@
         <v>107</v>
       </c>
       <c r="I10">
-        <v>45</v>
+        <v>46</v>
       </c>
     </row>
     <row r="11" spans="1:9">
@@ -31848,7 +31854,7 @@
         <v>273</v>
       </c>
       <c r="I11">
-        <v>106</v>
+        <v>108</v>
       </c>
     </row>
   </sheetData>
@@ -32530,7 +32536,7 @@
         <v>37</v>
       </c>
       <c r="I2">
-        <v>17</v>
+        <v>18</v>
       </c>
     </row>
     <row r="3" spans="1:9">
@@ -32559,7 +32565,7 @@
         <v>57</v>
       </c>
       <c r="I3">
-        <v>16</v>
+        <v>17</v>
       </c>
     </row>
     <row r="4" spans="1:9">
@@ -32756,7 +32762,7 @@
         <v>121</v>
       </c>
       <c r="I10">
-        <v>46</v>
+        <v>48</v>
       </c>
     </row>
     <row r="11" spans="1:9">
@@ -32785,7 +32791,7 @@
         <v>395</v>
       </c>
       <c r="I11">
-        <v>149</v>
+        <v>153</v>
       </c>
     </row>
   </sheetData>
@@ -32896,7 +32902,7 @@
         <v>60</v>
       </c>
       <c r="I3">
-        <v>26</v>
+        <v>27</v>
       </c>
     </row>
     <row r="4" spans="1:9">
@@ -33070,7 +33076,7 @@
         <v>88</v>
       </c>
       <c r="I9">
-        <v>36</v>
+        <v>37</v>
       </c>
     </row>
     <row r="10" spans="1:9">
@@ -33099,7 +33105,7 @@
         <v>716</v>
       </c>
       <c r="I10">
-        <v>270</v>
+        <v>273</v>
       </c>
     </row>
     <row r="11" spans="1:9">
@@ -33128,7 +33134,7 @@
         <v>1182</v>
       </c>
       <c r="I11">
-        <v>453</v>
+        <v>458</v>
       </c>
     </row>
   </sheetData>
@@ -33915,7 +33921,7 @@
         <v>6</v>
       </c>
       <c r="I6">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="7" spans="1:9">
@@ -34028,7 +34034,7 @@
         <v>136</v>
       </c>
       <c r="I10">
-        <v>78</v>
+        <v>79</v>
       </c>
     </row>
     <row r="11" spans="1:9">
@@ -34057,7 +34063,7 @@
         <v>296</v>
       </c>
       <c r="I11">
-        <v>126</v>
+        <v>128</v>
       </c>
     </row>
   </sheetData>
@@ -34313,7 +34319,7 @@
         <v>102</v>
       </c>
       <c r="I8">
-        <v>44</v>
+        <v>45</v>
       </c>
     </row>
     <row r="9" spans="1:9">
@@ -34371,7 +34377,7 @@
         <v>329</v>
       </c>
       <c r="I10">
-        <v>159</v>
+        <v>165</v>
       </c>
     </row>
     <row r="11" spans="1:9">
@@ -34400,7 +34406,7 @@
         <v>690</v>
       </c>
       <c r="I11">
-        <v>294</v>
+        <v>301</v>
       </c>
     </row>
   </sheetData>
@@ -34666,7 +34672,7 @@
         <v>158</v>
       </c>
       <c r="I10">
-        <v>104</v>
+        <v>106</v>
       </c>
     </row>
     <row r="11" spans="1:9">
@@ -34695,7 +34701,7 @@
         <v>198</v>
       </c>
       <c r="I11">
-        <v>139</v>
+        <v>141</v>
       </c>
     </row>
   </sheetData>
@@ -34944,7 +34950,7 @@
         <v>83</v>
       </c>
       <c r="I9">
-        <v>22</v>
+        <v>24</v>
       </c>
     </row>
     <row r="10" spans="1:9">
@@ -34973,7 +34979,7 @@
         <v>123</v>
       </c>
       <c r="I10">
-        <v>35</v>
+        <v>37</v>
       </c>
     </row>
   </sheetData>
@@ -35445,7 +35451,7 @@
         <v>10</v>
       </c>
       <c r="I7">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="8" spans="1:9">
@@ -35532,7 +35538,7 @@
         <v>104</v>
       </c>
       <c r="I10">
-        <v>26</v>
+        <v>27</v>
       </c>
     </row>
   </sheetData>
@@ -35695,7 +35701,7 @@
         <v>47</v>
       </c>
       <c r="I5">
-        <v>14</v>
+        <v>15</v>
       </c>
     </row>
     <row r="6" spans="1:9">
@@ -35819,7 +35825,7 @@
         <v>128</v>
       </c>
       <c r="I10">
-        <v>58</v>
+        <v>59</v>
       </c>
     </row>
     <row r="11" spans="1:9">
@@ -35848,7 +35854,7 @@
         <v>265</v>
       </c>
       <c r="I11">
-        <v>108</v>
+        <v>110</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add data for 2023-01-21
</commit_message>
<xml_diff>
--- a/output/index-crime-full-year.xlsx
+++ b/output/index-crime-full-year.xlsx
@@ -895,7 +895,7 @@
         <v>7270</v>
       </c>
       <c r="J2">
-        <v>369</v>
+        <v>381</v>
       </c>
     </row>
     <row r="3" spans="1:10">
@@ -927,7 +927,7 @@
         <v>7487</v>
       </c>
       <c r="J3">
-        <v>415</v>
+        <v>436</v>
       </c>
     </row>
     <row r="4" spans="1:10">
@@ -959,7 +959,7 @@
         <v>423</v>
       </c>
       <c r="J4">
-        <v>30</v>
+        <v>31</v>
       </c>
     </row>
     <row r="5" spans="1:10">
@@ -985,13 +985,13 @@
         <v>8757</v>
       </c>
       <c r="H5">
-        <v>6659</v>
+        <v>6658</v>
       </c>
       <c r="I5">
         <v>7578</v>
       </c>
       <c r="J5">
-        <v>419</v>
+        <v>444</v>
       </c>
     </row>
     <row r="6" spans="1:10">
@@ -1014,7 +1014,7 @@
         <v>1877</v>
       </c>
       <c r="G6">
-        <v>1451</v>
+        <v>1452</v>
       </c>
       <c r="H6">
         <v>1685</v>
@@ -1023,7 +1023,7 @@
         <v>1736</v>
       </c>
       <c r="J6">
-        <v>74</v>
+        <v>78</v>
       </c>
     </row>
     <row r="7" spans="1:10">
@@ -1055,7 +1055,7 @@
         <v>710</v>
       </c>
       <c r="J7">
-        <v>27</v>
+        <v>31</v>
       </c>
     </row>
     <row r="8" spans="1:10">
@@ -1084,10 +1084,10 @@
         <v>10596</v>
       </c>
       <c r="I8">
-        <v>21386</v>
+        <v>21389</v>
       </c>
       <c r="J8">
-        <v>1924</v>
+        <v>2032</v>
       </c>
     </row>
     <row r="9" spans="1:10">
@@ -1119,7 +1119,7 @@
         <v>8965</v>
       </c>
       <c r="J9">
-        <v>586</v>
+        <v>623</v>
       </c>
     </row>
     <row r="10" spans="1:10">
@@ -1145,13 +1145,13 @@
         <v>41311</v>
       </c>
       <c r="H10">
-        <v>40773</v>
+        <v>40774</v>
       </c>
       <c r="I10">
-        <v>54534</v>
+        <v>54541</v>
       </c>
       <c r="J10">
-        <v>2609</v>
+        <v>2769</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -1174,16 +1174,16 @@
         <v>105543</v>
       </c>
       <c r="G11">
-        <v>85285</v>
+        <v>85286</v>
       </c>
       <c r="H11">
         <v>84551</v>
       </c>
       <c r="I11">
-        <v>110089</v>
+        <v>110099</v>
       </c>
       <c r="J11">
-        <v>6453</v>
+        <v>6825</v>
       </c>
     </row>
   </sheetData>
@@ -1461,7 +1461,7 @@
         <v>567</v>
       </c>
       <c r="J8">
-        <v>51</v>
+        <v>53</v>
       </c>
     </row>
     <row r="9" spans="1:10">
@@ -1525,7 +1525,7 @@
         <v>1023</v>
       </c>
       <c r="J10">
-        <v>50</v>
+        <v>52</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -1557,7 +1557,7 @@
         <v>2687</v>
       </c>
       <c r="J11">
-        <v>175</v>
+        <v>179</v>
       </c>
     </row>
   </sheetData>
@@ -2097,7 +2097,7 @@
         <v>292</v>
       </c>
       <c r="J8">
-        <v>16</v>
+        <v>18</v>
       </c>
     </row>
     <row r="9" spans="1:10">
@@ -2161,7 +2161,7 @@
         <v>904</v>
       </c>
       <c r="J10">
-        <v>41</v>
+        <v>43</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -2193,7 +2193,7 @@
         <v>1670</v>
       </c>
       <c r="J11">
-        <v>83</v>
+        <v>87</v>
       </c>
     </row>
   </sheetData>
@@ -2496,7 +2496,7 @@
         <v>502</v>
       </c>
       <c r="J10">
-        <v>26</v>
+        <v>28</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -2528,7 +2528,7 @@
         <v>677</v>
       </c>
       <c r="J11">
-        <v>37</v>
+        <v>39</v>
       </c>
     </row>
   </sheetData>
@@ -2826,7 +2826,7 @@
         <v>50</v>
       </c>
       <c r="J9">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="10" spans="1:10">
@@ -2890,7 +2890,7 @@
         <v>718</v>
       </c>
       <c r="J11">
-        <v>39</v>
+        <v>40</v>
       </c>
     </row>
   </sheetData>
@@ -3223,7 +3223,7 @@
         <v>105</v>
       </c>
       <c r="J10">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -3255,7 +3255,7 @@
         <v>261</v>
       </c>
       <c r="J11">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
   </sheetData>
@@ -3437,7 +3437,7 @@
         <v>202</v>
       </c>
       <c r="J5">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="6" spans="1:10">
@@ -3533,7 +3533,7 @@
         <v>722</v>
       </c>
       <c r="J8">
-        <v>57</v>
+        <v>61</v>
       </c>
     </row>
     <row r="9" spans="1:10">
@@ -3597,7 +3597,7 @@
         <v>812</v>
       </c>
       <c r="J10">
-        <v>35</v>
+        <v>36</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -3629,7 +3629,7 @@
         <v>2548</v>
       </c>
       <c r="J11">
-        <v>150</v>
+        <v>156</v>
       </c>
     </row>
   </sheetData>
@@ -3814,7 +3814,7 @@
         <v>121</v>
       </c>
       <c r="J5">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="6" spans="1:10">
@@ -3907,7 +3907,7 @@
         <v>384</v>
       </c>
       <c r="J8">
-        <v>54</v>
+        <v>59</v>
       </c>
     </row>
     <row r="9" spans="1:10">
@@ -3971,7 +3971,7 @@
         <v>527</v>
       </c>
       <c r="J10">
-        <v>28</v>
+        <v>30</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -4003,7 +4003,7 @@
         <v>1489</v>
       </c>
       <c r="J11">
-        <v>113</v>
+        <v>121</v>
       </c>
     </row>
   </sheetData>
@@ -4092,7 +4092,7 @@
         <v>235</v>
       </c>
       <c r="J2">
-        <v>7</v>
+        <v>9</v>
       </c>
     </row>
     <row r="3" spans="1:10">
@@ -4124,7 +4124,7 @@
         <v>364</v>
       </c>
       <c r="J3">
-        <v>28</v>
+        <v>29</v>
       </c>
     </row>
     <row r="4" spans="1:10">
@@ -4188,7 +4188,7 @@
         <v>103</v>
       </c>
       <c r="J5">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="6" spans="1:10">
@@ -4281,7 +4281,7 @@
         <v>516</v>
       </c>
       <c r="J8">
-        <v>34</v>
+        <v>36</v>
       </c>
     </row>
     <row r="9" spans="1:10">
@@ -4345,7 +4345,7 @@
         <v>897</v>
       </c>
       <c r="J10">
-        <v>31</v>
+        <v>35</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -4377,7 +4377,7 @@
         <v>2512</v>
       </c>
       <c r="J11">
-        <v>131</v>
+        <v>141</v>
       </c>
     </row>
   </sheetData>
@@ -4652,7 +4652,7 @@
         <v>152</v>
       </c>
       <c r="J8">
-        <v>8</v>
+        <v>10</v>
       </c>
     </row>
     <row r="9" spans="1:10">
@@ -4713,7 +4713,7 @@
         <v>381</v>
       </c>
       <c r="J10">
-        <v>19</v>
+        <v>21</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -4745,7 +4745,7 @@
         <v>866</v>
       </c>
       <c r="J11">
-        <v>44</v>
+        <v>48</v>
       </c>
     </row>
   </sheetData>
@@ -5017,7 +5017,7 @@
         <v>190</v>
       </c>
       <c r="J8">
-        <v>18</v>
+        <v>20</v>
       </c>
     </row>
     <row r="9" spans="1:10">
@@ -5081,7 +5081,7 @@
         <v>271</v>
       </c>
       <c r="J10">
-        <v>14</v>
+        <v>15</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -5113,7 +5113,7 @@
         <v>729</v>
       </c>
       <c r="J11">
-        <v>47</v>
+        <v>50</v>
       </c>
     </row>
   </sheetData>
@@ -5202,7 +5202,7 @@
         <v>918</v>
       </c>
       <c r="J2">
-        <v>52</v>
+        <v>54</v>
       </c>
     </row>
     <row r="3" spans="1:10">
@@ -5234,7 +5234,7 @@
         <v>155</v>
       </c>
       <c r="J3">
-        <v>14</v>
+        <v>15</v>
       </c>
     </row>
     <row r="4" spans="1:10">
@@ -5266,7 +5266,7 @@
         <v>436</v>
       </c>
       <c r="J4">
-        <v>30</v>
+        <v>31</v>
       </c>
     </row>
     <row r="5" spans="1:10">
@@ -5330,7 +5330,7 @@
         <v>793</v>
       </c>
       <c r="J6">
-        <v>42</v>
+        <v>46</v>
       </c>
     </row>
     <row r="7" spans="1:10">
@@ -5362,7 +5362,7 @@
         <v>2687</v>
       </c>
       <c r="J7">
-        <v>175</v>
+        <v>179</v>
       </c>
     </row>
     <row r="8" spans="1:10">
@@ -5394,7 +5394,7 @@
         <v>4749</v>
       </c>
       <c r="J8">
-        <v>263</v>
+        <v>280</v>
       </c>
     </row>
     <row r="9" spans="1:10">
@@ -5458,7 +5458,7 @@
         <v>949</v>
       </c>
       <c r="J10">
-        <v>51</v>
+        <v>53</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -5490,7 +5490,7 @@
         <v>1711</v>
       </c>
       <c r="J11">
-        <v>122</v>
+        <v>131</v>
       </c>
     </row>
     <row r="12" spans="1:10">
@@ -5522,7 +5522,7 @@
         <v>413</v>
       </c>
       <c r="J12">
-        <v>31</v>
+        <v>33</v>
       </c>
     </row>
     <row r="13" spans="1:10">
@@ -5586,7 +5586,7 @@
         <v>718</v>
       </c>
       <c r="J14">
-        <v>39</v>
+        <v>40</v>
       </c>
     </row>
     <row r="15" spans="1:10">
@@ -5618,7 +5618,7 @@
         <v>886</v>
       </c>
       <c r="J15">
-        <v>55</v>
+        <v>59</v>
       </c>
     </row>
     <row r="16" spans="1:10">
@@ -5682,7 +5682,7 @@
         <v>175</v>
       </c>
       <c r="J17">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="18" spans="1:10">
@@ -5746,7 +5746,7 @@
         <v>2636</v>
       </c>
       <c r="J19">
-        <v>171</v>
+        <v>183</v>
       </c>
     </row>
     <row r="20" spans="1:10">
@@ -5778,7 +5778,7 @@
         <v>2048</v>
       </c>
       <c r="J20">
-        <v>93</v>
+        <v>96</v>
       </c>
     </row>
     <row r="21" spans="1:10">
@@ -5810,7 +5810,7 @@
         <v>337</v>
       </c>
       <c r="J21">
-        <v>13</v>
+        <v>15</v>
       </c>
     </row>
     <row r="22" spans="1:10">
@@ -5874,7 +5874,7 @@
         <v>1369</v>
       </c>
       <c r="J23">
-        <v>105</v>
+        <v>108</v>
       </c>
     </row>
     <row r="24" spans="1:10">
@@ -5906,7 +5906,7 @@
         <v>501</v>
       </c>
       <c r="J24">
-        <v>40</v>
+        <v>41</v>
       </c>
     </row>
     <row r="25" spans="1:10">
@@ -5938,7 +5938,7 @@
         <v>431</v>
       </c>
       <c r="J25">
-        <v>20</v>
+        <v>22</v>
       </c>
     </row>
     <row r="26" spans="1:10">
@@ -5970,7 +5970,7 @@
         <v>248</v>
       </c>
       <c r="J26">
-        <v>16</v>
+        <v>18</v>
       </c>
     </row>
     <row r="27" spans="1:10">
@@ -6002,7 +6002,7 @@
         <v>1259</v>
       </c>
       <c r="J27">
-        <v>80</v>
+        <v>82</v>
       </c>
     </row>
     <row r="28" spans="1:10">
@@ -6034,7 +6034,7 @@
         <v>99</v>
       </c>
       <c r="J28">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="29" spans="1:10">
@@ -6066,7 +6066,7 @@
         <v>3951</v>
       </c>
       <c r="J29">
-        <v>266</v>
+        <v>283</v>
       </c>
     </row>
     <row r="30" spans="1:10">
@@ -6098,7 +6098,7 @@
         <v>261</v>
       </c>
       <c r="J30">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="31" spans="1:10">
@@ -6130,7 +6130,7 @@
         <v>866</v>
       </c>
       <c r="J31">
-        <v>44</v>
+        <v>48</v>
       </c>
     </row>
     <row r="32" spans="1:10">
@@ -6162,7 +6162,7 @@
         <v>209</v>
       </c>
       <c r="J32">
-        <v>12</v>
+        <v>13</v>
       </c>
     </row>
     <row r="33" spans="1:10">
@@ -6194,7 +6194,7 @@
         <v>3016</v>
       </c>
       <c r="J33">
-        <v>166</v>
+        <v>174</v>
       </c>
     </row>
     <row r="34" spans="1:10">
@@ -6226,7 +6226,7 @@
         <v>764</v>
       </c>
       <c r="J34">
-        <v>52</v>
+        <v>53</v>
       </c>
     </row>
     <row r="35" spans="1:10">
@@ -6290,7 +6290,7 @@
         <v>1493</v>
       </c>
       <c r="J36">
-        <v>97</v>
+        <v>98</v>
       </c>
     </row>
     <row r="37" spans="1:10">
@@ -6322,7 +6322,7 @@
         <v>2548</v>
       </c>
       <c r="J37">
-        <v>150</v>
+        <v>156</v>
       </c>
     </row>
     <row r="38" spans="1:10">
@@ -6354,7 +6354,7 @@
         <v>191</v>
       </c>
       <c r="J38">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="39" spans="1:10">
@@ -6386,7 +6386,7 @@
         <v>153</v>
       </c>
       <c r="J39">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="40" spans="1:10">
@@ -6418,7 +6418,7 @@
         <v>236</v>
       </c>
       <c r="J40">
-        <v>15</v>
+        <v>17</v>
       </c>
     </row>
     <row r="41" spans="1:10">
@@ -6450,7 +6450,7 @@
         <v>438</v>
       </c>
       <c r="J41">
-        <v>30</v>
+        <v>31</v>
       </c>
     </row>
     <row r="42" spans="1:10">
@@ -6482,7 +6482,7 @@
         <v>2956</v>
       </c>
       <c r="J42">
-        <v>163</v>
+        <v>179</v>
       </c>
     </row>
     <row r="43" spans="1:10">
@@ -6514,7 +6514,7 @@
         <v>1153</v>
       </c>
       <c r="J43">
-        <v>83</v>
+        <v>86</v>
       </c>
     </row>
     <row r="44" spans="1:10">
@@ -6546,7 +6546,7 @@
         <v>1229</v>
       </c>
       <c r="J44">
-        <v>80</v>
+        <v>84</v>
       </c>
     </row>
     <row r="45" spans="1:10">
@@ -6610,7 +6610,7 @@
         <v>433</v>
       </c>
       <c r="J46">
-        <v>20</v>
+        <v>23</v>
       </c>
     </row>
     <row r="47" spans="1:10">
@@ -6642,7 +6642,7 @@
         <v>904</v>
       </c>
       <c r="J47">
-        <v>69</v>
+        <v>71</v>
       </c>
     </row>
     <row r="48" spans="1:10">
@@ -6674,7 +6674,7 @@
         <v>2621</v>
       </c>
       <c r="J48">
-        <v>127</v>
+        <v>139</v>
       </c>
     </row>
     <row r="49" spans="1:10">
@@ -6706,7 +6706,7 @@
         <v>1647</v>
       </c>
       <c r="J49">
-        <v>92</v>
+        <v>95</v>
       </c>
     </row>
     <row r="50" spans="1:10">
@@ -6738,7 +6738,7 @@
         <v>962</v>
       </c>
       <c r="J50">
-        <v>79</v>
+        <v>80</v>
       </c>
     </row>
     <row r="51" spans="1:10">
@@ -6770,7 +6770,7 @@
         <v>1337</v>
       </c>
       <c r="J51">
-        <v>94</v>
+        <v>100</v>
       </c>
     </row>
     <row r="52" spans="1:10">
@@ -6802,7 +6802,7 @@
         <v>1494</v>
       </c>
       <c r="J52">
-        <v>91</v>
+        <v>99</v>
       </c>
     </row>
     <row r="53" spans="1:10">
@@ -6834,7 +6834,7 @@
         <v>1603</v>
       </c>
       <c r="J53">
-        <v>100</v>
+        <v>108</v>
       </c>
     </row>
     <row r="54" spans="1:10">
@@ -6866,7 +6866,7 @@
         <v>3508</v>
       </c>
       <c r="J54">
-        <v>182</v>
+        <v>198</v>
       </c>
     </row>
     <row r="55" spans="1:10">
@@ -6898,7 +6898,7 @@
         <v>1244</v>
       </c>
       <c r="J55">
-        <v>60</v>
+        <v>67</v>
       </c>
     </row>
     <row r="56" spans="1:10">
@@ -6930,7 +6930,7 @@
         <v>629</v>
       </c>
       <c r="J56">
-        <v>31</v>
+        <v>33</v>
       </c>
     </row>
     <row r="57" spans="1:10">
@@ -6962,7 +6962,7 @@
         <v>408</v>
       </c>
       <c r="J57">
-        <v>32</v>
+        <v>34</v>
       </c>
     </row>
     <row r="58" spans="1:10">
@@ -7058,7 +7058,7 @@
         <v>770</v>
       </c>
       <c r="J60">
-        <v>31</v>
+        <v>32</v>
       </c>
     </row>
     <row r="61" spans="1:10">
@@ -7090,7 +7090,7 @@
         <v>160</v>
       </c>
       <c r="J61">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="62" spans="1:10">
@@ -7145,16 +7145,16 @@
         <v>1311</v>
       </c>
       <c r="G63">
-        <v>1624</v>
+        <v>1625</v>
       </c>
       <c r="H63">
         <v>2119</v>
       </c>
       <c r="I63">
-        <v>2014</v>
+        <v>2024</v>
       </c>
       <c r="J63">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="64" spans="1:10">
@@ -7186,7 +7186,7 @@
         <v>1187</v>
       </c>
       <c r="J64">
-        <v>45</v>
+        <v>48</v>
       </c>
     </row>
     <row r="65" spans="1:10">
@@ -7218,7 +7218,7 @@
         <v>1516</v>
       </c>
       <c r="J65">
-        <v>77</v>
+        <v>79</v>
       </c>
     </row>
     <row r="66" spans="1:10">
@@ -7250,7 +7250,7 @@
         <v>715</v>
       </c>
       <c r="J66">
-        <v>39</v>
+        <v>40</v>
       </c>
     </row>
     <row r="67" spans="1:10">
@@ -7282,7 +7282,7 @@
         <v>2512</v>
       </c>
       <c r="J67">
-        <v>131</v>
+        <v>141</v>
       </c>
     </row>
     <row r="68" spans="1:10">
@@ -7314,7 +7314,7 @@
         <v>438</v>
       </c>
       <c r="J68">
-        <v>18</v>
+        <v>21</v>
       </c>
     </row>
     <row r="69" spans="1:10">
@@ -7346,7 +7346,7 @@
         <v>493</v>
       </c>
       <c r="J69">
-        <v>28</v>
+        <v>30</v>
       </c>
     </row>
     <row r="70" spans="1:10">
@@ -7378,7 +7378,7 @@
         <v>677</v>
       </c>
       <c r="J70">
-        <v>37</v>
+        <v>39</v>
       </c>
     </row>
     <row r="71" spans="1:10">
@@ -7410,7 +7410,7 @@
         <v>336</v>
       </c>
       <c r="J71">
-        <v>25</v>
+        <v>27</v>
       </c>
     </row>
     <row r="72" spans="1:10">
@@ -7442,7 +7442,7 @@
         <v>708</v>
       </c>
       <c r="J72">
-        <v>27</v>
+        <v>30</v>
       </c>
     </row>
     <row r="73" spans="1:10">
@@ -7474,7 +7474,7 @@
         <v>1279</v>
       </c>
       <c r="J73">
-        <v>66</v>
+        <v>68</v>
       </c>
     </row>
     <row r="74" spans="1:10">
@@ -7506,7 +7506,7 @@
         <v>307</v>
       </c>
       <c r="J74">
-        <v>16</v>
+        <v>17</v>
       </c>
     </row>
     <row r="75" spans="1:10">
@@ -7538,7 +7538,7 @@
         <v>340</v>
       </c>
       <c r="J75">
-        <v>21</v>
+        <v>23</v>
       </c>
     </row>
     <row r="76" spans="1:10">
@@ -7570,7 +7570,7 @@
         <v>2924</v>
       </c>
       <c r="J76">
-        <v>184</v>
+        <v>203</v>
       </c>
     </row>
     <row r="77" spans="1:10">
@@ -7602,7 +7602,7 @@
         <v>462</v>
       </c>
       <c r="J77">
-        <v>37</v>
+        <v>38</v>
       </c>
     </row>
     <row r="78" spans="1:10">
@@ -7634,7 +7634,7 @@
         <v>1797</v>
       </c>
       <c r="J78">
-        <v>90</v>
+        <v>94</v>
       </c>
     </row>
     <row r="79" spans="1:10">
@@ -7666,7 +7666,7 @@
         <v>2476</v>
       </c>
       <c r="J79">
-        <v>153</v>
+        <v>165</v>
       </c>
     </row>
     <row r="80" spans="1:10">
@@ -7698,7 +7698,7 @@
         <v>393</v>
       </c>
       <c r="J80">
-        <v>17</v>
+        <v>18</v>
       </c>
     </row>
     <row r="81" spans="1:10">
@@ -7730,7 +7730,7 @@
         <v>218</v>
       </c>
       <c r="J81">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="82" spans="1:10">
@@ -7762,7 +7762,7 @@
         <v>233</v>
       </c>
       <c r="J82">
-        <v>18</v>
+        <v>20</v>
       </c>
     </row>
     <row r="83" spans="1:10">
@@ -7794,7 +7794,7 @@
         <v>1794</v>
       </c>
       <c r="J83">
-        <v>97</v>
+        <v>99</v>
       </c>
     </row>
     <row r="84" spans="1:10">
@@ -7826,7 +7826,7 @@
         <v>729</v>
       </c>
       <c r="J84">
-        <v>47</v>
+        <v>50</v>
       </c>
     </row>
     <row r="85" spans="1:10">
@@ -7858,7 +7858,7 @@
         <v>3855</v>
       </c>
       <c r="J85">
-        <v>235</v>
+        <v>257</v>
       </c>
     </row>
     <row r="86" spans="1:10">
@@ -7890,7 +7890,7 @@
         <v>1066</v>
       </c>
       <c r="J86">
-        <v>39</v>
+        <v>42</v>
       </c>
     </row>
     <row r="87" spans="1:10">
@@ -7922,7 +7922,7 @@
         <v>396</v>
       </c>
       <c r="J87">
-        <v>24</v>
+        <v>26</v>
       </c>
     </row>
     <row r="88" spans="1:10">
@@ -7954,7 +7954,7 @@
         <v>944</v>
       </c>
       <c r="J88">
-        <v>74</v>
+        <v>81</v>
       </c>
     </row>
     <row r="89" spans="1:10">
@@ -7986,7 +7986,7 @@
         <v>1879</v>
       </c>
       <c r="J89">
-        <v>93</v>
+        <v>96</v>
       </c>
     </row>
     <row r="90" spans="1:10">
@@ -8018,7 +8018,7 @@
         <v>1356</v>
       </c>
       <c r="J90">
-        <v>93</v>
+        <v>96</v>
       </c>
     </row>
     <row r="91" spans="1:10">
@@ -8050,7 +8050,7 @@
         <v>971</v>
       </c>
       <c r="J91">
-        <v>78</v>
+        <v>80</v>
       </c>
     </row>
     <row r="92" spans="1:10">
@@ -8082,7 +8082,7 @@
         <v>337</v>
       </c>
       <c r="J92">
-        <v>21</v>
+        <v>23</v>
       </c>
     </row>
     <row r="93" spans="1:10">
@@ -8114,7 +8114,7 @@
         <v>720</v>
       </c>
       <c r="J93">
-        <v>39</v>
+        <v>44</v>
       </c>
     </row>
     <row r="94" spans="1:10">
@@ -8146,7 +8146,7 @@
         <v>2664</v>
       </c>
       <c r="J94">
-        <v>114</v>
+        <v>122</v>
       </c>
     </row>
     <row r="95" spans="1:10">
@@ -8178,7 +8178,7 @@
         <v>1387</v>
       </c>
       <c r="J95">
-        <v>92</v>
+        <v>98</v>
       </c>
     </row>
     <row r="96" spans="1:10">
@@ -8210,7 +8210,7 @@
         <v>1670</v>
       </c>
       <c r="J96">
-        <v>83</v>
+        <v>87</v>
       </c>
     </row>
     <row r="97" spans="1:10">
@@ -8274,7 +8274,7 @@
         <v>1320</v>
       </c>
       <c r="J98">
-        <v>52</v>
+        <v>56</v>
       </c>
     </row>
     <row r="99" spans="1:10">
@@ -8306,7 +8306,7 @@
         <v>1489</v>
       </c>
       <c r="J99">
-        <v>113</v>
+        <v>121</v>
       </c>
     </row>
     <row r="100" spans="1:10">
@@ -8338,7 +8338,7 @@
         <v>237</v>
       </c>
       <c r="J100">
-        <v>19</v>
+        <v>20</v>
       </c>
     </row>
     <row r="101" spans="1:10">
@@ -8361,16 +8361,16 @@
         <v>105543</v>
       </c>
       <c r="G101">
-        <v>85285</v>
+        <v>85286</v>
       </c>
       <c r="H101">
         <v>84551</v>
       </c>
       <c r="I101">
-        <v>110089</v>
+        <v>110099</v>
       </c>
       <c r="J101">
-        <v>6453</v>
+        <v>6825</v>
       </c>
     </row>
   </sheetData>
@@ -8785,7 +8785,7 @@
         <v>190</v>
       </c>
       <c r="J9">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="10" spans="1:10">
@@ -8817,7 +8817,7 @@
         <v>586</v>
       </c>
       <c r="J10">
-        <v>24</v>
+        <v>25</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -8849,7 +8849,7 @@
         <v>1516</v>
       </c>
       <c r="J11">
-        <v>77</v>
+        <v>79</v>
       </c>
     </row>
   </sheetData>
@@ -9173,7 +9173,7 @@
         <v>785</v>
       </c>
       <c r="J10">
-        <v>47</v>
+        <v>49</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -9205,7 +9205,7 @@
         <v>1259</v>
       </c>
       <c r="J11">
-        <v>80</v>
+        <v>82</v>
       </c>
     </row>
   </sheetData>
@@ -9326,7 +9326,7 @@
         <v>206</v>
       </c>
       <c r="J3">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="4" spans="1:10">
@@ -9544,7 +9544,7 @@
         <v>612</v>
       </c>
       <c r="J10">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -9576,7 +9576,7 @@
         <v>1794</v>
       </c>
       <c r="J11">
-        <v>97</v>
+        <v>99</v>
       </c>
     </row>
   </sheetData>
@@ -9761,7 +9761,7 @@
         <v>170</v>
       </c>
       <c r="J5">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="6" spans="1:10">
@@ -9857,7 +9857,7 @@
         <v>707</v>
       </c>
       <c r="J8">
-        <v>48</v>
+        <v>52</v>
       </c>
     </row>
     <row r="9" spans="1:10">
@@ -9889,7 +9889,7 @@
         <v>366</v>
       </c>
       <c r="J9">
-        <v>25</v>
+        <v>27</v>
       </c>
     </row>
     <row r="10" spans="1:10">
@@ -9921,7 +9921,7 @@
         <v>968</v>
       </c>
       <c r="J10">
-        <v>50</v>
+        <v>53</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -9953,7 +9953,7 @@
         <v>3016</v>
       </c>
       <c r="J11">
-        <v>166</v>
+        <v>174</v>
       </c>
     </row>
   </sheetData>
@@ -10074,7 +10074,7 @@
         <v>137</v>
       </c>
       <c r="J3">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="4" spans="1:10">
@@ -10228,7 +10228,7 @@
         <v>392</v>
       </c>
       <c r="J8">
-        <v>38</v>
+        <v>40</v>
       </c>
     </row>
     <row r="9" spans="1:10">
@@ -10292,7 +10292,7 @@
         <v>433</v>
       </c>
       <c r="J10">
-        <v>22</v>
+        <v>25</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -10324,7 +10324,7 @@
         <v>1387</v>
       </c>
       <c r="J11">
-        <v>92</v>
+        <v>98</v>
       </c>
     </row>
   </sheetData>
@@ -10587,7 +10587,7 @@
         <v>90</v>
       </c>
       <c r="J8">
-        <v>3</v>
+        <v>5</v>
       </c>
     </row>
     <row r="9" spans="1:10">
@@ -10683,7 +10683,7 @@
         <v>340</v>
       </c>
       <c r="J11">
-        <v>21</v>
+        <v>23</v>
       </c>
     </row>
   </sheetData>
@@ -10804,7 +10804,7 @@
         <v>245</v>
       </c>
       <c r="J3">
-        <v>13</v>
+        <v>15</v>
       </c>
     </row>
     <row r="4" spans="1:10">
@@ -10865,7 +10865,7 @@
         <v>192</v>
       </c>
       <c r="J5">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="6" spans="1:10">
@@ -10897,7 +10897,7 @@
         <v>42</v>
       </c>
       <c r="J6">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="7" spans="1:10">
@@ -10929,7 +10929,7 @@
         <v>28</v>
       </c>
       <c r="J7">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="8" spans="1:10">
@@ -10961,7 +10961,7 @@
         <v>701</v>
       </c>
       <c r="J8">
-        <v>61</v>
+        <v>64</v>
       </c>
     </row>
     <row r="9" spans="1:10">
@@ -11025,7 +11025,7 @@
         <v>821</v>
       </c>
       <c r="J10">
-        <v>36</v>
+        <v>40</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -11057,7 +11057,7 @@
         <v>2476</v>
       </c>
       <c r="J11">
-        <v>153</v>
+        <v>165</v>
       </c>
     </row>
   </sheetData>
@@ -11308,7 +11308,7 @@
         <v>123</v>
       </c>
       <c r="J8">
-        <v>13</v>
+        <v>15</v>
       </c>
     </row>
     <row r="9" spans="1:10">
@@ -11404,7 +11404,7 @@
         <v>336</v>
       </c>
       <c r="J11">
-        <v>25</v>
+        <v>27</v>
       </c>
     </row>
   </sheetData>
@@ -11571,7 +11571,7 @@
         <v>50</v>
       </c>
       <c r="J5">
-        <v>4</v>
+        <v>7</v>
       </c>
     </row>
     <row r="6" spans="1:10">
@@ -11748,7 +11748,7 @@
         <v>433</v>
       </c>
       <c r="J11">
-        <v>20</v>
+        <v>23</v>
       </c>
     </row>
   </sheetData>
@@ -12087,7 +12087,7 @@
         <v>380</v>
       </c>
       <c r="J10">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -12119,7 +12119,7 @@
         <v>770</v>
       </c>
       <c r="J11">
-        <v>31</v>
+        <v>32</v>
       </c>
     </row>
   </sheetData>
@@ -12304,7 +12304,7 @@
         <v>131</v>
       </c>
       <c r="J5">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="6" spans="1:10">
@@ -12391,7 +12391,7 @@
         <v>216</v>
       </c>
       <c r="J8">
-        <v>30</v>
+        <v>31</v>
       </c>
     </row>
     <row r="9" spans="1:10">
@@ -12423,7 +12423,7 @@
         <v>107</v>
       </c>
       <c r="J9">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="10" spans="1:10">
@@ -12487,7 +12487,7 @@
         <v>1879</v>
       </c>
       <c r="J11">
-        <v>93</v>
+        <v>96</v>
       </c>
     </row>
   </sheetData>
@@ -12750,7 +12750,7 @@
         <v>335</v>
       </c>
       <c r="J8">
-        <v>18</v>
+        <v>20</v>
       </c>
     </row>
     <row r="9" spans="1:10">
@@ -12814,7 +12814,7 @@
         <v>606</v>
       </c>
       <c r="J10">
-        <v>20</v>
+        <v>21</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -12846,7 +12846,7 @@
         <v>1187</v>
       </c>
       <c r="J11">
-        <v>45</v>
+        <v>48</v>
       </c>
     </row>
   </sheetData>
@@ -13045,7 +13045,7 @@
         <v>2</v>
       </c>
       <c r="J6">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="7" spans="1:10">
@@ -13155,7 +13155,7 @@
         <v>116</v>
       </c>
       <c r="J10">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -13187,7 +13187,7 @@
         <v>236</v>
       </c>
       <c r="J11">
-        <v>15</v>
+        <v>17</v>
       </c>
     </row>
   </sheetData>
@@ -13447,7 +13447,7 @@
         <v>294</v>
       </c>
       <c r="J8">
-        <v>12</v>
+        <v>13</v>
       </c>
     </row>
     <row r="9" spans="1:10">
@@ -13511,7 +13511,7 @@
         <v>2021</v>
       </c>
       <c r="J10">
-        <v>89</v>
+        <v>96</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -13543,7 +13543,7 @@
         <v>2664</v>
       </c>
       <c r="J11">
-        <v>114</v>
+        <v>122</v>
       </c>
     </row>
   </sheetData>
@@ -13664,7 +13664,7 @@
         <v>80</v>
       </c>
       <c r="J3">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="4" spans="1:10">
@@ -13722,7 +13722,7 @@
         <v>73</v>
       </c>
       <c r="J5">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="6" spans="1:10">
@@ -13815,7 +13815,7 @@
         <v>336</v>
       </c>
       <c r="J8">
-        <v>19</v>
+        <v>20</v>
       </c>
     </row>
     <row r="9" spans="1:10">
@@ -13847,7 +13847,7 @@
         <v>179</v>
       </c>
       <c r="J9">
-        <v>12</v>
+        <v>13</v>
       </c>
     </row>
     <row r="10" spans="1:10">
@@ -13879,7 +13879,7 @@
         <v>2133</v>
       </c>
       <c r="J10">
-        <v>141</v>
+        <v>156</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -13911,7 +13911,7 @@
         <v>2924</v>
       </c>
       <c r="J11">
-        <v>184</v>
+        <v>203</v>
       </c>
     </row>
   </sheetData>
@@ -13999,6 +13999,9 @@
       <c r="I2">
         <v>21</v>
       </c>
+      <c r="J2">
+        <v>1</v>
+      </c>
     </row>
     <row r="3" spans="1:10">
       <c r="A3" s="1" t="s">
@@ -14246,7 +14249,7 @@
         <v>715</v>
       </c>
       <c r="J11">
-        <v>39</v>
+        <v>40</v>
       </c>
     </row>
   </sheetData>
@@ -14512,7 +14515,7 @@
         <v>70</v>
       </c>
       <c r="J8">
-        <v>6</v>
+        <v>8</v>
       </c>
     </row>
     <row r="9" spans="1:10">
@@ -14608,7 +14611,7 @@
         <v>396</v>
       </c>
       <c r="J11">
-        <v>24</v>
+        <v>26</v>
       </c>
     </row>
   </sheetData>
@@ -14827,7 +14830,7 @@
         <v>20</v>
       </c>
       <c r="J7">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="8" spans="1:10">
@@ -14920,7 +14923,7 @@
         <v>237</v>
       </c>
       <c r="J10">
-        <v>19</v>
+        <v>20</v>
       </c>
     </row>
   </sheetData>
@@ -15009,7 +15012,7 @@
         <v>50</v>
       </c>
       <c r="J2">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="3" spans="1:10">
@@ -15253,7 +15256,7 @@
         <v>189</v>
       </c>
       <c r="J10">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -15285,7 +15288,7 @@
         <v>431</v>
       </c>
       <c r="J11">
-        <v>20</v>
+        <v>22</v>
       </c>
     </row>
   </sheetData>
@@ -15947,7 +15950,7 @@
         <v>1135</v>
       </c>
       <c r="J10">
-        <v>65</v>
+        <v>68</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -15979,7 +15982,7 @@
         <v>1647</v>
       </c>
       <c r="J11">
-        <v>92</v>
+        <v>95</v>
       </c>
     </row>
   </sheetData>
@@ -16068,7 +16071,7 @@
         <v>326</v>
       </c>
       <c r="J2">
-        <v>10</v>
+        <v>12</v>
       </c>
     </row>
     <row r="3" spans="1:10">
@@ -16100,7 +16103,7 @@
         <v>441</v>
       </c>
       <c r="J3">
-        <v>16</v>
+        <v>21</v>
       </c>
     </row>
     <row r="4" spans="1:10">
@@ -16164,7 +16167,7 @@
         <v>382</v>
       </c>
       <c r="J5">
-        <v>19</v>
+        <v>23</v>
       </c>
     </row>
     <row r="6" spans="1:10">
@@ -16196,7 +16199,7 @@
         <v>55</v>
       </c>
       <c r="J6">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="7" spans="1:10">
@@ -16257,7 +16260,7 @@
         <v>1028</v>
       </c>
       <c r="J8">
-        <v>104</v>
+        <v>108</v>
       </c>
     </row>
     <row r="9" spans="1:10">
@@ -16289,7 +16292,7 @@
         <v>304</v>
       </c>
       <c r="J9">
-        <v>20</v>
+        <v>22</v>
       </c>
     </row>
     <row r="10" spans="1:10">
@@ -16321,7 +16324,7 @@
         <v>1272</v>
       </c>
       <c r="J10">
-        <v>62</v>
+        <v>66</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -16353,7 +16356,7 @@
         <v>3855</v>
       </c>
       <c r="J11">
-        <v>235</v>
+        <v>257</v>
       </c>
     </row>
   </sheetData>
@@ -16899,6 +16902,9 @@
       <c r="I5">
         <v>90</v>
       </c>
+      <c r="J5">
+        <v>1</v>
+      </c>
     </row>
     <row r="6" spans="1:10">
       <c r="A6" s="1" t="s">
@@ -16990,7 +16996,7 @@
         <v>224</v>
       </c>
       <c r="J8">
-        <v>22</v>
+        <v>26</v>
       </c>
     </row>
     <row r="9" spans="1:10">
@@ -17022,7 +17028,7 @@
         <v>109</v>
       </c>
       <c r="J9">
-        <v>15</v>
+        <v>16</v>
       </c>
     </row>
     <row r="10" spans="1:10">
@@ -17054,7 +17060,7 @@
         <v>610</v>
       </c>
       <c r="J10">
-        <v>18</v>
+        <v>19</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -17086,7 +17092,7 @@
         <v>1244</v>
       </c>
       <c r="J11">
-        <v>60</v>
+        <v>67</v>
       </c>
     </row>
   </sheetData>
@@ -17300,7 +17306,7 @@
         <v>34</v>
       </c>
       <c r="J6">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="7" spans="1:10">
@@ -17422,7 +17428,7 @@
         <v>2527</v>
       </c>
       <c r="J10">
-        <v>135</v>
+        <v>150</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -17454,7 +17460,7 @@
         <v>3508</v>
       </c>
       <c r="J11">
-        <v>182</v>
+        <v>198</v>
       </c>
     </row>
   </sheetData>
@@ -17793,7 +17799,7 @@
         <v>681</v>
       </c>
       <c r="J10">
-        <v>37</v>
+        <v>39</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -17825,7 +17831,7 @@
         <v>1279</v>
       </c>
       <c r="J11">
-        <v>66</v>
+        <v>68</v>
       </c>
     </row>
   </sheetData>
@@ -17914,7 +17920,7 @@
         <v>459</v>
       </c>
       <c r="J2">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="3" spans="1:10">
@@ -17946,7 +17952,7 @@
         <v>529</v>
       </c>
       <c r="J3">
-        <v>28</v>
+        <v>31</v>
       </c>
     </row>
     <row r="4" spans="1:10">
@@ -18010,7 +18016,7 @@
         <v>269</v>
       </c>
       <c r="J5">
-        <v>16</v>
+        <v>19</v>
       </c>
     </row>
     <row r="6" spans="1:10">
@@ -18074,7 +18080,7 @@
         <v>49</v>
       </c>
       <c r="J7">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="8" spans="1:10">
@@ -18106,7 +18112,7 @@
         <v>794</v>
       </c>
       <c r="J8">
-        <v>97</v>
+        <v>102</v>
       </c>
     </row>
     <row r="9" spans="1:10">
@@ -18138,7 +18144,7 @@
         <v>434</v>
       </c>
       <c r="J9">
-        <v>25</v>
+        <v>27</v>
       </c>
     </row>
     <row r="10" spans="1:10">
@@ -18170,7 +18176,7 @@
         <v>1302</v>
       </c>
       <c r="J10">
-        <v>69</v>
+        <v>71</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -18202,7 +18208,7 @@
         <v>3951</v>
       </c>
       <c r="J11">
-        <v>266</v>
+        <v>283</v>
       </c>
     </row>
   </sheetData>
@@ -18387,7 +18393,7 @@
         <v>229</v>
       </c>
       <c r="J5">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="6" spans="1:10">
@@ -18483,7 +18489,7 @@
         <v>753</v>
       </c>
       <c r="J8">
-        <v>51</v>
+        <v>58</v>
       </c>
     </row>
     <row r="9" spans="1:10">
@@ -18515,7 +18521,7 @@
         <v>233</v>
       </c>
       <c r="J9">
-        <v>27</v>
+        <v>28</v>
       </c>
     </row>
     <row r="10" spans="1:10">
@@ -18547,7 +18553,7 @@
         <v>912</v>
       </c>
       <c r="J10">
-        <v>52</v>
+        <v>55</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -18579,7 +18585,7 @@
         <v>2636</v>
       </c>
       <c r="J11">
-        <v>171</v>
+        <v>183</v>
       </c>
     </row>
   </sheetData>
@@ -19259,7 +19265,7 @@
         <v>712</v>
       </c>
       <c r="J10">
-        <v>40</v>
+        <v>44</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -19291,7 +19297,7 @@
         <v>1229</v>
       </c>
       <c r="J11">
-        <v>80</v>
+        <v>84</v>
       </c>
     </row>
   </sheetData>
@@ -19572,7 +19578,7 @@
         <v>653</v>
       </c>
       <c r="J8">
-        <v>55</v>
+        <v>64</v>
       </c>
     </row>
     <row r="9" spans="1:10">
@@ -19604,7 +19610,7 @@
         <v>428</v>
       </c>
       <c r="J9">
-        <v>41</v>
+        <v>44</v>
       </c>
     </row>
     <row r="10" spans="1:10">
@@ -19636,7 +19642,7 @@
         <v>1089</v>
       </c>
       <c r="J10">
-        <v>41</v>
+        <v>45</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -19668,7 +19674,7 @@
         <v>2956</v>
       </c>
       <c r="J11">
-        <v>163</v>
+        <v>179</v>
       </c>
     </row>
   </sheetData>
@@ -19853,7 +19859,7 @@
         <v>177</v>
       </c>
       <c r="J5">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="6" spans="1:10">
@@ -19885,7 +19891,7 @@
         <v>43</v>
       </c>
       <c r="J6">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="7" spans="1:10">
@@ -19940,7 +19946,7 @@
         <v>337</v>
       </c>
       <c r="J8">
-        <v>25</v>
+        <v>29</v>
       </c>
     </row>
     <row r="9" spans="1:10">
@@ -19972,7 +19978,7 @@
         <v>170</v>
       </c>
       <c r="J9">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="10" spans="1:10">
@@ -20004,7 +20010,7 @@
         <v>1774</v>
       </c>
       <c r="J10">
-        <v>85</v>
+        <v>90</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -20036,7 +20042,7 @@
         <v>2621</v>
       </c>
       <c r="J11">
-        <v>127</v>
+        <v>139</v>
       </c>
     </row>
   </sheetData>
@@ -20357,7 +20363,7 @@
         <v>312</v>
       </c>
       <c r="J10">
-        <v>11</v>
+        <v>13</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -20389,7 +20395,7 @@
         <v>493</v>
       </c>
       <c r="J11">
-        <v>28</v>
+        <v>30</v>
       </c>
     </row>
   </sheetData>
@@ -20658,7 +20664,7 @@
         <v>178</v>
       </c>
       <c r="J8">
-        <v>11</v>
+        <v>15</v>
       </c>
     </row>
     <row r="9" spans="1:10">
@@ -20754,7 +20760,7 @@
         <v>793</v>
       </c>
       <c r="J11">
-        <v>42</v>
+        <v>46</v>
       </c>
     </row>
   </sheetData>
@@ -21055,7 +21061,7 @@
         <v>35</v>
       </c>
       <c r="J9">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="10" spans="1:10">
@@ -21119,7 +21125,7 @@
         <v>438</v>
       </c>
       <c r="J11">
-        <v>30</v>
+        <v>31</v>
       </c>
     </row>
   </sheetData>
@@ -21394,7 +21400,7 @@
         <v>503</v>
       </c>
       <c r="J8">
-        <v>47</v>
+        <v>48</v>
       </c>
     </row>
     <row r="9" spans="1:10">
@@ -21490,7 +21496,7 @@
         <v>1493</v>
       </c>
       <c r="J11">
-        <v>97</v>
+        <v>98</v>
       </c>
     </row>
   </sheetData>
@@ -22109,7 +22115,7 @@
         <v>90</v>
       </c>
       <c r="J9">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="10" spans="1:10">
@@ -22141,7 +22147,7 @@
         <v>542</v>
       </c>
       <c r="J10">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -22173,7 +22179,7 @@
         <v>949</v>
       </c>
       <c r="J11">
-        <v>51</v>
+        <v>53</v>
       </c>
     </row>
   </sheetData>
@@ -22418,7 +22424,7 @@
         <v>160</v>
       </c>
       <c r="J8">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="9" spans="1:10">
@@ -22482,7 +22488,7 @@
         <v>717</v>
       </c>
       <c r="J10">
-        <v>27</v>
+        <v>29</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -22514,7 +22520,7 @@
         <v>1066</v>
       </c>
       <c r="J11">
-        <v>39</v>
+        <v>42</v>
       </c>
     </row>
   </sheetData>
@@ -22789,7 +22795,7 @@
         <v>197</v>
       </c>
       <c r="J8">
-        <v>21</v>
+        <v>23</v>
       </c>
     </row>
     <row r="9" spans="1:10">
@@ -22853,7 +22859,7 @@
         <v>1118</v>
       </c>
       <c r="J10">
-        <v>44</v>
+        <v>46</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -22885,7 +22891,7 @@
         <v>1797</v>
       </c>
       <c r="J11">
-        <v>90</v>
+        <v>94</v>
       </c>
     </row>
   </sheetData>
@@ -23209,7 +23215,7 @@
         <v>255</v>
       </c>
       <c r="J10">
-        <v>11</v>
+        <v>14</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -23241,7 +23247,7 @@
         <v>438</v>
       </c>
       <c r="J11">
-        <v>18</v>
+        <v>21</v>
       </c>
     </row>
   </sheetData>
@@ -23545,7 +23551,7 @@
         <v>113</v>
       </c>
       <c r="J9">
-        <v>6</v>
+        <v>9</v>
       </c>
     </row>
     <row r="10" spans="1:10">
@@ -23577,7 +23583,7 @@
         <v>389</v>
       </c>
       <c r="J10">
-        <v>15</v>
+        <v>16</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -23609,7 +23615,7 @@
         <v>886</v>
       </c>
       <c r="J11">
-        <v>55</v>
+        <v>59</v>
       </c>
     </row>
   </sheetData>
@@ -23791,7 +23797,7 @@
         <v>59</v>
       </c>
       <c r="J5">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="6" spans="1:10">
@@ -23971,7 +23977,7 @@
         <v>501</v>
       </c>
       <c r="J11">
-        <v>40</v>
+        <v>41</v>
       </c>
     </row>
   </sheetData>
@@ -24156,7 +24162,7 @@
         <v>82</v>
       </c>
       <c r="J5">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="6" spans="1:10">
@@ -24281,7 +24287,7 @@
         <v>193</v>
       </c>
       <c r="J9">
-        <v>16</v>
+        <v>19</v>
       </c>
     </row>
     <row r="10" spans="1:10">
@@ -24313,7 +24319,7 @@
         <v>591</v>
       </c>
       <c r="J10">
-        <v>34</v>
+        <v>38</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -24345,7 +24351,7 @@
         <v>1494</v>
       </c>
       <c r="J11">
-        <v>91</v>
+        <v>99</v>
       </c>
     </row>
   </sheetData>
@@ -24466,7 +24472,7 @@
         <v>89</v>
       </c>
       <c r="J3">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="4" spans="1:10">
@@ -24614,7 +24620,7 @@
         <v>406</v>
       </c>
       <c r="J8">
-        <v>52</v>
+        <v>53</v>
       </c>
     </row>
     <row r="9" spans="1:10">
@@ -24678,7 +24684,7 @@
         <v>670</v>
       </c>
       <c r="J10">
-        <v>39</v>
+        <v>40</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -24710,7 +24716,7 @@
         <v>1369</v>
       </c>
       <c r="J11">
-        <v>105</v>
+        <v>108</v>
       </c>
     </row>
   </sheetData>
@@ -24831,7 +24837,7 @@
         <v>177</v>
       </c>
       <c r="J3">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="4" spans="1:10">
@@ -24988,7 +24994,7 @@
         <v>365</v>
       </c>
       <c r="J8">
-        <v>26</v>
+        <v>27</v>
       </c>
     </row>
     <row r="9" spans="1:10">
@@ -25020,7 +25026,7 @@
         <v>224</v>
       </c>
       <c r="J9">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="10" spans="1:10">
@@ -25084,7 +25090,7 @@
         <v>2048</v>
       </c>
       <c r="J11">
-        <v>93</v>
+        <v>96</v>
       </c>
     </row>
   </sheetData>
@@ -25173,7 +25179,7 @@
         <v>64</v>
       </c>
       <c r="J2">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="3" spans="1:10">
@@ -25295,7 +25301,7 @@
         <v>27</v>
       </c>
       <c r="J6">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="7" spans="1:10">
@@ -25356,7 +25362,7 @@
         <v>297</v>
       </c>
       <c r="J8">
-        <v>48</v>
+        <v>50</v>
       </c>
     </row>
     <row r="9" spans="1:10">
@@ -25420,7 +25426,7 @@
         <v>670</v>
       </c>
       <c r="J10">
-        <v>28</v>
+        <v>30</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -25452,7 +25458,7 @@
         <v>1337</v>
       </c>
       <c r="J11">
-        <v>94</v>
+        <v>100</v>
       </c>
     </row>
   </sheetData>
@@ -25794,7 +25800,7 @@
         <v>318</v>
       </c>
       <c r="J10">
-        <v>17</v>
+        <v>19</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -25826,7 +25832,7 @@
         <v>971</v>
       </c>
       <c r="J11">
-        <v>78</v>
+        <v>80</v>
       </c>
     </row>
   </sheetData>
@@ -26126,7 +26132,7 @@
         <v>174</v>
       </c>
       <c r="J10">
-        <v>6</v>
+        <v>8</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -26158,7 +26164,7 @@
         <v>337</v>
       </c>
       <c r="J11">
-        <v>13</v>
+        <v>15</v>
       </c>
     </row>
   </sheetData>
@@ -26424,7 +26430,7 @@
         <v>250</v>
       </c>
       <c r="J8">
-        <v>24</v>
+        <v>25</v>
       </c>
     </row>
     <row r="9" spans="1:10">
@@ -26456,7 +26462,7 @@
         <v>61</v>
       </c>
       <c r="J9">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="10" spans="1:10">
@@ -26520,7 +26526,7 @@
         <v>904</v>
       </c>
       <c r="J11">
-        <v>69</v>
+        <v>71</v>
       </c>
     </row>
   </sheetData>
@@ -26609,7 +26615,7 @@
         <v>106</v>
       </c>
       <c r="J2">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="3" spans="1:10">
@@ -26792,7 +26798,7 @@
         <v>441</v>
       </c>
       <c r="J8">
-        <v>44</v>
+        <v>46</v>
       </c>
     </row>
     <row r="9" spans="1:10">
@@ -26888,7 +26894,7 @@
         <v>1356</v>
       </c>
       <c r="J11">
-        <v>93</v>
+        <v>96</v>
       </c>
     </row>
   </sheetData>
@@ -27064,7 +27070,7 @@
         <v>93</v>
       </c>
       <c r="J5">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="6" spans="1:10">
@@ -27250,7 +27256,7 @@
         <v>962</v>
       </c>
       <c r="J11">
-        <v>79</v>
+        <v>80</v>
       </c>
     </row>
   </sheetData>
@@ -27399,6 +27405,9 @@
       <c r="I4">
         <v>3</v>
       </c>
+      <c r="J4">
+        <v>1</v>
+      </c>
     </row>
     <row r="5" spans="1:10">
       <c r="A5" s="1" t="s">
@@ -27429,7 +27438,7 @@
         <v>64</v>
       </c>
       <c r="J5">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="6" spans="1:10">
@@ -27577,7 +27586,7 @@
         <v>381</v>
       </c>
       <c r="J10">
-        <v>18</v>
+        <v>21</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -27609,7 +27618,7 @@
         <v>720</v>
       </c>
       <c r="J11">
-        <v>39</v>
+        <v>44</v>
       </c>
     </row>
   </sheetData>
@@ -28228,6 +28237,9 @@
       <c r="I7">
         <v>9</v>
       </c>
+      <c r="J7">
+        <v>1</v>
+      </c>
     </row>
     <row r="8" spans="1:10">
       <c r="A8" s="1" t="s">
@@ -28258,7 +28270,7 @@
         <v>373</v>
       </c>
       <c r="J8">
-        <v>41</v>
+        <v>43</v>
       </c>
     </row>
     <row r="9" spans="1:10">
@@ -28290,7 +28302,7 @@
         <v>111</v>
       </c>
       <c r="J9">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="10" spans="1:10">
@@ -28322,7 +28334,7 @@
         <v>818</v>
       </c>
       <c r="J10">
-        <v>52</v>
+        <v>57</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -28354,7 +28366,7 @@
         <v>1711</v>
       </c>
       <c r="J11">
-        <v>122</v>
+        <v>131</v>
       </c>
     </row>
   </sheetData>
@@ -28629,7 +28641,7 @@
         <v>132</v>
       </c>
       <c r="J8">
-        <v>14</v>
+        <v>15</v>
       </c>
     </row>
     <row r="9" spans="1:10">
@@ -28725,7 +28737,7 @@
         <v>462</v>
       </c>
       <c r="J11">
-        <v>37</v>
+        <v>38</v>
       </c>
     </row>
   </sheetData>
@@ -29016,7 +29028,7 @@
         <v>576</v>
       </c>
       <c r="J10">
-        <v>28</v>
+        <v>30</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -29048,7 +29060,7 @@
         <v>629</v>
       </c>
       <c r="J11">
-        <v>31</v>
+        <v>33</v>
       </c>
     </row>
   </sheetData>
@@ -29481,7 +29493,7 @@
         <v>80</v>
       </c>
       <c r="J2">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="3" spans="1:10">
@@ -29731,7 +29743,7 @@
         <v>493</v>
       </c>
       <c r="J10">
-        <v>28</v>
+        <v>29</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -29763,7 +29775,7 @@
         <v>918</v>
       </c>
       <c r="J11">
-        <v>52</v>
+        <v>54</v>
       </c>
     </row>
   </sheetData>
@@ -29942,7 +29954,7 @@
         <v>64</v>
       </c>
       <c r="J5">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="6" spans="1:10">
@@ -30026,7 +30038,7 @@
         <v>90</v>
       </c>
       <c r="J8">
-        <v>4</v>
+        <v>6</v>
       </c>
     </row>
     <row r="9" spans="1:10">
@@ -30122,7 +30134,7 @@
         <v>708</v>
       </c>
       <c r="J11">
-        <v>27</v>
+        <v>30</v>
       </c>
     </row>
   </sheetData>
@@ -30376,7 +30388,7 @@
         <v>227</v>
       </c>
       <c r="J8">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="9" spans="1:10">
@@ -30440,7 +30452,7 @@
         <v>650</v>
       </c>
       <c r="J10">
-        <v>33</v>
+        <v>35</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -30472,7 +30484,7 @@
         <v>1153</v>
       </c>
       <c r="J11">
-        <v>83</v>
+        <v>86</v>
       </c>
     </row>
   </sheetData>
@@ -30590,7 +30602,7 @@
         <v>17</v>
       </c>
       <c r="J3">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="4" spans="1:10">
@@ -30813,7 +30825,7 @@
         <v>175</v>
       </c>
       <c r="J11">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
   </sheetData>
@@ -31076,7 +31088,7 @@
         <v>73</v>
       </c>
       <c r="J8">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="9" spans="1:10">
@@ -31172,7 +31184,7 @@
         <v>436</v>
       </c>
       <c r="J11">
-        <v>30</v>
+        <v>31</v>
       </c>
     </row>
   </sheetData>
@@ -31446,7 +31458,7 @@
         <v>47</v>
       </c>
       <c r="J9">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="10" spans="1:10">
@@ -31510,7 +31522,7 @@
         <v>393</v>
       </c>
       <c r="J11">
-        <v>17</v>
+        <v>18</v>
       </c>
     </row>
   </sheetData>
@@ -31782,7 +31794,7 @@
         <v>140</v>
       </c>
       <c r="J8">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="9" spans="1:10">
@@ -31878,7 +31890,7 @@
         <v>764</v>
       </c>
       <c r="J11">
-        <v>52</v>
+        <v>53</v>
       </c>
     </row>
   </sheetData>
@@ -31967,7 +31979,7 @@
         <v>457</v>
       </c>
       <c r="J2">
-        <v>27</v>
+        <v>29</v>
       </c>
     </row>
     <row r="3" spans="1:10">
@@ -31999,7 +32011,7 @@
         <v>448</v>
       </c>
       <c r="J3">
-        <v>32</v>
+        <v>34</v>
       </c>
     </row>
     <row r="4" spans="1:10">
@@ -32159,7 +32171,7 @@
         <v>1272</v>
       </c>
       <c r="J8">
-        <v>86</v>
+        <v>88</v>
       </c>
     </row>
     <row r="9" spans="1:10">
@@ -32191,7 +32203,7 @@
         <v>496</v>
       </c>
       <c r="J9">
-        <v>26</v>
+        <v>30</v>
       </c>
     </row>
     <row r="10" spans="1:10">
@@ -32223,7 +32235,7 @@
         <v>1653</v>
       </c>
       <c r="J10">
-        <v>70</v>
+        <v>77</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -32255,7 +32267,7 @@
         <v>4749</v>
       </c>
       <c r="J11">
-        <v>263</v>
+        <v>280</v>
       </c>
     </row>
   </sheetData>
@@ -32842,6 +32854,9 @@
       <c r="I9">
         <v>12</v>
       </c>
+      <c r="J9">
+        <v>1</v>
+      </c>
     </row>
     <row r="10" spans="1:10">
       <c r="A10" s="1" t="s">
@@ -32904,7 +32919,7 @@
         <v>209</v>
       </c>
       <c r="J11">
-        <v>12</v>
+        <v>13</v>
       </c>
     </row>
   </sheetData>
@@ -33395,7 +33410,7 @@
         <v>77</v>
       </c>
       <c r="J5">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="6" spans="1:10">
@@ -33479,7 +33494,7 @@
         <v>131</v>
       </c>
       <c r="J8">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="9" spans="1:10">
@@ -33511,7 +33526,7 @@
         <v>122</v>
       </c>
       <c r="J9">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="10" spans="1:10">
@@ -33543,7 +33558,7 @@
         <v>921</v>
       </c>
       <c r="J10">
-        <v>28</v>
+        <v>29</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -33575,7 +33590,7 @@
         <v>1320</v>
       </c>
       <c r="J11">
-        <v>52</v>
+        <v>56</v>
       </c>
     </row>
   </sheetData>
@@ -34098,7 +34113,7 @@
         <v>27</v>
       </c>
       <c r="J8">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="9" spans="1:10">
@@ -34162,7 +34177,7 @@
         <v>152</v>
       </c>
       <c r="J10">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -34194,7 +34209,7 @@
         <v>248</v>
       </c>
       <c r="J11">
-        <v>16</v>
+        <v>18</v>
       </c>
     </row>
   </sheetData>
@@ -34463,7 +34478,7 @@
         <v>68</v>
       </c>
       <c r="J8">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="9" spans="1:10">
@@ -34524,7 +34539,7 @@
         <v>157</v>
       </c>
       <c r="J10">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -34556,7 +34571,7 @@
         <v>337</v>
       </c>
       <c r="J11">
-        <v>21</v>
+        <v>23</v>
       </c>
     </row>
   </sheetData>
@@ -34847,7 +34862,7 @@
         <v>101</v>
       </c>
       <c r="J10">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -34879,7 +34894,7 @@
         <v>160</v>
       </c>
       <c r="J11">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
   </sheetData>
@@ -35165,7 +35180,7 @@
         <v>139</v>
       </c>
       <c r="J9">
-        <v>8</v>
+        <v>10</v>
       </c>
     </row>
     <row r="10" spans="1:10">
@@ -35197,7 +35212,7 @@
         <v>233</v>
       </c>
       <c r="J10">
-        <v>18</v>
+        <v>20</v>
       </c>
     </row>
   </sheetData>
@@ -35834,7 +35849,7 @@
         <v>260</v>
       </c>
       <c r="J8">
-        <v>39</v>
+        <v>42</v>
       </c>
     </row>
     <row r="9" spans="1:10">
@@ -35866,7 +35881,7 @@
         <v>151</v>
       </c>
       <c r="J9">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="10" spans="1:10">
@@ -35898,7 +35913,7 @@
         <v>914</v>
       </c>
       <c r="J10">
-        <v>41</v>
+        <v>45</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -35930,7 +35945,7 @@
         <v>1603</v>
       </c>
       <c r="J11">
-        <v>100</v>
+        <v>108</v>
       </c>
     </row>
   </sheetData>
@@ -36540,7 +36555,7 @@
         <v>116</v>
       </c>
       <c r="J8">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="9" spans="1:10">
@@ -36572,7 +36587,7 @@
         <v>153</v>
       </c>
       <c r="J9">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
   </sheetData>
@@ -36864,7 +36879,7 @@
         <v>27</v>
       </c>
       <c r="J9">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="10" spans="1:10">
@@ -36896,7 +36911,7 @@
         <v>211</v>
       </c>
       <c r="J10">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -36928,7 +36943,7 @@
         <v>408</v>
       </c>
       <c r="J11">
-        <v>32</v>
+        <v>34</v>
       </c>
     </row>
   </sheetData>
@@ -37049,7 +37064,7 @@
         <v>78</v>
       </c>
       <c r="J3">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="4" spans="1:10">
@@ -37200,7 +37215,7 @@
         <v>184</v>
       </c>
       <c r="J8">
-        <v>25</v>
+        <v>28</v>
       </c>
     </row>
     <row r="9" spans="1:10">
@@ -37232,7 +37247,7 @@
         <v>81</v>
       </c>
       <c r="J9">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="10" spans="1:10">
@@ -37264,7 +37279,7 @@
         <v>474</v>
       </c>
       <c r="J10">
-        <v>31</v>
+        <v>33</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -37296,7 +37311,7 @@
         <v>944</v>
       </c>
       <c r="J11">
-        <v>74</v>
+        <v>81</v>
       </c>
     </row>
   </sheetData>
@@ -37517,7 +37532,7 @@
         <v>32</v>
       </c>
       <c r="J8">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="9" spans="1:10">
@@ -37610,7 +37625,7 @@
         <v>307</v>
       </c>
       <c r="J11">
-        <v>16</v>
+        <v>17</v>
       </c>
     </row>
   </sheetData>
@@ -37875,7 +37890,7 @@
         <v>107</v>
       </c>
       <c r="J9">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="10" spans="1:10">
@@ -37907,7 +37922,7 @@
         <v>155</v>
       </c>
       <c r="J10">
-        <v>14</v>
+        <v>15</v>
       </c>
     </row>
   </sheetData>
@@ -38068,7 +38083,7 @@
         <v>39</v>
       </c>
       <c r="J5">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="6" spans="1:10">
@@ -38219,7 +38234,7 @@
         <v>218</v>
       </c>
       <c r="J10">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
   </sheetData>
@@ -38475,7 +38490,7 @@
         <v>155</v>
       </c>
       <c r="J9">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="10" spans="1:10">
@@ -38507,7 +38522,7 @@
         <v>191</v>
       </c>
       <c r="J10">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
   </sheetData>
@@ -38755,7 +38770,7 @@
         <v>89</v>
       </c>
       <c r="J8">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="9" spans="1:10">
@@ -38819,7 +38834,7 @@
         <v>207</v>
       </c>
       <c r="J10">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -38851,7 +38866,7 @@
         <v>413</v>
       </c>
       <c r="J11">
-        <v>31</v>
+        <v>33</v>
       </c>
     </row>
   </sheetData>
@@ -38968,6 +38983,9 @@
       <c r="I3">
         <v>7</v>
       </c>
+      <c r="J3">
+        <v>1</v>
+      </c>
     </row>
     <row r="4" spans="1:10">
       <c r="A4" s="1" t="s">
@@ -39168,7 +39186,7 @@
         <v>99</v>
       </c>
       <c r="J11">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add data for 2023-01-22
</commit_message>
<xml_diff>
--- a/output/index-crime-full-year.xlsx
+++ b/output/index-crime-full-year.xlsx
@@ -895,7 +895,7 @@
         <v>7270</v>
       </c>
       <c r="J2">
-        <v>381</v>
+        <v>394</v>
       </c>
     </row>
     <row r="3" spans="1:10">
@@ -927,7 +927,7 @@
         <v>7487</v>
       </c>
       <c r="J3">
-        <v>436</v>
+        <v>468</v>
       </c>
     </row>
     <row r="4" spans="1:10">
@@ -956,10 +956,10 @@
         <v>527</v>
       </c>
       <c r="I4">
-        <v>423</v>
+        <v>424</v>
       </c>
       <c r="J4">
-        <v>31</v>
+        <v>32</v>
       </c>
     </row>
     <row r="5" spans="1:10">
@@ -988,10 +988,10 @@
         <v>6658</v>
       </c>
       <c r="I5">
-        <v>7578</v>
+        <v>7579</v>
       </c>
       <c r="J5">
-        <v>444</v>
+        <v>454</v>
       </c>
     </row>
     <row r="6" spans="1:10">
@@ -999,7 +999,7 @@
         <v>5</v>
       </c>
       <c r="B6">
-        <v>1669</v>
+        <v>1670</v>
       </c>
       <c r="C6">
         <v>1816</v>
@@ -1020,10 +1020,10 @@
         <v>1685</v>
       </c>
       <c r="I6">
-        <v>1736</v>
+        <v>1737</v>
       </c>
       <c r="J6">
-        <v>78</v>
+        <v>83</v>
       </c>
     </row>
     <row r="7" spans="1:10">
@@ -1055,7 +1055,7 @@
         <v>710</v>
       </c>
       <c r="J7">
-        <v>31</v>
+        <v>34</v>
       </c>
     </row>
     <row r="8" spans="1:10">
@@ -1084,10 +1084,10 @@
         <v>10596</v>
       </c>
       <c r="I8">
-        <v>21389</v>
+        <v>21390</v>
       </c>
       <c r="J8">
-        <v>2032</v>
+        <v>2109</v>
       </c>
     </row>
     <row r="9" spans="1:10">
@@ -1116,10 +1116,10 @@
         <v>7919</v>
       </c>
       <c r="I9">
-        <v>8965</v>
+        <v>8966</v>
       </c>
       <c r="J9">
-        <v>623</v>
+        <v>647</v>
       </c>
     </row>
     <row r="10" spans="1:10">
@@ -1139,7 +1139,7 @@
         <v>65285</v>
       </c>
       <c r="F10">
-        <v>62485</v>
+        <v>62484</v>
       </c>
       <c r="G10">
         <v>41311</v>
@@ -1148,10 +1148,10 @@
         <v>40774</v>
       </c>
       <c r="I10">
-        <v>54541</v>
+        <v>54544</v>
       </c>
       <c r="J10">
-        <v>2769</v>
+        <v>2875</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -1159,7 +1159,7 @@
         <v>10</v>
       </c>
       <c r="B11">
-        <v>104351</v>
+        <v>104352</v>
       </c>
       <c r="C11">
         <v>116067</v>
@@ -1171,7 +1171,7 @@
         <v>113366</v>
       </c>
       <c r="F11">
-        <v>105543</v>
+        <v>105542</v>
       </c>
       <c r="G11">
         <v>85286</v>
@@ -1180,10 +1180,10 @@
         <v>84551</v>
       </c>
       <c r="I11">
-        <v>110099</v>
+        <v>110107</v>
       </c>
       <c r="J11">
-        <v>6825</v>
+        <v>7096</v>
       </c>
     </row>
   </sheetData>
@@ -1304,7 +1304,7 @@
         <v>248</v>
       </c>
       <c r="J3">
-        <v>18</v>
+        <v>20</v>
       </c>
     </row>
     <row r="4" spans="1:10">
@@ -1431,6 +1431,9 @@
       <c r="I7">
         <v>36</v>
       </c>
+      <c r="J7">
+        <v>1</v>
+      </c>
     </row>
     <row r="8" spans="1:10">
       <c r="A8" s="1" t="s">
@@ -1461,7 +1464,7 @@
         <v>567</v>
       </c>
       <c r="J8">
-        <v>53</v>
+        <v>55</v>
       </c>
     </row>
     <row r="9" spans="1:10">
@@ -1525,7 +1528,7 @@
         <v>1023</v>
       </c>
       <c r="J10">
-        <v>52</v>
+        <v>54</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -1557,7 +1560,7 @@
         <v>2687</v>
       </c>
       <c r="J11">
-        <v>179</v>
+        <v>186</v>
       </c>
     </row>
   </sheetData>
@@ -2001,7 +2004,7 @@
         <v>161</v>
       </c>
       <c r="J5">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="6" spans="1:10">
@@ -2097,7 +2100,7 @@
         <v>292</v>
       </c>
       <c r="J8">
-        <v>18</v>
+        <v>19</v>
       </c>
     </row>
     <row r="9" spans="1:10">
@@ -2161,7 +2164,7 @@
         <v>904</v>
       </c>
       <c r="J10">
-        <v>43</v>
+        <v>46</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -2193,7 +2196,7 @@
         <v>1670</v>
       </c>
       <c r="J11">
-        <v>87</v>
+        <v>92</v>
       </c>
     </row>
   </sheetData>
@@ -2432,7 +2435,7 @@
         <v>112</v>
       </c>
       <c r="J8">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="9" spans="1:10">
@@ -2496,7 +2499,7 @@
         <v>502</v>
       </c>
       <c r="J10">
-        <v>28</v>
+        <v>30</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -2528,7 +2531,7 @@
         <v>677</v>
       </c>
       <c r="J11">
-        <v>39</v>
+        <v>42</v>
       </c>
     </row>
   </sheetData>
@@ -2794,7 +2797,7 @@
         <v>109</v>
       </c>
       <c r="J8">
-        <v>12</v>
+        <v>13</v>
       </c>
     </row>
     <row r="9" spans="1:10">
@@ -2890,7 +2893,7 @@
         <v>718</v>
       </c>
       <c r="J11">
-        <v>40</v>
+        <v>41</v>
       </c>
     </row>
   </sheetData>
@@ -3223,7 +3226,7 @@
         <v>105</v>
       </c>
       <c r="J10">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -3255,7 +3258,7 @@
         <v>261</v>
       </c>
       <c r="J11">
-        <v>24</v>
+        <v>25</v>
       </c>
     </row>
   </sheetData>
@@ -3376,7 +3379,7 @@
         <v>261</v>
       </c>
       <c r="J3">
-        <v>17</v>
+        <v>20</v>
       </c>
     </row>
     <row r="4" spans="1:10">
@@ -3469,7 +3472,7 @@
         <v>39</v>
       </c>
       <c r="J6">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="7" spans="1:10">
@@ -3533,7 +3536,7 @@
         <v>722</v>
       </c>
       <c r="J8">
-        <v>61</v>
+        <v>65</v>
       </c>
     </row>
     <row r="9" spans="1:10">
@@ -3597,7 +3600,7 @@
         <v>812</v>
       </c>
       <c r="J10">
-        <v>36</v>
+        <v>40</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -3629,7 +3632,7 @@
         <v>2548</v>
       </c>
       <c r="J11">
-        <v>156</v>
+        <v>168</v>
       </c>
     </row>
   </sheetData>
@@ -3718,7 +3721,7 @@
         <v>128</v>
       </c>
       <c r="J2">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="3" spans="1:10">
@@ -3750,7 +3753,7 @@
         <v>157</v>
       </c>
       <c r="J3">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="4" spans="1:10">
@@ -3907,7 +3910,7 @@
         <v>384</v>
       </c>
       <c r="J8">
-        <v>59</v>
+        <v>60</v>
       </c>
     </row>
     <row r="9" spans="1:10">
@@ -3971,7 +3974,7 @@
         <v>527</v>
       </c>
       <c r="J10">
-        <v>30</v>
+        <v>31</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -4003,7 +4006,7 @@
         <v>1489</v>
       </c>
       <c r="J11">
-        <v>121</v>
+        <v>125</v>
       </c>
     </row>
   </sheetData>
@@ -4124,7 +4127,7 @@
         <v>364</v>
       </c>
       <c r="J3">
-        <v>29</v>
+        <v>31</v>
       </c>
     </row>
     <row r="4" spans="1:10">
@@ -4281,7 +4284,7 @@
         <v>516</v>
       </c>
       <c r="J8">
-        <v>36</v>
+        <v>41</v>
       </c>
     </row>
     <row r="9" spans="1:10">
@@ -4345,7 +4348,7 @@
         <v>897</v>
       </c>
       <c r="J10">
-        <v>35</v>
+        <v>37</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -4377,7 +4380,7 @@
         <v>2512</v>
       </c>
       <c r="J11">
-        <v>141</v>
+        <v>150</v>
       </c>
     </row>
   </sheetData>
@@ -4466,7 +4469,7 @@
         <v>78</v>
       </c>
       <c r="J2">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="3" spans="1:10">
@@ -4652,7 +4655,7 @@
         <v>152</v>
       </c>
       <c r="J8">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="9" spans="1:10">
@@ -4683,6 +4686,9 @@
       <c r="I9">
         <v>100</v>
       </c>
+      <c r="J9">
+        <v>1</v>
+      </c>
     </row>
     <row r="10" spans="1:10">
       <c r="A10" s="1" t="s">
@@ -4713,7 +4719,7 @@
         <v>381</v>
       </c>
       <c r="J10">
-        <v>21</v>
+        <v>22</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -4745,7 +4751,7 @@
         <v>866</v>
       </c>
       <c r="J11">
-        <v>48</v>
+        <v>52</v>
       </c>
     </row>
   </sheetData>
@@ -4834,7 +4840,7 @@
         <v>83</v>
       </c>
       <c r="J2">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="3" spans="1:10">
@@ -5017,7 +5023,7 @@
         <v>190</v>
       </c>
       <c r="J8">
-        <v>20</v>
+        <v>22</v>
       </c>
     </row>
     <row r="9" spans="1:10">
@@ -5049,7 +5055,7 @@
         <v>55</v>
       </c>
       <c r="J9">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="10" spans="1:10">
@@ -5081,7 +5087,7 @@
         <v>271</v>
       </c>
       <c r="J10">
-        <v>15</v>
+        <v>16</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -5113,7 +5119,7 @@
         <v>729</v>
       </c>
       <c r="J11">
-        <v>50</v>
+        <v>55</v>
       </c>
     </row>
   </sheetData>
@@ -5202,7 +5208,7 @@
         <v>918</v>
       </c>
       <c r="J2">
-        <v>54</v>
+        <v>57</v>
       </c>
     </row>
     <row r="3" spans="1:10">
@@ -5298,7 +5304,7 @@
         <v>248</v>
       </c>
       <c r="J5">
-        <v>19</v>
+        <v>21</v>
       </c>
     </row>
     <row r="6" spans="1:10">
@@ -5330,7 +5336,7 @@
         <v>793</v>
       </c>
       <c r="J6">
-        <v>46</v>
+        <v>50</v>
       </c>
     </row>
     <row r="7" spans="1:10">
@@ -5362,7 +5368,7 @@
         <v>2687</v>
       </c>
       <c r="J7">
-        <v>179</v>
+        <v>186</v>
       </c>
     </row>
     <row r="8" spans="1:10">
@@ -5394,7 +5400,7 @@
         <v>4749</v>
       </c>
       <c r="J8">
-        <v>280</v>
+        <v>304</v>
       </c>
     </row>
     <row r="9" spans="1:10">
@@ -5458,7 +5464,7 @@
         <v>949</v>
       </c>
       <c r="J10">
-        <v>53</v>
+        <v>57</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -5490,7 +5496,7 @@
         <v>1711</v>
       </c>
       <c r="J11">
-        <v>131</v>
+        <v>136</v>
       </c>
     </row>
     <row r="12" spans="1:10">
@@ -5522,7 +5528,7 @@
         <v>413</v>
       </c>
       <c r="J12">
-        <v>33</v>
+        <v>34</v>
       </c>
     </row>
     <row r="13" spans="1:10">
@@ -5554,7 +5560,7 @@
         <v>260</v>
       </c>
       <c r="J13">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="14" spans="1:10">
@@ -5586,7 +5592,7 @@
         <v>718</v>
       </c>
       <c r="J14">
-        <v>40</v>
+        <v>41</v>
       </c>
     </row>
     <row r="15" spans="1:10">
@@ -5618,7 +5624,7 @@
         <v>886</v>
       </c>
       <c r="J15">
-        <v>59</v>
+        <v>62</v>
       </c>
     </row>
     <row r="16" spans="1:10">
@@ -5714,7 +5720,7 @@
         <v>696</v>
       </c>
       <c r="J18">
-        <v>56</v>
+        <v>59</v>
       </c>
     </row>
     <row r="19" spans="1:10">
@@ -5746,7 +5752,7 @@
         <v>2636</v>
       </c>
       <c r="J19">
-        <v>183</v>
+        <v>197</v>
       </c>
     </row>
     <row r="20" spans="1:10">
@@ -5778,7 +5784,7 @@
         <v>2048</v>
       </c>
       <c r="J20">
-        <v>96</v>
+        <v>101</v>
       </c>
     </row>
     <row r="21" spans="1:10">
@@ -5842,7 +5848,7 @@
         <v>419</v>
       </c>
       <c r="J22">
-        <v>27</v>
+        <v>28</v>
       </c>
     </row>
     <row r="23" spans="1:10">
@@ -5874,7 +5880,7 @@
         <v>1369</v>
       </c>
       <c r="J23">
-        <v>108</v>
+        <v>111</v>
       </c>
     </row>
     <row r="24" spans="1:10">
@@ -5938,7 +5944,7 @@
         <v>431</v>
       </c>
       <c r="J25">
-        <v>22</v>
+        <v>23</v>
       </c>
     </row>
     <row r="26" spans="1:10">
@@ -6002,7 +6008,7 @@
         <v>1259</v>
       </c>
       <c r="J27">
-        <v>82</v>
+        <v>85</v>
       </c>
     </row>
     <row r="28" spans="1:10">
@@ -6034,7 +6040,7 @@
         <v>99</v>
       </c>
       <c r="J28">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="29" spans="1:10">
@@ -6066,7 +6072,7 @@
         <v>3951</v>
       </c>
       <c r="J29">
-        <v>283</v>
+        <v>291</v>
       </c>
     </row>
     <row r="30" spans="1:10">
@@ -6098,7 +6104,7 @@
         <v>261</v>
       </c>
       <c r="J30">
-        <v>24</v>
+        <v>25</v>
       </c>
     </row>
     <row r="31" spans="1:10">
@@ -6130,7 +6136,7 @@
         <v>866</v>
       </c>
       <c r="J31">
-        <v>48</v>
+        <v>52</v>
       </c>
     </row>
     <row r="32" spans="1:10">
@@ -6162,7 +6168,7 @@
         <v>209</v>
       </c>
       <c r="J32">
-        <v>13</v>
+        <v>17</v>
       </c>
     </row>
     <row r="33" spans="1:10">
@@ -6194,7 +6200,7 @@
         <v>3016</v>
       </c>
       <c r="J33">
-        <v>174</v>
+        <v>182</v>
       </c>
     </row>
     <row r="34" spans="1:10">
@@ -6226,7 +6232,7 @@
         <v>764</v>
       </c>
       <c r="J34">
-        <v>53</v>
+        <v>56</v>
       </c>
     </row>
     <row r="35" spans="1:10">
@@ -6290,7 +6296,7 @@
         <v>1493</v>
       </c>
       <c r="J36">
-        <v>98</v>
+        <v>100</v>
       </c>
     </row>
     <row r="37" spans="1:10">
@@ -6322,7 +6328,7 @@
         <v>2548</v>
       </c>
       <c r="J37">
-        <v>156</v>
+        <v>168</v>
       </c>
     </row>
     <row r="38" spans="1:10">
@@ -6386,7 +6392,7 @@
         <v>153</v>
       </c>
       <c r="J39">
-        <v>7</v>
+        <v>9</v>
       </c>
     </row>
     <row r="40" spans="1:10">
@@ -6418,7 +6424,7 @@
         <v>236</v>
       </c>
       <c r="J40">
-        <v>17</v>
+        <v>18</v>
       </c>
     </row>
     <row r="41" spans="1:10">
@@ -6450,7 +6456,7 @@
         <v>438</v>
       </c>
       <c r="J41">
-        <v>31</v>
+        <v>33</v>
       </c>
     </row>
     <row r="42" spans="1:10">
@@ -6479,10 +6485,10 @@
         <v>2423</v>
       </c>
       <c r="I42">
-        <v>2956</v>
+        <v>2957</v>
       </c>
       <c r="J42">
-        <v>179</v>
+        <v>186</v>
       </c>
     </row>
     <row r="43" spans="1:10">
@@ -6514,7 +6520,7 @@
         <v>1153</v>
       </c>
       <c r="J43">
-        <v>86</v>
+        <v>88</v>
       </c>
     </row>
     <row r="44" spans="1:10">
@@ -6546,7 +6552,7 @@
         <v>1229</v>
       </c>
       <c r="J44">
-        <v>84</v>
+        <v>85</v>
       </c>
     </row>
     <row r="45" spans="1:10">
@@ -6610,7 +6616,7 @@
         <v>433</v>
       </c>
       <c r="J46">
-        <v>23</v>
+        <v>25</v>
       </c>
     </row>
     <row r="47" spans="1:10">
@@ -6642,7 +6648,7 @@
         <v>904</v>
       </c>
       <c r="J47">
-        <v>71</v>
+        <v>73</v>
       </c>
     </row>
     <row r="48" spans="1:10">
@@ -6674,7 +6680,7 @@
         <v>2621</v>
       </c>
       <c r="J48">
-        <v>139</v>
+        <v>145</v>
       </c>
     </row>
     <row r="49" spans="1:10">
@@ -6706,7 +6712,7 @@
         <v>1647</v>
       </c>
       <c r="J49">
-        <v>95</v>
+        <v>97</v>
       </c>
     </row>
     <row r="50" spans="1:10">
@@ -6738,7 +6744,7 @@
         <v>962</v>
       </c>
       <c r="J50">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="51" spans="1:10">
@@ -6770,7 +6776,7 @@
         <v>1337</v>
       </c>
       <c r="J51">
-        <v>100</v>
+        <v>104</v>
       </c>
     </row>
     <row r="52" spans="1:10">
@@ -6802,7 +6808,7 @@
         <v>1494</v>
       </c>
       <c r="J52">
-        <v>99</v>
+        <v>101</v>
       </c>
     </row>
     <row r="53" spans="1:10">
@@ -6834,7 +6840,7 @@
         <v>1603</v>
       </c>
       <c r="J53">
-        <v>108</v>
+        <v>112</v>
       </c>
     </row>
     <row r="54" spans="1:10">
@@ -6866,7 +6872,7 @@
         <v>3508</v>
       </c>
       <c r="J54">
-        <v>198</v>
+        <v>205</v>
       </c>
     </row>
     <row r="55" spans="1:10">
@@ -6898,7 +6904,7 @@
         <v>1244</v>
       </c>
       <c r="J55">
-        <v>67</v>
+        <v>69</v>
       </c>
     </row>
     <row r="56" spans="1:10">
@@ -6930,7 +6936,7 @@
         <v>629</v>
       </c>
       <c r="J56">
-        <v>33</v>
+        <v>34</v>
       </c>
     </row>
     <row r="57" spans="1:10">
@@ -6962,7 +6968,7 @@
         <v>408</v>
       </c>
       <c r="J57">
-        <v>34</v>
+        <v>35</v>
       </c>
     </row>
     <row r="58" spans="1:10">
@@ -7026,7 +7032,7 @@
         <v>271</v>
       </c>
       <c r="J59">
-        <v>22</v>
+        <v>23</v>
       </c>
     </row>
     <row r="60" spans="1:10">
@@ -7130,7 +7136,7 @@
         <v>73</v>
       </c>
       <c r="B63">
-        <v>1464</v>
+        <v>1465</v>
       </c>
       <c r="C63">
         <v>1166</v>
@@ -7142,7 +7148,7 @@
         <v>2022</v>
       </c>
       <c r="F63">
-        <v>1311</v>
+        <v>1310</v>
       </c>
       <c r="G63">
         <v>1625</v>
@@ -7151,10 +7157,10 @@
         <v>2119</v>
       </c>
       <c r="I63">
-        <v>2024</v>
+        <v>2033</v>
       </c>
       <c r="J63">
-        <v>99</v>
+        <v>84</v>
       </c>
     </row>
     <row r="64" spans="1:10">
@@ -7186,7 +7192,7 @@
         <v>1187</v>
       </c>
       <c r="J64">
-        <v>48</v>
+        <v>50</v>
       </c>
     </row>
     <row r="65" spans="1:10">
@@ -7218,7 +7224,7 @@
         <v>1516</v>
       </c>
       <c r="J65">
-        <v>79</v>
+        <v>84</v>
       </c>
     </row>
     <row r="66" spans="1:10">
@@ -7250,7 +7256,7 @@
         <v>715</v>
       </c>
       <c r="J66">
-        <v>40</v>
+        <v>41</v>
       </c>
     </row>
     <row r="67" spans="1:10">
@@ -7282,7 +7288,7 @@
         <v>2512</v>
       </c>
       <c r="J67">
-        <v>141</v>
+        <v>150</v>
       </c>
     </row>
     <row r="68" spans="1:10">
@@ -7346,7 +7352,7 @@
         <v>493</v>
       </c>
       <c r="J69">
-        <v>30</v>
+        <v>31</v>
       </c>
     </row>
     <row r="70" spans="1:10">
@@ -7378,7 +7384,7 @@
         <v>677</v>
       </c>
       <c r="J70">
-        <v>39</v>
+        <v>42</v>
       </c>
     </row>
     <row r="71" spans="1:10">
@@ -7442,7 +7448,7 @@
         <v>708</v>
       </c>
       <c r="J72">
-        <v>30</v>
+        <v>32</v>
       </c>
     </row>
     <row r="73" spans="1:10">
@@ -7474,7 +7480,7 @@
         <v>1279</v>
       </c>
       <c r="J73">
-        <v>68</v>
+        <v>70</v>
       </c>
     </row>
     <row r="74" spans="1:10">
@@ -7538,7 +7544,7 @@
         <v>340</v>
       </c>
       <c r="J75">
-        <v>23</v>
+        <v>25</v>
       </c>
     </row>
     <row r="76" spans="1:10">
@@ -7567,10 +7573,10 @@
         <v>1998</v>
       </c>
       <c r="I76">
-        <v>2924</v>
+        <v>2923</v>
       </c>
       <c r="J76">
-        <v>203</v>
+        <v>210</v>
       </c>
     </row>
     <row r="77" spans="1:10">
@@ -7634,7 +7640,7 @@
         <v>1797</v>
       </c>
       <c r="J78">
-        <v>94</v>
+        <v>105</v>
       </c>
     </row>
     <row r="79" spans="1:10">
@@ -7663,10 +7669,10 @@
         <v>1893</v>
       </c>
       <c r="I79">
-        <v>2476</v>
+        <v>2475</v>
       </c>
       <c r="J79">
-        <v>165</v>
+        <v>166</v>
       </c>
     </row>
     <row r="80" spans="1:10">
@@ -7698,7 +7704,7 @@
         <v>393</v>
       </c>
       <c r="J80">
-        <v>18</v>
+        <v>19</v>
       </c>
     </row>
     <row r="81" spans="1:10">
@@ -7794,7 +7800,7 @@
         <v>1794</v>
       </c>
       <c r="J83">
-        <v>99</v>
+        <v>107</v>
       </c>
     </row>
     <row r="84" spans="1:10">
@@ -7826,7 +7832,7 @@
         <v>729</v>
       </c>
       <c r="J84">
-        <v>50</v>
+        <v>55</v>
       </c>
     </row>
     <row r="85" spans="1:10">
@@ -7858,7 +7864,7 @@
         <v>3855</v>
       </c>
       <c r="J85">
-        <v>257</v>
+        <v>268</v>
       </c>
     </row>
     <row r="86" spans="1:10">
@@ -7890,7 +7896,7 @@
         <v>1066</v>
       </c>
       <c r="J86">
-        <v>42</v>
+        <v>44</v>
       </c>
     </row>
     <row r="87" spans="1:10">
@@ -7922,7 +7928,7 @@
         <v>396</v>
       </c>
       <c r="J87">
-        <v>26</v>
+        <v>28</v>
       </c>
     </row>
     <row r="88" spans="1:10">
@@ -7954,7 +7960,7 @@
         <v>944</v>
       </c>
       <c r="J88">
-        <v>81</v>
+        <v>82</v>
       </c>
     </row>
     <row r="89" spans="1:10">
@@ -7986,7 +7992,7 @@
         <v>1879</v>
       </c>
       <c r="J89">
-        <v>96</v>
+        <v>98</v>
       </c>
     </row>
     <row r="90" spans="1:10">
@@ -8018,7 +8024,7 @@
         <v>1356</v>
       </c>
       <c r="J90">
-        <v>96</v>
+        <v>99</v>
       </c>
     </row>
     <row r="91" spans="1:10">
@@ -8050,7 +8056,7 @@
         <v>971</v>
       </c>
       <c r="J91">
-        <v>80</v>
+        <v>83</v>
       </c>
     </row>
     <row r="92" spans="1:10">
@@ -8082,7 +8088,7 @@
         <v>337</v>
       </c>
       <c r="J92">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="93" spans="1:10">
@@ -8114,7 +8120,7 @@
         <v>720</v>
       </c>
       <c r="J93">
-        <v>44</v>
+        <v>48</v>
       </c>
     </row>
     <row r="94" spans="1:10">
@@ -8146,7 +8152,7 @@
         <v>2664</v>
       </c>
       <c r="J94">
-        <v>122</v>
+        <v>130</v>
       </c>
     </row>
     <row r="95" spans="1:10">
@@ -8178,7 +8184,7 @@
         <v>1387</v>
       </c>
       <c r="J95">
-        <v>98</v>
+        <v>101</v>
       </c>
     </row>
     <row r="96" spans="1:10">
@@ -8210,7 +8216,7 @@
         <v>1670</v>
       </c>
       <c r="J96">
-        <v>87</v>
+        <v>92</v>
       </c>
     </row>
     <row r="97" spans="1:10">
@@ -8242,7 +8248,7 @@
         <v>1675</v>
       </c>
       <c r="J97">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="98" spans="1:10">
@@ -8274,7 +8280,7 @@
         <v>1320</v>
       </c>
       <c r="J98">
-        <v>56</v>
+        <v>58</v>
       </c>
     </row>
     <row r="99" spans="1:10">
@@ -8306,7 +8312,7 @@
         <v>1489</v>
       </c>
       <c r="J99">
-        <v>121</v>
+        <v>125</v>
       </c>
     </row>
     <row r="100" spans="1:10">
@@ -8346,7 +8352,7 @@
         <v>10</v>
       </c>
       <c r="B101">
-        <v>104351</v>
+        <v>104352</v>
       </c>
       <c r="C101">
         <v>116067</v>
@@ -8358,7 +8364,7 @@
         <v>113366</v>
       </c>
       <c r="F101">
-        <v>105543</v>
+        <v>105542</v>
       </c>
       <c r="G101">
         <v>85286</v>
@@ -8367,10 +8373,10 @@
         <v>84551</v>
       </c>
       <c r="I101">
-        <v>110099</v>
+        <v>110107</v>
       </c>
       <c r="J101">
-        <v>6825</v>
+        <v>7096</v>
       </c>
     </row>
   </sheetData>
@@ -8625,7 +8631,7 @@
         <v>8</v>
       </c>
       <c r="J4">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="5" spans="1:10">
@@ -8657,7 +8663,7 @@
         <v>107</v>
       </c>
       <c r="J5">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="6" spans="1:10">
@@ -8753,7 +8759,7 @@
         <v>202</v>
       </c>
       <c r="J8">
-        <v>20</v>
+        <v>22</v>
       </c>
     </row>
     <row r="9" spans="1:10">
@@ -8817,7 +8823,7 @@
         <v>586</v>
       </c>
       <c r="J10">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -8849,7 +8855,7 @@
         <v>1516</v>
       </c>
       <c r="J11">
-        <v>79</v>
+        <v>84</v>
       </c>
     </row>
   </sheetData>
@@ -9025,7 +9031,7 @@
         <v>81</v>
       </c>
       <c r="J5">
-        <v>10</v>
+        <v>12</v>
       </c>
     </row>
     <row r="6" spans="1:10">
@@ -9173,7 +9179,7 @@
         <v>785</v>
       </c>
       <c r="J10">
-        <v>49</v>
+        <v>50</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -9205,7 +9211,7 @@
         <v>1259</v>
       </c>
       <c r="J11">
-        <v>82</v>
+        <v>85</v>
       </c>
     </row>
   </sheetData>
@@ -9326,7 +9332,7 @@
         <v>206</v>
       </c>
       <c r="J3">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="4" spans="1:10">
@@ -9480,7 +9486,7 @@
         <v>484</v>
       </c>
       <c r="J8">
-        <v>36</v>
+        <v>41</v>
       </c>
     </row>
     <row r="9" spans="1:10">
@@ -9512,7 +9518,7 @@
         <v>123</v>
       </c>
       <c r="J9">
-        <v>12</v>
+        <v>13</v>
       </c>
     </row>
     <row r="10" spans="1:10">
@@ -9544,7 +9550,7 @@
         <v>612</v>
       </c>
       <c r="J10">
-        <v>26</v>
+        <v>27</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -9576,7 +9582,7 @@
         <v>1794</v>
       </c>
       <c r="J11">
-        <v>99</v>
+        <v>107</v>
       </c>
     </row>
   </sheetData>
@@ -9697,7 +9703,7 @@
         <v>416</v>
       </c>
       <c r="J3">
-        <v>17</v>
+        <v>19</v>
       </c>
     </row>
     <row r="4" spans="1:10">
@@ -9729,7 +9735,7 @@
         <v>24</v>
       </c>
       <c r="J4">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="5" spans="1:10">
@@ -9761,7 +9767,7 @@
         <v>170</v>
       </c>
       <c r="J5">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="6" spans="1:10">
@@ -9793,7 +9799,7 @@
         <v>50</v>
       </c>
       <c r="J6">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="7" spans="1:10">
@@ -9857,7 +9863,7 @@
         <v>707</v>
       </c>
       <c r="J8">
-        <v>52</v>
+        <v>53</v>
       </c>
     </row>
     <row r="9" spans="1:10">
@@ -9889,7 +9895,7 @@
         <v>366</v>
       </c>
       <c r="J9">
-        <v>27</v>
+        <v>28</v>
       </c>
     </row>
     <row r="10" spans="1:10">
@@ -9921,7 +9927,7 @@
         <v>968</v>
       </c>
       <c r="J10">
-        <v>53</v>
+        <v>54</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -9953,7 +9959,7 @@
         <v>3016</v>
       </c>
       <c r="J11">
-        <v>174</v>
+        <v>182</v>
       </c>
     </row>
   </sheetData>
@@ -10042,7 +10048,7 @@
         <v>142</v>
       </c>
       <c r="J2">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="3" spans="1:10">
@@ -10074,7 +10080,7 @@
         <v>137</v>
       </c>
       <c r="J3">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="4" spans="1:10">
@@ -10198,6 +10204,9 @@
       <c r="I7">
         <v>22</v>
       </c>
+      <c r="J7">
+        <v>1</v>
+      </c>
     </row>
     <row r="8" spans="1:10">
       <c r="A8" s="1" t="s">
@@ -10324,7 +10333,7 @@
         <v>1387</v>
       </c>
       <c r="J11">
-        <v>98</v>
+        <v>101</v>
       </c>
     </row>
   </sheetData>
@@ -10619,7 +10628,7 @@
         <v>21</v>
       </c>
       <c r="J9">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="10" spans="1:10">
@@ -10651,7 +10660,7 @@
         <v>148</v>
       </c>
       <c r="J10">
-        <v>12</v>
+        <v>13</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -10683,7 +10692,7 @@
         <v>340</v>
       </c>
       <c r="J11">
-        <v>23</v>
+        <v>25</v>
       </c>
     </row>
   </sheetData>
@@ -10862,7 +10871,7 @@
         <v>215</v>
       </c>
       <c r="I5">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="J5">
         <v>10</v>
@@ -10993,7 +11002,7 @@
         <v>216</v>
       </c>
       <c r="J9">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="10" spans="1:10">
@@ -11025,7 +11034,7 @@
         <v>821</v>
       </c>
       <c r="J10">
-        <v>40</v>
+        <v>42</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -11054,10 +11063,10 @@
         <v>1893</v>
       </c>
       <c r="I11">
-        <v>2476</v>
+        <v>2475</v>
       </c>
       <c r="J11">
-        <v>165</v>
+        <v>166</v>
       </c>
     </row>
   </sheetData>
@@ -11652,7 +11661,7 @@
         <v>44</v>
       </c>
       <c r="J8">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="9" spans="1:10">
@@ -11684,7 +11693,7 @@
         <v>18</v>
       </c>
       <c r="J9">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="10" spans="1:10">
@@ -11748,7 +11757,7 @@
         <v>433</v>
       </c>
       <c r="J11">
-        <v>23</v>
+        <v>25</v>
       </c>
     </row>
   </sheetData>
@@ -12272,7 +12281,7 @@
         <v>4</v>
       </c>
       <c r="J4">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="5" spans="1:10">
@@ -12361,6 +12370,9 @@
       <c r="I7">
         <v>9</v>
       </c>
+      <c r="J7">
+        <v>1</v>
+      </c>
     </row>
     <row r="8" spans="1:10">
       <c r="A8" s="1" t="s">
@@ -12455,7 +12467,7 @@
         <v>1222</v>
       </c>
       <c r="J10">
-        <v>37</v>
+        <v>39</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -12487,7 +12499,7 @@
         <v>1879</v>
       </c>
       <c r="J11">
-        <v>96</v>
+        <v>98</v>
       </c>
     </row>
   </sheetData>
@@ -12608,7 +12620,7 @@
         <v>58</v>
       </c>
       <c r="J3">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="4" spans="1:10">
@@ -12814,7 +12826,7 @@
         <v>606</v>
       </c>
       <c r="J10">
-        <v>21</v>
+        <v>22</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -12846,7 +12858,7 @@
         <v>1187</v>
       </c>
       <c r="J11">
-        <v>48</v>
+        <v>50</v>
       </c>
     </row>
   </sheetData>
@@ -13091,7 +13103,7 @@
         <v>54</v>
       </c>
       <c r="J8">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="9" spans="1:10">
@@ -13187,7 +13199,7 @@
         <v>236</v>
       </c>
       <c r="J11">
-        <v>17</v>
+        <v>18</v>
       </c>
     </row>
   </sheetData>
@@ -13276,7 +13288,7 @@
         <v>53</v>
       </c>
       <c r="J2">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="3" spans="1:10">
@@ -13447,7 +13459,7 @@
         <v>294</v>
       </c>
       <c r="J8">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="9" spans="1:10">
@@ -13479,7 +13491,7 @@
         <v>147</v>
       </c>
       <c r="J9">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="10" spans="1:10">
@@ -13511,7 +13523,7 @@
         <v>2021</v>
       </c>
       <c r="J10">
-        <v>96</v>
+        <v>101</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -13543,7 +13555,7 @@
         <v>2664</v>
       </c>
       <c r="J11">
-        <v>122</v>
+        <v>130</v>
       </c>
     </row>
   </sheetData>
@@ -13876,10 +13888,10 @@
         <v>1314</v>
       </c>
       <c r="I10">
-        <v>2133</v>
+        <v>2132</v>
       </c>
       <c r="J10">
-        <v>156</v>
+        <v>163</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -13908,10 +13920,10 @@
         <v>1998</v>
       </c>
       <c r="I11">
-        <v>2924</v>
+        <v>2923</v>
       </c>
       <c r="J11">
-        <v>203</v>
+        <v>210</v>
       </c>
     </row>
   </sheetData>
@@ -14217,7 +14229,7 @@
         <v>462</v>
       </c>
       <c r="J10">
-        <v>21</v>
+        <v>22</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -14249,7 +14261,7 @@
         <v>715</v>
       </c>
       <c r="J11">
-        <v>40</v>
+        <v>41</v>
       </c>
     </row>
   </sheetData>
@@ -14579,7 +14591,7 @@
         <v>216</v>
       </c>
       <c r="J10">
-        <v>7</v>
+        <v>9</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -14611,7 +14623,7 @@
         <v>396</v>
       </c>
       <c r="J11">
-        <v>26</v>
+        <v>28</v>
       </c>
     </row>
   </sheetData>
@@ -15256,7 +15268,7 @@
         <v>189</v>
       </c>
       <c r="J10">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -15288,7 +15300,7 @@
         <v>431</v>
       </c>
       <c r="J11">
-        <v>22</v>
+        <v>23</v>
       </c>
     </row>
   </sheetData>
@@ -15805,7 +15817,7 @@
         <v>120</v>
       </c>
       <c r="J5">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="6" spans="1:10">
@@ -15886,7 +15898,7 @@
         <v>219</v>
       </c>
       <c r="J8">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="9" spans="1:10">
@@ -15982,7 +15994,7 @@
         <v>1647</v>
       </c>
       <c r="J11">
-        <v>95</v>
+        <v>97</v>
       </c>
     </row>
   </sheetData>
@@ -16071,7 +16083,7 @@
         <v>326</v>
       </c>
       <c r="J2">
-        <v>12</v>
+        <v>14</v>
       </c>
     </row>
     <row r="3" spans="1:10">
@@ -16103,7 +16115,7 @@
         <v>441</v>
       </c>
       <c r="J3">
-        <v>21</v>
+        <v>22</v>
       </c>
     </row>
     <row r="4" spans="1:10">
@@ -16260,7 +16272,7 @@
         <v>1028</v>
       </c>
       <c r="J8">
-        <v>108</v>
+        <v>112</v>
       </c>
     </row>
     <row r="9" spans="1:10">
@@ -16292,7 +16304,7 @@
         <v>304</v>
       </c>
       <c r="J9">
-        <v>22</v>
+        <v>23</v>
       </c>
     </row>
     <row r="10" spans="1:10">
@@ -16324,7 +16336,7 @@
         <v>1272</v>
       </c>
       <c r="J10">
-        <v>66</v>
+        <v>69</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -16356,7 +16368,7 @@
         <v>3855</v>
       </c>
       <c r="J11">
-        <v>257</v>
+        <v>268</v>
       </c>
     </row>
   </sheetData>
@@ -16625,7 +16637,7 @@
         <v>280</v>
       </c>
       <c r="J8">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="9" spans="1:10">
@@ -16721,7 +16733,7 @@
         <v>1675</v>
       </c>
       <c r="J11">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
   </sheetData>
@@ -16842,7 +16854,7 @@
         <v>90</v>
       </c>
       <c r="J3">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="4" spans="1:10">
@@ -16996,7 +17008,7 @@
         <v>224</v>
       </c>
       <c r="J8">
-        <v>26</v>
+        <v>24</v>
       </c>
     </row>
     <row r="9" spans="1:10">
@@ -17028,7 +17040,7 @@
         <v>109</v>
       </c>
       <c r="J9">
-        <v>16</v>
+        <v>17</v>
       </c>
     </row>
     <row r="10" spans="1:10">
@@ -17060,7 +17072,7 @@
         <v>610</v>
       </c>
       <c r="J10">
-        <v>19</v>
+        <v>21</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -17092,7 +17104,7 @@
         <v>1244</v>
       </c>
       <c r="J11">
-        <v>67</v>
+        <v>69</v>
       </c>
     </row>
   </sheetData>
@@ -17181,7 +17193,7 @@
         <v>108</v>
       </c>
       <c r="J2">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="3" spans="1:10">
@@ -17213,7 +17225,7 @@
         <v>111</v>
       </c>
       <c r="J3">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="4" spans="1:10">
@@ -17364,7 +17376,7 @@
         <v>402</v>
       </c>
       <c r="J8">
-        <v>22</v>
+        <v>23</v>
       </c>
     </row>
     <row r="9" spans="1:10">
@@ -17428,7 +17440,7 @@
         <v>2527</v>
       </c>
       <c r="J10">
-        <v>150</v>
+        <v>154</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -17460,7 +17472,7 @@
         <v>3508</v>
       </c>
       <c r="J11">
-        <v>198</v>
+        <v>205</v>
       </c>
     </row>
   </sheetData>
@@ -17799,7 +17811,7 @@
         <v>681</v>
       </c>
       <c r="J10">
-        <v>39</v>
+        <v>41</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -17831,7 +17843,7 @@
         <v>1279</v>
       </c>
       <c r="J11">
-        <v>68</v>
+        <v>70</v>
       </c>
     </row>
   </sheetData>
@@ -18016,7 +18028,7 @@
         <v>269</v>
       </c>
       <c r="J5">
-        <v>19</v>
+        <v>20</v>
       </c>
     </row>
     <row r="6" spans="1:10">
@@ -18112,7 +18124,7 @@
         <v>794</v>
       </c>
       <c r="J8">
-        <v>102</v>
+        <v>104</v>
       </c>
     </row>
     <row r="9" spans="1:10">
@@ -18144,7 +18156,7 @@
         <v>434</v>
       </c>
       <c r="J9">
-        <v>27</v>
+        <v>28</v>
       </c>
     </row>
     <row r="10" spans="1:10">
@@ -18176,7 +18188,7 @@
         <v>1302</v>
       </c>
       <c r="J10">
-        <v>71</v>
+        <v>75</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -18208,7 +18220,7 @@
         <v>3951</v>
       </c>
       <c r="J11">
-        <v>283</v>
+        <v>291</v>
       </c>
     </row>
   </sheetData>
@@ -18297,7 +18309,7 @@
         <v>237</v>
       </c>
       <c r="J2">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="3" spans="1:10">
@@ -18329,7 +18341,7 @@
         <v>212</v>
       </c>
       <c r="J3">
-        <v>17</v>
+        <v>18</v>
       </c>
     </row>
     <row r="4" spans="1:10">
@@ -18489,7 +18501,7 @@
         <v>753</v>
       </c>
       <c r="J8">
-        <v>58</v>
+        <v>65</v>
       </c>
     </row>
     <row r="9" spans="1:10">
@@ -18521,7 +18533,7 @@
         <v>233</v>
       </c>
       <c r="J9">
-        <v>28</v>
+        <v>31</v>
       </c>
     </row>
     <row r="10" spans="1:10">
@@ -18553,7 +18565,7 @@
         <v>912</v>
       </c>
       <c r="J10">
-        <v>55</v>
+        <v>57</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -18585,7 +18597,7 @@
         <v>2636</v>
       </c>
       <c r="J11">
-        <v>183</v>
+        <v>197</v>
       </c>
     </row>
   </sheetData>
@@ -18903,7 +18915,7 @@
         <v>213</v>
       </c>
       <c r="J10">
-        <v>17</v>
+        <v>18</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -18935,7 +18947,7 @@
         <v>419</v>
       </c>
       <c r="J11">
-        <v>27</v>
+        <v>28</v>
       </c>
     </row>
   </sheetData>
@@ -19056,7 +19068,7 @@
         <v>55</v>
       </c>
       <c r="J3">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="4" spans="1:10">
@@ -19297,7 +19309,7 @@
         <v>1229</v>
       </c>
       <c r="J11">
-        <v>84</v>
+        <v>85</v>
       </c>
     </row>
   </sheetData>
@@ -19447,7 +19459,7 @@
         <v>27</v>
       </c>
       <c r="I4">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="J4">
         <v>1</v>
@@ -19546,7 +19558,7 @@
         <v>27</v>
       </c>
       <c r="J7">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="8" spans="1:10">
@@ -19610,7 +19622,7 @@
         <v>428</v>
       </c>
       <c r="J9">
-        <v>44</v>
+        <v>45</v>
       </c>
     </row>
     <row r="10" spans="1:10">
@@ -19642,7 +19654,7 @@
         <v>1089</v>
       </c>
       <c r="J10">
-        <v>45</v>
+        <v>50</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -19671,10 +19683,10 @@
         <v>2423</v>
       </c>
       <c r="I11">
-        <v>2956</v>
+        <v>2957</v>
       </c>
       <c r="J11">
-        <v>179</v>
+        <v>186</v>
       </c>
     </row>
   </sheetData>
@@ -19859,7 +19871,7 @@
         <v>177</v>
       </c>
       <c r="J5">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="6" spans="1:10">
@@ -19946,7 +19958,7 @@
         <v>337</v>
       </c>
       <c r="J8">
-        <v>29</v>
+        <v>30</v>
       </c>
     </row>
     <row r="9" spans="1:10">
@@ -20010,7 +20022,7 @@
         <v>1774</v>
       </c>
       <c r="J10">
-        <v>90</v>
+        <v>94</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -20042,7 +20054,7 @@
         <v>2621</v>
       </c>
       <c r="J11">
-        <v>139</v>
+        <v>145</v>
       </c>
     </row>
   </sheetData>
@@ -20363,7 +20375,7 @@
         <v>312</v>
       </c>
       <c r="J10">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -20395,7 +20407,7 @@
         <v>493</v>
       </c>
       <c r="J11">
-        <v>30</v>
+        <v>31</v>
       </c>
     </row>
   </sheetData>
@@ -20516,7 +20528,7 @@
         <v>47</v>
       </c>
       <c r="J3">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="4" spans="1:10">
@@ -20605,6 +20617,9 @@
       <c r="I6">
         <v>13</v>
       </c>
+      <c r="J6">
+        <v>1</v>
+      </c>
     </row>
     <row r="7" spans="1:10">
       <c r="A7" s="1" t="s">
@@ -20728,7 +20743,7 @@
         <v>349</v>
       </c>
       <c r="J10">
-        <v>17</v>
+        <v>19</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -20760,7 +20775,7 @@
         <v>793</v>
       </c>
       <c r="J11">
-        <v>46</v>
+        <v>50</v>
       </c>
     </row>
   </sheetData>
@@ -21061,7 +21076,7 @@
         <v>35</v>
       </c>
       <c r="J9">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="10" spans="1:10">
@@ -21093,7 +21108,7 @@
         <v>172</v>
       </c>
       <c r="J10">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -21125,7 +21140,7 @@
         <v>438</v>
       </c>
       <c r="J11">
-        <v>31</v>
+        <v>33</v>
       </c>
     </row>
   </sheetData>
@@ -21464,7 +21479,7 @@
         <v>527</v>
       </c>
       <c r="J10">
-        <v>26</v>
+        <v>28</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -21496,7 +21511,7 @@
         <v>1493</v>
       </c>
       <c r="J11">
-        <v>98</v>
+        <v>100</v>
       </c>
     </row>
   </sheetData>
@@ -21746,6 +21761,9 @@
       <c r="I8">
         <v>15</v>
       </c>
+      <c r="J8">
+        <v>1</v>
+      </c>
     </row>
     <row r="9" spans="1:10">
       <c r="A9" s="1" t="s">
@@ -21808,7 +21826,7 @@
         <v>260</v>
       </c>
       <c r="J10">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
   </sheetData>
@@ -21897,7 +21915,7 @@
         <v>55</v>
       </c>
       <c r="J2">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="3" spans="1:10">
@@ -22147,7 +22165,7 @@
         <v>542</v>
       </c>
       <c r="J10">
-        <v>24</v>
+        <v>27</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -22179,7 +22197,7 @@
         <v>949</v>
       </c>
       <c r="J11">
-        <v>53</v>
+        <v>57</v>
       </c>
     </row>
   </sheetData>
@@ -22381,7 +22399,7 @@
         <v>81</v>
       </c>
       <c r="J6">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="7" spans="1:10">
@@ -22488,7 +22506,7 @@
         <v>717</v>
       </c>
       <c r="J10">
-        <v>29</v>
+        <v>30</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -22520,7 +22538,7 @@
         <v>1066</v>
       </c>
       <c r="J11">
-        <v>42</v>
+        <v>44</v>
       </c>
     </row>
   </sheetData>
@@ -22641,7 +22659,7 @@
         <v>87</v>
       </c>
       <c r="J3">
-        <v>8</v>
+        <v>10</v>
       </c>
     </row>
     <row r="4" spans="1:10">
@@ -22795,7 +22813,7 @@
         <v>197</v>
       </c>
       <c r="J8">
-        <v>23</v>
+        <v>27</v>
       </c>
     </row>
     <row r="9" spans="1:10">
@@ -22859,7 +22877,7 @@
         <v>1118</v>
       </c>
       <c r="J10">
-        <v>46</v>
+        <v>51</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -22891,7 +22909,7 @@
         <v>1797</v>
       </c>
       <c r="J11">
-        <v>94</v>
+        <v>105</v>
       </c>
     </row>
   </sheetData>
@@ -23368,7 +23386,7 @@
         <v>69</v>
       </c>
       <c r="J3">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="4" spans="1:10">
@@ -23519,7 +23537,7 @@
         <v>122</v>
       </c>
       <c r="J8">
-        <v>20</v>
+        <v>21</v>
       </c>
     </row>
     <row r="9" spans="1:10">
@@ -23551,7 +23569,7 @@
         <v>113</v>
       </c>
       <c r="J9">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="10" spans="1:10">
@@ -23615,7 +23633,7 @@
         <v>886</v>
       </c>
       <c r="J11">
-        <v>59</v>
+        <v>62</v>
       </c>
     </row>
   </sheetData>
@@ -24287,7 +24305,7 @@
         <v>193</v>
       </c>
       <c r="J9">
-        <v>19</v>
+        <v>20</v>
       </c>
     </row>
     <row r="10" spans="1:10">
@@ -24319,7 +24337,7 @@
         <v>591</v>
       </c>
       <c r="J10">
-        <v>38</v>
+        <v>39</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -24351,7 +24369,7 @@
         <v>1494</v>
       </c>
       <c r="J11">
-        <v>99</v>
+        <v>101</v>
       </c>
     </row>
   </sheetData>
@@ -24620,7 +24638,7 @@
         <v>406</v>
       </c>
       <c r="J8">
-        <v>53</v>
+        <v>56</v>
       </c>
     </row>
     <row r="9" spans="1:10">
@@ -24716,7 +24734,7 @@
         <v>1369</v>
       </c>
       <c r="J11">
-        <v>108</v>
+        <v>111</v>
       </c>
     </row>
   </sheetData>
@@ -24837,7 +24855,7 @@
         <v>177</v>
       </c>
       <c r="J3">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="4" spans="1:10">
@@ -24901,7 +24919,7 @@
         <v>194</v>
       </c>
       <c r="J5">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="6" spans="1:10">
@@ -24994,7 +25012,7 @@
         <v>365</v>
       </c>
       <c r="J8">
-        <v>27</v>
+        <v>28</v>
       </c>
     </row>
     <row r="9" spans="1:10">
@@ -25058,7 +25076,7 @@
         <v>828</v>
       </c>
       <c r="J10">
-        <v>31</v>
+        <v>33</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -25090,7 +25108,7 @@
         <v>2048</v>
       </c>
       <c r="J11">
-        <v>96</v>
+        <v>101</v>
       </c>
     </row>
   </sheetData>
@@ -25211,7 +25229,7 @@
         <v>81</v>
       </c>
       <c r="J3">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="4" spans="1:10">
@@ -25362,7 +25380,7 @@
         <v>297</v>
       </c>
       <c r="J8">
-        <v>50</v>
+        <v>52</v>
       </c>
     </row>
     <row r="9" spans="1:10">
@@ -25426,7 +25444,7 @@
         <v>670</v>
       </c>
       <c r="J10">
-        <v>30</v>
+        <v>31</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -25458,7 +25476,7 @@
         <v>1337</v>
       </c>
       <c r="J11">
-        <v>100</v>
+        <v>104</v>
       </c>
     </row>
   </sheetData>
@@ -25579,7 +25597,7 @@
         <v>99</v>
       </c>
       <c r="J3">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="4" spans="1:10">
@@ -25736,7 +25754,7 @@
         <v>309</v>
       </c>
       <c r="J8">
-        <v>30</v>
+        <v>31</v>
       </c>
     </row>
     <row r="9" spans="1:10">
@@ -25800,7 +25818,7 @@
         <v>318</v>
       </c>
       <c r="J10">
-        <v>19</v>
+        <v>20</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -25832,7 +25850,7 @@
         <v>971</v>
       </c>
       <c r="J11">
-        <v>80</v>
+        <v>83</v>
       </c>
     </row>
   </sheetData>
@@ -26430,7 +26448,7 @@
         <v>250</v>
       </c>
       <c r="J8">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="9" spans="1:10">
@@ -26462,7 +26480,7 @@
         <v>61</v>
       </c>
       <c r="J9">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="10" spans="1:10">
@@ -26526,7 +26544,7 @@
         <v>904</v>
       </c>
       <c r="J11">
-        <v>71</v>
+        <v>73</v>
       </c>
     </row>
   </sheetData>
@@ -26798,7 +26816,7 @@
         <v>441</v>
       </c>
       <c r="J8">
-        <v>46</v>
+        <v>48</v>
       </c>
     </row>
     <row r="9" spans="1:10">
@@ -26862,7 +26880,7 @@
         <v>455</v>
       </c>
       <c r="J10">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -26894,7 +26912,7 @@
         <v>1356</v>
       </c>
       <c r="J11">
-        <v>96</v>
+        <v>99</v>
       </c>
     </row>
   </sheetData>
@@ -27160,7 +27178,7 @@
         <v>99</v>
       </c>
       <c r="J8">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="9" spans="1:10">
@@ -27256,7 +27274,7 @@
         <v>962</v>
       </c>
       <c r="J11">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
   </sheetData>
@@ -27374,7 +27392,7 @@
         <v>37</v>
       </c>
       <c r="J3">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="4" spans="1:10">
@@ -27522,7 +27540,7 @@
         <v>122</v>
       </c>
       <c r="J8">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="9" spans="1:10">
@@ -27586,7 +27604,7 @@
         <v>381</v>
       </c>
       <c r="J10">
-        <v>21</v>
+        <v>23</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -27618,7 +27636,7 @@
         <v>720</v>
       </c>
       <c r="J11">
-        <v>44</v>
+        <v>48</v>
       </c>
     </row>
   </sheetData>
@@ -27893,7 +27911,7 @@
         <v>196</v>
       </c>
       <c r="J8">
-        <v>16</v>
+        <v>17</v>
       </c>
     </row>
     <row r="9" spans="1:10">
@@ -27925,7 +27943,7 @@
         <v>99</v>
       </c>
       <c r="J9">
-        <v>18</v>
+        <v>20</v>
       </c>
     </row>
     <row r="10" spans="1:10">
@@ -27989,7 +28007,7 @@
         <v>696</v>
       </c>
       <c r="J11">
-        <v>56</v>
+        <v>59</v>
       </c>
     </row>
   </sheetData>
@@ -28110,7 +28128,7 @@
         <v>81</v>
       </c>
       <c r="J3">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="4" spans="1:10">
@@ -28270,7 +28288,7 @@
         <v>373</v>
       </c>
       <c r="J8">
-        <v>43</v>
+        <v>45</v>
       </c>
     </row>
     <row r="9" spans="1:10">
@@ -28334,7 +28352,7 @@
         <v>818</v>
       </c>
       <c r="J10">
-        <v>57</v>
+        <v>59</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -28366,7 +28384,7 @@
         <v>1711</v>
       </c>
       <c r="J11">
-        <v>131</v>
+        <v>136</v>
       </c>
     </row>
   </sheetData>
@@ -29028,7 +29046,7 @@
         <v>576</v>
       </c>
       <c r="J10">
-        <v>30</v>
+        <v>31</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -29060,7 +29078,7 @@
         <v>629</v>
       </c>
       <c r="J11">
-        <v>33</v>
+        <v>34</v>
       </c>
     </row>
   </sheetData>
@@ -29149,7 +29167,7 @@
         <v>22</v>
       </c>
       <c r="J2">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="3" spans="1:10">
@@ -29372,7 +29390,7 @@
         <v>94</v>
       </c>
       <c r="J10">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -29404,7 +29422,7 @@
         <v>248</v>
       </c>
       <c r="J11">
-        <v>19</v>
+        <v>21</v>
       </c>
     </row>
   </sheetData>
@@ -29708,7 +29726,7 @@
         <v>59</v>
       </c>
       <c r="I9">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="J9">
         <v>4</v>
@@ -29740,10 +29758,10 @@
         <v>405</v>
       </c>
       <c r="I10">
-        <v>493</v>
+        <v>492</v>
       </c>
       <c r="J10">
-        <v>29</v>
+        <v>32</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -29775,7 +29793,7 @@
         <v>918</v>
       </c>
       <c r="J11">
-        <v>54</v>
+        <v>57</v>
       </c>
     </row>
   </sheetData>
@@ -30038,7 +30056,7 @@
         <v>90</v>
       </c>
       <c r="J8">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="9" spans="1:10">
@@ -30070,7 +30088,7 @@
         <v>51</v>
       </c>
       <c r="J9">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="10" spans="1:10">
@@ -30134,7 +30152,7 @@
         <v>708</v>
       </c>
       <c r="J11">
-        <v>30</v>
+        <v>32</v>
       </c>
     </row>
   </sheetData>
@@ -30388,7 +30406,7 @@
         <v>227</v>
       </c>
       <c r="J8">
-        <v>24</v>
+        <v>26</v>
       </c>
     </row>
     <row r="9" spans="1:10">
@@ -30484,7 +30502,7 @@
         <v>1153</v>
       </c>
       <c r="J11">
-        <v>86</v>
+        <v>88</v>
       </c>
     </row>
   </sheetData>
@@ -31458,7 +31476,7 @@
         <v>47</v>
       </c>
       <c r="J9">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="10" spans="1:10">
@@ -31522,7 +31540,7 @@
         <v>393</v>
       </c>
       <c r="J11">
-        <v>18</v>
+        <v>19</v>
       </c>
     </row>
   </sheetData>
@@ -31794,7 +31812,7 @@
         <v>140</v>
       </c>
       <c r="J8">
-        <v>9</v>
+        <v>11</v>
       </c>
     </row>
     <row r="9" spans="1:10">
@@ -31858,7 +31876,7 @@
         <v>440</v>
       </c>
       <c r="J10">
-        <v>26</v>
+        <v>27</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -31890,7 +31908,7 @@
         <v>764</v>
       </c>
       <c r="J11">
-        <v>53</v>
+        <v>56</v>
       </c>
     </row>
   </sheetData>
@@ -31979,7 +31997,7 @@
         <v>457</v>
       </c>
       <c r="J2">
-        <v>29</v>
+        <v>30</v>
       </c>
     </row>
     <row r="3" spans="1:10">
@@ -32011,7 +32029,7 @@
         <v>448</v>
       </c>
       <c r="J3">
-        <v>34</v>
+        <v>37</v>
       </c>
     </row>
     <row r="4" spans="1:10">
@@ -32107,7 +32125,7 @@
         <v>94</v>
       </c>
       <c r="J6">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="7" spans="1:10">
@@ -32171,7 +32189,7 @@
         <v>1272</v>
       </c>
       <c r="J8">
-        <v>88</v>
+        <v>101</v>
       </c>
     </row>
     <row r="9" spans="1:10">
@@ -32203,7 +32221,7 @@
         <v>496</v>
       </c>
       <c r="J9">
-        <v>30</v>
+        <v>32</v>
       </c>
     </row>
     <row r="10" spans="1:10">
@@ -32235,7 +32253,7 @@
         <v>1653</v>
       </c>
       <c r="J10">
-        <v>77</v>
+        <v>81</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -32267,7 +32285,7 @@
         <v>4749</v>
       </c>
       <c r="J11">
-        <v>280</v>
+        <v>304</v>
       </c>
     </row>
   </sheetData>
@@ -32675,6 +32693,9 @@
       <c r="I2">
         <v>9</v>
       </c>
+      <c r="J2">
+        <v>1</v>
+      </c>
     </row>
     <row r="3" spans="1:10">
       <c r="A3" s="1" t="s">
@@ -32703,6 +32724,9 @@
       </c>
       <c r="I3">
         <v>5</v>
+      </c>
+      <c r="J3">
+        <v>1</v>
       </c>
     </row>
     <row r="4" spans="1:10">
@@ -32748,7 +32772,7 @@
         <v>14</v>
       </c>
       <c r="J5">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="6" spans="1:10">
@@ -32823,7 +32847,7 @@
         <v>65</v>
       </c>
       <c r="J8">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="9" spans="1:10">
@@ -32919,7 +32943,7 @@
         <v>209</v>
       </c>
       <c r="J11">
-        <v>13</v>
+        <v>17</v>
       </c>
     </row>
   </sheetData>
@@ -33494,7 +33518,7 @@
         <v>131</v>
       </c>
       <c r="J8">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="9" spans="1:10">
@@ -33558,7 +33582,7 @@
         <v>921</v>
       </c>
       <c r="J10">
-        <v>29</v>
+        <v>30</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -33590,7 +33614,7 @@
         <v>1320</v>
       </c>
       <c r="J11">
-        <v>56</v>
+        <v>58</v>
       </c>
     </row>
   </sheetData>
@@ -34478,7 +34502,7 @@
         <v>68</v>
       </c>
       <c r="J8">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="9" spans="1:10">
@@ -34571,7 +34595,7 @@
         <v>337</v>
       </c>
       <c r="J11">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
   </sheetData>
@@ -35698,7 +35722,7 @@
         <v>56</v>
       </c>
       <c r="J3">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="4" spans="1:10">
@@ -35849,7 +35873,7 @@
         <v>260</v>
       </c>
       <c r="J8">
-        <v>42</v>
+        <v>44</v>
       </c>
     </row>
     <row r="9" spans="1:10">
@@ -35913,7 +35937,7 @@
         <v>914</v>
       </c>
       <c r="J10">
-        <v>45</v>
+        <v>46</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -35945,7 +35969,7 @@
         <v>1603</v>
       </c>
       <c r="J11">
-        <v>108</v>
+        <v>112</v>
       </c>
     </row>
   </sheetData>
@@ -36263,7 +36287,7 @@
         <v>124</v>
       </c>
       <c r="J10">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -36295,7 +36319,7 @@
         <v>271</v>
       </c>
       <c r="J11">
-        <v>22</v>
+        <v>23</v>
       </c>
     </row>
   </sheetData>
@@ -36525,6 +36549,9 @@
       <c r="I7">
         <v>10</v>
       </c>
+      <c r="J7">
+        <v>1</v>
+      </c>
     </row>
     <row r="8" spans="1:10">
       <c r="A8" s="1" t="s">
@@ -36555,7 +36582,7 @@
         <v>116</v>
       </c>
       <c r="J8">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="9" spans="1:10">
@@ -36587,7 +36614,7 @@
         <v>153</v>
       </c>
       <c r="J9">
-        <v>7</v>
+        <v>9</v>
       </c>
     </row>
   </sheetData>
@@ -36760,7 +36787,7 @@
         <v>32</v>
       </c>
       <c r="J5">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="6" spans="1:10">
@@ -36943,7 +36970,7 @@
         <v>408</v>
       </c>
       <c r="J11">
-        <v>34</v>
+        <v>35</v>
       </c>
     </row>
   </sheetData>
@@ -37215,7 +37242,7 @@
         <v>184</v>
       </c>
       <c r="J8">
-        <v>28</v>
+        <v>29</v>
       </c>
     </row>
     <row r="9" spans="1:10">
@@ -37311,7 +37338,7 @@
         <v>944</v>
       </c>
       <c r="J11">
-        <v>81</v>
+        <v>82</v>
       </c>
     </row>
   </sheetData>
@@ -38692,7 +38719,7 @@
         <v>47</v>
       </c>
       <c r="I5">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="J5">
         <v>11</v>
@@ -38831,10 +38858,10 @@
         <v>128</v>
       </c>
       <c r="I10">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="J10">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -38866,7 +38893,7 @@
         <v>413</v>
       </c>
       <c r="J11">
-        <v>33</v>
+        <v>34</v>
       </c>
     </row>
   </sheetData>
@@ -39154,7 +39181,7 @@
         <v>47</v>
       </c>
       <c r="J10">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -39186,7 +39213,7 @@
         <v>99</v>
       </c>
       <c r="J11">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add data for 2023-07-09
</commit_message>
<xml_diff>
--- a/output/index-crime-full-year.xlsx
+++ b/output/index-crime-full-year.xlsx
@@ -895,7 +895,7 @@
         <v>7277</v>
       </c>
       <c r="J2">
-        <v>3797</v>
+        <v>3829</v>
       </c>
     </row>
     <row r="3" spans="1:10">
@@ -927,7 +927,7 @@
         <v>7486</v>
       </c>
       <c r="J3">
-        <v>4006</v>
+        <v>4023</v>
       </c>
     </row>
     <row r="4" spans="1:10">
@@ -959,7 +959,7 @@
         <v>422</v>
       </c>
       <c r="J4">
-        <v>254</v>
+        <v>256</v>
       </c>
     </row>
     <row r="5" spans="1:10">
@@ -991,7 +991,7 @@
         <v>7592</v>
       </c>
       <c r="J5">
-        <v>3733</v>
+        <v>3756</v>
       </c>
     </row>
     <row r="6" spans="1:10">
@@ -1023,7 +1023,7 @@
         <v>1767</v>
       </c>
       <c r="J6">
-        <v>903</v>
+        <v>908</v>
       </c>
     </row>
     <row r="7" spans="1:10">
@@ -1055,7 +1055,7 @@
         <v>718</v>
       </c>
       <c r="J7">
-        <v>318</v>
+        <v>320</v>
       </c>
     </row>
     <row r="8" spans="1:10">
@@ -1087,7 +1087,7 @@
         <v>21448</v>
       </c>
       <c r="J8">
-        <v>15135</v>
+        <v>15231</v>
       </c>
     </row>
     <row r="9" spans="1:10">
@@ -1119,7 +1119,7 @@
         <v>8964</v>
       </c>
       <c r="J9">
-        <v>4724</v>
+        <v>4778</v>
       </c>
     </row>
     <row r="10" spans="1:10">
@@ -1148,10 +1148,10 @@
         <v>40794</v>
       </c>
       <c r="I10">
-        <v>54803</v>
+        <v>54804</v>
       </c>
       <c r="J10">
-        <v>27492</v>
+        <v>27653</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -1180,10 +1180,10 @@
         <v>84587</v>
       </c>
       <c r="I11">
-        <v>110477</v>
+        <v>110478</v>
       </c>
       <c r="J11">
-        <v>60362</v>
+        <v>60754</v>
       </c>
     </row>
   </sheetData>
@@ -1440,7 +1440,7 @@
         <v>227</v>
       </c>
       <c r="J8">
-        <v>188</v>
+        <v>189</v>
       </c>
     </row>
     <row r="9" spans="1:10">
@@ -1504,7 +1504,7 @@
         <v>648</v>
       </c>
       <c r="J10">
-        <v>370</v>
+        <v>375</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -1536,7 +1536,7 @@
         <v>1153</v>
       </c>
       <c r="J11">
-        <v>714</v>
+        <v>720</v>
       </c>
     </row>
   </sheetData>
@@ -1899,7 +1899,7 @@
         <v>154</v>
       </c>
       <c r="J2">
-        <v>75</v>
+        <v>76</v>
       </c>
     </row>
     <row r="3" spans="1:10">
@@ -1931,7 +1931,7 @@
         <v>81</v>
       </c>
       <c r="J3">
-        <v>42</v>
+        <v>43</v>
       </c>
     </row>
     <row r="4" spans="1:10">
@@ -2091,7 +2091,7 @@
         <v>373</v>
       </c>
       <c r="J8">
-        <v>256</v>
+        <v>260</v>
       </c>
     </row>
     <row r="9" spans="1:10">
@@ -2155,7 +2155,7 @@
         <v>820</v>
       </c>
       <c r="J10">
-        <v>472</v>
+        <v>474</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -2187,7 +2187,7 @@
         <v>1713</v>
       </c>
       <c r="J11">
-        <v>1014</v>
+        <v>1022</v>
       </c>
     </row>
   </sheetData>
@@ -2494,7 +2494,7 @@
         <v>57</v>
       </c>
       <c r="J9">
-        <v>29</v>
+        <v>33</v>
       </c>
     </row>
     <row r="10" spans="1:10">
@@ -2526,7 +2526,7 @@
         <v>712</v>
       </c>
       <c r="J10">
-        <v>374</v>
+        <v>376</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -2558,7 +2558,7 @@
         <v>1228</v>
       </c>
       <c r="J11">
-        <v>674</v>
+        <v>680</v>
       </c>
     </row>
   </sheetData>
@@ -2647,7 +2647,7 @@
         <v>220</v>
       </c>
       <c r="J2">
-        <v>113</v>
+        <v>114</v>
       </c>
     </row>
     <row r="3" spans="1:10">
@@ -2839,7 +2839,7 @@
         <v>700</v>
       </c>
       <c r="J8">
-        <v>447</v>
+        <v>448</v>
       </c>
     </row>
     <row r="9" spans="1:10">
@@ -2871,7 +2871,7 @@
         <v>216</v>
       </c>
       <c r="J9">
-        <v>102</v>
+        <v>103</v>
       </c>
     </row>
     <row r="10" spans="1:10">
@@ -2935,7 +2935,7 @@
         <v>2472</v>
       </c>
       <c r="J11">
-        <v>1350</v>
+        <v>1353</v>
       </c>
     </row>
   </sheetData>
@@ -3024,7 +3024,7 @@
         <v>61</v>
       </c>
       <c r="J2">
-        <v>32</v>
+        <v>34</v>
       </c>
     </row>
     <row r="3" spans="1:10">
@@ -3056,7 +3056,7 @@
         <v>56</v>
       </c>
       <c r="J3">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="4" spans="1:10">
@@ -3245,7 +3245,7 @@
         <v>151</v>
       </c>
       <c r="J9">
-        <v>72</v>
+        <v>74</v>
       </c>
     </row>
     <row r="10" spans="1:10">
@@ -3277,7 +3277,7 @@
         <v>913</v>
       </c>
       <c r="J10">
-        <v>564</v>
+        <v>568</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -3309,7 +3309,7 @@
         <v>1601</v>
       </c>
       <c r="J11">
-        <v>1001</v>
+        <v>1010</v>
       </c>
     </row>
   </sheetData>
@@ -3801,7 +3801,7 @@
         <v>71</v>
       </c>
       <c r="J3">
-        <v>33</v>
+        <v>34</v>
       </c>
     </row>
     <row r="4" spans="1:10">
@@ -4025,7 +4025,7 @@
         <v>681</v>
       </c>
       <c r="J10">
-        <v>437</v>
+        <v>441</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -4057,7 +4057,7 @@
         <v>1279</v>
       </c>
       <c r="J11">
-        <v>806</v>
+        <v>811</v>
       </c>
     </row>
   </sheetData>
@@ -4146,7 +4146,7 @@
         <v>459</v>
       </c>
       <c r="J2">
-        <v>244</v>
+        <v>246</v>
       </c>
     </row>
     <row r="3" spans="1:10">
@@ -4178,7 +4178,7 @@
         <v>530</v>
       </c>
       <c r="J3">
-        <v>272</v>
+        <v>273</v>
       </c>
     </row>
     <row r="4" spans="1:10">
@@ -4338,7 +4338,7 @@
         <v>794</v>
       </c>
       <c r="J8">
-        <v>561</v>
+        <v>566</v>
       </c>
     </row>
     <row r="9" spans="1:10">
@@ -4370,7 +4370,7 @@
         <v>433</v>
       </c>
       <c r="J9">
-        <v>191</v>
+        <v>193</v>
       </c>
     </row>
     <row r="10" spans="1:10">
@@ -4402,7 +4402,7 @@
         <v>1302</v>
       </c>
       <c r="J10">
-        <v>662</v>
+        <v>667</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -4434,7 +4434,7 @@
         <v>3950</v>
       </c>
       <c r="J11">
-        <v>2175</v>
+        <v>2190</v>
       </c>
     </row>
   </sheetData>
@@ -4555,7 +4555,7 @@
         <v>16</v>
       </c>
       <c r="J3">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="4" spans="1:10">
@@ -4697,7 +4697,7 @@
         <v>131</v>
       </c>
       <c r="J8">
-        <v>130</v>
+        <v>131</v>
       </c>
     </row>
     <row r="9" spans="1:10">
@@ -4729,7 +4729,7 @@
         <v>122</v>
       </c>
       <c r="J9">
-        <v>45</v>
+        <v>46</v>
       </c>
     </row>
     <row r="10" spans="1:10">
@@ -4761,7 +4761,7 @@
         <v>921</v>
       </c>
       <c r="J10">
-        <v>370</v>
+        <v>372</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -4793,7 +4793,7 @@
         <v>1318</v>
       </c>
       <c r="J11">
-        <v>631</v>
+        <v>636</v>
       </c>
     </row>
   </sheetData>
@@ -4914,7 +4914,7 @@
         <v>280</v>
       </c>
       <c r="J3">
-        <v>113</v>
+        <v>112</v>
       </c>
     </row>
     <row r="4" spans="1:10">
@@ -4978,7 +4978,7 @@
         <v>191</v>
       </c>
       <c r="J5">
-        <v>86</v>
+        <v>87</v>
       </c>
     </row>
     <row r="6" spans="1:10">
@@ -5074,7 +5074,7 @@
         <v>653</v>
       </c>
       <c r="J8">
-        <v>494</v>
+        <v>495</v>
       </c>
     </row>
     <row r="9" spans="1:10">
@@ -5106,7 +5106,7 @@
         <v>428</v>
       </c>
       <c r="J9">
-        <v>265</v>
+        <v>267</v>
       </c>
     </row>
     <row r="10" spans="1:10">
@@ -5138,7 +5138,7 @@
         <v>1089</v>
       </c>
       <c r="J10">
-        <v>601</v>
+        <v>609</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -5170,7 +5170,7 @@
         <v>2956</v>
       </c>
       <c r="J11">
-        <v>1730</v>
+        <v>1741</v>
       </c>
     </row>
   </sheetData>
@@ -5259,7 +5259,7 @@
         <v>918</v>
       </c>
       <c r="J2">
-        <v>512</v>
+        <v>517</v>
       </c>
     </row>
     <row r="3" spans="1:10">
@@ -5323,7 +5323,7 @@
         <v>436</v>
       </c>
       <c r="J4">
-        <v>237</v>
+        <v>238</v>
       </c>
     </row>
     <row r="5" spans="1:10">
@@ -5355,7 +5355,7 @@
         <v>247</v>
       </c>
       <c r="J5">
-        <v>146</v>
+        <v>148</v>
       </c>
     </row>
     <row r="6" spans="1:10">
@@ -5387,7 +5387,7 @@
         <v>793</v>
       </c>
       <c r="J6">
-        <v>520</v>
+        <v>521</v>
       </c>
     </row>
     <row r="7" spans="1:10">
@@ -5419,7 +5419,7 @@
         <v>2685</v>
       </c>
       <c r="J7">
-        <v>1529</v>
+        <v>1537</v>
       </c>
     </row>
     <row r="8" spans="1:10">
@@ -5451,7 +5451,7 @@
         <v>4744</v>
       </c>
       <c r="J8">
-        <v>2570</v>
+        <v>2588</v>
       </c>
     </row>
     <row r="9" spans="1:10">
@@ -5483,7 +5483,7 @@
         <v>519</v>
       </c>
       <c r="J9">
-        <v>283</v>
+        <v>284</v>
       </c>
     </row>
     <row r="10" spans="1:10">
@@ -5515,7 +5515,7 @@
         <v>949</v>
       </c>
       <c r="J10">
-        <v>477</v>
+        <v>481</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -5547,7 +5547,7 @@
         <v>1713</v>
       </c>
       <c r="J11">
-        <v>1014</v>
+        <v>1022</v>
       </c>
     </row>
     <row r="12" spans="1:10">
@@ -5643,7 +5643,7 @@
         <v>719</v>
       </c>
       <c r="J14">
-        <v>323</v>
+        <v>328</v>
       </c>
     </row>
     <row r="15" spans="1:10">
@@ -5675,7 +5675,7 @@
         <v>886</v>
       </c>
       <c r="J15">
-        <v>538</v>
+        <v>541</v>
       </c>
     </row>
     <row r="16" spans="1:10">
@@ -5771,7 +5771,7 @@
         <v>695</v>
       </c>
       <c r="J18">
-        <v>396</v>
+        <v>399</v>
       </c>
     </row>
     <row r="19" spans="1:10">
@@ -5803,7 +5803,7 @@
         <v>2636</v>
       </c>
       <c r="J19">
-        <v>1403</v>
+        <v>1412</v>
       </c>
     </row>
     <row r="20" spans="1:10">
@@ -5835,7 +5835,7 @@
         <v>2046</v>
       </c>
       <c r="J20">
-        <v>991</v>
+        <v>1001</v>
       </c>
     </row>
     <row r="21" spans="1:10">
@@ -5899,7 +5899,7 @@
         <v>418</v>
       </c>
       <c r="J22">
-        <v>272</v>
+        <v>273</v>
       </c>
     </row>
     <row r="23" spans="1:10">
@@ -5931,7 +5931,7 @@
         <v>1368</v>
       </c>
       <c r="J23">
-        <v>786</v>
+        <v>789</v>
       </c>
     </row>
     <row r="24" spans="1:10">
@@ -5963,7 +5963,7 @@
         <v>500</v>
       </c>
       <c r="J24">
-        <v>316</v>
+        <v>322</v>
       </c>
     </row>
     <row r="25" spans="1:10">
@@ -6027,7 +6027,7 @@
         <v>248</v>
       </c>
       <c r="J26">
-        <v>149</v>
+        <v>150</v>
       </c>
     </row>
     <row r="27" spans="1:10">
@@ -6059,7 +6059,7 @@
         <v>1258</v>
       </c>
       <c r="J27">
-        <v>710</v>
+        <v>713</v>
       </c>
     </row>
     <row r="28" spans="1:10">
@@ -6123,7 +6123,7 @@
         <v>3950</v>
       </c>
       <c r="J29">
-        <v>2175</v>
+        <v>2190</v>
       </c>
     </row>
     <row r="30" spans="1:10">
@@ -6187,7 +6187,7 @@
         <v>867</v>
       </c>
       <c r="J31">
-        <v>451</v>
+        <v>453</v>
       </c>
     </row>
     <row r="32" spans="1:10">
@@ -6251,7 +6251,7 @@
         <v>3011</v>
       </c>
       <c r="J33">
-        <v>1718</v>
+        <v>1728</v>
       </c>
     </row>
     <row r="34" spans="1:10">
@@ -6283,7 +6283,7 @@
         <v>761</v>
       </c>
       <c r="J34">
-        <v>466</v>
+        <v>469</v>
       </c>
     </row>
     <row r="35" spans="1:10">
@@ -6315,7 +6315,7 @@
         <v>235</v>
       </c>
       <c r="J35">
-        <v>120</v>
+        <v>123</v>
       </c>
     </row>
     <row r="36" spans="1:10">
@@ -6347,7 +6347,7 @@
         <v>1491</v>
       </c>
       <c r="J36">
-        <v>866</v>
+        <v>871</v>
       </c>
     </row>
     <row r="37" spans="1:10">
@@ -6379,7 +6379,7 @@
         <v>2547</v>
       </c>
       <c r="J37">
-        <v>1447</v>
+        <v>1464</v>
       </c>
     </row>
     <row r="38" spans="1:10">
@@ -6443,7 +6443,7 @@
         <v>153</v>
       </c>
       <c r="J39">
-        <v>53</v>
+        <v>54</v>
       </c>
     </row>
     <row r="40" spans="1:10">
@@ -6475,7 +6475,7 @@
         <v>236</v>
       </c>
       <c r="J40">
-        <v>142</v>
+        <v>143</v>
       </c>
     </row>
     <row r="41" spans="1:10">
@@ -6539,7 +6539,7 @@
         <v>2956</v>
       </c>
       <c r="J42">
-        <v>1730</v>
+        <v>1741</v>
       </c>
     </row>
     <row r="43" spans="1:10">
@@ -6571,7 +6571,7 @@
         <v>1153</v>
       </c>
       <c r="J43">
-        <v>714</v>
+        <v>720</v>
       </c>
     </row>
     <row r="44" spans="1:10">
@@ -6603,7 +6603,7 @@
         <v>1228</v>
       </c>
       <c r="J44">
-        <v>674</v>
+        <v>680</v>
       </c>
     </row>
     <row r="45" spans="1:10">
@@ -6635,7 +6635,7 @@
         <v>181</v>
       </c>
       <c r="J45">
-        <v>81</v>
+        <v>82</v>
       </c>
     </row>
     <row r="46" spans="1:10">
@@ -6699,7 +6699,7 @@
         <v>903</v>
       </c>
       <c r="J47">
-        <v>488</v>
+        <v>498</v>
       </c>
     </row>
     <row r="48" spans="1:10">
@@ -6731,7 +6731,7 @@
         <v>2622</v>
       </c>
       <c r="J48">
-        <v>1384</v>
+        <v>1391</v>
       </c>
     </row>
     <row r="49" spans="1:10">
@@ -6763,7 +6763,7 @@
         <v>1648</v>
       </c>
       <c r="J49">
-        <v>849</v>
+        <v>853</v>
       </c>
     </row>
     <row r="50" spans="1:10">
@@ -6795,7 +6795,7 @@
         <v>960</v>
       </c>
       <c r="J50">
-        <v>521</v>
+        <v>526</v>
       </c>
     </row>
     <row r="51" spans="1:10">
@@ -6827,7 +6827,7 @@
         <v>1337</v>
       </c>
       <c r="J51">
-        <v>807</v>
+        <v>813</v>
       </c>
     </row>
     <row r="52" spans="1:10">
@@ -6859,7 +6859,7 @@
         <v>1491</v>
       </c>
       <c r="J52">
-        <v>974</v>
+        <v>979</v>
       </c>
     </row>
     <row r="53" spans="1:10">
@@ -6891,7 +6891,7 @@
         <v>1601</v>
       </c>
       <c r="J53">
-        <v>1001</v>
+        <v>1010</v>
       </c>
     </row>
     <row r="54" spans="1:10">
@@ -6923,7 +6923,7 @@
         <v>3507</v>
       </c>
       <c r="J54">
-        <v>1817</v>
+        <v>1840</v>
       </c>
     </row>
     <row r="55" spans="1:10">
@@ -6955,7 +6955,7 @@
         <v>1244</v>
       </c>
       <c r="J55">
-        <v>630</v>
+        <v>633</v>
       </c>
     </row>
     <row r="56" spans="1:10">
@@ -7019,7 +7019,7 @@
         <v>406</v>
       </c>
       <c r="J57">
-        <v>270</v>
+        <v>271</v>
       </c>
     </row>
     <row r="58" spans="1:10">
@@ -7115,7 +7115,7 @@
         <v>768</v>
       </c>
       <c r="J60">
-        <v>446</v>
+        <v>447</v>
       </c>
     </row>
     <row r="61" spans="1:10">
@@ -7208,10 +7208,10 @@
         <v>2161</v>
       </c>
       <c r="I63">
-        <v>2469</v>
+        <v>2470</v>
       </c>
       <c r="J63">
-        <v>687</v>
+        <v>679</v>
       </c>
     </row>
     <row r="64" spans="1:10">
@@ -7243,7 +7243,7 @@
         <v>1187</v>
       </c>
       <c r="J64">
-        <v>575</v>
+        <v>579</v>
       </c>
     </row>
     <row r="65" spans="1:10">
@@ -7275,7 +7275,7 @@
         <v>1515</v>
       </c>
       <c r="J65">
-        <v>940</v>
+        <v>944</v>
       </c>
     </row>
     <row r="66" spans="1:10">
@@ -7307,7 +7307,7 @@
         <v>715</v>
       </c>
       <c r="J66">
-        <v>404</v>
+        <v>406</v>
       </c>
     </row>
     <row r="67" spans="1:10">
@@ -7339,7 +7339,7 @@
         <v>2510</v>
       </c>
       <c r="J67">
-        <v>1408</v>
+        <v>1418</v>
       </c>
     </row>
     <row r="68" spans="1:10">
@@ -7371,7 +7371,7 @@
         <v>437</v>
       </c>
       <c r="J68">
-        <v>183</v>
+        <v>185</v>
       </c>
     </row>
     <row r="69" spans="1:10">
@@ -7403,7 +7403,7 @@
         <v>494</v>
       </c>
       <c r="J69">
-        <v>224</v>
+        <v>227</v>
       </c>
     </row>
     <row r="70" spans="1:10">
@@ -7467,7 +7467,7 @@
         <v>335</v>
       </c>
       <c r="J71">
-        <v>241</v>
+        <v>243</v>
       </c>
     </row>
     <row r="72" spans="1:10">
@@ -7499,7 +7499,7 @@
         <v>706</v>
       </c>
       <c r="J72">
-        <v>351</v>
+        <v>354</v>
       </c>
     </row>
     <row r="73" spans="1:10">
@@ -7531,7 +7531,7 @@
         <v>1279</v>
       </c>
       <c r="J73">
-        <v>806</v>
+        <v>811</v>
       </c>
     </row>
     <row r="74" spans="1:10">
@@ -7595,7 +7595,7 @@
         <v>340</v>
       </c>
       <c r="J75">
-        <v>192</v>
+        <v>194</v>
       </c>
     </row>
     <row r="76" spans="1:10">
@@ -7627,7 +7627,7 @@
         <v>2923</v>
       </c>
       <c r="J76">
-        <v>1560</v>
+        <v>1572</v>
       </c>
     </row>
     <row r="77" spans="1:10">
@@ -7659,7 +7659,7 @@
         <v>462</v>
       </c>
       <c r="J77">
-        <v>279</v>
+        <v>284</v>
       </c>
     </row>
     <row r="78" spans="1:10">
@@ -7691,7 +7691,7 @@
         <v>1797</v>
       </c>
       <c r="J78">
-        <v>947</v>
+        <v>954</v>
       </c>
     </row>
     <row r="79" spans="1:10">
@@ -7723,7 +7723,7 @@
         <v>2472</v>
       </c>
       <c r="J79">
-        <v>1350</v>
+        <v>1353</v>
       </c>
     </row>
     <row r="80" spans="1:10">
@@ -7755,7 +7755,7 @@
         <v>393</v>
       </c>
       <c r="J80">
-        <v>163</v>
+        <v>164</v>
       </c>
     </row>
     <row r="81" spans="1:10">
@@ -7787,7 +7787,7 @@
         <v>219</v>
       </c>
       <c r="J81">
-        <v>117</v>
+        <v>118</v>
       </c>
     </row>
     <row r="82" spans="1:10">
@@ -7851,7 +7851,7 @@
         <v>1793</v>
       </c>
       <c r="J83">
-        <v>941</v>
+        <v>944</v>
       </c>
     </row>
     <row r="84" spans="1:10">
@@ -7883,7 +7883,7 @@
         <v>729</v>
       </c>
       <c r="J84">
-        <v>447</v>
+        <v>452</v>
       </c>
     </row>
     <row r="85" spans="1:10">
@@ -7915,7 +7915,7 @@
         <v>3848</v>
       </c>
       <c r="J85">
-        <v>2230</v>
+        <v>2239</v>
       </c>
     </row>
     <row r="86" spans="1:10">
@@ -7947,7 +7947,7 @@
         <v>1066</v>
       </c>
       <c r="J86">
-        <v>438</v>
+        <v>441</v>
       </c>
     </row>
     <row r="87" spans="1:10">
@@ -7979,7 +7979,7 @@
         <v>396</v>
       </c>
       <c r="J87">
-        <v>208</v>
+        <v>210</v>
       </c>
     </row>
     <row r="88" spans="1:10">
@@ -8011,7 +8011,7 @@
         <v>943</v>
       </c>
       <c r="J88">
-        <v>547</v>
+        <v>552</v>
       </c>
     </row>
     <row r="89" spans="1:10">
@@ -8043,7 +8043,7 @@
         <v>1878</v>
       </c>
       <c r="J89">
-        <v>1048</v>
+        <v>1050</v>
       </c>
     </row>
     <row r="90" spans="1:10">
@@ -8075,7 +8075,7 @@
         <v>1354</v>
       </c>
       <c r="J90">
-        <v>796</v>
+        <v>800</v>
       </c>
     </row>
     <row r="91" spans="1:10">
@@ -8107,7 +8107,7 @@
         <v>970</v>
       </c>
       <c r="J91">
-        <v>555</v>
+        <v>561</v>
       </c>
     </row>
     <row r="92" spans="1:10">
@@ -8139,7 +8139,7 @@
         <v>337</v>
       </c>
       <c r="J92">
-        <v>210</v>
+        <v>212</v>
       </c>
     </row>
     <row r="93" spans="1:10">
@@ -8171,7 +8171,7 @@
         <v>721</v>
       </c>
       <c r="J93">
-        <v>412</v>
+        <v>415</v>
       </c>
     </row>
     <row r="94" spans="1:10">
@@ -8203,7 +8203,7 @@
         <v>2664</v>
       </c>
       <c r="J94">
-        <v>1295</v>
+        <v>1305</v>
       </c>
     </row>
     <row r="95" spans="1:10">
@@ -8267,7 +8267,7 @@
         <v>1669</v>
       </c>
       <c r="J96">
-        <v>853</v>
+        <v>865</v>
       </c>
     </row>
     <row r="97" spans="1:10">
@@ -8299,7 +8299,7 @@
         <v>1673</v>
       </c>
       <c r="J97">
-        <v>903</v>
+        <v>909</v>
       </c>
     </row>
     <row r="98" spans="1:10">
@@ -8331,7 +8331,7 @@
         <v>1318</v>
       </c>
       <c r="J98">
-        <v>631</v>
+        <v>636</v>
       </c>
     </row>
     <row r="99" spans="1:10">
@@ -8363,7 +8363,7 @@
         <v>1488</v>
       </c>
       <c r="J99">
-        <v>839</v>
+        <v>847</v>
       </c>
     </row>
     <row r="100" spans="1:10">
@@ -8395,7 +8395,7 @@
         <v>237</v>
       </c>
       <c r="J100">
-        <v>160</v>
+        <v>162</v>
       </c>
     </row>
     <row r="101" spans="1:10">
@@ -8424,10 +8424,10 @@
         <v>84587</v>
       </c>
       <c r="I101">
-        <v>110477</v>
+        <v>110478</v>
       </c>
       <c r="J101">
-        <v>60362</v>
+        <v>60754</v>
       </c>
     </row>
   </sheetData>
@@ -8827,7 +8827,7 @@
         <v>97</v>
       </c>
       <c r="J9">
-        <v>60</v>
+        <v>61</v>
       </c>
     </row>
     <row r="10" spans="1:10">
@@ -8859,7 +8859,7 @@
         <v>1135</v>
       </c>
       <c r="J10">
-        <v>577</v>
+        <v>580</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -8891,7 +8891,7 @@
         <v>1648</v>
       </c>
       <c r="J11">
-        <v>849</v>
+        <v>853</v>
       </c>
     </row>
   </sheetData>
@@ -8980,7 +8980,7 @@
         <v>327</v>
       </c>
       <c r="J2">
-        <v>156</v>
+        <v>158</v>
       </c>
     </row>
     <row r="3" spans="1:10">
@@ -9012,7 +9012,7 @@
         <v>439</v>
       </c>
       <c r="J3">
-        <v>228</v>
+        <v>229</v>
       </c>
     </row>
     <row r="4" spans="1:10">
@@ -9172,7 +9172,7 @@
         <v>1026</v>
       </c>
       <c r="J8">
-        <v>755</v>
+        <v>757</v>
       </c>
     </row>
     <row r="9" spans="1:10">
@@ -9204,7 +9204,7 @@
         <v>303</v>
       </c>
       <c r="J9">
-        <v>172</v>
+        <v>175</v>
       </c>
     </row>
     <row r="10" spans="1:10">
@@ -9236,7 +9236,7 @@
         <v>1271</v>
       </c>
       <c r="J10">
-        <v>684</v>
+        <v>685</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -9268,7 +9268,7 @@
         <v>3848</v>
       </c>
       <c r="J11">
-        <v>2230</v>
+        <v>2239</v>
       </c>
     </row>
   </sheetData>
@@ -9450,7 +9450,7 @@
         <v>73</v>
       </c>
       <c r="J5">
-        <v>64</v>
+        <v>65</v>
       </c>
     </row>
     <row r="6" spans="1:10">
@@ -9546,7 +9546,7 @@
         <v>336</v>
       </c>
       <c r="J8">
-        <v>163</v>
+        <v>167</v>
       </c>
     </row>
     <row r="9" spans="1:10">
@@ -9578,7 +9578,7 @@
         <v>179</v>
       </c>
       <c r="J9">
-        <v>105</v>
+        <v>106</v>
       </c>
     </row>
     <row r="10" spans="1:10">
@@ -9610,7 +9610,7 @@
         <v>2132</v>
       </c>
       <c r="J10">
-        <v>1131</v>
+        <v>1137</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -9642,7 +9642,7 @@
         <v>2923</v>
       </c>
       <c r="J11">
-        <v>1560</v>
+        <v>1572</v>
       </c>
     </row>
   </sheetData>
@@ -9946,7 +9946,7 @@
         <v>156</v>
       </c>
       <c r="J9">
-        <v>59</v>
+        <v>61</v>
       </c>
     </row>
     <row r="10" spans="1:10">
@@ -9978,7 +9978,7 @@
         <v>1034</v>
       </c>
       <c r="J10">
-        <v>448</v>
+        <v>452</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -10010,7 +10010,7 @@
         <v>1673</v>
       </c>
       <c r="J11">
-        <v>903</v>
+        <v>909</v>
       </c>
     </row>
   </sheetData>
@@ -10099,7 +10099,7 @@
         <v>235</v>
       </c>
       <c r="J2">
-        <v>119</v>
+        <v>120</v>
       </c>
     </row>
     <row r="3" spans="1:10">
@@ -10131,7 +10131,7 @@
         <v>365</v>
       </c>
       <c r="J3">
-        <v>214</v>
+        <v>215</v>
       </c>
     </row>
     <row r="4" spans="1:10">
@@ -10195,7 +10195,7 @@
         <v>102</v>
       </c>
       <c r="J5">
-        <v>58</v>
+        <v>60</v>
       </c>
     </row>
     <row r="6" spans="1:10">
@@ -10259,7 +10259,7 @@
         <v>29</v>
       </c>
       <c r="J7">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="8" spans="1:10">
@@ -10291,7 +10291,7 @@
         <v>516</v>
       </c>
       <c r="J8">
-        <v>370</v>
+        <v>372</v>
       </c>
     </row>
     <row r="9" spans="1:10">
@@ -10355,7 +10355,7 @@
         <v>895</v>
       </c>
       <c r="J10">
-        <v>439</v>
+        <v>442</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -10387,7 +10387,7 @@
         <v>2510</v>
       </c>
       <c r="J11">
-        <v>1408</v>
+        <v>1418</v>
       </c>
     </row>
   </sheetData>
@@ -10853,7 +10853,7 @@
         <v>83</v>
       </c>
       <c r="J2">
-        <v>38</v>
+        <v>40</v>
       </c>
     </row>
     <row r="3" spans="1:10">
@@ -10949,7 +10949,7 @@
         <v>39</v>
       </c>
       <c r="J5">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="6" spans="1:10">
@@ -11109,7 +11109,7 @@
         <v>271</v>
       </c>
       <c r="J10">
-        <v>135</v>
+        <v>137</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -11141,7 +11141,7 @@
         <v>729</v>
       </c>
       <c r="J11">
-        <v>447</v>
+        <v>452</v>
       </c>
     </row>
   </sheetData>
@@ -11230,7 +11230,7 @@
         <v>146</v>
       </c>
       <c r="J2">
-        <v>83</v>
+        <v>84</v>
       </c>
     </row>
     <row r="3" spans="1:10">
@@ -11422,7 +11422,7 @@
         <v>218</v>
       </c>
       <c r="J8">
-        <v>190</v>
+        <v>191</v>
       </c>
     </row>
     <row r="9" spans="1:10">
@@ -11454,7 +11454,7 @@
         <v>196</v>
       </c>
       <c r="J9">
-        <v>164</v>
+        <v>165</v>
       </c>
     </row>
     <row r="10" spans="1:10">
@@ -11486,7 +11486,7 @@
         <v>590</v>
       </c>
       <c r="J10">
-        <v>356</v>
+        <v>358</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -11518,7 +11518,7 @@
         <v>1491</v>
       </c>
       <c r="J11">
-        <v>974</v>
+        <v>979</v>
       </c>
     </row>
   </sheetData>
@@ -11607,7 +11607,7 @@
         <v>67</v>
       </c>
       <c r="J2">
-        <v>33</v>
+        <v>34</v>
       </c>
     </row>
     <row r="3" spans="1:10">
@@ -11639,7 +11639,7 @@
         <v>78</v>
       </c>
       <c r="J3">
-        <v>49</v>
+        <v>50</v>
       </c>
     </row>
     <row r="4" spans="1:10">
@@ -11671,7 +11671,7 @@
         <v>9</v>
       </c>
       <c r="J4">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="5" spans="1:10">
@@ -11799,7 +11799,7 @@
         <v>184</v>
       </c>
       <c r="J8">
-        <v>147</v>
+        <v>148</v>
       </c>
     </row>
     <row r="9" spans="1:10">
@@ -11863,7 +11863,7 @@
         <v>474</v>
       </c>
       <c r="J10">
-        <v>217</v>
+        <v>218</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -11895,7 +11895,7 @@
         <v>943</v>
       </c>
       <c r="J11">
-        <v>547</v>
+        <v>552</v>
       </c>
     </row>
   </sheetData>
@@ -12016,7 +12016,7 @@
         <v>111</v>
       </c>
       <c r="J3">
-        <v>53</v>
+        <v>54</v>
       </c>
     </row>
     <row r="4" spans="1:10">
@@ -12173,7 +12173,7 @@
         <v>401</v>
       </c>
       <c r="J8">
-        <v>217</v>
+        <v>219</v>
       </c>
     </row>
     <row r="9" spans="1:10">
@@ -12205,7 +12205,7 @@
         <v>243</v>
       </c>
       <c r="J9">
-        <v>124</v>
+        <v>131</v>
       </c>
     </row>
     <row r="10" spans="1:10">
@@ -12237,7 +12237,7 @@
         <v>2528</v>
       </c>
       <c r="J10">
-        <v>1303</v>
+        <v>1316</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -12269,7 +12269,7 @@
         <v>3507</v>
       </c>
       <c r="J11">
-        <v>1817</v>
+        <v>1840</v>
       </c>
     </row>
   </sheetData>
@@ -12550,7 +12550,7 @@
         <v>503</v>
       </c>
       <c r="J8">
-        <v>325</v>
+        <v>328</v>
       </c>
     </row>
     <row r="9" spans="1:10">
@@ -12614,7 +12614,7 @@
         <v>527</v>
       </c>
       <c r="J10">
-        <v>300</v>
+        <v>302</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -12646,7 +12646,7 @@
         <v>1491</v>
       </c>
       <c r="J11">
-        <v>866</v>
+        <v>871</v>
       </c>
     </row>
   </sheetData>
@@ -12735,7 +12735,7 @@
         <v>239</v>
       </c>
       <c r="J2">
-        <v>127</v>
+        <v>130</v>
       </c>
     </row>
     <row r="3" spans="1:10">
@@ -12767,7 +12767,7 @@
         <v>261</v>
       </c>
       <c r="J3">
-        <v>155</v>
+        <v>156</v>
       </c>
     </row>
     <row r="4" spans="1:10">
@@ -12831,7 +12831,7 @@
         <v>200</v>
       </c>
       <c r="J5">
-        <v>118</v>
+        <v>119</v>
       </c>
     </row>
     <row r="6" spans="1:10">
@@ -12927,7 +12927,7 @@
         <v>722</v>
       </c>
       <c r="J8">
-        <v>466</v>
+        <v>474</v>
       </c>
     </row>
     <row r="9" spans="1:10">
@@ -12959,7 +12959,7 @@
         <v>244</v>
       </c>
       <c r="J9">
-        <v>126</v>
+        <v>127</v>
       </c>
     </row>
     <row r="10" spans="1:10">
@@ -12991,7 +12991,7 @@
         <v>813</v>
       </c>
       <c r="J10">
-        <v>422</v>
+        <v>425</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -13023,7 +13023,7 @@
         <v>2547</v>
       </c>
       <c r="J11">
-        <v>1447</v>
+        <v>1464</v>
       </c>
     </row>
   </sheetData>
@@ -13347,7 +13347,7 @@
         <v>213</v>
       </c>
       <c r="J10">
-        <v>123</v>
+        <v>124</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -13379,7 +13379,7 @@
         <v>418</v>
       </c>
       <c r="J11">
-        <v>272</v>
+        <v>273</v>
       </c>
     </row>
   </sheetData>
@@ -13645,7 +13645,7 @@
         <v>89</v>
       </c>
       <c r="J8">
-        <v>67</v>
+        <v>69</v>
       </c>
     </row>
     <row r="9" spans="1:10">
@@ -13709,7 +13709,7 @@
         <v>448</v>
       </c>
       <c r="J10">
-        <v>206</v>
+        <v>207</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -13741,7 +13741,7 @@
         <v>706</v>
       </c>
       <c r="J11">
-        <v>351</v>
+        <v>354</v>
       </c>
     </row>
   </sheetData>
@@ -13862,7 +13862,7 @@
         <v>182</v>
       </c>
       <c r="J3">
-        <v>111</v>
+        <v>112</v>
       </c>
     </row>
     <row r="4" spans="1:10">
@@ -13958,7 +13958,7 @@
         <v>26</v>
       </c>
       <c r="J6">
-        <v>15</v>
+        <v>16</v>
       </c>
     </row>
     <row r="7" spans="1:10">
@@ -14022,7 +14022,7 @@
         <v>202</v>
       </c>
       <c r="J8">
-        <v>206</v>
+        <v>207</v>
       </c>
     </row>
     <row r="9" spans="1:10">
@@ -14054,7 +14054,7 @@
         <v>189</v>
       </c>
       <c r="J9">
-        <v>125</v>
+        <v>126</v>
       </c>
     </row>
     <row r="10" spans="1:10">
@@ -14118,7 +14118,7 @@
         <v>1515</v>
       </c>
       <c r="J11">
-        <v>940</v>
+        <v>944</v>
       </c>
     </row>
   </sheetData>
@@ -14734,7 +14734,7 @@
         <v>175</v>
       </c>
       <c r="J8">
-        <v>139</v>
+        <v>140</v>
       </c>
     </row>
     <row r="9" spans="1:10">
@@ -14830,7 +14830,7 @@
         <v>768</v>
       </c>
       <c r="J11">
-        <v>446</v>
+        <v>447</v>
       </c>
     </row>
   </sheetData>
@@ -14919,7 +14919,7 @@
         <v>29</v>
       </c>
       <c r="J2">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="3" spans="1:10">
@@ -15096,7 +15096,7 @@
         <v>57</v>
       </c>
       <c r="J8">
-        <v>29</v>
+        <v>30</v>
       </c>
     </row>
     <row r="9" spans="1:10">
@@ -15192,7 +15192,7 @@
         <v>437</v>
       </c>
       <c r="J11">
-        <v>183</v>
+        <v>185</v>
       </c>
     </row>
   </sheetData>
@@ -15281,7 +15281,7 @@
         <v>190</v>
       </c>
       <c r="J2">
-        <v>89</v>
+        <v>90</v>
       </c>
     </row>
     <row r="3" spans="1:10">
@@ -15377,7 +15377,7 @@
         <v>124</v>
       </c>
       <c r="J5">
-        <v>49</v>
+        <v>50</v>
       </c>
     </row>
     <row r="6" spans="1:10">
@@ -15537,7 +15537,7 @@
         <v>612</v>
       </c>
       <c r="J10">
-        <v>305</v>
+        <v>306</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -15569,7 +15569,7 @@
         <v>1793</v>
       </c>
       <c r="J11">
-        <v>941</v>
+        <v>944</v>
       </c>
     </row>
   </sheetData>
@@ -15754,7 +15754,7 @@
         <v>90</v>
       </c>
       <c r="J5">
-        <v>41</v>
+        <v>42</v>
       </c>
     </row>
     <row r="6" spans="1:10">
@@ -15850,7 +15850,7 @@
         <v>224</v>
       </c>
       <c r="J8">
-        <v>163</v>
+        <v>164</v>
       </c>
     </row>
     <row r="9" spans="1:10">
@@ -15882,7 +15882,7 @@
         <v>109</v>
       </c>
       <c r="J9">
-        <v>80</v>
+        <v>81</v>
       </c>
     </row>
     <row r="10" spans="1:10">
@@ -15946,7 +15946,7 @@
         <v>1244</v>
       </c>
       <c r="J11">
-        <v>630</v>
+        <v>633</v>
       </c>
     </row>
   </sheetData>
@@ -16119,7 +16119,7 @@
         <v>86</v>
       </c>
       <c r="J5">
-        <v>52</v>
+        <v>53</v>
       </c>
     </row>
     <row r="6" spans="1:10">
@@ -16244,7 +16244,7 @@
         <v>147</v>
       </c>
       <c r="J9">
-        <v>61</v>
+        <v>62</v>
       </c>
     </row>
     <row r="10" spans="1:10">
@@ -16276,7 +16276,7 @@
         <v>2021</v>
       </c>
       <c r="J10">
-        <v>926</v>
+        <v>934</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -16308,7 +16308,7 @@
         <v>2664</v>
       </c>
       <c r="J11">
-        <v>1295</v>
+        <v>1305</v>
       </c>
     </row>
   </sheetData>
@@ -16397,7 +16397,7 @@
         <v>267</v>
       </c>
       <c r="J2">
-        <v>163</v>
+        <v>164</v>
       </c>
     </row>
     <row r="3" spans="1:10">
@@ -16429,7 +16429,7 @@
         <v>416</v>
       </c>
       <c r="J3">
-        <v>201</v>
+        <v>204</v>
       </c>
     </row>
     <row r="4" spans="1:10">
@@ -16461,7 +16461,7 @@
         <v>24</v>
       </c>
       <c r="J4">
-        <v>12</v>
+        <v>13</v>
       </c>
     </row>
     <row r="5" spans="1:10">
@@ -16525,7 +16525,7 @@
         <v>49</v>
       </c>
       <c r="J6">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="7" spans="1:10">
@@ -16589,7 +16589,7 @@
         <v>707</v>
       </c>
       <c r="J8">
-        <v>522</v>
+        <v>524</v>
       </c>
     </row>
     <row r="9" spans="1:10">
@@ -16621,7 +16621,7 @@
         <v>363</v>
       </c>
       <c r="J9">
-        <v>201</v>
+        <v>203</v>
       </c>
     </row>
     <row r="10" spans="1:10">
@@ -16653,7 +16653,7 @@
         <v>968</v>
       </c>
       <c r="J10">
-        <v>504</v>
+        <v>506</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -16685,7 +16685,7 @@
         <v>3011</v>
       </c>
       <c r="J11">
-        <v>1718</v>
+        <v>1728</v>
       </c>
     </row>
   </sheetData>
@@ -16774,7 +16774,7 @@
         <v>264</v>
       </c>
       <c r="J2">
-        <v>134</v>
+        <v>135</v>
       </c>
     </row>
     <row r="3" spans="1:10">
@@ -16966,7 +16966,7 @@
         <v>567</v>
       </c>
       <c r="J8">
-        <v>517</v>
+        <v>521</v>
       </c>
     </row>
     <row r="9" spans="1:10">
@@ -17030,7 +17030,7 @@
         <v>1023</v>
       </c>
       <c r="J10">
-        <v>471</v>
+        <v>474</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -17062,7 +17062,7 @@
         <v>2685</v>
       </c>
       <c r="J11">
-        <v>1529</v>
+        <v>1537</v>
       </c>
     </row>
   </sheetData>
@@ -17151,7 +17151,7 @@
         <v>457</v>
       </c>
       <c r="J2">
-        <v>259</v>
+        <v>261</v>
       </c>
     </row>
     <row r="3" spans="1:10">
@@ -17183,7 +17183,7 @@
         <v>445</v>
       </c>
       <c r="J3">
-        <v>281</v>
+        <v>282</v>
       </c>
     </row>
     <row r="4" spans="1:10">
@@ -17215,7 +17215,7 @@
         <v>30</v>
       </c>
       <c r="J4">
-        <v>20</v>
+        <v>21</v>
       </c>
     </row>
     <row r="5" spans="1:10">
@@ -17279,7 +17279,7 @@
         <v>93</v>
       </c>
       <c r="J6">
-        <v>48</v>
+        <v>49</v>
       </c>
     </row>
     <row r="7" spans="1:10">
@@ -17343,7 +17343,7 @@
         <v>1270</v>
       </c>
       <c r="J8">
-        <v>701</v>
+        <v>706</v>
       </c>
     </row>
     <row r="9" spans="1:10">
@@ -17375,7 +17375,7 @@
         <v>497</v>
       </c>
       <c r="J9">
-        <v>279</v>
+        <v>281</v>
       </c>
     </row>
     <row r="10" spans="1:10">
@@ -17407,7 +17407,7 @@
         <v>1652</v>
       </c>
       <c r="J10">
-        <v>845</v>
+        <v>851</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -17439,7 +17439,7 @@
         <v>4744</v>
       </c>
       <c r="J11">
-        <v>2570</v>
+        <v>2588</v>
       </c>
     </row>
   </sheetData>
@@ -17720,7 +17720,7 @@
         <v>441</v>
       </c>
       <c r="J8">
-        <v>313</v>
+        <v>316</v>
       </c>
     </row>
     <row r="9" spans="1:10">
@@ -17784,7 +17784,7 @@
         <v>455</v>
       </c>
       <c r="J10">
-        <v>273</v>
+        <v>274</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -17816,7 +17816,7 @@
         <v>1354</v>
       </c>
       <c r="J11">
-        <v>796</v>
+        <v>800</v>
       </c>
     </row>
   </sheetData>
@@ -18085,7 +18085,7 @@
         <v>250</v>
       </c>
       <c r="J8">
-        <v>161</v>
+        <v>167</v>
       </c>
     </row>
     <row r="9" spans="1:10">
@@ -18149,7 +18149,7 @@
         <v>417</v>
       </c>
       <c r="J10">
-        <v>203</v>
+        <v>207</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -18181,7 +18181,7 @@
         <v>903</v>
       </c>
       <c r="J11">
-        <v>488</v>
+        <v>498</v>
       </c>
     </row>
   </sheetData>
@@ -18398,7 +18398,7 @@
         <v>27</v>
       </c>
       <c r="J6">
-        <v>22</v>
+        <v>23</v>
       </c>
     </row>
     <row r="7" spans="1:10">
@@ -18462,7 +18462,7 @@
         <v>754</v>
       </c>
       <c r="J8">
-        <v>395</v>
+        <v>399</v>
       </c>
     </row>
     <row r="9" spans="1:10">
@@ -18526,7 +18526,7 @@
         <v>911</v>
       </c>
       <c r="J10">
-        <v>495</v>
+        <v>499</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -18558,7 +18558,7 @@
         <v>2636</v>
       </c>
       <c r="J11">
-        <v>1403</v>
+        <v>1412</v>
       </c>
     </row>
   </sheetData>
@@ -18647,7 +18647,7 @@
         <v>22</v>
       </c>
       <c r="J2">
-        <v>12</v>
+        <v>13</v>
       </c>
     </row>
     <row r="3" spans="1:10">
@@ -18876,7 +18876,7 @@
         <v>94</v>
       </c>
       <c r="J10">
-        <v>53</v>
+        <v>54</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -18908,7 +18908,7 @@
         <v>247</v>
       </c>
       <c r="J11">
-        <v>146</v>
+        <v>148</v>
       </c>
     </row>
   </sheetData>
@@ -18997,7 +18997,7 @@
         <v>179</v>
       </c>
       <c r="J2">
-        <v>84</v>
+        <v>85</v>
       </c>
     </row>
     <row r="3" spans="1:10">
@@ -19189,7 +19189,7 @@
         <v>364</v>
       </c>
       <c r="J8">
-        <v>256</v>
+        <v>260</v>
       </c>
     </row>
     <row r="9" spans="1:10">
@@ -19221,7 +19221,7 @@
         <v>224</v>
       </c>
       <c r="J9">
-        <v>72</v>
+        <v>74</v>
       </c>
     </row>
     <row r="10" spans="1:10">
@@ -19253,7 +19253,7 @@
         <v>828</v>
       </c>
       <c r="J10">
-        <v>385</v>
+        <v>388</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -19285,7 +19285,7 @@
         <v>2046</v>
       </c>
       <c r="J11">
-        <v>991</v>
+        <v>1001</v>
       </c>
     </row>
   </sheetData>
@@ -19554,7 +19554,7 @@
         <v>98</v>
       </c>
       <c r="J8">
-        <v>86</v>
+        <v>88</v>
       </c>
     </row>
     <row r="9" spans="1:10">
@@ -19586,7 +19586,7 @@
         <v>45</v>
       </c>
       <c r="J9">
-        <v>21</v>
+        <v>23</v>
       </c>
     </row>
     <row r="10" spans="1:10">
@@ -19618,7 +19618,7 @@
         <v>630</v>
       </c>
       <c r="J10">
-        <v>286</v>
+        <v>287</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -19650,7 +19650,7 @@
         <v>960</v>
       </c>
       <c r="J11">
-        <v>521</v>
+        <v>526</v>
       </c>
     </row>
   </sheetData>
@@ -20101,7 +20101,7 @@
         <v>87</v>
       </c>
       <c r="J2">
-        <v>48</v>
+        <v>49</v>
       </c>
     </row>
     <row r="3" spans="1:10">
@@ -20261,7 +20261,7 @@
         <v>2</v>
       </c>
       <c r="J7">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="8" spans="1:10">
@@ -20293,7 +20293,7 @@
         <v>308</v>
       </c>
       <c r="J8">
-        <v>199</v>
+        <v>203</v>
       </c>
     </row>
     <row r="9" spans="1:10">
@@ -20389,7 +20389,7 @@
         <v>970</v>
       </c>
       <c r="J11">
-        <v>555</v>
+        <v>561</v>
       </c>
     </row>
   </sheetData>
@@ -20574,7 +20574,7 @@
         <v>64</v>
       </c>
       <c r="J5">
-        <v>44</v>
+        <v>45</v>
       </c>
     </row>
     <row r="6" spans="1:10">
@@ -20696,7 +20696,7 @@
         <v>62</v>
       </c>
       <c r="J9">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="10" spans="1:10">
@@ -20728,7 +20728,7 @@
         <v>381</v>
       </c>
       <c r="J10">
-        <v>181</v>
+        <v>182</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -20760,7 +20760,7 @@
         <v>721</v>
       </c>
       <c r="J11">
-        <v>412</v>
+        <v>415</v>
       </c>
     </row>
   </sheetData>
@@ -21452,7 +21452,7 @@
         <v>216</v>
       </c>
       <c r="J10">
-        <v>107</v>
+        <v>108</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -21484,7 +21484,7 @@
         <v>436</v>
       </c>
       <c r="J11">
-        <v>237</v>
+        <v>238</v>
       </c>
     </row>
   </sheetData>
@@ -21605,7 +21605,7 @@
         <v>81</v>
       </c>
       <c r="J3">
-        <v>49</v>
+        <v>50</v>
       </c>
     </row>
     <row r="4" spans="1:10">
@@ -21762,7 +21762,7 @@
         <v>297</v>
       </c>
       <c r="J8">
-        <v>257</v>
+        <v>260</v>
       </c>
     </row>
     <row r="9" spans="1:10">
@@ -21826,7 +21826,7 @@
         <v>670</v>
       </c>
       <c r="J10">
-        <v>327</v>
+        <v>329</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -21858,7 +21858,7 @@
         <v>1337</v>
       </c>
       <c r="J11">
-        <v>807</v>
+        <v>813</v>
       </c>
     </row>
   </sheetData>
@@ -22043,7 +22043,7 @@
         <v>83</v>
       </c>
       <c r="J5">
-        <v>47</v>
+        <v>48</v>
       </c>
     </row>
     <row r="6" spans="1:10">
@@ -22139,7 +22139,7 @@
         <v>126</v>
       </c>
       <c r="J8">
-        <v>73</v>
+        <v>74</v>
       </c>
     </row>
     <row r="9" spans="1:10">
@@ -22203,7 +22203,7 @@
         <v>492</v>
       </c>
       <c r="J10">
-        <v>294</v>
+        <v>297</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -22235,7 +22235,7 @@
         <v>918</v>
       </c>
       <c r="J11">
-        <v>512</v>
+        <v>517</v>
       </c>
     </row>
   </sheetData>
@@ -22863,7 +22863,7 @@
         <v>196</v>
       </c>
       <c r="J8">
-        <v>109</v>
+        <v>110</v>
       </c>
     </row>
     <row r="9" spans="1:10">
@@ -22927,7 +22927,7 @@
         <v>239</v>
       </c>
       <c r="J10">
-        <v>128</v>
+        <v>130</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -22959,7 +22959,7 @@
         <v>695</v>
       </c>
       <c r="J11">
-        <v>396</v>
+        <v>399</v>
       </c>
     </row>
   </sheetData>
@@ -23228,7 +23228,7 @@
         <v>92</v>
       </c>
       <c r="J8">
-        <v>87</v>
+        <v>90</v>
       </c>
     </row>
     <row r="9" spans="1:10">
@@ -23292,7 +23292,7 @@
         <v>277</v>
       </c>
       <c r="J10">
-        <v>159</v>
+        <v>162</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -23324,7 +23324,7 @@
         <v>500</v>
       </c>
       <c r="J11">
-        <v>316</v>
+        <v>322</v>
       </c>
     </row>
   </sheetData>
@@ -23880,7 +23880,7 @@
         <v>77</v>
       </c>
       <c r="J5">
-        <v>27</v>
+        <v>28</v>
       </c>
     </row>
     <row r="6" spans="1:10">
@@ -24072,7 +24072,7 @@
         <v>793</v>
       </c>
       <c r="J11">
-        <v>520</v>
+        <v>521</v>
       </c>
     </row>
   </sheetData>
@@ -24405,7 +24405,7 @@
         <v>216</v>
       </c>
       <c r="J10">
-        <v>105</v>
+        <v>107</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -24437,7 +24437,7 @@
         <v>396</v>
       </c>
       <c r="J11">
-        <v>208</v>
+        <v>210</v>
       </c>
     </row>
   </sheetData>
@@ -24770,7 +24770,7 @@
         <v>784</v>
       </c>
       <c r="J10">
-        <v>449</v>
+        <v>452</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -24802,7 +24802,7 @@
         <v>1258</v>
       </c>
       <c r="J11">
-        <v>710</v>
+        <v>713</v>
       </c>
     </row>
   </sheetData>
@@ -25147,7 +25147,7 @@
         <v>381</v>
       </c>
       <c r="J10">
-        <v>186</v>
+        <v>188</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -25179,7 +25179,7 @@
         <v>867</v>
       </c>
       <c r="J11">
-        <v>451</v>
+        <v>453</v>
       </c>
     </row>
   </sheetData>
@@ -25597,7 +25597,7 @@
         <v>53</v>
       </c>
       <c r="J2">
-        <v>38</v>
+        <v>40</v>
       </c>
     </row>
     <row r="3" spans="1:10">
@@ -25853,7 +25853,7 @@
         <v>130</v>
       </c>
       <c r="J10">
-        <v>74</v>
+        <v>77</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -25885,7 +25885,7 @@
         <v>462</v>
       </c>
       <c r="J11">
-        <v>279</v>
+        <v>284</v>
       </c>
     </row>
   </sheetData>
@@ -26298,7 +26298,7 @@
         <v>78</v>
       </c>
       <c r="J2">
-        <v>49</v>
+        <v>50</v>
       </c>
     </row>
     <row r="3" spans="1:10">
@@ -26554,7 +26554,7 @@
         <v>1118</v>
       </c>
       <c r="J10">
-        <v>556</v>
+        <v>562</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -26586,7 +26586,7 @@
         <v>1797</v>
       </c>
       <c r="J11">
-        <v>947</v>
+        <v>954</v>
       </c>
     </row>
   </sheetData>
@@ -26858,7 +26858,7 @@
         <v>110</v>
       </c>
       <c r="J8">
-        <v>79</v>
+        <v>82</v>
       </c>
     </row>
     <row r="9" spans="1:10">
@@ -26922,7 +26922,7 @@
         <v>371</v>
       </c>
       <c r="J10">
-        <v>143</v>
+        <v>145</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -26954,7 +26954,7 @@
         <v>719</v>
       </c>
       <c r="J11">
-        <v>323</v>
+        <v>328</v>
       </c>
     </row>
   </sheetData>
@@ -27237,7 +27237,7 @@
         <v>37</v>
       </c>
       <c r="J9">
-        <v>22</v>
+        <v>23</v>
       </c>
     </row>
     <row r="10" spans="1:10">
@@ -27269,7 +27269,7 @@
         <v>462</v>
       </c>
       <c r="J10">
-        <v>231</v>
+        <v>232</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -27301,7 +27301,7 @@
         <v>715</v>
       </c>
       <c r="J11">
-        <v>404</v>
+        <v>406</v>
       </c>
     </row>
   </sheetData>
@@ -27920,7 +27920,7 @@
         <v>141</v>
       </c>
       <c r="J8">
-        <v>94</v>
+        <v>95</v>
       </c>
     </row>
     <row r="9" spans="1:10">
@@ -28016,7 +28016,7 @@
         <v>519</v>
       </c>
       <c r="J11">
-        <v>283</v>
+        <v>284</v>
       </c>
     </row>
   </sheetData>
@@ -28644,7 +28644,7 @@
         <v>137</v>
       </c>
       <c r="J8">
-        <v>95</v>
+        <v>96</v>
       </c>
     </row>
     <row r="9" spans="1:10">
@@ -28676,7 +28676,7 @@
         <v>90</v>
       </c>
       <c r="J9">
-        <v>33</v>
+        <v>34</v>
       </c>
     </row>
     <row r="10" spans="1:10">
@@ -28708,7 +28708,7 @@
         <v>542</v>
       </c>
       <c r="J10">
-        <v>269</v>
+        <v>271</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -28740,7 +28740,7 @@
         <v>949</v>
       </c>
       <c r="J11">
-        <v>477</v>
+        <v>481</v>
       </c>
     </row>
   </sheetData>
@@ -29264,7 +29264,7 @@
         <v>4</v>
       </c>
       <c r="J4">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="5" spans="1:10">
@@ -29296,7 +29296,7 @@
         <v>131</v>
       </c>
       <c r="J5">
-        <v>68</v>
+        <v>70</v>
       </c>
     </row>
     <row r="6" spans="1:10">
@@ -29453,7 +29453,7 @@
         <v>1222</v>
       </c>
       <c r="J10">
-        <v>621</v>
+        <v>622</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -29485,7 +29485,7 @@
         <v>1878</v>
       </c>
       <c r="J11">
-        <v>1048</v>
+        <v>1050</v>
       </c>
     </row>
   </sheetData>
@@ -29827,7 +29827,7 @@
         <v>440</v>
       </c>
       <c r="J10">
-        <v>241</v>
+        <v>244</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -29859,7 +29859,7 @@
         <v>761</v>
       </c>
       <c r="J11">
-        <v>466</v>
+        <v>469</v>
       </c>
     </row>
   </sheetData>
@@ -29948,7 +29948,7 @@
         <v>128</v>
       </c>
       <c r="J2">
-        <v>59</v>
+        <v>60</v>
       </c>
     </row>
     <row r="3" spans="1:10">
@@ -29980,7 +29980,7 @@
         <v>158</v>
       </c>
       <c r="J3">
-        <v>71</v>
+        <v>74</v>
       </c>
     </row>
     <row r="4" spans="1:10">
@@ -30044,7 +30044,7 @@
         <v>120</v>
       </c>
       <c r="J5">
-        <v>72</v>
+        <v>73</v>
       </c>
     </row>
     <row r="6" spans="1:10">
@@ -30172,7 +30172,7 @@
         <v>118</v>
       </c>
       <c r="J9">
-        <v>52</v>
+        <v>53</v>
       </c>
     </row>
     <row r="10" spans="1:10">
@@ -30204,7 +30204,7 @@
         <v>527</v>
       </c>
       <c r="J10">
-        <v>292</v>
+        <v>294</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -30236,7 +30236,7 @@
         <v>1488</v>
       </c>
       <c r="J11">
-        <v>839</v>
+        <v>847</v>
       </c>
     </row>
   </sheetData>
@@ -30507,7 +30507,7 @@
         <v>22</v>
       </c>
       <c r="J9">
-        <v>17</v>
+        <v>18</v>
       </c>
     </row>
     <row r="10" spans="1:10">
@@ -30571,7 +30571,7 @@
         <v>248</v>
       </c>
       <c r="J11">
-        <v>149</v>
+        <v>150</v>
       </c>
     </row>
   </sheetData>
@@ -31183,7 +31183,7 @@
         <v>23</v>
       </c>
       <c r="J9">
-        <v>14</v>
+        <v>15</v>
       </c>
     </row>
     <row r="10" spans="1:10">
@@ -31215,7 +31215,7 @@
         <v>162</v>
       </c>
       <c r="J10">
-        <v>102</v>
+        <v>103</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -31247,7 +31247,7 @@
         <v>237</v>
       </c>
       <c r="J11">
-        <v>160</v>
+        <v>162</v>
       </c>
     </row>
   </sheetData>
@@ -31577,7 +31577,7 @@
         <v>124</v>
       </c>
       <c r="J10">
-        <v>68</v>
+        <v>70</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -31609,7 +31609,7 @@
         <v>335</v>
       </c>
       <c r="J11">
-        <v>241</v>
+        <v>243</v>
       </c>
     </row>
   </sheetData>
@@ -31794,7 +31794,7 @@
         <v>72</v>
       </c>
       <c r="J5">
-        <v>32</v>
+        <v>33</v>
       </c>
     </row>
     <row r="6" spans="1:10">
@@ -31890,7 +31890,7 @@
         <v>122</v>
       </c>
       <c r="J8">
-        <v>114</v>
+        <v>115</v>
       </c>
     </row>
     <row r="9" spans="1:10">
@@ -31922,7 +31922,7 @@
         <v>113</v>
       </c>
       <c r="J9">
-        <v>63</v>
+        <v>64</v>
       </c>
     </row>
     <row r="10" spans="1:10">
@@ -31986,7 +31986,7 @@
         <v>886</v>
       </c>
       <c r="J11">
-        <v>538</v>
+        <v>541</v>
       </c>
     </row>
   </sheetData>
@@ -32261,7 +32261,7 @@
         <v>405</v>
       </c>
       <c r="J8">
-        <v>334</v>
+        <v>335</v>
       </c>
     </row>
     <row r="9" spans="1:10">
@@ -32325,7 +32325,7 @@
         <v>670</v>
       </c>
       <c r="J10">
-        <v>300</v>
+        <v>302</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -32357,7 +32357,7 @@
         <v>1368</v>
       </c>
       <c r="J11">
-        <v>786</v>
+        <v>789</v>
       </c>
     </row>
   </sheetData>
@@ -32632,7 +32632,7 @@
         <v>338</v>
       </c>
       <c r="J8">
-        <v>237</v>
+        <v>239</v>
       </c>
     </row>
     <row r="9" spans="1:10">
@@ -32696,7 +32696,7 @@
         <v>1773</v>
       </c>
       <c r="J10">
-        <v>921</v>
+        <v>926</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -32728,7 +32728,7 @@
         <v>2622</v>
       </c>
       <c r="J11">
-        <v>1384</v>
+        <v>1391</v>
       </c>
     </row>
   </sheetData>
@@ -33058,7 +33058,7 @@
         <v>148</v>
       </c>
       <c r="J10">
-        <v>83</v>
+        <v>85</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -33090,7 +33090,7 @@
         <v>340</v>
       </c>
       <c r="J11">
-        <v>192</v>
+        <v>194</v>
       </c>
     </row>
   </sheetData>
@@ -33700,7 +33700,7 @@
         <v>334</v>
       </c>
       <c r="J8">
-        <v>178</v>
+        <v>180</v>
       </c>
     </row>
     <row r="9" spans="1:10">
@@ -33732,7 +33732,7 @@
         <v>66</v>
       </c>
       <c r="J9">
-        <v>32</v>
+        <v>33</v>
       </c>
     </row>
     <row r="10" spans="1:10">
@@ -33764,7 +33764,7 @@
         <v>606</v>
       </c>
       <c r="J10">
-        <v>270</v>
+        <v>271</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -33796,7 +33796,7 @@
         <v>1187</v>
       </c>
       <c r="J11">
-        <v>575</v>
+        <v>579</v>
       </c>
     </row>
   </sheetData>
@@ -34071,7 +34071,7 @@
         <v>116</v>
       </c>
       <c r="J8">
-        <v>38</v>
+        <v>39</v>
       </c>
     </row>
     <row r="9" spans="1:10">
@@ -34103,7 +34103,7 @@
         <v>153</v>
       </c>
       <c r="J9">
-        <v>53</v>
+        <v>54</v>
       </c>
     </row>
   </sheetData>
@@ -34192,7 +34192,7 @@
         <v>22</v>
       </c>
       <c r="J2">
-        <v>12</v>
+        <v>14</v>
       </c>
     </row>
     <row r="3" spans="1:10">
@@ -34427,7 +34427,7 @@
         <v>313</v>
       </c>
       <c r="J10">
-        <v>132</v>
+        <v>133</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -34459,7 +34459,7 @@
         <v>494</v>
       </c>
       <c r="J11">
-        <v>224</v>
+        <v>227</v>
       </c>
     </row>
   </sheetData>
@@ -34941,7 +34941,7 @@
         <v>32</v>
       </c>
       <c r="J5">
-        <v>20</v>
+        <v>21</v>
       </c>
     </row>
     <row r="6" spans="1:10">
@@ -35127,7 +35127,7 @@
         <v>406</v>
       </c>
       <c r="J11">
-        <v>270</v>
+        <v>271</v>
       </c>
     </row>
   </sheetData>
@@ -35280,7 +35280,7 @@
         <v>8</v>
       </c>
       <c r="J4">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="5" spans="1:10">
@@ -35454,7 +35454,7 @@
         <v>181</v>
       </c>
       <c r="J10">
-        <v>81</v>
+        <v>82</v>
       </c>
     </row>
   </sheetData>
@@ -36388,7 +36388,7 @@
         <v>291</v>
       </c>
       <c r="J8">
-        <v>175</v>
+        <v>178</v>
       </c>
     </row>
     <row r="9" spans="1:10">
@@ -36420,7 +36420,7 @@
         <v>125</v>
       </c>
       <c r="J9">
-        <v>49</v>
+        <v>54</v>
       </c>
     </row>
     <row r="10" spans="1:10">
@@ -36452,7 +36452,7 @@
         <v>905</v>
       </c>
       <c r="J10">
-        <v>434</v>
+        <v>438</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -36484,7 +36484,7 @@
         <v>1669</v>
       </c>
       <c r="J11">
-        <v>853</v>
+        <v>865</v>
       </c>
     </row>
   </sheetData>
@@ -36666,7 +36666,7 @@
         <v>32</v>
       </c>
       <c r="J5">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="6" spans="1:10">
@@ -36759,7 +36759,7 @@
         <v>68</v>
       </c>
       <c r="J8">
-        <v>59</v>
+        <v>60</v>
       </c>
     </row>
     <row r="9" spans="1:10">
@@ -36855,7 +36855,7 @@
         <v>337</v>
       </c>
       <c r="J11">
-        <v>210</v>
+        <v>212</v>
       </c>
     </row>
   </sheetData>
@@ -37279,7 +37279,7 @@
         <v>17</v>
       </c>
       <c r="J2">
-        <v>12</v>
+        <v>13</v>
       </c>
     </row>
     <row r="3" spans="1:10">
@@ -37540,7 +37540,7 @@
         <v>236</v>
       </c>
       <c r="J11">
-        <v>142</v>
+        <v>143</v>
       </c>
     </row>
   </sheetData>
@@ -37745,7 +37745,7 @@
         <v>80</v>
       </c>
       <c r="J6">
-        <v>41</v>
+        <v>42</v>
       </c>
     </row>
     <row r="7" spans="1:10">
@@ -37855,7 +37855,7 @@
         <v>717</v>
       </c>
       <c r="J10">
-        <v>299</v>
+        <v>301</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -37887,7 +37887,7 @@
         <v>1066</v>
       </c>
       <c r="J11">
-        <v>438</v>
+        <v>441</v>
       </c>
     </row>
   </sheetData>
@@ -38196,7 +38196,7 @@
         <v>260</v>
       </c>
       <c r="J10">
-        <v>113</v>
+        <v>114</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -38228,7 +38228,7 @@
         <v>393</v>
       </c>
       <c r="J11">
-        <v>163</v>
+        <v>164</v>
       </c>
     </row>
   </sheetData>
@@ -38525,7 +38525,7 @@
         <v>135</v>
       </c>
       <c r="J10">
-        <v>64</v>
+        <v>65</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -38557,7 +38557,7 @@
         <v>219</v>
       </c>
       <c r="J11">
-        <v>117</v>
+        <v>118</v>
       </c>
     </row>
   </sheetData>
@@ -39462,7 +39462,7 @@
         <v>14</v>
       </c>
       <c r="J9">
-        <v>12</v>
+        <v>13</v>
       </c>
     </row>
     <row r="10" spans="1:10">
@@ -39494,7 +39494,7 @@
         <v>174</v>
       </c>
       <c r="J10">
-        <v>82</v>
+        <v>84</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -39526,7 +39526,7 @@
         <v>235</v>
       </c>
       <c r="J11">
-        <v>120</v>
+        <v>123</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add data for 2023-07-10
</commit_message>
<xml_diff>
--- a/output/index-crime-full-year.xlsx
+++ b/output/index-crime-full-year.xlsx
@@ -895,7 +895,7 @@
         <v>7277</v>
       </c>
       <c r="J2">
-        <v>3829</v>
+        <v>3848</v>
       </c>
     </row>
     <row r="3" spans="1:10">
@@ -927,7 +927,7 @@
         <v>7486</v>
       </c>
       <c r="J3">
-        <v>4023</v>
+        <v>4048</v>
       </c>
     </row>
     <row r="4" spans="1:10">
@@ -959,7 +959,7 @@
         <v>422</v>
       </c>
       <c r="J4">
-        <v>256</v>
+        <v>258</v>
       </c>
     </row>
     <row r="5" spans="1:10">
@@ -991,7 +991,7 @@
         <v>7592</v>
       </c>
       <c r="J5">
-        <v>3756</v>
+        <v>3773</v>
       </c>
     </row>
     <row r="6" spans="1:10">
@@ -1020,10 +1020,10 @@
         <v>1695</v>
       </c>
       <c r="I6">
-        <v>1767</v>
+        <v>1768</v>
       </c>
       <c r="J6">
-        <v>908</v>
+        <v>912</v>
       </c>
     </row>
     <row r="7" spans="1:10">
@@ -1055,7 +1055,7 @@
         <v>718</v>
       </c>
       <c r="J7">
-        <v>320</v>
+        <v>324</v>
       </c>
     </row>
     <row r="8" spans="1:10">
@@ -1081,13 +1081,13 @@
         <v>9959</v>
       </c>
       <c r="H8">
-        <v>10601</v>
+        <v>10602</v>
       </c>
       <c r="I8">
         <v>21448</v>
       </c>
       <c r="J8">
-        <v>15231</v>
+        <v>15330</v>
       </c>
     </row>
     <row r="9" spans="1:10">
@@ -1119,7 +1119,7 @@
         <v>8964</v>
       </c>
       <c r="J9">
-        <v>4778</v>
+        <v>4820</v>
       </c>
     </row>
     <row r="10" spans="1:10">
@@ -1148,10 +1148,10 @@
         <v>40794</v>
       </c>
       <c r="I10">
-        <v>54804</v>
+        <v>54805</v>
       </c>
       <c r="J10">
-        <v>27653</v>
+        <v>27797</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -1177,13 +1177,13 @@
         <v>85314</v>
       </c>
       <c r="H11">
-        <v>84587</v>
+        <v>84588</v>
       </c>
       <c r="I11">
-        <v>110478</v>
+        <v>110480</v>
       </c>
       <c r="J11">
-        <v>60754</v>
+        <v>61110</v>
       </c>
     </row>
   </sheetData>
@@ -1353,7 +1353,7 @@
         <v>54</v>
       </c>
       <c r="J5">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="6" spans="1:10">
@@ -1536,7 +1536,7 @@
         <v>1153</v>
       </c>
       <c r="J11">
-        <v>720</v>
+        <v>719</v>
       </c>
     </row>
   </sheetData>
@@ -2091,7 +2091,7 @@
         <v>373</v>
       </c>
       <c r="J8">
-        <v>260</v>
+        <v>263</v>
       </c>
     </row>
     <row r="9" spans="1:10">
@@ -2123,7 +2123,7 @@
         <v>111</v>
       </c>
       <c r="J9">
-        <v>68</v>
+        <v>70</v>
       </c>
     </row>
     <row r="10" spans="1:10">
@@ -2155,7 +2155,7 @@
         <v>820</v>
       </c>
       <c r="J10">
-        <v>474</v>
+        <v>476</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -2187,7 +2187,7 @@
         <v>1713</v>
       </c>
       <c r="J11">
-        <v>1022</v>
+        <v>1029</v>
       </c>
     </row>
   </sheetData>
@@ -2308,7 +2308,7 @@
         <v>56</v>
       </c>
       <c r="J3">
-        <v>27</v>
+        <v>28</v>
       </c>
     </row>
     <row r="4" spans="1:10">
@@ -2369,7 +2369,7 @@
         <v>124</v>
       </c>
       <c r="J5">
-        <v>60</v>
+        <v>62</v>
       </c>
     </row>
     <row r="6" spans="1:10">
@@ -2462,7 +2462,7 @@
         <v>188</v>
       </c>
       <c r="J8">
-        <v>140</v>
+        <v>141</v>
       </c>
     </row>
     <row r="9" spans="1:10">
@@ -2526,7 +2526,7 @@
         <v>712</v>
       </c>
       <c r="J10">
-        <v>376</v>
+        <v>377</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -2558,7 +2558,7 @@
         <v>1228</v>
       </c>
       <c r="J11">
-        <v>680</v>
+        <v>685</v>
       </c>
     </row>
   </sheetData>
@@ -2647,7 +2647,7 @@
         <v>220</v>
       </c>
       <c r="J2">
-        <v>114</v>
+        <v>115</v>
       </c>
     </row>
     <row r="3" spans="1:10">
@@ -2679,7 +2679,7 @@
         <v>244</v>
       </c>
       <c r="J3">
-        <v>148</v>
+        <v>150</v>
       </c>
     </row>
     <row r="4" spans="1:10">
@@ -2839,7 +2839,7 @@
         <v>700</v>
       </c>
       <c r="J8">
-        <v>448</v>
+        <v>451</v>
       </c>
     </row>
     <row r="9" spans="1:10">
@@ -2903,7 +2903,7 @@
         <v>820</v>
       </c>
       <c r="J10">
-        <v>416</v>
+        <v>419</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -2935,7 +2935,7 @@
         <v>2472</v>
       </c>
       <c r="J11">
-        <v>1353</v>
+        <v>1362</v>
       </c>
     </row>
   </sheetData>
@@ -3024,7 +3024,7 @@
         <v>61</v>
       </c>
       <c r="J2">
-        <v>34</v>
+        <v>35</v>
       </c>
     </row>
     <row r="3" spans="1:10">
@@ -3213,7 +3213,7 @@
         <v>260</v>
       </c>
       <c r="J8">
-        <v>227</v>
+        <v>230</v>
       </c>
     </row>
     <row r="9" spans="1:10">
@@ -3277,7 +3277,7 @@
         <v>913</v>
       </c>
       <c r="J10">
-        <v>568</v>
+        <v>570</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -3309,7 +3309,7 @@
         <v>1601</v>
       </c>
       <c r="J11">
-        <v>1010</v>
+        <v>1016</v>
       </c>
     </row>
   </sheetData>
@@ -3801,7 +3801,7 @@
         <v>71</v>
       </c>
       <c r="J3">
-        <v>34</v>
+        <v>35</v>
       </c>
     </row>
     <row r="4" spans="1:10">
@@ -3961,7 +3961,7 @@
         <v>220</v>
       </c>
       <c r="J8">
-        <v>179</v>
+        <v>181</v>
       </c>
     </row>
     <row r="9" spans="1:10">
@@ -4025,7 +4025,7 @@
         <v>681</v>
       </c>
       <c r="J10">
-        <v>441</v>
+        <v>443</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -4057,7 +4057,7 @@
         <v>1279</v>
       </c>
       <c r="J11">
-        <v>811</v>
+        <v>816</v>
       </c>
     </row>
   </sheetData>
@@ -4178,7 +4178,7 @@
         <v>530</v>
       </c>
       <c r="J3">
-        <v>273</v>
+        <v>277</v>
       </c>
     </row>
     <row r="4" spans="1:10">
@@ -4242,7 +4242,7 @@
         <v>268</v>
       </c>
       <c r="J5">
-        <v>146</v>
+        <v>150</v>
       </c>
     </row>
     <row r="6" spans="1:10">
@@ -4274,7 +4274,7 @@
         <v>83</v>
       </c>
       <c r="J6">
-        <v>44</v>
+        <v>45</v>
       </c>
     </row>
     <row r="7" spans="1:10">
@@ -4338,7 +4338,7 @@
         <v>794</v>
       </c>
       <c r="J8">
-        <v>566</v>
+        <v>572</v>
       </c>
     </row>
     <row r="9" spans="1:10">
@@ -4370,7 +4370,7 @@
         <v>433</v>
       </c>
       <c r="J9">
-        <v>193</v>
+        <v>194</v>
       </c>
     </row>
     <row r="10" spans="1:10">
@@ -4402,7 +4402,7 @@
         <v>1302</v>
       </c>
       <c r="J10">
-        <v>667</v>
+        <v>668</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -4434,7 +4434,7 @@
         <v>3950</v>
       </c>
       <c r="J11">
-        <v>2190</v>
+        <v>2207</v>
       </c>
     </row>
   </sheetData>
@@ -4697,7 +4697,7 @@
         <v>131</v>
       </c>
       <c r="J8">
-        <v>131</v>
+        <v>132</v>
       </c>
     </row>
     <row r="9" spans="1:10">
@@ -4761,7 +4761,7 @@
         <v>921</v>
       </c>
       <c r="J10">
-        <v>372</v>
+        <v>373</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -4793,7 +4793,7 @@
         <v>1318</v>
       </c>
       <c r="J11">
-        <v>636</v>
+        <v>638</v>
       </c>
     </row>
   </sheetData>
@@ -4882,7 +4882,7 @@
         <v>216</v>
       </c>
       <c r="J2">
-        <v>117</v>
+        <v>118</v>
       </c>
     </row>
     <row r="3" spans="1:10">
@@ -4914,7 +4914,7 @@
         <v>280</v>
       </c>
       <c r="J3">
-        <v>112</v>
+        <v>113</v>
       </c>
     </row>
     <row r="4" spans="1:10">
@@ -4978,7 +4978,7 @@
         <v>191</v>
       </c>
       <c r="J5">
-        <v>87</v>
+        <v>88</v>
       </c>
     </row>
     <row r="6" spans="1:10">
@@ -5074,7 +5074,7 @@
         <v>653</v>
       </c>
       <c r="J8">
-        <v>495</v>
+        <v>499</v>
       </c>
     </row>
     <row r="9" spans="1:10">
@@ -5106,7 +5106,7 @@
         <v>428</v>
       </c>
       <c r="J9">
-        <v>267</v>
+        <v>270</v>
       </c>
     </row>
     <row r="10" spans="1:10">
@@ -5138,7 +5138,7 @@
         <v>1089</v>
       </c>
       <c r="J10">
-        <v>609</v>
+        <v>611</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -5170,7 +5170,7 @@
         <v>2956</v>
       </c>
       <c r="J11">
-        <v>1741</v>
+        <v>1753</v>
       </c>
     </row>
   </sheetData>
@@ -5259,7 +5259,7 @@
         <v>918</v>
       </c>
       <c r="J2">
-        <v>517</v>
+        <v>518</v>
       </c>
     </row>
     <row r="3" spans="1:10">
@@ -5323,7 +5323,7 @@
         <v>436</v>
       </c>
       <c r="J4">
-        <v>238</v>
+        <v>239</v>
       </c>
     </row>
     <row r="5" spans="1:10">
@@ -5355,7 +5355,7 @@
         <v>247</v>
       </c>
       <c r="J5">
-        <v>148</v>
+        <v>149</v>
       </c>
     </row>
     <row r="6" spans="1:10">
@@ -5387,7 +5387,7 @@
         <v>793</v>
       </c>
       <c r="J6">
-        <v>521</v>
+        <v>522</v>
       </c>
     </row>
     <row r="7" spans="1:10">
@@ -5419,7 +5419,7 @@
         <v>2685</v>
       </c>
       <c r="J7">
-        <v>1537</v>
+        <v>1545</v>
       </c>
     </row>
     <row r="8" spans="1:10">
@@ -5451,7 +5451,7 @@
         <v>4744</v>
       </c>
       <c r="J8">
-        <v>2588</v>
+        <v>2603</v>
       </c>
     </row>
     <row r="9" spans="1:10">
@@ -5483,7 +5483,7 @@
         <v>519</v>
       </c>
       <c r="J9">
-        <v>284</v>
+        <v>287</v>
       </c>
     </row>
     <row r="10" spans="1:10">
@@ -5515,7 +5515,7 @@
         <v>949</v>
       </c>
       <c r="J10">
-        <v>481</v>
+        <v>490</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -5547,7 +5547,7 @@
         <v>1713</v>
       </c>
       <c r="J11">
-        <v>1022</v>
+        <v>1029</v>
       </c>
     </row>
     <row r="12" spans="1:10">
@@ -5611,7 +5611,7 @@
         <v>258</v>
       </c>
       <c r="J13">
-        <v>143</v>
+        <v>145</v>
       </c>
     </row>
     <row r="14" spans="1:10">
@@ -5643,7 +5643,7 @@
         <v>719</v>
       </c>
       <c r="J14">
-        <v>328</v>
+        <v>330</v>
       </c>
     </row>
     <row r="15" spans="1:10">
@@ -5707,7 +5707,7 @@
         <v>595</v>
       </c>
       <c r="J16">
-        <v>388</v>
+        <v>392</v>
       </c>
     </row>
     <row r="17" spans="1:10">
@@ -5771,7 +5771,7 @@
         <v>695</v>
       </c>
       <c r="J18">
-        <v>399</v>
+        <v>403</v>
       </c>
     </row>
     <row r="19" spans="1:10">
@@ -5803,7 +5803,7 @@
         <v>2636</v>
       </c>
       <c r="J19">
-        <v>1412</v>
+        <v>1418</v>
       </c>
     </row>
     <row r="20" spans="1:10">
@@ -5835,7 +5835,7 @@
         <v>2046</v>
       </c>
       <c r="J20">
-        <v>1001</v>
+        <v>1007</v>
       </c>
     </row>
     <row r="21" spans="1:10">
@@ -5899,7 +5899,7 @@
         <v>418</v>
       </c>
       <c r="J22">
-        <v>273</v>
+        <v>276</v>
       </c>
     </row>
     <row r="23" spans="1:10">
@@ -5931,7 +5931,7 @@
         <v>1368</v>
       </c>
       <c r="J23">
-        <v>789</v>
+        <v>794</v>
       </c>
     </row>
     <row r="24" spans="1:10">
@@ -5963,7 +5963,7 @@
         <v>500</v>
       </c>
       <c r="J24">
-        <v>322</v>
+        <v>325</v>
       </c>
     </row>
     <row r="25" spans="1:10">
@@ -5995,7 +5995,7 @@
         <v>430</v>
       </c>
       <c r="J25">
-        <v>247</v>
+        <v>249</v>
       </c>
     </row>
     <row r="26" spans="1:10">
@@ -6027,7 +6027,7 @@
         <v>248</v>
       </c>
       <c r="J26">
-        <v>150</v>
+        <v>151</v>
       </c>
     </row>
     <row r="27" spans="1:10">
@@ -6059,7 +6059,7 @@
         <v>1258</v>
       </c>
       <c r="J27">
-        <v>713</v>
+        <v>718</v>
       </c>
     </row>
     <row r="28" spans="1:10">
@@ -6123,7 +6123,7 @@
         <v>3950</v>
       </c>
       <c r="J29">
-        <v>2190</v>
+        <v>2207</v>
       </c>
     </row>
     <row r="30" spans="1:10">
@@ -6187,7 +6187,7 @@
         <v>867</v>
       </c>
       <c r="J31">
-        <v>453</v>
+        <v>454</v>
       </c>
     </row>
     <row r="32" spans="1:10">
@@ -6251,7 +6251,7 @@
         <v>3011</v>
       </c>
       <c r="J33">
-        <v>1728</v>
+        <v>1741</v>
       </c>
     </row>
     <row r="34" spans="1:10">
@@ -6283,7 +6283,7 @@
         <v>761</v>
       </c>
       <c r="J34">
-        <v>469</v>
+        <v>472</v>
       </c>
     </row>
     <row r="35" spans="1:10">
@@ -6347,7 +6347,7 @@
         <v>1491</v>
       </c>
       <c r="J36">
-        <v>871</v>
+        <v>876</v>
       </c>
     </row>
     <row r="37" spans="1:10">
@@ -6379,7 +6379,7 @@
         <v>2547</v>
       </c>
       <c r="J37">
-        <v>1464</v>
+        <v>1481</v>
       </c>
     </row>
     <row r="38" spans="1:10">
@@ -6475,7 +6475,7 @@
         <v>236</v>
       </c>
       <c r="J40">
-        <v>143</v>
+        <v>144</v>
       </c>
     </row>
     <row r="41" spans="1:10">
@@ -6507,7 +6507,7 @@
         <v>437</v>
       </c>
       <c r="J41">
-        <v>296</v>
+        <v>297</v>
       </c>
     </row>
     <row r="42" spans="1:10">
@@ -6539,7 +6539,7 @@
         <v>2956</v>
       </c>
       <c r="J42">
-        <v>1741</v>
+        <v>1753</v>
       </c>
     </row>
     <row r="43" spans="1:10">
@@ -6571,7 +6571,7 @@
         <v>1153</v>
       </c>
       <c r="J43">
-        <v>720</v>
+        <v>719</v>
       </c>
     </row>
     <row r="44" spans="1:10">
@@ -6603,7 +6603,7 @@
         <v>1228</v>
       </c>
       <c r="J44">
-        <v>680</v>
+        <v>685</v>
       </c>
     </row>
     <row r="45" spans="1:10">
@@ -6667,7 +6667,7 @@
         <v>436</v>
       </c>
       <c r="J46">
-        <v>247</v>
+        <v>249</v>
       </c>
     </row>
     <row r="47" spans="1:10">
@@ -6699,7 +6699,7 @@
         <v>903</v>
       </c>
       <c r="J47">
-        <v>498</v>
+        <v>504</v>
       </c>
     </row>
     <row r="48" spans="1:10">
@@ -6731,7 +6731,7 @@
         <v>2622</v>
       </c>
       <c r="J48">
-        <v>1391</v>
+        <v>1401</v>
       </c>
     </row>
     <row r="49" spans="1:10">
@@ -6763,7 +6763,7 @@
         <v>1648</v>
       </c>
       <c r="J49">
-        <v>853</v>
+        <v>857</v>
       </c>
     </row>
     <row r="50" spans="1:10">
@@ -6795,7 +6795,7 @@
         <v>960</v>
       </c>
       <c r="J50">
-        <v>526</v>
+        <v>529</v>
       </c>
     </row>
     <row r="51" spans="1:10">
@@ -6827,7 +6827,7 @@
         <v>1337</v>
       </c>
       <c r="J51">
-        <v>813</v>
+        <v>815</v>
       </c>
     </row>
     <row r="52" spans="1:10">
@@ -6859,7 +6859,7 @@
         <v>1491</v>
       </c>
       <c r="J52">
-        <v>979</v>
+        <v>982</v>
       </c>
     </row>
     <row r="53" spans="1:10">
@@ -6891,7 +6891,7 @@
         <v>1601</v>
       </c>
       <c r="J53">
-        <v>1010</v>
+        <v>1016</v>
       </c>
     </row>
     <row r="54" spans="1:10">
@@ -6923,7 +6923,7 @@
         <v>3507</v>
       </c>
       <c r="J54">
-        <v>1840</v>
+        <v>1849</v>
       </c>
     </row>
     <row r="55" spans="1:10">
@@ -6955,7 +6955,7 @@
         <v>1244</v>
       </c>
       <c r="J55">
-        <v>633</v>
+        <v>634</v>
       </c>
     </row>
     <row r="56" spans="1:10">
@@ -6987,7 +6987,7 @@
         <v>628</v>
       </c>
       <c r="J56">
-        <v>305</v>
+        <v>311</v>
       </c>
     </row>
     <row r="57" spans="1:10">
@@ -7019,7 +7019,7 @@
         <v>406</v>
       </c>
       <c r="J57">
-        <v>271</v>
+        <v>272</v>
       </c>
     </row>
     <row r="58" spans="1:10">
@@ -7115,7 +7115,7 @@
         <v>768</v>
       </c>
       <c r="J60">
-        <v>447</v>
+        <v>452</v>
       </c>
     </row>
     <row r="61" spans="1:10">
@@ -7205,13 +7205,13 @@
         <v>1652</v>
       </c>
       <c r="H63">
-        <v>2161</v>
+        <v>2162</v>
       </c>
       <c r="I63">
-        <v>2470</v>
+        <v>2472</v>
       </c>
       <c r="J63">
-        <v>679</v>
+        <v>699</v>
       </c>
     </row>
     <row r="64" spans="1:10">
@@ -7243,7 +7243,7 @@
         <v>1187</v>
       </c>
       <c r="J64">
-        <v>579</v>
+        <v>580</v>
       </c>
     </row>
     <row r="65" spans="1:10">
@@ -7275,7 +7275,7 @@
         <v>1515</v>
       </c>
       <c r="J65">
-        <v>944</v>
+        <v>951</v>
       </c>
     </row>
     <row r="66" spans="1:10">
@@ -7307,7 +7307,7 @@
         <v>715</v>
       </c>
       <c r="J66">
-        <v>406</v>
+        <v>410</v>
       </c>
     </row>
     <row r="67" spans="1:10">
@@ -7339,7 +7339,7 @@
         <v>2510</v>
       </c>
       <c r="J67">
-        <v>1418</v>
+        <v>1429</v>
       </c>
     </row>
     <row r="68" spans="1:10">
@@ -7467,7 +7467,7 @@
         <v>335</v>
       </c>
       <c r="J71">
-        <v>243</v>
+        <v>244</v>
       </c>
     </row>
     <row r="72" spans="1:10">
@@ -7499,7 +7499,7 @@
         <v>706</v>
       </c>
       <c r="J72">
-        <v>354</v>
+        <v>356</v>
       </c>
     </row>
     <row r="73" spans="1:10">
@@ -7531,7 +7531,7 @@
         <v>1279</v>
       </c>
       <c r="J73">
-        <v>811</v>
+        <v>816</v>
       </c>
     </row>
     <row r="74" spans="1:10">
@@ -7563,7 +7563,7 @@
         <v>307</v>
       </c>
       <c r="J74">
-        <v>145</v>
+        <v>146</v>
       </c>
     </row>
     <row r="75" spans="1:10">
@@ -7627,7 +7627,7 @@
         <v>2923</v>
       </c>
       <c r="J76">
-        <v>1572</v>
+        <v>1580</v>
       </c>
     </row>
     <row r="77" spans="1:10">
@@ -7659,7 +7659,7 @@
         <v>462</v>
       </c>
       <c r="J77">
-        <v>284</v>
+        <v>286</v>
       </c>
     </row>
     <row r="78" spans="1:10">
@@ -7691,7 +7691,7 @@
         <v>1797</v>
       </c>
       <c r="J78">
-        <v>954</v>
+        <v>961</v>
       </c>
     </row>
     <row r="79" spans="1:10">
@@ -7723,7 +7723,7 @@
         <v>2472</v>
       </c>
       <c r="J79">
-        <v>1353</v>
+        <v>1362</v>
       </c>
     </row>
     <row r="80" spans="1:10">
@@ -7819,7 +7819,7 @@
         <v>233</v>
       </c>
       <c r="J82">
-        <v>144</v>
+        <v>145</v>
       </c>
     </row>
     <row r="83" spans="1:10">
@@ -7851,7 +7851,7 @@
         <v>1793</v>
       </c>
       <c r="J83">
-        <v>944</v>
+        <v>950</v>
       </c>
     </row>
     <row r="84" spans="1:10">
@@ -7883,7 +7883,7 @@
         <v>729</v>
       </c>
       <c r="J84">
-        <v>452</v>
+        <v>454</v>
       </c>
     </row>
     <row r="85" spans="1:10">
@@ -7915,7 +7915,7 @@
         <v>3848</v>
       </c>
       <c r="J85">
-        <v>2239</v>
+        <v>2250</v>
       </c>
     </row>
     <row r="86" spans="1:10">
@@ -7947,7 +7947,7 @@
         <v>1066</v>
       </c>
       <c r="J86">
-        <v>441</v>
+        <v>443</v>
       </c>
     </row>
     <row r="87" spans="1:10">
@@ -7979,7 +7979,7 @@
         <v>396</v>
       </c>
       <c r="J87">
-        <v>210</v>
+        <v>211</v>
       </c>
     </row>
     <row r="88" spans="1:10">
@@ -8011,7 +8011,7 @@
         <v>943</v>
       </c>
       <c r="J88">
-        <v>552</v>
+        <v>553</v>
       </c>
     </row>
     <row r="89" spans="1:10">
@@ -8043,7 +8043,7 @@
         <v>1878</v>
       </c>
       <c r="J89">
-        <v>1050</v>
+        <v>1054</v>
       </c>
     </row>
     <row r="90" spans="1:10">
@@ -8075,7 +8075,7 @@
         <v>1354</v>
       </c>
       <c r="J90">
-        <v>800</v>
+        <v>803</v>
       </c>
     </row>
     <row r="91" spans="1:10">
@@ -8107,7 +8107,7 @@
         <v>970</v>
       </c>
       <c r="J91">
-        <v>561</v>
+        <v>566</v>
       </c>
     </row>
     <row r="92" spans="1:10">
@@ -8171,7 +8171,7 @@
         <v>721</v>
       </c>
       <c r="J93">
-        <v>415</v>
+        <v>416</v>
       </c>
     </row>
     <row r="94" spans="1:10">
@@ -8203,7 +8203,7 @@
         <v>2664</v>
       </c>
       <c r="J94">
-        <v>1305</v>
+        <v>1310</v>
       </c>
     </row>
     <row r="95" spans="1:10">
@@ -8235,7 +8235,7 @@
         <v>1389</v>
       </c>
       <c r="J95">
-        <v>811</v>
+        <v>814</v>
       </c>
     </row>
     <row r="96" spans="1:10">
@@ -8267,7 +8267,7 @@
         <v>1669</v>
       </c>
       <c r="J96">
-        <v>865</v>
+        <v>867</v>
       </c>
     </row>
     <row r="97" spans="1:10">
@@ -8299,7 +8299,7 @@
         <v>1673</v>
       </c>
       <c r="J97">
-        <v>909</v>
+        <v>912</v>
       </c>
     </row>
     <row r="98" spans="1:10">
@@ -8331,7 +8331,7 @@
         <v>1318</v>
       </c>
       <c r="J98">
-        <v>636</v>
+        <v>638</v>
       </c>
     </row>
     <row r="99" spans="1:10">
@@ -8363,7 +8363,7 @@
         <v>1488</v>
       </c>
       <c r="J99">
-        <v>847</v>
+        <v>852</v>
       </c>
     </row>
     <row r="100" spans="1:10">
@@ -8421,13 +8421,13 @@
         <v>85314</v>
       </c>
       <c r="H101">
-        <v>84587</v>
+        <v>84588</v>
       </c>
       <c r="I101">
-        <v>110478</v>
+        <v>110480</v>
       </c>
       <c r="J101">
-        <v>60754</v>
+        <v>61110</v>
       </c>
     </row>
   </sheetData>
@@ -8795,7 +8795,7 @@
         <v>219</v>
       </c>
       <c r="J8">
-        <v>106</v>
+        <v>107</v>
       </c>
     </row>
     <row r="9" spans="1:10">
@@ -8859,7 +8859,7 @@
         <v>1135</v>
       </c>
       <c r="J10">
-        <v>580</v>
+        <v>583</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -8891,7 +8891,7 @@
         <v>1648</v>
       </c>
       <c r="J11">
-        <v>853</v>
+        <v>857</v>
       </c>
     </row>
   </sheetData>
@@ -9012,7 +9012,7 @@
         <v>439</v>
       </c>
       <c r="J3">
-        <v>229</v>
+        <v>231</v>
       </c>
     </row>
     <row r="4" spans="1:10">
@@ -9076,7 +9076,7 @@
         <v>381</v>
       </c>
       <c r="J5">
-        <v>162</v>
+        <v>163</v>
       </c>
     </row>
     <row r="6" spans="1:10">
@@ -9140,7 +9140,7 @@
         <v>36</v>
       </c>
       <c r="J7">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="8" spans="1:10">
@@ -9204,7 +9204,7 @@
         <v>303</v>
       </c>
       <c r="J9">
-        <v>175</v>
+        <v>177</v>
       </c>
     </row>
     <row r="10" spans="1:10">
@@ -9236,7 +9236,7 @@
         <v>1271</v>
       </c>
       <c r="J10">
-        <v>685</v>
+        <v>690</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -9268,7 +9268,7 @@
         <v>3848</v>
       </c>
       <c r="J11">
-        <v>2239</v>
+        <v>2250</v>
       </c>
     </row>
   </sheetData>
@@ -9546,7 +9546,7 @@
         <v>336</v>
       </c>
       <c r="J8">
-        <v>167</v>
+        <v>170</v>
       </c>
     </row>
     <row r="9" spans="1:10">
@@ -9578,7 +9578,7 @@
         <v>179</v>
       </c>
       <c r="J9">
-        <v>106</v>
+        <v>108</v>
       </c>
     </row>
     <row r="10" spans="1:10">
@@ -9610,7 +9610,7 @@
         <v>2132</v>
       </c>
       <c r="J10">
-        <v>1137</v>
+        <v>1140</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -9642,7 +9642,7 @@
         <v>2923</v>
       </c>
       <c r="J11">
-        <v>1572</v>
+        <v>1580</v>
       </c>
     </row>
   </sheetData>
@@ -9978,7 +9978,7 @@
         <v>1034</v>
       </c>
       <c r="J10">
-        <v>452</v>
+        <v>455</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -10010,7 +10010,7 @@
         <v>1673</v>
       </c>
       <c r="J11">
-        <v>909</v>
+        <v>912</v>
       </c>
     </row>
   </sheetData>
@@ -10099,7 +10099,7 @@
         <v>235</v>
       </c>
       <c r="J2">
-        <v>120</v>
+        <v>122</v>
       </c>
     </row>
     <row r="3" spans="1:10">
@@ -10131,7 +10131,7 @@
         <v>365</v>
       </c>
       <c r="J3">
-        <v>215</v>
+        <v>216</v>
       </c>
     </row>
     <row r="4" spans="1:10">
@@ -10195,7 +10195,7 @@
         <v>102</v>
       </c>
       <c r="J5">
-        <v>60</v>
+        <v>61</v>
       </c>
     </row>
     <row r="6" spans="1:10">
@@ -10259,7 +10259,7 @@
         <v>29</v>
       </c>
       <c r="J7">
-        <v>14</v>
+        <v>15</v>
       </c>
     </row>
     <row r="8" spans="1:10">
@@ -10291,7 +10291,7 @@
         <v>516</v>
       </c>
       <c r="J8">
-        <v>372</v>
+        <v>373</v>
       </c>
     </row>
     <row r="9" spans="1:10">
@@ -10323,7 +10323,7 @@
         <v>295</v>
       </c>
       <c r="J9">
-        <v>148</v>
+        <v>149</v>
       </c>
     </row>
     <row r="10" spans="1:10">
@@ -10355,7 +10355,7 @@
         <v>895</v>
       </c>
       <c r="J10">
-        <v>442</v>
+        <v>446</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -10387,7 +10387,7 @@
         <v>2510</v>
       </c>
       <c r="J11">
-        <v>1418</v>
+        <v>1429</v>
       </c>
     </row>
   </sheetData>
@@ -10540,7 +10540,7 @@
         <v>6</v>
       </c>
       <c r="J4">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="5" spans="1:10">
@@ -10668,7 +10668,7 @@
         <v>392</v>
       </c>
       <c r="J8">
-        <v>284</v>
+        <v>286</v>
       </c>
     </row>
     <row r="9" spans="1:10">
@@ -10764,7 +10764,7 @@
         <v>1389</v>
       </c>
       <c r="J11">
-        <v>811</v>
+        <v>814</v>
       </c>
     </row>
   </sheetData>
@@ -10885,7 +10885,7 @@
         <v>74</v>
       </c>
       <c r="J3">
-        <v>36</v>
+        <v>37</v>
       </c>
     </row>
     <row r="4" spans="1:10">
@@ -11045,7 +11045,7 @@
         <v>190</v>
       </c>
       <c r="J8">
-        <v>163</v>
+        <v>164</v>
       </c>
     </row>
     <row r="9" spans="1:10">
@@ -11141,7 +11141,7 @@
         <v>729</v>
       </c>
       <c r="J11">
-        <v>452</v>
+        <v>454</v>
       </c>
     </row>
   </sheetData>
@@ -11326,7 +11326,7 @@
         <v>81</v>
       </c>
       <c r="J5">
-        <v>43</v>
+        <v>44</v>
       </c>
     </row>
     <row r="6" spans="1:10">
@@ -11358,7 +11358,7 @@
         <v>39</v>
       </c>
       <c r="J6">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="7" spans="1:10">
@@ -11422,7 +11422,7 @@
         <v>218</v>
       </c>
       <c r="J8">
-        <v>191</v>
+        <v>192</v>
       </c>
     </row>
     <row r="9" spans="1:10">
@@ -11454,7 +11454,7 @@
         <v>196</v>
       </c>
       <c r="J9">
-        <v>165</v>
+        <v>166</v>
       </c>
     </row>
     <row r="10" spans="1:10">
@@ -11486,7 +11486,7 @@
         <v>590</v>
       </c>
       <c r="J10">
-        <v>358</v>
+        <v>359</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -11518,7 +11518,7 @@
         <v>1491</v>
       </c>
       <c r="J11">
-        <v>979</v>
+        <v>982</v>
       </c>
     </row>
   </sheetData>
@@ -11863,7 +11863,7 @@
         <v>474</v>
       </c>
       <c r="J10">
-        <v>218</v>
+        <v>219</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -11895,7 +11895,7 @@
         <v>943</v>
       </c>
       <c r="J11">
-        <v>552</v>
+        <v>553</v>
       </c>
     </row>
   </sheetData>
@@ -12080,7 +12080,7 @@
         <v>69</v>
       </c>
       <c r="J5">
-        <v>33</v>
+        <v>34</v>
       </c>
     </row>
     <row r="6" spans="1:10">
@@ -12173,7 +12173,7 @@
         <v>401</v>
       </c>
       <c r="J8">
-        <v>219</v>
+        <v>221</v>
       </c>
     </row>
     <row r="9" spans="1:10">
@@ -12205,7 +12205,7 @@
         <v>243</v>
       </c>
       <c r="J9">
-        <v>131</v>
+        <v>132</v>
       </c>
     </row>
     <row r="10" spans="1:10">
@@ -12237,7 +12237,7 @@
         <v>2528</v>
       </c>
       <c r="J10">
-        <v>1316</v>
+        <v>1321</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -12269,7 +12269,7 @@
         <v>3507</v>
       </c>
       <c r="J11">
-        <v>1840</v>
+        <v>1849</v>
       </c>
     </row>
   </sheetData>
@@ -12550,7 +12550,7 @@
         <v>503</v>
       </c>
       <c r="J8">
-        <v>328</v>
+        <v>332</v>
       </c>
     </row>
     <row r="9" spans="1:10">
@@ -12582,7 +12582,7 @@
         <v>112</v>
       </c>
       <c r="J9">
-        <v>58</v>
+        <v>59</v>
       </c>
     </row>
     <row r="10" spans="1:10">
@@ -12646,7 +12646,7 @@
         <v>1491</v>
       </c>
       <c r="J11">
-        <v>871</v>
+        <v>876</v>
       </c>
     </row>
   </sheetData>
@@ -12735,7 +12735,7 @@
         <v>239</v>
       </c>
       <c r="J2">
-        <v>130</v>
+        <v>131</v>
       </c>
     </row>
     <row r="3" spans="1:10">
@@ -12767,7 +12767,7 @@
         <v>261</v>
       </c>
       <c r="J3">
-        <v>156</v>
+        <v>157</v>
       </c>
     </row>
     <row r="4" spans="1:10">
@@ -12927,7 +12927,7 @@
         <v>722</v>
       </c>
       <c r="J8">
-        <v>474</v>
+        <v>477</v>
       </c>
     </row>
     <row r="9" spans="1:10">
@@ -12959,7 +12959,7 @@
         <v>244</v>
       </c>
       <c r="J9">
-        <v>127</v>
+        <v>133</v>
       </c>
     </row>
     <row r="10" spans="1:10">
@@ -12991,7 +12991,7 @@
         <v>813</v>
       </c>
       <c r="J10">
-        <v>425</v>
+        <v>431</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -13023,7 +13023,7 @@
         <v>2547</v>
       </c>
       <c r="J11">
-        <v>1464</v>
+        <v>1481</v>
       </c>
     </row>
   </sheetData>
@@ -13112,7 +13112,7 @@
         <v>30</v>
       </c>
       <c r="J2">
-        <v>17</v>
+        <v>18</v>
       </c>
     </row>
     <row r="3" spans="1:10">
@@ -13347,7 +13347,7 @@
         <v>213</v>
       </c>
       <c r="J10">
-        <v>124</v>
+        <v>126</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -13379,7 +13379,7 @@
         <v>418</v>
       </c>
       <c r="J11">
-        <v>273</v>
+        <v>276</v>
       </c>
     </row>
   </sheetData>
@@ -13645,7 +13645,7 @@
         <v>89</v>
       </c>
       <c r="J8">
-        <v>69</v>
+        <v>70</v>
       </c>
     </row>
     <row r="9" spans="1:10">
@@ -13677,7 +13677,7 @@
         <v>51</v>
       </c>
       <c r="J9">
-        <v>16</v>
+        <v>17</v>
       </c>
     </row>
     <row r="10" spans="1:10">
@@ -13741,7 +13741,7 @@
         <v>706</v>
       </c>
       <c r="J11">
-        <v>354</v>
+        <v>356</v>
       </c>
     </row>
   </sheetData>
@@ -13830,7 +13830,7 @@
         <v>194</v>
       </c>
       <c r="J2">
-        <v>99</v>
+        <v>100</v>
       </c>
     </row>
     <row r="3" spans="1:10">
@@ -13862,7 +13862,7 @@
         <v>182</v>
       </c>
       <c r="J3">
-        <v>112</v>
+        <v>113</v>
       </c>
     </row>
     <row r="4" spans="1:10">
@@ -13894,7 +13894,7 @@
         <v>8</v>
       </c>
       <c r="J4">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="5" spans="1:10">
@@ -14022,7 +14022,7 @@
         <v>202</v>
       </c>
       <c r="J8">
-        <v>207</v>
+        <v>208</v>
       </c>
     </row>
     <row r="9" spans="1:10">
@@ -14086,7 +14086,7 @@
         <v>587</v>
       </c>
       <c r="J10">
-        <v>320</v>
+        <v>323</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -14118,7 +14118,7 @@
         <v>1515</v>
       </c>
       <c r="J11">
-        <v>944</v>
+        <v>951</v>
       </c>
     </row>
   </sheetData>
@@ -14545,7 +14545,7 @@
         <v>55</v>
       </c>
       <c r="J2">
-        <v>33</v>
+        <v>34</v>
       </c>
     </row>
     <row r="3" spans="1:10">
@@ -14734,7 +14734,7 @@
         <v>175</v>
       </c>
       <c r="J8">
-        <v>140</v>
+        <v>142</v>
       </c>
     </row>
     <row r="9" spans="1:10">
@@ -14798,7 +14798,7 @@
         <v>379</v>
       </c>
       <c r="J10">
-        <v>188</v>
+        <v>190</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -14830,7 +14830,7 @@
         <v>768</v>
       </c>
       <c r="J11">
-        <v>447</v>
+        <v>452</v>
       </c>
     </row>
   </sheetData>
@@ -15281,7 +15281,7 @@
         <v>190</v>
       </c>
       <c r="J2">
-        <v>90</v>
+        <v>92</v>
       </c>
     </row>
     <row r="3" spans="1:10">
@@ -15313,7 +15313,7 @@
         <v>205</v>
       </c>
       <c r="J3">
-        <v>116</v>
+        <v>117</v>
       </c>
     </row>
     <row r="4" spans="1:10">
@@ -15441,7 +15441,7 @@
         <v>24</v>
       </c>
       <c r="J7">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="8" spans="1:10">
@@ -15473,7 +15473,7 @@
         <v>484</v>
       </c>
       <c r="J8">
-        <v>272</v>
+        <v>273</v>
       </c>
     </row>
     <row r="9" spans="1:10">
@@ -15537,7 +15537,7 @@
         <v>612</v>
       </c>
       <c r="J10">
-        <v>306</v>
+        <v>307</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -15569,7 +15569,7 @@
         <v>1793</v>
       </c>
       <c r="J11">
-        <v>944</v>
+        <v>950</v>
       </c>
     </row>
   </sheetData>
@@ -15882,7 +15882,7 @@
         <v>109</v>
       </c>
       <c r="J9">
-        <v>81</v>
+        <v>82</v>
       </c>
     </row>
     <row r="10" spans="1:10">
@@ -15946,7 +15946,7 @@
         <v>1244</v>
       </c>
       <c r="J11">
-        <v>633</v>
+        <v>634</v>
       </c>
     </row>
   </sheetData>
@@ -16212,7 +16212,7 @@
         <v>294</v>
       </c>
       <c r="J8">
-        <v>197</v>
+        <v>199</v>
       </c>
     </row>
     <row r="9" spans="1:10">
@@ -16276,7 +16276,7 @@
         <v>2021</v>
       </c>
       <c r="J10">
-        <v>934</v>
+        <v>937</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -16308,7 +16308,7 @@
         <v>2664</v>
       </c>
       <c r="J11">
-        <v>1305</v>
+        <v>1310</v>
       </c>
     </row>
   </sheetData>
@@ -16429,7 +16429,7 @@
         <v>416</v>
       </c>
       <c r="J3">
-        <v>204</v>
+        <v>205</v>
       </c>
     </row>
     <row r="4" spans="1:10">
@@ -16493,7 +16493,7 @@
         <v>170</v>
       </c>
       <c r="J5">
-        <v>58</v>
+        <v>59</v>
       </c>
     </row>
     <row r="6" spans="1:10">
@@ -16589,7 +16589,7 @@
         <v>707</v>
       </c>
       <c r="J8">
-        <v>524</v>
+        <v>529</v>
       </c>
     </row>
     <row r="9" spans="1:10">
@@ -16621,7 +16621,7 @@
         <v>363</v>
       </c>
       <c r="J9">
-        <v>203</v>
+        <v>205</v>
       </c>
     </row>
     <row r="10" spans="1:10">
@@ -16653,7 +16653,7 @@
         <v>968</v>
       </c>
       <c r="J10">
-        <v>506</v>
+        <v>510</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -16685,7 +16685,7 @@
         <v>3011</v>
       </c>
       <c r="J11">
-        <v>1728</v>
+        <v>1741</v>
       </c>
     </row>
   </sheetData>
@@ -16806,7 +16806,7 @@
         <v>248</v>
       </c>
       <c r="J3">
-        <v>116</v>
+        <v>118</v>
       </c>
     </row>
     <row r="4" spans="1:10">
@@ -16870,7 +16870,7 @@
         <v>261</v>
       </c>
       <c r="J5">
-        <v>126</v>
+        <v>128</v>
       </c>
     </row>
     <row r="6" spans="1:10">
@@ -16966,7 +16966,7 @@
         <v>567</v>
       </c>
       <c r="J8">
-        <v>521</v>
+        <v>524</v>
       </c>
     </row>
     <row r="9" spans="1:10">
@@ -17030,7 +17030,7 @@
         <v>1023</v>
       </c>
       <c r="J10">
-        <v>474</v>
+        <v>475</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -17062,7 +17062,7 @@
         <v>2685</v>
       </c>
       <c r="J11">
-        <v>1537</v>
+        <v>1545</v>
       </c>
     </row>
   </sheetData>
@@ -17183,7 +17183,7 @@
         <v>445</v>
       </c>
       <c r="J3">
-        <v>282</v>
+        <v>285</v>
       </c>
     </row>
     <row r="4" spans="1:10">
@@ -17247,7 +17247,7 @@
         <v>251</v>
       </c>
       <c r="J5">
-        <v>109</v>
+        <v>110</v>
       </c>
     </row>
     <row r="6" spans="1:10">
@@ -17279,7 +17279,7 @@
         <v>93</v>
       </c>
       <c r="J6">
-        <v>49</v>
+        <v>50</v>
       </c>
     </row>
     <row r="7" spans="1:10">
@@ -17311,7 +17311,7 @@
         <v>49</v>
       </c>
       <c r="J7">
-        <v>28</v>
+        <v>29</v>
       </c>
     </row>
     <row r="8" spans="1:10">
@@ -17343,7 +17343,7 @@
         <v>1270</v>
       </c>
       <c r="J8">
-        <v>706</v>
+        <v>708</v>
       </c>
     </row>
     <row r="9" spans="1:10">
@@ -17375,7 +17375,7 @@
         <v>497</v>
       </c>
       <c r="J9">
-        <v>281</v>
+        <v>285</v>
       </c>
     </row>
     <row r="10" spans="1:10">
@@ -17407,7 +17407,7 @@
         <v>1652</v>
       </c>
       <c r="J10">
-        <v>851</v>
+        <v>854</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -17439,7 +17439,7 @@
         <v>4744</v>
       </c>
       <c r="J11">
-        <v>2588</v>
+        <v>2603</v>
       </c>
     </row>
   </sheetData>
@@ -17720,7 +17720,7 @@
         <v>441</v>
       </c>
       <c r="J8">
-        <v>316</v>
+        <v>318</v>
       </c>
     </row>
     <row r="9" spans="1:10">
@@ -17784,7 +17784,7 @@
         <v>455</v>
       </c>
       <c r="J10">
-        <v>274</v>
+        <v>275</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -17816,7 +17816,7 @@
         <v>1354</v>
       </c>
       <c r="J11">
-        <v>800</v>
+        <v>803</v>
       </c>
     </row>
   </sheetData>
@@ -17905,7 +17905,7 @@
         <v>47</v>
       </c>
       <c r="J2">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="3" spans="1:10">
@@ -18085,7 +18085,7 @@
         <v>250</v>
       </c>
       <c r="J8">
-        <v>167</v>
+        <v>169</v>
       </c>
     </row>
     <row r="9" spans="1:10">
@@ -18117,7 +18117,7 @@
         <v>61</v>
       </c>
       <c r="J9">
-        <v>38</v>
+        <v>39</v>
       </c>
     </row>
     <row r="10" spans="1:10">
@@ -18149,7 +18149,7 @@
         <v>417</v>
       </c>
       <c r="J10">
-        <v>207</v>
+        <v>209</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -18181,7 +18181,7 @@
         <v>903</v>
       </c>
       <c r="J11">
-        <v>498</v>
+        <v>504</v>
       </c>
     </row>
   </sheetData>
@@ -18462,7 +18462,7 @@
         <v>754</v>
       </c>
       <c r="J8">
-        <v>399</v>
+        <v>401</v>
       </c>
     </row>
     <row r="9" spans="1:10">
@@ -18494,7 +18494,7 @@
         <v>233</v>
       </c>
       <c r="J9">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
     <row r="10" spans="1:10">
@@ -18526,7 +18526,7 @@
         <v>911</v>
       </c>
       <c r="J10">
-        <v>499</v>
+        <v>504</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -18558,7 +18558,7 @@
         <v>2636</v>
       </c>
       <c r="J11">
-        <v>1412</v>
+        <v>1418</v>
       </c>
     </row>
   </sheetData>
@@ -18647,7 +18647,7 @@
         <v>22</v>
       </c>
       <c r="J2">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="3" spans="1:10">
@@ -18908,7 +18908,7 @@
         <v>247</v>
       </c>
       <c r="J11">
-        <v>148</v>
+        <v>149</v>
       </c>
     </row>
   </sheetData>
@@ -18997,7 +18997,7 @@
         <v>179</v>
       </c>
       <c r="J2">
-        <v>85</v>
+        <v>86</v>
       </c>
     </row>
     <row r="3" spans="1:10">
@@ -19125,7 +19125,7 @@
         <v>41</v>
       </c>
       <c r="J6">
-        <v>26</v>
+        <v>27</v>
       </c>
     </row>
     <row r="7" spans="1:10">
@@ -19253,7 +19253,7 @@
         <v>828</v>
       </c>
       <c r="J10">
-        <v>388</v>
+        <v>392</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -19285,7 +19285,7 @@
         <v>2046</v>
       </c>
       <c r="J11">
-        <v>1001</v>
+        <v>1007</v>
       </c>
     </row>
   </sheetData>
@@ -19374,7 +19374,7 @@
         <v>37</v>
       </c>
       <c r="J2">
-        <v>20</v>
+        <v>21</v>
       </c>
     </row>
     <row r="3" spans="1:10">
@@ -19618,7 +19618,7 @@
         <v>630</v>
       </c>
       <c r="J10">
-        <v>287</v>
+        <v>289</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -19650,7 +19650,7 @@
         <v>960</v>
       </c>
       <c r="J11">
-        <v>526</v>
+        <v>529</v>
       </c>
     </row>
   </sheetData>
@@ -20293,7 +20293,7 @@
         <v>308</v>
       </c>
       <c r="J8">
-        <v>203</v>
+        <v>207</v>
       </c>
     </row>
     <row r="9" spans="1:10">
@@ -20357,7 +20357,7 @@
         <v>320</v>
       </c>
       <c r="J10">
-        <v>166</v>
+        <v>167</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -20389,7 +20389,7 @@
         <v>970</v>
       </c>
       <c r="J11">
-        <v>561</v>
+        <v>566</v>
       </c>
     </row>
   </sheetData>
@@ -20728,7 +20728,7 @@
         <v>381</v>
       </c>
       <c r="J10">
-        <v>182</v>
+        <v>183</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -20760,7 +20760,7 @@
         <v>721</v>
       </c>
       <c r="J11">
-        <v>415</v>
+        <v>416</v>
       </c>
     </row>
   </sheetData>
@@ -21084,7 +21084,7 @@
         <v>280</v>
       </c>
       <c r="J10">
-        <v>130</v>
+        <v>132</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -21116,7 +21116,7 @@
         <v>436</v>
       </c>
       <c r="J11">
-        <v>247</v>
+        <v>249</v>
       </c>
     </row>
   </sheetData>
@@ -21452,7 +21452,7 @@
         <v>216</v>
       </c>
       <c r="J10">
-        <v>108</v>
+        <v>109</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -21484,7 +21484,7 @@
         <v>436</v>
       </c>
       <c r="J11">
-        <v>238</v>
+        <v>239</v>
       </c>
     </row>
   </sheetData>
@@ -21826,7 +21826,7 @@
         <v>670</v>
       </c>
       <c r="J10">
-        <v>329</v>
+        <v>331</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -21858,7 +21858,7 @@
         <v>1337</v>
       </c>
       <c r="J11">
-        <v>813</v>
+        <v>815</v>
       </c>
     </row>
   </sheetData>
@@ -22139,7 +22139,7 @@
         <v>126</v>
       </c>
       <c r="J8">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="9" spans="1:10">
@@ -22171,7 +22171,7 @@
         <v>46</v>
       </c>
       <c r="J9">
-        <v>27</v>
+        <v>28</v>
       </c>
     </row>
     <row r="10" spans="1:10">
@@ -22203,7 +22203,7 @@
         <v>492</v>
       </c>
       <c r="J10">
-        <v>297</v>
+        <v>298</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -22235,7 +22235,7 @@
         <v>918</v>
       </c>
       <c r="J11">
-        <v>517</v>
+        <v>518</v>
       </c>
     </row>
   </sheetData>
@@ -22863,7 +22863,7 @@
         <v>196</v>
       </c>
       <c r="J8">
-        <v>110</v>
+        <v>114</v>
       </c>
     </row>
     <row r="9" spans="1:10">
@@ -22959,7 +22959,7 @@
         <v>695</v>
       </c>
       <c r="J11">
-        <v>399</v>
+        <v>403</v>
       </c>
     </row>
   </sheetData>
@@ -23228,7 +23228,7 @@
         <v>92</v>
       </c>
       <c r="J8">
-        <v>90</v>
+        <v>92</v>
       </c>
     </row>
     <row r="9" spans="1:10">
@@ -23292,7 +23292,7 @@
         <v>277</v>
       </c>
       <c r="J10">
-        <v>162</v>
+        <v>163</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -23324,7 +23324,7 @@
         <v>500</v>
       </c>
       <c r="J11">
-        <v>322</v>
+        <v>325</v>
       </c>
     </row>
   </sheetData>
@@ -23666,7 +23666,7 @@
         <v>189</v>
       </c>
       <c r="J10">
-        <v>117</v>
+        <v>119</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -23698,7 +23698,7 @@
         <v>430</v>
       </c>
       <c r="J11">
-        <v>247</v>
+        <v>249</v>
       </c>
     </row>
   </sheetData>
@@ -23880,7 +23880,7 @@
         <v>77</v>
       </c>
       <c r="J5">
-        <v>28</v>
+        <v>29</v>
       </c>
     </row>
     <row r="6" spans="1:10">
@@ -24072,7 +24072,7 @@
         <v>793</v>
       </c>
       <c r="J11">
-        <v>521</v>
+        <v>522</v>
       </c>
     </row>
   </sheetData>
@@ -24373,7 +24373,7 @@
         <v>41</v>
       </c>
       <c r="J9">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="10" spans="1:10">
@@ -24437,7 +24437,7 @@
         <v>396</v>
       </c>
       <c r="J11">
-        <v>210</v>
+        <v>211</v>
       </c>
     </row>
   </sheetData>
@@ -24616,7 +24616,7 @@
         <v>82</v>
       </c>
       <c r="J5">
-        <v>69</v>
+        <v>70</v>
       </c>
     </row>
     <row r="6" spans="1:10">
@@ -24706,7 +24706,7 @@
         <v>167</v>
       </c>
       <c r="J8">
-        <v>111</v>
+        <v>113</v>
       </c>
     </row>
     <row r="9" spans="1:10">
@@ -24770,7 +24770,7 @@
         <v>784</v>
       </c>
       <c r="J10">
-        <v>452</v>
+        <v>454</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -24802,7 +24802,7 @@
         <v>1258</v>
       </c>
       <c r="J11">
-        <v>713</v>
+        <v>718</v>
       </c>
     </row>
   </sheetData>
@@ -25083,7 +25083,7 @@
         <v>151</v>
       </c>
       <c r="J8">
-        <v>112</v>
+        <v>113</v>
       </c>
     </row>
     <row r="9" spans="1:10">
@@ -25179,7 +25179,7 @@
         <v>867</v>
       </c>
       <c r="J11">
-        <v>453</v>
+        <v>454</v>
       </c>
     </row>
   </sheetData>
@@ -25476,7 +25476,7 @@
         <v>576</v>
       </c>
       <c r="J10">
-        <v>284</v>
+        <v>290</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -25508,7 +25508,7 @@
         <v>628</v>
       </c>
       <c r="J11">
-        <v>305</v>
+        <v>311</v>
       </c>
     </row>
   </sheetData>
@@ -25597,7 +25597,7 @@
         <v>53</v>
       </c>
       <c r="J2">
-        <v>40</v>
+        <v>41</v>
       </c>
     </row>
     <row r="3" spans="1:10">
@@ -25629,7 +25629,7 @@
         <v>53</v>
       </c>
       <c r="J3">
-        <v>39</v>
+        <v>40</v>
       </c>
     </row>
     <row r="4" spans="1:10">
@@ -25885,7 +25885,7 @@
         <v>462</v>
       </c>
       <c r="J11">
-        <v>284</v>
+        <v>286</v>
       </c>
     </row>
   </sheetData>
@@ -26113,7 +26113,7 @@
         <v>28</v>
       </c>
       <c r="J7">
-        <v>31</v>
+        <v>32</v>
       </c>
     </row>
     <row r="8" spans="1:10">
@@ -26209,7 +26209,7 @@
         <v>233</v>
       </c>
       <c r="J10">
-        <v>144</v>
+        <v>145</v>
       </c>
     </row>
   </sheetData>
@@ -26298,7 +26298,7 @@
         <v>78</v>
       </c>
       <c r="J2">
-        <v>50</v>
+        <v>51</v>
       </c>
     </row>
     <row r="3" spans="1:10">
@@ -26330,7 +26330,7 @@
         <v>87</v>
       </c>
       <c r="J3">
-        <v>64</v>
+        <v>65</v>
       </c>
     </row>
     <row r="4" spans="1:10">
@@ -26394,7 +26394,7 @@
         <v>130</v>
       </c>
       <c r="J5">
-        <v>51</v>
+        <v>52</v>
       </c>
     </row>
     <row r="6" spans="1:10">
@@ -26490,7 +26490,7 @@
         <v>198</v>
       </c>
       <c r="J8">
-        <v>147</v>
+        <v>148</v>
       </c>
     </row>
     <row r="9" spans="1:10">
@@ -26522,7 +26522,7 @@
         <v>130</v>
       </c>
       <c r="J9">
-        <v>51</v>
+        <v>52</v>
       </c>
     </row>
     <row r="10" spans="1:10">
@@ -26554,7 +26554,7 @@
         <v>1118</v>
       </c>
       <c r="J10">
-        <v>562</v>
+        <v>564</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -26586,7 +26586,7 @@
         <v>1797</v>
       </c>
       <c r="J11">
-        <v>954</v>
+        <v>961</v>
       </c>
     </row>
   </sheetData>
@@ -26858,7 +26858,7 @@
         <v>110</v>
       </c>
       <c r="J8">
-        <v>82</v>
+        <v>83</v>
       </c>
     </row>
     <row r="9" spans="1:10">
@@ -26922,7 +26922,7 @@
         <v>371</v>
       </c>
       <c r="J10">
-        <v>145</v>
+        <v>146</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -26954,7 +26954,7 @@
         <v>719</v>
       </c>
       <c r="J11">
-        <v>328</v>
+        <v>330</v>
       </c>
     </row>
   </sheetData>
@@ -27127,7 +27127,7 @@
         <v>74</v>
       </c>
       <c r="J5">
-        <v>56</v>
+        <v>57</v>
       </c>
     </row>
     <row r="6" spans="1:10">
@@ -27237,7 +27237,7 @@
         <v>37</v>
       </c>
       <c r="J9">
-        <v>23</v>
+        <v>26</v>
       </c>
     </row>
     <row r="10" spans="1:10">
@@ -27301,7 +27301,7 @@
         <v>715</v>
       </c>
       <c r="J11">
-        <v>406</v>
+        <v>410</v>
       </c>
     </row>
   </sheetData>
@@ -27578,7 +27578,7 @@
         <v>52</v>
       </c>
       <c r="J9">
-        <v>31</v>
+        <v>33</v>
       </c>
     </row>
     <row r="10" spans="1:10">
@@ -27610,7 +27610,7 @@
         <v>376</v>
       </c>
       <c r="J10">
-        <v>236</v>
+        <v>238</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -27642,7 +27642,7 @@
         <v>595</v>
       </c>
       <c r="J11">
-        <v>388</v>
+        <v>392</v>
       </c>
     </row>
   </sheetData>
@@ -27920,7 +27920,7 @@
         <v>141</v>
       </c>
       <c r="J8">
-        <v>95</v>
+        <v>97</v>
       </c>
     </row>
     <row r="9" spans="1:10">
@@ -27984,7 +27984,7 @@
         <v>193</v>
       </c>
       <c r="J10">
-        <v>87</v>
+        <v>88</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -28016,7 +28016,7 @@
         <v>519</v>
       </c>
       <c r="J11">
-        <v>284</v>
+        <v>287</v>
       </c>
     </row>
   </sheetData>
@@ -28551,7 +28551,7 @@
         <v>79</v>
       </c>
       <c r="J5">
-        <v>37</v>
+        <v>38</v>
       </c>
     </row>
     <row r="6" spans="1:10">
@@ -28644,7 +28644,7 @@
         <v>137</v>
       </c>
       <c r="J8">
-        <v>96</v>
+        <v>98</v>
       </c>
     </row>
     <row r="9" spans="1:10">
@@ -28676,7 +28676,7 @@
         <v>90</v>
       </c>
       <c r="J9">
-        <v>34</v>
+        <v>35</v>
       </c>
     </row>
     <row r="10" spans="1:10">
@@ -28708,7 +28708,7 @@
         <v>542</v>
       </c>
       <c r="J10">
-        <v>271</v>
+        <v>276</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -28740,7 +28740,7 @@
         <v>949</v>
       </c>
       <c r="J11">
-        <v>481</v>
+        <v>490</v>
       </c>
     </row>
   </sheetData>
@@ -29015,7 +29015,7 @@
         <v>122</v>
       </c>
       <c r="J8">
-        <v>113</v>
+        <v>114</v>
       </c>
     </row>
     <row r="9" spans="1:10">
@@ -29111,7 +29111,7 @@
         <v>437</v>
       </c>
       <c r="J11">
-        <v>296</v>
+        <v>297</v>
       </c>
     </row>
   </sheetData>
@@ -29389,7 +29389,7 @@
         <v>216</v>
       </c>
       <c r="J8">
-        <v>182</v>
+        <v>183</v>
       </c>
     </row>
     <row r="9" spans="1:10">
@@ -29421,7 +29421,7 @@
         <v>107</v>
       </c>
       <c r="J9">
-        <v>51</v>
+        <v>52</v>
       </c>
     </row>
     <row r="10" spans="1:10">
@@ -29453,7 +29453,7 @@
         <v>1222</v>
       </c>
       <c r="J10">
-        <v>622</v>
+        <v>624</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -29485,7 +29485,7 @@
         <v>1878</v>
       </c>
       <c r="J11">
-        <v>1050</v>
+        <v>1054</v>
       </c>
     </row>
   </sheetData>
@@ -29763,7 +29763,7 @@
         <v>140</v>
       </c>
       <c r="J8">
-        <v>129</v>
+        <v>130</v>
       </c>
     </row>
     <row r="9" spans="1:10">
@@ -29827,7 +29827,7 @@
         <v>440</v>
       </c>
       <c r="J10">
-        <v>244</v>
+        <v>246</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -29859,7 +29859,7 @@
         <v>761</v>
       </c>
       <c r="J11">
-        <v>469</v>
+        <v>472</v>
       </c>
     </row>
   </sheetData>
@@ -29948,7 +29948,7 @@
         <v>128</v>
       </c>
       <c r="J2">
-        <v>60</v>
+        <v>61</v>
       </c>
     </row>
     <row r="3" spans="1:10">
@@ -30140,7 +30140,7 @@
         <v>383</v>
       </c>
       <c r="J8">
-        <v>272</v>
+        <v>274</v>
       </c>
     </row>
     <row r="9" spans="1:10">
@@ -30204,7 +30204,7 @@
         <v>527</v>
       </c>
       <c r="J10">
-        <v>294</v>
+        <v>296</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -30236,7 +30236,7 @@
         <v>1488</v>
       </c>
       <c r="J11">
-        <v>847</v>
+        <v>852</v>
       </c>
     </row>
   </sheetData>
@@ -30475,7 +30475,7 @@
         <v>27</v>
       </c>
       <c r="J8">
-        <v>42</v>
+        <v>43</v>
       </c>
     </row>
     <row r="9" spans="1:10">
@@ -30571,7 +30571,7 @@
         <v>248</v>
       </c>
       <c r="J11">
-        <v>150</v>
+        <v>151</v>
       </c>
     </row>
   </sheetData>
@@ -31513,7 +31513,7 @@
         <v>123</v>
       </c>
       <c r="J8">
-        <v>120</v>
+        <v>121</v>
       </c>
     </row>
     <row r="9" spans="1:10">
@@ -31609,7 +31609,7 @@
         <v>335</v>
       </c>
       <c r="J11">
-        <v>243</v>
+        <v>244</v>
       </c>
     </row>
   </sheetData>
@@ -32075,7 +32075,7 @@
         <v>70</v>
       </c>
       <c r="J2">
-        <v>39</v>
+        <v>40</v>
       </c>
     </row>
     <row r="3" spans="1:10">
@@ -32107,7 +32107,7 @@
         <v>89</v>
       </c>
       <c r="J3">
-        <v>43</v>
+        <v>44</v>
       </c>
     </row>
     <row r="4" spans="1:10">
@@ -32165,7 +32165,7 @@
         <v>39</v>
       </c>
       <c r="J5">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="6" spans="1:10">
@@ -32197,7 +32197,7 @@
         <v>14</v>
       </c>
       <c r="J6">
-        <v>14</v>
+        <v>15</v>
       </c>
     </row>
     <row r="7" spans="1:10">
@@ -32325,7 +32325,7 @@
         <v>670</v>
       </c>
       <c r="J10">
-        <v>302</v>
+        <v>305</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -32357,7 +32357,7 @@
         <v>1368</v>
       </c>
       <c r="J11">
-        <v>789</v>
+        <v>794</v>
       </c>
     </row>
   </sheetData>
@@ -32632,7 +32632,7 @@
         <v>338</v>
       </c>
       <c r="J8">
-        <v>239</v>
+        <v>240</v>
       </c>
     </row>
     <row r="9" spans="1:10">
@@ -32664,7 +32664,7 @@
         <v>169</v>
       </c>
       <c r="J9">
-        <v>71</v>
+        <v>74</v>
       </c>
     </row>
     <row r="10" spans="1:10">
@@ -32696,7 +32696,7 @@
         <v>1773</v>
       </c>
       <c r="J10">
-        <v>926</v>
+        <v>932</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -32728,7 +32728,7 @@
         <v>2622</v>
       </c>
       <c r="J11">
-        <v>1391</v>
+        <v>1401</v>
       </c>
     </row>
   </sheetData>
@@ -33732,7 +33732,7 @@
         <v>66</v>
       </c>
       <c r="J9">
-        <v>33</v>
+        <v>34</v>
       </c>
     </row>
     <row r="10" spans="1:10">
@@ -33796,7 +33796,7 @@
         <v>1187</v>
       </c>
       <c r="J11">
-        <v>579</v>
+        <v>580</v>
       </c>
     </row>
   </sheetData>
@@ -35095,7 +35095,7 @@
         <v>211</v>
       </c>
       <c r="J10">
-        <v>138</v>
+        <v>139</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -35127,7 +35127,7 @@
         <v>406</v>
       </c>
       <c r="J11">
-        <v>271</v>
+        <v>272</v>
       </c>
     </row>
   </sheetData>
@@ -35746,7 +35746,7 @@
         <v>187</v>
       </c>
       <c r="J9">
-        <v>110</v>
+        <v>112</v>
       </c>
     </row>
     <row r="10" spans="1:10">
@@ -35778,7 +35778,7 @@
         <v>258</v>
       </c>
       <c r="J10">
-        <v>143</v>
+        <v>145</v>
       </c>
     </row>
   </sheetData>
@@ -36388,7 +36388,7 @@
         <v>291</v>
       </c>
       <c r="J8">
-        <v>178</v>
+        <v>180</v>
       </c>
     </row>
     <row r="9" spans="1:10">
@@ -36484,7 +36484,7 @@
         <v>1669</v>
       </c>
       <c r="J11">
-        <v>865</v>
+        <v>867</v>
       </c>
     </row>
   </sheetData>
@@ -37508,7 +37508,7 @@
         <v>116</v>
       </c>
       <c r="J10">
-        <v>59</v>
+        <v>60</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -37540,7 +37540,7 @@
         <v>236</v>
       </c>
       <c r="J11">
-        <v>143</v>
+        <v>144</v>
       </c>
     </row>
   </sheetData>
@@ -37791,7 +37791,7 @@
         <v>160</v>
       </c>
       <c r="J8">
-        <v>56</v>
+        <v>57</v>
       </c>
     </row>
     <row r="9" spans="1:10">
@@ -37855,7 +37855,7 @@
         <v>717</v>
       </c>
       <c r="J10">
-        <v>301</v>
+        <v>302</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -37887,7 +37887,7 @@
         <v>1066</v>
       </c>
       <c r="J11">
-        <v>441</v>
+        <v>443</v>
       </c>
     </row>
   </sheetData>
@@ -38854,7 +38854,7 @@
         <v>225</v>
       </c>
       <c r="J10">
-        <v>104</v>
+        <v>105</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -38886,7 +38886,7 @@
         <v>307</v>
       </c>
       <c r="J11">
-        <v>145</v>
+        <v>146</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add data for 2023-07-14
</commit_message>
<xml_diff>
--- a/output/index-crime-full-year.xlsx
+++ b/output/index-crime-full-year.xlsx
@@ -895,7 +895,7 @@
         <v>7277</v>
       </c>
       <c r="J2">
-        <v>3907</v>
+        <v>3928</v>
       </c>
     </row>
     <row r="3" spans="1:10">
@@ -927,7 +927,7 @@
         <v>7486</v>
       </c>
       <c r="J3">
-        <v>4107</v>
+        <v>4129</v>
       </c>
     </row>
     <row r="4" spans="1:10">
@@ -959,7 +959,7 @@
         <v>422</v>
       </c>
       <c r="J4">
-        <v>259</v>
+        <v>262</v>
       </c>
     </row>
     <row r="5" spans="1:10">
@@ -991,7 +991,7 @@
         <v>7592</v>
       </c>
       <c r="J5">
-        <v>3848</v>
+        <v>3870</v>
       </c>
     </row>
     <row r="6" spans="1:10">
@@ -1020,10 +1020,10 @@
         <v>1698</v>
       </c>
       <c r="I6">
-        <v>1770</v>
+        <v>1771</v>
       </c>
       <c r="J6">
-        <v>927</v>
+        <v>936</v>
       </c>
     </row>
     <row r="7" spans="1:10">
@@ -1055,7 +1055,7 @@
         <v>718</v>
       </c>
       <c r="J7">
-        <v>329</v>
+        <v>330</v>
       </c>
     </row>
     <row r="8" spans="1:10">
@@ -1084,10 +1084,10 @@
         <v>10602</v>
       </c>
       <c r="I8">
-        <v>21449</v>
+        <v>21444</v>
       </c>
       <c r="J8">
-        <v>15588</v>
+        <v>15664</v>
       </c>
     </row>
     <row r="9" spans="1:10">
@@ -1119,7 +1119,7 @@
         <v>8965</v>
       </c>
       <c r="J9">
-        <v>4908</v>
+        <v>4934</v>
       </c>
     </row>
     <row r="10" spans="1:10">
@@ -1151,7 +1151,7 @@
         <v>54806</v>
       </c>
       <c r="J10">
-        <v>28344</v>
+        <v>28554</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -1180,10 +1180,10 @@
         <v>84592</v>
       </c>
       <c r="I11">
-        <v>110485</v>
+        <v>110481</v>
       </c>
       <c r="J11">
-        <v>62217</v>
+        <v>62607</v>
       </c>
     </row>
   </sheetData>
@@ -1353,7 +1353,7 @@
         <v>54</v>
       </c>
       <c r="J5">
-        <v>32</v>
+        <v>33</v>
       </c>
     </row>
     <row r="6" spans="1:10">
@@ -1440,7 +1440,7 @@
         <v>227</v>
       </c>
       <c r="J8">
-        <v>194</v>
+        <v>196</v>
       </c>
     </row>
     <row r="9" spans="1:10">
@@ -1504,7 +1504,7 @@
         <v>648</v>
       </c>
       <c r="J10">
-        <v>382</v>
+        <v>386</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -1536,7 +1536,7 @@
         <v>1153</v>
       </c>
       <c r="J11">
-        <v>734</v>
+        <v>741</v>
       </c>
     </row>
   </sheetData>
@@ -1931,7 +1931,7 @@
         <v>81</v>
       </c>
       <c r="J3">
-        <v>43</v>
+        <v>44</v>
       </c>
     </row>
     <row r="4" spans="1:10">
@@ -2155,7 +2155,7 @@
         <v>820</v>
       </c>
       <c r="J10">
-        <v>486</v>
+        <v>494</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -2187,7 +2187,7 @@
         <v>1713</v>
       </c>
       <c r="J11">
-        <v>1049</v>
+        <v>1058</v>
       </c>
     </row>
   </sheetData>
@@ -2526,7 +2526,7 @@
         <v>712</v>
       </c>
       <c r="J10">
-        <v>386</v>
+        <v>388</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -2558,7 +2558,7 @@
         <v>1228</v>
       </c>
       <c r="J11">
-        <v>698</v>
+        <v>700</v>
       </c>
     </row>
   </sheetData>
@@ -2647,7 +2647,7 @@
         <v>220</v>
       </c>
       <c r="J2">
-        <v>117</v>
+        <v>118</v>
       </c>
     </row>
     <row r="3" spans="1:10">
@@ -2839,7 +2839,7 @@
         <v>700</v>
       </c>
       <c r="J8">
-        <v>459</v>
+        <v>461</v>
       </c>
     </row>
     <row r="9" spans="1:10">
@@ -2871,7 +2871,7 @@
         <v>216</v>
       </c>
       <c r="J9">
-        <v>107</v>
+        <v>108</v>
       </c>
     </row>
     <row r="10" spans="1:10">
@@ -2903,7 +2903,7 @@
         <v>820</v>
       </c>
       <c r="J10">
-        <v>424</v>
+        <v>425</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -2935,7 +2935,7 @@
         <v>2472</v>
       </c>
       <c r="J11">
-        <v>1386</v>
+        <v>1391</v>
       </c>
     </row>
   </sheetData>
@@ -3056,7 +3056,7 @@
         <v>56</v>
       </c>
       <c r="J3">
-        <v>24</v>
+        <v>25</v>
       </c>
     </row>
     <row r="4" spans="1:10">
@@ -3210,10 +3210,10 @@
         <v>82</v>
       </c>
       <c r="I8">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="J8">
-        <v>241</v>
+        <v>243</v>
       </c>
     </row>
     <row r="9" spans="1:10">
@@ -3277,7 +3277,7 @@
         <v>913</v>
       </c>
       <c r="J10">
-        <v>575</v>
+        <v>581</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -3306,10 +3306,10 @@
         <v>1183</v>
       </c>
       <c r="I11">
-        <v>1601</v>
+        <v>1600</v>
       </c>
       <c r="J11">
-        <v>1033</v>
+        <v>1042</v>
       </c>
     </row>
   </sheetData>
@@ -3648,7 +3648,7 @@
         <v>106</v>
       </c>
       <c r="J10">
-        <v>42</v>
+        <v>43</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -3680,7 +3680,7 @@
         <v>260</v>
       </c>
       <c r="J11">
-        <v>158</v>
+        <v>159</v>
       </c>
     </row>
   </sheetData>
@@ -3897,7 +3897,7 @@
         <v>24</v>
       </c>
       <c r="J6">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="7" spans="1:10">
@@ -3961,7 +3961,7 @@
         <v>220</v>
       </c>
       <c r="J8">
-        <v>183</v>
+        <v>184</v>
       </c>
     </row>
     <row r="9" spans="1:10">
@@ -3993,7 +3993,7 @@
         <v>63</v>
       </c>
       <c r="J9">
-        <v>32</v>
+        <v>33</v>
       </c>
     </row>
     <row r="10" spans="1:10">
@@ -4025,7 +4025,7 @@
         <v>681</v>
       </c>
       <c r="J10">
-        <v>452</v>
+        <v>455</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -4057,7 +4057,7 @@
         <v>1279</v>
       </c>
       <c r="J11">
-        <v>830</v>
+        <v>836</v>
       </c>
     </row>
   </sheetData>
@@ -4178,7 +4178,7 @@
         <v>530</v>
       </c>
       <c r="J3">
-        <v>282</v>
+        <v>284</v>
       </c>
     </row>
     <row r="4" spans="1:10">
@@ -4274,7 +4274,7 @@
         <v>83</v>
       </c>
       <c r="J6">
-        <v>45</v>
+        <v>46</v>
       </c>
     </row>
     <row r="7" spans="1:10">
@@ -4338,7 +4338,7 @@
         <v>794</v>
       </c>
       <c r="J8">
-        <v>581</v>
+        <v>582</v>
       </c>
     </row>
     <row r="9" spans="1:10">
@@ -4370,7 +4370,7 @@
         <v>433</v>
       </c>
       <c r="J9">
-        <v>196</v>
+        <v>197</v>
       </c>
     </row>
     <row r="10" spans="1:10">
@@ -4402,7 +4402,7 @@
         <v>1302</v>
       </c>
       <c r="J10">
-        <v>683</v>
+        <v>689</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -4434,7 +4434,7 @@
         <v>3950</v>
       </c>
       <c r="J11">
-        <v>2245</v>
+        <v>2256</v>
       </c>
     </row>
   </sheetData>
@@ -4697,7 +4697,7 @@
         <v>131</v>
       </c>
       <c r="J8">
-        <v>135</v>
+        <v>136</v>
       </c>
     </row>
     <row r="9" spans="1:10">
@@ -4761,7 +4761,7 @@
         <v>921</v>
       </c>
       <c r="J10">
-        <v>377</v>
+        <v>380</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -4793,7 +4793,7 @@
         <v>1318</v>
       </c>
       <c r="J11">
-        <v>648</v>
+        <v>652</v>
       </c>
     </row>
   </sheetData>
@@ -4882,7 +4882,7 @@
         <v>216</v>
       </c>
       <c r="J2">
-        <v>121</v>
+        <v>122</v>
       </c>
     </row>
     <row r="3" spans="1:10">
@@ -4978,7 +4978,7 @@
         <v>191</v>
       </c>
       <c r="J5">
-        <v>93</v>
+        <v>96</v>
       </c>
     </row>
     <row r="6" spans="1:10">
@@ -5074,7 +5074,7 @@
         <v>653</v>
       </c>
       <c r="J8">
-        <v>508</v>
+        <v>514</v>
       </c>
     </row>
     <row r="9" spans="1:10">
@@ -5106,7 +5106,7 @@
         <v>428</v>
       </c>
       <c r="J9">
-        <v>273</v>
+        <v>276</v>
       </c>
     </row>
     <row r="10" spans="1:10">
@@ -5138,7 +5138,7 @@
         <v>1089</v>
       </c>
       <c r="J10">
-        <v>624</v>
+        <v>633</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -5170,7 +5170,7 @@
         <v>2956</v>
       </c>
       <c r="J11">
-        <v>1787</v>
+        <v>1809</v>
       </c>
     </row>
   </sheetData>
@@ -5256,10 +5256,10 @@
         <v>767</v>
       </c>
       <c r="I2">
-        <v>918</v>
+        <v>917</v>
       </c>
       <c r="J2">
-        <v>536</v>
+        <v>538</v>
       </c>
     </row>
     <row r="3" spans="1:10">
@@ -5323,7 +5323,7 @@
         <v>436</v>
       </c>
       <c r="J4">
-        <v>242</v>
+        <v>245</v>
       </c>
     </row>
     <row r="5" spans="1:10">
@@ -5355,7 +5355,7 @@
         <v>247</v>
       </c>
       <c r="J5">
-        <v>154</v>
+        <v>156</v>
       </c>
     </row>
     <row r="6" spans="1:10">
@@ -5387,7 +5387,7 @@
         <v>793</v>
       </c>
       <c r="J6">
-        <v>536</v>
+        <v>539</v>
       </c>
     </row>
     <row r="7" spans="1:10">
@@ -5419,7 +5419,7 @@
         <v>2685</v>
       </c>
       <c r="J7">
-        <v>1576</v>
+        <v>1585</v>
       </c>
     </row>
     <row r="8" spans="1:10">
@@ -5448,10 +5448,10 @@
         <v>3970</v>
       </c>
       <c r="I8">
-        <v>4744</v>
+        <v>4743</v>
       </c>
       <c r="J8">
-        <v>2646</v>
+        <v>2667</v>
       </c>
     </row>
     <row r="9" spans="1:10">
@@ -5483,7 +5483,7 @@
         <v>519</v>
       </c>
       <c r="J9">
-        <v>287</v>
+        <v>289</v>
       </c>
     </row>
     <row r="10" spans="1:10">
@@ -5512,10 +5512,10 @@
         <v>692</v>
       </c>
       <c r="I10">
-        <v>949</v>
+        <v>948</v>
       </c>
       <c r="J10">
-        <v>503</v>
+        <v>508</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -5547,7 +5547,7 @@
         <v>1713</v>
       </c>
       <c r="J11">
-        <v>1049</v>
+        <v>1058</v>
       </c>
     </row>
     <row r="12" spans="1:10">
@@ -5579,7 +5579,7 @@
         <v>412</v>
       </c>
       <c r="J12">
-        <v>220</v>
+        <v>221</v>
       </c>
     </row>
     <row r="13" spans="1:10">
@@ -5611,7 +5611,7 @@
         <v>258</v>
       </c>
       <c r="J13">
-        <v>146</v>
+        <v>147</v>
       </c>
     </row>
     <row r="14" spans="1:10">
@@ -5640,10 +5640,10 @@
         <v>474</v>
       </c>
       <c r="I14">
-        <v>719</v>
+        <v>718</v>
       </c>
       <c r="J14">
-        <v>338</v>
+        <v>339</v>
       </c>
     </row>
     <row r="15" spans="1:10">
@@ -5675,7 +5675,7 @@
         <v>886</v>
       </c>
       <c r="J15">
-        <v>553</v>
+        <v>557</v>
       </c>
     </row>
     <row r="16" spans="1:10">
@@ -5707,7 +5707,7 @@
         <v>595</v>
       </c>
       <c r="J16">
-        <v>405</v>
+        <v>408</v>
       </c>
     </row>
     <row r="17" spans="1:10">
@@ -5739,7 +5739,7 @@
         <v>175</v>
       </c>
       <c r="J17">
-        <v>81</v>
+        <v>82</v>
       </c>
     </row>
     <row r="18" spans="1:10">
@@ -5771,7 +5771,7 @@
         <v>695</v>
       </c>
       <c r="J18">
-        <v>413</v>
+        <v>417</v>
       </c>
     </row>
     <row r="19" spans="1:10">
@@ -5803,7 +5803,7 @@
         <v>2636</v>
       </c>
       <c r="J19">
-        <v>1449</v>
+        <v>1461</v>
       </c>
     </row>
     <row r="20" spans="1:10">
@@ -5835,7 +5835,7 @@
         <v>2045</v>
       </c>
       <c r="J20">
-        <v>1026</v>
+        <v>1037</v>
       </c>
     </row>
     <row r="21" spans="1:10">
@@ -5867,7 +5867,7 @@
         <v>337</v>
       </c>
       <c r="J21">
-        <v>141</v>
+        <v>144</v>
       </c>
     </row>
     <row r="22" spans="1:10">
@@ -5899,7 +5899,7 @@
         <v>418</v>
       </c>
       <c r="J22">
-        <v>283</v>
+        <v>284</v>
       </c>
     </row>
     <row r="23" spans="1:10">
@@ -5931,7 +5931,7 @@
         <v>1368</v>
       </c>
       <c r="J23">
-        <v>805</v>
+        <v>807</v>
       </c>
     </row>
     <row r="24" spans="1:10">
@@ -5963,7 +5963,7 @@
         <v>500</v>
       </c>
       <c r="J24">
-        <v>326</v>
+        <v>328</v>
       </c>
     </row>
     <row r="25" spans="1:10">
@@ -6027,7 +6027,7 @@
         <v>248</v>
       </c>
       <c r="J26">
-        <v>155</v>
+        <v>156</v>
       </c>
     </row>
     <row r="27" spans="1:10">
@@ -6059,7 +6059,7 @@
         <v>1258</v>
       </c>
       <c r="J27">
-        <v>731</v>
+        <v>739</v>
       </c>
     </row>
     <row r="28" spans="1:10">
@@ -6123,7 +6123,7 @@
         <v>3950</v>
       </c>
       <c r="J29">
-        <v>2245</v>
+        <v>2256</v>
       </c>
     </row>
     <row r="30" spans="1:10">
@@ -6155,7 +6155,7 @@
         <v>260</v>
       </c>
       <c r="J30">
-        <v>158</v>
+        <v>159</v>
       </c>
     </row>
     <row r="31" spans="1:10">
@@ -6187,7 +6187,7 @@
         <v>867</v>
       </c>
       <c r="J31">
-        <v>460</v>
+        <v>463</v>
       </c>
     </row>
     <row r="32" spans="1:10">
@@ -6251,7 +6251,7 @@
         <v>3011</v>
       </c>
       <c r="J33">
-        <v>1773</v>
+        <v>1779</v>
       </c>
     </row>
     <row r="34" spans="1:10">
@@ -6283,7 +6283,7 @@
         <v>761</v>
       </c>
       <c r="J34">
-        <v>478</v>
+        <v>481</v>
       </c>
     </row>
     <row r="35" spans="1:10">
@@ -6347,7 +6347,7 @@
         <v>1491</v>
       </c>
       <c r="J36">
-        <v>893</v>
+        <v>898</v>
       </c>
     </row>
     <row r="37" spans="1:10">
@@ -6379,7 +6379,7 @@
         <v>2547</v>
       </c>
       <c r="J37">
-        <v>1514</v>
+        <v>1525</v>
       </c>
     </row>
     <row r="38" spans="1:10">
@@ -6475,7 +6475,7 @@
         <v>236</v>
       </c>
       <c r="J40">
-        <v>145</v>
+        <v>147</v>
       </c>
     </row>
     <row r="41" spans="1:10">
@@ -6507,7 +6507,7 @@
         <v>437</v>
       </c>
       <c r="J41">
-        <v>306</v>
+        <v>307</v>
       </c>
     </row>
     <row r="42" spans="1:10">
@@ -6539,7 +6539,7 @@
         <v>2956</v>
       </c>
       <c r="J42">
-        <v>1787</v>
+        <v>1809</v>
       </c>
     </row>
     <row r="43" spans="1:10">
@@ -6571,7 +6571,7 @@
         <v>1153</v>
       </c>
       <c r="J43">
-        <v>734</v>
+        <v>741</v>
       </c>
     </row>
     <row r="44" spans="1:10">
@@ -6603,7 +6603,7 @@
         <v>1228</v>
       </c>
       <c r="J44">
-        <v>698</v>
+        <v>700</v>
       </c>
     </row>
     <row r="45" spans="1:10">
@@ -6635,7 +6635,7 @@
         <v>181</v>
       </c>
       <c r="J45">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="46" spans="1:10">
@@ -6699,7 +6699,7 @@
         <v>903</v>
       </c>
       <c r="J47">
-        <v>512</v>
+        <v>517</v>
       </c>
     </row>
     <row r="48" spans="1:10">
@@ -6731,7 +6731,7 @@
         <v>2623</v>
       </c>
       <c r="J48">
-        <v>1429</v>
+        <v>1446</v>
       </c>
     </row>
     <row r="49" spans="1:10">
@@ -6763,7 +6763,7 @@
         <v>1648</v>
       </c>
       <c r="J49">
-        <v>880</v>
+        <v>889</v>
       </c>
     </row>
     <row r="50" spans="1:10">
@@ -6795,7 +6795,7 @@
         <v>960</v>
       </c>
       <c r="J50">
-        <v>537</v>
+        <v>539</v>
       </c>
     </row>
     <row r="51" spans="1:10">
@@ -6827,7 +6827,7 @@
         <v>1337</v>
       </c>
       <c r="J51">
-        <v>830</v>
+        <v>836</v>
       </c>
     </row>
     <row r="52" spans="1:10">
@@ -6859,7 +6859,7 @@
         <v>1491</v>
       </c>
       <c r="J52">
-        <v>996</v>
+        <v>1011</v>
       </c>
     </row>
     <row r="53" spans="1:10">
@@ -6888,10 +6888,10 @@
         <v>1183</v>
       </c>
       <c r="I53">
-        <v>1601</v>
+        <v>1600</v>
       </c>
       <c r="J53">
-        <v>1033</v>
+        <v>1042</v>
       </c>
     </row>
     <row r="54" spans="1:10">
@@ -6923,7 +6923,7 @@
         <v>3507</v>
       </c>
       <c r="J54">
-        <v>1876</v>
+        <v>1897</v>
       </c>
     </row>
     <row r="55" spans="1:10">
@@ -6955,7 +6955,7 @@
         <v>1244</v>
       </c>
       <c r="J55">
-        <v>643</v>
+        <v>646</v>
       </c>
     </row>
     <row r="56" spans="1:10">
@@ -6987,7 +6987,7 @@
         <v>628</v>
       </c>
       <c r="J56">
-        <v>314</v>
+        <v>317</v>
       </c>
     </row>
     <row r="57" spans="1:10">
@@ -7083,7 +7083,7 @@
         <v>271</v>
       </c>
       <c r="J59">
-        <v>172</v>
+        <v>175</v>
       </c>
     </row>
     <row r="60" spans="1:10">
@@ -7147,7 +7147,7 @@
         <v>160</v>
       </c>
       <c r="J61">
-        <v>87</v>
+        <v>88</v>
       </c>
     </row>
     <row r="62" spans="1:10">
@@ -7208,10 +7208,10 @@
         <v>2166</v>
       </c>
       <c r="I63">
-        <v>2476</v>
+        <v>2477</v>
       </c>
       <c r="J63">
-        <v>745</v>
+        <v>703</v>
       </c>
     </row>
     <row r="64" spans="1:10">
@@ -7243,7 +7243,7 @@
         <v>1187</v>
       </c>
       <c r="J64">
-        <v>586</v>
+        <v>596</v>
       </c>
     </row>
     <row r="65" spans="1:10">
@@ -7275,7 +7275,7 @@
         <v>1515</v>
       </c>
       <c r="J65">
-        <v>964</v>
+        <v>969</v>
       </c>
     </row>
     <row r="66" spans="1:10">
@@ -7307,7 +7307,7 @@
         <v>715</v>
       </c>
       <c r="J66">
-        <v>417</v>
+        <v>419</v>
       </c>
     </row>
     <row r="67" spans="1:10">
@@ -7339,7 +7339,7 @@
         <v>2510</v>
       </c>
       <c r="J67">
-        <v>1456</v>
+        <v>1461</v>
       </c>
     </row>
     <row r="68" spans="1:10">
@@ -7371,7 +7371,7 @@
         <v>437</v>
       </c>
       <c r="J68">
-        <v>188</v>
+        <v>191</v>
       </c>
     </row>
     <row r="69" spans="1:10">
@@ -7435,7 +7435,7 @@
         <v>677</v>
       </c>
       <c r="J70">
-        <v>388</v>
+        <v>390</v>
       </c>
     </row>
     <row r="71" spans="1:10">
@@ -7467,7 +7467,7 @@
         <v>335</v>
       </c>
       <c r="J71">
-        <v>245</v>
+        <v>246</v>
       </c>
     </row>
     <row r="72" spans="1:10">
@@ -7499,7 +7499,7 @@
         <v>706</v>
       </c>
       <c r="J72">
-        <v>363</v>
+        <v>366</v>
       </c>
     </row>
     <row r="73" spans="1:10">
@@ -7531,7 +7531,7 @@
         <v>1279</v>
       </c>
       <c r="J73">
-        <v>830</v>
+        <v>836</v>
       </c>
     </row>
     <row r="74" spans="1:10">
@@ -7627,7 +7627,7 @@
         <v>2923</v>
       </c>
       <c r="J76">
-        <v>1602</v>
+        <v>1612</v>
       </c>
     </row>
     <row r="77" spans="1:10">
@@ -7659,7 +7659,7 @@
         <v>462</v>
       </c>
       <c r="J77">
-        <v>291</v>
+        <v>292</v>
       </c>
     </row>
     <row r="78" spans="1:10">
@@ -7691,7 +7691,7 @@
         <v>1797</v>
       </c>
       <c r="J78">
-        <v>971</v>
+        <v>973</v>
       </c>
     </row>
     <row r="79" spans="1:10">
@@ -7723,7 +7723,7 @@
         <v>2472</v>
       </c>
       <c r="J79">
-        <v>1386</v>
+        <v>1391</v>
       </c>
     </row>
     <row r="80" spans="1:10">
@@ -7755,7 +7755,7 @@
         <v>393</v>
       </c>
       <c r="J80">
-        <v>166</v>
+        <v>167</v>
       </c>
     </row>
     <row r="81" spans="1:10">
@@ -7787,7 +7787,7 @@
         <v>219</v>
       </c>
       <c r="J81">
-        <v>120</v>
+        <v>121</v>
       </c>
     </row>
     <row r="82" spans="1:10">
@@ -7819,7 +7819,7 @@
         <v>233</v>
       </c>
       <c r="J82">
-        <v>145</v>
+        <v>148</v>
       </c>
     </row>
     <row r="83" spans="1:10">
@@ -7851,7 +7851,7 @@
         <v>1793</v>
       </c>
       <c r="J83">
-        <v>965</v>
+        <v>968</v>
       </c>
     </row>
     <row r="84" spans="1:10">
@@ -7883,7 +7883,7 @@
         <v>729</v>
       </c>
       <c r="J84">
-        <v>463</v>
+        <v>467</v>
       </c>
     </row>
     <row r="85" spans="1:10">
@@ -7915,7 +7915,7 @@
         <v>3848</v>
       </c>
       <c r="J85">
-        <v>2277</v>
+        <v>2288</v>
       </c>
     </row>
     <row r="86" spans="1:10">
@@ -7947,7 +7947,7 @@
         <v>1066</v>
       </c>
       <c r="J86">
-        <v>453</v>
+        <v>463</v>
       </c>
     </row>
     <row r="87" spans="1:10">
@@ -7979,7 +7979,7 @@
         <v>396</v>
       </c>
       <c r="J87">
-        <v>214</v>
+        <v>215</v>
       </c>
     </row>
     <row r="88" spans="1:10">
@@ -8011,7 +8011,7 @@
         <v>943</v>
       </c>
       <c r="J88">
-        <v>559</v>
+        <v>561</v>
       </c>
     </row>
     <row r="89" spans="1:10">
@@ -8043,7 +8043,7 @@
         <v>1879</v>
       </c>
       <c r="J89">
-        <v>1072</v>
+        <v>1080</v>
       </c>
     </row>
     <row r="90" spans="1:10">
@@ -8075,7 +8075,7 @@
         <v>1354</v>
       </c>
       <c r="J90">
-        <v>819</v>
+        <v>825</v>
       </c>
     </row>
     <row r="91" spans="1:10">
@@ -8107,7 +8107,7 @@
         <v>970</v>
       </c>
       <c r="J91">
-        <v>586</v>
+        <v>590</v>
       </c>
     </row>
     <row r="92" spans="1:10">
@@ -8139,7 +8139,7 @@
         <v>337</v>
       </c>
       <c r="J92">
-        <v>213</v>
+        <v>215</v>
       </c>
     </row>
     <row r="93" spans="1:10">
@@ -8171,7 +8171,7 @@
         <v>721</v>
       </c>
       <c r="J93">
-        <v>420</v>
+        <v>426</v>
       </c>
     </row>
     <row r="94" spans="1:10">
@@ -8203,7 +8203,7 @@
         <v>2664</v>
       </c>
       <c r="J94">
-        <v>1325</v>
+        <v>1328</v>
       </c>
     </row>
     <row r="95" spans="1:10">
@@ -8235,7 +8235,7 @@
         <v>1389</v>
       </c>
       <c r="J95">
-        <v>825</v>
+        <v>828</v>
       </c>
     </row>
     <row r="96" spans="1:10">
@@ -8267,7 +8267,7 @@
         <v>1669</v>
       </c>
       <c r="J96">
-        <v>884</v>
+        <v>892</v>
       </c>
     </row>
     <row r="97" spans="1:10">
@@ -8299,7 +8299,7 @@
         <v>1673</v>
       </c>
       <c r="J97">
-        <v>927</v>
+        <v>933</v>
       </c>
     </row>
     <row r="98" spans="1:10">
@@ -8331,7 +8331,7 @@
         <v>1318</v>
       </c>
       <c r="J98">
-        <v>648</v>
+        <v>652</v>
       </c>
     </row>
     <row r="99" spans="1:10">
@@ -8363,7 +8363,7 @@
         <v>1488</v>
       </c>
       <c r="J99">
-        <v>869</v>
+        <v>882</v>
       </c>
     </row>
     <row r="100" spans="1:10">
@@ -8424,10 +8424,10 @@
         <v>84592</v>
       </c>
       <c r="I101">
-        <v>110485</v>
+        <v>110481</v>
       </c>
       <c r="J101">
-        <v>62217</v>
+        <v>62607</v>
       </c>
     </row>
   </sheetData>
@@ -8650,7 +8650,7 @@
         <v>18</v>
       </c>
       <c r="J3">
-        <v>18</v>
+        <v>19</v>
       </c>
     </row>
     <row r="4" spans="1:10">
@@ -8795,7 +8795,7 @@
         <v>219</v>
       </c>
       <c r="J8">
-        <v>115</v>
+        <v>116</v>
       </c>
     </row>
     <row r="9" spans="1:10">
@@ -8859,7 +8859,7 @@
         <v>1135</v>
       </c>
       <c r="J10">
-        <v>594</v>
+        <v>601</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -8891,7 +8891,7 @@
         <v>1648</v>
       </c>
       <c r="J11">
-        <v>880</v>
+        <v>889</v>
       </c>
     </row>
   </sheetData>
@@ -9012,7 +9012,7 @@
         <v>439</v>
       </c>
       <c r="J3">
-        <v>234</v>
+        <v>235</v>
       </c>
     </row>
     <row r="4" spans="1:10">
@@ -9076,7 +9076,7 @@
         <v>381</v>
       </c>
       <c r="J5">
-        <v>164</v>
+        <v>168</v>
       </c>
     </row>
     <row r="6" spans="1:10">
@@ -9172,7 +9172,7 @@
         <v>1026</v>
       </c>
       <c r="J8">
-        <v>765</v>
+        <v>768</v>
       </c>
     </row>
     <row r="9" spans="1:10">
@@ -9236,7 +9236,7 @@
         <v>1271</v>
       </c>
       <c r="J10">
-        <v>699</v>
+        <v>702</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -9268,7 +9268,7 @@
         <v>3848</v>
       </c>
       <c r="J11">
-        <v>2277</v>
+        <v>2288</v>
       </c>
     </row>
   </sheetData>
@@ -9357,7 +9357,7 @@
         <v>75</v>
       </c>
       <c r="J2">
-        <v>35</v>
+        <v>36</v>
       </c>
     </row>
     <row r="3" spans="1:10">
@@ -9546,7 +9546,7 @@
         <v>336</v>
       </c>
       <c r="J8">
-        <v>170</v>
+        <v>171</v>
       </c>
     </row>
     <row r="9" spans="1:10">
@@ -9610,7 +9610,7 @@
         <v>2132</v>
       </c>
       <c r="J10">
-        <v>1156</v>
+        <v>1164</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -9642,7 +9642,7 @@
         <v>2923</v>
       </c>
       <c r="J11">
-        <v>1602</v>
+        <v>1612</v>
       </c>
     </row>
   </sheetData>
@@ -9821,7 +9821,7 @@
         <v>122</v>
       </c>
       <c r="J5">
-        <v>72</v>
+        <v>73</v>
       </c>
     </row>
     <row r="6" spans="1:10">
@@ -9914,7 +9914,7 @@
         <v>280</v>
       </c>
       <c r="J8">
-        <v>296</v>
+        <v>298</v>
       </c>
     </row>
     <row r="9" spans="1:10">
@@ -9978,7 +9978,7 @@
         <v>1034</v>
       </c>
       <c r="J10">
-        <v>460</v>
+        <v>463</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -10010,7 +10010,7 @@
         <v>1673</v>
       </c>
       <c r="J11">
-        <v>927</v>
+        <v>933</v>
       </c>
     </row>
   </sheetData>
@@ -10227,7 +10227,7 @@
         <v>56</v>
       </c>
       <c r="J6">
-        <v>37</v>
+        <v>38</v>
       </c>
     </row>
     <row r="7" spans="1:10">
@@ -10291,7 +10291,7 @@
         <v>516</v>
       </c>
       <c r="J8">
-        <v>379</v>
+        <v>382</v>
       </c>
     </row>
     <row r="9" spans="1:10">
@@ -10355,7 +10355,7 @@
         <v>895</v>
       </c>
       <c r="J10">
-        <v>457</v>
+        <v>458</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -10387,7 +10387,7 @@
         <v>2510</v>
       </c>
       <c r="J11">
-        <v>1456</v>
+        <v>1461</v>
       </c>
     </row>
   </sheetData>
@@ -10572,7 +10572,7 @@
         <v>154</v>
       </c>
       <c r="J5">
-        <v>40</v>
+        <v>41</v>
       </c>
     </row>
     <row r="6" spans="1:10">
@@ -10732,7 +10732,7 @@
         <v>433</v>
       </c>
       <c r="J10">
-        <v>270</v>
+        <v>272</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -10764,7 +10764,7 @@
         <v>1389</v>
       </c>
       <c r="J11">
-        <v>825</v>
+        <v>828</v>
       </c>
     </row>
   </sheetData>
@@ -11045,7 +11045,7 @@
         <v>190</v>
       </c>
       <c r="J8">
-        <v>166</v>
+        <v>169</v>
       </c>
     </row>
     <row r="9" spans="1:10">
@@ -11109,7 +11109,7 @@
         <v>271</v>
       </c>
       <c r="J10">
-        <v>140</v>
+        <v>141</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -11141,7 +11141,7 @@
         <v>729</v>
       </c>
       <c r="J11">
-        <v>463</v>
+        <v>467</v>
       </c>
     </row>
   </sheetData>
@@ -11230,7 +11230,7 @@
         <v>146</v>
       </c>
       <c r="J2">
-        <v>87</v>
+        <v>90</v>
       </c>
     </row>
     <row r="3" spans="1:10">
@@ -11262,7 +11262,7 @@
         <v>190</v>
       </c>
       <c r="J3">
-        <v>107</v>
+        <v>110</v>
       </c>
     </row>
     <row r="4" spans="1:10">
@@ -11294,7 +11294,7 @@
         <v>11</v>
       </c>
       <c r="J4">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="5" spans="1:10">
@@ -11326,7 +11326,7 @@
         <v>81</v>
       </c>
       <c r="J5">
-        <v>44</v>
+        <v>45</v>
       </c>
     </row>
     <row r="6" spans="1:10">
@@ -11422,7 +11422,7 @@
         <v>218</v>
       </c>
       <c r="J8">
-        <v>192</v>
+        <v>193</v>
       </c>
     </row>
     <row r="9" spans="1:10">
@@ -11454,7 +11454,7 @@
         <v>196</v>
       </c>
       <c r="J9">
-        <v>170</v>
+        <v>173</v>
       </c>
     </row>
     <row r="10" spans="1:10">
@@ -11486,7 +11486,7 @@
         <v>590</v>
       </c>
       <c r="J10">
-        <v>365</v>
+        <v>368</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -11518,7 +11518,7 @@
         <v>1491</v>
       </c>
       <c r="J11">
-        <v>996</v>
+        <v>1011</v>
       </c>
     </row>
   </sheetData>
@@ -11735,7 +11735,7 @@
         <v>4</v>
       </c>
       <c r="J6">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="7" spans="1:10">
@@ -11863,7 +11863,7 @@
         <v>474</v>
       </c>
       <c r="J10">
-        <v>223</v>
+        <v>224</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -11895,7 +11895,7 @@
         <v>943</v>
       </c>
       <c r="J11">
-        <v>559</v>
+        <v>561</v>
       </c>
     </row>
   </sheetData>
@@ -12173,7 +12173,7 @@
         <v>401</v>
       </c>
       <c r="J8">
-        <v>221</v>
+        <v>224</v>
       </c>
     </row>
     <row r="9" spans="1:10">
@@ -12205,7 +12205,7 @@
         <v>243</v>
       </c>
       <c r="J9">
-        <v>134</v>
+        <v>135</v>
       </c>
     </row>
     <row r="10" spans="1:10">
@@ -12237,7 +12237,7 @@
         <v>2528</v>
       </c>
       <c r="J10">
-        <v>1341</v>
+        <v>1358</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -12269,7 +12269,7 @@
         <v>3507</v>
       </c>
       <c r="J11">
-        <v>1876</v>
+        <v>1897</v>
       </c>
     </row>
   </sheetData>
@@ -12486,7 +12486,7 @@
         <v>11</v>
       </c>
       <c r="J6">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="7" spans="1:10">
@@ -12614,7 +12614,7 @@
         <v>527</v>
       </c>
       <c r="J10">
-        <v>306</v>
+        <v>310</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -12646,7 +12646,7 @@
         <v>1491</v>
       </c>
       <c r="J11">
-        <v>893</v>
+        <v>898</v>
       </c>
     </row>
   </sheetData>
@@ -12767,7 +12767,7 @@
         <v>261</v>
       </c>
       <c r="J3">
-        <v>160</v>
+        <v>159</v>
       </c>
     </row>
     <row r="4" spans="1:10">
@@ -12927,7 +12927,7 @@
         <v>722</v>
       </c>
       <c r="J8">
-        <v>483</v>
+        <v>487</v>
       </c>
     </row>
     <row r="9" spans="1:10">
@@ -12959,7 +12959,7 @@
         <v>244</v>
       </c>
       <c r="J9">
-        <v>134</v>
+        <v>136</v>
       </c>
     </row>
     <row r="10" spans="1:10">
@@ -12991,7 +12991,7 @@
         <v>813</v>
       </c>
       <c r="J10">
-        <v>443</v>
+        <v>449</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -13023,7 +13023,7 @@
         <v>2547</v>
       </c>
       <c r="J11">
-        <v>1514</v>
+        <v>1525</v>
       </c>
     </row>
   </sheetData>
@@ -13283,7 +13283,7 @@
         <v>90</v>
       </c>
       <c r="J8">
-        <v>91</v>
+        <v>92</v>
       </c>
     </row>
     <row r="9" spans="1:10">
@@ -13379,7 +13379,7 @@
         <v>418</v>
       </c>
       <c r="J11">
-        <v>283</v>
+        <v>284</v>
       </c>
     </row>
   </sheetData>
@@ -13645,7 +13645,7 @@
         <v>89</v>
       </c>
       <c r="J8">
-        <v>71</v>
+        <v>73</v>
       </c>
     </row>
     <row r="9" spans="1:10">
@@ -13709,7 +13709,7 @@
         <v>448</v>
       </c>
       <c r="J10">
-        <v>212</v>
+        <v>213</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -13741,7 +13741,7 @@
         <v>706</v>
       </c>
       <c r="J11">
-        <v>363</v>
+        <v>366</v>
       </c>
     </row>
   </sheetData>
@@ -13926,7 +13926,7 @@
         <v>107</v>
       </c>
       <c r="J5">
-        <v>48</v>
+        <v>49</v>
       </c>
     </row>
     <row r="6" spans="1:10">
@@ -13958,7 +13958,7 @@
         <v>26</v>
       </c>
       <c r="J6">
-        <v>16</v>
+        <v>17</v>
       </c>
     </row>
     <row r="7" spans="1:10">
@@ -14022,7 +14022,7 @@
         <v>202</v>
       </c>
       <c r="J8">
-        <v>211</v>
+        <v>212</v>
       </c>
     </row>
     <row r="9" spans="1:10">
@@ -14086,7 +14086,7 @@
         <v>587</v>
       </c>
       <c r="J10">
-        <v>328</v>
+        <v>330</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -14118,7 +14118,7 @@
         <v>1515</v>
       </c>
       <c r="J11">
-        <v>964</v>
+        <v>969</v>
       </c>
     </row>
   </sheetData>
@@ -15096,7 +15096,7 @@
         <v>57</v>
       </c>
       <c r="J8">
-        <v>31</v>
+        <v>32</v>
       </c>
     </row>
     <row r="9" spans="1:10">
@@ -15160,7 +15160,7 @@
         <v>255</v>
       </c>
       <c r="J10">
-        <v>105</v>
+        <v>107</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -15192,7 +15192,7 @@
         <v>437</v>
       </c>
       <c r="J11">
-        <v>188</v>
+        <v>191</v>
       </c>
     </row>
   </sheetData>
@@ -15345,7 +15345,7 @@
         <v>7</v>
       </c>
       <c r="J4">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="5" spans="1:10">
@@ -15505,7 +15505,7 @@
         <v>123</v>
       </c>
       <c r="J9">
-        <v>88</v>
+        <v>89</v>
       </c>
     </row>
     <row r="10" spans="1:10">
@@ -15537,7 +15537,7 @@
         <v>612</v>
       </c>
       <c r="J10">
-        <v>316</v>
+        <v>317</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -15569,7 +15569,7 @@
         <v>1793</v>
       </c>
       <c r="J11">
-        <v>965</v>
+        <v>968</v>
       </c>
     </row>
   </sheetData>
@@ -15754,7 +15754,7 @@
         <v>90</v>
       </c>
       <c r="J5">
-        <v>43</v>
+        <v>44</v>
       </c>
     </row>
     <row r="6" spans="1:10">
@@ -15850,7 +15850,7 @@
         <v>224</v>
       </c>
       <c r="J8">
-        <v>165</v>
+        <v>166</v>
       </c>
     </row>
     <row r="9" spans="1:10">
@@ -15914,7 +15914,7 @@
         <v>610</v>
       </c>
       <c r="J10">
-        <v>265</v>
+        <v>266</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -15946,7 +15946,7 @@
         <v>1244</v>
       </c>
       <c r="J11">
-        <v>643</v>
+        <v>646</v>
       </c>
     </row>
   </sheetData>
@@ -16067,7 +16067,7 @@
         <v>42</v>
       </c>
       <c r="J3">
-        <v>21</v>
+        <v>22</v>
       </c>
     </row>
     <row r="4" spans="1:10">
@@ -16276,7 +16276,7 @@
         <v>2021</v>
       </c>
       <c r="J10">
-        <v>946</v>
+        <v>948</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -16308,7 +16308,7 @@
         <v>2664</v>
       </c>
       <c r="J11">
-        <v>1325</v>
+        <v>1328</v>
       </c>
     </row>
   </sheetData>
@@ -16397,7 +16397,7 @@
         <v>267</v>
       </c>
       <c r="J2">
-        <v>168</v>
+        <v>169</v>
       </c>
     </row>
     <row r="3" spans="1:10">
@@ -16429,7 +16429,7 @@
         <v>416</v>
       </c>
       <c r="J3">
-        <v>212</v>
+        <v>214</v>
       </c>
     </row>
     <row r="4" spans="1:10">
@@ -16461,7 +16461,7 @@
         <v>24</v>
       </c>
       <c r="J4">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="5" spans="1:10">
@@ -16493,7 +16493,7 @@
         <v>170</v>
       </c>
       <c r="J5">
-        <v>61</v>
+        <v>62</v>
       </c>
     </row>
     <row r="6" spans="1:10">
@@ -16589,7 +16589,7 @@
         <v>707</v>
       </c>
       <c r="J8">
-        <v>534</v>
+        <v>535</v>
       </c>
     </row>
     <row r="9" spans="1:10">
@@ -16685,7 +16685,7 @@
         <v>3011</v>
       </c>
       <c r="J11">
-        <v>1773</v>
+        <v>1779</v>
       </c>
     </row>
   </sheetData>
@@ -16806,7 +16806,7 @@
         <v>248</v>
       </c>
       <c r="J3">
-        <v>121</v>
+        <v>122</v>
       </c>
     </row>
     <row r="4" spans="1:10">
@@ -16902,7 +16902,7 @@
         <v>44</v>
       </c>
       <c r="J6">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="7" spans="1:10">
@@ -16966,7 +16966,7 @@
         <v>567</v>
       </c>
       <c r="J8">
-        <v>537</v>
+        <v>539</v>
       </c>
     </row>
     <row r="9" spans="1:10">
@@ -17030,7 +17030,7 @@
         <v>1023</v>
       </c>
       <c r="J10">
-        <v>488</v>
+        <v>493</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -17062,7 +17062,7 @@
         <v>2685</v>
       </c>
       <c r="J11">
-        <v>1576</v>
+        <v>1585</v>
       </c>
     </row>
   </sheetData>
@@ -17151,7 +17151,7 @@
         <v>457</v>
       </c>
       <c r="J2">
-        <v>264</v>
+        <v>266</v>
       </c>
     </row>
     <row r="3" spans="1:10">
@@ -17183,7 +17183,7 @@
         <v>445</v>
       </c>
       <c r="J3">
-        <v>288</v>
+        <v>291</v>
       </c>
     </row>
     <row r="4" spans="1:10">
@@ -17247,7 +17247,7 @@
         <v>251</v>
       </c>
       <c r="J5">
-        <v>113</v>
+        <v>114</v>
       </c>
     </row>
     <row r="6" spans="1:10">
@@ -17279,7 +17279,7 @@
         <v>93</v>
       </c>
       <c r="J6">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="7" spans="1:10">
@@ -17340,10 +17340,10 @@
         <v>560</v>
       </c>
       <c r="I8">
-        <v>1270</v>
+        <v>1269</v>
       </c>
       <c r="J8">
-        <v>714</v>
+        <v>720</v>
       </c>
     </row>
     <row r="9" spans="1:10">
@@ -17407,7 +17407,7 @@
         <v>1652</v>
       </c>
       <c r="J10">
-        <v>872</v>
+        <v>882</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -17436,10 +17436,10 @@
         <v>3970</v>
       </c>
       <c r="I11">
-        <v>4744</v>
+        <v>4743</v>
       </c>
       <c r="J11">
-        <v>2646</v>
+        <v>2667</v>
       </c>
     </row>
   </sheetData>
@@ -17528,7 +17528,7 @@
         <v>106</v>
       </c>
       <c r="J2">
-        <v>55</v>
+        <v>56</v>
       </c>
     </row>
     <row r="3" spans="1:10">
@@ -17624,7 +17624,7 @@
         <v>113</v>
       </c>
       <c r="J5">
-        <v>46</v>
+        <v>47</v>
       </c>
     </row>
     <row r="6" spans="1:10">
@@ -17784,7 +17784,7 @@
         <v>455</v>
       </c>
       <c r="J10">
-        <v>282</v>
+        <v>286</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -17816,7 +17816,7 @@
         <v>1354</v>
       </c>
       <c r="J11">
-        <v>819</v>
+        <v>825</v>
       </c>
     </row>
   </sheetData>
@@ -18085,7 +18085,7 @@
         <v>250</v>
       </c>
       <c r="J8">
-        <v>169</v>
+        <v>171</v>
       </c>
     </row>
     <row r="9" spans="1:10">
@@ -18117,7 +18117,7 @@
         <v>61</v>
       </c>
       <c r="J9">
-        <v>39</v>
+        <v>40</v>
       </c>
     </row>
     <row r="10" spans="1:10">
@@ -18149,7 +18149,7 @@
         <v>417</v>
       </c>
       <c r="J10">
-        <v>218</v>
+        <v>220</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -18181,7 +18181,7 @@
         <v>903</v>
       </c>
       <c r="J11">
-        <v>512</v>
+        <v>517</v>
       </c>
     </row>
   </sheetData>
@@ -18302,7 +18302,7 @@
         <v>212</v>
       </c>
       <c r="J3">
-        <v>115</v>
+        <v>116</v>
       </c>
     </row>
     <row r="4" spans="1:10">
@@ -18366,7 +18366,7 @@
         <v>229</v>
       </c>
       <c r="J5">
-        <v>97</v>
+        <v>98</v>
       </c>
     </row>
     <row r="6" spans="1:10">
@@ -18462,7 +18462,7 @@
         <v>754</v>
       </c>
       <c r="J8">
-        <v>410</v>
+        <v>413</v>
       </c>
     </row>
     <row r="9" spans="1:10">
@@ -18494,7 +18494,7 @@
         <v>233</v>
       </c>
       <c r="J9">
-        <v>153</v>
+        <v>155</v>
       </c>
     </row>
     <row r="10" spans="1:10">
@@ -18526,7 +18526,7 @@
         <v>911</v>
       </c>
       <c r="J10">
-        <v>517</v>
+        <v>522</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -18558,7 +18558,7 @@
         <v>2636</v>
       </c>
       <c r="J11">
-        <v>1449</v>
+        <v>1461</v>
       </c>
     </row>
   </sheetData>
@@ -18812,7 +18812,7 @@
         <v>49</v>
       </c>
       <c r="J8">
-        <v>49</v>
+        <v>50</v>
       </c>
     </row>
     <row r="9" spans="1:10">
@@ -18844,7 +18844,7 @@
         <v>31</v>
       </c>
       <c r="J9">
-        <v>22</v>
+        <v>23</v>
       </c>
     </row>
     <row r="10" spans="1:10">
@@ -18908,7 +18908,7 @@
         <v>247</v>
       </c>
       <c r="J11">
-        <v>154</v>
+        <v>156</v>
       </c>
     </row>
   </sheetData>
@@ -18997,7 +18997,7 @@
         <v>179</v>
       </c>
       <c r="J2">
-        <v>87</v>
+        <v>90</v>
       </c>
     </row>
     <row r="3" spans="1:10">
@@ -19029,7 +19029,7 @@
         <v>177</v>
       </c>
       <c r="J3">
-        <v>91</v>
+        <v>92</v>
       </c>
     </row>
     <row r="4" spans="1:10">
@@ -19093,7 +19093,7 @@
         <v>194</v>
       </c>
       <c r="J5">
-        <v>66</v>
+        <v>67</v>
       </c>
     </row>
     <row r="6" spans="1:10">
@@ -19125,7 +19125,7 @@
         <v>41</v>
       </c>
       <c r="J6">
-        <v>27</v>
+        <v>28</v>
       </c>
     </row>
     <row r="7" spans="1:10">
@@ -19253,7 +19253,7 @@
         <v>828</v>
       </c>
       <c r="J10">
-        <v>397</v>
+        <v>402</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -19285,7 +19285,7 @@
         <v>2045</v>
       </c>
       <c r="J11">
-        <v>1026</v>
+        <v>1037</v>
       </c>
     </row>
   </sheetData>
@@ -19618,7 +19618,7 @@
         <v>630</v>
       </c>
       <c r="J10">
-        <v>297</v>
+        <v>299</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -19650,7 +19650,7 @@
         <v>960</v>
       </c>
       <c r="J11">
-        <v>537</v>
+        <v>539</v>
       </c>
     </row>
   </sheetData>
@@ -19829,7 +19829,7 @@
         <v>31</v>
       </c>
       <c r="J5">
-        <v>7</v>
+        <v>9</v>
       </c>
     </row>
     <row r="6" spans="1:10">
@@ -19980,7 +19980,7 @@
         <v>124</v>
       </c>
       <c r="J10">
-        <v>85</v>
+        <v>86</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -20012,7 +20012,7 @@
         <v>271</v>
       </c>
       <c r="J11">
-        <v>172</v>
+        <v>175</v>
       </c>
     </row>
   </sheetData>
@@ -20101,7 +20101,7 @@
         <v>87</v>
       </c>
       <c r="J2">
-        <v>50</v>
+        <v>51</v>
       </c>
     </row>
     <row r="3" spans="1:10">
@@ -20133,7 +20133,7 @@
         <v>98</v>
       </c>
       <c r="J3">
-        <v>69</v>
+        <v>70</v>
       </c>
     </row>
     <row r="4" spans="1:10">
@@ -20357,7 +20357,7 @@
         <v>320</v>
       </c>
       <c r="J10">
-        <v>174</v>
+        <v>176</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -20389,7 +20389,7 @@
         <v>970</v>
       </c>
       <c r="J11">
-        <v>586</v>
+        <v>590</v>
       </c>
     </row>
   </sheetData>
@@ -20664,7 +20664,7 @@
         <v>122</v>
       </c>
       <c r="J8">
-        <v>121</v>
+        <v>123</v>
       </c>
     </row>
     <row r="9" spans="1:10">
@@ -20728,7 +20728,7 @@
         <v>381</v>
       </c>
       <c r="J10">
-        <v>186</v>
+        <v>190</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -20760,7 +20760,7 @@
         <v>721</v>
       </c>
       <c r="J11">
-        <v>420</v>
+        <v>426</v>
       </c>
     </row>
   </sheetData>
@@ -21330,7 +21330,7 @@
         <v>2</v>
       </c>
       <c r="J6">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="7" spans="1:10">
@@ -21452,7 +21452,7 @@
         <v>216</v>
       </c>
       <c r="J10">
-        <v>111</v>
+        <v>113</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -21484,7 +21484,7 @@
         <v>436</v>
       </c>
       <c r="J11">
-        <v>242</v>
+        <v>245</v>
       </c>
     </row>
   </sheetData>
@@ -21573,7 +21573,7 @@
         <v>64</v>
       </c>
       <c r="J2">
-        <v>45</v>
+        <v>46</v>
       </c>
     </row>
     <row r="3" spans="1:10">
@@ -21762,7 +21762,7 @@
         <v>297</v>
       </c>
       <c r="J8">
-        <v>265</v>
+        <v>267</v>
       </c>
     </row>
     <row r="9" spans="1:10">
@@ -21826,7 +21826,7 @@
         <v>670</v>
       </c>
       <c r="J10">
-        <v>338</v>
+        <v>341</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -21858,7 +21858,7 @@
         <v>1337</v>
       </c>
       <c r="J11">
-        <v>830</v>
+        <v>836</v>
       </c>
     </row>
   </sheetData>
@@ -22136,7 +22136,7 @@
         <v>75</v>
       </c>
       <c r="I8">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="J8">
         <v>76</v>
@@ -22203,7 +22203,7 @@
         <v>492</v>
       </c>
       <c r="J10">
-        <v>305</v>
+        <v>307</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -22232,10 +22232,10 @@
         <v>767</v>
       </c>
       <c r="I11">
-        <v>918</v>
+        <v>917</v>
       </c>
       <c r="J11">
-        <v>536</v>
+        <v>538</v>
       </c>
     </row>
   </sheetData>
@@ -22553,7 +22553,7 @@
         <v>205</v>
       </c>
       <c r="J10">
-        <v>94</v>
+        <v>95</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -22585,7 +22585,7 @@
         <v>412</v>
       </c>
       <c r="J11">
-        <v>220</v>
+        <v>221</v>
       </c>
     </row>
   </sheetData>
@@ -22674,7 +22674,7 @@
         <v>54</v>
       </c>
       <c r="J2">
-        <v>36</v>
+        <v>37</v>
       </c>
     </row>
     <row r="3" spans="1:10">
@@ -22706,7 +22706,7 @@
         <v>45</v>
       </c>
       <c r="J3">
-        <v>20</v>
+        <v>21</v>
       </c>
     </row>
     <row r="4" spans="1:10">
@@ -22863,7 +22863,7 @@
         <v>196</v>
       </c>
       <c r="J8">
-        <v>118</v>
+        <v>119</v>
       </c>
     </row>
     <row r="9" spans="1:10">
@@ -22927,7 +22927,7 @@
         <v>239</v>
       </c>
       <c r="J10">
-        <v>134</v>
+        <v>135</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -22959,7 +22959,7 @@
         <v>695</v>
       </c>
       <c r="J11">
-        <v>413</v>
+        <v>417</v>
       </c>
     </row>
   </sheetData>
@@ -23144,7 +23144,7 @@
         <v>59</v>
       </c>
       <c r="J5">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="6" spans="1:10">
@@ -23292,7 +23292,7 @@
         <v>277</v>
       </c>
       <c r="J10">
-        <v>163</v>
+        <v>164</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -23324,7 +23324,7 @@
         <v>500</v>
       </c>
       <c r="J11">
-        <v>326</v>
+        <v>328</v>
       </c>
     </row>
   </sheetData>
@@ -24040,7 +24040,7 @@
         <v>349</v>
       </c>
       <c r="J10">
-        <v>204</v>
+        <v>207</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -24072,7 +24072,7 @@
         <v>793</v>
       </c>
       <c r="J11">
-        <v>536</v>
+        <v>539</v>
       </c>
     </row>
   </sheetData>
@@ -24373,7 +24373,7 @@
         <v>41</v>
       </c>
       <c r="J9">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="10" spans="1:10">
@@ -24437,7 +24437,7 @@
         <v>396</v>
       </c>
       <c r="J11">
-        <v>214</v>
+        <v>215</v>
       </c>
     </row>
   </sheetData>
@@ -24526,7 +24526,7 @@
         <v>61</v>
       </c>
       <c r="J2">
-        <v>22</v>
+        <v>23</v>
       </c>
     </row>
     <row r="3" spans="1:10">
@@ -24770,7 +24770,7 @@
         <v>784</v>
       </c>
       <c r="J10">
-        <v>460</v>
+        <v>467</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -24802,7 +24802,7 @@
         <v>1258</v>
       </c>
       <c r="J11">
-        <v>731</v>
+        <v>739</v>
       </c>
     </row>
   </sheetData>
@@ -24923,7 +24923,7 @@
         <v>67</v>
       </c>
       <c r="J3">
-        <v>32</v>
+        <v>33</v>
       </c>
     </row>
     <row r="4" spans="1:10">
@@ -25147,7 +25147,7 @@
         <v>381</v>
       </c>
       <c r="J10">
-        <v>190</v>
+        <v>192</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -25179,7 +25179,7 @@
         <v>867</v>
       </c>
       <c r="J11">
-        <v>460</v>
+        <v>463</v>
       </c>
     </row>
   </sheetData>
@@ -25476,7 +25476,7 @@
         <v>576</v>
       </c>
       <c r="J10">
-        <v>293</v>
+        <v>296</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -25508,7 +25508,7 @@
         <v>628</v>
       </c>
       <c r="J11">
-        <v>314</v>
+        <v>317</v>
       </c>
     </row>
   </sheetData>
@@ -25789,7 +25789,7 @@
         <v>132</v>
       </c>
       <c r="J8">
-        <v>80</v>
+        <v>81</v>
       </c>
     </row>
     <row r="9" spans="1:10">
@@ -25885,7 +25885,7 @@
         <v>462</v>
       </c>
       <c r="J11">
-        <v>291</v>
+        <v>292</v>
       </c>
     </row>
   </sheetData>
@@ -26145,7 +26145,7 @@
         <v>15</v>
       </c>
       <c r="J8">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="9" spans="1:10">
@@ -26177,7 +26177,7 @@
         <v>139</v>
       </c>
       <c r="J9">
-        <v>75</v>
+        <v>77</v>
       </c>
     </row>
     <row r="10" spans="1:10">
@@ -26209,7 +26209,7 @@
         <v>233</v>
       </c>
       <c r="J10">
-        <v>145</v>
+        <v>148</v>
       </c>
     </row>
   </sheetData>
@@ -26298,7 +26298,7 @@
         <v>78</v>
       </c>
       <c r="J2">
-        <v>51</v>
+        <v>52</v>
       </c>
     </row>
     <row r="3" spans="1:10">
@@ -26330,7 +26330,7 @@
         <v>87</v>
       </c>
       <c r="J3">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="4" spans="1:10">
@@ -26554,7 +26554,7 @@
         <v>1118</v>
       </c>
       <c r="J10">
-        <v>568</v>
+        <v>570</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -26586,7 +26586,7 @@
         <v>1797</v>
       </c>
       <c r="J11">
-        <v>971</v>
+        <v>973</v>
       </c>
     </row>
   </sheetData>
@@ -26675,7 +26675,7 @@
         <v>47</v>
       </c>
       <c r="J2">
-        <v>26</v>
+        <v>27</v>
       </c>
     </row>
     <row r="3" spans="1:10">
@@ -26855,7 +26855,7 @@
         <v>49</v>
       </c>
       <c r="I8">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="J8">
         <v>86</v>
@@ -26951,10 +26951,10 @@
         <v>474</v>
       </c>
       <c r="I11">
-        <v>719</v>
+        <v>718</v>
       </c>
       <c r="J11">
-        <v>338</v>
+        <v>339</v>
       </c>
     </row>
   </sheetData>
@@ -27269,7 +27269,7 @@
         <v>462</v>
       </c>
       <c r="J10">
-        <v>238</v>
+        <v>240</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -27301,7 +27301,7 @@
         <v>715</v>
       </c>
       <c r="J11">
-        <v>417</v>
+        <v>419</v>
       </c>
     </row>
   </sheetData>
@@ -27613,7 +27613,7 @@
         <v>376</v>
       </c>
       <c r="J10">
-        <v>246</v>
+        <v>249</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -27645,7 +27645,7 @@
         <v>595</v>
       </c>
       <c r="J11">
-        <v>405</v>
+        <v>408</v>
       </c>
     </row>
   </sheetData>
@@ -27827,7 +27827,7 @@
         <v>48</v>
       </c>
       <c r="J5">
-        <v>24</v>
+        <v>25</v>
       </c>
     </row>
     <row r="6" spans="1:10">
@@ -27987,7 +27987,7 @@
         <v>193</v>
       </c>
       <c r="J10">
-        <v>88</v>
+        <v>89</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -28019,7 +28019,7 @@
         <v>519</v>
       </c>
       <c r="J11">
-        <v>287</v>
+        <v>289</v>
       </c>
     </row>
   </sheetData>
@@ -28273,7 +28273,7 @@
         <v>39</v>
       </c>
       <c r="J8">
-        <v>32</v>
+        <v>33</v>
       </c>
     </row>
     <row r="9" spans="1:10">
@@ -28369,7 +28369,7 @@
         <v>175</v>
       </c>
       <c r="J11">
-        <v>81</v>
+        <v>82</v>
       </c>
     </row>
   </sheetData>
@@ -28644,10 +28644,10 @@
         <v>82</v>
       </c>
       <c r="I8">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="J8">
-        <v>101</v>
+        <v>102</v>
       </c>
     </row>
     <row r="9" spans="1:10">
@@ -28679,7 +28679,7 @@
         <v>90</v>
       </c>
       <c r="J9">
-        <v>38</v>
+        <v>41</v>
       </c>
     </row>
     <row r="10" spans="1:10">
@@ -28711,7 +28711,7 @@
         <v>542</v>
       </c>
       <c r="J10">
-        <v>282</v>
+        <v>283</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -28740,10 +28740,10 @@
         <v>692</v>
       </c>
       <c r="I11">
-        <v>949</v>
+        <v>948</v>
       </c>
       <c r="J11">
-        <v>503</v>
+        <v>508</v>
       </c>
     </row>
   </sheetData>
@@ -29082,7 +29082,7 @@
         <v>172</v>
       </c>
       <c r="J10">
-        <v>93</v>
+        <v>94</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -29114,7 +29114,7 @@
         <v>437</v>
       </c>
       <c r="J11">
-        <v>306</v>
+        <v>307</v>
       </c>
     </row>
   </sheetData>
@@ -29299,7 +29299,7 @@
         <v>131</v>
       </c>
       <c r="J5">
-        <v>72</v>
+        <v>73</v>
       </c>
     </row>
     <row r="6" spans="1:10">
@@ -29360,7 +29360,7 @@
         <v>9</v>
       </c>
       <c r="J7">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="8" spans="1:10">
@@ -29392,7 +29392,7 @@
         <v>216</v>
       </c>
       <c r="J8">
-        <v>186</v>
+        <v>187</v>
       </c>
     </row>
     <row r="9" spans="1:10">
@@ -29456,7 +29456,7 @@
         <v>1222</v>
       </c>
       <c r="J10">
-        <v>632</v>
+        <v>637</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -29488,7 +29488,7 @@
         <v>1879</v>
       </c>
       <c r="J11">
-        <v>1072</v>
+        <v>1080</v>
       </c>
     </row>
   </sheetData>
@@ -29830,7 +29830,7 @@
         <v>440</v>
       </c>
       <c r="J10">
-        <v>252</v>
+        <v>255</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -29862,7 +29862,7 @@
         <v>761</v>
       </c>
       <c r="J11">
-        <v>478</v>
+        <v>481</v>
       </c>
     </row>
   </sheetData>
@@ -29951,7 +29951,7 @@
         <v>128</v>
       </c>
       <c r="J2">
-        <v>61</v>
+        <v>62</v>
       </c>
     </row>
     <row r="3" spans="1:10">
@@ -29983,7 +29983,7 @@
         <v>158</v>
       </c>
       <c r="J3">
-        <v>76</v>
+        <v>79</v>
       </c>
     </row>
     <row r="4" spans="1:10">
@@ -30143,7 +30143,7 @@
         <v>383</v>
       </c>
       <c r="J8">
-        <v>281</v>
+        <v>285</v>
       </c>
     </row>
     <row r="9" spans="1:10">
@@ -30207,7 +30207,7 @@
         <v>527</v>
       </c>
       <c r="J10">
-        <v>300</v>
+        <v>305</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -30239,7 +30239,7 @@
         <v>1488</v>
       </c>
       <c r="J11">
-        <v>869</v>
+        <v>882</v>
       </c>
     </row>
   </sheetData>
@@ -30542,7 +30542,7 @@
         <v>152</v>
       </c>
       <c r="J10">
-        <v>69</v>
+        <v>70</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -30574,7 +30574,7 @@
         <v>248</v>
       </c>
       <c r="J11">
-        <v>155</v>
+        <v>156</v>
       </c>
     </row>
   </sheetData>
@@ -30883,7 +30883,7 @@
         <v>502</v>
       </c>
       <c r="J10">
-        <v>294</v>
+        <v>296</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -30915,7 +30915,7 @@
         <v>677</v>
       </c>
       <c r="J11">
-        <v>388</v>
+        <v>390</v>
       </c>
     </row>
   </sheetData>
@@ -31580,7 +31580,7 @@
         <v>124</v>
       </c>
       <c r="J10">
-        <v>71</v>
+        <v>72</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -31612,7 +31612,7 @@
         <v>335</v>
       </c>
       <c r="J11">
-        <v>245</v>
+        <v>246</v>
       </c>
     </row>
   </sheetData>
@@ -31701,7 +31701,7 @@
         <v>90</v>
       </c>
       <c r="J2">
-        <v>44</v>
+        <v>45</v>
       </c>
     </row>
     <row r="3" spans="1:10">
@@ -31893,7 +31893,7 @@
         <v>122</v>
       </c>
       <c r="J8">
-        <v>117</v>
+        <v>118</v>
       </c>
     </row>
     <row r="9" spans="1:10">
@@ -31925,7 +31925,7 @@
         <v>113</v>
       </c>
       <c r="J9">
-        <v>65</v>
+        <v>66</v>
       </c>
     </row>
     <row r="10" spans="1:10">
@@ -31957,7 +31957,7 @@
         <v>389</v>
       </c>
       <c r="J10">
-        <v>245</v>
+        <v>246</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -31989,7 +31989,7 @@
         <v>886</v>
       </c>
       <c r="J11">
-        <v>553</v>
+        <v>557</v>
       </c>
     </row>
   </sheetData>
@@ -32264,7 +32264,7 @@
         <v>405</v>
       </c>
       <c r="J8">
-        <v>342</v>
+        <v>343</v>
       </c>
     </row>
     <row r="9" spans="1:10">
@@ -32328,7 +32328,7 @@
         <v>670</v>
       </c>
       <c r="J10">
-        <v>308</v>
+        <v>309</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -32360,7 +32360,7 @@
         <v>1368</v>
       </c>
       <c r="J11">
-        <v>805</v>
+        <v>807</v>
       </c>
     </row>
   </sheetData>
@@ -32545,7 +32545,7 @@
         <v>180</v>
       </c>
       <c r="J5">
-        <v>79</v>
+        <v>80</v>
       </c>
     </row>
     <row r="6" spans="1:10">
@@ -32577,7 +32577,7 @@
         <v>43</v>
       </c>
       <c r="J6">
-        <v>24</v>
+        <v>25</v>
       </c>
     </row>
     <row r="7" spans="1:10">
@@ -32667,7 +32667,7 @@
         <v>169</v>
       </c>
       <c r="J9">
-        <v>75</v>
+        <v>77</v>
       </c>
     </row>
     <row r="10" spans="1:10">
@@ -32699,7 +32699,7 @@
         <v>1773</v>
       </c>
       <c r="J10">
-        <v>952</v>
+        <v>965</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -32731,7 +32731,7 @@
         <v>2623</v>
       </c>
       <c r="J11">
-        <v>1429</v>
+        <v>1446</v>
       </c>
     </row>
   </sheetData>
@@ -33367,7 +33367,7 @@
         <v>87</v>
       </c>
       <c r="J9">
-        <v>19</v>
+        <v>21</v>
       </c>
     </row>
     <row r="10" spans="1:10">
@@ -33399,7 +33399,7 @@
         <v>174</v>
       </c>
       <c r="J10">
-        <v>71</v>
+        <v>72</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -33431,7 +33431,7 @@
         <v>337</v>
       </c>
       <c r="J11">
-        <v>141</v>
+        <v>144</v>
       </c>
     </row>
   </sheetData>
@@ -33520,7 +33520,7 @@
         <v>58</v>
       </c>
       <c r="J2">
-        <v>26</v>
+        <v>27</v>
       </c>
     </row>
     <row r="3" spans="1:10">
@@ -33703,7 +33703,7 @@
         <v>334</v>
       </c>
       <c r="J8">
-        <v>183</v>
+        <v>186</v>
       </c>
     </row>
     <row r="9" spans="1:10">
@@ -33767,7 +33767,7 @@
         <v>606</v>
       </c>
       <c r="J10">
-        <v>274</v>
+        <v>280</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -33799,7 +33799,7 @@
         <v>1187</v>
       </c>
       <c r="J11">
-        <v>586</v>
+        <v>596</v>
       </c>
     </row>
   </sheetData>
@@ -35219,7 +35219,7 @@
         <v>19</v>
       </c>
       <c r="J2">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="3" spans="1:10">
@@ -35457,7 +35457,7 @@
         <v>181</v>
       </c>
       <c r="J10">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
   </sheetData>
@@ -35685,7 +35685,7 @@
         <v>26</v>
       </c>
       <c r="J7">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="8" spans="1:10">
@@ -35781,7 +35781,7 @@
         <v>258</v>
       </c>
       <c r="J10">
-        <v>146</v>
+        <v>147</v>
       </c>
     </row>
   </sheetData>
@@ -36295,7 +36295,7 @@
         <v>161</v>
       </c>
       <c r="J5">
-        <v>89</v>
+        <v>90</v>
       </c>
     </row>
     <row r="6" spans="1:10">
@@ -36391,7 +36391,7 @@
         <v>291</v>
       </c>
       <c r="J8">
-        <v>185</v>
+        <v>188</v>
       </c>
     </row>
     <row r="9" spans="1:10">
@@ -36423,7 +36423,7 @@
         <v>125</v>
       </c>
       <c r="J9">
-        <v>57</v>
+        <v>58</v>
       </c>
     </row>
     <row r="10" spans="1:10">
@@ -36455,7 +36455,7 @@
         <v>905</v>
       </c>
       <c r="J10">
-        <v>443</v>
+        <v>446</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -36487,7 +36487,7 @@
         <v>1669</v>
       </c>
       <c r="J11">
-        <v>884</v>
+        <v>892</v>
       </c>
     </row>
   </sheetData>
@@ -36762,7 +36762,7 @@
         <v>68</v>
       </c>
       <c r="J8">
-        <v>60</v>
+        <v>61</v>
       </c>
     </row>
     <row r="9" spans="1:10">
@@ -36826,7 +36826,7 @@
         <v>157</v>
       </c>
       <c r="J10">
-        <v>84</v>
+        <v>85</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -36858,7 +36858,7 @@
         <v>337</v>
       </c>
       <c r="J11">
-        <v>213</v>
+        <v>215</v>
       </c>
     </row>
   </sheetData>
@@ -36947,7 +36947,7 @@
         <v>8</v>
       </c>
       <c r="J2">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="3" spans="1:10">
@@ -36979,7 +36979,7 @@
         <v>4</v>
       </c>
       <c r="J3">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="4" spans="1:10">
@@ -37161,7 +37161,7 @@
         <v>101</v>
       </c>
       <c r="J10">
-        <v>45</v>
+        <v>46</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -37193,7 +37193,7 @@
         <v>160</v>
       </c>
       <c r="J11">
-        <v>87</v>
+        <v>88</v>
       </c>
     </row>
   </sheetData>
@@ -37314,7 +37314,7 @@
         <v>22</v>
       </c>
       <c r="J3">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="4" spans="1:10">
@@ -37447,7 +37447,7 @@
         <v>54</v>
       </c>
       <c r="J8">
-        <v>46</v>
+        <v>47</v>
       </c>
     </row>
     <row r="9" spans="1:10">
@@ -37543,7 +37543,7 @@
         <v>236</v>
       </c>
       <c r="J11">
-        <v>145</v>
+        <v>147</v>
       </c>
     </row>
   </sheetData>
@@ -37716,7 +37716,7 @@
         <v>19</v>
       </c>
       <c r="J5">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="6" spans="1:10">
@@ -37858,7 +37858,7 @@
         <v>717</v>
       </c>
       <c r="J10">
-        <v>308</v>
+        <v>317</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -37890,7 +37890,7 @@
         <v>1066</v>
       </c>
       <c r="J11">
-        <v>453</v>
+        <v>463</v>
       </c>
     </row>
   </sheetData>
@@ -38199,7 +38199,7 @@
         <v>260</v>
       </c>
       <c r="J10">
-        <v>117</v>
+        <v>118</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -38231,7 +38231,7 @@
         <v>393</v>
       </c>
       <c r="J11">
-        <v>166</v>
+        <v>167</v>
       </c>
     </row>
   </sheetData>
@@ -38352,7 +38352,7 @@
         <v>6</v>
       </c>
       <c r="J3">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="4" spans="1:10">
@@ -38560,7 +38560,7 @@
         <v>219</v>
       </c>
       <c r="J11">
-        <v>120</v>
+        <v>121</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add data for 2023-07-15
</commit_message>
<xml_diff>
--- a/output/index-crime-full-year.xlsx
+++ b/output/index-crime-full-year.xlsx
@@ -895,7 +895,7 @@
         <v>7277</v>
       </c>
       <c r="J2">
-        <v>3928</v>
+        <v>3956</v>
       </c>
     </row>
     <row r="3" spans="1:10">
@@ -927,7 +927,7 @@
         <v>7486</v>
       </c>
       <c r="J3">
-        <v>4129</v>
+        <v>4155</v>
       </c>
     </row>
     <row r="4" spans="1:10">
@@ -959,7 +959,7 @@
         <v>422</v>
       </c>
       <c r="J4">
-        <v>262</v>
+        <v>263</v>
       </c>
     </row>
     <row r="5" spans="1:10">
@@ -991,7 +991,7 @@
         <v>7592</v>
       </c>
       <c r="J5">
-        <v>3870</v>
+        <v>3886</v>
       </c>
     </row>
     <row r="6" spans="1:10">
@@ -1020,10 +1020,10 @@
         <v>1698</v>
       </c>
       <c r="I6">
-        <v>1771</v>
+        <v>1770</v>
       </c>
       <c r="J6">
-        <v>936</v>
+        <v>939</v>
       </c>
     </row>
     <row r="7" spans="1:10">
@@ -1055,7 +1055,7 @@
         <v>718</v>
       </c>
       <c r="J7">
-        <v>330</v>
+        <v>332</v>
       </c>
     </row>
     <row r="8" spans="1:10">
@@ -1087,7 +1087,7 @@
         <v>21444</v>
       </c>
       <c r="J8">
-        <v>15664</v>
+        <v>15769</v>
       </c>
     </row>
     <row r="9" spans="1:10">
@@ -1119,7 +1119,7 @@
         <v>8965</v>
       </c>
       <c r="J9">
-        <v>4934</v>
+        <v>4957</v>
       </c>
     </row>
     <row r="10" spans="1:10">
@@ -1151,7 +1151,7 @@
         <v>54806</v>
       </c>
       <c r="J10">
-        <v>28554</v>
+        <v>28725</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -1180,10 +1180,10 @@
         <v>84592</v>
       </c>
       <c r="I11">
-        <v>110481</v>
+        <v>110480</v>
       </c>
       <c r="J11">
-        <v>62607</v>
+        <v>62982</v>
       </c>
     </row>
   </sheetData>
@@ -1440,7 +1440,7 @@
         <v>227</v>
       </c>
       <c r="J8">
-        <v>196</v>
+        <v>198</v>
       </c>
     </row>
     <row r="9" spans="1:10">
@@ -1504,7 +1504,7 @@
         <v>648</v>
       </c>
       <c r="J10">
-        <v>386</v>
+        <v>388</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -1536,7 +1536,7 @@
         <v>1153</v>
       </c>
       <c r="J11">
-        <v>741</v>
+        <v>745</v>
       </c>
     </row>
   </sheetData>
@@ -1720,7 +1720,7 @@
         <v>7</v>
       </c>
       <c r="J6">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="7" spans="1:10">
@@ -1810,7 +1810,7 @@
         <v>57</v>
       </c>
       <c r="J9">
-        <v>32</v>
+        <v>33</v>
       </c>
     </row>
   </sheetData>
@@ -1899,7 +1899,7 @@
         <v>154</v>
       </c>
       <c r="J2">
-        <v>78</v>
+        <v>79</v>
       </c>
     </row>
     <row r="3" spans="1:10">
@@ -1931,7 +1931,7 @@
         <v>81</v>
       </c>
       <c r="J3">
-        <v>44</v>
+        <v>45</v>
       </c>
     </row>
     <row r="4" spans="1:10">
@@ -1995,7 +1995,7 @@
         <v>116</v>
       </c>
       <c r="J5">
-        <v>77</v>
+        <v>78</v>
       </c>
     </row>
     <row r="6" spans="1:10">
@@ -2091,7 +2091,7 @@
         <v>373</v>
       </c>
       <c r="J8">
-        <v>268</v>
+        <v>271</v>
       </c>
     </row>
     <row r="9" spans="1:10">
@@ -2155,7 +2155,7 @@
         <v>820</v>
       </c>
       <c r="J10">
-        <v>494</v>
+        <v>495</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -2187,7 +2187,7 @@
         <v>1713</v>
       </c>
       <c r="J11">
-        <v>1058</v>
+        <v>1065</v>
       </c>
     </row>
   </sheetData>
@@ -2462,7 +2462,7 @@
         <v>188</v>
       </c>
       <c r="J8">
-        <v>142</v>
+        <v>143</v>
       </c>
     </row>
     <row r="9" spans="1:10">
@@ -2558,7 +2558,7 @@
         <v>1228</v>
       </c>
       <c r="J11">
-        <v>700</v>
+        <v>701</v>
       </c>
     </row>
   </sheetData>
@@ -2775,7 +2775,7 @@
         <v>42</v>
       </c>
       <c r="J6">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="7" spans="1:10">
@@ -2839,7 +2839,7 @@
         <v>700</v>
       </c>
       <c r="J8">
-        <v>461</v>
+        <v>466</v>
       </c>
     </row>
     <row r="9" spans="1:10">
@@ -2871,7 +2871,7 @@
         <v>216</v>
       </c>
       <c r="J9">
-        <v>108</v>
+        <v>109</v>
       </c>
     </row>
     <row r="10" spans="1:10">
@@ -2903,7 +2903,7 @@
         <v>820</v>
       </c>
       <c r="J10">
-        <v>425</v>
+        <v>427</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -2935,7 +2935,7 @@
         <v>2472</v>
       </c>
       <c r="J11">
-        <v>1391</v>
+        <v>1398</v>
       </c>
     </row>
   </sheetData>
@@ -3024,7 +3024,7 @@
         <v>61</v>
       </c>
       <c r="J2">
-        <v>35</v>
+        <v>36</v>
       </c>
     </row>
     <row r="3" spans="1:10">
@@ -3213,7 +3213,7 @@
         <v>259</v>
       </c>
       <c r="J8">
-        <v>243</v>
+        <v>248</v>
       </c>
     </row>
     <row r="9" spans="1:10">
@@ -3245,7 +3245,7 @@
         <v>151</v>
       </c>
       <c r="J9">
-        <v>75</v>
+        <v>77</v>
       </c>
     </row>
     <row r="10" spans="1:10">
@@ -3277,7 +3277,7 @@
         <v>913</v>
       </c>
       <c r="J10">
-        <v>581</v>
+        <v>583</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -3309,7 +3309,7 @@
         <v>1600</v>
       </c>
       <c r="J11">
-        <v>1042</v>
+        <v>1052</v>
       </c>
     </row>
   </sheetData>
@@ -3616,7 +3616,7 @@
         <v>23</v>
       </c>
       <c r="J9">
-        <v>16</v>
+        <v>17</v>
       </c>
     </row>
     <row r="10" spans="1:10">
@@ -3648,7 +3648,7 @@
         <v>106</v>
       </c>
       <c r="J10">
-        <v>43</v>
+        <v>44</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -3680,7 +3680,7 @@
         <v>260</v>
       </c>
       <c r="J11">
-        <v>159</v>
+        <v>161</v>
       </c>
     </row>
   </sheetData>
@@ -3961,7 +3961,7 @@
         <v>220</v>
       </c>
       <c r="J8">
-        <v>184</v>
+        <v>185</v>
       </c>
     </row>
     <row r="9" spans="1:10">
@@ -3993,7 +3993,7 @@
         <v>63</v>
       </c>
       <c r="J9">
-        <v>33</v>
+        <v>35</v>
       </c>
     </row>
     <row r="10" spans="1:10">
@@ -4025,7 +4025,7 @@
         <v>681</v>
       </c>
       <c r="J10">
-        <v>455</v>
+        <v>458</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -4057,7 +4057,7 @@
         <v>1279</v>
       </c>
       <c r="J11">
-        <v>836</v>
+        <v>842</v>
       </c>
     </row>
   </sheetData>
@@ -4146,7 +4146,7 @@
         <v>459</v>
       </c>
       <c r="J2">
-        <v>250</v>
+        <v>251</v>
       </c>
     </row>
     <row r="3" spans="1:10">
@@ -4178,7 +4178,7 @@
         <v>530</v>
       </c>
       <c r="J3">
-        <v>284</v>
+        <v>286</v>
       </c>
     </row>
     <row r="4" spans="1:10">
@@ -4242,7 +4242,7 @@
         <v>268</v>
       </c>
       <c r="J5">
-        <v>153</v>
+        <v>154</v>
       </c>
     </row>
     <row r="6" spans="1:10">
@@ -4338,7 +4338,7 @@
         <v>794</v>
       </c>
       <c r="J8">
-        <v>582</v>
+        <v>585</v>
       </c>
     </row>
     <row r="9" spans="1:10">
@@ -4402,7 +4402,7 @@
         <v>1302</v>
       </c>
       <c r="J10">
-        <v>689</v>
+        <v>699</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -4434,7 +4434,7 @@
         <v>3950</v>
       </c>
       <c r="J11">
-        <v>2256</v>
+        <v>2273</v>
       </c>
     </row>
   </sheetData>
@@ -4523,7 +4523,7 @@
         <v>34</v>
       </c>
       <c r="J2">
-        <v>19</v>
+        <v>20</v>
       </c>
     </row>
     <row r="3" spans="1:10">
@@ -4610,7 +4610,7 @@
         <v>77</v>
       </c>
       <c r="J5">
-        <v>47</v>
+        <v>48</v>
       </c>
     </row>
     <row r="6" spans="1:10">
@@ -4697,7 +4697,7 @@
         <v>131</v>
       </c>
       <c r="J8">
-        <v>136</v>
+        <v>138</v>
       </c>
     </row>
     <row r="9" spans="1:10">
@@ -4761,7 +4761,7 @@
         <v>921</v>
       </c>
       <c r="J10">
-        <v>380</v>
+        <v>385</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -4793,7 +4793,7 @@
         <v>1318</v>
       </c>
       <c r="J11">
-        <v>652</v>
+        <v>661</v>
       </c>
     </row>
   </sheetData>
@@ -4914,7 +4914,7 @@
         <v>280</v>
       </c>
       <c r="J3">
-        <v>113</v>
+        <v>114</v>
       </c>
     </row>
     <row r="4" spans="1:10">
@@ -4978,7 +4978,7 @@
         <v>191</v>
       </c>
       <c r="J5">
-        <v>96</v>
+        <v>97</v>
       </c>
     </row>
     <row r="6" spans="1:10">
@@ -5074,7 +5074,7 @@
         <v>653</v>
       </c>
       <c r="J8">
-        <v>514</v>
+        <v>516</v>
       </c>
     </row>
     <row r="9" spans="1:10">
@@ -5106,7 +5106,7 @@
         <v>428</v>
       </c>
       <c r="J9">
-        <v>276</v>
+        <v>277</v>
       </c>
     </row>
     <row r="10" spans="1:10">
@@ -5138,7 +5138,7 @@
         <v>1089</v>
       </c>
       <c r="J10">
-        <v>633</v>
+        <v>641</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -5170,7 +5170,7 @@
         <v>2956</v>
       </c>
       <c r="J11">
-        <v>1809</v>
+        <v>1822</v>
       </c>
     </row>
   </sheetData>
@@ -5259,7 +5259,7 @@
         <v>917</v>
       </c>
       <c r="J2">
-        <v>538</v>
+        <v>540</v>
       </c>
     </row>
     <row r="3" spans="1:10">
@@ -5323,7 +5323,7 @@
         <v>436</v>
       </c>
       <c r="J4">
-        <v>245</v>
+        <v>246</v>
       </c>
     </row>
     <row r="5" spans="1:10">
@@ -5355,7 +5355,7 @@
         <v>247</v>
       </c>
       <c r="J5">
-        <v>156</v>
+        <v>157</v>
       </c>
     </row>
     <row r="6" spans="1:10">
@@ -5387,7 +5387,7 @@
         <v>793</v>
       </c>
       <c r="J6">
-        <v>539</v>
+        <v>544</v>
       </c>
     </row>
     <row r="7" spans="1:10">
@@ -5419,7 +5419,7 @@
         <v>2685</v>
       </c>
       <c r="J7">
-        <v>1585</v>
+        <v>1590</v>
       </c>
     </row>
     <row r="8" spans="1:10">
@@ -5451,7 +5451,7 @@
         <v>4743</v>
       </c>
       <c r="J8">
-        <v>2667</v>
+        <v>2681</v>
       </c>
     </row>
     <row r="9" spans="1:10">
@@ -5483,7 +5483,7 @@
         <v>519</v>
       </c>
       <c r="J9">
-        <v>289</v>
+        <v>292</v>
       </c>
     </row>
     <row r="10" spans="1:10">
@@ -5515,7 +5515,7 @@
         <v>948</v>
       </c>
       <c r="J10">
-        <v>508</v>
+        <v>510</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -5547,7 +5547,7 @@
         <v>1713</v>
       </c>
       <c r="J11">
-        <v>1058</v>
+        <v>1065</v>
       </c>
     </row>
     <row r="12" spans="1:10">
@@ -5579,7 +5579,7 @@
         <v>412</v>
       </c>
       <c r="J12">
-        <v>221</v>
+        <v>222</v>
       </c>
     </row>
     <row r="13" spans="1:10">
@@ -5611,7 +5611,7 @@
         <v>258</v>
       </c>
       <c r="J13">
-        <v>147</v>
+        <v>149</v>
       </c>
     </row>
     <row r="14" spans="1:10">
@@ -5675,7 +5675,7 @@
         <v>886</v>
       </c>
       <c r="J15">
-        <v>557</v>
+        <v>561</v>
       </c>
     </row>
     <row r="16" spans="1:10">
@@ -5707,7 +5707,7 @@
         <v>595</v>
       </c>
       <c r="J16">
-        <v>408</v>
+        <v>411</v>
       </c>
     </row>
     <row r="17" spans="1:10">
@@ -5739,7 +5739,7 @@
         <v>175</v>
       </c>
       <c r="J17">
-        <v>82</v>
+        <v>84</v>
       </c>
     </row>
     <row r="18" spans="1:10">
@@ -5771,7 +5771,7 @@
         <v>695</v>
       </c>
       <c r="J18">
-        <v>417</v>
+        <v>419</v>
       </c>
     </row>
     <row r="19" spans="1:10">
@@ -5803,7 +5803,7 @@
         <v>2636</v>
       </c>
       <c r="J19">
-        <v>1461</v>
+        <v>1468</v>
       </c>
     </row>
     <row r="20" spans="1:10">
@@ -5835,7 +5835,7 @@
         <v>2045</v>
       </c>
       <c r="J20">
-        <v>1037</v>
+        <v>1047</v>
       </c>
     </row>
     <row r="21" spans="1:10">
@@ -5899,7 +5899,7 @@
         <v>418</v>
       </c>
       <c r="J22">
-        <v>284</v>
+        <v>287</v>
       </c>
     </row>
     <row r="23" spans="1:10">
@@ -5931,7 +5931,7 @@
         <v>1368</v>
       </c>
       <c r="J23">
-        <v>807</v>
+        <v>808</v>
       </c>
     </row>
     <row r="24" spans="1:10">
@@ -5963,7 +5963,7 @@
         <v>500</v>
       </c>
       <c r="J24">
-        <v>328</v>
+        <v>329</v>
       </c>
     </row>
     <row r="25" spans="1:10">
@@ -5995,7 +5995,7 @@
         <v>430</v>
       </c>
       <c r="J25">
-        <v>254</v>
+        <v>255</v>
       </c>
     </row>
     <row r="26" spans="1:10">
@@ -6027,7 +6027,7 @@
         <v>248</v>
       </c>
       <c r="J26">
-        <v>156</v>
+        <v>157</v>
       </c>
     </row>
     <row r="27" spans="1:10">
@@ -6059,7 +6059,7 @@
         <v>1258</v>
       </c>
       <c r="J27">
-        <v>739</v>
+        <v>742</v>
       </c>
     </row>
     <row r="28" spans="1:10">
@@ -6123,7 +6123,7 @@
         <v>3950</v>
       </c>
       <c r="J29">
-        <v>2256</v>
+        <v>2273</v>
       </c>
     </row>
     <row r="30" spans="1:10">
@@ -6155,7 +6155,7 @@
         <v>260</v>
       </c>
       <c r="J30">
-        <v>159</v>
+        <v>161</v>
       </c>
     </row>
     <row r="31" spans="1:10">
@@ -6187,7 +6187,7 @@
         <v>867</v>
       </c>
       <c r="J31">
-        <v>463</v>
+        <v>468</v>
       </c>
     </row>
     <row r="32" spans="1:10">
@@ -6219,7 +6219,7 @@
         <v>209</v>
       </c>
       <c r="J32">
-        <v>153</v>
+        <v>155</v>
       </c>
     </row>
     <row r="33" spans="1:10">
@@ -6251,7 +6251,7 @@
         <v>3011</v>
       </c>
       <c r="J33">
-        <v>1779</v>
+        <v>1790</v>
       </c>
     </row>
     <row r="34" spans="1:10">
@@ -6283,7 +6283,7 @@
         <v>761</v>
       </c>
       <c r="J34">
-        <v>481</v>
+        <v>484</v>
       </c>
     </row>
     <row r="35" spans="1:10">
@@ -6315,7 +6315,7 @@
         <v>235</v>
       </c>
       <c r="J35">
-        <v>125</v>
+        <v>128</v>
       </c>
     </row>
     <row r="36" spans="1:10">
@@ -6347,7 +6347,7 @@
         <v>1491</v>
       </c>
       <c r="J36">
-        <v>898</v>
+        <v>905</v>
       </c>
     </row>
     <row r="37" spans="1:10">
@@ -6379,7 +6379,7 @@
         <v>2547</v>
       </c>
       <c r="J37">
-        <v>1525</v>
+        <v>1536</v>
       </c>
     </row>
     <row r="38" spans="1:10">
@@ -6411,7 +6411,7 @@
         <v>191</v>
       </c>
       <c r="J38">
-        <v>101</v>
+        <v>102</v>
       </c>
     </row>
     <row r="39" spans="1:10">
@@ -6507,7 +6507,7 @@
         <v>437</v>
       </c>
       <c r="J41">
-        <v>307</v>
+        <v>309</v>
       </c>
     </row>
     <row r="42" spans="1:10">
@@ -6539,7 +6539,7 @@
         <v>2956</v>
       </c>
       <c r="J42">
-        <v>1809</v>
+        <v>1822</v>
       </c>
     </row>
     <row r="43" spans="1:10">
@@ -6571,7 +6571,7 @@
         <v>1153</v>
       </c>
       <c r="J43">
-        <v>741</v>
+        <v>745</v>
       </c>
     </row>
     <row r="44" spans="1:10">
@@ -6603,7 +6603,7 @@
         <v>1228</v>
       </c>
       <c r="J44">
-        <v>700</v>
+        <v>701</v>
       </c>
     </row>
     <row r="45" spans="1:10">
@@ -6667,7 +6667,7 @@
         <v>436</v>
       </c>
       <c r="J46">
-        <v>253</v>
+        <v>256</v>
       </c>
     </row>
     <row r="47" spans="1:10">
@@ -6699,7 +6699,7 @@
         <v>903</v>
       </c>
       <c r="J47">
-        <v>517</v>
+        <v>520</v>
       </c>
     </row>
     <row r="48" spans="1:10">
@@ -6728,10 +6728,10 @@
         <v>1997</v>
       </c>
       <c r="I48">
-        <v>2623</v>
+        <v>2622</v>
       </c>
       <c r="J48">
-        <v>1446</v>
+        <v>1457</v>
       </c>
     </row>
     <row r="49" spans="1:10">
@@ -6763,7 +6763,7 @@
         <v>1648</v>
       </c>
       <c r="J49">
-        <v>889</v>
+        <v>894</v>
       </c>
     </row>
     <row r="50" spans="1:10">
@@ -6795,7 +6795,7 @@
         <v>960</v>
       </c>
       <c r="J50">
-        <v>539</v>
+        <v>543</v>
       </c>
     </row>
     <row r="51" spans="1:10">
@@ -6827,7 +6827,7 @@
         <v>1337</v>
       </c>
       <c r="J51">
-        <v>836</v>
+        <v>839</v>
       </c>
     </row>
     <row r="52" spans="1:10">
@@ -6859,7 +6859,7 @@
         <v>1491</v>
       </c>
       <c r="J52">
-        <v>1011</v>
+        <v>1020</v>
       </c>
     </row>
     <row r="53" spans="1:10">
@@ -6891,7 +6891,7 @@
         <v>1600</v>
       </c>
       <c r="J53">
-        <v>1042</v>
+        <v>1052</v>
       </c>
     </row>
     <row r="54" spans="1:10">
@@ -6923,7 +6923,7 @@
         <v>3507</v>
       </c>
       <c r="J54">
-        <v>1897</v>
+        <v>1916</v>
       </c>
     </row>
     <row r="55" spans="1:10">
@@ -6955,7 +6955,7 @@
         <v>1244</v>
       </c>
       <c r="J55">
-        <v>646</v>
+        <v>653</v>
       </c>
     </row>
     <row r="56" spans="1:10">
@@ -6987,7 +6987,7 @@
         <v>628</v>
       </c>
       <c r="J56">
-        <v>317</v>
+        <v>318</v>
       </c>
     </row>
     <row r="57" spans="1:10">
@@ -7019,7 +7019,7 @@
         <v>406</v>
       </c>
       <c r="J57">
-        <v>275</v>
+        <v>277</v>
       </c>
     </row>
     <row r="58" spans="1:10">
@@ -7115,7 +7115,7 @@
         <v>768</v>
       </c>
       <c r="J60">
-        <v>459</v>
+        <v>460</v>
       </c>
     </row>
     <row r="61" spans="1:10">
@@ -7179,7 +7179,7 @@
         <v>57</v>
       </c>
       <c r="J62">
-        <v>32</v>
+        <v>33</v>
       </c>
     </row>
     <row r="63" spans="1:10">
@@ -7211,7 +7211,7 @@
         <v>2477</v>
       </c>
       <c r="J63">
-        <v>703</v>
+        <v>701</v>
       </c>
     </row>
     <row r="64" spans="1:10">
@@ -7243,7 +7243,7 @@
         <v>1187</v>
       </c>
       <c r="J64">
-        <v>596</v>
+        <v>599</v>
       </c>
     </row>
     <row r="65" spans="1:10">
@@ -7275,7 +7275,7 @@
         <v>1515</v>
       </c>
       <c r="J65">
-        <v>969</v>
+        <v>975</v>
       </c>
     </row>
     <row r="66" spans="1:10">
@@ -7307,7 +7307,7 @@
         <v>715</v>
       </c>
       <c r="J66">
-        <v>419</v>
+        <v>420</v>
       </c>
     </row>
     <row r="67" spans="1:10">
@@ -7339,7 +7339,7 @@
         <v>2510</v>
       </c>
       <c r="J67">
-        <v>1461</v>
+        <v>1474</v>
       </c>
     </row>
     <row r="68" spans="1:10">
@@ -7403,7 +7403,7 @@
         <v>494</v>
       </c>
       <c r="J69">
-        <v>237</v>
+        <v>238</v>
       </c>
     </row>
     <row r="70" spans="1:10">
@@ -7435,7 +7435,7 @@
         <v>677</v>
       </c>
       <c r="J70">
-        <v>390</v>
+        <v>391</v>
       </c>
     </row>
     <row r="71" spans="1:10">
@@ -7467,7 +7467,7 @@
         <v>335</v>
       </c>
       <c r="J71">
-        <v>246</v>
+        <v>247</v>
       </c>
     </row>
     <row r="72" spans="1:10">
@@ -7499,7 +7499,7 @@
         <v>706</v>
       </c>
       <c r="J72">
-        <v>366</v>
+        <v>369</v>
       </c>
     </row>
     <row r="73" spans="1:10">
@@ -7531,7 +7531,7 @@
         <v>1279</v>
       </c>
       <c r="J73">
-        <v>836</v>
+        <v>842</v>
       </c>
     </row>
     <row r="74" spans="1:10">
@@ -7595,7 +7595,7 @@
         <v>340</v>
       </c>
       <c r="J75">
-        <v>198</v>
+        <v>200</v>
       </c>
     </row>
     <row r="76" spans="1:10">
@@ -7627,7 +7627,7 @@
         <v>2923</v>
       </c>
       <c r="J76">
-        <v>1612</v>
+        <v>1623</v>
       </c>
     </row>
     <row r="77" spans="1:10">
@@ -7659,7 +7659,7 @@
         <v>462</v>
       </c>
       <c r="J77">
-        <v>292</v>
+        <v>296</v>
       </c>
     </row>
     <row r="78" spans="1:10">
@@ -7691,7 +7691,7 @@
         <v>1797</v>
       </c>
       <c r="J78">
-        <v>973</v>
+        <v>981</v>
       </c>
     </row>
     <row r="79" spans="1:10">
@@ -7723,7 +7723,7 @@
         <v>2472</v>
       </c>
       <c r="J79">
-        <v>1391</v>
+        <v>1398</v>
       </c>
     </row>
     <row r="80" spans="1:10">
@@ -7755,7 +7755,7 @@
         <v>393</v>
       </c>
       <c r="J80">
-        <v>167</v>
+        <v>168</v>
       </c>
     </row>
     <row r="81" spans="1:10">
@@ -7819,7 +7819,7 @@
         <v>233</v>
       </c>
       <c r="J82">
-        <v>148</v>
+        <v>149</v>
       </c>
     </row>
     <row r="83" spans="1:10">
@@ -7851,7 +7851,7 @@
         <v>1793</v>
       </c>
       <c r="J83">
-        <v>968</v>
+        <v>970</v>
       </c>
     </row>
     <row r="84" spans="1:10">
@@ -7883,7 +7883,7 @@
         <v>729</v>
       </c>
       <c r="J84">
-        <v>467</v>
+        <v>469</v>
       </c>
     </row>
     <row r="85" spans="1:10">
@@ -7915,7 +7915,7 @@
         <v>3848</v>
       </c>
       <c r="J85">
-        <v>2288</v>
+        <v>2300</v>
       </c>
     </row>
     <row r="86" spans="1:10">
@@ -7947,7 +7947,7 @@
         <v>1066</v>
       </c>
       <c r="J86">
-        <v>463</v>
+        <v>465</v>
       </c>
     </row>
     <row r="87" spans="1:10">
@@ -7979,7 +7979,7 @@
         <v>396</v>
       </c>
       <c r="J87">
-        <v>215</v>
+        <v>216</v>
       </c>
     </row>
     <row r="88" spans="1:10">
@@ -8011,7 +8011,7 @@
         <v>943</v>
       </c>
       <c r="J88">
-        <v>561</v>
+        <v>562</v>
       </c>
     </row>
     <row r="89" spans="1:10">
@@ -8043,7 +8043,7 @@
         <v>1879</v>
       </c>
       <c r="J89">
-        <v>1080</v>
+        <v>1084</v>
       </c>
     </row>
     <row r="90" spans="1:10">
@@ -8075,7 +8075,7 @@
         <v>1354</v>
       </c>
       <c r="J90">
-        <v>825</v>
+        <v>833</v>
       </c>
     </row>
     <row r="91" spans="1:10">
@@ -8107,7 +8107,7 @@
         <v>970</v>
       </c>
       <c r="J91">
-        <v>590</v>
+        <v>595</v>
       </c>
     </row>
     <row r="92" spans="1:10">
@@ -8139,7 +8139,7 @@
         <v>337</v>
       </c>
       <c r="J92">
-        <v>215</v>
+        <v>216</v>
       </c>
     </row>
     <row r="93" spans="1:10">
@@ -8171,7 +8171,7 @@
         <v>721</v>
       </c>
       <c r="J93">
-        <v>426</v>
+        <v>428</v>
       </c>
     </row>
     <row r="94" spans="1:10">
@@ -8203,7 +8203,7 @@
         <v>2664</v>
       </c>
       <c r="J94">
-        <v>1328</v>
+        <v>1332</v>
       </c>
     </row>
     <row r="95" spans="1:10">
@@ -8235,7 +8235,7 @@
         <v>1389</v>
       </c>
       <c r="J95">
-        <v>828</v>
+        <v>829</v>
       </c>
     </row>
     <row r="96" spans="1:10">
@@ -8267,7 +8267,7 @@
         <v>1669</v>
       </c>
       <c r="J96">
-        <v>892</v>
+        <v>895</v>
       </c>
     </row>
     <row r="97" spans="1:10">
@@ -8299,7 +8299,7 @@
         <v>1673</v>
       </c>
       <c r="J97">
-        <v>933</v>
+        <v>938</v>
       </c>
     </row>
     <row r="98" spans="1:10">
@@ -8331,7 +8331,7 @@
         <v>1318</v>
       </c>
       <c r="J98">
-        <v>652</v>
+        <v>661</v>
       </c>
     </row>
     <row r="99" spans="1:10">
@@ -8363,7 +8363,7 @@
         <v>1488</v>
       </c>
       <c r="J99">
-        <v>882</v>
+        <v>884</v>
       </c>
     </row>
     <row r="100" spans="1:10">
@@ -8395,7 +8395,7 @@
         <v>237</v>
       </c>
       <c r="J100">
-        <v>162</v>
+        <v>164</v>
       </c>
     </row>
     <row r="101" spans="1:10">
@@ -8424,10 +8424,10 @@
         <v>84592</v>
       </c>
       <c r="I101">
-        <v>110481</v>
+        <v>110480</v>
       </c>
       <c r="J101">
-        <v>62607</v>
+        <v>62982</v>
       </c>
     </row>
   </sheetData>
@@ -8859,7 +8859,7 @@
         <v>1135</v>
       </c>
       <c r="J10">
-        <v>601</v>
+        <v>606</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -8891,7 +8891,7 @@
         <v>1648</v>
       </c>
       <c r="J11">
-        <v>889</v>
+        <v>894</v>
       </c>
     </row>
   </sheetData>
@@ -8980,7 +8980,7 @@
         <v>327</v>
       </c>
       <c r="J2">
-        <v>160</v>
+        <v>162</v>
       </c>
     </row>
     <row r="3" spans="1:10">
@@ -9172,7 +9172,7 @@
         <v>1026</v>
       </c>
       <c r="J8">
-        <v>768</v>
+        <v>776</v>
       </c>
     </row>
     <row r="9" spans="1:10">
@@ -9236,7 +9236,7 @@
         <v>1271</v>
       </c>
       <c r="J10">
-        <v>702</v>
+        <v>704</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -9268,7 +9268,7 @@
         <v>3848</v>
       </c>
       <c r="J11">
-        <v>2288</v>
+        <v>2300</v>
       </c>
     </row>
   </sheetData>
@@ -9357,7 +9357,7 @@
         <v>75</v>
       </c>
       <c r="J2">
-        <v>36</v>
+        <v>37</v>
       </c>
     </row>
     <row r="3" spans="1:10">
@@ -9450,7 +9450,7 @@
         <v>73</v>
       </c>
       <c r="J5">
-        <v>65</v>
+        <v>66</v>
       </c>
     </row>
     <row r="6" spans="1:10">
@@ -9578,7 +9578,7 @@
         <v>179</v>
       </c>
       <c r="J9">
-        <v>113</v>
+        <v>114</v>
       </c>
     </row>
     <row r="10" spans="1:10">
@@ -9610,7 +9610,7 @@
         <v>2132</v>
       </c>
       <c r="J10">
-        <v>1164</v>
+        <v>1172</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -9642,7 +9642,7 @@
         <v>2923</v>
       </c>
       <c r="J11">
-        <v>1612</v>
+        <v>1623</v>
       </c>
     </row>
   </sheetData>
@@ -9731,7 +9731,7 @@
         <v>38</v>
       </c>
       <c r="J2">
-        <v>18</v>
+        <v>19</v>
       </c>
     </row>
     <row r="3" spans="1:10">
@@ -9914,7 +9914,7 @@
         <v>280</v>
       </c>
       <c r="J8">
-        <v>298</v>
+        <v>299</v>
       </c>
     </row>
     <row r="9" spans="1:10">
@@ -9978,7 +9978,7 @@
         <v>1034</v>
       </c>
       <c r="J10">
-        <v>463</v>
+        <v>466</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -10010,7 +10010,7 @@
         <v>1673</v>
       </c>
       <c r="J11">
-        <v>933</v>
+        <v>938</v>
       </c>
     </row>
   </sheetData>
@@ -10099,7 +10099,7 @@
         <v>235</v>
       </c>
       <c r="J2">
-        <v>125</v>
+        <v>127</v>
       </c>
     </row>
     <row r="3" spans="1:10">
@@ -10131,7 +10131,7 @@
         <v>365</v>
       </c>
       <c r="J3">
-        <v>218</v>
+        <v>222</v>
       </c>
     </row>
     <row r="4" spans="1:10">
@@ -10291,7 +10291,7 @@
         <v>516</v>
       </c>
       <c r="J8">
-        <v>382</v>
+        <v>384</v>
       </c>
     </row>
     <row r="9" spans="1:10">
@@ -10355,7 +10355,7 @@
         <v>895</v>
       </c>
       <c r="J10">
-        <v>458</v>
+        <v>463</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -10387,7 +10387,7 @@
         <v>2510</v>
       </c>
       <c r="J11">
-        <v>1461</v>
+        <v>1474</v>
       </c>
     </row>
   </sheetData>
@@ -10732,7 +10732,7 @@
         <v>433</v>
       </c>
       <c r="J10">
-        <v>272</v>
+        <v>273</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -10764,7 +10764,7 @@
         <v>1389</v>
       </c>
       <c r="J11">
-        <v>828</v>
+        <v>829</v>
       </c>
     </row>
   </sheetData>
@@ -11045,7 +11045,7 @@
         <v>190</v>
       </c>
       <c r="J8">
-        <v>169</v>
+        <v>171</v>
       </c>
     </row>
     <row r="9" spans="1:10">
@@ -11141,7 +11141,7 @@
         <v>729</v>
       </c>
       <c r="J11">
-        <v>467</v>
+        <v>469</v>
       </c>
     </row>
   </sheetData>
@@ -11230,7 +11230,7 @@
         <v>146</v>
       </c>
       <c r="J2">
-        <v>90</v>
+        <v>94</v>
       </c>
     </row>
     <row r="3" spans="1:10">
@@ -11262,7 +11262,7 @@
         <v>190</v>
       </c>
       <c r="J3">
-        <v>110</v>
+        <v>111</v>
       </c>
     </row>
     <row r="4" spans="1:10">
@@ -11422,7 +11422,7 @@
         <v>218</v>
       </c>
       <c r="J8">
-        <v>193</v>
+        <v>195</v>
       </c>
     </row>
     <row r="9" spans="1:10">
@@ -11454,7 +11454,7 @@
         <v>196</v>
       </c>
       <c r="J9">
-        <v>173</v>
+        <v>174</v>
       </c>
     </row>
     <row r="10" spans="1:10">
@@ -11486,7 +11486,7 @@
         <v>590</v>
       </c>
       <c r="J10">
-        <v>368</v>
+        <v>369</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -11518,7 +11518,7 @@
         <v>1491</v>
       </c>
       <c r="J11">
-        <v>1011</v>
+        <v>1020</v>
       </c>
     </row>
   </sheetData>
@@ -11863,7 +11863,7 @@
         <v>474</v>
       </c>
       <c r="J10">
-        <v>224</v>
+        <v>225</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -11895,7 +11895,7 @@
         <v>943</v>
       </c>
       <c r="J11">
-        <v>561</v>
+        <v>562</v>
       </c>
     </row>
   </sheetData>
@@ -12016,7 +12016,7 @@
         <v>111</v>
       </c>
       <c r="J3">
-        <v>55</v>
+        <v>56</v>
       </c>
     </row>
     <row r="4" spans="1:10">
@@ -12205,7 +12205,7 @@
         <v>243</v>
       </c>
       <c r="J9">
-        <v>135</v>
+        <v>136</v>
       </c>
     </row>
     <row r="10" spans="1:10">
@@ -12237,7 +12237,7 @@
         <v>2528</v>
       </c>
       <c r="J10">
-        <v>1358</v>
+        <v>1375</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -12269,7 +12269,7 @@
         <v>3507</v>
       </c>
       <c r="J11">
-        <v>1897</v>
+        <v>1916</v>
       </c>
     </row>
   </sheetData>
@@ -12390,7 +12390,7 @@
         <v>118</v>
       </c>
       <c r="J3">
-        <v>62</v>
+        <v>63</v>
       </c>
     </row>
     <row r="4" spans="1:10">
@@ -12454,7 +12454,7 @@
         <v>95</v>
       </c>
       <c r="J5">
-        <v>40</v>
+        <v>41</v>
       </c>
     </row>
     <row r="6" spans="1:10">
@@ -12550,7 +12550,7 @@
         <v>503</v>
       </c>
       <c r="J8">
-        <v>340</v>
+        <v>343</v>
       </c>
     </row>
     <row r="9" spans="1:10">
@@ -12614,7 +12614,7 @@
         <v>527</v>
       </c>
       <c r="J10">
-        <v>310</v>
+        <v>312</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -12646,7 +12646,7 @@
         <v>1491</v>
       </c>
       <c r="J11">
-        <v>898</v>
+        <v>905</v>
       </c>
     </row>
   </sheetData>
@@ -12735,7 +12735,7 @@
         <v>239</v>
       </c>
       <c r="J2">
-        <v>132</v>
+        <v>133</v>
       </c>
     </row>
     <row r="3" spans="1:10">
@@ -12767,7 +12767,7 @@
         <v>261</v>
       </c>
       <c r="J3">
-        <v>159</v>
+        <v>160</v>
       </c>
     </row>
     <row r="4" spans="1:10">
@@ -12927,7 +12927,7 @@
         <v>722</v>
       </c>
       <c r="J8">
-        <v>487</v>
+        <v>491</v>
       </c>
     </row>
     <row r="9" spans="1:10">
@@ -12991,7 +12991,7 @@
         <v>813</v>
       </c>
       <c r="J10">
-        <v>449</v>
+        <v>454</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -13023,7 +13023,7 @@
         <v>2547</v>
       </c>
       <c r="J11">
-        <v>1525</v>
+        <v>1536</v>
       </c>
     </row>
   </sheetData>
@@ -13112,7 +13112,7 @@
         <v>30</v>
       </c>
       <c r="J2">
-        <v>18</v>
+        <v>19</v>
       </c>
     </row>
     <row r="3" spans="1:10">
@@ -13202,7 +13202,7 @@
         <v>46</v>
       </c>
       <c r="J5">
-        <v>26</v>
+        <v>27</v>
       </c>
     </row>
     <row r="6" spans="1:10">
@@ -13283,7 +13283,7 @@
         <v>90</v>
       </c>
       <c r="J8">
-        <v>92</v>
+        <v>93</v>
       </c>
     </row>
     <row r="9" spans="1:10">
@@ -13379,7 +13379,7 @@
         <v>418</v>
       </c>
       <c r="J11">
-        <v>284</v>
+        <v>287</v>
       </c>
     </row>
   </sheetData>
@@ -13645,7 +13645,7 @@
         <v>89</v>
       </c>
       <c r="J8">
-        <v>73</v>
+        <v>74</v>
       </c>
     </row>
     <row r="9" spans="1:10">
@@ -13677,7 +13677,7 @@
         <v>51</v>
       </c>
       <c r="J9">
-        <v>17</v>
+        <v>18</v>
       </c>
     </row>
     <row r="10" spans="1:10">
@@ -13709,7 +13709,7 @@
         <v>448</v>
       </c>
       <c r="J10">
-        <v>213</v>
+        <v>214</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -13741,7 +13741,7 @@
         <v>706</v>
       </c>
       <c r="J11">
-        <v>366</v>
+        <v>369</v>
       </c>
     </row>
   </sheetData>
@@ -13830,7 +13830,7 @@
         <v>194</v>
       </c>
       <c r="J2">
-        <v>102</v>
+        <v>104</v>
       </c>
     </row>
     <row r="3" spans="1:10">
@@ -13862,7 +13862,7 @@
         <v>182</v>
       </c>
       <c r="J3">
-        <v>114</v>
+        <v>115</v>
       </c>
     </row>
     <row r="4" spans="1:10">
@@ -14022,7 +14022,7 @@
         <v>202</v>
       </c>
       <c r="J8">
-        <v>212</v>
+        <v>213</v>
       </c>
     </row>
     <row r="9" spans="1:10">
@@ -14054,7 +14054,7 @@
         <v>189</v>
       </c>
       <c r="J9">
-        <v>128</v>
+        <v>130</v>
       </c>
     </row>
     <row r="10" spans="1:10">
@@ -14118,7 +14118,7 @@
         <v>1515</v>
       </c>
       <c r="J11">
-        <v>969</v>
+        <v>975</v>
       </c>
     </row>
   </sheetData>
@@ -14285,7 +14285,7 @@
         <v>14</v>
       </c>
       <c r="J5">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="6" spans="1:10">
@@ -14360,7 +14360,7 @@
         <v>65</v>
       </c>
       <c r="J8">
-        <v>71</v>
+        <v>72</v>
       </c>
     </row>
     <row r="9" spans="1:10">
@@ -14456,7 +14456,7 @@
         <v>209</v>
       </c>
       <c r="J11">
-        <v>153</v>
+        <v>155</v>
       </c>
     </row>
   </sheetData>
@@ -14766,7 +14766,7 @@
         <v>46</v>
       </c>
       <c r="J9">
-        <v>29</v>
+        <v>30</v>
       </c>
     </row>
     <row r="10" spans="1:10">
@@ -14830,7 +14830,7 @@
         <v>768</v>
       </c>
       <c r="J11">
-        <v>459</v>
+        <v>460</v>
       </c>
     </row>
   </sheetData>
@@ -15313,7 +15313,7 @@
         <v>205</v>
       </c>
       <c r="J3">
-        <v>118</v>
+        <v>119</v>
       </c>
     </row>
     <row r="4" spans="1:10">
@@ -15537,7 +15537,7 @@
         <v>612</v>
       </c>
       <c r="J10">
-        <v>317</v>
+        <v>318</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -15569,7 +15569,7 @@
         <v>1793</v>
       </c>
       <c r="J11">
-        <v>968</v>
+        <v>970</v>
       </c>
     </row>
   </sheetData>
@@ -15658,7 +15658,7 @@
         <v>92</v>
       </c>
       <c r="J2">
-        <v>39</v>
+        <v>40</v>
       </c>
     </row>
     <row r="3" spans="1:10">
@@ -15786,7 +15786,7 @@
         <v>15</v>
       </c>
       <c r="J6">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="7" spans="1:10">
@@ -15914,7 +15914,7 @@
         <v>610</v>
       </c>
       <c r="J10">
-        <v>266</v>
+        <v>271</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -15946,7 +15946,7 @@
         <v>1244</v>
       </c>
       <c r="J11">
-        <v>646</v>
+        <v>653</v>
       </c>
     </row>
   </sheetData>
@@ -16212,7 +16212,7 @@
         <v>294</v>
       </c>
       <c r="J8">
-        <v>203</v>
+        <v>205</v>
       </c>
     </row>
     <row r="9" spans="1:10">
@@ -16244,7 +16244,7 @@
         <v>147</v>
       </c>
       <c r="J9">
-        <v>63</v>
+        <v>64</v>
       </c>
     </row>
     <row r="10" spans="1:10">
@@ -16276,7 +16276,7 @@
         <v>2021</v>
       </c>
       <c r="J10">
-        <v>948</v>
+        <v>949</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -16308,7 +16308,7 @@
         <v>2664</v>
       </c>
       <c r="J11">
-        <v>1328</v>
+        <v>1332</v>
       </c>
     </row>
   </sheetData>
@@ -16493,7 +16493,7 @@
         <v>170</v>
       </c>
       <c r="J5">
-        <v>62</v>
+        <v>63</v>
       </c>
     </row>
     <row r="6" spans="1:10">
@@ -16589,7 +16589,7 @@
         <v>707</v>
       </c>
       <c r="J8">
-        <v>535</v>
+        <v>539</v>
       </c>
     </row>
     <row r="9" spans="1:10">
@@ -16653,7 +16653,7 @@
         <v>968</v>
       </c>
       <c r="J10">
-        <v>520</v>
+        <v>526</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -16685,7 +16685,7 @@
         <v>3011</v>
       </c>
       <c r="J11">
-        <v>1779</v>
+        <v>1790</v>
       </c>
     </row>
   </sheetData>
@@ -16806,7 +16806,7 @@
         <v>248</v>
       </c>
       <c r="J3">
-        <v>122</v>
+        <v>123</v>
       </c>
     </row>
     <row r="4" spans="1:10">
@@ -16870,7 +16870,7 @@
         <v>261</v>
       </c>
       <c r="J5">
-        <v>129</v>
+        <v>130</v>
       </c>
     </row>
     <row r="6" spans="1:10">
@@ -16966,7 +16966,7 @@
         <v>567</v>
       </c>
       <c r="J8">
-        <v>539</v>
+        <v>540</v>
       </c>
     </row>
     <row r="9" spans="1:10">
@@ -17030,7 +17030,7 @@
         <v>1023</v>
       </c>
       <c r="J10">
-        <v>493</v>
+        <v>495</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -17062,7 +17062,7 @@
         <v>2685</v>
       </c>
       <c r="J11">
-        <v>1585</v>
+        <v>1590</v>
       </c>
     </row>
   </sheetData>
@@ -17151,7 +17151,7 @@
         <v>457</v>
       </c>
       <c r="J2">
-        <v>266</v>
+        <v>269</v>
       </c>
     </row>
     <row r="3" spans="1:10">
@@ -17183,7 +17183,7 @@
         <v>445</v>
       </c>
       <c r="J3">
-        <v>291</v>
+        <v>293</v>
       </c>
     </row>
     <row r="4" spans="1:10">
@@ -17247,7 +17247,7 @@
         <v>251</v>
       </c>
       <c r="J5">
-        <v>114</v>
+        <v>115</v>
       </c>
     </row>
     <row r="6" spans="1:10">
@@ -17343,7 +17343,7 @@
         <v>1269</v>
       </c>
       <c r="J8">
-        <v>720</v>
+        <v>722</v>
       </c>
     </row>
     <row r="9" spans="1:10">
@@ -17375,7 +17375,7 @@
         <v>497</v>
       </c>
       <c r="J9">
-        <v>290</v>
+        <v>292</v>
       </c>
     </row>
     <row r="10" spans="1:10">
@@ -17407,7 +17407,7 @@
         <v>1652</v>
       </c>
       <c r="J10">
-        <v>882</v>
+        <v>886</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -17439,7 +17439,7 @@
         <v>4743</v>
       </c>
       <c r="J11">
-        <v>2667</v>
+        <v>2681</v>
       </c>
     </row>
   </sheetData>
@@ -17528,7 +17528,7 @@
         <v>106</v>
       </c>
       <c r="J2">
-        <v>56</v>
+        <v>57</v>
       </c>
     </row>
     <row r="3" spans="1:10">
@@ -17560,7 +17560,7 @@
         <v>88</v>
       </c>
       <c r="J3">
-        <v>50</v>
+        <v>51</v>
       </c>
     </row>
     <row r="4" spans="1:10">
@@ -17720,7 +17720,7 @@
         <v>441</v>
       </c>
       <c r="J8">
-        <v>326</v>
+        <v>329</v>
       </c>
     </row>
     <row r="9" spans="1:10">
@@ -17784,7 +17784,7 @@
         <v>455</v>
       </c>
       <c r="J10">
-        <v>286</v>
+        <v>289</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -17816,7 +17816,7 @@
         <v>1354</v>
       </c>
       <c r="J11">
-        <v>825</v>
+        <v>833</v>
       </c>
     </row>
   </sheetData>
@@ -18085,7 +18085,7 @@
         <v>250</v>
       </c>
       <c r="J8">
-        <v>171</v>
+        <v>173</v>
       </c>
     </row>
     <row r="9" spans="1:10">
@@ -18149,7 +18149,7 @@
         <v>417</v>
       </c>
       <c r="J10">
-        <v>220</v>
+        <v>221</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -18181,7 +18181,7 @@
         <v>903</v>
       </c>
       <c r="J11">
-        <v>517</v>
+        <v>520</v>
       </c>
     </row>
   </sheetData>
@@ -18366,7 +18366,7 @@
         <v>229</v>
       </c>
       <c r="J5">
-        <v>98</v>
+        <v>99</v>
       </c>
     </row>
     <row r="6" spans="1:10">
@@ -18462,7 +18462,7 @@
         <v>754</v>
       </c>
       <c r="J8">
-        <v>413</v>
+        <v>418</v>
       </c>
     </row>
     <row r="9" spans="1:10">
@@ -18526,7 +18526,7 @@
         <v>911</v>
       </c>
       <c r="J10">
-        <v>522</v>
+        <v>523</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -18558,7 +18558,7 @@
         <v>2636</v>
       </c>
       <c r="J11">
-        <v>1461</v>
+        <v>1468</v>
       </c>
     </row>
   </sheetData>
@@ -18812,7 +18812,7 @@
         <v>49</v>
       </c>
       <c r="J8">
-        <v>50</v>
+        <v>51</v>
       </c>
     </row>
     <row r="9" spans="1:10">
@@ -18908,7 +18908,7 @@
         <v>247</v>
       </c>
       <c r="J11">
-        <v>156</v>
+        <v>157</v>
       </c>
     </row>
   </sheetData>
@@ -18997,7 +18997,7 @@
         <v>179</v>
       </c>
       <c r="J2">
-        <v>90</v>
+        <v>91</v>
       </c>
     </row>
     <row r="3" spans="1:10">
@@ -19029,7 +19029,7 @@
         <v>177</v>
       </c>
       <c r="J3">
-        <v>92</v>
+        <v>93</v>
       </c>
     </row>
     <row r="4" spans="1:10">
@@ -19189,7 +19189,7 @@
         <v>363</v>
       </c>
       <c r="J8">
-        <v>269</v>
+        <v>271</v>
       </c>
     </row>
     <row r="9" spans="1:10">
@@ -19221,7 +19221,7 @@
         <v>224</v>
       </c>
       <c r="J9">
-        <v>75</v>
+        <v>76</v>
       </c>
     </row>
     <row r="10" spans="1:10">
@@ -19253,7 +19253,7 @@
         <v>828</v>
       </c>
       <c r="J10">
-        <v>402</v>
+        <v>407</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -19285,7 +19285,7 @@
         <v>2045</v>
       </c>
       <c r="J11">
-        <v>1037</v>
+        <v>1047</v>
       </c>
     </row>
   </sheetData>
@@ -19554,7 +19554,7 @@
         <v>98</v>
       </c>
       <c r="J8">
-        <v>87</v>
+        <v>88</v>
       </c>
     </row>
     <row r="9" spans="1:10">
@@ -19586,7 +19586,7 @@
         <v>45</v>
       </c>
       <c r="J9">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="10" spans="1:10">
@@ -19618,7 +19618,7 @@
         <v>630</v>
       </c>
       <c r="J10">
-        <v>299</v>
+        <v>301</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -19650,7 +19650,7 @@
         <v>960</v>
       </c>
       <c r="J11">
-        <v>539</v>
+        <v>543</v>
       </c>
     </row>
   </sheetData>
@@ -20133,7 +20133,7 @@
         <v>98</v>
       </c>
       <c r="J3">
-        <v>70</v>
+        <v>71</v>
       </c>
     </row>
     <row r="4" spans="1:10">
@@ -20293,7 +20293,7 @@
         <v>308</v>
       </c>
       <c r="J8">
-        <v>215</v>
+        <v>219</v>
       </c>
     </row>
     <row r="9" spans="1:10">
@@ -20389,7 +20389,7 @@
         <v>970</v>
       </c>
       <c r="J11">
-        <v>590</v>
+        <v>595</v>
       </c>
     </row>
   </sheetData>
@@ -20664,7 +20664,7 @@
         <v>122</v>
       </c>
       <c r="J8">
-        <v>123</v>
+        <v>125</v>
       </c>
     </row>
     <row r="9" spans="1:10">
@@ -20760,7 +20760,7 @@
         <v>721</v>
       </c>
       <c r="J11">
-        <v>426</v>
+        <v>428</v>
       </c>
     </row>
   </sheetData>
@@ -20933,7 +20933,7 @@
         <v>50</v>
       </c>
       <c r="J5">
-        <v>26</v>
+        <v>27</v>
       </c>
     </row>
     <row r="6" spans="1:10">
@@ -21020,7 +21020,7 @@
         <v>44</v>
       </c>
       <c r="J8">
-        <v>40</v>
+        <v>41</v>
       </c>
     </row>
     <row r="9" spans="1:10">
@@ -21084,7 +21084,7 @@
         <v>280</v>
       </c>
       <c r="J10">
-        <v>133</v>
+        <v>134</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -21116,7 +21116,7 @@
         <v>436</v>
       </c>
       <c r="J11">
-        <v>253</v>
+        <v>256</v>
       </c>
     </row>
   </sheetData>
@@ -21452,7 +21452,7 @@
         <v>216</v>
       </c>
       <c r="J10">
-        <v>113</v>
+        <v>114</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -21484,7 +21484,7 @@
         <v>436</v>
       </c>
       <c r="J11">
-        <v>245</v>
+        <v>246</v>
       </c>
     </row>
   </sheetData>
@@ -21605,7 +21605,7 @@
         <v>81</v>
       </c>
       <c r="J3">
-        <v>51</v>
+        <v>53</v>
       </c>
     </row>
     <row r="4" spans="1:10">
@@ -21826,7 +21826,7 @@
         <v>670</v>
       </c>
       <c r="J10">
-        <v>341</v>
+        <v>342</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -21858,7 +21858,7 @@
         <v>1337</v>
       </c>
       <c r="J11">
-        <v>836</v>
+        <v>839</v>
       </c>
     </row>
   </sheetData>
@@ -22075,7 +22075,7 @@
         <v>19</v>
       </c>
       <c r="J6">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="7" spans="1:10">
@@ -22203,7 +22203,7 @@
         <v>492</v>
       </c>
       <c r="J10">
-        <v>307</v>
+        <v>308</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -22235,7 +22235,7 @@
         <v>917</v>
       </c>
       <c r="J11">
-        <v>538</v>
+        <v>540</v>
       </c>
     </row>
   </sheetData>
@@ -22553,7 +22553,7 @@
         <v>205</v>
       </c>
       <c r="J10">
-        <v>95</v>
+        <v>96</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -22585,7 +22585,7 @@
         <v>412</v>
       </c>
       <c r="J11">
-        <v>221</v>
+        <v>222</v>
       </c>
     </row>
   </sheetData>
@@ -22895,7 +22895,7 @@
         <v>99</v>
       </c>
       <c r="J9">
-        <v>71</v>
+        <v>72</v>
       </c>
     </row>
     <row r="10" spans="1:10">
@@ -22927,7 +22927,7 @@
         <v>239</v>
       </c>
       <c r="J10">
-        <v>135</v>
+        <v>136</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -22959,7 +22959,7 @@
         <v>695</v>
       </c>
       <c r="J11">
-        <v>417</v>
+        <v>419</v>
       </c>
     </row>
   </sheetData>
@@ -23292,7 +23292,7 @@
         <v>277</v>
       </c>
       <c r="J10">
-        <v>164</v>
+        <v>165</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -23324,7 +23324,7 @@
         <v>500</v>
       </c>
       <c r="J11">
-        <v>328</v>
+        <v>329</v>
       </c>
     </row>
   </sheetData>
@@ -23445,7 +23445,7 @@
         <v>35</v>
       </c>
       <c r="J3">
-        <v>19</v>
+        <v>20</v>
       </c>
     </row>
     <row r="4" spans="1:10">
@@ -23698,7 +23698,7 @@
         <v>430</v>
       </c>
       <c r="J11">
-        <v>254</v>
+        <v>255</v>
       </c>
     </row>
   </sheetData>
@@ -23787,7 +23787,7 @@
         <v>69</v>
       </c>
       <c r="J2">
-        <v>34</v>
+        <v>35</v>
       </c>
     </row>
     <row r="3" spans="1:10">
@@ -24040,7 +24040,7 @@
         <v>349</v>
       </c>
       <c r="J10">
-        <v>207</v>
+        <v>211</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -24072,7 +24072,7 @@
         <v>793</v>
       </c>
       <c r="J11">
-        <v>539</v>
+        <v>544</v>
       </c>
     </row>
   </sheetData>
@@ -24405,7 +24405,7 @@
         <v>216</v>
       </c>
       <c r="J10">
-        <v>107</v>
+        <v>108</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -24437,7 +24437,7 @@
         <v>396</v>
       </c>
       <c r="J11">
-        <v>215</v>
+        <v>216</v>
       </c>
     </row>
   </sheetData>
@@ -24616,7 +24616,7 @@
         <v>82</v>
       </c>
       <c r="J5">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="6" spans="1:10">
@@ -24770,7 +24770,7 @@
         <v>784</v>
       </c>
       <c r="J10">
-        <v>467</v>
+        <v>471</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -24802,7 +24802,7 @@
         <v>1258</v>
       </c>
       <c r="J11">
-        <v>739</v>
+        <v>742</v>
       </c>
     </row>
   </sheetData>
@@ -24891,7 +24891,7 @@
         <v>78</v>
       </c>
       <c r="J2">
-        <v>40</v>
+        <v>41</v>
       </c>
     </row>
     <row r="3" spans="1:10">
@@ -24923,7 +24923,7 @@
         <v>67</v>
       </c>
       <c r="J3">
-        <v>33</v>
+        <v>34</v>
       </c>
     </row>
     <row r="4" spans="1:10">
@@ -25051,7 +25051,7 @@
         <v>2</v>
       </c>
       <c r="J7">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="8" spans="1:10">
@@ -25147,7 +25147,7 @@
         <v>381</v>
       </c>
       <c r="J10">
-        <v>192</v>
+        <v>194</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -25179,7 +25179,7 @@
         <v>867</v>
       </c>
       <c r="J11">
-        <v>463</v>
+        <v>468</v>
       </c>
     </row>
   </sheetData>
@@ -25476,7 +25476,7 @@
         <v>576</v>
       </c>
       <c r="J10">
-        <v>296</v>
+        <v>297</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -25508,7 +25508,7 @@
         <v>628</v>
       </c>
       <c r="J11">
-        <v>317</v>
+        <v>318</v>
       </c>
     </row>
   </sheetData>
@@ -25693,7 +25693,7 @@
         <v>38</v>
       </c>
       <c r="J5">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="6" spans="1:10">
@@ -25789,7 +25789,7 @@
         <v>132</v>
       </c>
       <c r="J8">
-        <v>81</v>
+        <v>83</v>
       </c>
     </row>
     <row r="9" spans="1:10">
@@ -25853,7 +25853,7 @@
         <v>130</v>
       </c>
       <c r="J10">
-        <v>80</v>
+        <v>81</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -25885,7 +25885,7 @@
         <v>462</v>
       </c>
       <c r="J11">
-        <v>292</v>
+        <v>296</v>
       </c>
     </row>
   </sheetData>
@@ -26177,7 +26177,7 @@
         <v>139</v>
       </c>
       <c r="J9">
-        <v>77</v>
+        <v>78</v>
       </c>
     </row>
     <row r="10" spans="1:10">
@@ -26209,7 +26209,7 @@
         <v>233</v>
       </c>
       <c r="J10">
-        <v>148</v>
+        <v>149</v>
       </c>
     </row>
   </sheetData>
@@ -26426,7 +26426,7 @@
         <v>42</v>
       </c>
       <c r="J6">
-        <v>22</v>
+        <v>23</v>
       </c>
     </row>
     <row r="7" spans="1:10">
@@ -26490,7 +26490,7 @@
         <v>198</v>
       </c>
       <c r="J8">
-        <v>151</v>
+        <v>152</v>
       </c>
     </row>
     <row r="9" spans="1:10">
@@ -26554,7 +26554,7 @@
         <v>1118</v>
       </c>
       <c r="J10">
-        <v>570</v>
+        <v>576</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -26586,7 +26586,7 @@
         <v>1797</v>
       </c>
       <c r="J11">
-        <v>973</v>
+        <v>981</v>
       </c>
     </row>
   </sheetData>
@@ -27269,7 +27269,7 @@
         <v>462</v>
       </c>
       <c r="J10">
-        <v>240</v>
+        <v>241</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -27301,7 +27301,7 @@
         <v>715</v>
       </c>
       <c r="J11">
-        <v>419</v>
+        <v>420</v>
       </c>
     </row>
   </sheetData>
@@ -27613,7 +27613,7 @@
         <v>376</v>
       </c>
       <c r="J10">
-        <v>249</v>
+        <v>252</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -27645,7 +27645,7 @@
         <v>595</v>
       </c>
       <c r="J11">
-        <v>408</v>
+        <v>411</v>
       </c>
     </row>
   </sheetData>
@@ -27923,7 +27923,7 @@
         <v>141</v>
       </c>
       <c r="J8">
-        <v>97</v>
+        <v>100</v>
       </c>
     </row>
     <row r="9" spans="1:10">
@@ -28019,7 +28019,7 @@
         <v>519</v>
       </c>
       <c r="J11">
-        <v>289</v>
+        <v>292</v>
       </c>
     </row>
   </sheetData>
@@ -28337,7 +28337,7 @@
         <v>63</v>
       </c>
       <c r="J10">
-        <v>23</v>
+        <v>25</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -28369,7 +28369,7 @@
         <v>175</v>
       </c>
       <c r="J11">
-        <v>82</v>
+        <v>84</v>
       </c>
     </row>
   </sheetData>
@@ -28711,7 +28711,7 @@
         <v>542</v>
       </c>
       <c r="J10">
-        <v>283</v>
+        <v>285</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -28743,7 +28743,7 @@
         <v>948</v>
       </c>
       <c r="J11">
-        <v>508</v>
+        <v>510</v>
       </c>
     </row>
   </sheetData>
@@ -29018,7 +29018,7 @@
         <v>122</v>
       </c>
       <c r="J8">
-        <v>117</v>
+        <v>118</v>
       </c>
     </row>
     <row r="9" spans="1:10">
@@ -29050,7 +29050,7 @@
         <v>35</v>
       </c>
       <c r="J9">
-        <v>44</v>
+        <v>45</v>
       </c>
     </row>
     <row r="10" spans="1:10">
@@ -29114,7 +29114,7 @@
         <v>437</v>
       </c>
       <c r="J11">
-        <v>307</v>
+        <v>309</v>
       </c>
     </row>
   </sheetData>
@@ -29360,7 +29360,7 @@
         <v>9</v>
       </c>
       <c r="J7">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="8" spans="1:10">
@@ -29456,7 +29456,7 @@
         <v>1222</v>
       </c>
       <c r="J10">
-        <v>637</v>
+        <v>640</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -29488,7 +29488,7 @@
         <v>1879</v>
       </c>
       <c r="J11">
-        <v>1080</v>
+        <v>1084</v>
       </c>
     </row>
   </sheetData>
@@ -29609,7 +29609,7 @@
         <v>32</v>
       </c>
       <c r="J3">
-        <v>15</v>
+        <v>16</v>
       </c>
     </row>
     <row r="4" spans="1:10">
@@ -29705,7 +29705,7 @@
         <v>12</v>
       </c>
       <c r="J6">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="7" spans="1:10">
@@ -29830,7 +29830,7 @@
         <v>440</v>
       </c>
       <c r="J10">
-        <v>255</v>
+        <v>256</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -29862,7 +29862,7 @@
         <v>761</v>
       </c>
       <c r="J11">
-        <v>481</v>
+        <v>484</v>
       </c>
     </row>
   </sheetData>
@@ -30143,7 +30143,7 @@
         <v>383</v>
       </c>
       <c r="J8">
-        <v>285</v>
+        <v>286</v>
       </c>
     </row>
     <row r="9" spans="1:10">
@@ -30207,7 +30207,7 @@
         <v>527</v>
       </c>
       <c r="J10">
-        <v>305</v>
+        <v>306</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -30239,7 +30239,7 @@
         <v>1488</v>
       </c>
       <c r="J11">
-        <v>882</v>
+        <v>884</v>
       </c>
     </row>
   </sheetData>
@@ -30542,7 +30542,7 @@
         <v>152</v>
       </c>
       <c r="J10">
-        <v>70</v>
+        <v>71</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -30574,7 +30574,7 @@
         <v>248</v>
       </c>
       <c r="J11">
-        <v>156</v>
+        <v>157</v>
       </c>
     </row>
   </sheetData>
@@ -30819,7 +30819,7 @@
         <v>112</v>
       </c>
       <c r="J8">
-        <v>67</v>
+        <v>68</v>
       </c>
     </row>
     <row r="9" spans="1:10">
@@ -30915,7 +30915,7 @@
         <v>677</v>
       </c>
       <c r="J11">
-        <v>390</v>
+        <v>391</v>
       </c>
     </row>
   </sheetData>
@@ -31154,7 +31154,7 @@
         <v>20</v>
       </c>
       <c r="J8">
-        <v>19</v>
+        <v>20</v>
       </c>
     </row>
     <row r="9" spans="1:10">
@@ -31218,7 +31218,7 @@
         <v>162</v>
       </c>
       <c r="J10">
-        <v>103</v>
+        <v>104</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -31250,7 +31250,7 @@
         <v>237</v>
       </c>
       <c r="J11">
-        <v>162</v>
+        <v>164</v>
       </c>
     </row>
   </sheetData>
@@ -31516,7 +31516,7 @@
         <v>123</v>
       </c>
       <c r="J8">
-        <v>121</v>
+        <v>122</v>
       </c>
     </row>
     <row r="9" spans="1:10">
@@ -31612,7 +31612,7 @@
         <v>335</v>
       </c>
       <c r="J11">
-        <v>246</v>
+        <v>247</v>
       </c>
     </row>
   </sheetData>
@@ -31701,7 +31701,7 @@
         <v>90</v>
       </c>
       <c r="J2">
-        <v>45</v>
+        <v>46</v>
       </c>
     </row>
     <row r="3" spans="1:10">
@@ -31893,7 +31893,7 @@
         <v>122</v>
       </c>
       <c r="J8">
-        <v>118</v>
+        <v>119</v>
       </c>
     </row>
     <row r="9" spans="1:10">
@@ -31925,7 +31925,7 @@
         <v>113</v>
       </c>
       <c r="J9">
-        <v>66</v>
+        <v>67</v>
       </c>
     </row>
     <row r="10" spans="1:10">
@@ -31957,7 +31957,7 @@
         <v>389</v>
       </c>
       <c r="J10">
-        <v>246</v>
+        <v>247</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -31989,7 +31989,7 @@
         <v>886</v>
       </c>
       <c r="J11">
-        <v>557</v>
+        <v>561</v>
       </c>
     </row>
   </sheetData>
@@ -32328,7 +32328,7 @@
         <v>670</v>
       </c>
       <c r="J10">
-        <v>309</v>
+        <v>310</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -32360,7 +32360,7 @@
         <v>1368</v>
       </c>
       <c r="J11">
-        <v>807</v>
+        <v>808</v>
       </c>
     </row>
   </sheetData>
@@ -32574,10 +32574,10 @@
         <v>41</v>
       </c>
       <c r="I6">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="J6">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="7" spans="1:10">
@@ -32635,7 +32635,7 @@
         <v>338</v>
       </c>
       <c r="J8">
-        <v>245</v>
+        <v>247</v>
       </c>
     </row>
     <row r="9" spans="1:10">
@@ -32699,7 +32699,7 @@
         <v>1773</v>
       </c>
       <c r="J10">
-        <v>965</v>
+        <v>973</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -32728,10 +32728,10 @@
         <v>1997</v>
       </c>
       <c r="I11">
-        <v>2623</v>
+        <v>2622</v>
       </c>
       <c r="J11">
-        <v>1446</v>
+        <v>1457</v>
       </c>
     </row>
   </sheetData>
@@ -32997,7 +32997,7 @@
         <v>90</v>
       </c>
       <c r="J8">
-        <v>61</v>
+        <v>62</v>
       </c>
     </row>
     <row r="9" spans="1:10">
@@ -33029,7 +33029,7 @@
         <v>21</v>
       </c>
       <c r="J9">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="10" spans="1:10">
@@ -33093,7 +33093,7 @@
         <v>340</v>
       </c>
       <c r="J11">
-        <v>198</v>
+        <v>200</v>
       </c>
     </row>
   </sheetData>
@@ -33703,7 +33703,7 @@
         <v>334</v>
       </c>
       <c r="J8">
-        <v>186</v>
+        <v>187</v>
       </c>
     </row>
     <row r="9" spans="1:10">
@@ -33767,7 +33767,7 @@
         <v>606</v>
       </c>
       <c r="J10">
-        <v>280</v>
+        <v>282</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -33799,7 +33799,7 @@
         <v>1187</v>
       </c>
       <c r="J11">
-        <v>596</v>
+        <v>599</v>
       </c>
     </row>
   </sheetData>
@@ -34430,7 +34430,7 @@
         <v>313</v>
       </c>
       <c r="J10">
-        <v>140</v>
+        <v>141</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -34462,7 +34462,7 @@
         <v>494</v>
       </c>
       <c r="J11">
-        <v>237</v>
+        <v>238</v>
       </c>
     </row>
   </sheetData>
@@ -35098,7 +35098,7 @@
         <v>211</v>
       </c>
       <c r="J10">
-        <v>139</v>
+        <v>141</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -35130,7 +35130,7 @@
         <v>406</v>
       </c>
       <c r="J11">
-        <v>275</v>
+        <v>277</v>
       </c>
     </row>
   </sheetData>
@@ -35749,7 +35749,7 @@
         <v>187</v>
       </c>
       <c r="J9">
-        <v>113</v>
+        <v>115</v>
       </c>
     </row>
     <row r="10" spans="1:10">
@@ -35781,7 +35781,7 @@
         <v>258</v>
       </c>
       <c r="J10">
-        <v>147</v>
+        <v>149</v>
       </c>
     </row>
   </sheetData>
@@ -36263,7 +36263,7 @@
         <v>7</v>
       </c>
       <c r="J4">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="5" spans="1:10">
@@ -36391,7 +36391,7 @@
         <v>291</v>
       </c>
       <c r="J8">
-        <v>188</v>
+        <v>189</v>
       </c>
     </row>
     <row r="9" spans="1:10">
@@ -36455,7 +36455,7 @@
         <v>905</v>
       </c>
       <c r="J10">
-        <v>446</v>
+        <v>447</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -36487,7 +36487,7 @@
         <v>1669</v>
       </c>
       <c r="J11">
-        <v>892</v>
+        <v>895</v>
       </c>
     </row>
   </sheetData>
@@ -36576,7 +36576,7 @@
         <v>27</v>
       </c>
       <c r="J2">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="3" spans="1:10">
@@ -36858,7 +36858,7 @@
         <v>337</v>
       </c>
       <c r="J11">
-        <v>215</v>
+        <v>216</v>
       </c>
     </row>
   </sheetData>
@@ -37794,7 +37794,7 @@
         <v>160</v>
       </c>
       <c r="J8">
-        <v>59</v>
+        <v>60</v>
       </c>
     </row>
     <row r="9" spans="1:10">
@@ -37858,7 +37858,7 @@
         <v>717</v>
       </c>
       <c r="J10">
-        <v>317</v>
+        <v>318</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -37890,7 +37890,7 @@
         <v>1066</v>
       </c>
       <c r="J11">
-        <v>463</v>
+        <v>465</v>
       </c>
     </row>
   </sheetData>
@@ -38011,7 +38011,7 @@
         <v>15</v>
       </c>
       <c r="J3">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="4" spans="1:10">
@@ -38231,7 +38231,7 @@
         <v>393</v>
       </c>
       <c r="J11">
-        <v>167</v>
+        <v>168</v>
       </c>
     </row>
   </sheetData>
@@ -39497,7 +39497,7 @@
         <v>174</v>
       </c>
       <c r="J10">
-        <v>85</v>
+        <v>88</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -39529,7 +39529,7 @@
         <v>235</v>
       </c>
       <c r="J11">
-        <v>125</v>
+        <v>128</v>
       </c>
     </row>
   </sheetData>
@@ -39797,7 +39797,7 @@
         <v>155</v>
       </c>
       <c r="J9">
-        <v>88</v>
+        <v>89</v>
       </c>
     </row>
     <row r="10" spans="1:10">
@@ -39829,7 +39829,7 @@
         <v>191</v>
       </c>
       <c r="J10">
-        <v>101</v>
+        <v>102</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add data for 2023-07-17
</commit_message>
<xml_diff>
--- a/output/index-crime-full-year.xlsx
+++ b/output/index-crime-full-year.xlsx
@@ -895,7 +895,7 @@
         <v>7277</v>
       </c>
       <c r="J2">
-        <v>3992</v>
+        <v>4017</v>
       </c>
     </row>
     <row r="3" spans="1:10">
@@ -927,7 +927,7 @@
         <v>7486</v>
       </c>
       <c r="J3">
-        <v>4187</v>
+        <v>4217</v>
       </c>
     </row>
     <row r="4" spans="1:10">
@@ -959,7 +959,7 @@
         <v>422</v>
       </c>
       <c r="J4">
-        <v>264</v>
+        <v>269</v>
       </c>
     </row>
     <row r="5" spans="1:10">
@@ -991,7 +991,7 @@
         <v>7592</v>
       </c>
       <c r="J5">
-        <v>3897</v>
+        <v>3909</v>
       </c>
     </row>
     <row r="6" spans="1:10">
@@ -1005,7 +1005,7 @@
         <v>1825</v>
       </c>
       <c r="D6">
-        <v>1954</v>
+        <v>1955</v>
       </c>
       <c r="E6">
         <v>1995</v>
@@ -1023,7 +1023,7 @@
         <v>1770</v>
       </c>
       <c r="J6">
-        <v>941</v>
+        <v>948</v>
       </c>
     </row>
     <row r="7" spans="1:10">
@@ -1055,7 +1055,7 @@
         <v>718</v>
       </c>
       <c r="J7">
-        <v>334</v>
+        <v>335</v>
       </c>
     </row>
     <row r="8" spans="1:10">
@@ -1084,10 +1084,10 @@
         <v>10602</v>
       </c>
       <c r="I8">
-        <v>21444</v>
+        <v>21445</v>
       </c>
       <c r="J8">
-        <v>15844</v>
+        <v>15926</v>
       </c>
     </row>
     <row r="9" spans="1:10">
@@ -1119,7 +1119,7 @@
         <v>8965</v>
       </c>
       <c r="J9">
-        <v>4990</v>
+        <v>5022</v>
       </c>
     </row>
     <row r="10" spans="1:10">
@@ -1133,7 +1133,7 @@
         <v>61621</v>
       </c>
       <c r="D10">
-        <v>64383</v>
+        <v>64384</v>
       </c>
       <c r="E10">
         <v>65287</v>
@@ -1148,10 +1148,10 @@
         <v>40795</v>
       </c>
       <c r="I10">
-        <v>54807</v>
+        <v>54806</v>
       </c>
       <c r="J10">
-        <v>28899</v>
+        <v>29077</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -1165,7 +1165,7 @@
         <v>116079</v>
       </c>
       <c r="D11">
-        <v>117352</v>
+        <v>117354</v>
       </c>
       <c r="E11">
         <v>113390</v>
@@ -1183,7 +1183,7 @@
         <v>110481</v>
       </c>
       <c r="J11">
-        <v>63348</v>
+        <v>63720</v>
       </c>
     </row>
   </sheetData>
@@ -1440,7 +1440,7 @@
         <v>227</v>
       </c>
       <c r="J8">
-        <v>198</v>
+        <v>199</v>
       </c>
     </row>
     <row r="9" spans="1:10">
@@ -1504,7 +1504,7 @@
         <v>648</v>
       </c>
       <c r="J10">
-        <v>390</v>
+        <v>394</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -1536,7 +1536,7 @@
         <v>1153</v>
       </c>
       <c r="J11">
-        <v>747</v>
+        <v>752</v>
       </c>
     </row>
   </sheetData>
@@ -1931,7 +1931,7 @@
         <v>81</v>
       </c>
       <c r="J3">
-        <v>45</v>
+        <v>46</v>
       </c>
     </row>
     <row r="4" spans="1:10">
@@ -2027,7 +2027,7 @@
         <v>38</v>
       </c>
       <c r="J6">
-        <v>15</v>
+        <v>16</v>
       </c>
     </row>
     <row r="7" spans="1:10">
@@ -2155,7 +2155,7 @@
         <v>820</v>
       </c>
       <c r="J10">
-        <v>498</v>
+        <v>500</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -2187,7 +2187,7 @@
         <v>1713</v>
       </c>
       <c r="J11">
-        <v>1069</v>
+        <v>1073</v>
       </c>
     </row>
   </sheetData>
@@ -2308,7 +2308,7 @@
         <v>56</v>
       </c>
       <c r="J3">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="4" spans="1:10">
@@ -2526,7 +2526,7 @@
         <v>712</v>
       </c>
       <c r="J10">
-        <v>391</v>
+        <v>394</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -2558,7 +2558,7 @@
         <v>1228</v>
       </c>
       <c r="J11">
-        <v>705</v>
+        <v>707</v>
       </c>
     </row>
   </sheetData>
@@ -2679,7 +2679,7 @@
         <v>244</v>
       </c>
       <c r="J3">
-        <v>151</v>
+        <v>152</v>
       </c>
     </row>
     <row r="4" spans="1:10">
@@ -2711,7 +2711,7 @@
         <v>11</v>
       </c>
       <c r="J4">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="5" spans="1:10">
@@ -2839,7 +2839,7 @@
         <v>700</v>
       </c>
       <c r="J8">
-        <v>467</v>
+        <v>469</v>
       </c>
     </row>
     <row r="9" spans="1:10">
@@ -2871,7 +2871,7 @@
         <v>216</v>
       </c>
       <c r="J9">
-        <v>109</v>
+        <v>110</v>
       </c>
     </row>
     <row r="10" spans="1:10">
@@ -2903,7 +2903,7 @@
         <v>820</v>
       </c>
       <c r="J10">
-        <v>428</v>
+        <v>431</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -2935,7 +2935,7 @@
         <v>2472</v>
       </c>
       <c r="J11">
-        <v>1403</v>
+        <v>1411</v>
       </c>
     </row>
   </sheetData>
@@ -3213,7 +3213,7 @@
         <v>259</v>
       </c>
       <c r="J8">
-        <v>248</v>
+        <v>253</v>
       </c>
     </row>
     <row r="9" spans="1:10">
@@ -3277,7 +3277,7 @@
         <v>913</v>
       </c>
       <c r="J10">
-        <v>586</v>
+        <v>587</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -3309,7 +3309,7 @@
         <v>1600</v>
       </c>
       <c r="J11">
-        <v>1057</v>
+        <v>1063</v>
       </c>
     </row>
   </sheetData>
@@ -3769,7 +3769,7 @@
         <v>74</v>
       </c>
       <c r="J2">
-        <v>47</v>
+        <v>48</v>
       </c>
     </row>
     <row r="3" spans="1:10">
@@ -3801,7 +3801,7 @@
         <v>71</v>
       </c>
       <c r="J3">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="4" spans="1:10">
@@ -4025,7 +4025,7 @@
         <v>681</v>
       </c>
       <c r="J10">
-        <v>462</v>
+        <v>467</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -4057,7 +4057,7 @@
         <v>1279</v>
       </c>
       <c r="J11">
-        <v>845</v>
+        <v>850</v>
       </c>
     </row>
   </sheetData>
@@ -4146,7 +4146,7 @@
         <v>459</v>
       </c>
       <c r="J2">
-        <v>253</v>
+        <v>256</v>
       </c>
     </row>
     <row r="3" spans="1:10">
@@ -4178,7 +4178,7 @@
         <v>530</v>
       </c>
       <c r="J3">
-        <v>286</v>
+        <v>288</v>
       </c>
     </row>
     <row r="4" spans="1:10">
@@ -4274,7 +4274,7 @@
         <v>83</v>
       </c>
       <c r="J6">
-        <v>46</v>
+        <v>48</v>
       </c>
     </row>
     <row r="7" spans="1:10">
@@ -4338,7 +4338,7 @@
         <v>794</v>
       </c>
       <c r="J8">
-        <v>589</v>
+        <v>591</v>
       </c>
     </row>
     <row r="9" spans="1:10">
@@ -4370,7 +4370,7 @@
         <v>433</v>
       </c>
       <c r="J9">
-        <v>198</v>
+        <v>199</v>
       </c>
     </row>
     <row r="10" spans="1:10">
@@ -4402,7 +4402,7 @@
         <v>1302</v>
       </c>
       <c r="J10">
-        <v>701</v>
+        <v>704</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -4434,7 +4434,7 @@
         <v>3950</v>
       </c>
       <c r="J11">
-        <v>2283</v>
+        <v>2296</v>
       </c>
     </row>
   </sheetData>
@@ -4697,7 +4697,7 @@
         <v>131</v>
       </c>
       <c r="J8">
-        <v>140</v>
+        <v>142</v>
       </c>
     </row>
     <row r="9" spans="1:10">
@@ -4761,7 +4761,7 @@
         <v>921</v>
       </c>
       <c r="J10">
-        <v>387</v>
+        <v>388</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -4793,7 +4793,7 @@
         <v>1318</v>
       </c>
       <c r="J11">
-        <v>666</v>
+        <v>669</v>
       </c>
     </row>
   </sheetData>
@@ -4914,7 +4914,7 @@
         <v>280</v>
       </c>
       <c r="J3">
-        <v>116</v>
+        <v>117</v>
       </c>
     </row>
     <row r="4" spans="1:10">
@@ -5074,7 +5074,7 @@
         <v>653</v>
       </c>
       <c r="J8">
-        <v>520</v>
+        <v>523</v>
       </c>
     </row>
     <row r="9" spans="1:10">
@@ -5138,7 +5138,7 @@
         <v>1089</v>
       </c>
       <c r="J10">
-        <v>646</v>
+        <v>652</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -5170,7 +5170,7 @@
         <v>2956</v>
       </c>
       <c r="J11">
-        <v>1835</v>
+        <v>1845</v>
       </c>
     </row>
   </sheetData>
@@ -5323,7 +5323,7 @@
         <v>436</v>
       </c>
       <c r="J4">
-        <v>247</v>
+        <v>250</v>
       </c>
     </row>
     <row r="5" spans="1:10">
@@ -5355,7 +5355,7 @@
         <v>247</v>
       </c>
       <c r="J5">
-        <v>158</v>
+        <v>159</v>
       </c>
     </row>
     <row r="6" spans="1:10">
@@ -5387,7 +5387,7 @@
         <v>793</v>
       </c>
       <c r="J6">
-        <v>546</v>
+        <v>551</v>
       </c>
     </row>
     <row r="7" spans="1:10">
@@ -5419,7 +5419,7 @@
         <v>2685</v>
       </c>
       <c r="J7">
-        <v>1598</v>
+        <v>1605</v>
       </c>
     </row>
     <row r="8" spans="1:10">
@@ -5451,7 +5451,7 @@
         <v>4743</v>
       </c>
       <c r="J8">
-        <v>2691</v>
+        <v>2703</v>
       </c>
     </row>
     <row r="9" spans="1:10">
@@ -5483,7 +5483,7 @@
         <v>519</v>
       </c>
       <c r="J9">
-        <v>296</v>
+        <v>298</v>
       </c>
     </row>
     <row r="10" spans="1:10">
@@ -5515,7 +5515,7 @@
         <v>948</v>
       </c>
       <c r="J10">
-        <v>512</v>
+        <v>514</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -5547,7 +5547,7 @@
         <v>1713</v>
       </c>
       <c r="J11">
-        <v>1069</v>
+        <v>1073</v>
       </c>
     </row>
     <row r="12" spans="1:10">
@@ -5611,7 +5611,7 @@
         <v>258</v>
       </c>
       <c r="J13">
-        <v>150</v>
+        <v>151</v>
       </c>
     </row>
     <row r="14" spans="1:10">
@@ -5675,7 +5675,7 @@
         <v>886</v>
       </c>
       <c r="J15">
-        <v>562</v>
+        <v>564</v>
       </c>
     </row>
     <row r="16" spans="1:10">
@@ -5707,7 +5707,7 @@
         <v>595</v>
       </c>
       <c r="J16">
-        <v>416</v>
+        <v>417</v>
       </c>
     </row>
     <row r="17" spans="1:10">
@@ -5739,7 +5739,7 @@
         <v>175</v>
       </c>
       <c r="J17">
-        <v>84</v>
+        <v>85</v>
       </c>
     </row>
     <row r="18" spans="1:10">
@@ -5771,7 +5771,7 @@
         <v>695</v>
       </c>
       <c r="J18">
-        <v>420</v>
+        <v>423</v>
       </c>
     </row>
     <row r="19" spans="1:10">
@@ -5803,7 +5803,7 @@
         <v>2636</v>
       </c>
       <c r="J19">
-        <v>1474</v>
+        <v>1480</v>
       </c>
     </row>
     <row r="20" spans="1:10">
@@ -5835,7 +5835,7 @@
         <v>2045</v>
       </c>
       <c r="J20">
-        <v>1052</v>
+        <v>1061</v>
       </c>
     </row>
     <row r="21" spans="1:10">
@@ -5899,7 +5899,7 @@
         <v>418</v>
       </c>
       <c r="J22">
-        <v>288</v>
+        <v>290</v>
       </c>
     </row>
     <row r="23" spans="1:10">
@@ -5931,7 +5931,7 @@
         <v>1368</v>
       </c>
       <c r="J23">
-        <v>810</v>
+        <v>813</v>
       </c>
     </row>
     <row r="24" spans="1:10">
@@ -5963,7 +5963,7 @@
         <v>500</v>
       </c>
       <c r="J24">
-        <v>330</v>
+        <v>332</v>
       </c>
     </row>
     <row r="25" spans="1:10">
@@ -6027,7 +6027,7 @@
         <v>248</v>
       </c>
       <c r="J26">
-        <v>160</v>
+        <v>161</v>
       </c>
     </row>
     <row r="27" spans="1:10">
@@ -6059,7 +6059,7 @@
         <v>1258</v>
       </c>
       <c r="J27">
-        <v>749</v>
+        <v>756</v>
       </c>
     </row>
     <row r="28" spans="1:10">
@@ -6123,7 +6123,7 @@
         <v>3950</v>
       </c>
       <c r="J29">
-        <v>2283</v>
+        <v>2296</v>
       </c>
     </row>
     <row r="30" spans="1:10">
@@ -6187,7 +6187,7 @@
         <v>867</v>
       </c>
       <c r="J31">
-        <v>469</v>
+        <v>472</v>
       </c>
     </row>
     <row r="32" spans="1:10">
@@ -6251,7 +6251,7 @@
         <v>3011</v>
       </c>
       <c r="J33">
-        <v>1807</v>
+        <v>1822</v>
       </c>
     </row>
     <row r="34" spans="1:10">
@@ -6347,7 +6347,7 @@
         <v>1491</v>
       </c>
       <c r="J36">
-        <v>910</v>
+        <v>912</v>
       </c>
     </row>
     <row r="37" spans="1:10">
@@ -6379,7 +6379,7 @@
         <v>2547</v>
       </c>
       <c r="J37">
-        <v>1546</v>
+        <v>1552</v>
       </c>
     </row>
     <row r="38" spans="1:10">
@@ -6411,7 +6411,7 @@
         <v>191</v>
       </c>
       <c r="J38">
-        <v>102</v>
+        <v>103</v>
       </c>
     </row>
     <row r="39" spans="1:10">
@@ -6475,7 +6475,7 @@
         <v>236</v>
       </c>
       <c r="J40">
-        <v>150</v>
+        <v>153</v>
       </c>
     </row>
     <row r="41" spans="1:10">
@@ -6539,7 +6539,7 @@
         <v>2956</v>
       </c>
       <c r="J42">
-        <v>1835</v>
+        <v>1845</v>
       </c>
     </row>
     <row r="43" spans="1:10">
@@ -6571,7 +6571,7 @@
         <v>1153</v>
       </c>
       <c r="J43">
-        <v>747</v>
+        <v>752</v>
       </c>
     </row>
     <row r="44" spans="1:10">
@@ -6603,7 +6603,7 @@
         <v>1228</v>
       </c>
       <c r="J44">
-        <v>705</v>
+        <v>707</v>
       </c>
     </row>
     <row r="45" spans="1:10">
@@ -6667,7 +6667,7 @@
         <v>436</v>
       </c>
       <c r="J46">
-        <v>259</v>
+        <v>261</v>
       </c>
     </row>
     <row r="47" spans="1:10">
@@ -6699,7 +6699,7 @@
         <v>903</v>
       </c>
       <c r="J47">
-        <v>525</v>
+        <v>532</v>
       </c>
     </row>
     <row r="48" spans="1:10">
@@ -6731,7 +6731,7 @@
         <v>2622</v>
       </c>
       <c r="J48">
-        <v>1469</v>
+        <v>1478</v>
       </c>
     </row>
     <row r="49" spans="1:10">
@@ -6763,7 +6763,7 @@
         <v>1648</v>
       </c>
       <c r="J49">
-        <v>903</v>
+        <v>908</v>
       </c>
     </row>
     <row r="50" spans="1:10">
@@ -6795,7 +6795,7 @@
         <v>960</v>
       </c>
       <c r="J50">
-        <v>544</v>
+        <v>547</v>
       </c>
     </row>
     <row r="51" spans="1:10">
@@ -6827,7 +6827,7 @@
         <v>1337</v>
       </c>
       <c r="J51">
-        <v>841</v>
+        <v>847</v>
       </c>
     </row>
     <row r="52" spans="1:10">
@@ -6859,7 +6859,7 @@
         <v>1491</v>
       </c>
       <c r="J52">
-        <v>1024</v>
+        <v>1031</v>
       </c>
     </row>
     <row r="53" spans="1:10">
@@ -6891,7 +6891,7 @@
         <v>1600</v>
       </c>
       <c r="J53">
-        <v>1057</v>
+        <v>1063</v>
       </c>
     </row>
     <row r="54" spans="1:10">
@@ -6923,7 +6923,7 @@
         <v>3507</v>
       </c>
       <c r="J54">
-        <v>1930</v>
+        <v>1939</v>
       </c>
     </row>
     <row r="55" spans="1:10">
@@ -6955,7 +6955,7 @@
         <v>1244</v>
       </c>
       <c r="J55">
-        <v>654</v>
+        <v>657</v>
       </c>
     </row>
     <row r="56" spans="1:10">
@@ -6987,7 +6987,7 @@
         <v>628</v>
       </c>
       <c r="J56">
-        <v>320</v>
+        <v>322</v>
       </c>
     </row>
     <row r="57" spans="1:10">
@@ -7019,7 +7019,7 @@
         <v>406</v>
       </c>
       <c r="J57">
-        <v>278</v>
+        <v>279</v>
       </c>
     </row>
     <row r="58" spans="1:10">
@@ -7115,7 +7115,7 @@
         <v>768</v>
       </c>
       <c r="J60">
-        <v>463</v>
+        <v>466</v>
       </c>
     </row>
     <row r="61" spans="1:10">
@@ -7147,7 +7147,7 @@
         <v>160</v>
       </c>
       <c r="J61">
-        <v>90</v>
+        <v>91</v>
       </c>
     </row>
     <row r="62" spans="1:10">
@@ -7193,7 +7193,7 @@
         <v>1176</v>
       </c>
       <c r="D63">
-        <v>1520</v>
+        <v>1522</v>
       </c>
       <c r="E63">
         <v>2043</v>
@@ -7211,7 +7211,7 @@
         <v>2478</v>
       </c>
       <c r="J63">
-        <v>698</v>
+        <v>714</v>
       </c>
     </row>
     <row r="64" spans="1:10">
@@ -7275,7 +7275,7 @@
         <v>1515</v>
       </c>
       <c r="J65">
-        <v>984</v>
+        <v>992</v>
       </c>
     </row>
     <row r="66" spans="1:10">
@@ -7307,7 +7307,7 @@
         <v>715</v>
       </c>
       <c r="J66">
-        <v>421</v>
+        <v>427</v>
       </c>
     </row>
     <row r="67" spans="1:10">
@@ -7339,7 +7339,7 @@
         <v>2510</v>
       </c>
       <c r="J67">
-        <v>1484</v>
+        <v>1492</v>
       </c>
     </row>
     <row r="68" spans="1:10">
@@ -7371,7 +7371,7 @@
         <v>437</v>
       </c>
       <c r="J68">
-        <v>192</v>
+        <v>195</v>
       </c>
     </row>
     <row r="69" spans="1:10">
@@ -7403,7 +7403,7 @@
         <v>494</v>
       </c>
       <c r="J69">
-        <v>240</v>
+        <v>242</v>
       </c>
     </row>
     <row r="70" spans="1:10">
@@ -7435,7 +7435,7 @@
         <v>677</v>
       </c>
       <c r="J70">
-        <v>393</v>
+        <v>395</v>
       </c>
     </row>
     <row r="71" spans="1:10">
@@ -7467,7 +7467,7 @@
         <v>335</v>
       </c>
       <c r="J71">
-        <v>249</v>
+        <v>251</v>
       </c>
     </row>
     <row r="72" spans="1:10">
@@ -7531,7 +7531,7 @@
         <v>1279</v>
       </c>
       <c r="J73">
-        <v>845</v>
+        <v>850</v>
       </c>
     </row>
     <row r="74" spans="1:10">
@@ -7563,7 +7563,7 @@
         <v>307</v>
       </c>
       <c r="J74">
-        <v>150</v>
+        <v>153</v>
       </c>
     </row>
     <row r="75" spans="1:10">
@@ -7595,7 +7595,7 @@
         <v>340</v>
       </c>
       <c r="J75">
-        <v>200</v>
+        <v>202</v>
       </c>
     </row>
     <row r="76" spans="1:10">
@@ -7627,7 +7627,7 @@
         <v>2923</v>
       </c>
       <c r="J76">
-        <v>1639</v>
+        <v>1650</v>
       </c>
     </row>
     <row r="77" spans="1:10">
@@ -7659,7 +7659,7 @@
         <v>462</v>
       </c>
       <c r="J77">
-        <v>297</v>
+        <v>299</v>
       </c>
     </row>
     <row r="78" spans="1:10">
@@ -7691,7 +7691,7 @@
         <v>1797</v>
       </c>
       <c r="J78">
-        <v>986</v>
+        <v>992</v>
       </c>
     </row>
     <row r="79" spans="1:10">
@@ -7723,7 +7723,7 @@
         <v>2472</v>
       </c>
       <c r="J79">
-        <v>1403</v>
+        <v>1411</v>
       </c>
     </row>
     <row r="80" spans="1:10">
@@ -7755,7 +7755,7 @@
         <v>393</v>
       </c>
       <c r="J80">
-        <v>170</v>
+        <v>171</v>
       </c>
     </row>
     <row r="81" spans="1:10">
@@ -7819,7 +7819,7 @@
         <v>233</v>
       </c>
       <c r="J82">
-        <v>150</v>
+        <v>151</v>
       </c>
     </row>
     <row r="83" spans="1:10">
@@ -7851,7 +7851,7 @@
         <v>1793</v>
       </c>
       <c r="J83">
-        <v>979</v>
+        <v>985</v>
       </c>
     </row>
     <row r="84" spans="1:10">
@@ -7883,7 +7883,7 @@
         <v>729</v>
       </c>
       <c r="J84">
-        <v>471</v>
+        <v>472</v>
       </c>
     </row>
     <row r="85" spans="1:10">
@@ -7915,7 +7915,7 @@
         <v>3848</v>
       </c>
       <c r="J85">
-        <v>2311</v>
+        <v>2322</v>
       </c>
     </row>
     <row r="86" spans="1:10">
@@ -7947,7 +7947,7 @@
         <v>1066</v>
       </c>
       <c r="J86">
-        <v>465</v>
+        <v>467</v>
       </c>
     </row>
     <row r="87" spans="1:10">
@@ -7979,7 +7979,7 @@
         <v>396</v>
       </c>
       <c r="J87">
-        <v>217</v>
+        <v>220</v>
       </c>
     </row>
     <row r="88" spans="1:10">
@@ -8011,7 +8011,7 @@
         <v>943</v>
       </c>
       <c r="J88">
-        <v>569</v>
+        <v>573</v>
       </c>
     </row>
     <row r="89" spans="1:10">
@@ -8043,7 +8043,7 @@
         <v>1879</v>
       </c>
       <c r="J89">
-        <v>1090</v>
+        <v>1103</v>
       </c>
     </row>
     <row r="90" spans="1:10">
@@ -8075,7 +8075,7 @@
         <v>1354</v>
       </c>
       <c r="J90">
-        <v>838</v>
+        <v>842</v>
       </c>
     </row>
     <row r="91" spans="1:10">
@@ -8107,7 +8107,7 @@
         <v>970</v>
       </c>
       <c r="J91">
-        <v>598</v>
+        <v>600</v>
       </c>
     </row>
     <row r="92" spans="1:10">
@@ -8139,7 +8139,7 @@
         <v>337</v>
       </c>
       <c r="J92">
-        <v>218</v>
+        <v>222</v>
       </c>
     </row>
     <row r="93" spans="1:10">
@@ -8171,7 +8171,7 @@
         <v>721</v>
       </c>
       <c r="J93">
-        <v>430</v>
+        <v>433</v>
       </c>
     </row>
     <row r="94" spans="1:10">
@@ -8203,7 +8203,7 @@
         <v>2664</v>
       </c>
       <c r="J94">
-        <v>1344</v>
+        <v>1357</v>
       </c>
     </row>
     <row r="95" spans="1:10">
@@ -8235,7 +8235,7 @@
         <v>1389</v>
       </c>
       <c r="J95">
-        <v>832</v>
+        <v>838</v>
       </c>
     </row>
     <row r="96" spans="1:10">
@@ -8267,7 +8267,7 @@
         <v>1669</v>
       </c>
       <c r="J96">
-        <v>902</v>
+        <v>906</v>
       </c>
     </row>
     <row r="97" spans="1:10">
@@ -8299,7 +8299,7 @@
         <v>1673</v>
       </c>
       <c r="J97">
-        <v>946</v>
+        <v>950</v>
       </c>
     </row>
     <row r="98" spans="1:10">
@@ -8331,7 +8331,7 @@
         <v>1318</v>
       </c>
       <c r="J98">
-        <v>666</v>
+        <v>669</v>
       </c>
     </row>
     <row r="99" spans="1:10">
@@ -8363,7 +8363,7 @@
         <v>1488</v>
       </c>
       <c r="J99">
-        <v>890</v>
+        <v>894</v>
       </c>
     </row>
     <row r="100" spans="1:10">
@@ -8395,7 +8395,7 @@
         <v>237</v>
       </c>
       <c r="J100">
-        <v>164</v>
+        <v>165</v>
       </c>
     </row>
     <row r="101" spans="1:10">
@@ -8409,7 +8409,7 @@
         <v>116079</v>
       </c>
       <c r="D101">
-        <v>117352</v>
+        <v>117354</v>
       </c>
       <c r="E101">
         <v>113390</v>
@@ -8427,7 +8427,7 @@
         <v>110481</v>
       </c>
       <c r="J101">
-        <v>63348</v>
+        <v>63720</v>
       </c>
     </row>
   </sheetData>
@@ -8859,7 +8859,7 @@
         <v>1135</v>
       </c>
       <c r="J10">
-        <v>615</v>
+        <v>620</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -8891,7 +8891,7 @@
         <v>1648</v>
       </c>
       <c r="J11">
-        <v>903</v>
+        <v>908</v>
       </c>
     </row>
   </sheetData>
@@ -8980,7 +8980,7 @@
         <v>327</v>
       </c>
       <c r="J2">
-        <v>163</v>
+        <v>164</v>
       </c>
     </row>
     <row r="3" spans="1:10">
@@ -9012,7 +9012,7 @@
         <v>439</v>
       </c>
       <c r="J3">
-        <v>236</v>
+        <v>238</v>
       </c>
     </row>
     <row r="4" spans="1:10">
@@ -9172,7 +9172,7 @@
         <v>1026</v>
       </c>
       <c r="J8">
-        <v>780</v>
+        <v>785</v>
       </c>
     </row>
     <row r="9" spans="1:10">
@@ -9236,7 +9236,7 @@
         <v>1271</v>
       </c>
       <c r="J10">
-        <v>709</v>
+        <v>712</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -9268,7 +9268,7 @@
         <v>3848</v>
       </c>
       <c r="J11">
-        <v>2311</v>
+        <v>2322</v>
       </c>
     </row>
   </sheetData>
@@ -9546,7 +9546,7 @@
         <v>336</v>
       </c>
       <c r="J8">
-        <v>171</v>
+        <v>174</v>
       </c>
     </row>
     <row r="9" spans="1:10">
@@ -9578,7 +9578,7 @@
         <v>179</v>
       </c>
       <c r="J9">
-        <v>118</v>
+        <v>119</v>
       </c>
     </row>
     <row r="10" spans="1:10">
@@ -9610,7 +9610,7 @@
         <v>2132</v>
       </c>
       <c r="J10">
-        <v>1182</v>
+        <v>1189</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -9642,7 +9642,7 @@
         <v>2923</v>
       </c>
       <c r="J11">
-        <v>1639</v>
+        <v>1650</v>
       </c>
     </row>
   </sheetData>
@@ -9821,7 +9821,7 @@
         <v>122</v>
       </c>
       <c r="J5">
-        <v>73</v>
+        <v>74</v>
       </c>
     </row>
     <row r="6" spans="1:10">
@@ -9946,7 +9946,7 @@
         <v>156</v>
       </c>
       <c r="J9">
-        <v>64</v>
+        <v>65</v>
       </c>
     </row>
     <row r="10" spans="1:10">
@@ -9978,7 +9978,7 @@
         <v>1034</v>
       </c>
       <c r="J10">
-        <v>472</v>
+        <v>474</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -10010,7 +10010,7 @@
         <v>1673</v>
       </c>
       <c r="J11">
-        <v>946</v>
+        <v>950</v>
       </c>
     </row>
   </sheetData>
@@ -10099,7 +10099,7 @@
         <v>235</v>
       </c>
       <c r="J2">
-        <v>128</v>
+        <v>129</v>
       </c>
     </row>
     <row r="3" spans="1:10">
@@ -10131,7 +10131,7 @@
         <v>365</v>
       </c>
       <c r="J3">
-        <v>224</v>
+        <v>227</v>
       </c>
     </row>
     <row r="4" spans="1:10">
@@ -10195,7 +10195,7 @@
         <v>102</v>
       </c>
       <c r="J5">
-        <v>63</v>
+        <v>64</v>
       </c>
     </row>
     <row r="6" spans="1:10">
@@ -10227,7 +10227,7 @@
         <v>56</v>
       </c>
       <c r="J6">
-        <v>38</v>
+        <v>39</v>
       </c>
     </row>
     <row r="7" spans="1:10">
@@ -10355,7 +10355,7 @@
         <v>895</v>
       </c>
       <c r="J10">
-        <v>467</v>
+        <v>469</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -10387,7 +10387,7 @@
         <v>2510</v>
       </c>
       <c r="J11">
-        <v>1484</v>
+        <v>1492</v>
       </c>
     </row>
   </sheetData>
@@ -10508,7 +10508,7 @@
         <v>137</v>
       </c>
       <c r="J3">
-        <v>71</v>
+        <v>72</v>
       </c>
     </row>
     <row r="4" spans="1:10">
@@ -10540,7 +10540,7 @@
         <v>6</v>
       </c>
       <c r="J4">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="5" spans="1:10">
@@ -10668,7 +10668,7 @@
         <v>392</v>
       </c>
       <c r="J8">
-        <v>287</v>
+        <v>290</v>
       </c>
     </row>
     <row r="9" spans="1:10">
@@ -10732,7 +10732,7 @@
         <v>433</v>
       </c>
       <c r="J10">
-        <v>273</v>
+        <v>274</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -10764,7 +10764,7 @@
         <v>1389</v>
       </c>
       <c r="J11">
-        <v>832</v>
+        <v>838</v>
       </c>
     </row>
   </sheetData>
@@ -10853,7 +10853,7 @@
         <v>83</v>
       </c>
       <c r="J2">
-        <v>43</v>
+        <v>44</v>
       </c>
     </row>
     <row r="3" spans="1:10">
@@ -11141,7 +11141,7 @@
         <v>729</v>
       </c>
       <c r="J11">
-        <v>471</v>
+        <v>472</v>
       </c>
     </row>
   </sheetData>
@@ -11422,7 +11422,7 @@
         <v>218</v>
       </c>
       <c r="J8">
-        <v>195</v>
+        <v>199</v>
       </c>
     </row>
     <row r="9" spans="1:10">
@@ -11454,7 +11454,7 @@
         <v>196</v>
       </c>
       <c r="J9">
-        <v>174</v>
+        <v>176</v>
       </c>
     </row>
     <row r="10" spans="1:10">
@@ -11486,7 +11486,7 @@
         <v>590</v>
       </c>
       <c r="J10">
-        <v>372</v>
+        <v>373</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -11518,7 +11518,7 @@
         <v>1491</v>
       </c>
       <c r="J11">
-        <v>1024</v>
+        <v>1031</v>
       </c>
     </row>
   </sheetData>
@@ -11639,7 +11639,7 @@
         <v>78</v>
       </c>
       <c r="J3">
-        <v>51</v>
+        <v>53</v>
       </c>
     </row>
     <row r="4" spans="1:10">
@@ -11799,7 +11799,7 @@
         <v>184</v>
       </c>
       <c r="J8">
-        <v>150</v>
+        <v>151</v>
       </c>
     </row>
     <row r="9" spans="1:10">
@@ -11863,7 +11863,7 @@
         <v>474</v>
       </c>
       <c r="J10">
-        <v>227</v>
+        <v>228</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -11895,7 +11895,7 @@
         <v>943</v>
       </c>
       <c r="J11">
-        <v>569</v>
+        <v>573</v>
       </c>
     </row>
   </sheetData>
@@ -11984,7 +11984,7 @@
         <v>108</v>
       </c>
       <c r="J2">
-        <v>66</v>
+        <v>67</v>
       </c>
     </row>
     <row r="3" spans="1:10">
@@ -12016,7 +12016,7 @@
         <v>111</v>
       </c>
       <c r="J3">
-        <v>56</v>
+        <v>57</v>
       </c>
     </row>
     <row r="4" spans="1:10">
@@ -12173,7 +12173,7 @@
         <v>401</v>
       </c>
       <c r="J8">
-        <v>225</v>
+        <v>226</v>
       </c>
     </row>
     <row r="9" spans="1:10">
@@ -12205,7 +12205,7 @@
         <v>243</v>
       </c>
       <c r="J9">
-        <v>137</v>
+        <v>138</v>
       </c>
     </row>
     <row r="10" spans="1:10">
@@ -12237,7 +12237,7 @@
         <v>2528</v>
       </c>
       <c r="J10">
-        <v>1387</v>
+        <v>1392</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -12269,7 +12269,7 @@
         <v>3507</v>
       </c>
       <c r="J11">
-        <v>1930</v>
+        <v>1939</v>
       </c>
     </row>
   </sheetData>
@@ -12358,7 +12358,7 @@
         <v>103</v>
       </c>
       <c r="J2">
-        <v>75</v>
+        <v>76</v>
       </c>
     </row>
     <row r="3" spans="1:10">
@@ -12486,7 +12486,7 @@
         <v>11</v>
       </c>
       <c r="J6">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="7" spans="1:10">
@@ -12646,7 +12646,7 @@
         <v>1491</v>
       </c>
       <c r="J11">
-        <v>910</v>
+        <v>912</v>
       </c>
     </row>
   </sheetData>
@@ -12767,7 +12767,7 @@
         <v>261</v>
       </c>
       <c r="J3">
-        <v>160</v>
+        <v>163</v>
       </c>
     </row>
     <row r="4" spans="1:10">
@@ -12831,7 +12831,7 @@
         <v>200</v>
       </c>
       <c r="J5">
-        <v>131</v>
+        <v>132</v>
       </c>
     </row>
     <row r="6" spans="1:10">
@@ -12991,7 +12991,7 @@
         <v>813</v>
       </c>
       <c r="J10">
-        <v>456</v>
+        <v>458</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -13023,7 +13023,7 @@
         <v>2547</v>
       </c>
       <c r="J11">
-        <v>1546</v>
+        <v>1552</v>
       </c>
     </row>
   </sheetData>
@@ -13202,7 +13202,7 @@
         <v>46</v>
       </c>
       <c r="J5">
-        <v>27</v>
+        <v>28</v>
       </c>
     </row>
     <row r="6" spans="1:10">
@@ -13283,7 +13283,7 @@
         <v>90</v>
       </c>
       <c r="J8">
-        <v>94</v>
+        <v>95</v>
       </c>
     </row>
     <row r="9" spans="1:10">
@@ -13379,7 +13379,7 @@
         <v>418</v>
       </c>
       <c r="J11">
-        <v>288</v>
+        <v>290</v>
       </c>
     </row>
   </sheetData>
@@ -13830,7 +13830,7 @@
         <v>194</v>
       </c>
       <c r="J2">
-        <v>106</v>
+        <v>109</v>
       </c>
     </row>
     <row r="3" spans="1:10">
@@ -14022,7 +14022,7 @@
         <v>202</v>
       </c>
       <c r="J8">
-        <v>215</v>
+        <v>216</v>
       </c>
     </row>
     <row r="9" spans="1:10">
@@ -14054,7 +14054,7 @@
         <v>189</v>
       </c>
       <c r="J9">
-        <v>132</v>
+        <v>134</v>
       </c>
     </row>
     <row r="10" spans="1:10">
@@ -14086,7 +14086,7 @@
         <v>587</v>
       </c>
       <c r="J10">
-        <v>331</v>
+        <v>333</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -14118,7 +14118,7 @@
         <v>1515</v>
       </c>
       <c r="J11">
-        <v>984</v>
+        <v>992</v>
       </c>
     </row>
   </sheetData>
@@ -14734,7 +14734,7 @@
         <v>175</v>
       </c>
       <c r="J8">
-        <v>148</v>
+        <v>149</v>
       </c>
     </row>
     <row r="9" spans="1:10">
@@ -14798,7 +14798,7 @@
         <v>379</v>
       </c>
       <c r="J10">
-        <v>193</v>
+        <v>195</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -14830,7 +14830,7 @@
         <v>768</v>
       </c>
       <c r="J11">
-        <v>463</v>
+        <v>466</v>
       </c>
     </row>
   </sheetData>
@@ -14919,7 +14919,7 @@
         <v>29</v>
       </c>
       <c r="J2">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="3" spans="1:10">
@@ -15096,7 +15096,7 @@
         <v>57</v>
       </c>
       <c r="J8">
-        <v>32</v>
+        <v>34</v>
       </c>
     </row>
     <row r="9" spans="1:10">
@@ -15192,7 +15192,7 @@
         <v>437</v>
       </c>
       <c r="J11">
-        <v>192</v>
+        <v>195</v>
       </c>
     </row>
   </sheetData>
@@ -15441,7 +15441,7 @@
         <v>24</v>
       </c>
       <c r="J7">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="8" spans="1:10">
@@ -15537,7 +15537,7 @@
         <v>612</v>
       </c>
       <c r="J10">
-        <v>320</v>
+        <v>325</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -15569,7 +15569,7 @@
         <v>1793</v>
       </c>
       <c r="J11">
-        <v>979</v>
+        <v>985</v>
       </c>
     </row>
   </sheetData>
@@ -15850,7 +15850,7 @@
         <v>224</v>
       </c>
       <c r="J8">
-        <v>166</v>
+        <v>168</v>
       </c>
     </row>
     <row r="9" spans="1:10">
@@ -15914,7 +15914,7 @@
         <v>610</v>
       </c>
       <c r="J10">
-        <v>272</v>
+        <v>273</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -15946,7 +15946,7 @@
         <v>1244</v>
       </c>
       <c r="J11">
-        <v>654</v>
+        <v>657</v>
       </c>
     </row>
   </sheetData>
@@ -16067,7 +16067,7 @@
         <v>42</v>
       </c>
       <c r="J3">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="4" spans="1:10">
@@ -16212,7 +16212,7 @@
         <v>294</v>
       </c>
       <c r="J8">
-        <v>205</v>
+        <v>206</v>
       </c>
     </row>
     <row r="9" spans="1:10">
@@ -16244,7 +16244,7 @@
         <v>147</v>
       </c>
       <c r="J9">
-        <v>66</v>
+        <v>69</v>
       </c>
     </row>
     <row r="10" spans="1:10">
@@ -16276,7 +16276,7 @@
         <v>2021</v>
       </c>
       <c r="J10">
-        <v>957</v>
+        <v>965</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -16308,7 +16308,7 @@
         <v>2664</v>
       </c>
       <c r="J11">
-        <v>1344</v>
+        <v>1357</v>
       </c>
     </row>
   </sheetData>
@@ -16397,7 +16397,7 @@
         <v>267</v>
       </c>
       <c r="J2">
-        <v>170</v>
+        <v>172</v>
       </c>
     </row>
     <row r="3" spans="1:10">
@@ -16429,7 +16429,7 @@
         <v>416</v>
       </c>
       <c r="J3">
-        <v>216</v>
+        <v>217</v>
       </c>
     </row>
     <row r="4" spans="1:10">
@@ -16493,7 +16493,7 @@
         <v>170</v>
       </c>
       <c r="J5">
-        <v>63</v>
+        <v>65</v>
       </c>
     </row>
     <row r="6" spans="1:10">
@@ -16589,7 +16589,7 @@
         <v>707</v>
       </c>
       <c r="J8">
-        <v>546</v>
+        <v>548</v>
       </c>
     </row>
     <row r="9" spans="1:10">
@@ -16621,7 +16621,7 @@
         <v>363</v>
       </c>
       <c r="J9">
-        <v>209</v>
+        <v>212</v>
       </c>
     </row>
     <row r="10" spans="1:10">
@@ -16653,7 +16653,7 @@
         <v>968</v>
       </c>
       <c r="J10">
-        <v>530</v>
+        <v>535</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -16685,7 +16685,7 @@
         <v>3011</v>
       </c>
       <c r="J11">
-        <v>1807</v>
+        <v>1822</v>
       </c>
     </row>
   </sheetData>
@@ -16774,7 +16774,7 @@
         <v>264</v>
       </c>
       <c r="J2">
-        <v>135</v>
+        <v>136</v>
       </c>
     </row>
     <row r="3" spans="1:10">
@@ -16806,7 +16806,7 @@
         <v>248</v>
       </c>
       <c r="J3">
-        <v>123</v>
+        <v>124</v>
       </c>
     </row>
     <row r="4" spans="1:10">
@@ -16870,7 +16870,7 @@
         <v>261</v>
       </c>
       <c r="J5">
-        <v>130</v>
+        <v>131</v>
       </c>
     </row>
     <row r="6" spans="1:10">
@@ -16966,7 +16966,7 @@
         <v>567</v>
       </c>
       <c r="J8">
-        <v>545</v>
+        <v>547</v>
       </c>
     </row>
     <row r="9" spans="1:10">
@@ -17030,7 +17030,7 @@
         <v>1023</v>
       </c>
       <c r="J10">
-        <v>497</v>
+        <v>499</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -17062,7 +17062,7 @@
         <v>2685</v>
       </c>
       <c r="J11">
-        <v>1598</v>
+        <v>1605</v>
       </c>
     </row>
   </sheetData>
@@ -17183,7 +17183,7 @@
         <v>445</v>
       </c>
       <c r="J3">
-        <v>294</v>
+        <v>296</v>
       </c>
     </row>
     <row r="4" spans="1:10">
@@ -17343,7 +17343,7 @@
         <v>1269</v>
       </c>
       <c r="J8">
-        <v>725</v>
+        <v>728</v>
       </c>
     </row>
     <row r="9" spans="1:10">
@@ -17375,7 +17375,7 @@
         <v>497</v>
       </c>
       <c r="J9">
-        <v>293</v>
+        <v>296</v>
       </c>
     </row>
     <row r="10" spans="1:10">
@@ -17407,7 +17407,7 @@
         <v>1652</v>
       </c>
       <c r="J10">
-        <v>887</v>
+        <v>891</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -17439,7 +17439,7 @@
         <v>4743</v>
       </c>
       <c r="J11">
-        <v>2691</v>
+        <v>2703</v>
       </c>
     </row>
   </sheetData>
@@ -17720,7 +17720,7 @@
         <v>441</v>
       </c>
       <c r="J8">
-        <v>329</v>
+        <v>331</v>
       </c>
     </row>
     <row r="9" spans="1:10">
@@ -17784,7 +17784,7 @@
         <v>455</v>
       </c>
       <c r="J10">
-        <v>289</v>
+        <v>291</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -17816,7 +17816,7 @@
         <v>1354</v>
       </c>
       <c r="J11">
-        <v>838</v>
+        <v>842</v>
       </c>
     </row>
   </sheetData>
@@ -17962,6 +17962,9 @@
       <c r="I4">
         <v>4</v>
       </c>
+      <c r="J4">
+        <v>1</v>
+      </c>
     </row>
     <row r="5" spans="1:10">
       <c r="A5" s="1" t="s">
@@ -18085,7 +18088,7 @@
         <v>250</v>
       </c>
       <c r="J8">
-        <v>175</v>
+        <v>177</v>
       </c>
     </row>
     <row r="9" spans="1:10">
@@ -18117,7 +18120,7 @@
         <v>61</v>
       </c>
       <c r="J9">
-        <v>41</v>
+        <v>42</v>
       </c>
     </row>
     <row r="10" spans="1:10">
@@ -18149,7 +18152,7 @@
         <v>417</v>
       </c>
       <c r="J10">
-        <v>222</v>
+        <v>225</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -18181,7 +18184,7 @@
         <v>903</v>
       </c>
       <c r="J11">
-        <v>525</v>
+        <v>532</v>
       </c>
     </row>
   </sheetData>
@@ -18270,7 +18273,7 @@
         <v>237</v>
       </c>
       <c r="J2">
-        <v>106</v>
+        <v>107</v>
       </c>
     </row>
     <row r="3" spans="1:10">
@@ -18302,7 +18305,7 @@
         <v>212</v>
       </c>
       <c r="J3">
-        <v>117</v>
+        <v>118</v>
       </c>
     </row>
     <row r="4" spans="1:10">
@@ -18462,7 +18465,7 @@
         <v>754</v>
       </c>
       <c r="J8">
-        <v>419</v>
+        <v>420</v>
       </c>
     </row>
     <row r="9" spans="1:10">
@@ -18526,7 +18529,7 @@
         <v>911</v>
       </c>
       <c r="J10">
-        <v>526</v>
+        <v>529</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -18558,7 +18561,7 @@
         <v>2636</v>
       </c>
       <c r="J11">
-        <v>1474</v>
+        <v>1480</v>
       </c>
     </row>
   </sheetData>
@@ -18812,7 +18815,7 @@
         <v>49</v>
       </c>
       <c r="J8">
-        <v>52</v>
+        <v>53</v>
       </c>
     </row>
     <row r="9" spans="1:10">
@@ -18908,7 +18911,7 @@
         <v>247</v>
       </c>
       <c r="J11">
-        <v>158</v>
+        <v>159</v>
       </c>
     </row>
   </sheetData>
@@ -19029,7 +19032,7 @@
         <v>177</v>
       </c>
       <c r="J3">
-        <v>93</v>
+        <v>96</v>
       </c>
     </row>
     <row r="4" spans="1:10">
@@ -19189,7 +19192,7 @@
         <v>363</v>
       </c>
       <c r="J8">
-        <v>271</v>
+        <v>274</v>
       </c>
     </row>
     <row r="9" spans="1:10">
@@ -19221,7 +19224,7 @@
         <v>224</v>
       </c>
       <c r="J9">
-        <v>76</v>
+        <v>77</v>
       </c>
     </row>
     <row r="10" spans="1:10">
@@ -19253,7 +19256,7 @@
         <v>828</v>
       </c>
       <c r="J10">
-        <v>412</v>
+        <v>414</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -19285,7 +19288,7 @@
         <v>2045</v>
       </c>
       <c r="J11">
-        <v>1052</v>
+        <v>1061</v>
       </c>
     </row>
   </sheetData>
@@ -19374,7 +19377,7 @@
         <v>37</v>
       </c>
       <c r="J2">
-        <v>21</v>
+        <v>22</v>
       </c>
     </row>
     <row r="3" spans="1:10">
@@ -19618,7 +19621,7 @@
         <v>630</v>
       </c>
       <c r="J10">
-        <v>302</v>
+        <v>304</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -19650,7 +19653,7 @@
         <v>960</v>
       </c>
       <c r="J11">
-        <v>544</v>
+        <v>547</v>
       </c>
     </row>
   </sheetData>
@@ -20101,7 +20104,7 @@
         <v>87</v>
       </c>
       <c r="J2">
-        <v>51</v>
+        <v>52</v>
       </c>
     </row>
     <row r="3" spans="1:10">
@@ -20357,7 +20360,7 @@
         <v>320</v>
       </c>
       <c r="J10">
-        <v>176</v>
+        <v>177</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -20389,7 +20392,7 @@
         <v>970</v>
       </c>
       <c r="J11">
-        <v>598</v>
+        <v>600</v>
       </c>
     </row>
   </sheetData>
@@ -20664,7 +20667,7 @@
         <v>122</v>
       </c>
       <c r="J8">
-        <v>126</v>
+        <v>127</v>
       </c>
     </row>
     <row r="9" spans="1:10">
@@ -20696,7 +20699,7 @@
         <v>62</v>
       </c>
       <c r="J9">
-        <v>24</v>
+        <v>25</v>
       </c>
     </row>
     <row r="10" spans="1:10">
@@ -20728,7 +20731,7 @@
         <v>381</v>
       </c>
       <c r="J10">
-        <v>190</v>
+        <v>191</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -20760,7 +20763,7 @@
         <v>721</v>
       </c>
       <c r="J11">
-        <v>430</v>
+        <v>433</v>
       </c>
     </row>
   </sheetData>
@@ -21020,7 +21023,7 @@
         <v>44</v>
       </c>
       <c r="J8">
-        <v>42</v>
+        <v>43</v>
       </c>
     </row>
     <row r="9" spans="1:10">
@@ -21084,7 +21087,7 @@
         <v>280</v>
       </c>
       <c r="J10">
-        <v>135</v>
+        <v>136</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -21116,7 +21119,7 @@
         <v>436</v>
       </c>
       <c r="J11">
-        <v>259</v>
+        <v>261</v>
       </c>
     </row>
   </sheetData>
@@ -21420,7 +21423,7 @@
         <v>32</v>
       </c>
       <c r="J9">
-        <v>19</v>
+        <v>20</v>
       </c>
     </row>
     <row r="10" spans="1:10">
@@ -21452,7 +21455,7 @@
         <v>216</v>
       </c>
       <c r="J10">
-        <v>115</v>
+        <v>117</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -21484,7 +21487,7 @@
         <v>436</v>
       </c>
       <c r="J11">
-        <v>247</v>
+        <v>250</v>
       </c>
     </row>
   </sheetData>
@@ -21762,7 +21765,7 @@
         <v>297</v>
       </c>
       <c r="J8">
-        <v>267</v>
+        <v>269</v>
       </c>
     </row>
     <row r="9" spans="1:10">
@@ -21794,7 +21797,7 @@
         <v>121</v>
       </c>
       <c r="J9">
-        <v>65</v>
+        <v>66</v>
       </c>
     </row>
     <row r="10" spans="1:10">
@@ -21826,7 +21829,7 @@
         <v>670</v>
       </c>
       <c r="J10">
-        <v>342</v>
+        <v>345</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -21858,7 +21861,7 @@
         <v>1337</v>
       </c>
       <c r="J11">
-        <v>841</v>
+        <v>847</v>
       </c>
     </row>
   </sheetData>
@@ -22770,7 +22773,7 @@
         <v>49</v>
       </c>
       <c r="J5">
-        <v>27</v>
+        <v>28</v>
       </c>
     </row>
     <row r="6" spans="1:10">
@@ -22863,7 +22866,7 @@
         <v>196</v>
       </c>
       <c r="J8">
-        <v>119</v>
+        <v>120</v>
       </c>
     </row>
     <row r="9" spans="1:10">
@@ -22927,7 +22930,7 @@
         <v>239</v>
       </c>
       <c r="J10">
-        <v>136</v>
+        <v>137</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -22959,7 +22962,7 @@
         <v>695</v>
       </c>
       <c r="J11">
-        <v>420</v>
+        <v>423</v>
       </c>
     </row>
   </sheetData>
@@ -23112,7 +23115,7 @@
         <v>3</v>
       </c>
       <c r="J4">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="5" spans="1:10">
@@ -23292,7 +23295,7 @@
         <v>277</v>
       </c>
       <c r="J10">
-        <v>165</v>
+        <v>166</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -23324,7 +23327,7 @@
         <v>500</v>
       </c>
       <c r="J11">
-        <v>330</v>
+        <v>332</v>
       </c>
     </row>
   </sheetData>
@@ -23819,7 +23822,7 @@
         <v>47</v>
       </c>
       <c r="J3">
-        <v>30</v>
+        <v>31</v>
       </c>
     </row>
     <row r="4" spans="1:10">
@@ -23880,7 +23883,7 @@
         <v>77</v>
       </c>
       <c r="J5">
-        <v>32</v>
+        <v>33</v>
       </c>
     </row>
     <row r="6" spans="1:10">
@@ -23976,7 +23979,7 @@
         <v>178</v>
       </c>
       <c r="J8">
-        <v>187</v>
+        <v>188</v>
       </c>
     </row>
     <row r="9" spans="1:10">
@@ -24008,7 +24011,7 @@
         <v>55</v>
       </c>
       <c r="J9">
-        <v>39</v>
+        <v>40</v>
       </c>
     </row>
     <row r="10" spans="1:10">
@@ -24040,7 +24043,7 @@
         <v>349</v>
       </c>
       <c r="J10">
-        <v>212</v>
+        <v>213</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -24072,7 +24075,7 @@
         <v>793</v>
       </c>
       <c r="J11">
-        <v>546</v>
+        <v>551</v>
       </c>
     </row>
   </sheetData>
@@ -24161,7 +24164,7 @@
         <v>10</v>
       </c>
       <c r="J2">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="3" spans="1:10">
@@ -24341,7 +24344,7 @@
         <v>70</v>
       </c>
       <c r="J8">
-        <v>44</v>
+        <v>45</v>
       </c>
     </row>
     <row r="9" spans="1:10">
@@ -24405,7 +24408,7 @@
         <v>216</v>
       </c>
       <c r="J10">
-        <v>108</v>
+        <v>109</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -24437,7 +24440,7 @@
         <v>396</v>
       </c>
       <c r="J11">
-        <v>217</v>
+        <v>220</v>
       </c>
     </row>
   </sheetData>
@@ -24526,7 +24529,7 @@
         <v>61</v>
       </c>
       <c r="J2">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="3" spans="1:10">
@@ -24770,7 +24773,7 @@
         <v>784</v>
       </c>
       <c r="J10">
-        <v>476</v>
+        <v>482</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -24802,7 +24805,7 @@
         <v>1258</v>
       </c>
       <c r="J11">
-        <v>749</v>
+        <v>756</v>
       </c>
     </row>
   </sheetData>
@@ -25147,7 +25150,7 @@
         <v>381</v>
       </c>
       <c r="J10">
-        <v>194</v>
+        <v>197</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -25179,7 +25182,7 @@
         <v>867</v>
       </c>
       <c r="J11">
-        <v>469</v>
+        <v>472</v>
       </c>
     </row>
   </sheetData>
@@ -25476,7 +25479,7 @@
         <v>576</v>
       </c>
       <c r="J10">
-        <v>298</v>
+        <v>300</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -25508,7 +25511,7 @@
         <v>628</v>
       </c>
       <c r="J11">
-        <v>320</v>
+        <v>322</v>
       </c>
     </row>
   </sheetData>
@@ -25597,7 +25600,7 @@
         <v>53</v>
       </c>
       <c r="J2">
-        <v>41</v>
+        <v>42</v>
       </c>
     </row>
     <row r="3" spans="1:10">
@@ -25853,7 +25856,7 @@
         <v>130</v>
       </c>
       <c r="J10">
-        <v>81</v>
+        <v>82</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -25885,7 +25888,7 @@
         <v>462</v>
       </c>
       <c r="J11">
-        <v>297</v>
+        <v>299</v>
       </c>
     </row>
   </sheetData>
@@ -26177,7 +26180,7 @@
         <v>139</v>
       </c>
       <c r="J9">
-        <v>79</v>
+        <v>80</v>
       </c>
     </row>
     <row r="10" spans="1:10">
@@ -26209,7 +26212,7 @@
         <v>233</v>
       </c>
       <c r="J10">
-        <v>150</v>
+        <v>151</v>
       </c>
     </row>
   </sheetData>
@@ -26330,7 +26333,7 @@
         <v>87</v>
       </c>
       <c r="J3">
-        <v>64</v>
+        <v>66</v>
       </c>
     </row>
     <row r="4" spans="1:10">
@@ -26554,7 +26557,7 @@
         <v>1118</v>
       </c>
       <c r="J10">
-        <v>579</v>
+        <v>583</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -26586,7 +26589,7 @@
         <v>1797</v>
       </c>
       <c r="J11">
-        <v>986</v>
+        <v>992</v>
       </c>
     </row>
   </sheetData>
@@ -27205,7 +27208,7 @@
         <v>99</v>
       </c>
       <c r="J8">
-        <v>77</v>
+        <v>79</v>
       </c>
     </row>
     <row r="9" spans="1:10">
@@ -27269,7 +27272,7 @@
         <v>462</v>
       </c>
       <c r="J10">
-        <v>242</v>
+        <v>246</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -27301,7 +27304,7 @@
         <v>715</v>
       </c>
       <c r="J11">
-        <v>421</v>
+        <v>427</v>
       </c>
     </row>
   </sheetData>
@@ -27613,7 +27616,7 @@
         <v>376</v>
       </c>
       <c r="J10">
-        <v>257</v>
+        <v>258</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -27645,7 +27648,7 @@
         <v>595</v>
       </c>
       <c r="J11">
-        <v>416</v>
+        <v>417</v>
       </c>
     </row>
   </sheetData>
@@ -27797,6 +27800,9 @@
       <c r="I4">
         <v>2</v>
       </c>
+      <c r="J4">
+        <v>1</v>
+      </c>
     </row>
     <row r="5" spans="1:10">
       <c r="A5" s="1" t="s">
@@ -27987,7 +27993,7 @@
         <v>193</v>
       </c>
       <c r="J10">
-        <v>89</v>
+        <v>90</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -28019,7 +28025,7 @@
         <v>519</v>
       </c>
       <c r="J11">
-        <v>296</v>
+        <v>298</v>
       </c>
     </row>
   </sheetData>
@@ -28273,7 +28279,7 @@
         <v>39</v>
       </c>
       <c r="J8">
-        <v>33</v>
+        <v>34</v>
       </c>
     </row>
     <row r="9" spans="1:10">
@@ -28369,7 +28375,7 @@
         <v>175</v>
       </c>
       <c r="J11">
-        <v>84</v>
+        <v>85</v>
       </c>
     </row>
   </sheetData>
@@ -28679,7 +28685,7 @@
         <v>90</v>
       </c>
       <c r="J9">
-        <v>41</v>
+        <v>42</v>
       </c>
     </row>
     <row r="10" spans="1:10">
@@ -28711,7 +28717,7 @@
         <v>542</v>
       </c>
       <c r="J10">
-        <v>287</v>
+        <v>288</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -28743,7 +28749,7 @@
         <v>948</v>
       </c>
       <c r="J11">
-        <v>512</v>
+        <v>514</v>
       </c>
     </row>
   </sheetData>
@@ -29392,7 +29398,7 @@
         <v>216</v>
       </c>
       <c r="J8">
-        <v>187</v>
+        <v>188</v>
       </c>
     </row>
     <row r="9" spans="1:10">
@@ -29424,7 +29430,7 @@
         <v>107</v>
       </c>
       <c r="J9">
-        <v>55</v>
+        <v>56</v>
       </c>
     </row>
     <row r="10" spans="1:10">
@@ -29456,7 +29462,7 @@
         <v>1222</v>
       </c>
       <c r="J10">
-        <v>644</v>
+        <v>655</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -29488,7 +29494,7 @@
         <v>1879</v>
       </c>
       <c r="J11">
-        <v>1090</v>
+        <v>1103</v>
       </c>
     </row>
   </sheetData>
@@ -29983,7 +29989,7 @@
         <v>158</v>
       </c>
       <c r="J3">
-        <v>79</v>
+        <v>80</v>
       </c>
     </row>
     <row r="4" spans="1:10">
@@ -30143,7 +30149,7 @@
         <v>383</v>
       </c>
       <c r="J8">
-        <v>288</v>
+        <v>289</v>
       </c>
     </row>
     <row r="9" spans="1:10">
@@ -30175,7 +30181,7 @@
         <v>118</v>
       </c>
       <c r="J9">
-        <v>53</v>
+        <v>54</v>
       </c>
     </row>
     <row r="10" spans="1:10">
@@ -30207,7 +30213,7 @@
         <v>527</v>
       </c>
       <c r="J10">
-        <v>310</v>
+        <v>311</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -30239,7 +30245,7 @@
         <v>1488</v>
       </c>
       <c r="J11">
-        <v>890</v>
+        <v>894</v>
       </c>
     </row>
   </sheetData>
@@ -30542,7 +30548,7 @@
         <v>152</v>
       </c>
       <c r="J10">
-        <v>74</v>
+        <v>75</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -30574,7 +30580,7 @@
         <v>248</v>
       </c>
       <c r="J11">
-        <v>160</v>
+        <v>161</v>
       </c>
     </row>
   </sheetData>
@@ -30819,7 +30825,7 @@
         <v>112</v>
       </c>
       <c r="J8">
-        <v>69</v>
+        <v>70</v>
       </c>
     </row>
     <row r="9" spans="1:10">
@@ -30883,7 +30889,7 @@
         <v>502</v>
       </c>
       <c r="J10">
-        <v>297</v>
+        <v>298</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -30915,7 +30921,7 @@
         <v>677</v>
       </c>
       <c r="J11">
-        <v>393</v>
+        <v>395</v>
       </c>
     </row>
   </sheetData>
@@ -31218,7 +31224,7 @@
         <v>162</v>
       </c>
       <c r="J10">
-        <v>104</v>
+        <v>105</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -31250,7 +31256,7 @@
         <v>237</v>
       </c>
       <c r="J11">
-        <v>164</v>
+        <v>165</v>
       </c>
     </row>
   </sheetData>
@@ -31371,7 +31377,7 @@
         <v>27</v>
       </c>
       <c r="J3">
-        <v>12</v>
+        <v>13</v>
       </c>
     </row>
     <row r="4" spans="1:10">
@@ -31516,7 +31522,7 @@
         <v>123</v>
       </c>
       <c r="J8">
-        <v>123</v>
+        <v>124</v>
       </c>
     </row>
     <row r="9" spans="1:10">
@@ -31612,7 +31618,7 @@
         <v>335</v>
       </c>
       <c r="J11">
-        <v>249</v>
+        <v>251</v>
       </c>
     </row>
   </sheetData>
@@ -31733,7 +31739,7 @@
         <v>69</v>
       </c>
       <c r="J3">
-        <v>42</v>
+        <v>43</v>
       </c>
     </row>
     <row r="4" spans="1:10">
@@ -31957,7 +31963,7 @@
         <v>389</v>
       </c>
       <c r="J10">
-        <v>247</v>
+        <v>248</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -31989,7 +31995,7 @@
         <v>886</v>
       </c>
       <c r="J11">
-        <v>562</v>
+        <v>564</v>
       </c>
     </row>
   </sheetData>
@@ -32078,7 +32084,7 @@
         <v>70</v>
       </c>
       <c r="J2">
-        <v>40</v>
+        <v>41</v>
       </c>
     </row>
     <row r="3" spans="1:10">
@@ -32168,7 +32174,7 @@
         <v>39</v>
       </c>
       <c r="J5">
-        <v>18</v>
+        <v>19</v>
       </c>
     </row>
     <row r="6" spans="1:10">
@@ -32328,7 +32334,7 @@
         <v>670</v>
       </c>
       <c r="J10">
-        <v>310</v>
+        <v>311</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -32360,7 +32366,7 @@
         <v>1368</v>
       </c>
       <c r="J11">
-        <v>810</v>
+        <v>813</v>
       </c>
     </row>
   </sheetData>
@@ -32635,7 +32641,7 @@
         <v>338</v>
       </c>
       <c r="J8">
-        <v>251</v>
+        <v>252</v>
       </c>
     </row>
     <row r="9" spans="1:10">
@@ -32699,7 +32705,7 @@
         <v>1773</v>
       </c>
       <c r="J10">
-        <v>979</v>
+        <v>987</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -32731,7 +32737,7 @@
         <v>2622</v>
       </c>
       <c r="J11">
-        <v>1469</v>
+        <v>1478</v>
       </c>
     </row>
   </sheetData>
@@ -32997,7 +33003,7 @@
         <v>90</v>
       </c>
       <c r="J8">
-        <v>62</v>
+        <v>63</v>
       </c>
     </row>
     <row r="9" spans="1:10">
@@ -33029,7 +33035,7 @@
         <v>21</v>
       </c>
       <c r="J9">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="10" spans="1:10">
@@ -33093,7 +33099,7 @@
         <v>340</v>
       </c>
       <c r="J11">
-        <v>200</v>
+        <v>202</v>
       </c>
     </row>
   </sheetData>
@@ -34366,7 +34372,7 @@
         <v>50</v>
       </c>
       <c r="J8">
-        <v>23</v>
+        <v>25</v>
       </c>
     </row>
     <row r="9" spans="1:10">
@@ -34462,7 +34468,7 @@
         <v>494</v>
       </c>
       <c r="J11">
-        <v>240</v>
+        <v>242</v>
       </c>
     </row>
   </sheetData>
@@ -35034,7 +35040,7 @@
         <v>61</v>
       </c>
       <c r="J8">
-        <v>50</v>
+        <v>51</v>
       </c>
     </row>
     <row r="9" spans="1:10">
@@ -35130,7 +35136,7 @@
         <v>406</v>
       </c>
       <c r="J11">
-        <v>278</v>
+        <v>279</v>
       </c>
     </row>
   </sheetData>
@@ -35621,7 +35627,7 @@
         <v>6</v>
       </c>
       <c r="J5">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="6" spans="1:10">
@@ -35781,7 +35787,7 @@
         <v>258</v>
       </c>
       <c r="J10">
-        <v>150</v>
+        <v>151</v>
       </c>
     </row>
   </sheetData>
@@ -36327,7 +36333,7 @@
         <v>19</v>
       </c>
       <c r="J6">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="7" spans="1:10">
@@ -36423,7 +36429,7 @@
         <v>125</v>
       </c>
       <c r="J9">
-        <v>59</v>
+        <v>60</v>
       </c>
     </row>
     <row r="10" spans="1:10">
@@ -36455,7 +36461,7 @@
         <v>905</v>
       </c>
       <c r="J10">
-        <v>450</v>
+        <v>452</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -36487,7 +36493,7 @@
         <v>1669</v>
       </c>
       <c r="J11">
-        <v>902</v>
+        <v>906</v>
       </c>
     </row>
   </sheetData>
@@ -36762,7 +36768,7 @@
         <v>68</v>
       </c>
       <c r="J8">
-        <v>61</v>
+        <v>62</v>
       </c>
     </row>
     <row r="9" spans="1:10">
@@ -36826,7 +36832,7 @@
         <v>157</v>
       </c>
       <c r="J10">
-        <v>86</v>
+        <v>89</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -36858,7 +36864,7 @@
         <v>337</v>
       </c>
       <c r="J11">
-        <v>218</v>
+        <v>222</v>
       </c>
     </row>
   </sheetData>
@@ -37097,7 +37103,7 @@
         <v>15</v>
       </c>
       <c r="J8">
-        <v>20</v>
+        <v>21</v>
       </c>
     </row>
     <row r="9" spans="1:10">
@@ -37193,7 +37199,7 @@
         <v>160</v>
       </c>
       <c r="J11">
-        <v>90</v>
+        <v>91</v>
       </c>
     </row>
   </sheetData>
@@ -37282,7 +37288,7 @@
         <v>17</v>
       </c>
       <c r="J2">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="3" spans="1:10">
@@ -37447,7 +37453,7 @@
         <v>54</v>
       </c>
       <c r="J8">
-        <v>48</v>
+        <v>49</v>
       </c>
     </row>
     <row r="9" spans="1:10">
@@ -37479,7 +37485,7 @@
         <v>8</v>
       </c>
       <c r="J9">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="10" spans="1:10">
@@ -37543,7 +37549,7 @@
         <v>236</v>
       </c>
       <c r="J11">
-        <v>150</v>
+        <v>153</v>
       </c>
     </row>
   </sheetData>
@@ -37716,7 +37722,7 @@
         <v>19</v>
       </c>
       <c r="J5">
-        <v>6</v>
+        <v>8</v>
       </c>
     </row>
     <row r="6" spans="1:10">
@@ -37748,7 +37754,7 @@
         <v>80</v>
       </c>
       <c r="J6">
-        <v>43</v>
+        <v>44</v>
       </c>
     </row>
     <row r="7" spans="1:10">
@@ -37858,7 +37864,7 @@
         <v>717</v>
       </c>
       <c r="J10">
-        <v>318</v>
+        <v>317</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -37890,7 +37896,7 @@
         <v>1066</v>
       </c>
       <c r="J11">
-        <v>465</v>
+        <v>467</v>
       </c>
     </row>
   </sheetData>
@@ -38199,7 +38205,7 @@
         <v>260</v>
       </c>
       <c r="J10">
-        <v>120</v>
+        <v>121</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -38231,7 +38237,7 @@
         <v>393</v>
       </c>
       <c r="J11">
-        <v>170</v>
+        <v>171</v>
       </c>
     </row>
   </sheetData>
@@ -38793,7 +38799,7 @@
         <v>32</v>
       </c>
       <c r="J8">
-        <v>20</v>
+        <v>21</v>
       </c>
     </row>
     <row r="9" spans="1:10">
@@ -38857,7 +38863,7 @@
         <v>225</v>
       </c>
       <c r="J10">
-        <v>107</v>
+        <v>109</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -38889,7 +38895,7 @@
         <v>307</v>
       </c>
       <c r="J11">
-        <v>150</v>
+        <v>153</v>
       </c>
     </row>
   </sheetData>
@@ -39797,7 +39803,7 @@
         <v>155</v>
       </c>
       <c r="J9">
-        <v>89</v>
+        <v>90</v>
       </c>
     </row>
     <row r="10" spans="1:10">
@@ -39829,7 +39835,7 @@
         <v>191</v>
       </c>
       <c r="J10">
-        <v>102</v>
+        <v>103</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add data for 2023-07-18
</commit_message>
<xml_diff>
--- a/output/index-crime-full-year.xlsx
+++ b/output/index-crime-full-year.xlsx
@@ -895,7 +895,7 @@
         <v>7277</v>
       </c>
       <c r="J2">
-        <v>4017</v>
+        <v>4036</v>
       </c>
     </row>
     <row r="3" spans="1:10">
@@ -927,7 +927,7 @@
         <v>7486</v>
       </c>
       <c r="J3">
-        <v>4217</v>
+        <v>4242</v>
       </c>
     </row>
     <row r="4" spans="1:10">
@@ -959,7 +959,7 @@
         <v>422</v>
       </c>
       <c r="J4">
-        <v>269</v>
+        <v>271</v>
       </c>
     </row>
     <row r="5" spans="1:10">
@@ -991,7 +991,7 @@
         <v>7592</v>
       </c>
       <c r="J5">
-        <v>3909</v>
+        <v>3936</v>
       </c>
     </row>
     <row r="6" spans="1:10">
@@ -1002,13 +1002,13 @@
         <v>1679</v>
       </c>
       <c r="C6">
-        <v>1825</v>
+        <v>1827</v>
       </c>
       <c r="D6">
-        <v>1955</v>
+        <v>1956</v>
       </c>
       <c r="E6">
-        <v>1995</v>
+        <v>1996</v>
       </c>
       <c r="F6">
         <v>1888</v>
@@ -1020,10 +1020,10 @@
         <v>1698</v>
       </c>
       <c r="I6">
-        <v>1770</v>
+        <v>1768</v>
       </c>
       <c r="J6">
-        <v>948</v>
+        <v>950</v>
       </c>
     </row>
     <row r="7" spans="1:10">
@@ -1055,7 +1055,7 @@
         <v>718</v>
       </c>
       <c r="J7">
-        <v>335</v>
+        <v>336</v>
       </c>
     </row>
     <row r="8" spans="1:10">
@@ -1087,7 +1087,7 @@
         <v>21445</v>
       </c>
       <c r="J8">
-        <v>15926</v>
+        <v>16009</v>
       </c>
     </row>
     <row r="9" spans="1:10">
@@ -1119,7 +1119,7 @@
         <v>8965</v>
       </c>
       <c r="J9">
-        <v>5022</v>
+        <v>5065</v>
       </c>
     </row>
     <row r="10" spans="1:10">
@@ -1145,13 +1145,13 @@
         <v>41320</v>
       </c>
       <c r="H10">
-        <v>40795</v>
+        <v>40796</v>
       </c>
       <c r="I10">
         <v>54806</v>
       </c>
       <c r="J10">
-        <v>29077</v>
+        <v>29253</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -1162,13 +1162,13 @@
         <v>104361</v>
       </c>
       <c r="C11">
-        <v>116079</v>
+        <v>116081</v>
       </c>
       <c r="D11">
-        <v>117354</v>
+        <v>117355</v>
       </c>
       <c r="E11">
-        <v>113390</v>
+        <v>113391</v>
       </c>
       <c r="F11">
         <v>105560</v>
@@ -1177,13 +1177,13 @@
         <v>85313</v>
       </c>
       <c r="H11">
-        <v>84592</v>
+        <v>84593</v>
       </c>
       <c r="I11">
-        <v>110481</v>
+        <v>110479</v>
       </c>
       <c r="J11">
-        <v>63720</v>
+        <v>64098</v>
       </c>
     </row>
   </sheetData>
@@ -1353,7 +1353,7 @@
         <v>54</v>
       </c>
       <c r="J5">
-        <v>33</v>
+        <v>34</v>
       </c>
     </row>
     <row r="6" spans="1:10">
@@ -1440,7 +1440,7 @@
         <v>227</v>
       </c>
       <c r="J8">
-        <v>199</v>
+        <v>202</v>
       </c>
     </row>
     <row r="9" spans="1:10">
@@ -1472,7 +1472,7 @@
         <v>120</v>
       </c>
       <c r="J9">
-        <v>72</v>
+        <v>73</v>
       </c>
     </row>
     <row r="10" spans="1:10">
@@ -1504,7 +1504,7 @@
         <v>648</v>
       </c>
       <c r="J10">
-        <v>394</v>
+        <v>395</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -1536,7 +1536,7 @@
         <v>1153</v>
       </c>
       <c r="J11">
-        <v>752</v>
+        <v>758</v>
       </c>
     </row>
   </sheetData>
@@ -1931,7 +1931,7 @@
         <v>81</v>
       </c>
       <c r="J3">
-        <v>46</v>
+        <v>48</v>
       </c>
     </row>
     <row r="4" spans="1:10">
@@ -1963,7 +1963,7 @@
         <v>11</v>
       </c>
       <c r="J4">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="5" spans="1:10">
@@ -1995,7 +1995,7 @@
         <v>116</v>
       </c>
       <c r="J5">
-        <v>78</v>
+        <v>79</v>
       </c>
     </row>
     <row r="6" spans="1:10">
@@ -2024,7 +2024,7 @@
         <v>26</v>
       </c>
       <c r="I6">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="J6">
         <v>16</v>
@@ -2091,7 +2091,7 @@
         <v>373</v>
       </c>
       <c r="J8">
-        <v>271</v>
+        <v>273</v>
       </c>
     </row>
     <row r="9" spans="1:10">
@@ -2123,7 +2123,7 @@
         <v>111</v>
       </c>
       <c r="J9">
-        <v>71</v>
+        <v>72</v>
       </c>
     </row>
     <row r="10" spans="1:10">
@@ -2184,10 +2184,10 @@
         <v>1312</v>
       </c>
       <c r="I11">
-        <v>1713</v>
+        <v>1712</v>
       </c>
       <c r="J11">
-        <v>1073</v>
+        <v>1080</v>
       </c>
     </row>
   </sheetData>
@@ -2462,7 +2462,7 @@
         <v>188</v>
       </c>
       <c r="J8">
-        <v>143</v>
+        <v>144</v>
       </c>
     </row>
     <row r="9" spans="1:10">
@@ -2558,7 +2558,7 @@
         <v>1228</v>
       </c>
       <c r="J11">
-        <v>707</v>
+        <v>708</v>
       </c>
     </row>
   </sheetData>
@@ -2647,7 +2647,7 @@
         <v>220</v>
       </c>
       <c r="J2">
-        <v>121</v>
+        <v>123</v>
       </c>
     </row>
     <row r="3" spans="1:10">
@@ -2871,7 +2871,7 @@
         <v>216</v>
       </c>
       <c r="J9">
-        <v>110</v>
+        <v>112</v>
       </c>
     </row>
     <row r="10" spans="1:10">
@@ -2935,7 +2935,7 @@
         <v>2472</v>
       </c>
       <c r="J11">
-        <v>1411</v>
+        <v>1415</v>
       </c>
     </row>
   </sheetData>
@@ -3117,7 +3117,7 @@
         <v>129</v>
       </c>
       <c r="J5">
-        <v>77</v>
+        <v>78</v>
       </c>
     </row>
     <row r="6" spans="1:10">
@@ -3149,7 +3149,7 @@
         <v>21</v>
       </c>
       <c r="J6">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="7" spans="1:10">
@@ -3213,7 +3213,7 @@
         <v>259</v>
       </c>
       <c r="J8">
-        <v>253</v>
+        <v>255</v>
       </c>
     </row>
     <row r="9" spans="1:10">
@@ -3245,7 +3245,7 @@
         <v>151</v>
       </c>
       <c r="J9">
-        <v>78</v>
+        <v>79</v>
       </c>
     </row>
     <row r="10" spans="1:10">
@@ -3277,7 +3277,7 @@
         <v>913</v>
       </c>
       <c r="J10">
-        <v>587</v>
+        <v>589</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -3309,7 +3309,7 @@
         <v>1600</v>
       </c>
       <c r="J11">
-        <v>1063</v>
+        <v>1070</v>
       </c>
     </row>
   </sheetData>
@@ -3648,7 +3648,7 @@
         <v>106</v>
       </c>
       <c r="J10">
-        <v>45</v>
+        <v>46</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -3680,7 +3680,7 @@
         <v>260</v>
       </c>
       <c r="J11">
-        <v>165</v>
+        <v>166</v>
       </c>
     </row>
   </sheetData>
@@ -3993,7 +3993,7 @@
         <v>63</v>
       </c>
       <c r="J9">
-        <v>35</v>
+        <v>36</v>
       </c>
     </row>
     <row r="10" spans="1:10">
@@ -4025,7 +4025,7 @@
         <v>681</v>
       </c>
       <c r="J10">
-        <v>467</v>
+        <v>475</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -4057,7 +4057,7 @@
         <v>1279</v>
       </c>
       <c r="J11">
-        <v>850</v>
+        <v>859</v>
       </c>
     </row>
   </sheetData>
@@ -4146,7 +4146,7 @@
         <v>459</v>
       </c>
       <c r="J2">
-        <v>256</v>
+        <v>258</v>
       </c>
     </row>
     <row r="3" spans="1:10">
@@ -4178,7 +4178,7 @@
         <v>530</v>
       </c>
       <c r="J3">
-        <v>288</v>
+        <v>289</v>
       </c>
     </row>
     <row r="4" spans="1:10">
@@ -4338,7 +4338,7 @@
         <v>794</v>
       </c>
       <c r="J8">
-        <v>591</v>
+        <v>593</v>
       </c>
     </row>
     <row r="9" spans="1:10">
@@ -4370,7 +4370,7 @@
         <v>433</v>
       </c>
       <c r="J9">
-        <v>199</v>
+        <v>200</v>
       </c>
     </row>
     <row r="10" spans="1:10">
@@ -4402,7 +4402,7 @@
         <v>1302</v>
       </c>
       <c r="J10">
-        <v>704</v>
+        <v>711</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -4434,7 +4434,7 @@
         <v>3950</v>
       </c>
       <c r="J11">
-        <v>2296</v>
+        <v>2309</v>
       </c>
     </row>
   </sheetData>
@@ -4697,7 +4697,7 @@
         <v>131</v>
       </c>
       <c r="J8">
-        <v>142</v>
+        <v>145</v>
       </c>
     </row>
     <row r="9" spans="1:10">
@@ -4761,7 +4761,7 @@
         <v>921</v>
       </c>
       <c r="J10">
-        <v>388</v>
+        <v>389</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -4793,7 +4793,7 @@
         <v>1318</v>
       </c>
       <c r="J11">
-        <v>669</v>
+        <v>673</v>
       </c>
     </row>
   </sheetData>
@@ -4882,7 +4882,7 @@
         <v>216</v>
       </c>
       <c r="J2">
-        <v>122</v>
+        <v>123</v>
       </c>
     </row>
     <row r="3" spans="1:10">
@@ -4978,7 +4978,7 @@
         <v>191</v>
       </c>
       <c r="J5">
-        <v>97</v>
+        <v>99</v>
       </c>
     </row>
     <row r="6" spans="1:10">
@@ -5010,7 +5010,7 @@
         <v>58</v>
       </c>
       <c r="J6">
-        <v>29</v>
+        <v>30</v>
       </c>
     </row>
     <row r="7" spans="1:10">
@@ -5074,7 +5074,7 @@
         <v>653</v>
       </c>
       <c r="J8">
-        <v>523</v>
+        <v>526</v>
       </c>
     </row>
     <row r="9" spans="1:10">
@@ -5106,7 +5106,7 @@
         <v>428</v>
       </c>
       <c r="J9">
-        <v>278</v>
+        <v>283</v>
       </c>
     </row>
     <row r="10" spans="1:10">
@@ -5138,7 +5138,7 @@
         <v>1089</v>
       </c>
       <c r="J10">
-        <v>652</v>
+        <v>658</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -5170,7 +5170,7 @@
         <v>2956</v>
       </c>
       <c r="J11">
-        <v>1845</v>
+        <v>1863</v>
       </c>
     </row>
   </sheetData>
@@ -5259,7 +5259,7 @@
         <v>917</v>
       </c>
       <c r="J2">
-        <v>542</v>
+        <v>548</v>
       </c>
     </row>
     <row r="3" spans="1:10">
@@ -5291,7 +5291,7 @@
         <v>155</v>
       </c>
       <c r="J3">
-        <v>97</v>
+        <v>98</v>
       </c>
     </row>
     <row r="4" spans="1:10">
@@ -5323,7 +5323,7 @@
         <v>436</v>
       </c>
       <c r="J4">
-        <v>250</v>
+        <v>252</v>
       </c>
     </row>
     <row r="5" spans="1:10">
@@ -5355,7 +5355,7 @@
         <v>247</v>
       </c>
       <c r="J5">
-        <v>159</v>
+        <v>165</v>
       </c>
     </row>
     <row r="6" spans="1:10">
@@ -5387,7 +5387,7 @@
         <v>793</v>
       </c>
       <c r="J6">
-        <v>551</v>
+        <v>557</v>
       </c>
     </row>
     <row r="7" spans="1:10">
@@ -5419,7 +5419,7 @@
         <v>2685</v>
       </c>
       <c r="J7">
-        <v>1605</v>
+        <v>1609</v>
       </c>
     </row>
     <row r="8" spans="1:10">
@@ -5451,7 +5451,7 @@
         <v>4743</v>
       </c>
       <c r="J8">
-        <v>2703</v>
+        <v>2712</v>
       </c>
     </row>
     <row r="9" spans="1:10">
@@ -5483,7 +5483,7 @@
         <v>519</v>
       </c>
       <c r="J9">
-        <v>298</v>
+        <v>299</v>
       </c>
     </row>
     <row r="10" spans="1:10">
@@ -5515,7 +5515,7 @@
         <v>948</v>
       </c>
       <c r="J10">
-        <v>514</v>
+        <v>516</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -5544,10 +5544,10 @@
         <v>1312</v>
       </c>
       <c r="I11">
-        <v>1713</v>
+        <v>1712</v>
       </c>
       <c r="J11">
-        <v>1073</v>
+        <v>1080</v>
       </c>
     </row>
     <row r="12" spans="1:10">
@@ -5643,7 +5643,7 @@
         <v>718</v>
       </c>
       <c r="J14">
-        <v>341</v>
+        <v>343</v>
       </c>
     </row>
     <row r="15" spans="1:10">
@@ -5675,7 +5675,7 @@
         <v>886</v>
       </c>
       <c r="J15">
-        <v>564</v>
+        <v>565</v>
       </c>
     </row>
     <row r="16" spans="1:10">
@@ -5739,7 +5739,7 @@
         <v>175</v>
       </c>
       <c r="J17">
-        <v>85</v>
+        <v>86</v>
       </c>
     </row>
     <row r="18" spans="1:10">
@@ -5771,7 +5771,7 @@
         <v>695</v>
       </c>
       <c r="J18">
-        <v>423</v>
+        <v>430</v>
       </c>
     </row>
     <row r="19" spans="1:10">
@@ -5803,7 +5803,7 @@
         <v>2636</v>
       </c>
       <c r="J19">
-        <v>1480</v>
+        <v>1497</v>
       </c>
     </row>
     <row r="20" spans="1:10">
@@ -5835,7 +5835,7 @@
         <v>2045</v>
       </c>
       <c r="J20">
-        <v>1061</v>
+        <v>1070</v>
       </c>
     </row>
     <row r="21" spans="1:10">
@@ -5867,7 +5867,7 @@
         <v>337</v>
       </c>
       <c r="J21">
-        <v>145</v>
+        <v>146</v>
       </c>
     </row>
     <row r="22" spans="1:10">
@@ -5899,7 +5899,7 @@
         <v>418</v>
       </c>
       <c r="J22">
-        <v>290</v>
+        <v>293</v>
       </c>
     </row>
     <row r="23" spans="1:10">
@@ -5931,7 +5931,7 @@
         <v>1368</v>
       </c>
       <c r="J23">
-        <v>813</v>
+        <v>814</v>
       </c>
     </row>
     <row r="24" spans="1:10">
@@ -5963,7 +5963,7 @@
         <v>500</v>
       </c>
       <c r="J24">
-        <v>332</v>
+        <v>336</v>
       </c>
     </row>
     <row r="25" spans="1:10">
@@ -5992,10 +5992,10 @@
         <v>325</v>
       </c>
       <c r="I25">
-        <v>430</v>
+        <v>429</v>
       </c>
       <c r="J25">
-        <v>255</v>
+        <v>257</v>
       </c>
     </row>
     <row r="26" spans="1:10">
@@ -6027,7 +6027,7 @@
         <v>248</v>
       </c>
       <c r="J26">
-        <v>161</v>
+        <v>162</v>
       </c>
     </row>
     <row r="27" spans="1:10">
@@ -6059,7 +6059,7 @@
         <v>1258</v>
       </c>
       <c r="J27">
-        <v>756</v>
+        <v>761</v>
       </c>
     </row>
     <row r="28" spans="1:10">
@@ -6123,7 +6123,7 @@
         <v>3950</v>
       </c>
       <c r="J29">
-        <v>2296</v>
+        <v>2309</v>
       </c>
     </row>
     <row r="30" spans="1:10">
@@ -6155,7 +6155,7 @@
         <v>260</v>
       </c>
       <c r="J30">
-        <v>165</v>
+        <v>166</v>
       </c>
     </row>
     <row r="31" spans="1:10">
@@ -6187,7 +6187,7 @@
         <v>867</v>
       </c>
       <c r="J31">
-        <v>472</v>
+        <v>475</v>
       </c>
     </row>
     <row r="32" spans="1:10">
@@ -6251,7 +6251,7 @@
         <v>3011</v>
       </c>
       <c r="J33">
-        <v>1822</v>
+        <v>1831</v>
       </c>
     </row>
     <row r="34" spans="1:10">
@@ -6265,7 +6265,7 @@
         <v>876</v>
       </c>
       <c r="D34">
-        <v>742</v>
+        <v>743</v>
       </c>
       <c r="E34">
         <v>790</v>
@@ -6283,7 +6283,7 @@
         <v>761</v>
       </c>
       <c r="J34">
-        <v>485</v>
+        <v>487</v>
       </c>
     </row>
     <row r="35" spans="1:10">
@@ -6315,7 +6315,7 @@
         <v>235</v>
       </c>
       <c r="J35">
-        <v>132</v>
+        <v>133</v>
       </c>
     </row>
     <row r="36" spans="1:10">
@@ -6347,7 +6347,7 @@
         <v>1491</v>
       </c>
       <c r="J36">
-        <v>912</v>
+        <v>915</v>
       </c>
     </row>
     <row r="37" spans="1:10">
@@ -6379,7 +6379,7 @@
         <v>2547</v>
       </c>
       <c r="J37">
-        <v>1552</v>
+        <v>1558</v>
       </c>
     </row>
     <row r="38" spans="1:10">
@@ -6411,7 +6411,7 @@
         <v>191</v>
       </c>
       <c r="J38">
-        <v>103</v>
+        <v>104</v>
       </c>
     </row>
     <row r="39" spans="1:10">
@@ -6539,7 +6539,7 @@
         <v>2956</v>
       </c>
       <c r="J42">
-        <v>1845</v>
+        <v>1863</v>
       </c>
     </row>
     <row r="43" spans="1:10">
@@ -6571,7 +6571,7 @@
         <v>1153</v>
       </c>
       <c r="J43">
-        <v>752</v>
+        <v>758</v>
       </c>
     </row>
     <row r="44" spans="1:10">
@@ -6603,7 +6603,7 @@
         <v>1228</v>
       </c>
       <c r="J44">
-        <v>707</v>
+        <v>708</v>
       </c>
     </row>
     <row r="45" spans="1:10">
@@ -6667,7 +6667,7 @@
         <v>436</v>
       </c>
       <c r="J46">
-        <v>261</v>
+        <v>264</v>
       </c>
     </row>
     <row r="47" spans="1:10">
@@ -6699,7 +6699,7 @@
         <v>903</v>
       </c>
       <c r="J47">
-        <v>532</v>
+        <v>537</v>
       </c>
     </row>
     <row r="48" spans="1:10">
@@ -6731,7 +6731,7 @@
         <v>2622</v>
       </c>
       <c r="J48">
-        <v>1478</v>
+        <v>1493</v>
       </c>
     </row>
     <row r="49" spans="1:10">
@@ -6763,7 +6763,7 @@
         <v>1648</v>
       </c>
       <c r="J49">
-        <v>908</v>
+        <v>912</v>
       </c>
     </row>
     <row r="50" spans="1:10">
@@ -6806,7 +6806,7 @@
         <v>1044</v>
       </c>
       <c r="C51">
-        <v>1208</v>
+        <v>1209</v>
       </c>
       <c r="D51">
         <v>1258</v>
@@ -6827,7 +6827,7 @@
         <v>1337</v>
       </c>
       <c r="J51">
-        <v>847</v>
+        <v>856</v>
       </c>
     </row>
     <row r="52" spans="1:10">
@@ -6859,7 +6859,7 @@
         <v>1491</v>
       </c>
       <c r="J52">
-        <v>1031</v>
+        <v>1034</v>
       </c>
     </row>
     <row r="53" spans="1:10">
@@ -6891,7 +6891,7 @@
         <v>1600</v>
       </c>
       <c r="J53">
-        <v>1063</v>
+        <v>1070</v>
       </c>
     </row>
     <row r="54" spans="1:10">
@@ -6923,7 +6923,7 @@
         <v>3507</v>
       </c>
       <c r="J54">
-        <v>1939</v>
+        <v>1952</v>
       </c>
     </row>
     <row r="55" spans="1:10">
@@ -6955,7 +6955,7 @@
         <v>1244</v>
       </c>
       <c r="J55">
-        <v>657</v>
+        <v>670</v>
       </c>
     </row>
     <row r="56" spans="1:10">
@@ -6987,7 +6987,7 @@
         <v>628</v>
       </c>
       <c r="J56">
-        <v>322</v>
+        <v>324</v>
       </c>
     </row>
     <row r="57" spans="1:10">
@@ -7019,7 +7019,7 @@
         <v>406</v>
       </c>
       <c r="J57">
-        <v>279</v>
+        <v>281</v>
       </c>
     </row>
     <row r="58" spans="1:10">
@@ -7083,7 +7083,7 @@
         <v>271</v>
       </c>
       <c r="J59">
-        <v>175</v>
+        <v>176</v>
       </c>
     </row>
     <row r="60" spans="1:10">
@@ -7115,7 +7115,7 @@
         <v>768</v>
       </c>
       <c r="J60">
-        <v>466</v>
+        <v>467</v>
       </c>
     </row>
     <row r="61" spans="1:10">
@@ -7190,13 +7190,13 @@
         <v>1473</v>
       </c>
       <c r="C63">
-        <v>1176</v>
+        <v>1177</v>
       </c>
       <c r="D63">
         <v>1522</v>
       </c>
       <c r="E63">
-        <v>2043</v>
+        <v>2044</v>
       </c>
       <c r="F63">
         <v>1326</v>
@@ -7205,13 +7205,13 @@
         <v>1651</v>
       </c>
       <c r="H63">
-        <v>2166</v>
+        <v>2167</v>
       </c>
       <c r="I63">
         <v>2478</v>
       </c>
       <c r="J63">
-        <v>714</v>
+        <v>718</v>
       </c>
     </row>
     <row r="64" spans="1:10">
@@ -7243,7 +7243,7 @@
         <v>1187</v>
       </c>
       <c r="J64">
-        <v>603</v>
+        <v>610</v>
       </c>
     </row>
     <row r="65" spans="1:10">
@@ -7275,7 +7275,7 @@
         <v>1515</v>
       </c>
       <c r="J65">
-        <v>992</v>
+        <v>995</v>
       </c>
     </row>
     <row r="66" spans="1:10">
@@ -7307,7 +7307,7 @@
         <v>715</v>
       </c>
       <c r="J66">
-        <v>427</v>
+        <v>430</v>
       </c>
     </row>
     <row r="67" spans="1:10">
@@ -7339,7 +7339,7 @@
         <v>2510</v>
       </c>
       <c r="J67">
-        <v>1492</v>
+        <v>1498</v>
       </c>
     </row>
     <row r="68" spans="1:10">
@@ -7371,7 +7371,7 @@
         <v>437</v>
       </c>
       <c r="J68">
-        <v>195</v>
+        <v>196</v>
       </c>
     </row>
     <row r="69" spans="1:10">
@@ -7403,7 +7403,7 @@
         <v>494</v>
       </c>
       <c r="J69">
-        <v>242</v>
+        <v>243</v>
       </c>
     </row>
     <row r="70" spans="1:10">
@@ -7435,7 +7435,7 @@
         <v>677</v>
       </c>
       <c r="J70">
-        <v>395</v>
+        <v>402</v>
       </c>
     </row>
     <row r="71" spans="1:10">
@@ -7467,7 +7467,7 @@
         <v>335</v>
       </c>
       <c r="J71">
-        <v>251</v>
+        <v>253</v>
       </c>
     </row>
     <row r="72" spans="1:10">
@@ -7499,7 +7499,7 @@
         <v>706</v>
       </c>
       <c r="J72">
-        <v>373</v>
+        <v>376</v>
       </c>
     </row>
     <row r="73" spans="1:10">
@@ -7531,7 +7531,7 @@
         <v>1279</v>
       </c>
       <c r="J73">
-        <v>850</v>
+        <v>859</v>
       </c>
     </row>
     <row r="74" spans="1:10">
@@ -7627,7 +7627,7 @@
         <v>2923</v>
       </c>
       <c r="J76">
-        <v>1650</v>
+        <v>1658</v>
       </c>
     </row>
     <row r="77" spans="1:10">
@@ -7659,7 +7659,7 @@
         <v>462</v>
       </c>
       <c r="J77">
-        <v>299</v>
+        <v>302</v>
       </c>
     </row>
     <row r="78" spans="1:10">
@@ -7691,7 +7691,7 @@
         <v>1797</v>
       </c>
       <c r="J78">
-        <v>992</v>
+        <v>1001</v>
       </c>
     </row>
     <row r="79" spans="1:10">
@@ -7723,7 +7723,7 @@
         <v>2472</v>
       </c>
       <c r="J79">
-        <v>1411</v>
+        <v>1415</v>
       </c>
     </row>
     <row r="80" spans="1:10">
@@ -7755,7 +7755,7 @@
         <v>393</v>
       </c>
       <c r="J80">
-        <v>171</v>
+        <v>172</v>
       </c>
     </row>
     <row r="81" spans="1:10">
@@ -7851,7 +7851,7 @@
         <v>1793</v>
       </c>
       <c r="J83">
-        <v>985</v>
+        <v>987</v>
       </c>
     </row>
     <row r="84" spans="1:10">
@@ -7883,7 +7883,7 @@
         <v>729</v>
       </c>
       <c r="J84">
-        <v>472</v>
+        <v>476</v>
       </c>
     </row>
     <row r="85" spans="1:10">
@@ -7915,7 +7915,7 @@
         <v>3848</v>
       </c>
       <c r="J85">
-        <v>2322</v>
+        <v>2329</v>
       </c>
     </row>
     <row r="86" spans="1:10">
@@ -7947,7 +7947,7 @@
         <v>1066</v>
       </c>
       <c r="J86">
-        <v>467</v>
+        <v>471</v>
       </c>
     </row>
     <row r="87" spans="1:10">
@@ -7979,7 +7979,7 @@
         <v>396</v>
       </c>
       <c r="J87">
-        <v>220</v>
+        <v>221</v>
       </c>
     </row>
     <row r="88" spans="1:10">
@@ -8043,7 +8043,7 @@
         <v>1879</v>
       </c>
       <c r="J89">
-        <v>1103</v>
+        <v>1108</v>
       </c>
     </row>
     <row r="90" spans="1:10">
@@ -8075,7 +8075,7 @@
         <v>1354</v>
       </c>
       <c r="J90">
-        <v>842</v>
+        <v>844</v>
       </c>
     </row>
     <row r="91" spans="1:10">
@@ -8107,7 +8107,7 @@
         <v>970</v>
       </c>
       <c r="J91">
-        <v>600</v>
+        <v>605</v>
       </c>
     </row>
     <row r="92" spans="1:10">
@@ -8139,7 +8139,7 @@
         <v>337</v>
       </c>
       <c r="J92">
-        <v>222</v>
+        <v>227</v>
       </c>
     </row>
     <row r="93" spans="1:10">
@@ -8171,7 +8171,7 @@
         <v>721</v>
       </c>
       <c r="J93">
-        <v>433</v>
+        <v>435</v>
       </c>
     </row>
     <row r="94" spans="1:10">
@@ -8203,7 +8203,7 @@
         <v>2664</v>
       </c>
       <c r="J94">
-        <v>1357</v>
+        <v>1367</v>
       </c>
     </row>
     <row r="95" spans="1:10">
@@ -8235,7 +8235,7 @@
         <v>1389</v>
       </c>
       <c r="J95">
-        <v>838</v>
+        <v>843</v>
       </c>
     </row>
     <row r="96" spans="1:10">
@@ -8267,7 +8267,7 @@
         <v>1669</v>
       </c>
       <c r="J96">
-        <v>906</v>
+        <v>910</v>
       </c>
     </row>
     <row r="97" spans="1:10">
@@ -8299,7 +8299,7 @@
         <v>1673</v>
       </c>
       <c r="J97">
-        <v>950</v>
+        <v>957</v>
       </c>
     </row>
     <row r="98" spans="1:10">
@@ -8331,7 +8331,7 @@
         <v>1318</v>
       </c>
       <c r="J98">
-        <v>669</v>
+        <v>673</v>
       </c>
     </row>
     <row r="99" spans="1:10">
@@ -8406,13 +8406,13 @@
         <v>104361</v>
       </c>
       <c r="C101">
-        <v>116079</v>
+        <v>116081</v>
       </c>
       <c r="D101">
-        <v>117354</v>
+        <v>117355</v>
       </c>
       <c r="E101">
-        <v>113390</v>
+        <v>113391</v>
       </c>
       <c r="F101">
         <v>105560</v>
@@ -8421,13 +8421,13 @@
         <v>85313</v>
       </c>
       <c r="H101">
-        <v>84592</v>
+        <v>84593</v>
       </c>
       <c r="I101">
-        <v>110481</v>
+        <v>110479</v>
       </c>
       <c r="J101">
-        <v>63720</v>
+        <v>64098</v>
       </c>
     </row>
   </sheetData>
@@ -8618,7 +8618,7 @@
         <v>34</v>
       </c>
       <c r="J2">
-        <v>15</v>
+        <v>16</v>
       </c>
     </row>
     <row r="3" spans="1:10">
@@ -8711,7 +8711,7 @@
         <v>121</v>
       </c>
       <c r="J5">
-        <v>68</v>
+        <v>69</v>
       </c>
     </row>
     <row r="6" spans="1:10">
@@ -8859,7 +8859,7 @@
         <v>1135</v>
       </c>
       <c r="J10">
-        <v>620</v>
+        <v>622</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -8891,7 +8891,7 @@
         <v>1648</v>
       </c>
       <c r="J11">
-        <v>908</v>
+        <v>912</v>
       </c>
     </row>
   </sheetData>
@@ -9012,7 +9012,7 @@
         <v>439</v>
       </c>
       <c r="J3">
-        <v>238</v>
+        <v>240</v>
       </c>
     </row>
     <row r="4" spans="1:10">
@@ -9172,7 +9172,7 @@
         <v>1026</v>
       </c>
       <c r="J8">
-        <v>785</v>
+        <v>786</v>
       </c>
     </row>
     <row r="9" spans="1:10">
@@ -9204,7 +9204,7 @@
         <v>303</v>
       </c>
       <c r="J9">
-        <v>181</v>
+        <v>183</v>
       </c>
     </row>
     <row r="10" spans="1:10">
@@ -9236,7 +9236,7 @@
         <v>1271</v>
       </c>
       <c r="J10">
-        <v>712</v>
+        <v>714</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -9268,7 +9268,7 @@
         <v>3848</v>
       </c>
       <c r="J11">
-        <v>2322</v>
+        <v>2329</v>
       </c>
     </row>
   </sheetData>
@@ -9357,7 +9357,7 @@
         <v>75</v>
       </c>
       <c r="J2">
-        <v>38</v>
+        <v>39</v>
       </c>
     </row>
     <row r="3" spans="1:10">
@@ -9389,7 +9389,7 @@
         <v>80</v>
       </c>
       <c r="J3">
-        <v>41</v>
+        <v>42</v>
       </c>
     </row>
     <row r="4" spans="1:10">
@@ -9578,7 +9578,7 @@
         <v>179</v>
       </c>
       <c r="J9">
-        <v>119</v>
+        <v>121</v>
       </c>
     </row>
     <row r="10" spans="1:10">
@@ -9610,7 +9610,7 @@
         <v>2132</v>
       </c>
       <c r="J10">
-        <v>1189</v>
+        <v>1193</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -9642,7 +9642,7 @@
         <v>2923</v>
       </c>
       <c r="J11">
-        <v>1650</v>
+        <v>1658</v>
       </c>
     </row>
   </sheetData>
@@ -9821,7 +9821,7 @@
         <v>122</v>
       </c>
       <c r="J5">
-        <v>74</v>
+        <v>76</v>
       </c>
     </row>
     <row r="6" spans="1:10">
@@ -9946,7 +9946,7 @@
         <v>156</v>
       </c>
       <c r="J9">
-        <v>65</v>
+        <v>68</v>
       </c>
     </row>
     <row r="10" spans="1:10">
@@ -9978,7 +9978,7 @@
         <v>1034</v>
       </c>
       <c r="J10">
-        <v>474</v>
+        <v>476</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -10010,7 +10010,7 @@
         <v>1673</v>
       </c>
       <c r="J11">
-        <v>950</v>
+        <v>957</v>
       </c>
     </row>
   </sheetData>
@@ -10131,7 +10131,7 @@
         <v>365</v>
       </c>
       <c r="J3">
-        <v>227</v>
+        <v>229</v>
       </c>
     </row>
     <row r="4" spans="1:10">
@@ -10291,7 +10291,7 @@
         <v>516</v>
       </c>
       <c r="J8">
-        <v>385</v>
+        <v>386</v>
       </c>
     </row>
     <row r="9" spans="1:10">
@@ -10323,7 +10323,7 @@
         <v>295</v>
       </c>
       <c r="J9">
-        <v>152</v>
+        <v>153</v>
       </c>
     </row>
     <row r="10" spans="1:10">
@@ -10355,7 +10355,7 @@
         <v>895</v>
       </c>
       <c r="J10">
-        <v>469</v>
+        <v>471</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -10387,7 +10387,7 @@
         <v>2510</v>
       </c>
       <c r="J11">
-        <v>1492</v>
+        <v>1498</v>
       </c>
     </row>
   </sheetData>
@@ -10668,7 +10668,7 @@
         <v>392</v>
       </c>
       <c r="J8">
-        <v>290</v>
+        <v>292</v>
       </c>
     </row>
     <row r="9" spans="1:10">
@@ -10732,7 +10732,7 @@
         <v>433</v>
       </c>
       <c r="J10">
-        <v>274</v>
+        <v>277</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -10764,7 +10764,7 @@
         <v>1389</v>
       </c>
       <c r="J11">
-        <v>838</v>
+        <v>843</v>
       </c>
     </row>
   </sheetData>
@@ -11045,7 +11045,7 @@
         <v>190</v>
       </c>
       <c r="J8">
-        <v>171</v>
+        <v>174</v>
       </c>
     </row>
     <row r="9" spans="1:10">
@@ -11109,7 +11109,7 @@
         <v>271</v>
       </c>
       <c r="J10">
-        <v>143</v>
+        <v>144</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -11141,7 +11141,7 @@
         <v>729</v>
       </c>
       <c r="J11">
-        <v>472</v>
+        <v>476</v>
       </c>
     </row>
   </sheetData>
@@ -11262,7 +11262,7 @@
         <v>190</v>
       </c>
       <c r="J3">
-        <v>111</v>
+        <v>112</v>
       </c>
     </row>
     <row r="4" spans="1:10">
@@ -11422,7 +11422,7 @@
         <v>218</v>
       </c>
       <c r="J8">
-        <v>199</v>
+        <v>200</v>
       </c>
     </row>
     <row r="9" spans="1:10">
@@ -11486,7 +11486,7 @@
         <v>590</v>
       </c>
       <c r="J10">
-        <v>373</v>
+        <v>374</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -11518,7 +11518,7 @@
         <v>1491</v>
       </c>
       <c r="J11">
-        <v>1031</v>
+        <v>1034</v>
       </c>
     </row>
   </sheetData>
@@ -12080,7 +12080,7 @@
         <v>69</v>
       </c>
       <c r="J5">
-        <v>37</v>
+        <v>38</v>
       </c>
     </row>
     <row r="6" spans="1:10">
@@ -12173,7 +12173,7 @@
         <v>401</v>
       </c>
       <c r="J8">
-        <v>226</v>
+        <v>229</v>
       </c>
     </row>
     <row r="9" spans="1:10">
@@ -12205,7 +12205,7 @@
         <v>243</v>
       </c>
       <c r="J9">
-        <v>138</v>
+        <v>141</v>
       </c>
     </row>
     <row r="10" spans="1:10">
@@ -12237,7 +12237,7 @@
         <v>2528</v>
       </c>
       <c r="J10">
-        <v>1392</v>
+        <v>1398</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -12269,7 +12269,7 @@
         <v>3507</v>
       </c>
       <c r="J11">
-        <v>1939</v>
+        <v>1952</v>
       </c>
     </row>
   </sheetData>
@@ -12550,7 +12550,7 @@
         <v>503</v>
       </c>
       <c r="J8">
-        <v>347</v>
+        <v>348</v>
       </c>
     </row>
     <row r="9" spans="1:10">
@@ -12614,7 +12614,7 @@
         <v>527</v>
       </c>
       <c r="J10">
-        <v>313</v>
+        <v>315</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -12646,7 +12646,7 @@
         <v>1491</v>
       </c>
       <c r="J11">
-        <v>912</v>
+        <v>915</v>
       </c>
     </row>
   </sheetData>
@@ -12927,7 +12927,7 @@
         <v>722</v>
       </c>
       <c r="J8">
-        <v>494</v>
+        <v>495</v>
       </c>
     </row>
     <row r="9" spans="1:10">
@@ -12991,7 +12991,7 @@
         <v>813</v>
       </c>
       <c r="J10">
-        <v>458</v>
+        <v>463</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -13023,7 +13023,7 @@
         <v>2547</v>
       </c>
       <c r="J11">
-        <v>1552</v>
+        <v>1558</v>
       </c>
     </row>
   </sheetData>
@@ -13112,7 +13112,7 @@
         <v>30</v>
       </c>
       <c r="J2">
-        <v>19</v>
+        <v>20</v>
       </c>
     </row>
     <row r="3" spans="1:10">
@@ -13283,7 +13283,7 @@
         <v>90</v>
       </c>
       <c r="J8">
-        <v>95</v>
+        <v>96</v>
       </c>
     </row>
     <row r="9" spans="1:10">
@@ -13347,7 +13347,7 @@
         <v>213</v>
       </c>
       <c r="J10">
-        <v>131</v>
+        <v>132</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -13379,7 +13379,7 @@
         <v>418</v>
       </c>
       <c r="J11">
-        <v>290</v>
+        <v>293</v>
       </c>
     </row>
   </sheetData>
@@ -13709,7 +13709,7 @@
         <v>448</v>
       </c>
       <c r="J10">
-        <v>217</v>
+        <v>220</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -13741,7 +13741,7 @@
         <v>706</v>
       </c>
       <c r="J11">
-        <v>373</v>
+        <v>376</v>
       </c>
     </row>
   </sheetData>
@@ -13830,7 +13830,7 @@
         <v>194</v>
       </c>
       <c r="J2">
-        <v>109</v>
+        <v>110</v>
       </c>
     </row>
     <row r="3" spans="1:10">
@@ -13926,7 +13926,7 @@
         <v>107</v>
       </c>
       <c r="J5">
-        <v>49</v>
+        <v>50</v>
       </c>
     </row>
     <row r="6" spans="1:10">
@@ -14086,7 +14086,7 @@
         <v>587</v>
       </c>
       <c r="J10">
-        <v>333</v>
+        <v>334</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -14118,7 +14118,7 @@
         <v>1515</v>
       </c>
       <c r="J11">
-        <v>992</v>
+        <v>995</v>
       </c>
     </row>
   </sheetData>
@@ -14577,7 +14577,7 @@
         <v>42</v>
       </c>
       <c r="J3">
-        <v>27</v>
+        <v>28</v>
       </c>
     </row>
     <row r="4" spans="1:10">
@@ -14830,7 +14830,7 @@
         <v>768</v>
       </c>
       <c r="J11">
-        <v>466</v>
+        <v>467</v>
       </c>
     </row>
   </sheetData>
@@ -15096,7 +15096,7 @@
         <v>57</v>
       </c>
       <c r="J8">
-        <v>34</v>
+        <v>35</v>
       </c>
     </row>
     <row r="9" spans="1:10">
@@ -15192,7 +15192,7 @@
         <v>437</v>
       </c>
       <c r="J11">
-        <v>195</v>
+        <v>196</v>
       </c>
     </row>
   </sheetData>
@@ -15377,7 +15377,7 @@
         <v>124</v>
       </c>
       <c r="J5">
-        <v>51</v>
+        <v>52</v>
       </c>
     </row>
     <row r="6" spans="1:10">
@@ -15537,7 +15537,7 @@
         <v>612</v>
       </c>
       <c r="J10">
-        <v>325</v>
+        <v>326</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -15569,7 +15569,7 @@
         <v>1793</v>
       </c>
       <c r="J11">
-        <v>985</v>
+        <v>987</v>
       </c>
     </row>
   </sheetData>
@@ -15658,7 +15658,7 @@
         <v>92</v>
       </c>
       <c r="J2">
-        <v>40</v>
+        <v>41</v>
       </c>
     </row>
     <row r="3" spans="1:10">
@@ -15754,7 +15754,7 @@
         <v>90</v>
       </c>
       <c r="J5">
-        <v>44</v>
+        <v>45</v>
       </c>
     </row>
     <row r="6" spans="1:10">
@@ -15850,7 +15850,7 @@
         <v>224</v>
       </c>
       <c r="J8">
-        <v>168</v>
+        <v>169</v>
       </c>
     </row>
     <row r="9" spans="1:10">
@@ -15882,7 +15882,7 @@
         <v>109</v>
       </c>
       <c r="J9">
-        <v>83</v>
+        <v>89</v>
       </c>
     </row>
     <row r="10" spans="1:10">
@@ -15914,7 +15914,7 @@
         <v>610</v>
       </c>
       <c r="J10">
-        <v>273</v>
+        <v>277</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -15946,7 +15946,7 @@
         <v>1244</v>
       </c>
       <c r="J11">
-        <v>657</v>
+        <v>670</v>
       </c>
     </row>
   </sheetData>
@@ -16212,7 +16212,7 @@
         <v>294</v>
       </c>
       <c r="J8">
-        <v>206</v>
+        <v>209</v>
       </c>
     </row>
     <row r="9" spans="1:10">
@@ -16244,7 +16244,7 @@
         <v>147</v>
       </c>
       <c r="J9">
-        <v>69</v>
+        <v>70</v>
       </c>
     </row>
     <row r="10" spans="1:10">
@@ -16276,7 +16276,7 @@
         <v>2021</v>
       </c>
       <c r="J10">
-        <v>965</v>
+        <v>971</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -16308,7 +16308,7 @@
         <v>2664</v>
       </c>
       <c r="J11">
-        <v>1357</v>
+        <v>1367</v>
       </c>
     </row>
   </sheetData>
@@ -16397,7 +16397,7 @@
         <v>267</v>
       </c>
       <c r="J2">
-        <v>172</v>
+        <v>174</v>
       </c>
     </row>
     <row r="3" spans="1:10">
@@ -16589,7 +16589,7 @@
         <v>707</v>
       </c>
       <c r="J8">
-        <v>548</v>
+        <v>552</v>
       </c>
     </row>
     <row r="9" spans="1:10">
@@ -16621,7 +16621,7 @@
         <v>363</v>
       </c>
       <c r="J9">
-        <v>212</v>
+        <v>214</v>
       </c>
     </row>
     <row r="10" spans="1:10">
@@ -16653,7 +16653,7 @@
         <v>968</v>
       </c>
       <c r="J10">
-        <v>535</v>
+        <v>536</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -16685,7 +16685,7 @@
         <v>3011</v>
       </c>
       <c r="J11">
-        <v>1822</v>
+        <v>1831</v>
       </c>
     </row>
   </sheetData>
@@ -16806,7 +16806,7 @@
         <v>248</v>
       </c>
       <c r="J3">
-        <v>124</v>
+        <v>125</v>
       </c>
     </row>
     <row r="4" spans="1:10">
@@ -16966,7 +16966,7 @@
         <v>567</v>
       </c>
       <c r="J8">
-        <v>547</v>
+        <v>548</v>
       </c>
     </row>
     <row r="9" spans="1:10">
@@ -16998,7 +16998,7 @@
         <v>226</v>
       </c>
       <c r="J9">
-        <v>142</v>
+        <v>143</v>
       </c>
     </row>
     <row r="10" spans="1:10">
@@ -17030,7 +17030,7 @@
         <v>1023</v>
       </c>
       <c r="J10">
-        <v>499</v>
+        <v>500</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -17062,7 +17062,7 @@
         <v>2685</v>
       </c>
       <c r="J11">
-        <v>1605</v>
+        <v>1609</v>
       </c>
     </row>
   </sheetData>
@@ -17151,7 +17151,7 @@
         <v>457</v>
       </c>
       <c r="J2">
-        <v>272</v>
+        <v>273</v>
       </c>
     </row>
     <row r="3" spans="1:10">
@@ -17183,7 +17183,7 @@
         <v>445</v>
       </c>
       <c r="J3">
-        <v>296</v>
+        <v>298</v>
       </c>
     </row>
     <row r="4" spans="1:10">
@@ -17343,7 +17343,7 @@
         <v>1269</v>
       </c>
       <c r="J8">
-        <v>728</v>
+        <v>729</v>
       </c>
     </row>
     <row r="9" spans="1:10">
@@ -17375,7 +17375,7 @@
         <v>497</v>
       </c>
       <c r="J9">
-        <v>296</v>
+        <v>298</v>
       </c>
     </row>
     <row r="10" spans="1:10">
@@ -17407,7 +17407,7 @@
         <v>1652</v>
       </c>
       <c r="J10">
-        <v>891</v>
+        <v>894</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -17439,7 +17439,7 @@
         <v>4743</v>
       </c>
       <c r="J11">
-        <v>2703</v>
+        <v>2712</v>
       </c>
     </row>
   </sheetData>
@@ -17720,7 +17720,7 @@
         <v>441</v>
       </c>
       <c r="J8">
-        <v>331</v>
+        <v>332</v>
       </c>
     </row>
     <row r="9" spans="1:10">
@@ -17784,7 +17784,7 @@
         <v>455</v>
       </c>
       <c r="J10">
-        <v>291</v>
+        <v>292</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -17816,7 +17816,7 @@
         <v>1354</v>
       </c>
       <c r="J11">
-        <v>842</v>
+        <v>844</v>
       </c>
     </row>
   </sheetData>
@@ -18027,7 +18027,7 @@
         <v>13</v>
       </c>
       <c r="J6">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="7" spans="1:10">
@@ -18152,7 +18152,7 @@
         <v>417</v>
       </c>
       <c r="J10">
-        <v>225</v>
+        <v>229</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -18184,7 +18184,7 @@
         <v>903</v>
       </c>
       <c r="J11">
-        <v>532</v>
+        <v>537</v>
       </c>
     </row>
   </sheetData>
@@ -18273,7 +18273,7 @@
         <v>237</v>
       </c>
       <c r="J2">
-        <v>107</v>
+        <v>110</v>
       </c>
     </row>
     <row r="3" spans="1:10">
@@ -18305,7 +18305,7 @@
         <v>212</v>
       </c>
       <c r="J3">
-        <v>118</v>
+        <v>120</v>
       </c>
     </row>
     <row r="4" spans="1:10">
@@ -18369,7 +18369,7 @@
         <v>229</v>
       </c>
       <c r="J5">
-        <v>99</v>
+        <v>100</v>
       </c>
     </row>
     <row r="6" spans="1:10">
@@ -18433,7 +18433,7 @@
         <v>23</v>
       </c>
       <c r="J7">
-        <v>18</v>
+        <v>19</v>
       </c>
     </row>
     <row r="8" spans="1:10">
@@ -18465,7 +18465,7 @@
         <v>754</v>
       </c>
       <c r="J8">
-        <v>420</v>
+        <v>422</v>
       </c>
     </row>
     <row r="9" spans="1:10">
@@ -18497,7 +18497,7 @@
         <v>233</v>
       </c>
       <c r="J9">
-        <v>156</v>
+        <v>160</v>
       </c>
     </row>
     <row r="10" spans="1:10">
@@ -18529,7 +18529,7 @@
         <v>911</v>
       </c>
       <c r="J10">
-        <v>529</v>
+        <v>533</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -18561,7 +18561,7 @@
         <v>2636</v>
       </c>
       <c r="J11">
-        <v>1480</v>
+        <v>1497</v>
       </c>
     </row>
   </sheetData>
@@ -18650,7 +18650,7 @@
         <v>22</v>
       </c>
       <c r="J2">
-        <v>14</v>
+        <v>15</v>
       </c>
     </row>
     <row r="3" spans="1:10">
@@ -18682,7 +18682,7 @@
         <v>19</v>
       </c>
       <c r="J3">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="4" spans="1:10">
@@ -18815,7 +18815,7 @@
         <v>49</v>
       </c>
       <c r="J8">
-        <v>53</v>
+        <v>55</v>
       </c>
     </row>
     <row r="9" spans="1:10">
@@ -18879,7 +18879,7 @@
         <v>94</v>
       </c>
       <c r="J10">
-        <v>55</v>
+        <v>57</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -18911,7 +18911,7 @@
         <v>247</v>
       </c>
       <c r="J11">
-        <v>159</v>
+        <v>165</v>
       </c>
     </row>
   </sheetData>
@@ -19032,7 +19032,7 @@
         <v>177</v>
       </c>
       <c r="J3">
-        <v>96</v>
+        <v>98</v>
       </c>
     </row>
     <row r="4" spans="1:10">
@@ -19192,7 +19192,7 @@
         <v>363</v>
       </c>
       <c r="J8">
-        <v>274</v>
+        <v>276</v>
       </c>
     </row>
     <row r="9" spans="1:10">
@@ -19256,7 +19256,7 @@
         <v>828</v>
       </c>
       <c r="J10">
-        <v>414</v>
+        <v>419</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -19288,7 +19288,7 @@
         <v>2045</v>
       </c>
       <c r="J11">
-        <v>1061</v>
+        <v>1070</v>
       </c>
     </row>
   </sheetData>
@@ -19919,7 +19919,7 @@
         <v>68</v>
       </c>
       <c r="J8">
-        <v>58</v>
+        <v>59</v>
       </c>
     </row>
     <row r="9" spans="1:10">
@@ -20015,7 +20015,7 @@
         <v>271</v>
       </c>
       <c r="J11">
-        <v>175</v>
+        <v>176</v>
       </c>
     </row>
   </sheetData>
@@ -20104,7 +20104,7 @@
         <v>87</v>
       </c>
       <c r="J2">
-        <v>52</v>
+        <v>53</v>
       </c>
     </row>
     <row r="3" spans="1:10">
@@ -20136,7 +20136,7 @@
         <v>98</v>
       </c>
       <c r="J3">
-        <v>72</v>
+        <v>73</v>
       </c>
     </row>
     <row r="4" spans="1:10">
@@ -20296,7 +20296,7 @@
         <v>308</v>
       </c>
       <c r="J8">
-        <v>221</v>
+        <v>222</v>
       </c>
     </row>
     <row r="9" spans="1:10">
@@ -20328,7 +20328,7 @@
         <v>77</v>
       </c>
       <c r="J9">
-        <v>29</v>
+        <v>30</v>
       </c>
     </row>
     <row r="10" spans="1:10">
@@ -20360,7 +20360,7 @@
         <v>320</v>
       </c>
       <c r="J10">
-        <v>177</v>
+        <v>178</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -20392,7 +20392,7 @@
         <v>970</v>
       </c>
       <c r="J11">
-        <v>600</v>
+        <v>605</v>
       </c>
     </row>
   </sheetData>
@@ -20577,7 +20577,7 @@
         <v>64</v>
       </c>
       <c r="J5">
-        <v>46</v>
+        <v>47</v>
       </c>
     </row>
     <row r="6" spans="1:10">
@@ -20731,7 +20731,7 @@
         <v>381</v>
       </c>
       <c r="J10">
-        <v>191</v>
+        <v>192</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -20763,7 +20763,7 @@
         <v>721</v>
       </c>
       <c r="J11">
-        <v>433</v>
+        <v>435</v>
       </c>
     </row>
   </sheetData>
@@ -20936,7 +20936,7 @@
         <v>50</v>
       </c>
       <c r="J5">
-        <v>28</v>
+        <v>29</v>
       </c>
     </row>
     <row r="6" spans="1:10">
@@ -21087,7 +21087,7 @@
         <v>280</v>
       </c>
       <c r="J10">
-        <v>136</v>
+        <v>138</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -21119,7 +21119,7 @@
         <v>436</v>
       </c>
       <c r="J11">
-        <v>261</v>
+        <v>264</v>
       </c>
     </row>
   </sheetData>
@@ -21455,7 +21455,7 @@
         <v>216</v>
       </c>
       <c r="J10">
-        <v>117</v>
+        <v>119</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -21487,7 +21487,7 @@
         <v>436</v>
       </c>
       <c r="J11">
-        <v>250</v>
+        <v>252</v>
       </c>
     </row>
   </sheetData>
@@ -21576,7 +21576,7 @@
         <v>64</v>
       </c>
       <c r="J2">
-        <v>46</v>
+        <v>47</v>
       </c>
     </row>
     <row r="3" spans="1:10">
@@ -21669,7 +21669,7 @@
         <v>67</v>
       </c>
       <c r="J5">
-        <v>37</v>
+        <v>39</v>
       </c>
     </row>
     <row r="6" spans="1:10">
@@ -21680,7 +21680,7 @@
         <v>17</v>
       </c>
       <c r="C6">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="D6">
         <v>33</v>
@@ -21701,7 +21701,7 @@
         <v>27</v>
       </c>
       <c r="J6">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="7" spans="1:10">
@@ -21765,7 +21765,7 @@
         <v>297</v>
       </c>
       <c r="J8">
-        <v>269</v>
+        <v>271</v>
       </c>
     </row>
     <row r="9" spans="1:10">
@@ -21797,7 +21797,7 @@
         <v>121</v>
       </c>
       <c r="J9">
-        <v>66</v>
+        <v>67</v>
       </c>
     </row>
     <row r="10" spans="1:10">
@@ -21829,7 +21829,7 @@
         <v>670</v>
       </c>
       <c r="J10">
-        <v>345</v>
+        <v>349</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -21840,7 +21840,7 @@
         <v>1044</v>
       </c>
       <c r="C11">
-        <v>1208</v>
+        <v>1209</v>
       </c>
       <c r="D11">
         <v>1258</v>
@@ -21861,7 +21861,7 @@
         <v>1337</v>
       </c>
       <c r="J11">
-        <v>847</v>
+        <v>856</v>
       </c>
     </row>
   </sheetData>
@@ -22142,7 +22142,7 @@
         <v>125</v>
       </c>
       <c r="J8">
-        <v>76</v>
+        <v>77</v>
       </c>
     </row>
     <row r="9" spans="1:10">
@@ -22174,7 +22174,7 @@
         <v>46</v>
       </c>
       <c r="J9">
-        <v>34</v>
+        <v>35</v>
       </c>
     </row>
     <row r="10" spans="1:10">
@@ -22206,7 +22206,7 @@
         <v>492</v>
       </c>
       <c r="J10">
-        <v>310</v>
+        <v>314</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -22238,7 +22238,7 @@
         <v>917</v>
       </c>
       <c r="J11">
-        <v>542</v>
+        <v>548</v>
       </c>
     </row>
   </sheetData>
@@ -22741,7 +22741,7 @@
         <v>5</v>
       </c>
       <c r="J4">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="5" spans="1:10">
@@ -22866,7 +22866,7 @@
         <v>196</v>
       </c>
       <c r="J8">
-        <v>120</v>
+        <v>124</v>
       </c>
     </row>
     <row r="9" spans="1:10">
@@ -22930,7 +22930,7 @@
         <v>239</v>
       </c>
       <c r="J10">
-        <v>137</v>
+        <v>139</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -22962,7 +22962,7 @@
         <v>695</v>
       </c>
       <c r="J11">
-        <v>423</v>
+        <v>430</v>
       </c>
     </row>
   </sheetData>
@@ -23231,7 +23231,7 @@
         <v>92</v>
       </c>
       <c r="J8">
-        <v>93</v>
+        <v>95</v>
       </c>
     </row>
     <row r="9" spans="1:10">
@@ -23295,7 +23295,7 @@
         <v>277</v>
       </c>
       <c r="J10">
-        <v>166</v>
+        <v>168</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -23327,7 +23327,7 @@
         <v>500</v>
       </c>
       <c r="J11">
-        <v>332</v>
+        <v>336</v>
       </c>
     </row>
   </sheetData>
@@ -23509,7 +23509,7 @@
         <v>34</v>
       </c>
       <c r="J5">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="6" spans="1:10">
@@ -23538,7 +23538,7 @@
         <v>7</v>
       </c>
       <c r="I6">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="J6">
         <v>6</v>
@@ -23669,7 +23669,7 @@
         <v>189</v>
       </c>
       <c r="J10">
-        <v>123</v>
+        <v>124</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -23698,10 +23698,10 @@
         <v>325</v>
       </c>
       <c r="I11">
-        <v>430</v>
+        <v>429</v>
       </c>
       <c r="J11">
-        <v>255</v>
+        <v>257</v>
       </c>
     </row>
   </sheetData>
@@ -23822,7 +23822,7 @@
         <v>47</v>
       </c>
       <c r="J3">
-        <v>31</v>
+        <v>33</v>
       </c>
     </row>
     <row r="4" spans="1:10">
@@ -23883,7 +23883,7 @@
         <v>77</v>
       </c>
       <c r="J5">
-        <v>33</v>
+        <v>34</v>
       </c>
     </row>
     <row r="6" spans="1:10">
@@ -24043,7 +24043,7 @@
         <v>349</v>
       </c>
       <c r="J10">
-        <v>213</v>
+        <v>216</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -24075,7 +24075,7 @@
         <v>793</v>
       </c>
       <c r="J11">
-        <v>551</v>
+        <v>557</v>
       </c>
     </row>
   </sheetData>
@@ -24376,7 +24376,7 @@
         <v>41</v>
       </c>
       <c r="J9">
-        <v>27</v>
+        <v>28</v>
       </c>
     </row>
     <row r="10" spans="1:10">
@@ -24440,7 +24440,7 @@
         <v>396</v>
       </c>
       <c r="J11">
-        <v>220</v>
+        <v>221</v>
       </c>
     </row>
   </sheetData>
@@ -24529,7 +24529,7 @@
         <v>61</v>
       </c>
       <c r="J2">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="3" spans="1:10">
@@ -24619,7 +24619,7 @@
         <v>82</v>
       </c>
       <c r="J5">
-        <v>72</v>
+        <v>73</v>
       </c>
     </row>
     <row r="6" spans="1:10">
@@ -24651,7 +24651,7 @@
         <v>29</v>
       </c>
       <c r="J6">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="7" spans="1:10">
@@ -24709,7 +24709,7 @@
         <v>167</v>
       </c>
       <c r="J8">
-        <v>116</v>
+        <v>120</v>
       </c>
     </row>
     <row r="9" spans="1:10">
@@ -24773,7 +24773,7 @@
         <v>784</v>
       </c>
       <c r="J10">
-        <v>482</v>
+        <v>484</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -24805,7 +24805,7 @@
         <v>1258</v>
       </c>
       <c r="J11">
-        <v>756</v>
+        <v>761</v>
       </c>
     </row>
   </sheetData>
@@ -24926,7 +24926,7 @@
         <v>67</v>
       </c>
       <c r="J3">
-        <v>35</v>
+        <v>36</v>
       </c>
     </row>
     <row r="4" spans="1:10">
@@ -25150,7 +25150,7 @@
         <v>381</v>
       </c>
       <c r="J10">
-        <v>197</v>
+        <v>199</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -25182,7 +25182,7 @@
         <v>867</v>
       </c>
       <c r="J11">
-        <v>472</v>
+        <v>475</v>
       </c>
     </row>
   </sheetData>
@@ -25479,7 +25479,7 @@
         <v>576</v>
       </c>
       <c r="J10">
-        <v>300</v>
+        <v>302</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -25511,7 +25511,7 @@
         <v>628</v>
       </c>
       <c r="J11">
-        <v>322</v>
+        <v>324</v>
       </c>
     </row>
   </sheetData>
@@ -25600,7 +25600,7 @@
         <v>53</v>
       </c>
       <c r="J2">
-        <v>42</v>
+        <v>43</v>
       </c>
     </row>
     <row r="3" spans="1:10">
@@ -25856,7 +25856,7 @@
         <v>130</v>
       </c>
       <c r="J10">
-        <v>82</v>
+        <v>84</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -25888,7 +25888,7 @@
         <v>462</v>
       </c>
       <c r="J11">
-        <v>299</v>
+        <v>302</v>
       </c>
     </row>
   </sheetData>
@@ -26397,7 +26397,7 @@
         <v>130</v>
       </c>
       <c r="J5">
-        <v>55</v>
+        <v>56</v>
       </c>
     </row>
     <row r="6" spans="1:10">
@@ -26493,7 +26493,7 @@
         <v>198</v>
       </c>
       <c r="J8">
-        <v>152</v>
+        <v>156</v>
       </c>
     </row>
     <row r="9" spans="1:10">
@@ -26557,7 +26557,7 @@
         <v>1118</v>
       </c>
       <c r="J10">
-        <v>583</v>
+        <v>587</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -26589,7 +26589,7 @@
         <v>1797</v>
       </c>
       <c r="J11">
-        <v>992</v>
+        <v>1001</v>
       </c>
     </row>
   </sheetData>
@@ -26710,7 +26710,7 @@
         <v>36</v>
       </c>
       <c r="J3">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="4" spans="1:10">
@@ -26925,7 +26925,7 @@
         <v>371</v>
       </c>
       <c r="J10">
-        <v>152</v>
+        <v>153</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -26957,7 +26957,7 @@
         <v>718</v>
       </c>
       <c r="J11">
-        <v>341</v>
+        <v>343</v>
       </c>
     </row>
   </sheetData>
@@ -27130,7 +27130,7 @@
         <v>74</v>
       </c>
       <c r="J5">
-        <v>58</v>
+        <v>59</v>
       </c>
     </row>
     <row r="6" spans="1:10">
@@ -27272,7 +27272,7 @@
         <v>462</v>
       </c>
       <c r="J10">
-        <v>246</v>
+        <v>248</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -27304,7 +27304,7 @@
         <v>715</v>
       </c>
       <c r="J11">
-        <v>427</v>
+        <v>430</v>
       </c>
     </row>
   </sheetData>
@@ -27929,7 +27929,7 @@
         <v>141</v>
       </c>
       <c r="J8">
-        <v>101</v>
+        <v>102</v>
       </c>
     </row>
     <row r="9" spans="1:10">
@@ -28025,7 +28025,7 @@
         <v>519</v>
       </c>
       <c r="J11">
-        <v>298</v>
+        <v>299</v>
       </c>
     </row>
   </sheetData>
@@ -28279,7 +28279,7 @@
         <v>39</v>
       </c>
       <c r="J8">
-        <v>34</v>
+        <v>35</v>
       </c>
     </row>
     <row r="9" spans="1:10">
@@ -28375,7 +28375,7 @@
         <v>175</v>
       </c>
       <c r="J11">
-        <v>85</v>
+        <v>86</v>
       </c>
     </row>
   </sheetData>
@@ -28717,7 +28717,7 @@
         <v>542</v>
       </c>
       <c r="J10">
-        <v>288</v>
+        <v>290</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -28749,7 +28749,7 @@
         <v>948</v>
       </c>
       <c r="J11">
-        <v>514</v>
+        <v>516</v>
       </c>
     </row>
   </sheetData>
@@ -29305,7 +29305,7 @@
         <v>131</v>
       </c>
       <c r="J5">
-        <v>73</v>
+        <v>74</v>
       </c>
     </row>
     <row r="6" spans="1:10">
@@ -29398,7 +29398,7 @@
         <v>216</v>
       </c>
       <c r="J8">
-        <v>188</v>
+        <v>189</v>
       </c>
     </row>
     <row r="9" spans="1:10">
@@ -29462,7 +29462,7 @@
         <v>1222</v>
       </c>
       <c r="J10">
-        <v>655</v>
+        <v>658</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -29494,7 +29494,7 @@
         <v>1879</v>
       </c>
       <c r="J11">
-        <v>1103</v>
+        <v>1108</v>
       </c>
     </row>
   </sheetData>
@@ -29693,7 +29693,7 @@
         <v>16</v>
       </c>
       <c r="D6">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="E6">
         <v>12</v>
@@ -29836,7 +29836,7 @@
         <v>440</v>
       </c>
       <c r="J10">
-        <v>256</v>
+        <v>258</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -29850,7 +29850,7 @@
         <v>876</v>
       </c>
       <c r="D11">
-        <v>742</v>
+        <v>743</v>
       </c>
       <c r="E11">
         <v>790</v>
@@ -29868,7 +29868,7 @@
         <v>761</v>
       </c>
       <c r="J11">
-        <v>485</v>
+        <v>487</v>
       </c>
     </row>
   </sheetData>
@@ -29957,7 +29957,7 @@
         <v>128</v>
       </c>
       <c r="J2">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="3" spans="1:10">
@@ -30213,7 +30213,7 @@
         <v>527</v>
       </c>
       <c r="J10">
-        <v>311</v>
+        <v>312</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -30548,7 +30548,7 @@
         <v>152</v>
       </c>
       <c r="J10">
-        <v>75</v>
+        <v>76</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -30580,7 +30580,7 @@
         <v>248</v>
       </c>
       <c r="J11">
-        <v>161</v>
+        <v>162</v>
       </c>
     </row>
   </sheetData>
@@ -30825,7 +30825,7 @@
         <v>112</v>
       </c>
       <c r="J8">
-        <v>70</v>
+        <v>71</v>
       </c>
     </row>
     <row r="9" spans="1:10">
@@ -30889,7 +30889,7 @@
         <v>502</v>
       </c>
       <c r="J10">
-        <v>298</v>
+        <v>304</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -30921,7 +30921,7 @@
         <v>677</v>
       </c>
       <c r="J11">
-        <v>395</v>
+        <v>402</v>
       </c>
     </row>
   </sheetData>
@@ -31522,7 +31522,7 @@
         <v>123</v>
       </c>
       <c r="J8">
-        <v>124</v>
+        <v>125</v>
       </c>
     </row>
     <row r="9" spans="1:10">
@@ -31586,7 +31586,7 @@
         <v>124</v>
       </c>
       <c r="J10">
-        <v>73</v>
+        <v>74</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -31618,7 +31618,7 @@
         <v>335</v>
       </c>
       <c r="J11">
-        <v>251</v>
+        <v>253</v>
       </c>
     </row>
   </sheetData>
@@ -31963,7 +31963,7 @@
         <v>389</v>
       </c>
       <c r="J10">
-        <v>248</v>
+        <v>249</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -31995,7 +31995,7 @@
         <v>886</v>
       </c>
       <c r="J11">
-        <v>564</v>
+        <v>565</v>
       </c>
     </row>
   </sheetData>
@@ -32174,7 +32174,7 @@
         <v>39</v>
       </c>
       <c r="J5">
-        <v>19</v>
+        <v>20</v>
       </c>
     </row>
     <row r="6" spans="1:10">
@@ -32366,7 +32366,7 @@
         <v>1368</v>
       </c>
       <c r="J11">
-        <v>813</v>
+        <v>814</v>
       </c>
     </row>
   </sheetData>
@@ -32551,7 +32551,7 @@
         <v>180</v>
       </c>
       <c r="J5">
-        <v>81</v>
+        <v>83</v>
       </c>
     </row>
     <row r="6" spans="1:10">
@@ -32641,7 +32641,7 @@
         <v>338</v>
       </c>
       <c r="J8">
-        <v>252</v>
+        <v>254</v>
       </c>
     </row>
     <row r="9" spans="1:10">
@@ -32673,7 +32673,7 @@
         <v>169</v>
       </c>
       <c r="J9">
-        <v>77</v>
+        <v>79</v>
       </c>
     </row>
     <row r="10" spans="1:10">
@@ -32705,7 +32705,7 @@
         <v>1773</v>
       </c>
       <c r="J10">
-        <v>987</v>
+        <v>996</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -32737,7 +32737,7 @@
         <v>2622</v>
       </c>
       <c r="J11">
-        <v>1478</v>
+        <v>1493</v>
       </c>
     </row>
   </sheetData>
@@ -33341,7 +33341,7 @@
         <v>36</v>
       </c>
       <c r="J8">
-        <v>26</v>
+        <v>27</v>
       </c>
     </row>
     <row r="9" spans="1:10">
@@ -33437,7 +33437,7 @@
         <v>337</v>
       </c>
       <c r="J11">
-        <v>145</v>
+        <v>146</v>
       </c>
     </row>
   </sheetData>
@@ -33526,7 +33526,7 @@
         <v>58</v>
       </c>
       <c r="J2">
-        <v>27</v>
+        <v>28</v>
       </c>
     </row>
     <row r="3" spans="1:10">
@@ -33709,7 +33709,7 @@
         <v>334</v>
       </c>
       <c r="J8">
-        <v>188</v>
+        <v>189</v>
       </c>
     </row>
     <row r="9" spans="1:10">
@@ -33773,7 +33773,7 @@
         <v>606</v>
       </c>
       <c r="J10">
-        <v>284</v>
+        <v>289</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -33805,7 +33805,7 @@
         <v>1187</v>
       </c>
       <c r="J11">
-        <v>603</v>
+        <v>610</v>
       </c>
     </row>
   </sheetData>
@@ -34436,7 +34436,7 @@
         <v>313</v>
       </c>
       <c r="J10">
-        <v>142</v>
+        <v>143</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -34468,7 +34468,7 @@
         <v>494</v>
       </c>
       <c r="J11">
-        <v>242</v>
+        <v>243</v>
       </c>
     </row>
   </sheetData>
@@ -34620,7 +34620,7 @@
         <v>12</v>
       </c>
       <c r="J5">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="6" spans="1:10">
@@ -34771,7 +34771,7 @@
         <v>155</v>
       </c>
       <c r="J10">
-        <v>97</v>
+        <v>98</v>
       </c>
     </row>
   </sheetData>
@@ -35040,7 +35040,7 @@
         <v>61</v>
       </c>
       <c r="J8">
-        <v>51</v>
+        <v>52</v>
       </c>
     </row>
     <row r="9" spans="1:10">
@@ -35104,7 +35104,7 @@
         <v>211</v>
       </c>
       <c r="J10">
-        <v>141</v>
+        <v>142</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -35136,7 +35136,7 @@
         <v>406</v>
       </c>
       <c r="J11">
-        <v>279</v>
+        <v>281</v>
       </c>
     </row>
   </sheetData>
@@ -36205,7 +36205,7 @@
         <v>89</v>
       </c>
       <c r="J2">
-        <v>48</v>
+        <v>50</v>
       </c>
     </row>
     <row r="3" spans="1:10">
@@ -36461,7 +36461,7 @@
         <v>905</v>
       </c>
       <c r="J10">
-        <v>452</v>
+        <v>454</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -36493,7 +36493,7 @@
         <v>1669</v>
       </c>
       <c r="J11">
-        <v>906</v>
+        <v>910</v>
       </c>
     </row>
   </sheetData>
@@ -36768,7 +36768,7 @@
         <v>68</v>
       </c>
       <c r="J8">
-        <v>62</v>
+        <v>64</v>
       </c>
     </row>
     <row r="9" spans="1:10">
@@ -36832,7 +36832,7 @@
         <v>157</v>
       </c>
       <c r="J10">
-        <v>89</v>
+        <v>92</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -36864,7 +36864,7 @@
         <v>337</v>
       </c>
       <c r="J11">
-        <v>222</v>
+        <v>227</v>
       </c>
     </row>
   </sheetData>
@@ -37670,7 +37670,7 @@
         <v>15</v>
       </c>
       <c r="J3">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="4" spans="1:10">
@@ -37800,7 +37800,7 @@
         <v>160</v>
       </c>
       <c r="J8">
-        <v>60</v>
+        <v>61</v>
       </c>
     </row>
     <row r="9" spans="1:10">
@@ -37864,7 +37864,7 @@
         <v>717</v>
       </c>
       <c r="J10">
-        <v>317</v>
+        <v>319</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -37896,7 +37896,7 @@
         <v>1066</v>
       </c>
       <c r="J11">
-        <v>467</v>
+        <v>471</v>
       </c>
     </row>
   </sheetData>
@@ -38141,7 +38141,7 @@
         <v>39</v>
       </c>
       <c r="J8">
-        <v>17</v>
+        <v>18</v>
       </c>
     </row>
     <row r="9" spans="1:10">
@@ -38237,7 +38237,7 @@
         <v>393</v>
       </c>
       <c r="J11">
-        <v>171</v>
+        <v>172</v>
       </c>
     </row>
   </sheetData>
@@ -39503,7 +39503,7 @@
         <v>174</v>
       </c>
       <c r="J10">
-        <v>90</v>
+        <v>91</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -39535,7 +39535,7 @@
         <v>235</v>
       </c>
       <c r="J11">
-        <v>132</v>
+        <v>133</v>
       </c>
     </row>
   </sheetData>
@@ -39803,7 +39803,7 @@
         <v>155</v>
       </c>
       <c r="J9">
-        <v>90</v>
+        <v>91</v>
       </c>
     </row>
     <row r="10" spans="1:10">
@@ -39835,7 +39835,7 @@
         <v>191</v>
       </c>
       <c r="J10">
-        <v>103</v>
+        <v>104</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add data for 2023-07-21
</commit_message>
<xml_diff>
--- a/output/index-crime-full-year.xlsx
+++ b/output/index-crime-full-year.xlsx
@@ -895,7 +895,7 @@
         <v>7277</v>
       </c>
       <c r="J2">
-        <v>4082</v>
+        <v>4113</v>
       </c>
     </row>
     <row r="3" spans="1:10">
@@ -927,7 +927,7 @@
         <v>7486</v>
       </c>
       <c r="J3">
-        <v>4303</v>
+        <v>4318</v>
       </c>
     </row>
     <row r="4" spans="1:10">
@@ -976,7 +976,7 @@
         <v>13001</v>
       </c>
       <c r="E5">
-        <v>11746</v>
+        <v>11747</v>
       </c>
       <c r="F5">
         <v>9638</v>
@@ -991,7 +991,7 @@
         <v>7592</v>
       </c>
       <c r="J5">
-        <v>3989</v>
+        <v>4008</v>
       </c>
     </row>
     <row r="6" spans="1:10">
@@ -1002,13 +1002,13 @@
         <v>1679</v>
       </c>
       <c r="C6">
-        <v>1827</v>
+        <v>1828</v>
       </c>
       <c r="D6">
         <v>1957</v>
       </c>
       <c r="E6">
-        <v>1996</v>
+        <v>1997</v>
       </c>
       <c r="F6">
         <v>1888</v>
@@ -1020,10 +1020,10 @@
         <v>1698</v>
       </c>
       <c r="I6">
-        <v>1767</v>
+        <v>1768</v>
       </c>
       <c r="J6">
-        <v>961</v>
+        <v>971</v>
       </c>
     </row>
     <row r="7" spans="1:10">
@@ -1055,7 +1055,7 @@
         <v>718</v>
       </c>
       <c r="J7">
-        <v>340</v>
+        <v>343</v>
       </c>
     </row>
     <row r="8" spans="1:10">
@@ -1084,10 +1084,10 @@
         <v>10602</v>
       </c>
       <c r="I8">
-        <v>21445</v>
+        <v>21446</v>
       </c>
       <c r="J8">
-        <v>16184</v>
+        <v>16280</v>
       </c>
     </row>
     <row r="9" spans="1:10">
@@ -1119,7 +1119,7 @@
         <v>8965</v>
       </c>
       <c r="J9">
-        <v>5117</v>
+        <v>5149</v>
       </c>
     </row>
     <row r="10" spans="1:10">
@@ -1148,10 +1148,10 @@
         <v>40796</v>
       </c>
       <c r="I10">
-        <v>54807</v>
+        <v>54808</v>
       </c>
       <c r="J10">
-        <v>29618</v>
+        <v>29792</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -1162,13 +1162,13 @@
         <v>104361</v>
       </c>
       <c r="C11">
-        <v>116081</v>
+        <v>116082</v>
       </c>
       <c r="D11">
         <v>117356</v>
       </c>
       <c r="E11">
-        <v>113390</v>
+        <v>113392</v>
       </c>
       <c r="F11">
         <v>105560</v>
@@ -1180,10 +1180,10 @@
         <v>84594</v>
       </c>
       <c r="I11">
-        <v>110479</v>
+        <v>110482</v>
       </c>
       <c r="J11">
-        <v>64868</v>
+        <v>65248</v>
       </c>
     </row>
   </sheetData>
@@ -1440,7 +1440,7 @@
         <v>227</v>
       </c>
       <c r="J8">
-        <v>209</v>
+        <v>210</v>
       </c>
     </row>
     <row r="9" spans="1:10">
@@ -1472,7 +1472,7 @@
         <v>120</v>
       </c>
       <c r="J9">
-        <v>73</v>
+        <v>74</v>
       </c>
     </row>
     <row r="10" spans="1:10">
@@ -1504,7 +1504,7 @@
         <v>648</v>
       </c>
       <c r="J10">
-        <v>398</v>
+        <v>402</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -1536,7 +1536,7 @@
         <v>1153</v>
       </c>
       <c r="J11">
-        <v>768</v>
+        <v>774</v>
       </c>
     </row>
   </sheetData>
@@ -1899,7 +1899,7 @@
         <v>154</v>
       </c>
       <c r="J2">
-        <v>79</v>
+        <v>80</v>
       </c>
     </row>
     <row r="3" spans="1:10">
@@ -2091,7 +2091,7 @@
         <v>373</v>
       </c>
       <c r="J8">
-        <v>277</v>
+        <v>280</v>
       </c>
     </row>
     <row r="9" spans="1:10">
@@ -2155,7 +2155,7 @@
         <v>820</v>
       </c>
       <c r="J10">
-        <v>504</v>
+        <v>509</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -2187,7 +2187,7 @@
         <v>1712</v>
       </c>
       <c r="J11">
-        <v>1094</v>
+        <v>1103</v>
       </c>
     </row>
   </sheetData>
@@ -2276,7 +2276,7 @@
         <v>64</v>
       </c>
       <c r="J2">
-        <v>35</v>
+        <v>36</v>
       </c>
     </row>
     <row r="3" spans="1:10">
@@ -2526,7 +2526,7 @@
         <v>712</v>
       </c>
       <c r="J10">
-        <v>400</v>
+        <v>403</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -2558,7 +2558,7 @@
         <v>1228</v>
       </c>
       <c r="J11">
-        <v>719</v>
+        <v>723</v>
       </c>
     </row>
   </sheetData>
@@ -2647,7 +2647,7 @@
         <v>220</v>
       </c>
       <c r="J2">
-        <v>123</v>
+        <v>124</v>
       </c>
     </row>
     <row r="3" spans="1:10">
@@ -2679,7 +2679,7 @@
         <v>244</v>
       </c>
       <c r="J3">
-        <v>154</v>
+        <v>155</v>
       </c>
     </row>
     <row r="4" spans="1:10">
@@ -2839,7 +2839,7 @@
         <v>700</v>
       </c>
       <c r="J8">
-        <v>472</v>
+        <v>475</v>
       </c>
     </row>
     <row r="9" spans="1:10">
@@ -2903,7 +2903,7 @@
         <v>820</v>
       </c>
       <c r="J10">
-        <v>438</v>
+        <v>439</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -2935,7 +2935,7 @@
         <v>2472</v>
       </c>
       <c r="J11">
-        <v>1429</v>
+        <v>1435</v>
       </c>
     </row>
   </sheetData>
@@ -3024,7 +3024,7 @@
         <v>61</v>
       </c>
       <c r="J2">
-        <v>40</v>
+        <v>41</v>
       </c>
     </row>
     <row r="3" spans="1:10">
@@ -3056,7 +3056,7 @@
         <v>56</v>
       </c>
       <c r="J3">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="4" spans="1:10">
@@ -3277,7 +3277,7 @@
         <v>913</v>
       </c>
       <c r="J10">
-        <v>597</v>
+        <v>599</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -3309,7 +3309,7 @@
         <v>1600</v>
       </c>
       <c r="J11">
-        <v>1087</v>
+        <v>1091</v>
       </c>
     </row>
   </sheetData>
@@ -3769,7 +3769,7 @@
         <v>74</v>
       </c>
       <c r="J2">
-        <v>50</v>
+        <v>51</v>
       </c>
     </row>
     <row r="3" spans="1:10">
@@ -3865,7 +3865,7 @@
         <v>139</v>
       </c>
       <c r="J5">
-        <v>69</v>
+        <v>70</v>
       </c>
     </row>
     <row r="6" spans="1:10">
@@ -3897,7 +3897,7 @@
         <v>24</v>
       </c>
       <c r="J6">
-        <v>9</v>
+        <v>11</v>
       </c>
     </row>
     <row r="7" spans="1:10">
@@ -3961,7 +3961,7 @@
         <v>220</v>
       </c>
       <c r="J8">
-        <v>188</v>
+        <v>193</v>
       </c>
     </row>
     <row r="9" spans="1:10">
@@ -4025,7 +4025,7 @@
         <v>681</v>
       </c>
       <c r="J10">
-        <v>483</v>
+        <v>488</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -4057,7 +4057,7 @@
         <v>1279</v>
       </c>
       <c r="J11">
-        <v>873</v>
+        <v>887</v>
       </c>
     </row>
   </sheetData>
@@ -4146,7 +4146,7 @@
         <v>459</v>
       </c>
       <c r="J2">
-        <v>261</v>
+        <v>264</v>
       </c>
     </row>
     <row r="3" spans="1:10">
@@ -4178,7 +4178,7 @@
         <v>530</v>
       </c>
       <c r="J3">
-        <v>291</v>
+        <v>293</v>
       </c>
     </row>
     <row r="4" spans="1:10">
@@ -4306,7 +4306,7 @@
         <v>49</v>
       </c>
       <c r="J7">
-        <v>35</v>
+        <v>36</v>
       </c>
     </row>
     <row r="8" spans="1:10">
@@ -4338,7 +4338,7 @@
         <v>794</v>
       </c>
       <c r="J8">
-        <v>598</v>
+        <v>600</v>
       </c>
     </row>
     <row r="9" spans="1:10">
@@ -4370,7 +4370,7 @@
         <v>433</v>
       </c>
       <c r="J9">
-        <v>201</v>
+        <v>202</v>
       </c>
     </row>
     <row r="10" spans="1:10">
@@ -4402,7 +4402,7 @@
         <v>1302</v>
       </c>
       <c r="J10">
-        <v>716</v>
+        <v>720</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -4434,7 +4434,7 @@
         <v>3950</v>
       </c>
       <c r="J11">
-        <v>2327</v>
+        <v>2340</v>
       </c>
     </row>
   </sheetData>
@@ -4761,7 +4761,7 @@
         <v>921</v>
       </c>
       <c r="J10">
-        <v>393</v>
+        <v>394</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -4793,7 +4793,7 @@
         <v>1318</v>
       </c>
       <c r="J11">
-        <v>677</v>
+        <v>678</v>
       </c>
     </row>
   </sheetData>
@@ -5074,7 +5074,7 @@
         <v>653</v>
       </c>
       <c r="J8">
-        <v>532</v>
+        <v>535</v>
       </c>
     </row>
     <row r="9" spans="1:10">
@@ -5106,7 +5106,7 @@
         <v>428</v>
       </c>
       <c r="J9">
-        <v>284</v>
+        <v>286</v>
       </c>
     </row>
     <row r="10" spans="1:10">
@@ -5138,7 +5138,7 @@
         <v>1089</v>
       </c>
       <c r="J10">
-        <v>667</v>
+        <v>674</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -5170,7 +5170,7 @@
         <v>2956</v>
       </c>
       <c r="J11">
-        <v>1881</v>
+        <v>1893</v>
       </c>
     </row>
   </sheetData>
@@ -5259,7 +5259,7 @@
         <v>917</v>
       </c>
       <c r="J2">
-        <v>553</v>
+        <v>556</v>
       </c>
     </row>
     <row r="3" spans="1:10">
@@ -5323,7 +5323,7 @@
         <v>436</v>
       </c>
       <c r="J4">
-        <v>253</v>
+        <v>254</v>
       </c>
     </row>
     <row r="5" spans="1:10">
@@ -5387,7 +5387,7 @@
         <v>793</v>
       </c>
       <c r="J6">
-        <v>565</v>
+        <v>566</v>
       </c>
     </row>
     <row r="7" spans="1:10">
@@ -5416,10 +5416,10 @@
         <v>2237</v>
       </c>
       <c r="I7">
-        <v>2685</v>
+        <v>2686</v>
       </c>
       <c r="J7">
-        <v>1626</v>
+        <v>1644</v>
       </c>
     </row>
     <row r="8" spans="1:10">
@@ -5451,7 +5451,7 @@
         <v>4743</v>
       </c>
       <c r="J8">
-        <v>2748</v>
+        <v>2763</v>
       </c>
     </row>
     <row r="9" spans="1:10">
@@ -5515,7 +5515,7 @@
         <v>948</v>
       </c>
       <c r="J10">
-        <v>526</v>
+        <v>530</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -5547,7 +5547,7 @@
         <v>1712</v>
       </c>
       <c r="J11">
-        <v>1094</v>
+        <v>1103</v>
       </c>
     </row>
     <row r="12" spans="1:10">
@@ -5611,7 +5611,7 @@
         <v>258</v>
       </c>
       <c r="J13">
-        <v>151</v>
+        <v>152</v>
       </c>
     </row>
     <row r="14" spans="1:10">
@@ -5643,7 +5643,7 @@
         <v>718</v>
       </c>
       <c r="J14">
-        <v>346</v>
+        <v>348</v>
       </c>
     </row>
     <row r="15" spans="1:10">
@@ -5675,7 +5675,7 @@
         <v>886</v>
       </c>
       <c r="J15">
-        <v>577</v>
+        <v>579</v>
       </c>
     </row>
     <row r="16" spans="1:10">
@@ -5707,7 +5707,7 @@
         <v>595</v>
       </c>
       <c r="J16">
-        <v>422</v>
+        <v>425</v>
       </c>
     </row>
     <row r="17" spans="1:10">
@@ -5771,7 +5771,7 @@
         <v>695</v>
       </c>
       <c r="J18">
-        <v>433</v>
+        <v>434</v>
       </c>
     </row>
     <row r="19" spans="1:10">
@@ -5803,7 +5803,7 @@
         <v>2636</v>
       </c>
       <c r="J19">
-        <v>1514</v>
+        <v>1521</v>
       </c>
     </row>
     <row r="20" spans="1:10">
@@ -5835,7 +5835,7 @@
         <v>2045</v>
       </c>
       <c r="J20">
-        <v>1083</v>
+        <v>1086</v>
       </c>
     </row>
     <row r="21" spans="1:10">
@@ -5867,7 +5867,7 @@
         <v>337</v>
       </c>
       <c r="J21">
-        <v>146</v>
+        <v>150</v>
       </c>
     </row>
     <row r="22" spans="1:10">
@@ -5899,7 +5899,7 @@
         <v>418</v>
       </c>
       <c r="J22">
-        <v>297</v>
+        <v>298</v>
       </c>
     </row>
     <row r="23" spans="1:10">
@@ -5931,7 +5931,7 @@
         <v>1368</v>
       </c>
       <c r="J23">
-        <v>824</v>
+        <v>828</v>
       </c>
     </row>
     <row r="24" spans="1:10">
@@ -6027,7 +6027,7 @@
         <v>248</v>
       </c>
       <c r="J26">
-        <v>163</v>
+        <v>165</v>
       </c>
     </row>
     <row r="27" spans="1:10">
@@ -6059,7 +6059,7 @@
         <v>1258</v>
       </c>
       <c r="J27">
-        <v>768</v>
+        <v>773</v>
       </c>
     </row>
     <row r="28" spans="1:10">
@@ -6123,7 +6123,7 @@
         <v>3950</v>
       </c>
       <c r="J29">
-        <v>2327</v>
+        <v>2340</v>
       </c>
     </row>
     <row r="30" spans="1:10">
@@ -6187,7 +6187,7 @@
         <v>867</v>
       </c>
       <c r="J31">
-        <v>481</v>
+        <v>483</v>
       </c>
     </row>
     <row r="32" spans="1:10">
@@ -6251,7 +6251,7 @@
         <v>3011</v>
       </c>
       <c r="J33">
-        <v>1855</v>
+        <v>1867</v>
       </c>
     </row>
     <row r="34" spans="1:10">
@@ -6283,7 +6283,7 @@
         <v>761</v>
       </c>
       <c r="J34">
-        <v>492</v>
+        <v>496</v>
       </c>
     </row>
     <row r="35" spans="1:10">
@@ -6315,7 +6315,7 @@
         <v>235</v>
       </c>
       <c r="J35">
-        <v>132</v>
+        <v>135</v>
       </c>
     </row>
     <row r="36" spans="1:10">
@@ -6347,7 +6347,7 @@
         <v>1491</v>
       </c>
       <c r="J36">
-        <v>926</v>
+        <v>933</v>
       </c>
     </row>
     <row r="37" spans="1:10">
@@ -6379,7 +6379,7 @@
         <v>2547</v>
       </c>
       <c r="J37">
-        <v>1577</v>
+        <v>1582</v>
       </c>
     </row>
     <row r="38" spans="1:10">
@@ -6411,7 +6411,7 @@
         <v>191</v>
       </c>
       <c r="J38">
-        <v>106</v>
+        <v>107</v>
       </c>
     </row>
     <row r="39" spans="1:10">
@@ -6475,7 +6475,7 @@
         <v>236</v>
       </c>
       <c r="J40">
-        <v>153</v>
+        <v>154</v>
       </c>
     </row>
     <row r="41" spans="1:10">
@@ -6507,7 +6507,7 @@
         <v>437</v>
       </c>
       <c r="J41">
-        <v>314</v>
+        <v>320</v>
       </c>
     </row>
     <row r="42" spans="1:10">
@@ -6539,7 +6539,7 @@
         <v>2956</v>
       </c>
       <c r="J42">
-        <v>1881</v>
+        <v>1893</v>
       </c>
     </row>
     <row r="43" spans="1:10">
@@ -6571,7 +6571,7 @@
         <v>1153</v>
       </c>
       <c r="J43">
-        <v>768</v>
+        <v>774</v>
       </c>
     </row>
     <row r="44" spans="1:10">
@@ -6603,7 +6603,7 @@
         <v>1228</v>
       </c>
       <c r="J44">
-        <v>719</v>
+        <v>723</v>
       </c>
     </row>
     <row r="45" spans="1:10">
@@ -6635,7 +6635,7 @@
         <v>181</v>
       </c>
       <c r="J45">
-        <v>84</v>
+        <v>85</v>
       </c>
     </row>
     <row r="46" spans="1:10">
@@ -6667,7 +6667,7 @@
         <v>436</v>
       </c>
       <c r="J46">
-        <v>269</v>
+        <v>270</v>
       </c>
     </row>
     <row r="47" spans="1:10">
@@ -6699,7 +6699,7 @@
         <v>903</v>
       </c>
       <c r="J47">
-        <v>546</v>
+        <v>548</v>
       </c>
     </row>
     <row r="48" spans="1:10">
@@ -6731,7 +6731,7 @@
         <v>2622</v>
       </c>
       <c r="J48">
-        <v>1510</v>
+        <v>1518</v>
       </c>
     </row>
     <row r="49" spans="1:10">
@@ -6763,7 +6763,7 @@
         <v>1648</v>
       </c>
       <c r="J49">
-        <v>929</v>
+        <v>933</v>
       </c>
     </row>
     <row r="50" spans="1:10">
@@ -6795,7 +6795,7 @@
         <v>960</v>
       </c>
       <c r="J50">
-        <v>555</v>
+        <v>558</v>
       </c>
     </row>
     <row r="51" spans="1:10">
@@ -6827,7 +6827,7 @@
         <v>1337</v>
       </c>
       <c r="J51">
-        <v>865</v>
+        <v>871</v>
       </c>
     </row>
     <row r="52" spans="1:10">
@@ -6859,7 +6859,7 @@
         <v>1491</v>
       </c>
       <c r="J52">
-        <v>1039</v>
+        <v>1044</v>
       </c>
     </row>
     <row r="53" spans="1:10">
@@ -6891,7 +6891,7 @@
         <v>1600</v>
       </c>
       <c r="J53">
-        <v>1087</v>
+        <v>1091</v>
       </c>
     </row>
     <row r="54" spans="1:10">
@@ -6923,7 +6923,7 @@
         <v>3507</v>
       </c>
       <c r="J54">
-        <v>1970</v>
+        <v>1988</v>
       </c>
     </row>
     <row r="55" spans="1:10">
@@ -6955,7 +6955,7 @@
         <v>1244</v>
       </c>
       <c r="J55">
-        <v>682</v>
+        <v>690</v>
       </c>
     </row>
     <row r="56" spans="1:10">
@@ -6987,7 +6987,7 @@
         <v>628</v>
       </c>
       <c r="J56">
-        <v>328</v>
+        <v>330</v>
       </c>
     </row>
     <row r="57" spans="1:10">
@@ -7019,7 +7019,7 @@
         <v>406</v>
       </c>
       <c r="J57">
-        <v>284</v>
+        <v>286</v>
       </c>
     </row>
     <row r="58" spans="1:10">
@@ -7051,7 +7051,7 @@
         <v>390</v>
       </c>
       <c r="J58">
-        <v>65</v>
+        <v>66</v>
       </c>
     </row>
     <row r="59" spans="1:10">
@@ -7083,7 +7083,7 @@
         <v>271</v>
       </c>
       <c r="J59">
-        <v>176</v>
+        <v>178</v>
       </c>
     </row>
     <row r="60" spans="1:10">
@@ -7115,7 +7115,7 @@
         <v>768</v>
       </c>
       <c r="J60">
-        <v>470</v>
+        <v>471</v>
       </c>
     </row>
     <row r="61" spans="1:10">
@@ -7190,13 +7190,13 @@
         <v>1473</v>
       </c>
       <c r="C63">
-        <v>1177</v>
+        <v>1178</v>
       </c>
       <c r="D63">
         <v>1523</v>
       </c>
       <c r="E63">
-        <v>2044</v>
+        <v>2046</v>
       </c>
       <c r="F63">
         <v>1326</v>
@@ -7208,10 +7208,10 @@
         <v>2167</v>
       </c>
       <c r="I63">
-        <v>2479</v>
+        <v>2481</v>
       </c>
       <c r="J63">
-        <v>726</v>
+        <v>729</v>
       </c>
     </row>
     <row r="64" spans="1:10">
@@ -7243,7 +7243,7 @@
         <v>1187</v>
       </c>
       <c r="J64">
-        <v>627</v>
+        <v>630</v>
       </c>
     </row>
     <row r="65" spans="1:10">
@@ -7275,7 +7275,7 @@
         <v>1515</v>
       </c>
       <c r="J65">
-        <v>1007</v>
+        <v>1014</v>
       </c>
     </row>
     <row r="66" spans="1:10">
@@ -7307,7 +7307,7 @@
         <v>715</v>
       </c>
       <c r="J66">
-        <v>432</v>
+        <v>433</v>
       </c>
     </row>
     <row r="67" spans="1:10">
@@ -7339,7 +7339,7 @@
         <v>2510</v>
       </c>
       <c r="J67">
-        <v>1519</v>
+        <v>1524</v>
       </c>
     </row>
     <row r="68" spans="1:10">
@@ -7371,7 +7371,7 @@
         <v>437</v>
       </c>
       <c r="J68">
-        <v>200</v>
+        <v>201</v>
       </c>
     </row>
     <row r="69" spans="1:10">
@@ -7403,7 +7403,7 @@
         <v>494</v>
       </c>
       <c r="J69">
-        <v>244</v>
+        <v>246</v>
       </c>
     </row>
     <row r="70" spans="1:10">
@@ -7435,7 +7435,7 @@
         <v>677</v>
       </c>
       <c r="J70">
-        <v>407</v>
+        <v>410</v>
       </c>
     </row>
     <row r="71" spans="1:10">
@@ -7467,7 +7467,7 @@
         <v>335</v>
       </c>
       <c r="J71">
-        <v>254</v>
+        <v>255</v>
       </c>
     </row>
     <row r="72" spans="1:10">
@@ -7499,7 +7499,7 @@
         <v>706</v>
       </c>
       <c r="J72">
-        <v>383</v>
+        <v>385</v>
       </c>
     </row>
     <row r="73" spans="1:10">
@@ -7531,7 +7531,7 @@
         <v>1279</v>
       </c>
       <c r="J73">
-        <v>873</v>
+        <v>887</v>
       </c>
     </row>
     <row r="74" spans="1:10">
@@ -7563,7 +7563,7 @@
         <v>307</v>
       </c>
       <c r="J74">
-        <v>156</v>
+        <v>157</v>
       </c>
     </row>
     <row r="75" spans="1:10">
@@ -7627,7 +7627,7 @@
         <v>2923</v>
       </c>
       <c r="J76">
-        <v>1673</v>
+        <v>1686</v>
       </c>
     </row>
     <row r="77" spans="1:10">
@@ -7691,7 +7691,7 @@
         <v>1797</v>
       </c>
       <c r="J78">
-        <v>1014</v>
+        <v>1018</v>
       </c>
     </row>
     <row r="79" spans="1:10">
@@ -7723,7 +7723,7 @@
         <v>2472</v>
       </c>
       <c r="J79">
-        <v>1429</v>
+        <v>1435</v>
       </c>
     </row>
     <row r="80" spans="1:10">
@@ -7755,7 +7755,7 @@
         <v>393</v>
       </c>
       <c r="J80">
-        <v>175</v>
+        <v>178</v>
       </c>
     </row>
     <row r="81" spans="1:10">
@@ -7787,7 +7787,7 @@
         <v>219</v>
       </c>
       <c r="J81">
-        <v>123</v>
+        <v>125</v>
       </c>
     </row>
     <row r="82" spans="1:10">
@@ -7819,7 +7819,7 @@
         <v>233</v>
       </c>
       <c r="J82">
-        <v>153</v>
+        <v>154</v>
       </c>
     </row>
     <row r="83" spans="1:10">
@@ -7851,7 +7851,7 @@
         <v>1793</v>
       </c>
       <c r="J83">
-        <v>997</v>
+        <v>1000</v>
       </c>
     </row>
     <row r="84" spans="1:10">
@@ -7883,7 +7883,7 @@
         <v>729</v>
       </c>
       <c r="J84">
-        <v>480</v>
+        <v>482</v>
       </c>
     </row>
     <row r="85" spans="1:10">
@@ -7915,7 +7915,7 @@
         <v>3848</v>
       </c>
       <c r="J85">
-        <v>2360</v>
+        <v>2374</v>
       </c>
     </row>
     <row r="86" spans="1:10">
@@ -7947,7 +7947,7 @@
         <v>1066</v>
       </c>
       <c r="J86">
-        <v>480</v>
+        <v>486</v>
       </c>
     </row>
     <row r="87" spans="1:10">
@@ -7979,7 +7979,7 @@
         <v>396</v>
       </c>
       <c r="J87">
-        <v>225</v>
+        <v>226</v>
       </c>
     </row>
     <row r="88" spans="1:10">
@@ -8011,7 +8011,7 @@
         <v>943</v>
       </c>
       <c r="J88">
-        <v>576</v>
+        <v>577</v>
       </c>
     </row>
     <row r="89" spans="1:10">
@@ -8043,7 +8043,7 @@
         <v>1879</v>
       </c>
       <c r="J89">
-        <v>1130</v>
+        <v>1141</v>
       </c>
     </row>
     <row r="90" spans="1:10">
@@ -8075,7 +8075,7 @@
         <v>1354</v>
       </c>
       <c r="J90">
-        <v>852</v>
+        <v>853</v>
       </c>
     </row>
     <row r="91" spans="1:10">
@@ -8107,7 +8107,7 @@
         <v>970</v>
       </c>
       <c r="J91">
-        <v>613</v>
+        <v>616</v>
       </c>
     </row>
     <row r="92" spans="1:10">
@@ -8139,7 +8139,7 @@
         <v>337</v>
       </c>
       <c r="J92">
-        <v>230</v>
+        <v>231</v>
       </c>
     </row>
     <row r="93" spans="1:10">
@@ -8171,7 +8171,7 @@
         <v>721</v>
       </c>
       <c r="J93">
-        <v>437</v>
+        <v>442</v>
       </c>
     </row>
     <row r="94" spans="1:10">
@@ -8203,7 +8203,7 @@
         <v>2663</v>
       </c>
       <c r="J94">
-        <v>1386</v>
+        <v>1390</v>
       </c>
     </row>
     <row r="95" spans="1:10">
@@ -8235,7 +8235,7 @@
         <v>1389</v>
       </c>
       <c r="J95">
-        <v>847</v>
+        <v>851</v>
       </c>
     </row>
     <row r="96" spans="1:10">
@@ -8267,7 +8267,7 @@
         <v>1669</v>
       </c>
       <c r="J96">
-        <v>921</v>
+        <v>928</v>
       </c>
     </row>
     <row r="97" spans="1:10">
@@ -8299,7 +8299,7 @@
         <v>1673</v>
       </c>
       <c r="J97">
-        <v>970</v>
+        <v>974</v>
       </c>
     </row>
     <row r="98" spans="1:10">
@@ -8331,7 +8331,7 @@
         <v>1318</v>
       </c>
       <c r="J98">
-        <v>677</v>
+        <v>678</v>
       </c>
     </row>
     <row r="99" spans="1:10">
@@ -8363,7 +8363,7 @@
         <v>1488</v>
       </c>
       <c r="J99">
-        <v>904</v>
+        <v>913</v>
       </c>
     </row>
     <row r="100" spans="1:10">
@@ -8395,7 +8395,7 @@
         <v>237</v>
       </c>
       <c r="J100">
-        <v>169</v>
+        <v>170</v>
       </c>
     </row>
     <row r="101" spans="1:10">
@@ -8406,13 +8406,13 @@
         <v>104361</v>
       </c>
       <c r="C101">
-        <v>116081</v>
+        <v>116082</v>
       </c>
       <c r="D101">
         <v>117356</v>
       </c>
       <c r="E101">
-        <v>113390</v>
+        <v>113392</v>
       </c>
       <c r="F101">
         <v>105560</v>
@@ -8424,10 +8424,10 @@
         <v>84594</v>
       </c>
       <c r="I101">
-        <v>110479</v>
+        <v>110482</v>
       </c>
       <c r="J101">
-        <v>64868</v>
+        <v>65248</v>
       </c>
     </row>
   </sheetData>
@@ -8711,7 +8711,7 @@
         <v>121</v>
       </c>
       <c r="J5">
-        <v>69</v>
+        <v>70</v>
       </c>
     </row>
     <row r="6" spans="1:10">
@@ -8795,7 +8795,7 @@
         <v>219</v>
       </c>
       <c r="J8">
-        <v>120</v>
+        <v>123</v>
       </c>
     </row>
     <row r="9" spans="1:10">
@@ -8891,7 +8891,7 @@
         <v>1648</v>
       </c>
       <c r="J11">
-        <v>929</v>
+        <v>933</v>
       </c>
     </row>
   </sheetData>
@@ -8980,7 +8980,7 @@
         <v>327</v>
       </c>
       <c r="J2">
-        <v>165</v>
+        <v>166</v>
       </c>
     </row>
     <row r="3" spans="1:10">
@@ -9108,7 +9108,7 @@
         <v>54</v>
       </c>
       <c r="J6">
-        <v>53</v>
+        <v>55</v>
       </c>
     </row>
     <row r="7" spans="1:10">
@@ -9172,7 +9172,7 @@
         <v>1026</v>
       </c>
       <c r="J8">
-        <v>801</v>
+        <v>809</v>
       </c>
     </row>
     <row r="9" spans="1:10">
@@ -9204,7 +9204,7 @@
         <v>303</v>
       </c>
       <c r="J9">
-        <v>185</v>
+        <v>186</v>
       </c>
     </row>
     <row r="10" spans="1:10">
@@ -9236,7 +9236,7 @@
         <v>1271</v>
       </c>
       <c r="J10">
-        <v>724</v>
+        <v>726</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -9268,7 +9268,7 @@
         <v>3848</v>
       </c>
       <c r="J11">
-        <v>2360</v>
+        <v>2374</v>
       </c>
     </row>
   </sheetData>
@@ -9450,7 +9450,7 @@
         <v>73</v>
       </c>
       <c r="J5">
-        <v>66</v>
+        <v>67</v>
       </c>
     </row>
     <row r="6" spans="1:10">
@@ -9546,7 +9546,7 @@
         <v>336</v>
       </c>
       <c r="J8">
-        <v>175</v>
+        <v>176</v>
       </c>
     </row>
     <row r="9" spans="1:10">
@@ -9578,7 +9578,7 @@
         <v>179</v>
       </c>
       <c r="J9">
-        <v>123</v>
+        <v>124</v>
       </c>
     </row>
     <row r="10" spans="1:10">
@@ -9610,7 +9610,7 @@
         <v>2132</v>
       </c>
       <c r="J10">
-        <v>1205</v>
+        <v>1215</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -9642,7 +9642,7 @@
         <v>2923</v>
       </c>
       <c r="J11">
-        <v>1673</v>
+        <v>1686</v>
       </c>
     </row>
   </sheetData>
@@ -9853,7 +9853,7 @@
         <v>4</v>
       </c>
       <c r="J6">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="7" spans="1:10">
@@ -9914,7 +9914,7 @@
         <v>280</v>
       </c>
       <c r="J8">
-        <v>302</v>
+        <v>303</v>
       </c>
     </row>
     <row r="9" spans="1:10">
@@ -9978,7 +9978,7 @@
         <v>1034</v>
       </c>
       <c r="J10">
-        <v>481</v>
+        <v>483</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -10010,7 +10010,7 @@
         <v>1673</v>
       </c>
       <c r="J11">
-        <v>970</v>
+        <v>974</v>
       </c>
     </row>
   </sheetData>
@@ -10131,7 +10131,7 @@
         <v>365</v>
       </c>
       <c r="J3">
-        <v>231</v>
+        <v>232</v>
       </c>
     </row>
     <row r="4" spans="1:10">
@@ -10227,7 +10227,7 @@
         <v>56</v>
       </c>
       <c r="J6">
-        <v>39</v>
+        <v>40</v>
       </c>
     </row>
     <row r="7" spans="1:10">
@@ -10323,7 +10323,7 @@
         <v>295</v>
       </c>
       <c r="J9">
-        <v>153</v>
+        <v>154</v>
       </c>
     </row>
     <row r="10" spans="1:10">
@@ -10355,7 +10355,7 @@
         <v>895</v>
       </c>
       <c r="J10">
-        <v>479</v>
+        <v>481</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -10387,7 +10387,7 @@
         <v>2510</v>
       </c>
       <c r="J11">
-        <v>1519</v>
+        <v>1524</v>
       </c>
     </row>
   </sheetData>
@@ -10668,7 +10668,7 @@
         <v>392</v>
       </c>
       <c r="J8">
-        <v>293</v>
+        <v>294</v>
       </c>
     </row>
     <row r="9" spans="1:10">
@@ -10700,7 +10700,7 @@
         <v>86</v>
       </c>
       <c r="J9">
-        <v>53</v>
+        <v>54</v>
       </c>
     </row>
     <row r="10" spans="1:10">
@@ -10732,7 +10732,7 @@
         <v>433</v>
       </c>
       <c r="J10">
-        <v>279</v>
+        <v>281</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -10764,7 +10764,7 @@
         <v>1389</v>
       </c>
       <c r="J11">
-        <v>847</v>
+        <v>851</v>
       </c>
     </row>
   </sheetData>
@@ -11045,7 +11045,7 @@
         <v>190</v>
       </c>
       <c r="J8">
-        <v>175</v>
+        <v>177</v>
       </c>
     </row>
     <row r="9" spans="1:10">
@@ -11141,7 +11141,7 @@
         <v>729</v>
       </c>
       <c r="J11">
-        <v>480</v>
+        <v>482</v>
       </c>
     </row>
   </sheetData>
@@ -11262,7 +11262,7 @@
         <v>190</v>
       </c>
       <c r="J3">
-        <v>112</v>
+        <v>113</v>
       </c>
     </row>
     <row r="4" spans="1:10">
@@ -11422,7 +11422,7 @@
         <v>218</v>
       </c>
       <c r="J8">
-        <v>201</v>
+        <v>202</v>
       </c>
     </row>
     <row r="9" spans="1:10">
@@ -11486,7 +11486,7 @@
         <v>590</v>
       </c>
       <c r="J10">
-        <v>377</v>
+        <v>380</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -11518,7 +11518,7 @@
         <v>1491</v>
       </c>
       <c r="J11">
-        <v>1039</v>
+        <v>1044</v>
       </c>
     </row>
   </sheetData>
@@ -11607,7 +11607,7 @@
         <v>67</v>
       </c>
       <c r="J2">
-        <v>36</v>
+        <v>37</v>
       </c>
     </row>
     <row r="3" spans="1:10">
@@ -11895,7 +11895,7 @@
         <v>943</v>
       </c>
       <c r="J11">
-        <v>576</v>
+        <v>577</v>
       </c>
     </row>
   </sheetData>
@@ -11984,7 +11984,7 @@
         <v>108</v>
       </c>
       <c r="J2">
-        <v>69</v>
+        <v>70</v>
       </c>
     </row>
     <row r="3" spans="1:10">
@@ -12016,7 +12016,7 @@
         <v>111</v>
       </c>
       <c r="J3">
-        <v>58</v>
+        <v>59</v>
       </c>
     </row>
     <row r="4" spans="1:10">
@@ -12080,7 +12080,7 @@
         <v>69</v>
       </c>
       <c r="J5">
-        <v>38</v>
+        <v>39</v>
       </c>
     </row>
     <row r="6" spans="1:10">
@@ -12173,7 +12173,7 @@
         <v>401</v>
       </c>
       <c r="J8">
-        <v>230</v>
+        <v>231</v>
       </c>
     </row>
     <row r="9" spans="1:10">
@@ -12237,7 +12237,7 @@
         <v>2528</v>
       </c>
       <c r="J10">
-        <v>1411</v>
+        <v>1425</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -12269,7 +12269,7 @@
         <v>3507</v>
       </c>
       <c r="J11">
-        <v>1970</v>
+        <v>1988</v>
       </c>
     </row>
   </sheetData>
@@ -12550,7 +12550,7 @@
         <v>503</v>
       </c>
       <c r="J8">
-        <v>353</v>
+        <v>358</v>
       </c>
     </row>
     <row r="9" spans="1:10">
@@ -12614,7 +12614,7 @@
         <v>527</v>
       </c>
       <c r="J10">
-        <v>319</v>
+        <v>321</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -12646,7 +12646,7 @@
         <v>1491</v>
       </c>
       <c r="J11">
-        <v>926</v>
+        <v>933</v>
       </c>
     </row>
   </sheetData>
@@ -12735,7 +12735,7 @@
         <v>239</v>
       </c>
       <c r="J2">
-        <v>138</v>
+        <v>139</v>
       </c>
     </row>
     <row r="3" spans="1:10">
@@ -12767,7 +12767,7 @@
         <v>261</v>
       </c>
       <c r="J3">
-        <v>164</v>
+        <v>165</v>
       </c>
     </row>
     <row r="4" spans="1:10">
@@ -12831,7 +12831,7 @@
         <v>200</v>
       </c>
       <c r="J5">
-        <v>134</v>
+        <v>135</v>
       </c>
     </row>
     <row r="6" spans="1:10">
@@ -12991,7 +12991,7 @@
         <v>813</v>
       </c>
       <c r="J10">
-        <v>469</v>
+        <v>471</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -13023,7 +13023,7 @@
         <v>2547</v>
       </c>
       <c r="J11">
-        <v>1577</v>
+        <v>1582</v>
       </c>
     </row>
   </sheetData>
@@ -13347,7 +13347,7 @@
         <v>213</v>
       </c>
       <c r="J10">
-        <v>134</v>
+        <v>135</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -13379,7 +13379,7 @@
         <v>418</v>
       </c>
       <c r="J11">
-        <v>297</v>
+        <v>298</v>
       </c>
     </row>
   </sheetData>
@@ -13645,7 +13645,7 @@
         <v>89</v>
       </c>
       <c r="J8">
-        <v>77</v>
+        <v>78</v>
       </c>
     </row>
     <row r="9" spans="1:10">
@@ -13709,7 +13709,7 @@
         <v>448</v>
       </c>
       <c r="J10">
-        <v>224</v>
+        <v>225</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -13741,7 +13741,7 @@
         <v>706</v>
       </c>
       <c r="J11">
-        <v>383</v>
+        <v>385</v>
       </c>
     </row>
   </sheetData>
@@ -13830,7 +13830,7 @@
         <v>194</v>
       </c>
       <c r="J2">
-        <v>112</v>
+        <v>113</v>
       </c>
     </row>
     <row r="3" spans="1:10">
@@ -13862,7 +13862,7 @@
         <v>182</v>
       </c>
       <c r="J3">
-        <v>117</v>
+        <v>120</v>
       </c>
     </row>
     <row r="4" spans="1:10">
@@ -14022,7 +14022,7 @@
         <v>202</v>
       </c>
       <c r="J8">
-        <v>216</v>
+        <v>217</v>
       </c>
     </row>
     <row r="9" spans="1:10">
@@ -14054,7 +14054,7 @@
         <v>189</v>
       </c>
       <c r="J9">
-        <v>133</v>
+        <v>134</v>
       </c>
     </row>
     <row r="10" spans="1:10">
@@ -14086,7 +14086,7 @@
         <v>587</v>
       </c>
       <c r="J10">
-        <v>341</v>
+        <v>342</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -14118,7 +14118,7 @@
         <v>1515</v>
       </c>
       <c r="J11">
-        <v>1007</v>
+        <v>1014</v>
       </c>
     </row>
   </sheetData>
@@ -14734,7 +14734,7 @@
         <v>175</v>
       </c>
       <c r="J8">
-        <v>151</v>
+        <v>152</v>
       </c>
     </row>
     <row r="9" spans="1:10">
@@ -14830,7 +14830,7 @@
         <v>768</v>
       </c>
       <c r="J11">
-        <v>470</v>
+        <v>471</v>
       </c>
     </row>
   </sheetData>
@@ -15009,7 +15009,7 @@
         <v>38</v>
       </c>
       <c r="J5">
-        <v>28</v>
+        <v>29</v>
       </c>
     </row>
     <row r="6" spans="1:10">
@@ -15192,7 +15192,7 @@
         <v>437</v>
       </c>
       <c r="J11">
-        <v>200</v>
+        <v>201</v>
       </c>
     </row>
   </sheetData>
@@ -15313,7 +15313,7 @@
         <v>205</v>
       </c>
       <c r="J3">
-        <v>121</v>
+        <v>122</v>
       </c>
     </row>
     <row r="4" spans="1:10">
@@ -15473,7 +15473,7 @@
         <v>484</v>
       </c>
       <c r="J8">
-        <v>279</v>
+        <v>281</v>
       </c>
     </row>
     <row r="9" spans="1:10">
@@ -15569,7 +15569,7 @@
         <v>1793</v>
       </c>
       <c r="J11">
-        <v>997</v>
+        <v>1000</v>
       </c>
     </row>
   </sheetData>
@@ -15658,7 +15658,7 @@
         <v>92</v>
       </c>
       <c r="J2">
-        <v>41</v>
+        <v>42</v>
       </c>
     </row>
     <row r="3" spans="1:10">
@@ -15850,7 +15850,7 @@
         <v>224</v>
       </c>
       <c r="J8">
-        <v>171</v>
+        <v>172</v>
       </c>
     </row>
     <row r="9" spans="1:10">
@@ -15882,7 +15882,7 @@
         <v>109</v>
       </c>
       <c r="J9">
-        <v>92</v>
+        <v>93</v>
       </c>
     </row>
     <row r="10" spans="1:10">
@@ -15914,7 +15914,7 @@
         <v>610</v>
       </c>
       <c r="J10">
-        <v>283</v>
+        <v>288</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -15946,7 +15946,7 @@
         <v>1244</v>
       </c>
       <c r="J11">
-        <v>682</v>
+        <v>690</v>
       </c>
     </row>
   </sheetData>
@@ -16212,7 +16212,7 @@
         <v>294</v>
       </c>
       <c r="J8">
-        <v>213</v>
+        <v>214</v>
       </c>
     </row>
     <row r="9" spans="1:10">
@@ -16276,7 +16276,7 @@
         <v>2021</v>
       </c>
       <c r="J10">
-        <v>983</v>
+        <v>986</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -16308,7 +16308,7 @@
         <v>2663</v>
       </c>
       <c r="J11">
-        <v>1386</v>
+        <v>1390</v>
       </c>
     </row>
   </sheetData>
@@ -16493,7 +16493,7 @@
         <v>170</v>
       </c>
       <c r="J5">
-        <v>65</v>
+        <v>66</v>
       </c>
     </row>
     <row r="6" spans="1:10">
@@ -16589,7 +16589,7 @@
         <v>707</v>
       </c>
       <c r="J8">
-        <v>556</v>
+        <v>563</v>
       </c>
     </row>
     <row r="9" spans="1:10">
@@ -16653,7 +16653,7 @@
         <v>968</v>
       </c>
       <c r="J10">
-        <v>545</v>
+        <v>549</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -16685,7 +16685,7 @@
         <v>3011</v>
       </c>
       <c r="J11">
-        <v>1855</v>
+        <v>1867</v>
       </c>
     </row>
   </sheetData>
@@ -16774,7 +16774,7 @@
         <v>264</v>
       </c>
       <c r="J2">
-        <v>140</v>
+        <v>141</v>
       </c>
     </row>
     <row r="3" spans="1:10">
@@ -16870,7 +16870,7 @@
         <v>261</v>
       </c>
       <c r="J5">
-        <v>133</v>
+        <v>137</v>
       </c>
     </row>
     <row r="6" spans="1:10">
@@ -16899,7 +16899,7 @@
         <v>33</v>
       </c>
       <c r="I6">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="J6">
         <v>14</v>
@@ -16934,7 +16934,7 @@
         <v>36</v>
       </c>
       <c r="J7">
-        <v>7</v>
+        <v>9</v>
       </c>
     </row>
     <row r="8" spans="1:10">
@@ -16966,7 +16966,7 @@
         <v>567</v>
       </c>
       <c r="J8">
-        <v>553</v>
+        <v>559</v>
       </c>
     </row>
     <row r="9" spans="1:10">
@@ -16998,7 +16998,7 @@
         <v>226</v>
       </c>
       <c r="J9">
-        <v>144</v>
+        <v>146</v>
       </c>
     </row>
     <row r="10" spans="1:10">
@@ -17030,7 +17030,7 @@
         <v>1023</v>
       </c>
       <c r="J10">
-        <v>501</v>
+        <v>504</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -17059,10 +17059,10 @@
         <v>2237</v>
       </c>
       <c r="I11">
-        <v>2685</v>
+        <v>2686</v>
       </c>
       <c r="J11">
-        <v>1626</v>
+        <v>1644</v>
       </c>
     </row>
   </sheetData>
@@ -17151,7 +17151,7 @@
         <v>457</v>
       </c>
       <c r="J2">
-        <v>275</v>
+        <v>277</v>
       </c>
     </row>
     <row r="3" spans="1:10">
@@ -17183,7 +17183,7 @@
         <v>445</v>
       </c>
       <c r="J3">
-        <v>299</v>
+        <v>300</v>
       </c>
     </row>
     <row r="4" spans="1:10">
@@ -17279,7 +17279,7 @@
         <v>93</v>
       </c>
       <c r="J6">
-        <v>53</v>
+        <v>54</v>
       </c>
     </row>
     <row r="7" spans="1:10">
@@ -17343,7 +17343,7 @@
         <v>1269</v>
       </c>
       <c r="J8">
-        <v>743</v>
+        <v>746</v>
       </c>
     </row>
     <row r="9" spans="1:10">
@@ -17375,7 +17375,7 @@
         <v>497</v>
       </c>
       <c r="J9">
-        <v>304</v>
+        <v>308</v>
       </c>
     </row>
     <row r="10" spans="1:10">
@@ -17407,7 +17407,7 @@
         <v>1652</v>
       </c>
       <c r="J10">
-        <v>904</v>
+        <v>908</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -17439,7 +17439,7 @@
         <v>4743</v>
       </c>
       <c r="J11">
-        <v>2748</v>
+        <v>2763</v>
       </c>
     </row>
   </sheetData>
@@ -17720,7 +17720,7 @@
         <v>441</v>
       </c>
       <c r="J8">
-        <v>335</v>
+        <v>336</v>
       </c>
     </row>
     <row r="9" spans="1:10">
@@ -17816,7 +17816,7 @@
         <v>1354</v>
       </c>
       <c r="J11">
-        <v>852</v>
+        <v>853</v>
       </c>
     </row>
   </sheetData>
@@ -17905,7 +17905,7 @@
         <v>47</v>
       </c>
       <c r="J2">
-        <v>26</v>
+        <v>27</v>
       </c>
     </row>
     <row r="3" spans="1:10">
@@ -18120,7 +18120,7 @@
         <v>61</v>
       </c>
       <c r="J9">
-        <v>42</v>
+        <v>43</v>
       </c>
     </row>
     <row r="10" spans="1:10">
@@ -18184,7 +18184,7 @@
         <v>903</v>
       </c>
       <c r="J11">
-        <v>546</v>
+        <v>548</v>
       </c>
     </row>
   </sheetData>
@@ -18369,7 +18369,7 @@
         <v>229</v>
       </c>
       <c r="J5">
-        <v>104</v>
+        <v>106</v>
       </c>
     </row>
     <row r="6" spans="1:10">
@@ -18465,7 +18465,7 @@
         <v>754</v>
       </c>
       <c r="J8">
-        <v>425</v>
+        <v>427</v>
       </c>
     </row>
     <row r="9" spans="1:10">
@@ -18497,7 +18497,7 @@
         <v>233</v>
       </c>
       <c r="J9">
-        <v>160</v>
+        <v>162</v>
       </c>
     </row>
     <row r="10" spans="1:10">
@@ -18529,7 +18529,7 @@
         <v>911</v>
       </c>
       <c r="J10">
-        <v>539</v>
+        <v>540</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -18561,7 +18561,7 @@
         <v>2636</v>
       </c>
       <c r="J11">
-        <v>1514</v>
+        <v>1521</v>
       </c>
     </row>
   </sheetData>
@@ -19224,7 +19224,7 @@
         <v>224</v>
       </c>
       <c r="J9">
-        <v>78</v>
+        <v>79</v>
       </c>
     </row>
     <row r="10" spans="1:10">
@@ -19256,7 +19256,7 @@
         <v>828</v>
       </c>
       <c r="J10">
-        <v>425</v>
+        <v>427</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -19288,7 +19288,7 @@
         <v>2045</v>
       </c>
       <c r="J11">
-        <v>1083</v>
+        <v>1086</v>
       </c>
     </row>
   </sheetData>
@@ -19377,7 +19377,7 @@
         <v>37</v>
       </c>
       <c r="J2">
-        <v>22</v>
+        <v>23</v>
       </c>
     </row>
     <row r="3" spans="1:10">
@@ -19467,7 +19467,7 @@
         <v>94</v>
       </c>
       <c r="J5">
-        <v>71</v>
+        <v>73</v>
       </c>
     </row>
     <row r="6" spans="1:10">
@@ -19653,7 +19653,7 @@
         <v>960</v>
       </c>
       <c r="J11">
-        <v>555</v>
+        <v>558</v>
       </c>
     </row>
   </sheetData>
@@ -19919,7 +19919,7 @@
         <v>68</v>
       </c>
       <c r="J8">
-        <v>59</v>
+        <v>60</v>
       </c>
     </row>
     <row r="9" spans="1:10">
@@ -19983,7 +19983,7 @@
         <v>124</v>
       </c>
       <c r="J10">
-        <v>86</v>
+        <v>87</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -20015,7 +20015,7 @@
         <v>271</v>
       </c>
       <c r="J11">
-        <v>176</v>
+        <v>178</v>
       </c>
     </row>
   </sheetData>
@@ -20104,7 +20104,7 @@
         <v>87</v>
       </c>
       <c r="J2">
-        <v>53</v>
+        <v>54</v>
       </c>
     </row>
     <row r="3" spans="1:10">
@@ -20360,7 +20360,7 @@
         <v>320</v>
       </c>
       <c r="J10">
-        <v>181</v>
+        <v>183</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -20392,7 +20392,7 @@
         <v>970</v>
       </c>
       <c r="J11">
-        <v>613</v>
+        <v>616</v>
       </c>
     </row>
   </sheetData>
@@ -20667,7 +20667,7 @@
         <v>122</v>
       </c>
       <c r="J8">
-        <v>127</v>
+        <v>128</v>
       </c>
     </row>
     <row r="9" spans="1:10">
@@ -20731,7 +20731,7 @@
         <v>381</v>
       </c>
       <c r="J10">
-        <v>193</v>
+        <v>197</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -20763,7 +20763,7 @@
         <v>721</v>
       </c>
       <c r="J11">
-        <v>437</v>
+        <v>442</v>
       </c>
     </row>
   </sheetData>
@@ -21023,7 +21023,7 @@
         <v>44</v>
       </c>
       <c r="J8">
-        <v>45</v>
+        <v>46</v>
       </c>
     </row>
     <row r="9" spans="1:10">
@@ -21119,7 +21119,7 @@
         <v>436</v>
       </c>
       <c r="J11">
-        <v>269</v>
+        <v>270</v>
       </c>
     </row>
   </sheetData>
@@ -21208,7 +21208,7 @@
         <v>38</v>
       </c>
       <c r="J2">
-        <v>18</v>
+        <v>19</v>
       </c>
     </row>
     <row r="3" spans="1:10">
@@ -21487,7 +21487,7 @@
         <v>436</v>
       </c>
       <c r="J11">
-        <v>253</v>
+        <v>254</v>
       </c>
     </row>
   </sheetData>
@@ -21608,7 +21608,7 @@
         <v>81</v>
       </c>
       <c r="J3">
-        <v>53</v>
+        <v>54</v>
       </c>
     </row>
     <row r="4" spans="1:10">
@@ -21765,7 +21765,7 @@
         <v>297</v>
       </c>
       <c r="J8">
-        <v>276</v>
+        <v>278</v>
       </c>
     </row>
     <row r="9" spans="1:10">
@@ -21829,7 +21829,7 @@
         <v>670</v>
       </c>
       <c r="J10">
-        <v>353</v>
+        <v>356</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -21861,7 +21861,7 @@
         <v>1337</v>
       </c>
       <c r="J11">
-        <v>865</v>
+        <v>871</v>
       </c>
     </row>
   </sheetData>
@@ -22046,7 +22046,7 @@
         <v>83</v>
       </c>
       <c r="J5">
-        <v>50</v>
+        <v>51</v>
       </c>
     </row>
     <row r="6" spans="1:10">
@@ -22142,7 +22142,7 @@
         <v>125</v>
       </c>
       <c r="J8">
-        <v>77</v>
+        <v>78</v>
       </c>
     </row>
     <row r="9" spans="1:10">
@@ -22206,7 +22206,7 @@
         <v>492</v>
       </c>
       <c r="J10">
-        <v>316</v>
+        <v>317</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -22238,7 +22238,7 @@
         <v>917</v>
       </c>
       <c r="J11">
-        <v>553</v>
+        <v>556</v>
       </c>
     </row>
   </sheetData>
@@ -22677,7 +22677,7 @@
         <v>54</v>
       </c>
       <c r="J2">
-        <v>37</v>
+        <v>38</v>
       </c>
     </row>
     <row r="3" spans="1:10">
@@ -22962,7 +22962,7 @@
         <v>695</v>
       </c>
       <c r="J11">
-        <v>433</v>
+        <v>434</v>
       </c>
     </row>
   </sheetData>
@@ -23883,7 +23883,7 @@
         <v>77</v>
       </c>
       <c r="J5">
-        <v>34</v>
+        <v>35</v>
       </c>
     </row>
     <row r="6" spans="1:10">
@@ -24075,7 +24075,7 @@
         <v>793</v>
       </c>
       <c r="J11">
-        <v>565</v>
+        <v>566</v>
       </c>
     </row>
   </sheetData>
@@ -24408,7 +24408,7 @@
         <v>216</v>
       </c>
       <c r="J10">
-        <v>110</v>
+        <v>111</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -24440,7 +24440,7 @@
         <v>396</v>
       </c>
       <c r="J11">
-        <v>225</v>
+        <v>226</v>
       </c>
     </row>
   </sheetData>
@@ -24741,7 +24741,7 @@
         <v>88</v>
       </c>
       <c r="J9">
-        <v>31</v>
+        <v>32</v>
       </c>
     </row>
     <row r="10" spans="1:10">
@@ -24773,7 +24773,7 @@
         <v>784</v>
       </c>
       <c r="J10">
-        <v>490</v>
+        <v>494</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -24805,7 +24805,7 @@
         <v>1258</v>
       </c>
       <c r="J11">
-        <v>768</v>
+        <v>773</v>
       </c>
     </row>
   </sheetData>
@@ -24894,7 +24894,7 @@
         <v>78</v>
       </c>
       <c r="J2">
-        <v>41</v>
+        <v>42</v>
       </c>
     </row>
     <row r="3" spans="1:10">
@@ -25150,7 +25150,7 @@
         <v>381</v>
       </c>
       <c r="J10">
-        <v>203</v>
+        <v>204</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -25182,7 +25182,7 @@
         <v>867</v>
       </c>
       <c r="J11">
-        <v>481</v>
+        <v>483</v>
       </c>
     </row>
   </sheetData>
@@ -25447,7 +25447,7 @@
         <v>17</v>
       </c>
       <c r="J9">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="10" spans="1:10">
@@ -25479,7 +25479,7 @@
         <v>576</v>
       </c>
       <c r="J10">
-        <v>305</v>
+        <v>306</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -25511,7 +25511,7 @@
         <v>628</v>
       </c>
       <c r="J11">
-        <v>328</v>
+        <v>330</v>
       </c>
     </row>
   </sheetData>
@@ -26180,7 +26180,7 @@
         <v>139</v>
       </c>
       <c r="J9">
-        <v>81</v>
+        <v>82</v>
       </c>
     </row>
     <row r="10" spans="1:10">
@@ -26212,7 +26212,7 @@
         <v>233</v>
       </c>
       <c r="J10">
-        <v>153</v>
+        <v>154</v>
       </c>
     </row>
   </sheetData>
@@ -26301,7 +26301,7 @@
         <v>78</v>
       </c>
       <c r="J2">
-        <v>52</v>
+        <v>53</v>
       </c>
     </row>
     <row r="3" spans="1:10">
@@ -26557,7 +26557,7 @@
         <v>1118</v>
       </c>
       <c r="J10">
-        <v>595</v>
+        <v>598</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -26589,7 +26589,7 @@
         <v>1797</v>
       </c>
       <c r="J11">
-        <v>1014</v>
+        <v>1018</v>
       </c>
     </row>
   </sheetData>
@@ -26925,7 +26925,7 @@
         <v>371</v>
       </c>
       <c r="J10">
-        <v>156</v>
+        <v>158</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -26957,7 +26957,7 @@
         <v>718</v>
       </c>
       <c r="J11">
-        <v>346</v>
+        <v>348</v>
       </c>
     </row>
   </sheetData>
@@ -27208,7 +27208,7 @@
         <v>99</v>
       </c>
       <c r="J8">
-        <v>80</v>
+        <v>81</v>
       </c>
     </row>
     <row r="9" spans="1:10">
@@ -27304,7 +27304,7 @@
         <v>715</v>
       </c>
       <c r="J11">
-        <v>432</v>
+        <v>433</v>
       </c>
     </row>
   </sheetData>
@@ -27584,7 +27584,7 @@
         <v>52</v>
       </c>
       <c r="J9">
-        <v>34</v>
+        <v>36</v>
       </c>
     </row>
     <row r="10" spans="1:10">
@@ -27616,7 +27616,7 @@
         <v>376</v>
       </c>
       <c r="J10">
-        <v>262</v>
+        <v>263</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -27648,7 +27648,7 @@
         <v>595</v>
       </c>
       <c r="J11">
-        <v>422</v>
+        <v>425</v>
       </c>
     </row>
   </sheetData>
@@ -28464,7 +28464,7 @@
         <v>55</v>
       </c>
       <c r="J2">
-        <v>21</v>
+        <v>22</v>
       </c>
     </row>
     <row r="3" spans="1:10">
@@ -28653,7 +28653,7 @@
         <v>136</v>
       </c>
       <c r="J8">
-        <v>104</v>
+        <v>106</v>
       </c>
     </row>
     <row r="9" spans="1:10">
@@ -28685,7 +28685,7 @@
         <v>90</v>
       </c>
       <c r="J9">
-        <v>42</v>
+        <v>43</v>
       </c>
     </row>
     <row r="10" spans="1:10">
@@ -28749,7 +28749,7 @@
         <v>948</v>
       </c>
       <c r="J11">
-        <v>526</v>
+        <v>530</v>
       </c>
     </row>
   </sheetData>
@@ -28838,7 +28838,7 @@
         <v>34</v>
       </c>
       <c r="J2">
-        <v>19</v>
+        <v>21</v>
       </c>
     </row>
     <row r="3" spans="1:10">
@@ -29024,7 +29024,7 @@
         <v>122</v>
       </c>
       <c r="J8">
-        <v>120</v>
+        <v>122</v>
       </c>
     </row>
     <row r="9" spans="1:10">
@@ -29056,7 +29056,7 @@
         <v>35</v>
       </c>
       <c r="J9">
-        <v>45</v>
+        <v>46</v>
       </c>
     </row>
     <row r="10" spans="1:10">
@@ -29088,7 +29088,7 @@
         <v>172</v>
       </c>
       <c r="J10">
-        <v>96</v>
+        <v>97</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -29120,7 +29120,7 @@
         <v>437</v>
       </c>
       <c r="J11">
-        <v>314</v>
+        <v>320</v>
       </c>
     </row>
   </sheetData>
@@ -29209,7 +29209,7 @@
         <v>77</v>
       </c>
       <c r="J2">
-        <v>62</v>
+        <v>63</v>
       </c>
     </row>
     <row r="3" spans="1:10">
@@ -29305,7 +29305,7 @@
         <v>131</v>
       </c>
       <c r="J5">
-        <v>76</v>
+        <v>77</v>
       </c>
     </row>
     <row r="6" spans="1:10">
@@ -29398,7 +29398,7 @@
         <v>216</v>
       </c>
       <c r="J8">
-        <v>193</v>
+        <v>194</v>
       </c>
     </row>
     <row r="9" spans="1:10">
@@ -29430,7 +29430,7 @@
         <v>107</v>
       </c>
       <c r="J9">
-        <v>57</v>
+        <v>59</v>
       </c>
     </row>
     <row r="10" spans="1:10">
@@ -29462,7 +29462,7 @@
         <v>1222</v>
       </c>
       <c r="J10">
-        <v>665</v>
+        <v>671</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -29494,7 +29494,7 @@
         <v>1879</v>
       </c>
       <c r="J11">
-        <v>1130</v>
+        <v>1141</v>
       </c>
     </row>
   </sheetData>
@@ -29772,7 +29772,7 @@
         <v>140</v>
       </c>
       <c r="J8">
-        <v>131</v>
+        <v>132</v>
       </c>
     </row>
     <row r="9" spans="1:10">
@@ -29804,7 +29804,7 @@
         <v>24</v>
       </c>
       <c r="J9">
-        <v>24</v>
+        <v>25</v>
       </c>
     </row>
     <row r="10" spans="1:10">
@@ -29836,7 +29836,7 @@
         <v>440</v>
       </c>
       <c r="J10">
-        <v>261</v>
+        <v>263</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -29868,7 +29868,7 @@
         <v>761</v>
       </c>
       <c r="J11">
-        <v>492</v>
+        <v>496</v>
       </c>
     </row>
   </sheetData>
@@ -30149,7 +30149,7 @@
         <v>383</v>
       </c>
       <c r="J8">
-        <v>295</v>
+        <v>299</v>
       </c>
     </row>
     <row r="9" spans="1:10">
@@ -30213,7 +30213,7 @@
         <v>527</v>
       </c>
       <c r="J10">
-        <v>312</v>
+        <v>317</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -30245,7 +30245,7 @@
         <v>1488</v>
       </c>
       <c r="J11">
-        <v>904</v>
+        <v>913</v>
       </c>
     </row>
   </sheetData>
@@ -30406,7 +30406,7 @@
         <v>32</v>
       </c>
       <c r="J5">
-        <v>16</v>
+        <v>17</v>
       </c>
     </row>
     <row r="6" spans="1:10">
@@ -30516,7 +30516,7 @@
         <v>22</v>
       </c>
       <c r="J9">
-        <v>18</v>
+        <v>19</v>
       </c>
     </row>
     <row r="10" spans="1:10">
@@ -30580,7 +30580,7 @@
         <v>248</v>
       </c>
       <c r="J11">
-        <v>163</v>
+        <v>165</v>
       </c>
     </row>
   </sheetData>
@@ -30782,7 +30782,7 @@
         <v>9</v>
       </c>
       <c r="J6">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="7" spans="1:10">
@@ -30825,7 +30825,7 @@
         <v>112</v>
       </c>
       <c r="J8">
-        <v>73</v>
+        <v>74</v>
       </c>
     </row>
     <row r="9" spans="1:10">
@@ -30889,7 +30889,7 @@
         <v>502</v>
       </c>
       <c r="J10">
-        <v>306</v>
+        <v>307</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -30921,7 +30921,7 @@
         <v>677</v>
       </c>
       <c r="J11">
-        <v>407</v>
+        <v>410</v>
       </c>
     </row>
   </sheetData>
@@ -31224,7 +31224,7 @@
         <v>162</v>
       </c>
       <c r="J10">
-        <v>107</v>
+        <v>108</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -31256,7 +31256,7 @@
         <v>237</v>
       </c>
       <c r="J11">
-        <v>169</v>
+        <v>170</v>
       </c>
     </row>
   </sheetData>
@@ -31522,7 +31522,7 @@
         <v>123</v>
       </c>
       <c r="J8">
-        <v>126</v>
+        <v>127</v>
       </c>
     </row>
     <row r="9" spans="1:10">
@@ -31618,7 +31618,7 @@
         <v>335</v>
       </c>
       <c r="J11">
-        <v>254</v>
+        <v>255</v>
       </c>
     </row>
   </sheetData>
@@ -31707,7 +31707,7 @@
         <v>90</v>
       </c>
       <c r="J2">
-        <v>46</v>
+        <v>47</v>
       </c>
     </row>
     <row r="3" spans="1:10">
@@ -31963,7 +31963,7 @@
         <v>389</v>
       </c>
       <c r="J10">
-        <v>252</v>
+        <v>253</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -31995,7 +31995,7 @@
         <v>886</v>
       </c>
       <c r="J11">
-        <v>577</v>
+        <v>579</v>
       </c>
     </row>
   </sheetData>
@@ -32270,7 +32270,7 @@
         <v>405</v>
       </c>
       <c r="J8">
-        <v>347</v>
+        <v>349</v>
       </c>
     </row>
     <row r="9" spans="1:10">
@@ -32302,7 +32302,7 @@
         <v>71</v>
       </c>
       <c r="J9">
-        <v>31</v>
+        <v>32</v>
       </c>
     </row>
     <row r="10" spans="1:10">
@@ -32334,7 +32334,7 @@
         <v>670</v>
       </c>
       <c r="J10">
-        <v>317</v>
+        <v>318</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -32366,7 +32366,7 @@
         <v>1368</v>
       </c>
       <c r="J11">
-        <v>824</v>
+        <v>828</v>
       </c>
     </row>
   </sheetData>
@@ -32641,7 +32641,7 @@
         <v>338</v>
       </c>
       <c r="J8">
-        <v>256</v>
+        <v>258</v>
       </c>
     </row>
     <row r="9" spans="1:10">
@@ -32705,7 +32705,7 @@
         <v>1773</v>
       </c>
       <c r="J10">
-        <v>1007</v>
+        <v>1013</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -32737,7 +32737,7 @@
         <v>2622</v>
       </c>
       <c r="J11">
-        <v>1510</v>
+        <v>1518</v>
       </c>
     </row>
   </sheetData>
@@ -33373,7 +33373,7 @@
         <v>87</v>
       </c>
       <c r="J9">
-        <v>21</v>
+        <v>22</v>
       </c>
     </row>
     <row r="10" spans="1:10">
@@ -33405,7 +33405,7 @@
         <v>174</v>
       </c>
       <c r="J10">
-        <v>73</v>
+        <v>76</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -33437,7 +33437,7 @@
         <v>337</v>
       </c>
       <c r="J11">
-        <v>146</v>
+        <v>150</v>
       </c>
     </row>
   </sheetData>
@@ -33709,7 +33709,7 @@
         <v>334</v>
       </c>
       <c r="J8">
-        <v>191</v>
+        <v>192</v>
       </c>
     </row>
     <row r="9" spans="1:10">
@@ -33773,7 +33773,7 @@
         <v>606</v>
       </c>
       <c r="J10">
-        <v>302</v>
+        <v>304</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -33805,7 +33805,7 @@
         <v>1187</v>
       </c>
       <c r="J11">
-        <v>627</v>
+        <v>630</v>
       </c>
     </row>
   </sheetData>
@@ -34436,7 +34436,7 @@
         <v>313</v>
       </c>
       <c r="J10">
-        <v>143</v>
+        <v>145</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -34468,7 +34468,7 @@
         <v>494</v>
       </c>
       <c r="J11">
-        <v>244</v>
+        <v>246</v>
       </c>
     </row>
   </sheetData>
@@ -34860,7 +34860,7 @@
         <v>38</v>
       </c>
       <c r="J2">
-        <v>18</v>
+        <v>19</v>
       </c>
     </row>
     <row r="3" spans="1:10">
@@ -35104,7 +35104,7 @@
         <v>211</v>
       </c>
       <c r="J10">
-        <v>144</v>
+        <v>145</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -35136,7 +35136,7 @@
         <v>406</v>
       </c>
       <c r="J11">
-        <v>284</v>
+        <v>286</v>
       </c>
     </row>
   </sheetData>
@@ -35367,7 +35367,7 @@
         <v>30</v>
       </c>
       <c r="J7">
-        <v>18</v>
+        <v>19</v>
       </c>
     </row>
     <row r="8" spans="1:10">
@@ -35463,7 +35463,7 @@
         <v>181</v>
       </c>
       <c r="J10">
-        <v>84</v>
+        <v>85</v>
       </c>
     </row>
   </sheetData>
@@ -35755,7 +35755,7 @@
         <v>187</v>
       </c>
       <c r="J9">
-        <v>116</v>
+        <v>117</v>
       </c>
     </row>
     <row r="10" spans="1:10">
@@ -35787,7 +35787,7 @@
         <v>258</v>
       </c>
       <c r="J10">
-        <v>151</v>
+        <v>152</v>
       </c>
     </row>
   </sheetData>
@@ -36237,7 +36237,7 @@
         <v>66</v>
       </c>
       <c r="J3">
-        <v>48</v>
+        <v>49</v>
       </c>
     </row>
     <row r="4" spans="1:10">
@@ -36397,7 +36397,7 @@
         <v>291</v>
       </c>
       <c r="J8">
-        <v>192</v>
+        <v>193</v>
       </c>
     </row>
     <row r="9" spans="1:10">
@@ -36461,7 +36461,7 @@
         <v>905</v>
       </c>
       <c r="J10">
-        <v>460</v>
+        <v>465</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -36493,7 +36493,7 @@
         <v>1669</v>
       </c>
       <c r="J11">
-        <v>921</v>
+        <v>928</v>
       </c>
     </row>
   </sheetData>
@@ -36768,7 +36768,7 @@
         <v>68</v>
       </c>
       <c r="J8">
-        <v>64</v>
+        <v>65</v>
       </c>
     </row>
     <row r="9" spans="1:10">
@@ -36864,7 +36864,7 @@
         <v>337</v>
       </c>
       <c r="J11">
-        <v>230</v>
+        <v>231</v>
       </c>
     </row>
   </sheetData>
@@ -37453,7 +37453,7 @@
         <v>54</v>
       </c>
       <c r="J8">
-        <v>49</v>
+        <v>50</v>
       </c>
     </row>
     <row r="9" spans="1:10">
@@ -37549,7 +37549,7 @@
         <v>236</v>
       </c>
       <c r="J11">
-        <v>153</v>
+        <v>154</v>
       </c>
     </row>
   </sheetData>
@@ -37638,7 +37638,7 @@
         <v>31</v>
       </c>
       <c r="J2">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="3" spans="1:10">
@@ -37722,7 +37722,7 @@
         <v>19</v>
       </c>
       <c r="J5">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="6" spans="1:10">
@@ -37800,7 +37800,7 @@
         <v>160</v>
       </c>
       <c r="J8">
-        <v>61</v>
+        <v>63</v>
       </c>
     </row>
     <row r="9" spans="1:10">
@@ -37864,7 +37864,7 @@
         <v>717</v>
       </c>
       <c r="J10">
-        <v>324</v>
+        <v>326</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -37896,7 +37896,7 @@
         <v>1066</v>
       </c>
       <c r="J11">
-        <v>480</v>
+        <v>486</v>
       </c>
     </row>
   </sheetData>
@@ -38205,7 +38205,7 @@
         <v>260</v>
       </c>
       <c r="J10">
-        <v>122</v>
+        <v>125</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -38237,7 +38237,7 @@
         <v>393</v>
       </c>
       <c r="J11">
-        <v>175</v>
+        <v>178</v>
       </c>
     </row>
   </sheetData>
@@ -38534,7 +38534,7 @@
         <v>135</v>
       </c>
       <c r="J10">
-        <v>67</v>
+        <v>69</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -38566,7 +38566,7 @@
         <v>219</v>
       </c>
       <c r="J11">
-        <v>123</v>
+        <v>125</v>
       </c>
     </row>
   </sheetData>
@@ -38863,7 +38863,7 @@
         <v>225</v>
       </c>
       <c r="J10">
-        <v>112</v>
+        <v>113</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -38895,7 +38895,7 @@
         <v>307</v>
       </c>
       <c r="J11">
-        <v>156</v>
+        <v>157</v>
       </c>
     </row>
   </sheetData>
@@ -39171,7 +39171,7 @@
         <v>366</v>
       </c>
       <c r="J10">
-        <v>56</v>
+        <v>57</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -39203,7 +39203,7 @@
         <v>390</v>
       </c>
       <c r="J11">
-        <v>65</v>
+        <v>66</v>
       </c>
     </row>
   </sheetData>
@@ -39292,7 +39292,7 @@
         <v>7</v>
       </c>
       <c r="J2">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="3" spans="1:10">
@@ -39503,7 +39503,7 @@
         <v>174</v>
       </c>
       <c r="J10">
-        <v>90</v>
+        <v>92</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -39535,7 +39535,7 @@
         <v>235</v>
       </c>
       <c r="J11">
-        <v>132</v>
+        <v>135</v>
       </c>
     </row>
   </sheetData>
@@ -39803,7 +39803,7 @@
         <v>155</v>
       </c>
       <c r="J9">
-        <v>93</v>
+        <v>94</v>
       </c>
     </row>
     <row r="10" spans="1:10">
@@ -39835,7 +39835,7 @@
         <v>191</v>
       </c>
       <c r="J10">
-        <v>106</v>
+        <v>107</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add data for 2023-07-22
</commit_message>
<xml_diff>
--- a/output/index-crime-full-year.xlsx
+++ b/output/index-crime-full-year.xlsx
@@ -895,7 +895,7 @@
         <v>7277</v>
       </c>
       <c r="J2">
-        <v>4113</v>
+        <v>4134</v>
       </c>
     </row>
     <row r="3" spans="1:10">
@@ -927,7 +927,7 @@
         <v>7486</v>
       </c>
       <c r="J3">
-        <v>4318</v>
+        <v>4350</v>
       </c>
     </row>
     <row r="4" spans="1:10">
@@ -959,7 +959,7 @@
         <v>422</v>
       </c>
       <c r="J4">
-        <v>274</v>
+        <v>275</v>
       </c>
     </row>
     <row r="5" spans="1:10">
@@ -991,7 +991,7 @@
         <v>7592</v>
       </c>
       <c r="J5">
-        <v>4008</v>
+        <v>4027</v>
       </c>
     </row>
     <row r="6" spans="1:10">
@@ -1008,7 +1008,7 @@
         <v>1957</v>
       </c>
       <c r="E6">
-        <v>1997</v>
+        <v>1998</v>
       </c>
       <c r="F6">
         <v>1888</v>
@@ -1017,13 +1017,13 @@
         <v>1466</v>
       </c>
       <c r="H6">
-        <v>1698</v>
+        <v>1699</v>
       </c>
       <c r="I6">
         <v>1768</v>
       </c>
       <c r="J6">
-        <v>971</v>
+        <v>974</v>
       </c>
     </row>
     <row r="7" spans="1:10">
@@ -1055,7 +1055,7 @@
         <v>718</v>
       </c>
       <c r="J7">
-        <v>343</v>
+        <v>347</v>
       </c>
     </row>
     <row r="8" spans="1:10">
@@ -1087,7 +1087,7 @@
         <v>21446</v>
       </c>
       <c r="J8">
-        <v>16280</v>
+        <v>16361</v>
       </c>
     </row>
     <row r="9" spans="1:10">
@@ -1119,7 +1119,7 @@
         <v>8965</v>
       </c>
       <c r="J9">
-        <v>5149</v>
+        <v>5175</v>
       </c>
     </row>
     <row r="10" spans="1:10">
@@ -1151,7 +1151,7 @@
         <v>54808</v>
       </c>
       <c r="J10">
-        <v>29792</v>
+        <v>29962</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -1168,7 +1168,7 @@
         <v>117356</v>
       </c>
       <c r="E11">
-        <v>113392</v>
+        <v>113393</v>
       </c>
       <c r="F11">
         <v>105560</v>
@@ -1177,13 +1177,13 @@
         <v>85314</v>
       </c>
       <c r="H11">
-        <v>84594</v>
+        <v>84595</v>
       </c>
       <c r="I11">
         <v>110482</v>
       </c>
       <c r="J11">
-        <v>65248</v>
+        <v>65605</v>
       </c>
     </row>
   </sheetData>
@@ -1353,7 +1353,7 @@
         <v>54</v>
       </c>
       <c r="J5">
-        <v>34</v>
+        <v>35</v>
       </c>
     </row>
     <row r="6" spans="1:10">
@@ -1440,7 +1440,7 @@
         <v>227</v>
       </c>
       <c r="J8">
-        <v>210</v>
+        <v>211</v>
       </c>
     </row>
     <row r="9" spans="1:10">
@@ -1504,7 +1504,7 @@
         <v>648</v>
       </c>
       <c r="J10">
-        <v>402</v>
+        <v>406</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -1536,7 +1536,7 @@
         <v>1153</v>
       </c>
       <c r="J11">
-        <v>774</v>
+        <v>780</v>
       </c>
     </row>
   </sheetData>
@@ -1899,7 +1899,7 @@
         <v>154</v>
       </c>
       <c r="J2">
-        <v>80</v>
+        <v>81</v>
       </c>
     </row>
     <row r="3" spans="1:10">
@@ -1931,7 +1931,7 @@
         <v>81</v>
       </c>
       <c r="J3">
-        <v>49</v>
+        <v>50</v>
       </c>
     </row>
     <row r="4" spans="1:10">
@@ -2027,7 +2027,7 @@
         <v>37</v>
       </c>
       <c r="J6">
-        <v>16</v>
+        <v>17</v>
       </c>
     </row>
     <row r="7" spans="1:10">
@@ -2091,7 +2091,7 @@
         <v>373</v>
       </c>
       <c r="J8">
-        <v>280</v>
+        <v>281</v>
       </c>
     </row>
     <row r="9" spans="1:10">
@@ -2155,7 +2155,7 @@
         <v>820</v>
       </c>
       <c r="J10">
-        <v>509</v>
+        <v>515</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -2187,7 +2187,7 @@
         <v>1712</v>
       </c>
       <c r="J11">
-        <v>1103</v>
+        <v>1113</v>
       </c>
     </row>
   </sheetData>
@@ -2526,7 +2526,7 @@
         <v>712</v>
       </c>
       <c r="J10">
-        <v>403</v>
+        <v>404</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -2558,7 +2558,7 @@
         <v>1228</v>
       </c>
       <c r="J11">
-        <v>723</v>
+        <v>724</v>
       </c>
     </row>
   </sheetData>
@@ -2839,7 +2839,7 @@
         <v>700</v>
       </c>
       <c r="J8">
-        <v>475</v>
+        <v>479</v>
       </c>
     </row>
     <row r="9" spans="1:10">
@@ -2871,7 +2871,7 @@
         <v>216</v>
       </c>
       <c r="J9">
-        <v>112</v>
+        <v>114</v>
       </c>
     </row>
     <row r="10" spans="1:10">
@@ -2903,7 +2903,7 @@
         <v>820</v>
       </c>
       <c r="J10">
-        <v>439</v>
+        <v>441</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -2935,7 +2935,7 @@
         <v>2472</v>
       </c>
       <c r="J11">
-        <v>1435</v>
+        <v>1443</v>
       </c>
     </row>
   </sheetData>
@@ -3213,7 +3213,7 @@
         <v>259</v>
       </c>
       <c r="J8">
-        <v>258</v>
+        <v>260</v>
       </c>
     </row>
     <row r="9" spans="1:10">
@@ -3277,7 +3277,7 @@
         <v>913</v>
       </c>
       <c r="J10">
-        <v>599</v>
+        <v>604</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -3309,7 +3309,7 @@
         <v>1600</v>
       </c>
       <c r="J11">
-        <v>1091</v>
+        <v>1098</v>
       </c>
     </row>
   </sheetData>
@@ -3801,7 +3801,7 @@
         <v>71</v>
       </c>
       <c r="J3">
-        <v>34</v>
+        <v>35</v>
       </c>
     </row>
     <row r="4" spans="1:10">
@@ -4025,7 +4025,7 @@
         <v>681</v>
       </c>
       <c r="J10">
-        <v>488</v>
+        <v>489</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -4057,7 +4057,7 @@
         <v>1279</v>
       </c>
       <c r="J11">
-        <v>887</v>
+        <v>889</v>
       </c>
     </row>
   </sheetData>
@@ -4178,7 +4178,7 @@
         <v>530</v>
       </c>
       <c r="J3">
-        <v>293</v>
+        <v>297</v>
       </c>
     </row>
     <row r="4" spans="1:10">
@@ -4242,7 +4242,7 @@
         <v>268</v>
       </c>
       <c r="J5">
-        <v>158</v>
+        <v>159</v>
       </c>
     </row>
     <row r="6" spans="1:10">
@@ -4370,7 +4370,7 @@
         <v>433</v>
       </c>
       <c r="J9">
-        <v>202</v>
+        <v>203</v>
       </c>
     </row>
     <row r="10" spans="1:10">
@@ -4402,7 +4402,7 @@
         <v>1302</v>
       </c>
       <c r="J10">
-        <v>720</v>
+        <v>725</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -4434,7 +4434,7 @@
         <v>3950</v>
       </c>
       <c r="J11">
-        <v>2340</v>
+        <v>2351</v>
       </c>
     </row>
   </sheetData>
@@ -4642,7 +4642,7 @@
         <v>12</v>
       </c>
       <c r="J6">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="7" spans="1:10">
@@ -4697,7 +4697,7 @@
         <v>131</v>
       </c>
       <c r="J8">
-        <v>145</v>
+        <v>146</v>
       </c>
     </row>
     <row r="9" spans="1:10">
@@ -4729,7 +4729,7 @@
         <v>122</v>
       </c>
       <c r="J9">
-        <v>49</v>
+        <v>50</v>
       </c>
     </row>
     <row r="10" spans="1:10">
@@ -4761,7 +4761,7 @@
         <v>921</v>
       </c>
       <c r="J10">
-        <v>394</v>
+        <v>397</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -4793,7 +4793,7 @@
         <v>1318</v>
       </c>
       <c r="J11">
-        <v>678</v>
+        <v>684</v>
       </c>
     </row>
   </sheetData>
@@ -4914,7 +4914,7 @@
         <v>280</v>
       </c>
       <c r="J3">
-        <v>117</v>
+        <v>118</v>
       </c>
     </row>
     <row r="4" spans="1:10">
@@ -5074,7 +5074,7 @@
         <v>653</v>
       </c>
       <c r="J8">
-        <v>535</v>
+        <v>537</v>
       </c>
     </row>
     <row r="9" spans="1:10">
@@ -5106,7 +5106,7 @@
         <v>428</v>
       </c>
       <c r="J9">
-        <v>286</v>
+        <v>288</v>
       </c>
     </row>
     <row r="10" spans="1:10">
@@ -5138,7 +5138,7 @@
         <v>1089</v>
       </c>
       <c r="J10">
-        <v>674</v>
+        <v>677</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -5170,7 +5170,7 @@
         <v>2956</v>
       </c>
       <c r="J11">
-        <v>1893</v>
+        <v>1901</v>
       </c>
     </row>
   </sheetData>
@@ -5259,7 +5259,7 @@
         <v>917</v>
       </c>
       <c r="J2">
-        <v>556</v>
+        <v>559</v>
       </c>
     </row>
     <row r="3" spans="1:10">
@@ -5355,7 +5355,7 @@
         <v>247</v>
       </c>
       <c r="J5">
-        <v>168</v>
+        <v>169</v>
       </c>
     </row>
     <row r="6" spans="1:10">
@@ -5419,7 +5419,7 @@
         <v>2686</v>
       </c>
       <c r="J7">
-        <v>1644</v>
+        <v>1657</v>
       </c>
     </row>
     <row r="8" spans="1:10">
@@ -5436,7 +5436,7 @@
         <v>5095</v>
       </c>
       <c r="E8">
-        <v>5162</v>
+        <v>5163</v>
       </c>
       <c r="F8">
         <v>5008</v>
@@ -5451,7 +5451,7 @@
         <v>4743</v>
       </c>
       <c r="J8">
-        <v>2763</v>
+        <v>2780</v>
       </c>
     </row>
     <row r="9" spans="1:10">
@@ -5483,7 +5483,7 @@
         <v>519</v>
       </c>
       <c r="J9">
-        <v>302</v>
+        <v>305</v>
       </c>
     </row>
     <row r="10" spans="1:10">
@@ -5515,7 +5515,7 @@
         <v>948</v>
       </c>
       <c r="J10">
-        <v>530</v>
+        <v>534</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -5547,7 +5547,7 @@
         <v>1712</v>
       </c>
       <c r="J11">
-        <v>1103</v>
+        <v>1113</v>
       </c>
     </row>
     <row r="12" spans="1:10">
@@ -5579,7 +5579,7 @@
         <v>412</v>
       </c>
       <c r="J12">
-        <v>227</v>
+        <v>229</v>
       </c>
     </row>
     <row r="13" spans="1:10">
@@ -5675,7 +5675,7 @@
         <v>886</v>
       </c>
       <c r="J15">
-        <v>579</v>
+        <v>581</v>
       </c>
     </row>
     <row r="16" spans="1:10">
@@ -5707,7 +5707,7 @@
         <v>595</v>
       </c>
       <c r="J16">
-        <v>425</v>
+        <v>427</v>
       </c>
     </row>
     <row r="17" spans="1:10">
@@ -5771,7 +5771,7 @@
         <v>695</v>
       </c>
       <c r="J18">
-        <v>434</v>
+        <v>435</v>
       </c>
     </row>
     <row r="19" spans="1:10">
@@ -5803,7 +5803,7 @@
         <v>2636</v>
       </c>
       <c r="J19">
-        <v>1521</v>
+        <v>1526</v>
       </c>
     </row>
     <row r="20" spans="1:10">
@@ -5835,7 +5835,7 @@
         <v>2045</v>
       </c>
       <c r="J20">
-        <v>1086</v>
+        <v>1099</v>
       </c>
     </row>
     <row r="21" spans="1:10">
@@ -5867,7 +5867,7 @@
         <v>337</v>
       </c>
       <c r="J21">
-        <v>150</v>
+        <v>153</v>
       </c>
     </row>
     <row r="22" spans="1:10">
@@ -5899,7 +5899,7 @@
         <v>418</v>
       </c>
       <c r="J22">
-        <v>298</v>
+        <v>299</v>
       </c>
     </row>
     <row r="23" spans="1:10">
@@ -5931,7 +5931,7 @@
         <v>1368</v>
       </c>
       <c r="J23">
-        <v>828</v>
+        <v>831</v>
       </c>
     </row>
     <row r="24" spans="1:10">
@@ -5963,7 +5963,7 @@
         <v>500</v>
       </c>
       <c r="J24">
-        <v>344</v>
+        <v>348</v>
       </c>
     </row>
     <row r="25" spans="1:10">
@@ -5995,7 +5995,7 @@
         <v>429</v>
       </c>
       <c r="J25">
-        <v>264</v>
+        <v>269</v>
       </c>
     </row>
     <row r="26" spans="1:10">
@@ -6027,7 +6027,7 @@
         <v>248</v>
       </c>
       <c r="J26">
-        <v>165</v>
+        <v>168</v>
       </c>
     </row>
     <row r="27" spans="1:10">
@@ -6059,7 +6059,7 @@
         <v>1258</v>
       </c>
       <c r="J27">
-        <v>773</v>
+        <v>776</v>
       </c>
     </row>
     <row r="28" spans="1:10">
@@ -6091,7 +6091,7 @@
         <v>99</v>
       </c>
       <c r="J28">
-        <v>34</v>
+        <v>35</v>
       </c>
     </row>
     <row r="29" spans="1:10">
@@ -6123,7 +6123,7 @@
         <v>3950</v>
       </c>
       <c r="J29">
-        <v>2340</v>
+        <v>2351</v>
       </c>
     </row>
     <row r="30" spans="1:10">
@@ -6187,7 +6187,7 @@
         <v>867</v>
       </c>
       <c r="J31">
-        <v>483</v>
+        <v>487</v>
       </c>
     </row>
     <row r="32" spans="1:10">
@@ -6251,7 +6251,7 @@
         <v>3011</v>
       </c>
       <c r="J33">
-        <v>1867</v>
+        <v>1876</v>
       </c>
     </row>
     <row r="34" spans="1:10">
@@ -6283,7 +6283,7 @@
         <v>761</v>
       </c>
       <c r="J34">
-        <v>496</v>
+        <v>498</v>
       </c>
     </row>
     <row r="35" spans="1:10">
@@ -6315,7 +6315,7 @@
         <v>235</v>
       </c>
       <c r="J35">
-        <v>135</v>
+        <v>136</v>
       </c>
     </row>
     <row r="36" spans="1:10">
@@ -6347,7 +6347,7 @@
         <v>1491</v>
       </c>
       <c r="J36">
-        <v>933</v>
+        <v>936</v>
       </c>
     </row>
     <row r="37" spans="1:10">
@@ -6379,7 +6379,7 @@
         <v>2547</v>
       </c>
       <c r="J37">
-        <v>1582</v>
+        <v>1595</v>
       </c>
     </row>
     <row r="38" spans="1:10">
@@ -6475,7 +6475,7 @@
         <v>236</v>
       </c>
       <c r="J40">
-        <v>154</v>
+        <v>156</v>
       </c>
     </row>
     <row r="41" spans="1:10">
@@ -6507,7 +6507,7 @@
         <v>437</v>
       </c>
       <c r="J41">
-        <v>320</v>
+        <v>321</v>
       </c>
     </row>
     <row r="42" spans="1:10">
@@ -6539,7 +6539,7 @@
         <v>2956</v>
       </c>
       <c r="J42">
-        <v>1893</v>
+        <v>1901</v>
       </c>
     </row>
     <row r="43" spans="1:10">
@@ -6571,7 +6571,7 @@
         <v>1153</v>
       </c>
       <c r="J43">
-        <v>774</v>
+        <v>780</v>
       </c>
     </row>
     <row r="44" spans="1:10">
@@ -6603,7 +6603,7 @@
         <v>1228</v>
       </c>
       <c r="J44">
-        <v>723</v>
+        <v>724</v>
       </c>
     </row>
     <row r="45" spans="1:10">
@@ -6635,7 +6635,7 @@
         <v>181</v>
       </c>
       <c r="J45">
-        <v>85</v>
+        <v>86</v>
       </c>
     </row>
     <row r="46" spans="1:10">
@@ -6667,7 +6667,7 @@
         <v>436</v>
       </c>
       <c r="J46">
-        <v>270</v>
+        <v>274</v>
       </c>
     </row>
     <row r="47" spans="1:10">
@@ -6699,7 +6699,7 @@
         <v>903</v>
       </c>
       <c r="J47">
-        <v>548</v>
+        <v>552</v>
       </c>
     </row>
     <row r="48" spans="1:10">
@@ -6731,7 +6731,7 @@
         <v>2622</v>
       </c>
       <c r="J48">
-        <v>1518</v>
+        <v>1529</v>
       </c>
     </row>
     <row r="49" spans="1:10">
@@ -6763,7 +6763,7 @@
         <v>1648</v>
       </c>
       <c r="J49">
-        <v>933</v>
+        <v>939</v>
       </c>
     </row>
     <row r="50" spans="1:10">
@@ -6827,7 +6827,7 @@
         <v>1337</v>
       </c>
       <c r="J51">
-        <v>871</v>
+        <v>873</v>
       </c>
     </row>
     <row r="52" spans="1:10">
@@ -6859,7 +6859,7 @@
         <v>1491</v>
       </c>
       <c r="J52">
-        <v>1044</v>
+        <v>1049</v>
       </c>
     </row>
     <row r="53" spans="1:10">
@@ -6891,7 +6891,7 @@
         <v>1600</v>
       </c>
       <c r="J53">
-        <v>1091</v>
+        <v>1098</v>
       </c>
     </row>
     <row r="54" spans="1:10">
@@ -6923,7 +6923,7 @@
         <v>3507</v>
       </c>
       <c r="J54">
-        <v>1988</v>
+        <v>2005</v>
       </c>
     </row>
     <row r="55" spans="1:10">
@@ -6955,7 +6955,7 @@
         <v>1244</v>
       </c>
       <c r="J55">
-        <v>690</v>
+        <v>693</v>
       </c>
     </row>
     <row r="56" spans="1:10">
@@ -6987,7 +6987,7 @@
         <v>628</v>
       </c>
       <c r="J56">
-        <v>330</v>
+        <v>332</v>
       </c>
     </row>
     <row r="57" spans="1:10">
@@ -7019,7 +7019,7 @@
         <v>406</v>
       </c>
       <c r="J57">
-        <v>286</v>
+        <v>287</v>
       </c>
     </row>
     <row r="58" spans="1:10">
@@ -7083,7 +7083,7 @@
         <v>271</v>
       </c>
       <c r="J59">
-        <v>178</v>
+        <v>180</v>
       </c>
     </row>
     <row r="60" spans="1:10">
@@ -7115,7 +7115,7 @@
         <v>768</v>
       </c>
       <c r="J60">
-        <v>471</v>
+        <v>472</v>
       </c>
     </row>
     <row r="61" spans="1:10">
@@ -7205,13 +7205,13 @@
         <v>1651</v>
       </c>
       <c r="H63">
-        <v>2167</v>
+        <v>2168</v>
       </c>
       <c r="I63">
         <v>2481</v>
       </c>
       <c r="J63">
-        <v>729</v>
+        <v>711</v>
       </c>
     </row>
     <row r="64" spans="1:10">
@@ -7243,7 +7243,7 @@
         <v>1187</v>
       </c>
       <c r="J64">
-        <v>630</v>
+        <v>633</v>
       </c>
     </row>
     <row r="65" spans="1:10">
@@ -7275,7 +7275,7 @@
         <v>1515</v>
       </c>
       <c r="J65">
-        <v>1014</v>
+        <v>1018</v>
       </c>
     </row>
     <row r="66" spans="1:10">
@@ -7307,7 +7307,7 @@
         <v>715</v>
       </c>
       <c r="J66">
-        <v>433</v>
+        <v>434</v>
       </c>
     </row>
     <row r="67" spans="1:10">
@@ -7339,7 +7339,7 @@
         <v>2510</v>
       </c>
       <c r="J67">
-        <v>1524</v>
+        <v>1531</v>
       </c>
     </row>
     <row r="68" spans="1:10">
@@ -7371,7 +7371,7 @@
         <v>437</v>
       </c>
       <c r="J68">
-        <v>201</v>
+        <v>204</v>
       </c>
     </row>
     <row r="69" spans="1:10">
@@ -7403,7 +7403,7 @@
         <v>494</v>
       </c>
       <c r="J69">
-        <v>246</v>
+        <v>252</v>
       </c>
     </row>
     <row r="70" spans="1:10">
@@ -7435,7 +7435,7 @@
         <v>677</v>
       </c>
       <c r="J70">
-        <v>410</v>
+        <v>414</v>
       </c>
     </row>
     <row r="71" spans="1:10">
@@ -7467,7 +7467,7 @@
         <v>335</v>
       </c>
       <c r="J71">
-        <v>255</v>
+        <v>257</v>
       </c>
     </row>
     <row r="72" spans="1:10">
@@ -7499,7 +7499,7 @@
         <v>706</v>
       </c>
       <c r="J72">
-        <v>385</v>
+        <v>388</v>
       </c>
     </row>
     <row r="73" spans="1:10">
@@ -7531,7 +7531,7 @@
         <v>1279</v>
       </c>
       <c r="J73">
-        <v>887</v>
+        <v>889</v>
       </c>
     </row>
     <row r="74" spans="1:10">
@@ -7627,7 +7627,7 @@
         <v>2923</v>
       </c>
       <c r="J76">
-        <v>1686</v>
+        <v>1695</v>
       </c>
     </row>
     <row r="77" spans="1:10">
@@ -7659,7 +7659,7 @@
         <v>462</v>
       </c>
       <c r="J77">
-        <v>304</v>
+        <v>306</v>
       </c>
     </row>
     <row r="78" spans="1:10">
@@ -7691,7 +7691,7 @@
         <v>1797</v>
       </c>
       <c r="J78">
-        <v>1018</v>
+        <v>1021</v>
       </c>
     </row>
     <row r="79" spans="1:10">
@@ -7723,7 +7723,7 @@
         <v>2472</v>
       </c>
       <c r="J79">
-        <v>1435</v>
+        <v>1443</v>
       </c>
     </row>
     <row r="80" spans="1:10">
@@ -7755,7 +7755,7 @@
         <v>393</v>
       </c>
       <c r="J80">
-        <v>178</v>
+        <v>179</v>
       </c>
     </row>
     <row r="81" spans="1:10">
@@ -7787,7 +7787,7 @@
         <v>219</v>
       </c>
       <c r="J81">
-        <v>125</v>
+        <v>127</v>
       </c>
     </row>
     <row r="82" spans="1:10">
@@ -7819,7 +7819,7 @@
         <v>233</v>
       </c>
       <c r="J82">
-        <v>154</v>
+        <v>156</v>
       </c>
     </row>
     <row r="83" spans="1:10">
@@ -7851,7 +7851,7 @@
         <v>1793</v>
       </c>
       <c r="J83">
-        <v>1000</v>
+        <v>1005</v>
       </c>
     </row>
     <row r="84" spans="1:10">
@@ -7883,7 +7883,7 @@
         <v>729</v>
       </c>
       <c r="J84">
-        <v>482</v>
+        <v>483</v>
       </c>
     </row>
     <row r="85" spans="1:10">
@@ -7915,7 +7915,7 @@
         <v>3848</v>
       </c>
       <c r="J85">
-        <v>2374</v>
+        <v>2385</v>
       </c>
     </row>
     <row r="86" spans="1:10">
@@ -7947,7 +7947,7 @@
         <v>1066</v>
       </c>
       <c r="J86">
-        <v>486</v>
+        <v>488</v>
       </c>
     </row>
     <row r="87" spans="1:10">
@@ -7979,7 +7979,7 @@
         <v>396</v>
       </c>
       <c r="J87">
-        <v>226</v>
+        <v>227</v>
       </c>
     </row>
     <row r="88" spans="1:10">
@@ -8011,7 +8011,7 @@
         <v>943</v>
       </c>
       <c r="J88">
-        <v>577</v>
+        <v>579</v>
       </c>
     </row>
     <row r="89" spans="1:10">
@@ -8043,7 +8043,7 @@
         <v>1879</v>
       </c>
       <c r="J89">
-        <v>1141</v>
+        <v>1147</v>
       </c>
     </row>
     <row r="90" spans="1:10">
@@ -8075,7 +8075,7 @@
         <v>1354</v>
       </c>
       <c r="J90">
-        <v>853</v>
+        <v>857</v>
       </c>
     </row>
     <row r="91" spans="1:10">
@@ -8107,7 +8107,7 @@
         <v>970</v>
       </c>
       <c r="J91">
-        <v>616</v>
+        <v>619</v>
       </c>
     </row>
     <row r="92" spans="1:10">
@@ -8139,7 +8139,7 @@
         <v>337</v>
       </c>
       <c r="J92">
-        <v>231</v>
+        <v>232</v>
       </c>
     </row>
     <row r="93" spans="1:10">
@@ -8171,7 +8171,7 @@
         <v>721</v>
       </c>
       <c r="J93">
-        <v>442</v>
+        <v>446</v>
       </c>
     </row>
     <row r="94" spans="1:10">
@@ -8203,7 +8203,7 @@
         <v>2663</v>
       </c>
       <c r="J94">
-        <v>1390</v>
+        <v>1406</v>
       </c>
     </row>
     <row r="95" spans="1:10">
@@ -8235,7 +8235,7 @@
         <v>1389</v>
       </c>
       <c r="J95">
-        <v>851</v>
+        <v>856</v>
       </c>
     </row>
     <row r="96" spans="1:10">
@@ -8267,7 +8267,7 @@
         <v>1669</v>
       </c>
       <c r="J96">
-        <v>928</v>
+        <v>933</v>
       </c>
     </row>
     <row r="97" spans="1:10">
@@ -8299,7 +8299,7 @@
         <v>1673</v>
       </c>
       <c r="J97">
-        <v>974</v>
+        <v>976</v>
       </c>
     </row>
     <row r="98" spans="1:10">
@@ -8331,7 +8331,7 @@
         <v>1318</v>
       </c>
       <c r="J98">
-        <v>678</v>
+        <v>684</v>
       </c>
     </row>
     <row r="99" spans="1:10">
@@ -8363,7 +8363,7 @@
         <v>1488</v>
       </c>
       <c r="J99">
-        <v>913</v>
+        <v>925</v>
       </c>
     </row>
     <row r="100" spans="1:10">
@@ -8395,7 +8395,7 @@
         <v>237</v>
       </c>
       <c r="J100">
-        <v>170</v>
+        <v>171</v>
       </c>
     </row>
     <row r="101" spans="1:10">
@@ -8412,7 +8412,7 @@
         <v>117356</v>
       </c>
       <c r="E101">
-        <v>113392</v>
+        <v>113393</v>
       </c>
       <c r="F101">
         <v>105560</v>
@@ -8421,13 +8421,13 @@
         <v>85314</v>
       </c>
       <c r="H101">
-        <v>84594</v>
+        <v>84595</v>
       </c>
       <c r="I101">
         <v>110482</v>
       </c>
       <c r="J101">
-        <v>65248</v>
+        <v>65605</v>
       </c>
     </row>
   </sheetData>
@@ -8711,7 +8711,7 @@
         <v>121</v>
       </c>
       <c r="J5">
-        <v>70</v>
+        <v>71</v>
       </c>
     </row>
     <row r="6" spans="1:10">
@@ -8795,7 +8795,7 @@
         <v>219</v>
       </c>
       <c r="J8">
-        <v>123</v>
+        <v>124</v>
       </c>
     </row>
     <row r="9" spans="1:10">
@@ -8827,7 +8827,7 @@
         <v>97</v>
       </c>
       <c r="J9">
-        <v>63</v>
+        <v>64</v>
       </c>
     </row>
     <row r="10" spans="1:10">
@@ -8859,7 +8859,7 @@
         <v>1135</v>
       </c>
       <c r="J10">
-        <v>634</v>
+        <v>637</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -8891,7 +8891,7 @@
         <v>1648</v>
       </c>
       <c r="J11">
-        <v>933</v>
+        <v>939</v>
       </c>
     </row>
   </sheetData>
@@ -8980,7 +8980,7 @@
         <v>327</v>
       </c>
       <c r="J2">
-        <v>166</v>
+        <v>167</v>
       </c>
     </row>
     <row r="3" spans="1:10">
@@ -9012,7 +9012,7 @@
         <v>439</v>
       </c>
       <c r="J3">
-        <v>242</v>
+        <v>244</v>
       </c>
     </row>
     <row r="4" spans="1:10">
@@ -9076,7 +9076,7 @@
         <v>381</v>
       </c>
       <c r="J5">
-        <v>169</v>
+        <v>170</v>
       </c>
     </row>
     <row r="6" spans="1:10">
@@ -9172,7 +9172,7 @@
         <v>1026</v>
       </c>
       <c r="J8">
-        <v>809</v>
+        <v>810</v>
       </c>
     </row>
     <row r="9" spans="1:10">
@@ -9204,7 +9204,7 @@
         <v>303</v>
       </c>
       <c r="J9">
-        <v>186</v>
+        <v>187</v>
       </c>
     </row>
     <row r="10" spans="1:10">
@@ -9236,7 +9236,7 @@
         <v>1271</v>
       </c>
       <c r="J10">
-        <v>726</v>
+        <v>731</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -9268,7 +9268,7 @@
         <v>3848</v>
       </c>
       <c r="J11">
-        <v>2374</v>
+        <v>2385</v>
       </c>
     </row>
   </sheetData>
@@ -9389,7 +9389,7 @@
         <v>80</v>
       </c>
       <c r="J3">
-        <v>42</v>
+        <v>44</v>
       </c>
     </row>
     <row r="4" spans="1:10">
@@ -9546,7 +9546,7 @@
         <v>336</v>
       </c>
       <c r="J8">
-        <v>176</v>
+        <v>178</v>
       </c>
     </row>
     <row r="9" spans="1:10">
@@ -9610,7 +9610,7 @@
         <v>2132</v>
       </c>
       <c r="J10">
-        <v>1215</v>
+        <v>1220</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -9642,7 +9642,7 @@
         <v>2923</v>
       </c>
       <c r="J11">
-        <v>1686</v>
+        <v>1695</v>
       </c>
     </row>
   </sheetData>
@@ -9763,7 +9763,7 @@
         <v>35</v>
       </c>
       <c r="J3">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="4" spans="1:10">
@@ -9914,7 +9914,7 @@
         <v>280</v>
       </c>
       <c r="J8">
-        <v>303</v>
+        <v>304</v>
       </c>
     </row>
     <row r="9" spans="1:10">
@@ -9946,7 +9946,7 @@
         <v>156</v>
       </c>
       <c r="J9">
-        <v>68</v>
+        <v>69</v>
       </c>
     </row>
     <row r="10" spans="1:10">
@@ -9978,7 +9978,7 @@
         <v>1034</v>
       </c>
       <c r="J10">
-        <v>483</v>
+        <v>484</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -10010,7 +10010,7 @@
         <v>1673</v>
       </c>
       <c r="J11">
-        <v>974</v>
+        <v>976</v>
       </c>
     </row>
   </sheetData>
@@ -10131,7 +10131,7 @@
         <v>365</v>
       </c>
       <c r="J3">
-        <v>232</v>
+        <v>234</v>
       </c>
     </row>
     <row r="4" spans="1:10">
@@ -10259,7 +10259,7 @@
         <v>29</v>
       </c>
       <c r="J7">
-        <v>15</v>
+        <v>16</v>
       </c>
     </row>
     <row r="8" spans="1:10">
@@ -10291,7 +10291,7 @@
         <v>516</v>
       </c>
       <c r="J8">
-        <v>391</v>
+        <v>393</v>
       </c>
     </row>
     <row r="9" spans="1:10">
@@ -10355,7 +10355,7 @@
         <v>895</v>
       </c>
       <c r="J10">
-        <v>481</v>
+        <v>483</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -10387,7 +10387,7 @@
         <v>2510</v>
       </c>
       <c r="J11">
-        <v>1524</v>
+        <v>1531</v>
       </c>
     </row>
   </sheetData>
@@ -10508,7 +10508,7 @@
         <v>137</v>
       </c>
       <c r="J3">
-        <v>72</v>
+        <v>73</v>
       </c>
     </row>
     <row r="4" spans="1:10">
@@ -10572,7 +10572,7 @@
         <v>154</v>
       </c>
       <c r="J5">
-        <v>42</v>
+        <v>43</v>
       </c>
     </row>
     <row r="6" spans="1:10">
@@ -10668,7 +10668,7 @@
         <v>392</v>
       </c>
       <c r="J8">
-        <v>294</v>
+        <v>295</v>
       </c>
     </row>
     <row r="9" spans="1:10">
@@ -10732,7 +10732,7 @@
         <v>433</v>
       </c>
       <c r="J10">
-        <v>281</v>
+        <v>283</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -10764,7 +10764,7 @@
         <v>1389</v>
       </c>
       <c r="J11">
-        <v>851</v>
+        <v>856</v>
       </c>
     </row>
   </sheetData>
@@ -11109,7 +11109,7 @@
         <v>271</v>
       </c>
       <c r="J10">
-        <v>144</v>
+        <v>145</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -11141,7 +11141,7 @@
         <v>729</v>
       </c>
       <c r="J11">
-        <v>482</v>
+        <v>483</v>
       </c>
     </row>
   </sheetData>
@@ -11326,7 +11326,7 @@
         <v>81</v>
       </c>
       <c r="J5">
-        <v>45</v>
+        <v>46</v>
       </c>
     </row>
     <row r="6" spans="1:10">
@@ -11422,7 +11422,7 @@
         <v>218</v>
       </c>
       <c r="J8">
-        <v>202</v>
+        <v>203</v>
       </c>
     </row>
     <row r="9" spans="1:10">
@@ -11486,7 +11486,7 @@
         <v>590</v>
       </c>
       <c r="J10">
-        <v>380</v>
+        <v>383</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -11518,7 +11518,7 @@
         <v>1491</v>
       </c>
       <c r="J11">
-        <v>1044</v>
+        <v>1049</v>
       </c>
     </row>
   </sheetData>
@@ -11799,7 +11799,7 @@
         <v>184</v>
       </c>
       <c r="J8">
-        <v>151</v>
+        <v>153</v>
       </c>
     </row>
     <row r="9" spans="1:10">
@@ -11895,7 +11895,7 @@
         <v>943</v>
       </c>
       <c r="J11">
-        <v>577</v>
+        <v>579</v>
       </c>
     </row>
   </sheetData>
@@ -12141,7 +12141,7 @@
         <v>8</v>
       </c>
       <c r="J7">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="8" spans="1:10">
@@ -12173,7 +12173,7 @@
         <v>401</v>
       </c>
       <c r="J8">
-        <v>231</v>
+        <v>234</v>
       </c>
     </row>
     <row r="9" spans="1:10">
@@ -12205,7 +12205,7 @@
         <v>243</v>
       </c>
       <c r="J9">
-        <v>142</v>
+        <v>143</v>
       </c>
     </row>
     <row r="10" spans="1:10">
@@ -12237,7 +12237,7 @@
         <v>2528</v>
       </c>
       <c r="J10">
-        <v>1425</v>
+        <v>1437</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -12269,7 +12269,7 @@
         <v>3507</v>
       </c>
       <c r="J11">
-        <v>1988</v>
+        <v>2005</v>
       </c>
     </row>
   </sheetData>
@@ -12550,7 +12550,7 @@
         <v>503</v>
       </c>
       <c r="J8">
-        <v>358</v>
+        <v>359</v>
       </c>
     </row>
     <row r="9" spans="1:10">
@@ -12614,7 +12614,7 @@
         <v>527</v>
       </c>
       <c r="J10">
-        <v>321</v>
+        <v>323</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -12646,7 +12646,7 @@
         <v>1491</v>
       </c>
       <c r="J11">
-        <v>933</v>
+        <v>936</v>
       </c>
     </row>
   </sheetData>
@@ -12735,7 +12735,7 @@
         <v>239</v>
       </c>
       <c r="J2">
-        <v>139</v>
+        <v>140</v>
       </c>
     </row>
     <row r="3" spans="1:10">
@@ -12767,7 +12767,7 @@
         <v>261</v>
       </c>
       <c r="J3">
-        <v>165</v>
+        <v>167</v>
       </c>
     </row>
     <row r="4" spans="1:10">
@@ -12927,7 +12927,7 @@
         <v>722</v>
       </c>
       <c r="J8">
-        <v>498</v>
+        <v>501</v>
       </c>
     </row>
     <row r="9" spans="1:10">
@@ -12991,7 +12991,7 @@
         <v>813</v>
       </c>
       <c r="J10">
-        <v>471</v>
+        <v>478</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -13023,7 +13023,7 @@
         <v>2547</v>
       </c>
       <c r="J11">
-        <v>1582</v>
+        <v>1595</v>
       </c>
     </row>
   </sheetData>
@@ -13112,7 +13112,7 @@
         <v>30</v>
       </c>
       <c r="J2">
-        <v>20</v>
+        <v>21</v>
       </c>
     </row>
     <row r="3" spans="1:10">
@@ -13379,7 +13379,7 @@
         <v>418</v>
       </c>
       <c r="J11">
-        <v>298</v>
+        <v>299</v>
       </c>
     </row>
   </sheetData>
@@ -13709,7 +13709,7 @@
         <v>448</v>
       </c>
       <c r="J10">
-        <v>225</v>
+        <v>228</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -13741,7 +13741,7 @@
         <v>706</v>
       </c>
       <c r="J11">
-        <v>385</v>
+        <v>388</v>
       </c>
     </row>
   </sheetData>
@@ -13862,7 +13862,7 @@
         <v>182</v>
       </c>
       <c r="J3">
-        <v>120</v>
+        <v>121</v>
       </c>
     </row>
     <row r="4" spans="1:10">
@@ -14022,7 +14022,7 @@
         <v>202</v>
       </c>
       <c r="J8">
-        <v>217</v>
+        <v>218</v>
       </c>
     </row>
     <row r="9" spans="1:10">
@@ -14086,7 +14086,7 @@
         <v>587</v>
       </c>
       <c r="J10">
-        <v>342</v>
+        <v>344</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -14118,7 +14118,7 @@
         <v>1515</v>
       </c>
       <c r="J11">
-        <v>1014</v>
+        <v>1018</v>
       </c>
     </row>
   </sheetData>
@@ -14734,7 +14734,7 @@
         <v>175</v>
       </c>
       <c r="J8">
-        <v>152</v>
+        <v>153</v>
       </c>
     </row>
     <row r="9" spans="1:10">
@@ -14830,7 +14830,7 @@
         <v>768</v>
       </c>
       <c r="J11">
-        <v>471</v>
+        <v>472</v>
       </c>
     </row>
   </sheetData>
@@ -14951,7 +14951,7 @@
         <v>23</v>
       </c>
       <c r="J3">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="4" spans="1:10">
@@ -15160,7 +15160,7 @@
         <v>255</v>
       </c>
       <c r="J10">
-        <v>111</v>
+        <v>113</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -15192,7 +15192,7 @@
         <v>437</v>
       </c>
       <c r="J11">
-        <v>201</v>
+        <v>204</v>
       </c>
     </row>
   </sheetData>
@@ -15281,7 +15281,7 @@
         <v>190</v>
       </c>
       <c r="J2">
-        <v>98</v>
+        <v>99</v>
       </c>
     </row>
     <row r="3" spans="1:10">
@@ -15473,7 +15473,7 @@
         <v>484</v>
       </c>
       <c r="J8">
-        <v>281</v>
+        <v>283</v>
       </c>
     </row>
     <row r="9" spans="1:10">
@@ -15537,7 +15537,7 @@
         <v>612</v>
       </c>
       <c r="J10">
-        <v>329</v>
+        <v>331</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -15569,7 +15569,7 @@
         <v>1793</v>
       </c>
       <c r="J11">
-        <v>1000</v>
+        <v>1005</v>
       </c>
     </row>
   </sheetData>
@@ -15690,7 +15690,7 @@
         <v>90</v>
       </c>
       <c r="J3">
-        <v>39</v>
+        <v>40</v>
       </c>
     </row>
     <row r="4" spans="1:10">
@@ -15914,7 +15914,7 @@
         <v>610</v>
       </c>
       <c r="J10">
-        <v>288</v>
+        <v>290</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -15946,7 +15946,7 @@
         <v>1244</v>
       </c>
       <c r="J11">
-        <v>690</v>
+        <v>693</v>
       </c>
     </row>
   </sheetData>
@@ -16212,7 +16212,7 @@
         <v>294</v>
       </c>
       <c r="J8">
-        <v>214</v>
+        <v>216</v>
       </c>
     </row>
     <row r="9" spans="1:10">
@@ -16244,7 +16244,7 @@
         <v>147</v>
       </c>
       <c r="J9">
-        <v>71</v>
+        <v>72</v>
       </c>
     </row>
     <row r="10" spans="1:10">
@@ -16276,7 +16276,7 @@
         <v>2021</v>
       </c>
       <c r="J10">
-        <v>986</v>
+        <v>999</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -16308,7 +16308,7 @@
         <v>2663</v>
       </c>
       <c r="J11">
-        <v>1390</v>
+        <v>1406</v>
       </c>
     </row>
   </sheetData>
@@ -16397,7 +16397,7 @@
         <v>267</v>
       </c>
       <c r="J2">
-        <v>175</v>
+        <v>176</v>
       </c>
     </row>
     <row r="3" spans="1:10">
@@ -16429,7 +16429,7 @@
         <v>416</v>
       </c>
       <c r="J3">
-        <v>224</v>
+        <v>225</v>
       </c>
     </row>
     <row r="4" spans="1:10">
@@ -16493,7 +16493,7 @@
         <v>170</v>
       </c>
       <c r="J5">
-        <v>66</v>
+        <v>68</v>
       </c>
     </row>
     <row r="6" spans="1:10">
@@ -16589,7 +16589,7 @@
         <v>707</v>
       </c>
       <c r="J8">
-        <v>563</v>
+        <v>567</v>
       </c>
     </row>
     <row r="9" spans="1:10">
@@ -16621,7 +16621,7 @@
         <v>363</v>
       </c>
       <c r="J9">
-        <v>217</v>
+        <v>218</v>
       </c>
     </row>
     <row r="10" spans="1:10">
@@ -16685,7 +16685,7 @@
         <v>3011</v>
       </c>
       <c r="J11">
-        <v>1867</v>
+        <v>1876</v>
       </c>
     </row>
   </sheetData>
@@ -16806,7 +16806,7 @@
         <v>248</v>
       </c>
       <c r="J3">
-        <v>129</v>
+        <v>130</v>
       </c>
     </row>
     <row r="4" spans="1:10">
@@ -16870,7 +16870,7 @@
         <v>261</v>
       </c>
       <c r="J5">
-        <v>137</v>
+        <v>140</v>
       </c>
     </row>
     <row r="6" spans="1:10">
@@ -16934,7 +16934,7 @@
         <v>36</v>
       </c>
       <c r="J7">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="8" spans="1:10">
@@ -16966,7 +16966,7 @@
         <v>567</v>
       </c>
       <c r="J8">
-        <v>559</v>
+        <v>562</v>
       </c>
     </row>
     <row r="9" spans="1:10">
@@ -17030,7 +17030,7 @@
         <v>1023</v>
       </c>
       <c r="J10">
-        <v>504</v>
+        <v>509</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -17062,7 +17062,7 @@
         <v>2686</v>
       </c>
       <c r="J11">
-        <v>1644</v>
+        <v>1657</v>
       </c>
     </row>
   </sheetData>
@@ -17151,7 +17151,7 @@
         <v>457</v>
       </c>
       <c r="J2">
-        <v>277</v>
+        <v>278</v>
       </c>
     </row>
     <row r="3" spans="1:10">
@@ -17183,7 +17183,7 @@
         <v>445</v>
       </c>
       <c r="J3">
-        <v>300</v>
+        <v>304</v>
       </c>
     </row>
     <row r="4" spans="1:10">
@@ -17247,7 +17247,7 @@
         <v>251</v>
       </c>
       <c r="J5">
-        <v>117</v>
+        <v>118</v>
       </c>
     </row>
     <row r="6" spans="1:10">
@@ -17264,7 +17264,7 @@
         <v>90</v>
       </c>
       <c r="E6">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="F6">
         <v>102</v>
@@ -17343,7 +17343,7 @@
         <v>1269</v>
       </c>
       <c r="J8">
-        <v>746</v>
+        <v>752</v>
       </c>
     </row>
     <row r="9" spans="1:10">
@@ -17375,7 +17375,7 @@
         <v>497</v>
       </c>
       <c r="J9">
-        <v>308</v>
+        <v>311</v>
       </c>
     </row>
     <row r="10" spans="1:10">
@@ -17407,7 +17407,7 @@
         <v>1652</v>
       </c>
       <c r="J10">
-        <v>908</v>
+        <v>910</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -17424,7 +17424,7 @@
         <v>5095</v>
       </c>
       <c r="E11">
-        <v>5162</v>
+        <v>5163</v>
       </c>
       <c r="F11">
         <v>5008</v>
@@ -17439,7 +17439,7 @@
         <v>4743</v>
       </c>
       <c r="J11">
-        <v>2763</v>
+        <v>2780</v>
       </c>
     </row>
   </sheetData>
@@ -17720,7 +17720,7 @@
         <v>441</v>
       </c>
       <c r="J8">
-        <v>336</v>
+        <v>337</v>
       </c>
     </row>
     <row r="9" spans="1:10">
@@ -17784,7 +17784,7 @@
         <v>455</v>
       </c>
       <c r="J10">
-        <v>296</v>
+        <v>299</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -17816,7 +17816,7 @@
         <v>1354</v>
       </c>
       <c r="J11">
-        <v>853</v>
+        <v>857</v>
       </c>
     </row>
   </sheetData>
@@ -17905,7 +17905,7 @@
         <v>47</v>
       </c>
       <c r="J2">
-        <v>27</v>
+        <v>28</v>
       </c>
     </row>
     <row r="3" spans="1:10">
@@ -18088,7 +18088,7 @@
         <v>250</v>
       </c>
       <c r="J8">
-        <v>179</v>
+        <v>180</v>
       </c>
     </row>
     <row r="9" spans="1:10">
@@ -18152,7 +18152,7 @@
         <v>417</v>
       </c>
       <c r="J10">
-        <v>235</v>
+        <v>237</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -18184,7 +18184,7 @@
         <v>903</v>
       </c>
       <c r="J11">
-        <v>548</v>
+        <v>552</v>
       </c>
     </row>
   </sheetData>
@@ -18369,7 +18369,7 @@
         <v>229</v>
       </c>
       <c r="J5">
-        <v>106</v>
+        <v>107</v>
       </c>
     </row>
     <row r="6" spans="1:10">
@@ -18465,7 +18465,7 @@
         <v>754</v>
       </c>
       <c r="J8">
-        <v>427</v>
+        <v>429</v>
       </c>
     </row>
     <row r="9" spans="1:10">
@@ -18529,7 +18529,7 @@
         <v>911</v>
       </c>
       <c r="J10">
-        <v>540</v>
+        <v>542</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -18561,7 +18561,7 @@
         <v>2636</v>
       </c>
       <c r="J11">
-        <v>1521</v>
+        <v>1526</v>
       </c>
     </row>
   </sheetData>
@@ -18879,7 +18879,7 @@
         <v>94</v>
       </c>
       <c r="J10">
-        <v>59</v>
+        <v>60</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -18911,7 +18911,7 @@
         <v>247</v>
       </c>
       <c r="J11">
-        <v>168</v>
+        <v>169</v>
       </c>
     </row>
   </sheetData>
@@ -19000,7 +19000,7 @@
         <v>179</v>
       </c>
       <c r="J2">
-        <v>92</v>
+        <v>93</v>
       </c>
     </row>
     <row r="3" spans="1:10">
@@ -19032,7 +19032,7 @@
         <v>177</v>
       </c>
       <c r="J3">
-        <v>99</v>
+        <v>100</v>
       </c>
     </row>
     <row r="4" spans="1:10">
@@ -19160,7 +19160,7 @@
         <v>18</v>
       </c>
       <c r="J7">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="8" spans="1:10">
@@ -19192,7 +19192,7 @@
         <v>363</v>
       </c>
       <c r="J8">
-        <v>278</v>
+        <v>280</v>
       </c>
     </row>
     <row r="9" spans="1:10">
@@ -19224,7 +19224,7 @@
         <v>224</v>
       </c>
       <c r="J9">
-        <v>79</v>
+        <v>81</v>
       </c>
     </row>
     <row r="10" spans="1:10">
@@ -19256,7 +19256,7 @@
         <v>828</v>
       </c>
       <c r="J10">
-        <v>427</v>
+        <v>433</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -19288,7 +19288,7 @@
         <v>2045</v>
       </c>
       <c r="J11">
-        <v>1086</v>
+        <v>1099</v>
       </c>
     </row>
   </sheetData>
@@ -19919,7 +19919,7 @@
         <v>68</v>
       </c>
       <c r="J8">
-        <v>60</v>
+        <v>62</v>
       </c>
     </row>
     <row r="9" spans="1:10">
@@ -20015,7 +20015,7 @@
         <v>271</v>
       </c>
       <c r="J11">
-        <v>178</v>
+        <v>180</v>
       </c>
     </row>
   </sheetData>
@@ -20296,7 +20296,7 @@
         <v>308</v>
       </c>
       <c r="J8">
-        <v>226</v>
+        <v>227</v>
       </c>
     </row>
     <row r="9" spans="1:10">
@@ -20360,7 +20360,7 @@
         <v>320</v>
       </c>
       <c r="J10">
-        <v>183</v>
+        <v>185</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -20392,7 +20392,7 @@
         <v>970</v>
       </c>
       <c r="J11">
-        <v>616</v>
+        <v>619</v>
       </c>
     </row>
   </sheetData>
@@ -20577,7 +20577,7 @@
         <v>64</v>
       </c>
       <c r="J5">
-        <v>47</v>
+        <v>49</v>
       </c>
     </row>
     <row r="6" spans="1:10">
@@ -20667,7 +20667,7 @@
         <v>122</v>
       </c>
       <c r="J8">
-        <v>128</v>
+        <v>130</v>
       </c>
     </row>
     <row r="9" spans="1:10">
@@ -20763,7 +20763,7 @@
         <v>721</v>
       </c>
       <c r="J11">
-        <v>442</v>
+        <v>446</v>
       </c>
     </row>
   </sheetData>
@@ -20852,7 +20852,7 @@
         <v>19</v>
       </c>
       <c r="J2">
-        <v>16</v>
+        <v>17</v>
       </c>
     </row>
     <row r="3" spans="1:10">
@@ -21023,7 +21023,7 @@
         <v>44</v>
       </c>
       <c r="J8">
-        <v>46</v>
+        <v>47</v>
       </c>
     </row>
     <row r="9" spans="1:10">
@@ -21087,7 +21087,7 @@
         <v>280</v>
       </c>
       <c r="J10">
-        <v>138</v>
+        <v>140</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -21119,7 +21119,7 @@
         <v>436</v>
       </c>
       <c r="J11">
-        <v>270</v>
+        <v>274</v>
       </c>
     </row>
   </sheetData>
@@ -21765,7 +21765,7 @@
         <v>297</v>
       </c>
       <c r="J8">
-        <v>278</v>
+        <v>280</v>
       </c>
     </row>
     <row r="9" spans="1:10">
@@ -21861,7 +21861,7 @@
         <v>1337</v>
       </c>
       <c r="J11">
-        <v>871</v>
+        <v>873</v>
       </c>
     </row>
   </sheetData>
@@ -21950,7 +21950,7 @@
         <v>80</v>
       </c>
       <c r="J2">
-        <v>30</v>
+        <v>31</v>
       </c>
     </row>
     <row r="3" spans="1:10">
@@ -22142,7 +22142,7 @@
         <v>125</v>
       </c>
       <c r="J8">
-        <v>78</v>
+        <v>79</v>
       </c>
     </row>
     <row r="9" spans="1:10">
@@ -22206,7 +22206,7 @@
         <v>492</v>
       </c>
       <c r="J10">
-        <v>317</v>
+        <v>318</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -22238,7 +22238,7 @@
         <v>917</v>
       </c>
       <c r="J11">
-        <v>556</v>
+        <v>559</v>
       </c>
     </row>
   </sheetData>
@@ -22492,7 +22492,7 @@
         <v>89</v>
       </c>
       <c r="J8">
-        <v>61</v>
+        <v>62</v>
       </c>
     </row>
     <row r="9" spans="1:10">
@@ -22556,7 +22556,7 @@
         <v>205</v>
       </c>
       <c r="J10">
-        <v>97</v>
+        <v>98</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -22588,7 +22588,7 @@
         <v>412</v>
       </c>
       <c r="J11">
-        <v>227</v>
+        <v>229</v>
       </c>
     </row>
   </sheetData>
@@ -22773,7 +22773,7 @@
         <v>49</v>
       </c>
       <c r="J5">
-        <v>28</v>
+        <v>29</v>
       </c>
     </row>
     <row r="6" spans="1:10">
@@ -22962,7 +22962,7 @@
         <v>695</v>
       </c>
       <c r="J11">
-        <v>434</v>
+        <v>435</v>
       </c>
     </row>
   </sheetData>
@@ -23147,7 +23147,7 @@
         <v>59</v>
       </c>
       <c r="J5">
-        <v>26</v>
+        <v>27</v>
       </c>
     </row>
     <row r="6" spans="1:10">
@@ -23231,7 +23231,7 @@
         <v>92</v>
       </c>
       <c r="J8">
-        <v>96</v>
+        <v>97</v>
       </c>
     </row>
     <row r="9" spans="1:10">
@@ -23295,7 +23295,7 @@
         <v>277</v>
       </c>
       <c r="J10">
-        <v>174</v>
+        <v>176</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -23327,7 +23327,7 @@
         <v>500</v>
       </c>
       <c r="J11">
-        <v>344</v>
+        <v>348</v>
       </c>
     </row>
   </sheetData>
@@ -23416,7 +23416,7 @@
         <v>50</v>
       </c>
       <c r="J2">
-        <v>34</v>
+        <v>35</v>
       </c>
     </row>
     <row r="3" spans="1:10">
@@ -23448,7 +23448,7 @@
         <v>35</v>
       </c>
       <c r="J3">
-        <v>20</v>
+        <v>21</v>
       </c>
     </row>
     <row r="4" spans="1:10">
@@ -23605,7 +23605,7 @@
         <v>72</v>
       </c>
       <c r="J8">
-        <v>47</v>
+        <v>48</v>
       </c>
     </row>
     <row r="9" spans="1:10">
@@ -23669,7 +23669,7 @@
         <v>189</v>
       </c>
       <c r="J10">
-        <v>128</v>
+        <v>130</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -23701,7 +23701,7 @@
         <v>429</v>
       </c>
       <c r="J11">
-        <v>264</v>
+        <v>269</v>
       </c>
     </row>
   </sheetData>
@@ -23979,7 +23979,7 @@
         <v>178</v>
       </c>
       <c r="J8">
-        <v>191</v>
+        <v>192</v>
       </c>
     </row>
     <row r="9" spans="1:10">
@@ -24043,7 +24043,7 @@
         <v>349</v>
       </c>
       <c r="J10">
-        <v>217</v>
+        <v>216</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -24408,7 +24408,7 @@
         <v>216</v>
       </c>
       <c r="J10">
-        <v>111</v>
+        <v>112</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -24440,7 +24440,7 @@
         <v>396</v>
       </c>
       <c r="J11">
-        <v>226</v>
+        <v>227</v>
       </c>
     </row>
   </sheetData>
@@ -24709,7 +24709,7 @@
         <v>167</v>
       </c>
       <c r="J8">
-        <v>121</v>
+        <v>122</v>
       </c>
     </row>
     <row r="9" spans="1:10">
@@ -24773,7 +24773,7 @@
         <v>784</v>
       </c>
       <c r="J10">
-        <v>494</v>
+        <v>496</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -24805,7 +24805,7 @@
         <v>1258</v>
       </c>
       <c r="J11">
-        <v>773</v>
+        <v>776</v>
       </c>
     </row>
   </sheetData>
@@ -24894,7 +24894,7 @@
         <v>78</v>
       </c>
       <c r="J2">
-        <v>42</v>
+        <v>43</v>
       </c>
     </row>
     <row r="3" spans="1:10">
@@ -25118,7 +25118,7 @@
         <v>101</v>
       </c>
       <c r="J9">
-        <v>29</v>
+        <v>30</v>
       </c>
     </row>
     <row r="10" spans="1:10">
@@ -25150,7 +25150,7 @@
         <v>381</v>
       </c>
       <c r="J10">
-        <v>204</v>
+        <v>206</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -25182,7 +25182,7 @@
         <v>867</v>
       </c>
       <c r="J11">
-        <v>483</v>
+        <v>487</v>
       </c>
     </row>
   </sheetData>
@@ -25479,7 +25479,7 @@
         <v>576</v>
       </c>
       <c r="J10">
-        <v>306</v>
+        <v>308</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -25511,7 +25511,7 @@
         <v>628</v>
       </c>
       <c r="J11">
-        <v>330</v>
+        <v>332</v>
       </c>
     </row>
   </sheetData>
@@ -25792,7 +25792,7 @@
         <v>132</v>
       </c>
       <c r="J8">
-        <v>84</v>
+        <v>85</v>
       </c>
     </row>
     <row r="9" spans="1:10">
@@ -25856,7 +25856,7 @@
         <v>130</v>
       </c>
       <c r="J10">
-        <v>84</v>
+        <v>85</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -25888,7 +25888,7 @@
         <v>462</v>
       </c>
       <c r="J11">
-        <v>304</v>
+        <v>306</v>
       </c>
     </row>
   </sheetData>
@@ -26025,6 +26025,9 @@
       <c r="G4">
         <v>3</v>
       </c>
+      <c r="J4">
+        <v>1</v>
+      </c>
     </row>
     <row r="5" spans="1:10">
       <c r="A5" s="1" t="s">
@@ -26180,7 +26183,7 @@
         <v>139</v>
       </c>
       <c r="J9">
-        <v>82</v>
+        <v>83</v>
       </c>
     </row>
     <row r="10" spans="1:10">
@@ -26212,7 +26215,7 @@
         <v>233</v>
       </c>
       <c r="J10">
-        <v>154</v>
+        <v>156</v>
       </c>
     </row>
   </sheetData>
@@ -26333,7 +26336,7 @@
         <v>87</v>
       </c>
       <c r="J3">
-        <v>67</v>
+        <v>68</v>
       </c>
     </row>
     <row r="4" spans="1:10">
@@ -26397,7 +26400,7 @@
         <v>130</v>
       </c>
       <c r="J5">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="6" spans="1:10">
@@ -26493,7 +26496,7 @@
         <v>198</v>
       </c>
       <c r="J8">
-        <v>158</v>
+        <v>159</v>
       </c>
     </row>
     <row r="9" spans="1:10">
@@ -26557,7 +26560,7 @@
         <v>1118</v>
       </c>
       <c r="J10">
-        <v>598</v>
+        <v>600</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -26589,7 +26592,7 @@
         <v>1797</v>
       </c>
       <c r="J11">
-        <v>1018</v>
+        <v>1021</v>
       </c>
     </row>
   </sheetData>
@@ -27130,7 +27133,7 @@
         <v>74</v>
       </c>
       <c r="J5">
-        <v>59</v>
+        <v>60</v>
       </c>
     </row>
     <row r="6" spans="1:10">
@@ -27304,7 +27307,7 @@
         <v>715</v>
       </c>
       <c r="J11">
-        <v>433</v>
+        <v>434</v>
       </c>
     </row>
   </sheetData>
@@ -27393,7 +27396,7 @@
         <v>14</v>
       </c>
       <c r="J2">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="3" spans="1:10">
@@ -27616,7 +27619,7 @@
         <v>376</v>
       </c>
       <c r="J10">
-        <v>263</v>
+        <v>264</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -27648,7 +27651,7 @@
         <v>595</v>
       </c>
       <c r="J11">
-        <v>425</v>
+        <v>427</v>
       </c>
     </row>
   </sheetData>
@@ -27929,7 +27932,7 @@
         <v>141</v>
       </c>
       <c r="J8">
-        <v>105</v>
+        <v>107</v>
       </c>
     </row>
     <row r="9" spans="1:10">
@@ -27961,7 +27964,7 @@
         <v>40</v>
       </c>
       <c r="J9">
-        <v>27</v>
+        <v>28</v>
       </c>
     </row>
     <row r="10" spans="1:10">
@@ -28025,7 +28028,7 @@
         <v>519</v>
       </c>
       <c r="J11">
-        <v>302</v>
+        <v>305</v>
       </c>
     </row>
   </sheetData>
@@ -28560,7 +28563,7 @@
         <v>79</v>
       </c>
       <c r="J5">
-        <v>39</v>
+        <v>40</v>
       </c>
     </row>
     <row r="6" spans="1:10">
@@ -28717,7 +28720,7 @@
         <v>542</v>
       </c>
       <c r="J10">
-        <v>297</v>
+        <v>300</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -28749,7 +28752,7 @@
         <v>948</v>
       </c>
       <c r="J11">
-        <v>530</v>
+        <v>534</v>
       </c>
     </row>
   </sheetData>
@@ -29056,7 +29059,7 @@
         <v>35</v>
       </c>
       <c r="J9">
-        <v>46</v>
+        <v>47</v>
       </c>
     </row>
     <row r="10" spans="1:10">
@@ -29120,7 +29123,7 @@
         <v>437</v>
       </c>
       <c r="J11">
-        <v>320</v>
+        <v>321</v>
       </c>
     </row>
   </sheetData>
@@ -29209,7 +29212,7 @@
         <v>77</v>
       </c>
       <c r="J2">
-        <v>63</v>
+        <v>64</v>
       </c>
     </row>
     <row r="3" spans="1:10">
@@ -29305,7 +29308,7 @@
         <v>131</v>
       </c>
       <c r="J5">
-        <v>77</v>
+        <v>78</v>
       </c>
     </row>
     <row r="6" spans="1:10">
@@ -29337,7 +29340,7 @@
         <v>42</v>
       </c>
       <c r="J6">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="7" spans="1:10">
@@ -29430,7 +29433,7 @@
         <v>107</v>
       </c>
       <c r="J9">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="10" spans="1:10">
@@ -29462,7 +29465,7 @@
         <v>1222</v>
       </c>
       <c r="J10">
-        <v>671</v>
+        <v>675</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -29494,7 +29497,7 @@
         <v>1879</v>
       </c>
       <c r="J11">
-        <v>1141</v>
+        <v>1147</v>
       </c>
     </row>
   </sheetData>
@@ -29583,7 +29586,7 @@
         <v>46</v>
       </c>
       <c r="J2">
-        <v>20</v>
+        <v>21</v>
       </c>
     </row>
     <row r="3" spans="1:10">
@@ -29679,7 +29682,7 @@
         <v>66</v>
       </c>
       <c r="J5">
-        <v>31</v>
+        <v>32</v>
       </c>
     </row>
     <row r="6" spans="1:10">
@@ -29804,7 +29807,7 @@
         <v>24</v>
       </c>
       <c r="J9">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="10" spans="1:10">
@@ -29836,7 +29839,7 @@
         <v>440</v>
       </c>
       <c r="J10">
-        <v>263</v>
+        <v>264</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -29868,7 +29871,7 @@
         <v>761</v>
       </c>
       <c r="J11">
-        <v>496</v>
+        <v>498</v>
       </c>
     </row>
   </sheetData>
@@ -29957,7 +29960,7 @@
         <v>128</v>
       </c>
       <c r="J2">
-        <v>61</v>
+        <v>63</v>
       </c>
     </row>
     <row r="3" spans="1:10">
@@ -29989,7 +29992,7 @@
         <v>158</v>
       </c>
       <c r="J3">
-        <v>80</v>
+        <v>84</v>
       </c>
     </row>
     <row r="4" spans="1:10">
@@ -30053,7 +30056,7 @@
         <v>120</v>
       </c>
       <c r="J5">
-        <v>78</v>
+        <v>80</v>
       </c>
     </row>
     <row r="6" spans="1:10">
@@ -30149,7 +30152,7 @@
         <v>383</v>
       </c>
       <c r="J8">
-        <v>299</v>
+        <v>300</v>
       </c>
     </row>
     <row r="9" spans="1:10">
@@ -30213,7 +30216,7 @@
         <v>527</v>
       </c>
       <c r="J10">
-        <v>317</v>
+        <v>320</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -30245,7 +30248,7 @@
         <v>1488</v>
       </c>
       <c r="J11">
-        <v>913</v>
+        <v>925</v>
       </c>
     </row>
   </sheetData>
@@ -30516,7 +30519,7 @@
         <v>22</v>
       </c>
       <c r="J9">
-        <v>19</v>
+        <v>20</v>
       </c>
     </row>
     <row r="10" spans="1:10">
@@ -30548,7 +30551,7 @@
         <v>152</v>
       </c>
       <c r="J10">
-        <v>76</v>
+        <v>78</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -30580,7 +30583,7 @@
         <v>248</v>
       </c>
       <c r="J11">
-        <v>165</v>
+        <v>168</v>
       </c>
     </row>
   </sheetData>
@@ -30889,7 +30892,7 @@
         <v>502</v>
       </c>
       <c r="J10">
-        <v>307</v>
+        <v>311</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -30921,7 +30924,7 @@
         <v>677</v>
       </c>
       <c r="J11">
-        <v>410</v>
+        <v>414</v>
       </c>
     </row>
   </sheetData>
@@ -31224,7 +31227,7 @@
         <v>162</v>
       </c>
       <c r="J10">
-        <v>108</v>
+        <v>109</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -31256,7 +31259,7 @@
         <v>237</v>
       </c>
       <c r="J11">
-        <v>170</v>
+        <v>171</v>
       </c>
     </row>
   </sheetData>
@@ -31522,7 +31525,7 @@
         <v>123</v>
       </c>
       <c r="J8">
-        <v>127</v>
+        <v>128</v>
       </c>
     </row>
     <row r="9" spans="1:10">
@@ -31586,7 +31589,7 @@
         <v>124</v>
       </c>
       <c r="J10">
-        <v>74</v>
+        <v>75</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -31618,7 +31621,7 @@
         <v>335</v>
       </c>
       <c r="J11">
-        <v>255</v>
+        <v>257</v>
       </c>
     </row>
   </sheetData>
@@ -31963,7 +31966,7 @@
         <v>389</v>
       </c>
       <c r="J10">
-        <v>253</v>
+        <v>255</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -31995,7 +31998,7 @@
         <v>886</v>
       </c>
       <c r="J11">
-        <v>579</v>
+        <v>581</v>
       </c>
     </row>
   </sheetData>
@@ -32084,7 +32087,7 @@
         <v>70</v>
       </c>
       <c r="J2">
-        <v>42</v>
+        <v>43</v>
       </c>
     </row>
     <row r="3" spans="1:10">
@@ -32270,7 +32273,7 @@
         <v>405</v>
       </c>
       <c r="J8">
-        <v>349</v>
+        <v>350</v>
       </c>
     </row>
     <row r="9" spans="1:10">
@@ -32302,7 +32305,7 @@
         <v>71</v>
       </c>
       <c r="J9">
-        <v>32</v>
+        <v>33</v>
       </c>
     </row>
     <row r="10" spans="1:10">
@@ -32366,7 +32369,7 @@
         <v>1368</v>
       </c>
       <c r="J11">
-        <v>828</v>
+        <v>831</v>
       </c>
     </row>
   </sheetData>
@@ -32641,7 +32644,7 @@
         <v>338</v>
       </c>
       <c r="J8">
-        <v>258</v>
+        <v>259</v>
       </c>
     </row>
     <row r="9" spans="1:10">
@@ -32673,7 +32676,7 @@
         <v>169</v>
       </c>
       <c r="J9">
-        <v>81</v>
+        <v>84</v>
       </c>
     </row>
     <row r="10" spans="1:10">
@@ -32705,7 +32708,7 @@
         <v>1773</v>
       </c>
       <c r="J10">
-        <v>1013</v>
+        <v>1020</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -32737,7 +32740,7 @@
         <v>2622</v>
       </c>
       <c r="J11">
-        <v>1518</v>
+        <v>1529</v>
       </c>
     </row>
   </sheetData>
@@ -33341,7 +33344,7 @@
         <v>36</v>
       </c>
       <c r="J8">
-        <v>27</v>
+        <v>28</v>
       </c>
     </row>
     <row r="9" spans="1:10">
@@ -33405,7 +33408,7 @@
         <v>174</v>
       </c>
       <c r="J10">
-        <v>76</v>
+        <v>78</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -33437,7 +33440,7 @@
         <v>337</v>
       </c>
       <c r="J11">
-        <v>150</v>
+        <v>153</v>
       </c>
     </row>
   </sheetData>
@@ -33526,7 +33529,7 @@
         <v>58</v>
       </c>
       <c r="J2">
-        <v>28</v>
+        <v>29</v>
       </c>
     </row>
     <row r="3" spans="1:10">
@@ -33709,7 +33712,7 @@
         <v>334</v>
       </c>
       <c r="J8">
-        <v>192</v>
+        <v>193</v>
       </c>
     </row>
     <row r="9" spans="1:10">
@@ -33773,7 +33776,7 @@
         <v>606</v>
       </c>
       <c r="J10">
-        <v>304</v>
+        <v>305</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -33805,7 +33808,7 @@
         <v>1187</v>
       </c>
       <c r="J11">
-        <v>630</v>
+        <v>633</v>
       </c>
     </row>
   </sheetData>
@@ -34436,7 +34439,7 @@
         <v>313</v>
       </c>
       <c r="J10">
-        <v>145</v>
+        <v>151</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -34468,7 +34471,7 @@
         <v>494</v>
       </c>
       <c r="J11">
-        <v>246</v>
+        <v>252</v>
       </c>
     </row>
   </sheetData>
@@ -35072,7 +35075,7 @@
         <v>28</v>
       </c>
       <c r="J9">
-        <v>22</v>
+        <v>23</v>
       </c>
     </row>
     <row r="10" spans="1:10">
@@ -35136,7 +35139,7 @@
         <v>406</v>
       </c>
       <c r="J11">
-        <v>286</v>
+        <v>287</v>
       </c>
     </row>
   </sheetData>
@@ -35257,7 +35260,7 @@
         <v>9</v>
       </c>
       <c r="J3">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="4" spans="1:10">
@@ -35463,7 +35466,7 @@
         <v>181</v>
       </c>
       <c r="J10">
-        <v>85</v>
+        <v>86</v>
       </c>
     </row>
   </sheetData>
@@ -36084,7 +36087,7 @@
         <v>47</v>
       </c>
       <c r="J10">
-        <v>16</v>
+        <v>17</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -36116,7 +36119,7 @@
         <v>99</v>
       </c>
       <c r="J11">
-        <v>34</v>
+        <v>35</v>
       </c>
     </row>
   </sheetData>
@@ -36205,7 +36208,7 @@
         <v>89</v>
       </c>
       <c r="J2">
-        <v>50</v>
+        <v>51</v>
       </c>
     </row>
     <row r="3" spans="1:10">
@@ -36397,7 +36400,7 @@
         <v>291</v>
       </c>
       <c r="J8">
-        <v>193</v>
+        <v>194</v>
       </c>
     </row>
     <row r="9" spans="1:10">
@@ -36429,7 +36432,7 @@
         <v>125</v>
       </c>
       <c r="J9">
-        <v>61</v>
+        <v>62</v>
       </c>
     </row>
     <row r="10" spans="1:10">
@@ -36461,7 +36464,7 @@
         <v>905</v>
       </c>
       <c r="J10">
-        <v>465</v>
+        <v>467</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -36493,7 +36496,7 @@
         <v>1669</v>
       </c>
       <c r="J11">
-        <v>928</v>
+        <v>933</v>
       </c>
     </row>
   </sheetData>
@@ -36768,7 +36771,7 @@
         <v>68</v>
       </c>
       <c r="J8">
-        <v>65</v>
+        <v>66</v>
       </c>
     </row>
     <row r="9" spans="1:10">
@@ -36864,7 +36867,7 @@
         <v>337</v>
       </c>
       <c r="J11">
-        <v>231</v>
+        <v>232</v>
       </c>
     </row>
   </sheetData>
@@ -37453,7 +37456,7 @@
         <v>54</v>
       </c>
       <c r="J8">
-        <v>50</v>
+        <v>51</v>
       </c>
     </row>
     <row r="9" spans="1:10">
@@ -37517,7 +37520,7 @@
         <v>116</v>
       </c>
       <c r="J10">
-        <v>60</v>
+        <v>61</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -37549,7 +37552,7 @@
         <v>236</v>
       </c>
       <c r="J11">
-        <v>154</v>
+        <v>156</v>
       </c>
     </row>
   </sheetData>
@@ -37754,7 +37757,7 @@
         <v>80</v>
       </c>
       <c r="J6">
-        <v>46</v>
+        <v>47</v>
       </c>
     </row>
     <row r="7" spans="1:10">
@@ -37800,7 +37803,7 @@
         <v>160</v>
       </c>
       <c r="J8">
-        <v>63</v>
+        <v>64</v>
       </c>
     </row>
     <row r="9" spans="1:10">
@@ -37896,7 +37899,7 @@
         <v>1066</v>
       </c>
       <c r="J11">
-        <v>486</v>
+        <v>488</v>
       </c>
     </row>
   </sheetData>
@@ -38205,7 +38208,7 @@
         <v>260</v>
       </c>
       <c r="J10">
-        <v>125</v>
+        <v>126</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -38237,7 +38240,7 @@
         <v>393</v>
       </c>
       <c r="J11">
-        <v>178</v>
+        <v>179</v>
       </c>
     </row>
   </sheetData>
@@ -38358,7 +38361,7 @@
         <v>6</v>
       </c>
       <c r="J3">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="4" spans="1:10">
@@ -38534,7 +38537,7 @@
         <v>135</v>
       </c>
       <c r="J10">
-        <v>69</v>
+        <v>70</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -38566,7 +38569,7 @@
         <v>219</v>
       </c>
       <c r="J11">
-        <v>125</v>
+        <v>127</v>
       </c>
     </row>
   </sheetData>
@@ -39503,7 +39506,7 @@
         <v>174</v>
       </c>
       <c r="J10">
-        <v>92</v>
+        <v>93</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -39535,7 +39538,7 @@
         <v>235</v>
       </c>
       <c r="J11">
-        <v>135</v>
+        <v>136</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add data for 2023-07-24
</commit_message>
<xml_diff>
--- a/output/index-crime-full-year.xlsx
+++ b/output/index-crime-full-year.xlsx
@@ -895,7 +895,7 @@
         <v>7277</v>
       </c>
       <c r="J2">
-        <v>4162</v>
+        <v>4185</v>
       </c>
     </row>
     <row r="3" spans="1:10">
@@ -927,7 +927,7 @@
         <v>7486</v>
       </c>
       <c r="J3">
-        <v>4387</v>
+        <v>4407</v>
       </c>
     </row>
     <row r="4" spans="1:10">
@@ -991,7 +991,7 @@
         <v>7592</v>
       </c>
       <c r="J5">
-        <v>4043</v>
+        <v>4063</v>
       </c>
     </row>
     <row r="6" spans="1:10">
@@ -1020,10 +1020,10 @@
         <v>1699</v>
       </c>
       <c r="I6">
-        <v>1768</v>
+        <v>1767</v>
       </c>
       <c r="J6">
-        <v>980</v>
+        <v>986</v>
       </c>
     </row>
     <row r="7" spans="1:10">
@@ -1055,7 +1055,7 @@
         <v>718</v>
       </c>
       <c r="J7">
-        <v>349</v>
+        <v>351</v>
       </c>
     </row>
     <row r="8" spans="1:10">
@@ -1087,7 +1087,7 @@
         <v>21446</v>
       </c>
       <c r="J8">
-        <v>16455</v>
+        <v>16540</v>
       </c>
     </row>
     <row r="9" spans="1:10">
@@ -1119,7 +1119,7 @@
         <v>8965</v>
       </c>
       <c r="J9">
-        <v>5219</v>
+        <v>5243</v>
       </c>
     </row>
     <row r="10" spans="1:10">
@@ -1151,7 +1151,7 @@
         <v>54808</v>
       </c>
       <c r="J10">
-        <v>30114</v>
+        <v>30269</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -1180,10 +1180,10 @@
         <v>84595</v>
       </c>
       <c r="I11">
-        <v>110482</v>
+        <v>110481</v>
       </c>
       <c r="J11">
-        <v>65985</v>
+        <v>66320</v>
       </c>
     </row>
   </sheetData>
@@ -1272,7 +1272,7 @@
         <v>51</v>
       </c>
       <c r="J2">
-        <v>14</v>
+        <v>15</v>
       </c>
     </row>
     <row r="3" spans="1:10">
@@ -1440,7 +1440,7 @@
         <v>227</v>
       </c>
       <c r="J8">
-        <v>214</v>
+        <v>219</v>
       </c>
     </row>
     <row r="9" spans="1:10">
@@ -1472,7 +1472,7 @@
         <v>120</v>
       </c>
       <c r="J9">
-        <v>75</v>
+        <v>76</v>
       </c>
     </row>
     <row r="10" spans="1:10">
@@ -1536,7 +1536,7 @@
         <v>1153</v>
       </c>
       <c r="J11">
-        <v>787</v>
+        <v>794</v>
       </c>
     </row>
   </sheetData>
@@ -2091,7 +2091,7 @@
         <v>373</v>
       </c>
       <c r="J8">
-        <v>284</v>
+        <v>286</v>
       </c>
     </row>
     <row r="9" spans="1:10">
@@ -2155,7 +2155,7 @@
         <v>820</v>
       </c>
       <c r="J10">
-        <v>519</v>
+        <v>520</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -2187,7 +2187,7 @@
         <v>1712</v>
       </c>
       <c r="J11">
-        <v>1124</v>
+        <v>1127</v>
       </c>
     </row>
   </sheetData>
@@ -2462,7 +2462,7 @@
         <v>188</v>
       </c>
       <c r="J8">
-        <v>147</v>
+        <v>148</v>
       </c>
     </row>
     <row r="9" spans="1:10">
@@ -2494,7 +2494,7 @@
         <v>57</v>
       </c>
       <c r="J9">
-        <v>35</v>
+        <v>36</v>
       </c>
     </row>
     <row r="10" spans="1:10">
@@ -2526,7 +2526,7 @@
         <v>712</v>
       </c>
       <c r="J10">
-        <v>405</v>
+        <v>406</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -2558,7 +2558,7 @@
         <v>1228</v>
       </c>
       <c r="J11">
-        <v>727</v>
+        <v>730</v>
       </c>
     </row>
   </sheetData>
@@ -2839,7 +2839,7 @@
         <v>700</v>
       </c>
       <c r="J8">
-        <v>484</v>
+        <v>487</v>
       </c>
     </row>
     <row r="9" spans="1:10">
@@ -2871,7 +2871,7 @@
         <v>216</v>
       </c>
       <c r="J9">
-        <v>114</v>
+        <v>115</v>
       </c>
     </row>
     <row r="10" spans="1:10">
@@ -2903,7 +2903,7 @@
         <v>820</v>
       </c>
       <c r="J10">
-        <v>444</v>
+        <v>445</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -2935,7 +2935,7 @@
         <v>2472</v>
       </c>
       <c r="J11">
-        <v>1456</v>
+        <v>1461</v>
       </c>
     </row>
   </sheetData>
@@ -3117,7 +3117,7 @@
         <v>129</v>
       </c>
       <c r="J5">
-        <v>79</v>
+        <v>80</v>
       </c>
     </row>
     <row r="6" spans="1:10">
@@ -3149,7 +3149,7 @@
         <v>21</v>
       </c>
       <c r="J6">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="7" spans="1:10">
@@ -3245,7 +3245,7 @@
         <v>151</v>
       </c>
       <c r="J9">
-        <v>82</v>
+        <v>83</v>
       </c>
     </row>
     <row r="10" spans="1:10">
@@ -3277,7 +3277,7 @@
         <v>913</v>
       </c>
       <c r="J10">
-        <v>607</v>
+        <v>614</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -3309,7 +3309,7 @@
         <v>1600</v>
       </c>
       <c r="J11">
-        <v>1104</v>
+        <v>1114</v>
       </c>
     </row>
   </sheetData>
@@ -4025,7 +4025,7 @@
         <v>681</v>
       </c>
       <c r="J10">
-        <v>490</v>
+        <v>492</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -4057,7 +4057,7 @@
         <v>1279</v>
       </c>
       <c r="J11">
-        <v>890</v>
+        <v>892</v>
       </c>
     </row>
   </sheetData>
@@ -4146,7 +4146,7 @@
         <v>459</v>
       </c>
       <c r="J2">
-        <v>267</v>
+        <v>268</v>
       </c>
     </row>
     <row r="3" spans="1:10">
@@ -4178,7 +4178,7 @@
         <v>530</v>
       </c>
       <c r="J3">
-        <v>298</v>
+        <v>299</v>
       </c>
     </row>
     <row r="4" spans="1:10">
@@ -4338,7 +4338,7 @@
         <v>794</v>
       </c>
       <c r="J8">
-        <v>604</v>
+        <v>606</v>
       </c>
     </row>
     <row r="9" spans="1:10">
@@ -4370,7 +4370,7 @@
         <v>433</v>
       </c>
       <c r="J9">
-        <v>207</v>
+        <v>208</v>
       </c>
     </row>
     <row r="10" spans="1:10">
@@ -4402,7 +4402,7 @@
         <v>1302</v>
       </c>
       <c r="J10">
-        <v>731</v>
+        <v>734</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -4434,7 +4434,7 @@
         <v>3950</v>
       </c>
       <c r="J11">
-        <v>2371</v>
+        <v>2379</v>
       </c>
     </row>
   </sheetData>
@@ -4697,7 +4697,7 @@
         <v>131</v>
       </c>
       <c r="J8">
-        <v>146</v>
+        <v>147</v>
       </c>
     </row>
     <row r="9" spans="1:10">
@@ -4729,7 +4729,7 @@
         <v>122</v>
       </c>
       <c r="J9">
-        <v>50</v>
+        <v>51</v>
       </c>
     </row>
     <row r="10" spans="1:10">
@@ -4793,7 +4793,7 @@
         <v>1318</v>
       </c>
       <c r="J11">
-        <v>686</v>
+        <v>688</v>
       </c>
     </row>
   </sheetData>
@@ -4882,7 +4882,7 @@
         <v>216</v>
       </c>
       <c r="J2">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="3" spans="1:10">
@@ -4914,7 +4914,7 @@
         <v>280</v>
       </c>
       <c r="J3">
-        <v>118</v>
+        <v>121</v>
       </c>
     </row>
     <row r="4" spans="1:10">
@@ -5074,7 +5074,7 @@
         <v>653</v>
       </c>
       <c r="J8">
-        <v>540</v>
+        <v>544</v>
       </c>
     </row>
     <row r="9" spans="1:10">
@@ -5106,7 +5106,7 @@
         <v>428</v>
       </c>
       <c r="J9">
-        <v>288</v>
+        <v>289</v>
       </c>
     </row>
     <row r="10" spans="1:10">
@@ -5138,7 +5138,7 @@
         <v>1089</v>
       </c>
       <c r="J10">
-        <v>680</v>
+        <v>683</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -5170,7 +5170,7 @@
         <v>2956</v>
       </c>
       <c r="J11">
-        <v>1911</v>
+        <v>1921</v>
       </c>
     </row>
   </sheetData>
@@ -5259,7 +5259,7 @@
         <v>917</v>
       </c>
       <c r="J2">
-        <v>567</v>
+        <v>572</v>
       </c>
     </row>
     <row r="3" spans="1:10">
@@ -5323,7 +5323,7 @@
         <v>436</v>
       </c>
       <c r="J4">
-        <v>254</v>
+        <v>255</v>
       </c>
     </row>
     <row r="5" spans="1:10">
@@ -5355,7 +5355,7 @@
         <v>247</v>
       </c>
       <c r="J5">
-        <v>169</v>
+        <v>171</v>
       </c>
     </row>
     <row r="6" spans="1:10">
@@ -5387,7 +5387,7 @@
         <v>793</v>
       </c>
       <c r="J6">
-        <v>570</v>
+        <v>572</v>
       </c>
     </row>
     <row r="7" spans="1:10">
@@ -5419,7 +5419,7 @@
         <v>2686</v>
       </c>
       <c r="J7">
-        <v>1666</v>
+        <v>1671</v>
       </c>
     </row>
     <row r="8" spans="1:10">
@@ -5451,7 +5451,7 @@
         <v>4743</v>
       </c>
       <c r="J8">
-        <v>2798</v>
+        <v>2812</v>
       </c>
     </row>
     <row r="9" spans="1:10">
@@ -5483,7 +5483,7 @@
         <v>519</v>
       </c>
       <c r="J9">
-        <v>310</v>
+        <v>311</v>
       </c>
     </row>
     <row r="10" spans="1:10">
@@ -5547,7 +5547,7 @@
         <v>1712</v>
       </c>
       <c r="J11">
-        <v>1124</v>
+        <v>1127</v>
       </c>
     </row>
     <row r="12" spans="1:10">
@@ -5579,7 +5579,7 @@
         <v>412</v>
       </c>
       <c r="J12">
-        <v>230</v>
+        <v>233</v>
       </c>
     </row>
     <row r="13" spans="1:10">
@@ -5643,7 +5643,7 @@
         <v>718</v>
       </c>
       <c r="J14">
-        <v>351</v>
+        <v>356</v>
       </c>
     </row>
     <row r="15" spans="1:10">
@@ -5675,7 +5675,7 @@
         <v>886</v>
       </c>
       <c r="J15">
-        <v>585</v>
+        <v>589</v>
       </c>
     </row>
     <row r="16" spans="1:10">
@@ -5707,7 +5707,7 @@
         <v>595</v>
       </c>
       <c r="J16">
-        <v>430</v>
+        <v>432</v>
       </c>
     </row>
     <row r="17" spans="1:10">
@@ -5739,7 +5739,7 @@
         <v>175</v>
       </c>
       <c r="J17">
-        <v>86</v>
+        <v>87</v>
       </c>
     </row>
     <row r="18" spans="1:10">
@@ -5803,7 +5803,7 @@
         <v>2636</v>
       </c>
       <c r="J19">
-        <v>1536</v>
+        <v>1539</v>
       </c>
     </row>
     <row r="20" spans="1:10">
@@ -5835,7 +5835,7 @@
         <v>2045</v>
       </c>
       <c r="J20">
-        <v>1102</v>
+        <v>1111</v>
       </c>
     </row>
     <row r="21" spans="1:10">
@@ -5867,7 +5867,7 @@
         <v>337</v>
       </c>
       <c r="J21">
-        <v>153</v>
+        <v>155</v>
       </c>
     </row>
     <row r="22" spans="1:10">
@@ -5899,7 +5899,7 @@
         <v>418</v>
       </c>
       <c r="J22">
-        <v>303</v>
+        <v>305</v>
       </c>
     </row>
     <row r="23" spans="1:10">
@@ -5931,7 +5931,7 @@
         <v>1368</v>
       </c>
       <c r="J23">
-        <v>837</v>
+        <v>840</v>
       </c>
     </row>
     <row r="24" spans="1:10">
@@ -5963,7 +5963,7 @@
         <v>500</v>
       </c>
       <c r="J24">
-        <v>351</v>
+        <v>352</v>
       </c>
     </row>
     <row r="25" spans="1:10">
@@ -5995,7 +5995,7 @@
         <v>429</v>
       </c>
       <c r="J25">
-        <v>276</v>
+        <v>280</v>
       </c>
     </row>
     <row r="26" spans="1:10">
@@ -6027,7 +6027,7 @@
         <v>248</v>
       </c>
       <c r="J26">
-        <v>170</v>
+        <v>171</v>
       </c>
     </row>
     <row r="27" spans="1:10">
@@ -6059,7 +6059,7 @@
         <v>1258</v>
       </c>
       <c r="J27">
-        <v>777</v>
+        <v>779</v>
       </c>
     </row>
     <row r="28" spans="1:10">
@@ -6091,7 +6091,7 @@
         <v>99</v>
       </c>
       <c r="J28">
-        <v>35</v>
+        <v>36</v>
       </c>
     </row>
     <row r="29" spans="1:10">
@@ -6123,7 +6123,7 @@
         <v>3950</v>
       </c>
       <c r="J29">
-        <v>2371</v>
+        <v>2379</v>
       </c>
     </row>
     <row r="30" spans="1:10">
@@ -6187,7 +6187,7 @@
         <v>867</v>
       </c>
       <c r="J31">
-        <v>489</v>
+        <v>491</v>
       </c>
     </row>
     <row r="32" spans="1:10">
@@ -6251,7 +6251,7 @@
         <v>3011</v>
       </c>
       <c r="J33">
-        <v>1882</v>
+        <v>1892</v>
       </c>
     </row>
     <row r="34" spans="1:10">
@@ -6283,7 +6283,7 @@
         <v>761</v>
       </c>
       <c r="J34">
-        <v>499</v>
+        <v>501</v>
       </c>
     </row>
     <row r="35" spans="1:10">
@@ -6347,7 +6347,7 @@
         <v>1491</v>
       </c>
       <c r="J36">
-        <v>938</v>
+        <v>945</v>
       </c>
     </row>
     <row r="37" spans="1:10">
@@ -6379,7 +6379,7 @@
         <v>2547</v>
       </c>
       <c r="J37">
-        <v>1598</v>
+        <v>1603</v>
       </c>
     </row>
     <row r="38" spans="1:10">
@@ -6443,7 +6443,7 @@
         <v>153</v>
       </c>
       <c r="J39">
-        <v>56</v>
+        <v>57</v>
       </c>
     </row>
     <row r="40" spans="1:10">
@@ -6475,7 +6475,7 @@
         <v>236</v>
       </c>
       <c r="J40">
-        <v>157</v>
+        <v>158</v>
       </c>
     </row>
     <row r="41" spans="1:10">
@@ -6539,7 +6539,7 @@
         <v>2956</v>
       </c>
       <c r="J42">
-        <v>1911</v>
+        <v>1921</v>
       </c>
     </row>
     <row r="43" spans="1:10">
@@ -6571,7 +6571,7 @@
         <v>1153</v>
       </c>
       <c r="J43">
-        <v>787</v>
+        <v>794</v>
       </c>
     </row>
     <row r="44" spans="1:10">
@@ -6603,7 +6603,7 @@
         <v>1228</v>
       </c>
       <c r="J44">
-        <v>727</v>
+        <v>730</v>
       </c>
     </row>
     <row r="45" spans="1:10">
@@ -6635,7 +6635,7 @@
         <v>181</v>
       </c>
       <c r="J45">
-        <v>89</v>
+        <v>91</v>
       </c>
     </row>
     <row r="46" spans="1:10">
@@ -6667,7 +6667,7 @@
         <v>436</v>
       </c>
       <c r="J46">
-        <v>277</v>
+        <v>278</v>
       </c>
     </row>
     <row r="47" spans="1:10">
@@ -6699,7 +6699,7 @@
         <v>903</v>
       </c>
       <c r="J47">
-        <v>556</v>
+        <v>559</v>
       </c>
     </row>
     <row r="48" spans="1:10">
@@ -6731,7 +6731,7 @@
         <v>2622</v>
       </c>
       <c r="J48">
-        <v>1536</v>
+        <v>1545</v>
       </c>
     </row>
     <row r="49" spans="1:10">
@@ -6763,7 +6763,7 @@
         <v>1648</v>
       </c>
       <c r="J49">
-        <v>943</v>
+        <v>947</v>
       </c>
     </row>
     <row r="50" spans="1:10">
@@ -6795,7 +6795,7 @@
         <v>960</v>
       </c>
       <c r="J50">
-        <v>560</v>
+        <v>561</v>
       </c>
     </row>
     <row r="51" spans="1:10">
@@ -6827,7 +6827,7 @@
         <v>1337</v>
       </c>
       <c r="J51">
-        <v>878</v>
+        <v>886</v>
       </c>
     </row>
     <row r="52" spans="1:10">
@@ -6859,7 +6859,7 @@
         <v>1491</v>
       </c>
       <c r="J52">
-        <v>1056</v>
+        <v>1060</v>
       </c>
     </row>
     <row r="53" spans="1:10">
@@ -6891,7 +6891,7 @@
         <v>1600</v>
       </c>
       <c r="J53">
-        <v>1104</v>
+        <v>1114</v>
       </c>
     </row>
     <row r="54" spans="1:10">
@@ -6920,10 +6920,10 @@
         <v>2198</v>
       </c>
       <c r="I54">
-        <v>3507</v>
+        <v>3506</v>
       </c>
       <c r="J54">
-        <v>2016</v>
+        <v>2023</v>
       </c>
     </row>
     <row r="55" spans="1:10">
@@ -6955,7 +6955,7 @@
         <v>1244</v>
       </c>
       <c r="J55">
-        <v>703</v>
+        <v>706</v>
       </c>
     </row>
     <row r="56" spans="1:10">
@@ -6987,7 +6987,7 @@
         <v>628</v>
       </c>
       <c r="J56">
-        <v>334</v>
+        <v>335</v>
       </c>
     </row>
     <row r="57" spans="1:10">
@@ -7083,7 +7083,7 @@
         <v>271</v>
       </c>
       <c r="J59">
-        <v>181</v>
+        <v>182</v>
       </c>
     </row>
     <row r="60" spans="1:10">
@@ -7115,7 +7115,7 @@
         <v>768</v>
       </c>
       <c r="J60">
-        <v>475</v>
+        <v>480</v>
       </c>
     </row>
     <row r="61" spans="1:10">
@@ -7211,7 +7211,7 @@
         <v>2481</v>
       </c>
       <c r="J63">
-        <v>706</v>
+        <v>739</v>
       </c>
     </row>
     <row r="64" spans="1:10">
@@ -7243,7 +7243,7 @@
         <v>1187</v>
       </c>
       <c r="J64">
-        <v>638</v>
+        <v>640</v>
       </c>
     </row>
     <row r="65" spans="1:10">
@@ -7339,7 +7339,7 @@
         <v>2510</v>
       </c>
       <c r="J67">
-        <v>1544</v>
+        <v>1555</v>
       </c>
     </row>
     <row r="68" spans="1:10">
@@ -7403,7 +7403,7 @@
         <v>494</v>
       </c>
       <c r="J69">
-        <v>253</v>
+        <v>255</v>
       </c>
     </row>
     <row r="70" spans="1:10">
@@ -7435,7 +7435,7 @@
         <v>677</v>
       </c>
       <c r="J70">
-        <v>416</v>
+        <v>417</v>
       </c>
     </row>
     <row r="71" spans="1:10">
@@ -7467,7 +7467,7 @@
         <v>335</v>
       </c>
       <c r="J71">
-        <v>258</v>
+        <v>259</v>
       </c>
     </row>
     <row r="72" spans="1:10">
@@ -7499,7 +7499,7 @@
         <v>706</v>
       </c>
       <c r="J72">
-        <v>390</v>
+        <v>391</v>
       </c>
     </row>
     <row r="73" spans="1:10">
@@ -7531,7 +7531,7 @@
         <v>1279</v>
       </c>
       <c r="J73">
-        <v>890</v>
+        <v>892</v>
       </c>
     </row>
     <row r="74" spans="1:10">
@@ -7563,7 +7563,7 @@
         <v>307</v>
       </c>
       <c r="J74">
-        <v>157</v>
+        <v>158</v>
       </c>
     </row>
     <row r="75" spans="1:10">
@@ -7627,7 +7627,7 @@
         <v>2923</v>
       </c>
       <c r="J76">
-        <v>1701</v>
+        <v>1706</v>
       </c>
     </row>
     <row r="77" spans="1:10">
@@ -7659,7 +7659,7 @@
         <v>462</v>
       </c>
       <c r="J77">
-        <v>307</v>
+        <v>308</v>
       </c>
     </row>
     <row r="78" spans="1:10">
@@ -7691,7 +7691,7 @@
         <v>1797</v>
       </c>
       <c r="J78">
-        <v>1026</v>
+        <v>1027</v>
       </c>
     </row>
     <row r="79" spans="1:10">
@@ -7723,7 +7723,7 @@
         <v>2472</v>
       </c>
       <c r="J79">
-        <v>1456</v>
+        <v>1461</v>
       </c>
     </row>
     <row r="80" spans="1:10">
@@ -7851,7 +7851,7 @@
         <v>1793</v>
       </c>
       <c r="J83">
-        <v>1010</v>
+        <v>1019</v>
       </c>
     </row>
     <row r="84" spans="1:10">
@@ -7883,7 +7883,7 @@
         <v>729</v>
       </c>
       <c r="J84">
-        <v>485</v>
+        <v>487</v>
       </c>
     </row>
     <row r="85" spans="1:10">
@@ -7915,7 +7915,7 @@
         <v>3848</v>
       </c>
       <c r="J85">
-        <v>2405</v>
+        <v>2422</v>
       </c>
     </row>
     <row r="86" spans="1:10">
@@ -7947,7 +7947,7 @@
         <v>1066</v>
       </c>
       <c r="J86">
-        <v>491</v>
+        <v>494</v>
       </c>
     </row>
     <row r="87" spans="1:10">
@@ -8043,7 +8043,7 @@
         <v>1879</v>
       </c>
       <c r="J89">
-        <v>1155</v>
+        <v>1163</v>
       </c>
     </row>
     <row r="90" spans="1:10">
@@ -8075,7 +8075,7 @@
         <v>1354</v>
       </c>
       <c r="J90">
-        <v>861</v>
+        <v>865</v>
       </c>
     </row>
     <row r="91" spans="1:10">
@@ -8107,7 +8107,7 @@
         <v>970</v>
       </c>
       <c r="J91">
-        <v>621</v>
+        <v>623</v>
       </c>
     </row>
     <row r="92" spans="1:10">
@@ -8171,7 +8171,7 @@
         <v>721</v>
       </c>
       <c r="J93">
-        <v>450</v>
+        <v>452</v>
       </c>
     </row>
     <row r="94" spans="1:10">
@@ -8203,7 +8203,7 @@
         <v>2663</v>
       </c>
       <c r="J94">
-        <v>1413</v>
+        <v>1414</v>
       </c>
     </row>
     <row r="95" spans="1:10">
@@ -8235,7 +8235,7 @@
         <v>1389</v>
       </c>
       <c r="J95">
-        <v>860</v>
+        <v>866</v>
       </c>
     </row>
     <row r="96" spans="1:10">
@@ -8267,7 +8267,7 @@
         <v>1669</v>
       </c>
       <c r="J96">
-        <v>937</v>
+        <v>943</v>
       </c>
     </row>
     <row r="97" spans="1:10">
@@ -8299,7 +8299,7 @@
         <v>1673</v>
       </c>
       <c r="J97">
-        <v>982</v>
+        <v>988</v>
       </c>
     </row>
     <row r="98" spans="1:10">
@@ -8331,7 +8331,7 @@
         <v>1318</v>
       </c>
       <c r="J98">
-        <v>686</v>
+        <v>688</v>
       </c>
     </row>
     <row r="99" spans="1:10">
@@ -8363,7 +8363,7 @@
         <v>1488</v>
       </c>
       <c r="J99">
-        <v>930</v>
+        <v>937</v>
       </c>
     </row>
     <row r="100" spans="1:10">
@@ -8395,7 +8395,7 @@
         <v>237</v>
       </c>
       <c r="J100">
-        <v>172</v>
+        <v>175</v>
       </c>
     </row>
     <row r="101" spans="1:10">
@@ -8424,10 +8424,10 @@
         <v>84595</v>
       </c>
       <c r="I101">
-        <v>110482</v>
+        <v>110481</v>
       </c>
       <c r="J101">
-        <v>65985</v>
+        <v>66320</v>
       </c>
     </row>
   </sheetData>
@@ -8711,7 +8711,7 @@
         <v>121</v>
       </c>
       <c r="J5">
-        <v>70</v>
+        <v>71</v>
       </c>
     </row>
     <row r="6" spans="1:10">
@@ -8859,7 +8859,7 @@
         <v>1135</v>
       </c>
       <c r="J10">
-        <v>640</v>
+        <v>643</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -8891,7 +8891,7 @@
         <v>1648</v>
       </c>
       <c r="J11">
-        <v>943</v>
+        <v>947</v>
       </c>
     </row>
   </sheetData>
@@ -9012,7 +9012,7 @@
         <v>439</v>
       </c>
       <c r="J3">
-        <v>249</v>
+        <v>250</v>
       </c>
     </row>
     <row r="4" spans="1:10">
@@ -9076,7 +9076,7 @@
         <v>381</v>
       </c>
       <c r="J5">
-        <v>170</v>
+        <v>171</v>
       </c>
     </row>
     <row r="6" spans="1:10">
@@ -9140,7 +9140,7 @@
         <v>36</v>
       </c>
       <c r="J7">
-        <v>14</v>
+        <v>15</v>
       </c>
     </row>
     <row r="8" spans="1:10">
@@ -9172,7 +9172,7 @@
         <v>1026</v>
       </c>
       <c r="J8">
-        <v>817</v>
+        <v>821</v>
       </c>
     </row>
     <row r="9" spans="1:10">
@@ -9204,7 +9204,7 @@
         <v>303</v>
       </c>
       <c r="J9">
-        <v>189</v>
+        <v>190</v>
       </c>
     </row>
     <row r="10" spans="1:10">
@@ -9236,7 +9236,7 @@
         <v>1271</v>
       </c>
       <c r="J10">
-        <v>736</v>
+        <v>745</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -9268,7 +9268,7 @@
         <v>3848</v>
       </c>
       <c r="J11">
-        <v>2405</v>
+        <v>2422</v>
       </c>
     </row>
   </sheetData>
@@ -9546,7 +9546,7 @@
         <v>336</v>
       </c>
       <c r="J8">
-        <v>178</v>
+        <v>179</v>
       </c>
     </row>
     <row r="9" spans="1:10">
@@ -9578,7 +9578,7 @@
         <v>179</v>
       </c>
       <c r="J9">
-        <v>124</v>
+        <v>125</v>
       </c>
     </row>
     <row r="10" spans="1:10">
@@ -9610,7 +9610,7 @@
         <v>2132</v>
       </c>
       <c r="J10">
-        <v>1225</v>
+        <v>1228</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -9642,7 +9642,7 @@
         <v>2923</v>
       </c>
       <c r="J11">
-        <v>1701</v>
+        <v>1706</v>
       </c>
     </row>
   </sheetData>
@@ -9821,7 +9821,7 @@
         <v>122</v>
       </c>
       <c r="J5">
-        <v>80</v>
+        <v>81</v>
       </c>
     </row>
     <row r="6" spans="1:10">
@@ -9978,7 +9978,7 @@
         <v>1034</v>
       </c>
       <c r="J10">
-        <v>486</v>
+        <v>491</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -10010,7 +10010,7 @@
         <v>1673</v>
       </c>
       <c r="J11">
-        <v>982</v>
+        <v>988</v>
       </c>
     </row>
   </sheetData>
@@ -10099,7 +10099,7 @@
         <v>235</v>
       </c>
       <c r="J2">
-        <v>136</v>
+        <v>139</v>
       </c>
     </row>
     <row r="3" spans="1:10">
@@ -10131,7 +10131,7 @@
         <v>365</v>
       </c>
       <c r="J3">
-        <v>238</v>
+        <v>240</v>
       </c>
     </row>
     <row r="4" spans="1:10">
@@ -10195,7 +10195,7 @@
         <v>102</v>
       </c>
       <c r="J5">
-        <v>64</v>
+        <v>65</v>
       </c>
     </row>
     <row r="6" spans="1:10">
@@ -10227,7 +10227,7 @@
         <v>56</v>
       </c>
       <c r="J6">
-        <v>41</v>
+        <v>42</v>
       </c>
     </row>
     <row r="7" spans="1:10">
@@ -10291,7 +10291,7 @@
         <v>516</v>
       </c>
       <c r="J8">
-        <v>398</v>
+        <v>399</v>
       </c>
     </row>
     <row r="9" spans="1:10">
@@ -10323,7 +10323,7 @@
         <v>295</v>
       </c>
       <c r="J9">
-        <v>155</v>
+        <v>157</v>
       </c>
     </row>
     <row r="10" spans="1:10">
@@ -10355,7 +10355,7 @@
         <v>895</v>
       </c>
       <c r="J10">
-        <v>484</v>
+        <v>485</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -10387,7 +10387,7 @@
         <v>2510</v>
       </c>
       <c r="J11">
-        <v>1544</v>
+        <v>1555</v>
       </c>
     </row>
   </sheetData>
@@ -10508,7 +10508,7 @@
         <v>137</v>
       </c>
       <c r="J3">
-        <v>74</v>
+        <v>75</v>
       </c>
     </row>
     <row r="4" spans="1:10">
@@ -10668,7 +10668,7 @@
         <v>392</v>
       </c>
       <c r="J8">
-        <v>298</v>
+        <v>303</v>
       </c>
     </row>
     <row r="9" spans="1:10">
@@ -10764,7 +10764,7 @@
         <v>1389</v>
       </c>
       <c r="J11">
-        <v>860</v>
+        <v>866</v>
       </c>
     </row>
   </sheetData>
@@ -11045,7 +11045,7 @@
         <v>190</v>
       </c>
       <c r="J8">
-        <v>178</v>
+        <v>179</v>
       </c>
     </row>
     <row r="9" spans="1:10">
@@ -11109,7 +11109,7 @@
         <v>271</v>
       </c>
       <c r="J10">
-        <v>145</v>
+        <v>146</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -11141,7 +11141,7 @@
         <v>729</v>
       </c>
       <c r="J11">
-        <v>485</v>
+        <v>487</v>
       </c>
     </row>
   </sheetData>
@@ -11230,7 +11230,7 @@
         <v>146</v>
       </c>
       <c r="J2">
-        <v>95</v>
+        <v>96</v>
       </c>
     </row>
     <row r="3" spans="1:10">
@@ -11262,7 +11262,7 @@
         <v>190</v>
       </c>
       <c r="J3">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="4" spans="1:10">
@@ -11422,7 +11422,7 @@
         <v>218</v>
       </c>
       <c r="J8">
-        <v>205</v>
+        <v>206</v>
       </c>
     </row>
     <row r="9" spans="1:10">
@@ -11486,7 +11486,7 @@
         <v>590</v>
       </c>
       <c r="J10">
-        <v>385</v>
+        <v>388</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -11518,7 +11518,7 @@
         <v>1491</v>
       </c>
       <c r="J11">
-        <v>1056</v>
+        <v>1060</v>
       </c>
     </row>
   </sheetData>
@@ -12109,7 +12109,7 @@
         <v>43</v>
       </c>
       <c r="I6">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="J6">
         <v>20</v>
@@ -12237,7 +12237,7 @@
         <v>2528</v>
       </c>
       <c r="J10">
-        <v>1445</v>
+        <v>1452</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -12266,10 +12266,10 @@
         <v>2198</v>
       </c>
       <c r="I11">
-        <v>3507</v>
+        <v>3506</v>
       </c>
       <c r="J11">
-        <v>2016</v>
+        <v>2023</v>
       </c>
     </row>
   </sheetData>
@@ -12550,7 +12550,7 @@
         <v>503</v>
       </c>
       <c r="J8">
-        <v>361</v>
+        <v>363</v>
       </c>
     </row>
     <row r="9" spans="1:10">
@@ -12614,7 +12614,7 @@
         <v>527</v>
       </c>
       <c r="J10">
-        <v>323</v>
+        <v>328</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -12646,7 +12646,7 @@
         <v>1491</v>
       </c>
       <c r="J11">
-        <v>938</v>
+        <v>945</v>
       </c>
     </row>
   </sheetData>
@@ -12767,7 +12767,7 @@
         <v>261</v>
       </c>
       <c r="J3">
-        <v>168</v>
+        <v>169</v>
       </c>
     </row>
     <row r="4" spans="1:10">
@@ -12831,7 +12831,7 @@
         <v>200</v>
       </c>
       <c r="J5">
-        <v>135</v>
+        <v>136</v>
       </c>
     </row>
     <row r="6" spans="1:10">
@@ -12895,7 +12895,7 @@
         <v>23</v>
       </c>
       <c r="J7">
-        <v>17</v>
+        <v>18</v>
       </c>
     </row>
     <row r="8" spans="1:10">
@@ -12927,7 +12927,7 @@
         <v>722</v>
       </c>
       <c r="J8">
-        <v>501</v>
+        <v>502</v>
       </c>
     </row>
     <row r="9" spans="1:10">
@@ -12991,7 +12991,7 @@
         <v>813</v>
       </c>
       <c r="J10">
-        <v>479</v>
+        <v>480</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -13023,7 +13023,7 @@
         <v>2547</v>
       </c>
       <c r="J11">
-        <v>1598</v>
+        <v>1603</v>
       </c>
     </row>
   </sheetData>
@@ -13144,7 +13144,7 @@
         <v>16</v>
       </c>
       <c r="J3">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="4" spans="1:10">
@@ -13347,7 +13347,7 @@
         <v>213</v>
       </c>
       <c r="J10">
-        <v>137</v>
+        <v>138</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -13379,7 +13379,7 @@
         <v>418</v>
       </c>
       <c r="J11">
-        <v>303</v>
+        <v>305</v>
       </c>
     </row>
   </sheetData>
@@ -13709,7 +13709,7 @@
         <v>448</v>
       </c>
       <c r="J10">
-        <v>228</v>
+        <v>229</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -13741,7 +13741,7 @@
         <v>706</v>
       </c>
       <c r="J11">
-        <v>390</v>
+        <v>391</v>
       </c>
     </row>
   </sheetData>
@@ -14734,7 +14734,7 @@
         <v>175</v>
       </c>
       <c r="J8">
-        <v>154</v>
+        <v>159</v>
       </c>
     </row>
     <row r="9" spans="1:10">
@@ -14830,7 +14830,7 @@
         <v>768</v>
       </c>
       <c r="J11">
-        <v>475</v>
+        <v>480</v>
       </c>
     </row>
   </sheetData>
@@ -15281,7 +15281,7 @@
         <v>190</v>
       </c>
       <c r="J2">
-        <v>99</v>
+        <v>100</v>
       </c>
     </row>
     <row r="3" spans="1:10">
@@ -15313,7 +15313,7 @@
         <v>205</v>
       </c>
       <c r="J3">
-        <v>122</v>
+        <v>123</v>
       </c>
     </row>
     <row r="4" spans="1:10">
@@ -15377,7 +15377,7 @@
         <v>124</v>
       </c>
       <c r="J5">
-        <v>53</v>
+        <v>54</v>
       </c>
     </row>
     <row r="6" spans="1:10">
@@ -15473,7 +15473,7 @@
         <v>484</v>
       </c>
       <c r="J8">
-        <v>285</v>
+        <v>287</v>
       </c>
     </row>
     <row r="9" spans="1:10">
@@ -15505,7 +15505,7 @@
         <v>123</v>
       </c>
       <c r="J9">
-        <v>91</v>
+        <v>92</v>
       </c>
     </row>
     <row r="10" spans="1:10">
@@ -15537,7 +15537,7 @@
         <v>612</v>
       </c>
       <c r="J10">
-        <v>333</v>
+        <v>336</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -15569,7 +15569,7 @@
         <v>1793</v>
       </c>
       <c r="J11">
-        <v>1010</v>
+        <v>1019</v>
       </c>
     </row>
   </sheetData>
@@ -15658,7 +15658,7 @@
         <v>92</v>
       </c>
       <c r="J2">
-        <v>42</v>
+        <v>43</v>
       </c>
     </row>
     <row r="3" spans="1:10">
@@ -15850,7 +15850,7 @@
         <v>224</v>
       </c>
       <c r="J8">
-        <v>173</v>
+        <v>175</v>
       </c>
     </row>
     <row r="9" spans="1:10">
@@ -15946,7 +15946,7 @@
         <v>1244</v>
       </c>
       <c r="J11">
-        <v>703</v>
+        <v>706</v>
       </c>
     </row>
   </sheetData>
@@ -16276,7 +16276,7 @@
         <v>2021</v>
       </c>
       <c r="J10">
-        <v>1002</v>
+        <v>1003</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -16308,7 +16308,7 @@
         <v>2663</v>
       </c>
       <c r="J11">
-        <v>1413</v>
+        <v>1414</v>
       </c>
     </row>
   </sheetData>
@@ -16429,7 +16429,7 @@
         <v>416</v>
       </c>
       <c r="J3">
-        <v>225</v>
+        <v>227</v>
       </c>
     </row>
     <row r="4" spans="1:10">
@@ -16525,7 +16525,7 @@
         <v>49</v>
       </c>
       <c r="J6">
-        <v>29</v>
+        <v>30</v>
       </c>
     </row>
     <row r="7" spans="1:10">
@@ -16589,7 +16589,7 @@
         <v>707</v>
       </c>
       <c r="J8">
-        <v>569</v>
+        <v>573</v>
       </c>
     </row>
     <row r="9" spans="1:10">
@@ -16621,7 +16621,7 @@
         <v>363</v>
       </c>
       <c r="J9">
-        <v>220</v>
+        <v>222</v>
       </c>
     </row>
     <row r="10" spans="1:10">
@@ -16653,7 +16653,7 @@
         <v>968</v>
       </c>
       <c r="J10">
-        <v>550</v>
+        <v>551</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -16685,7 +16685,7 @@
         <v>3011</v>
       </c>
       <c r="J11">
-        <v>1882</v>
+        <v>1892</v>
       </c>
     </row>
   </sheetData>
@@ -16774,7 +16774,7 @@
         <v>264</v>
       </c>
       <c r="J2">
-        <v>143</v>
+        <v>145</v>
       </c>
     </row>
     <row r="3" spans="1:10">
@@ -16870,7 +16870,7 @@
         <v>261</v>
       </c>
       <c r="J5">
-        <v>140</v>
+        <v>141</v>
       </c>
     </row>
     <row r="6" spans="1:10">
@@ -16966,7 +16966,7 @@
         <v>567</v>
       </c>
       <c r="J8">
-        <v>564</v>
+        <v>565</v>
       </c>
     </row>
     <row r="9" spans="1:10">
@@ -17030,7 +17030,7 @@
         <v>1023</v>
       </c>
       <c r="J10">
-        <v>511</v>
+        <v>512</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -17062,7 +17062,7 @@
         <v>2686</v>
       </c>
       <c r="J11">
-        <v>1666</v>
+        <v>1671</v>
       </c>
     </row>
   </sheetData>
@@ -17151,7 +17151,7 @@
         <v>457</v>
       </c>
       <c r="J2">
-        <v>280</v>
+        <v>282</v>
       </c>
     </row>
     <row r="3" spans="1:10">
@@ -17247,7 +17247,7 @@
         <v>251</v>
       </c>
       <c r="J5">
-        <v>120</v>
+        <v>121</v>
       </c>
     </row>
     <row r="6" spans="1:10">
@@ -17343,7 +17343,7 @@
         <v>1269</v>
       </c>
       <c r="J8">
-        <v>756</v>
+        <v>766</v>
       </c>
     </row>
     <row r="9" spans="1:10">
@@ -17375,7 +17375,7 @@
         <v>497</v>
       </c>
       <c r="J9">
-        <v>315</v>
+        <v>316</v>
       </c>
     </row>
     <row r="10" spans="1:10">
@@ -17439,7 +17439,7 @@
         <v>4743</v>
       </c>
       <c r="J11">
-        <v>2798</v>
+        <v>2812</v>
       </c>
     </row>
   </sheetData>
@@ -17528,7 +17528,7 @@
         <v>106</v>
       </c>
       <c r="J2">
-        <v>60</v>
+        <v>61</v>
       </c>
     </row>
     <row r="3" spans="1:10">
@@ -17720,7 +17720,7 @@
         <v>441</v>
       </c>
       <c r="J8">
-        <v>337</v>
+        <v>338</v>
       </c>
     </row>
     <row r="9" spans="1:10">
@@ -17752,7 +17752,7 @@
         <v>120</v>
       </c>
       <c r="J9">
-        <v>50</v>
+        <v>51</v>
       </c>
     </row>
     <row r="10" spans="1:10">
@@ -17784,7 +17784,7 @@
         <v>455</v>
       </c>
       <c r="J10">
-        <v>301</v>
+        <v>302</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -17816,7 +17816,7 @@
         <v>1354</v>
       </c>
       <c r="J11">
-        <v>861</v>
+        <v>865</v>
       </c>
     </row>
   </sheetData>
@@ -17905,7 +17905,7 @@
         <v>47</v>
       </c>
       <c r="J2">
-        <v>28</v>
+        <v>29</v>
       </c>
     </row>
     <row r="3" spans="1:10">
@@ -18152,7 +18152,7 @@
         <v>417</v>
       </c>
       <c r="J10">
-        <v>239</v>
+        <v>241</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -18184,7 +18184,7 @@
         <v>903</v>
       </c>
       <c r="J11">
-        <v>556</v>
+        <v>559</v>
       </c>
     </row>
   </sheetData>
@@ -18305,7 +18305,7 @@
         <v>212</v>
       </c>
       <c r="J3">
-        <v>125</v>
+        <v>126</v>
       </c>
     </row>
     <row r="4" spans="1:10">
@@ -18529,7 +18529,7 @@
         <v>911</v>
       </c>
       <c r="J10">
-        <v>545</v>
+        <v>547</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -18561,7 +18561,7 @@
         <v>2636</v>
       </c>
       <c r="J11">
-        <v>1536</v>
+        <v>1539</v>
       </c>
     </row>
   </sheetData>
@@ -18879,7 +18879,7 @@
         <v>94</v>
       </c>
       <c r="J10">
-        <v>60</v>
+        <v>62</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -18911,7 +18911,7 @@
         <v>247</v>
       </c>
       <c r="J11">
-        <v>169</v>
+        <v>171</v>
       </c>
     </row>
   </sheetData>
@@ -19000,7 +19000,7 @@
         <v>179</v>
       </c>
       <c r="J2">
-        <v>93</v>
+        <v>94</v>
       </c>
     </row>
     <row r="3" spans="1:10">
@@ -19192,7 +19192,7 @@
         <v>363</v>
       </c>
       <c r="J8">
-        <v>280</v>
+        <v>282</v>
       </c>
     </row>
     <row r="9" spans="1:10">
@@ -19224,7 +19224,7 @@
         <v>224</v>
       </c>
       <c r="J9">
-        <v>83</v>
+        <v>85</v>
       </c>
     </row>
     <row r="10" spans="1:10">
@@ -19256,7 +19256,7 @@
         <v>828</v>
       </c>
       <c r="J10">
-        <v>433</v>
+        <v>437</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -19288,7 +19288,7 @@
         <v>2045</v>
       </c>
       <c r="J11">
-        <v>1102</v>
+        <v>1111</v>
       </c>
     </row>
   </sheetData>
@@ -19621,7 +19621,7 @@
         <v>630</v>
       </c>
       <c r="J10">
-        <v>310</v>
+        <v>311</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -19653,7 +19653,7 @@
         <v>960</v>
       </c>
       <c r="J11">
-        <v>560</v>
+        <v>561</v>
       </c>
     </row>
   </sheetData>
@@ -19983,7 +19983,7 @@
         <v>124</v>
       </c>
       <c r="J10">
-        <v>88</v>
+        <v>89</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -20015,7 +20015,7 @@
         <v>271</v>
       </c>
       <c r="J11">
-        <v>181</v>
+        <v>182</v>
       </c>
     </row>
   </sheetData>
@@ -20328,7 +20328,7 @@
         <v>77</v>
       </c>
       <c r="J9">
-        <v>31</v>
+        <v>32</v>
       </c>
     </row>
     <row r="10" spans="1:10">
@@ -20360,7 +20360,7 @@
         <v>320</v>
       </c>
       <c r="J10">
-        <v>186</v>
+        <v>187</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -20392,7 +20392,7 @@
         <v>970</v>
       </c>
       <c r="J11">
-        <v>621</v>
+        <v>623</v>
       </c>
     </row>
   </sheetData>
@@ -20577,7 +20577,7 @@
         <v>64</v>
       </c>
       <c r="J5">
-        <v>49</v>
+        <v>50</v>
       </c>
     </row>
     <row r="6" spans="1:10">
@@ -20667,7 +20667,7 @@
         <v>122</v>
       </c>
       <c r="J8">
-        <v>131</v>
+        <v>132</v>
       </c>
     </row>
     <row r="9" spans="1:10">
@@ -20763,7 +20763,7 @@
         <v>721</v>
       </c>
       <c r="J11">
-        <v>450</v>
+        <v>452</v>
       </c>
     </row>
   </sheetData>
@@ -21087,7 +21087,7 @@
         <v>280</v>
       </c>
       <c r="J10">
-        <v>142</v>
+        <v>143</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -21119,7 +21119,7 @@
         <v>436</v>
       </c>
       <c r="J11">
-        <v>277</v>
+        <v>278</v>
       </c>
     </row>
   </sheetData>
@@ -21301,7 +21301,7 @@
         <v>44</v>
       </c>
       <c r="J5">
-        <v>15</v>
+        <v>16</v>
       </c>
     </row>
     <row r="6" spans="1:10">
@@ -21487,7 +21487,7 @@
         <v>436</v>
       </c>
       <c r="J11">
-        <v>254</v>
+        <v>255</v>
       </c>
     </row>
   </sheetData>
@@ -21576,7 +21576,7 @@
         <v>64</v>
       </c>
       <c r="J2">
-        <v>47</v>
+        <v>49</v>
       </c>
     </row>
     <row r="3" spans="1:10">
@@ -21765,7 +21765,7 @@
         <v>297</v>
       </c>
       <c r="J8">
-        <v>283</v>
+        <v>286</v>
       </c>
     </row>
     <row r="9" spans="1:10">
@@ -21797,7 +21797,7 @@
         <v>121</v>
       </c>
       <c r="J9">
-        <v>67</v>
+        <v>68</v>
       </c>
     </row>
     <row r="10" spans="1:10">
@@ -21829,7 +21829,7 @@
         <v>670</v>
       </c>
       <c r="J10">
-        <v>358</v>
+        <v>360</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -21861,7 +21861,7 @@
         <v>1337</v>
       </c>
       <c r="J11">
-        <v>878</v>
+        <v>886</v>
       </c>
     </row>
   </sheetData>
@@ -21982,7 +21982,7 @@
         <v>64</v>
       </c>
       <c r="J3">
-        <v>29</v>
+        <v>30</v>
       </c>
     </row>
     <row r="4" spans="1:10">
@@ -22142,7 +22142,7 @@
         <v>125</v>
       </c>
       <c r="J8">
-        <v>81</v>
+        <v>83</v>
       </c>
     </row>
     <row r="9" spans="1:10">
@@ -22206,7 +22206,7 @@
         <v>492</v>
       </c>
       <c r="J10">
-        <v>323</v>
+        <v>325</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -22238,7 +22238,7 @@
         <v>917</v>
       </c>
       <c r="J11">
-        <v>567</v>
+        <v>572</v>
       </c>
     </row>
   </sheetData>
@@ -22327,7 +22327,7 @@
         <v>12</v>
       </c>
       <c r="J2">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="3" spans="1:10">
@@ -22417,7 +22417,7 @@
         <v>49</v>
       </c>
       <c r="J5">
-        <v>38</v>
+        <v>39</v>
       </c>
     </row>
     <row r="6" spans="1:10">
@@ -22492,7 +22492,7 @@
         <v>89</v>
       </c>
       <c r="J8">
-        <v>62</v>
+        <v>63</v>
       </c>
     </row>
     <row r="9" spans="1:10">
@@ -22588,7 +22588,7 @@
         <v>412</v>
       </c>
       <c r="J11">
-        <v>230</v>
+        <v>233</v>
       </c>
     </row>
   </sheetData>
@@ -23295,7 +23295,7 @@
         <v>277</v>
       </c>
       <c r="J10">
-        <v>179</v>
+        <v>180</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -23327,7 +23327,7 @@
         <v>500</v>
       </c>
       <c r="J11">
-        <v>351</v>
+        <v>352</v>
       </c>
     </row>
   </sheetData>
@@ -23669,7 +23669,7 @@
         <v>189</v>
       </c>
       <c r="J10">
-        <v>133</v>
+        <v>137</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -23701,7 +23701,7 @@
         <v>429</v>
       </c>
       <c r="J11">
-        <v>276</v>
+        <v>280</v>
       </c>
     </row>
   </sheetData>
@@ -23947,7 +23947,7 @@
         <v>4</v>
       </c>
       <c r="J7">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="8" spans="1:10">
@@ -24043,7 +24043,7 @@
         <v>349</v>
       </c>
       <c r="J10">
-        <v>217</v>
+        <v>218</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -24075,7 +24075,7 @@
         <v>793</v>
       </c>
       <c r="J11">
-        <v>570</v>
+        <v>572</v>
       </c>
     </row>
   </sheetData>
@@ -24773,7 +24773,7 @@
         <v>784</v>
       </c>
       <c r="J10">
-        <v>496</v>
+        <v>498</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -24805,7 +24805,7 @@
         <v>1258</v>
       </c>
       <c r="J11">
-        <v>777</v>
+        <v>779</v>
       </c>
     </row>
   </sheetData>
@@ -24926,7 +24926,7 @@
         <v>67</v>
       </c>
       <c r="J3">
-        <v>36</v>
+        <v>37</v>
       </c>
     </row>
     <row r="4" spans="1:10">
@@ -25150,7 +25150,7 @@
         <v>381</v>
       </c>
       <c r="J10">
-        <v>207</v>
+        <v>208</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -25182,7 +25182,7 @@
         <v>867</v>
       </c>
       <c r="J11">
-        <v>489</v>
+        <v>491</v>
       </c>
     </row>
   </sheetData>
@@ -25479,7 +25479,7 @@
         <v>576</v>
       </c>
       <c r="J10">
-        <v>309</v>
+        <v>310</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -25511,7 +25511,7 @@
         <v>628</v>
       </c>
       <c r="J11">
-        <v>334</v>
+        <v>335</v>
       </c>
     </row>
   </sheetData>
@@ -25856,7 +25856,7 @@
         <v>130</v>
       </c>
       <c r="J10">
-        <v>85</v>
+        <v>86</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -25888,7 +25888,7 @@
         <v>462</v>
       </c>
       <c r="J11">
-        <v>307</v>
+        <v>308</v>
       </c>
     </row>
   </sheetData>
@@ -26560,7 +26560,7 @@
         <v>1118</v>
       </c>
       <c r="J10">
-        <v>603</v>
+        <v>604</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -26592,7 +26592,7 @@
         <v>1797</v>
       </c>
       <c r="J11">
-        <v>1026</v>
+        <v>1027</v>
       </c>
     </row>
   </sheetData>
@@ -26713,7 +26713,7 @@
         <v>36</v>
       </c>
       <c r="J3">
-        <v>14</v>
+        <v>15</v>
       </c>
     </row>
     <row r="4" spans="1:10">
@@ -26774,7 +26774,7 @@
         <v>94</v>
       </c>
       <c r="J5">
-        <v>39</v>
+        <v>40</v>
       </c>
     </row>
     <row r="6" spans="1:10">
@@ -26896,7 +26896,7 @@
         <v>50</v>
       </c>
       <c r="J9">
-        <v>14</v>
+        <v>15</v>
       </c>
     </row>
     <row r="10" spans="1:10">
@@ -26928,7 +26928,7 @@
         <v>371</v>
       </c>
       <c r="J10">
-        <v>159</v>
+        <v>161</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -26960,7 +26960,7 @@
         <v>718</v>
       </c>
       <c r="J11">
-        <v>351</v>
+        <v>356</v>
       </c>
     </row>
   </sheetData>
@@ -27619,7 +27619,7 @@
         <v>376</v>
       </c>
       <c r="J10">
-        <v>265</v>
+        <v>267</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -27651,7 +27651,7 @@
         <v>595</v>
       </c>
       <c r="J11">
-        <v>430</v>
+        <v>432</v>
       </c>
     </row>
   </sheetData>
@@ -27996,7 +27996,7 @@
         <v>193</v>
       </c>
       <c r="J10">
-        <v>90</v>
+        <v>91</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -28028,7 +28028,7 @@
         <v>519</v>
       </c>
       <c r="J11">
-        <v>310</v>
+        <v>311</v>
       </c>
     </row>
   </sheetData>
@@ -28117,7 +28117,7 @@
         <v>11</v>
       </c>
       <c r="J2">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="3" spans="1:10">
@@ -28378,7 +28378,7 @@
         <v>175</v>
       </c>
       <c r="J11">
-        <v>86</v>
+        <v>87</v>
       </c>
     </row>
   </sheetData>
@@ -29308,7 +29308,7 @@
         <v>131</v>
       </c>
       <c r="J5">
-        <v>79</v>
+        <v>80</v>
       </c>
     </row>
     <row r="6" spans="1:10">
@@ -29401,7 +29401,7 @@
         <v>216</v>
       </c>
       <c r="J8">
-        <v>195</v>
+        <v>197</v>
       </c>
     </row>
     <row r="9" spans="1:10">
@@ -29433,7 +29433,7 @@
         <v>107</v>
       </c>
       <c r="J9">
-        <v>58</v>
+        <v>59</v>
       </c>
     </row>
     <row r="10" spans="1:10">
@@ -29465,7 +29465,7 @@
         <v>1222</v>
       </c>
       <c r="J10">
-        <v>680</v>
+        <v>684</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -29497,7 +29497,7 @@
         <v>1879</v>
       </c>
       <c r="J11">
-        <v>1155</v>
+        <v>1163</v>
       </c>
     </row>
   </sheetData>
@@ -29618,7 +29618,7 @@
         <v>32</v>
       </c>
       <c r="J3">
-        <v>18</v>
+        <v>19</v>
       </c>
     </row>
     <row r="4" spans="1:10">
@@ -29682,7 +29682,7 @@
         <v>66</v>
       </c>
       <c r="J5">
-        <v>32</v>
+        <v>33</v>
       </c>
     </row>
     <row r="6" spans="1:10">
@@ -29871,7 +29871,7 @@
         <v>761</v>
       </c>
       <c r="J11">
-        <v>499</v>
+        <v>501</v>
       </c>
     </row>
   </sheetData>
@@ -29960,7 +29960,7 @@
         <v>128</v>
       </c>
       <c r="J2">
-        <v>64</v>
+        <v>65</v>
       </c>
     </row>
     <row r="3" spans="1:10">
@@ -30152,7 +30152,7 @@
         <v>383</v>
       </c>
       <c r="J8">
-        <v>300</v>
+        <v>303</v>
       </c>
     </row>
     <row r="9" spans="1:10">
@@ -30216,7 +30216,7 @@
         <v>527</v>
       </c>
       <c r="J10">
-        <v>322</v>
+        <v>325</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -30248,7 +30248,7 @@
         <v>1488</v>
       </c>
       <c r="J11">
-        <v>930</v>
+        <v>937</v>
       </c>
     </row>
   </sheetData>
@@ -30551,7 +30551,7 @@
         <v>152</v>
       </c>
       <c r="J10">
-        <v>79</v>
+        <v>80</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -30583,7 +30583,7 @@
         <v>248</v>
       </c>
       <c r="J11">
-        <v>170</v>
+        <v>171</v>
       </c>
     </row>
   </sheetData>
@@ -30828,7 +30828,7 @@
         <v>112</v>
       </c>
       <c r="J8">
-        <v>75</v>
+        <v>76</v>
       </c>
     </row>
     <row r="9" spans="1:10">
@@ -30924,7 +30924,7 @@
         <v>677</v>
       </c>
       <c r="J11">
-        <v>416</v>
+        <v>417</v>
       </c>
     </row>
   </sheetData>
@@ -31163,7 +31163,7 @@
         <v>20</v>
       </c>
       <c r="J8">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="9" spans="1:10">
@@ -31227,7 +31227,7 @@
         <v>162</v>
       </c>
       <c r="J10">
-        <v>109</v>
+        <v>111</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -31259,7 +31259,7 @@
         <v>237</v>
       </c>
       <c r="J11">
-        <v>172</v>
+        <v>175</v>
       </c>
     </row>
   </sheetData>
@@ -31589,7 +31589,7 @@
         <v>124</v>
       </c>
       <c r="J10">
-        <v>75</v>
+        <v>76</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -31621,7 +31621,7 @@
         <v>335</v>
       </c>
       <c r="J11">
-        <v>258</v>
+        <v>259</v>
       </c>
     </row>
   </sheetData>
@@ -31710,7 +31710,7 @@
         <v>90</v>
       </c>
       <c r="J2">
-        <v>47</v>
+        <v>48</v>
       </c>
     </row>
     <row r="3" spans="1:10">
@@ -31902,7 +31902,7 @@
         <v>122</v>
       </c>
       <c r="J8">
-        <v>126</v>
+        <v>128</v>
       </c>
     </row>
     <row r="9" spans="1:10">
@@ -31966,7 +31966,7 @@
         <v>389</v>
       </c>
       <c r="J10">
-        <v>255</v>
+        <v>256</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -31998,7 +31998,7 @@
         <v>886</v>
       </c>
       <c r="J11">
-        <v>585</v>
+        <v>589</v>
       </c>
     </row>
   </sheetData>
@@ -32273,7 +32273,7 @@
         <v>405</v>
       </c>
       <c r="J8">
-        <v>352</v>
+        <v>353</v>
       </c>
     </row>
     <row r="9" spans="1:10">
@@ -32337,7 +32337,7 @@
         <v>670</v>
       </c>
       <c r="J10">
-        <v>319</v>
+        <v>321</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -32369,7 +32369,7 @@
         <v>1368</v>
       </c>
       <c r="J11">
-        <v>837</v>
+        <v>840</v>
       </c>
     </row>
   </sheetData>
@@ -32644,7 +32644,7 @@
         <v>338</v>
       </c>
       <c r="J8">
-        <v>259</v>
+        <v>262</v>
       </c>
     </row>
     <row r="9" spans="1:10">
@@ -32708,7 +32708,7 @@
         <v>1773</v>
       </c>
       <c r="J10">
-        <v>1027</v>
+        <v>1033</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -32740,7 +32740,7 @@
         <v>2622</v>
       </c>
       <c r="J11">
-        <v>1536</v>
+        <v>1545</v>
       </c>
     </row>
   </sheetData>
@@ -33223,7 +33223,7 @@
         <v>17</v>
       </c>
       <c r="J3">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="4" spans="1:10">
@@ -33376,7 +33376,7 @@
         <v>87</v>
       </c>
       <c r="J9">
-        <v>22</v>
+        <v>23</v>
       </c>
     </row>
     <row r="10" spans="1:10">
@@ -33440,7 +33440,7 @@
         <v>337</v>
       </c>
       <c r="J11">
-        <v>153</v>
+        <v>155</v>
       </c>
     </row>
   </sheetData>
@@ -33561,7 +33561,7 @@
         <v>58</v>
       </c>
       <c r="J3">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="4" spans="1:10">
@@ -33712,7 +33712,7 @@
         <v>334</v>
       </c>
       <c r="J8">
-        <v>194</v>
+        <v>195</v>
       </c>
     </row>
     <row r="9" spans="1:10">
@@ -33808,7 +33808,7 @@
         <v>1187</v>
       </c>
       <c r="J11">
-        <v>638</v>
+        <v>640</v>
       </c>
     </row>
   </sheetData>
@@ -34083,7 +34083,7 @@
         <v>116</v>
       </c>
       <c r="J8">
-        <v>40</v>
+        <v>41</v>
       </c>
     </row>
     <row r="9" spans="1:10">
@@ -34115,7 +34115,7 @@
         <v>153</v>
       </c>
       <c r="J9">
-        <v>56</v>
+        <v>57</v>
       </c>
     </row>
   </sheetData>
@@ -34439,7 +34439,7 @@
         <v>313</v>
       </c>
       <c r="J10">
-        <v>151</v>
+        <v>153</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -34471,7 +34471,7 @@
         <v>494</v>
       </c>
       <c r="J11">
-        <v>253</v>
+        <v>255</v>
       </c>
     </row>
   </sheetData>
@@ -35231,7 +35231,7 @@
         <v>19</v>
       </c>
       <c r="J2">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="3" spans="1:10">
@@ -35437,7 +35437,7 @@
         <v>93</v>
       </c>
       <c r="J9">
-        <v>43</v>
+        <v>44</v>
       </c>
     </row>
     <row r="10" spans="1:10">
@@ -35469,7 +35469,7 @@
         <v>181</v>
       </c>
       <c r="J10">
-        <v>89</v>
+        <v>91</v>
       </c>
     </row>
   </sheetData>
@@ -35881,6 +35881,9 @@
       <c r="I2">
         <v>3</v>
       </c>
+      <c r="J2">
+        <v>1</v>
+      </c>
     </row>
     <row r="3" spans="1:10">
       <c r="A3" s="1" t="s">
@@ -36122,7 +36125,7 @@
         <v>99</v>
       </c>
       <c r="J11">
-        <v>35</v>
+        <v>36</v>
       </c>
     </row>
   </sheetData>
@@ -36307,7 +36310,7 @@
         <v>161</v>
       </c>
       <c r="J5">
-        <v>91</v>
+        <v>92</v>
       </c>
     </row>
     <row r="6" spans="1:10">
@@ -36403,7 +36406,7 @@
         <v>291</v>
       </c>
       <c r="J8">
-        <v>195</v>
+        <v>196</v>
       </c>
     </row>
     <row r="9" spans="1:10">
@@ -36435,7 +36438,7 @@
         <v>125</v>
       </c>
       <c r="J9">
-        <v>62</v>
+        <v>63</v>
       </c>
     </row>
     <row r="10" spans="1:10">
@@ -36467,7 +36470,7 @@
         <v>905</v>
       </c>
       <c r="J10">
-        <v>468</v>
+        <v>471</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -36499,7 +36502,7 @@
         <v>1669</v>
       </c>
       <c r="J11">
-        <v>937</v>
+        <v>943</v>
       </c>
     </row>
   </sheetData>
@@ -37523,7 +37526,7 @@
         <v>116</v>
       </c>
       <c r="J10">
-        <v>61</v>
+        <v>62</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -37555,7 +37558,7 @@
         <v>236</v>
       </c>
       <c r="J11">
-        <v>157</v>
+        <v>158</v>
       </c>
     </row>
   </sheetData>
@@ -37760,7 +37763,7 @@
         <v>80</v>
       </c>
       <c r="J6">
-        <v>47</v>
+        <v>48</v>
       </c>
     </row>
     <row r="7" spans="1:10">
@@ -37806,7 +37809,7 @@
         <v>160</v>
       </c>
       <c r="J8">
-        <v>64</v>
+        <v>65</v>
       </c>
     </row>
     <row r="9" spans="1:10">
@@ -37870,7 +37873,7 @@
         <v>717</v>
       </c>
       <c r="J10">
-        <v>328</v>
+        <v>329</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -37902,7 +37905,7 @@
         <v>1066</v>
       </c>
       <c r="J11">
-        <v>491</v>
+        <v>494</v>
       </c>
     </row>
   </sheetData>
@@ -38693,7 +38696,7 @@
         <v>2</v>
       </c>
       <c r="J3">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="4" spans="1:10">
@@ -38901,7 +38904,7 @@
         <v>307</v>
       </c>
       <c r="J11">
-        <v>157</v>
+        <v>158</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add data for 2023-07-25
</commit_message>
<xml_diff>
--- a/output/index-crime-full-year.xlsx
+++ b/output/index-crime-full-year.xlsx
@@ -892,10 +892,10 @@
         <v>7243</v>
       </c>
       <c r="I2">
-        <v>7277</v>
+        <v>7278</v>
       </c>
       <c r="J2">
-        <v>4185</v>
+        <v>4213</v>
       </c>
     </row>
     <row r="3" spans="1:10">
@@ -927,7 +927,7 @@
         <v>7486</v>
       </c>
       <c r="J3">
-        <v>4407</v>
+        <v>4434</v>
       </c>
     </row>
     <row r="4" spans="1:10">
@@ -959,7 +959,7 @@
         <v>422</v>
       </c>
       <c r="J4">
-        <v>276</v>
+        <v>280</v>
       </c>
     </row>
     <row r="5" spans="1:10">
@@ -991,7 +991,7 @@
         <v>7592</v>
       </c>
       <c r="J5">
-        <v>4063</v>
+        <v>4083</v>
       </c>
     </row>
     <row r="6" spans="1:10">
@@ -1002,7 +1002,7 @@
         <v>1680</v>
       </c>
       <c r="C6">
-        <v>1829</v>
+        <v>1830</v>
       </c>
       <c r="D6">
         <v>1957</v>
@@ -1017,13 +1017,13 @@
         <v>1466</v>
       </c>
       <c r="H6">
-        <v>1699</v>
+        <v>1700</v>
       </c>
       <c r="I6">
         <v>1767</v>
       </c>
       <c r="J6">
-        <v>986</v>
+        <v>991</v>
       </c>
     </row>
     <row r="7" spans="1:10">
@@ -1055,7 +1055,7 @@
         <v>718</v>
       </c>
       <c r="J7">
-        <v>351</v>
+        <v>353</v>
       </c>
     </row>
     <row r="8" spans="1:10">
@@ -1087,7 +1087,7 @@
         <v>21446</v>
       </c>
       <c r="J8">
-        <v>16540</v>
+        <v>16632</v>
       </c>
     </row>
     <row r="9" spans="1:10">
@@ -1113,13 +1113,13 @@
         <v>7855</v>
       </c>
       <c r="H9">
-        <v>7917</v>
+        <v>7918</v>
       </c>
       <c r="I9">
         <v>8965</v>
       </c>
       <c r="J9">
-        <v>5243</v>
+        <v>5292</v>
       </c>
     </row>
     <row r="10" spans="1:10">
@@ -1151,7 +1151,7 @@
         <v>54808</v>
       </c>
       <c r="J10">
-        <v>30269</v>
+        <v>30442</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -1162,7 +1162,7 @@
         <v>104362</v>
       </c>
       <c r="C11">
-        <v>116083</v>
+        <v>116084</v>
       </c>
       <c r="D11">
         <v>117356</v>
@@ -1177,13 +1177,13 @@
         <v>85314</v>
       </c>
       <c r="H11">
-        <v>84595</v>
+        <v>84597</v>
       </c>
       <c r="I11">
-        <v>110481</v>
+        <v>110482</v>
       </c>
       <c r="J11">
-        <v>66320</v>
+        <v>66720</v>
       </c>
     </row>
   </sheetData>
@@ -1304,7 +1304,7 @@
         <v>38</v>
       </c>
       <c r="J3">
-        <v>24</v>
+        <v>25</v>
       </c>
     </row>
     <row r="4" spans="1:10">
@@ -1440,7 +1440,7 @@
         <v>227</v>
       </c>
       <c r="J8">
-        <v>219</v>
+        <v>221</v>
       </c>
     </row>
     <row r="9" spans="1:10">
@@ -1504,7 +1504,7 @@
         <v>648</v>
       </c>
       <c r="J10">
-        <v>408</v>
+        <v>412</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -1536,7 +1536,7 @@
         <v>1153</v>
       </c>
       <c r="J11">
-        <v>794</v>
+        <v>801</v>
       </c>
     </row>
   </sheetData>
@@ -2123,7 +2123,7 @@
         <v>111</v>
       </c>
       <c r="J9">
-        <v>79</v>
+        <v>81</v>
       </c>
     </row>
     <row r="10" spans="1:10">
@@ -2187,7 +2187,7 @@
         <v>1712</v>
       </c>
       <c r="J11">
-        <v>1127</v>
+        <v>1129</v>
       </c>
     </row>
   </sheetData>
@@ -2308,7 +2308,7 @@
         <v>56</v>
       </c>
       <c r="J3">
-        <v>29</v>
+        <v>30</v>
       </c>
     </row>
     <row r="4" spans="1:10">
@@ -2369,7 +2369,7 @@
         <v>124</v>
       </c>
       <c r="J5">
-        <v>64</v>
+        <v>67</v>
       </c>
     </row>
     <row r="6" spans="1:10">
@@ -2462,7 +2462,7 @@
         <v>188</v>
       </c>
       <c r="J8">
-        <v>148</v>
+        <v>149</v>
       </c>
     </row>
     <row r="9" spans="1:10">
@@ -2526,7 +2526,7 @@
         <v>712</v>
       </c>
       <c r="J10">
-        <v>406</v>
+        <v>408</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -2558,7 +2558,7 @@
         <v>1228</v>
       </c>
       <c r="J11">
-        <v>730</v>
+        <v>737</v>
       </c>
     </row>
   </sheetData>
@@ -2679,7 +2679,7 @@
         <v>244</v>
       </c>
       <c r="J3">
-        <v>158</v>
+        <v>159</v>
       </c>
     </row>
     <row r="4" spans="1:10">
@@ -2775,7 +2775,7 @@
         <v>42</v>
       </c>
       <c r="J6">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="7" spans="1:10">
@@ -2839,7 +2839,7 @@
         <v>700</v>
       </c>
       <c r="J8">
-        <v>487</v>
+        <v>488</v>
       </c>
     </row>
     <row r="9" spans="1:10">
@@ -2903,7 +2903,7 @@
         <v>820</v>
       </c>
       <c r="J10">
-        <v>445</v>
+        <v>447</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -2935,7 +2935,7 @@
         <v>2472</v>
       </c>
       <c r="J11">
-        <v>1461</v>
+        <v>1466</v>
       </c>
     </row>
   </sheetData>
@@ -3024,7 +3024,7 @@
         <v>61</v>
       </c>
       <c r="J2">
-        <v>42</v>
+        <v>43</v>
       </c>
     </row>
     <row r="3" spans="1:10">
@@ -3245,7 +3245,7 @@
         <v>151</v>
       </c>
       <c r="J9">
-        <v>83</v>
+        <v>85</v>
       </c>
     </row>
     <row r="10" spans="1:10">
@@ -3277,7 +3277,7 @@
         <v>913</v>
       </c>
       <c r="J10">
-        <v>614</v>
+        <v>620</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -3309,7 +3309,7 @@
         <v>1600</v>
       </c>
       <c r="J11">
-        <v>1114</v>
+        <v>1123</v>
       </c>
     </row>
   </sheetData>
@@ -3584,7 +3584,7 @@
         <v>57</v>
       </c>
       <c r="J8">
-        <v>52</v>
+        <v>53</v>
       </c>
     </row>
     <row r="9" spans="1:10">
@@ -3648,7 +3648,7 @@
         <v>106</v>
       </c>
       <c r="J10">
-        <v>46</v>
+        <v>47</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -3680,7 +3680,7 @@
         <v>260</v>
       </c>
       <c r="J11">
-        <v>167</v>
+        <v>169</v>
       </c>
     </row>
   </sheetData>
@@ -3961,7 +3961,7 @@
         <v>220</v>
       </c>
       <c r="J8">
-        <v>193</v>
+        <v>194</v>
       </c>
     </row>
     <row r="9" spans="1:10">
@@ -4025,7 +4025,7 @@
         <v>681</v>
       </c>
       <c r="J10">
-        <v>492</v>
+        <v>494</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -4057,7 +4057,7 @@
         <v>1279</v>
       </c>
       <c r="J11">
-        <v>892</v>
+        <v>895</v>
       </c>
     </row>
   </sheetData>
@@ -4146,7 +4146,7 @@
         <v>459</v>
       </c>
       <c r="J2">
-        <v>268</v>
+        <v>269</v>
       </c>
     </row>
     <row r="3" spans="1:10">
@@ -4338,7 +4338,7 @@
         <v>794</v>
       </c>
       <c r="J8">
-        <v>606</v>
+        <v>608</v>
       </c>
     </row>
     <row r="9" spans="1:10">
@@ -4370,7 +4370,7 @@
         <v>433</v>
       </c>
       <c r="J9">
-        <v>208</v>
+        <v>213</v>
       </c>
     </row>
     <row r="10" spans="1:10">
@@ -4402,7 +4402,7 @@
         <v>1302</v>
       </c>
       <c r="J10">
-        <v>734</v>
+        <v>737</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -4434,7 +4434,7 @@
         <v>3950</v>
       </c>
       <c r="J11">
-        <v>2379</v>
+        <v>2390</v>
       </c>
     </row>
   </sheetData>
@@ -4697,7 +4697,7 @@
         <v>131</v>
       </c>
       <c r="J8">
-        <v>147</v>
+        <v>149</v>
       </c>
     </row>
     <row r="9" spans="1:10">
@@ -4761,7 +4761,7 @@
         <v>921</v>
       </c>
       <c r="J10">
-        <v>399</v>
+        <v>400</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -4793,7 +4793,7 @@
         <v>1318</v>
       </c>
       <c r="J11">
-        <v>688</v>
+        <v>691</v>
       </c>
     </row>
   </sheetData>
@@ -4882,7 +4882,7 @@
         <v>216</v>
       </c>
       <c r="J2">
-        <v>124</v>
+        <v>126</v>
       </c>
     </row>
     <row r="3" spans="1:10">
@@ -4914,7 +4914,7 @@
         <v>280</v>
       </c>
       <c r="J3">
-        <v>121</v>
+        <v>124</v>
       </c>
     </row>
     <row r="4" spans="1:10">
@@ -4946,7 +4946,7 @@
         <v>14</v>
       </c>
       <c r="J4">
-        <v>12</v>
+        <v>14</v>
       </c>
     </row>
     <row r="5" spans="1:10">
@@ -5074,7 +5074,7 @@
         <v>653</v>
       </c>
       <c r="J8">
-        <v>544</v>
+        <v>547</v>
       </c>
     </row>
     <row r="9" spans="1:10">
@@ -5138,7 +5138,7 @@
         <v>1089</v>
       </c>
       <c r="J10">
-        <v>683</v>
+        <v>689</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -5170,7 +5170,7 @@
         <v>2956</v>
       </c>
       <c r="J11">
-        <v>1921</v>
+        <v>1937</v>
       </c>
     </row>
   </sheetData>
@@ -5259,7 +5259,7 @@
         <v>917</v>
       </c>
       <c r="J2">
-        <v>572</v>
+        <v>579</v>
       </c>
     </row>
     <row r="3" spans="1:10">
@@ -5291,7 +5291,7 @@
         <v>155</v>
       </c>
       <c r="J3">
-        <v>103</v>
+        <v>106</v>
       </c>
     </row>
     <row r="4" spans="1:10">
@@ -5355,7 +5355,7 @@
         <v>247</v>
       </c>
       <c r="J5">
-        <v>171</v>
+        <v>172</v>
       </c>
     </row>
     <row r="6" spans="1:10">
@@ -5387,7 +5387,7 @@
         <v>793</v>
       </c>
       <c r="J6">
-        <v>572</v>
+        <v>574</v>
       </c>
     </row>
     <row r="7" spans="1:10">
@@ -5419,7 +5419,7 @@
         <v>2686</v>
       </c>
       <c r="J7">
-        <v>1671</v>
+        <v>1678</v>
       </c>
     </row>
     <row r="8" spans="1:10">
@@ -5451,7 +5451,7 @@
         <v>4743</v>
       </c>
       <c r="J8">
-        <v>2812</v>
+        <v>2830</v>
       </c>
     </row>
     <row r="9" spans="1:10">
@@ -5483,7 +5483,7 @@
         <v>519</v>
       </c>
       <c r="J9">
-        <v>311</v>
+        <v>316</v>
       </c>
     </row>
     <row r="10" spans="1:10">
@@ -5515,7 +5515,7 @@
         <v>948</v>
       </c>
       <c r="J10">
-        <v>536</v>
+        <v>541</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -5547,7 +5547,7 @@
         <v>1712</v>
       </c>
       <c r="J11">
-        <v>1127</v>
+        <v>1129</v>
       </c>
     </row>
     <row r="12" spans="1:10">
@@ -5579,7 +5579,7 @@
         <v>412</v>
       </c>
       <c r="J12">
-        <v>233</v>
+        <v>235</v>
       </c>
     </row>
     <row r="13" spans="1:10">
@@ -5611,7 +5611,7 @@
         <v>258</v>
       </c>
       <c r="J13">
-        <v>154</v>
+        <v>156</v>
       </c>
     </row>
     <row r="14" spans="1:10">
@@ -5643,7 +5643,7 @@
         <v>718</v>
       </c>
       <c r="J14">
-        <v>356</v>
+        <v>360</v>
       </c>
     </row>
     <row r="15" spans="1:10">
@@ -5675,7 +5675,7 @@
         <v>886</v>
       </c>
       <c r="J15">
-        <v>589</v>
+        <v>592</v>
       </c>
     </row>
     <row r="16" spans="1:10">
@@ -5707,7 +5707,7 @@
         <v>595</v>
       </c>
       <c r="J16">
-        <v>432</v>
+        <v>434</v>
       </c>
     </row>
     <row r="17" spans="1:10">
@@ -5771,7 +5771,7 @@
         <v>695</v>
       </c>
       <c r="J18">
-        <v>439</v>
+        <v>440</v>
       </c>
     </row>
     <row r="19" spans="1:10">
@@ -5803,7 +5803,7 @@
         <v>2636</v>
       </c>
       <c r="J19">
-        <v>1539</v>
+        <v>1554</v>
       </c>
     </row>
     <row r="20" spans="1:10">
@@ -5835,7 +5835,7 @@
         <v>2045</v>
       </c>
       <c r="J20">
-        <v>1111</v>
+        <v>1116</v>
       </c>
     </row>
     <row r="21" spans="1:10">
@@ -5867,7 +5867,7 @@
         <v>337</v>
       </c>
       <c r="J21">
-        <v>155</v>
+        <v>158</v>
       </c>
     </row>
     <row r="22" spans="1:10">
@@ -5899,7 +5899,7 @@
         <v>418</v>
       </c>
       <c r="J22">
-        <v>305</v>
+        <v>308</v>
       </c>
     </row>
     <row r="23" spans="1:10">
@@ -5931,7 +5931,7 @@
         <v>1368</v>
       </c>
       <c r="J23">
-        <v>840</v>
+        <v>844</v>
       </c>
     </row>
     <row r="24" spans="1:10">
@@ -5963,7 +5963,7 @@
         <v>500</v>
       </c>
       <c r="J24">
-        <v>352</v>
+        <v>354</v>
       </c>
     </row>
     <row r="25" spans="1:10">
@@ -5995,7 +5995,7 @@
         <v>429</v>
       </c>
       <c r="J25">
-        <v>280</v>
+        <v>284</v>
       </c>
     </row>
     <row r="26" spans="1:10">
@@ -6027,7 +6027,7 @@
         <v>248</v>
       </c>
       <c r="J26">
-        <v>171</v>
+        <v>173</v>
       </c>
     </row>
     <row r="27" spans="1:10">
@@ -6059,7 +6059,7 @@
         <v>1258</v>
       </c>
       <c r="J27">
-        <v>779</v>
+        <v>780</v>
       </c>
     </row>
     <row r="28" spans="1:10">
@@ -6091,7 +6091,7 @@
         <v>99</v>
       </c>
       <c r="J28">
-        <v>36</v>
+        <v>37</v>
       </c>
     </row>
     <row r="29" spans="1:10">
@@ -6123,7 +6123,7 @@
         <v>3950</v>
       </c>
       <c r="J29">
-        <v>2379</v>
+        <v>2390</v>
       </c>
     </row>
     <row r="30" spans="1:10">
@@ -6155,7 +6155,7 @@
         <v>260</v>
       </c>
       <c r="J30">
-        <v>167</v>
+        <v>169</v>
       </c>
     </row>
     <row r="31" spans="1:10">
@@ -6184,10 +6184,10 @@
         <v>613</v>
       </c>
       <c r="I31">
-        <v>867</v>
+        <v>868</v>
       </c>
       <c r="J31">
-        <v>491</v>
+        <v>494</v>
       </c>
     </row>
     <row r="32" spans="1:10">
@@ -6219,7 +6219,7 @@
         <v>209</v>
       </c>
       <c r="J32">
-        <v>158</v>
+        <v>159</v>
       </c>
     </row>
     <row r="33" spans="1:10">
@@ -6251,7 +6251,7 @@
         <v>3011</v>
       </c>
       <c r="J33">
-        <v>1892</v>
+        <v>1907</v>
       </c>
     </row>
     <row r="34" spans="1:10">
@@ -6283,7 +6283,7 @@
         <v>761</v>
       </c>
       <c r="J34">
-        <v>501</v>
+        <v>502</v>
       </c>
     </row>
     <row r="35" spans="1:10">
@@ -6315,7 +6315,7 @@
         <v>235</v>
       </c>
       <c r="J35">
-        <v>138</v>
+        <v>139</v>
       </c>
     </row>
     <row r="36" spans="1:10">
@@ -6347,7 +6347,7 @@
         <v>1491</v>
       </c>
       <c r="J36">
-        <v>945</v>
+        <v>950</v>
       </c>
     </row>
     <row r="37" spans="1:10">
@@ -6379,7 +6379,7 @@
         <v>2547</v>
       </c>
       <c r="J37">
-        <v>1603</v>
+        <v>1610</v>
       </c>
     </row>
     <row r="38" spans="1:10">
@@ -6443,7 +6443,7 @@
         <v>153</v>
       </c>
       <c r="J39">
-        <v>57</v>
+        <v>58</v>
       </c>
     </row>
     <row r="40" spans="1:10">
@@ -6475,7 +6475,7 @@
         <v>236</v>
       </c>
       <c r="J40">
-        <v>158</v>
+        <v>159</v>
       </c>
     </row>
     <row r="41" spans="1:10">
@@ -6539,7 +6539,7 @@
         <v>2956</v>
       </c>
       <c r="J42">
-        <v>1921</v>
+        <v>1937</v>
       </c>
     </row>
     <row r="43" spans="1:10">
@@ -6571,7 +6571,7 @@
         <v>1153</v>
       </c>
       <c r="J43">
-        <v>794</v>
+        <v>801</v>
       </c>
     </row>
     <row r="44" spans="1:10">
@@ -6603,7 +6603,7 @@
         <v>1228</v>
       </c>
       <c r="J44">
-        <v>730</v>
+        <v>737</v>
       </c>
     </row>
     <row r="45" spans="1:10">
@@ -6667,7 +6667,7 @@
         <v>436</v>
       </c>
       <c r="J46">
-        <v>278</v>
+        <v>280</v>
       </c>
     </row>
     <row r="47" spans="1:10">
@@ -6699,7 +6699,7 @@
         <v>903</v>
       </c>
       <c r="J47">
-        <v>559</v>
+        <v>566</v>
       </c>
     </row>
     <row r="48" spans="1:10">
@@ -6731,7 +6731,7 @@
         <v>2622</v>
       </c>
       <c r="J48">
-        <v>1545</v>
+        <v>1553</v>
       </c>
     </row>
     <row r="49" spans="1:10">
@@ -6763,7 +6763,7 @@
         <v>1648</v>
       </c>
       <c r="J49">
-        <v>947</v>
+        <v>952</v>
       </c>
     </row>
     <row r="50" spans="1:10">
@@ -6795,7 +6795,7 @@
         <v>960</v>
       </c>
       <c r="J50">
-        <v>561</v>
+        <v>565</v>
       </c>
     </row>
     <row r="51" spans="1:10">
@@ -6827,7 +6827,7 @@
         <v>1337</v>
       </c>
       <c r="J51">
-        <v>886</v>
+        <v>892</v>
       </c>
     </row>
     <row r="52" spans="1:10">
@@ -6859,7 +6859,7 @@
         <v>1491</v>
       </c>
       <c r="J52">
-        <v>1060</v>
+        <v>1063</v>
       </c>
     </row>
     <row r="53" spans="1:10">
@@ -6891,7 +6891,7 @@
         <v>1600</v>
       </c>
       <c r="J53">
-        <v>1114</v>
+        <v>1123</v>
       </c>
     </row>
     <row r="54" spans="1:10">
@@ -6923,7 +6923,7 @@
         <v>3506</v>
       </c>
       <c r="J54">
-        <v>2023</v>
+        <v>2033</v>
       </c>
     </row>
     <row r="55" spans="1:10">
@@ -6955,7 +6955,7 @@
         <v>1244</v>
       </c>
       <c r="J55">
-        <v>706</v>
+        <v>710</v>
       </c>
     </row>
     <row r="56" spans="1:10">
@@ -7019,7 +7019,7 @@
         <v>406</v>
       </c>
       <c r="J57">
-        <v>289</v>
+        <v>290</v>
       </c>
     </row>
     <row r="58" spans="1:10">
@@ -7083,7 +7083,7 @@
         <v>271</v>
       </c>
       <c r="J59">
-        <v>182</v>
+        <v>185</v>
       </c>
     </row>
     <row r="60" spans="1:10">
@@ -7115,7 +7115,7 @@
         <v>768</v>
       </c>
       <c r="J60">
-        <v>480</v>
+        <v>481</v>
       </c>
     </row>
     <row r="61" spans="1:10">
@@ -7190,7 +7190,7 @@
         <v>1473</v>
       </c>
       <c r="C63">
-        <v>1179</v>
+        <v>1180</v>
       </c>
       <c r="D63">
         <v>1523</v>
@@ -7205,13 +7205,13 @@
         <v>1651</v>
       </c>
       <c r="H63">
-        <v>2168</v>
+        <v>2170</v>
       </c>
       <c r="I63">
         <v>2481</v>
       </c>
       <c r="J63">
-        <v>739</v>
+        <v>744</v>
       </c>
     </row>
     <row r="64" spans="1:10">
@@ -7243,7 +7243,7 @@
         <v>1187</v>
       </c>
       <c r="J64">
-        <v>640</v>
+        <v>641</v>
       </c>
     </row>
     <row r="65" spans="1:10">
@@ -7275,7 +7275,7 @@
         <v>1515</v>
       </c>
       <c r="J65">
-        <v>1020</v>
+        <v>1024</v>
       </c>
     </row>
     <row r="66" spans="1:10">
@@ -7307,7 +7307,7 @@
         <v>715</v>
       </c>
       <c r="J66">
-        <v>438</v>
+        <v>439</v>
       </c>
     </row>
     <row r="67" spans="1:10">
@@ -7339,7 +7339,7 @@
         <v>2510</v>
       </c>
       <c r="J67">
-        <v>1555</v>
+        <v>1560</v>
       </c>
     </row>
     <row r="68" spans="1:10">
@@ -7371,7 +7371,7 @@
         <v>437</v>
       </c>
       <c r="J68">
-        <v>204</v>
+        <v>205</v>
       </c>
     </row>
     <row r="69" spans="1:10">
@@ -7403,7 +7403,7 @@
         <v>494</v>
       </c>
       <c r="J69">
-        <v>255</v>
+        <v>260</v>
       </c>
     </row>
     <row r="70" spans="1:10">
@@ -7435,7 +7435,7 @@
         <v>677</v>
       </c>
       <c r="J70">
-        <v>417</v>
+        <v>420</v>
       </c>
     </row>
     <row r="71" spans="1:10">
@@ -7467,7 +7467,7 @@
         <v>335</v>
       </c>
       <c r="J71">
-        <v>259</v>
+        <v>260</v>
       </c>
     </row>
     <row r="72" spans="1:10">
@@ -7499,7 +7499,7 @@
         <v>706</v>
       </c>
       <c r="J72">
-        <v>391</v>
+        <v>392</v>
       </c>
     </row>
     <row r="73" spans="1:10">
@@ -7531,7 +7531,7 @@
         <v>1279</v>
       </c>
       <c r="J73">
-        <v>892</v>
+        <v>895</v>
       </c>
     </row>
     <row r="74" spans="1:10">
@@ -7595,7 +7595,7 @@
         <v>340</v>
       </c>
       <c r="J75">
-        <v>204</v>
+        <v>205</v>
       </c>
     </row>
     <row r="76" spans="1:10">
@@ -7627,7 +7627,7 @@
         <v>2923</v>
       </c>
       <c r="J76">
-        <v>1706</v>
+        <v>1715</v>
       </c>
     </row>
     <row r="77" spans="1:10">
@@ -7659,7 +7659,7 @@
         <v>462</v>
       </c>
       <c r="J77">
-        <v>308</v>
+        <v>309</v>
       </c>
     </row>
     <row r="78" spans="1:10">
@@ -7691,7 +7691,7 @@
         <v>1797</v>
       </c>
       <c r="J78">
-        <v>1027</v>
+        <v>1029</v>
       </c>
     </row>
     <row r="79" spans="1:10">
@@ -7723,7 +7723,7 @@
         <v>2472</v>
       </c>
       <c r="J79">
-        <v>1461</v>
+        <v>1466</v>
       </c>
     </row>
     <row r="80" spans="1:10">
@@ -7755,7 +7755,7 @@
         <v>393</v>
       </c>
       <c r="J80">
-        <v>180</v>
+        <v>181</v>
       </c>
     </row>
     <row r="81" spans="1:10">
@@ -7787,7 +7787,7 @@
         <v>219</v>
       </c>
       <c r="J81">
-        <v>127</v>
+        <v>128</v>
       </c>
     </row>
     <row r="82" spans="1:10">
@@ -7819,7 +7819,7 @@
         <v>233</v>
       </c>
       <c r="J82">
-        <v>157</v>
+        <v>159</v>
       </c>
     </row>
     <row r="83" spans="1:10">
@@ -7851,7 +7851,7 @@
         <v>1793</v>
       </c>
       <c r="J83">
-        <v>1019</v>
+        <v>1033</v>
       </c>
     </row>
     <row r="84" spans="1:10">
@@ -7883,7 +7883,7 @@
         <v>729</v>
       </c>
       <c r="J84">
-        <v>487</v>
+        <v>494</v>
       </c>
     </row>
     <row r="85" spans="1:10">
@@ -7915,7 +7915,7 @@
         <v>3848</v>
       </c>
       <c r="J85">
-        <v>2422</v>
+        <v>2435</v>
       </c>
     </row>
     <row r="86" spans="1:10">
@@ -7947,7 +7947,7 @@
         <v>1066</v>
       </c>
       <c r="J86">
-        <v>494</v>
+        <v>499</v>
       </c>
     </row>
     <row r="87" spans="1:10">
@@ -7979,7 +7979,7 @@
         <v>396</v>
       </c>
       <c r="J87">
-        <v>227</v>
+        <v>226</v>
       </c>
     </row>
     <row r="88" spans="1:10">
@@ -8011,7 +8011,7 @@
         <v>943</v>
       </c>
       <c r="J88">
-        <v>584</v>
+        <v>587</v>
       </c>
     </row>
     <row r="89" spans="1:10">
@@ -8043,7 +8043,7 @@
         <v>1879</v>
       </c>
       <c r="J89">
-        <v>1163</v>
+        <v>1170</v>
       </c>
     </row>
     <row r="90" spans="1:10">
@@ -8075,7 +8075,7 @@
         <v>1354</v>
       </c>
       <c r="J90">
-        <v>865</v>
+        <v>867</v>
       </c>
     </row>
     <row r="91" spans="1:10">
@@ -8107,7 +8107,7 @@
         <v>970</v>
       </c>
       <c r="J91">
-        <v>623</v>
+        <v>632</v>
       </c>
     </row>
     <row r="92" spans="1:10">
@@ -8139,7 +8139,7 @@
         <v>337</v>
       </c>
       <c r="J92">
-        <v>233</v>
+        <v>237</v>
       </c>
     </row>
     <row r="93" spans="1:10">
@@ -8171,7 +8171,7 @@
         <v>721</v>
       </c>
       <c r="J93">
-        <v>452</v>
+        <v>453</v>
       </c>
     </row>
     <row r="94" spans="1:10">
@@ -8203,7 +8203,7 @@
         <v>2663</v>
       </c>
       <c r="J94">
-        <v>1414</v>
+        <v>1429</v>
       </c>
     </row>
     <row r="95" spans="1:10">
@@ -8235,7 +8235,7 @@
         <v>1389</v>
       </c>
       <c r="J95">
-        <v>866</v>
+        <v>870</v>
       </c>
     </row>
     <row r="96" spans="1:10">
@@ -8267,7 +8267,7 @@
         <v>1669</v>
       </c>
       <c r="J96">
-        <v>943</v>
+        <v>948</v>
       </c>
     </row>
     <row r="97" spans="1:10">
@@ -8299,7 +8299,7 @@
         <v>1673</v>
       </c>
       <c r="J97">
-        <v>988</v>
+        <v>996</v>
       </c>
     </row>
     <row r="98" spans="1:10">
@@ -8331,7 +8331,7 @@
         <v>1318</v>
       </c>
       <c r="J98">
-        <v>688</v>
+        <v>691</v>
       </c>
     </row>
     <row r="99" spans="1:10">
@@ -8363,7 +8363,7 @@
         <v>1488</v>
       </c>
       <c r="J99">
-        <v>937</v>
+        <v>941</v>
       </c>
     </row>
     <row r="100" spans="1:10">
@@ -8406,7 +8406,7 @@
         <v>104362</v>
       </c>
       <c r="C101">
-        <v>116083</v>
+        <v>116084</v>
       </c>
       <c r="D101">
         <v>117356</v>
@@ -8421,13 +8421,13 @@
         <v>85314</v>
       </c>
       <c r="H101">
-        <v>84595</v>
+        <v>84597</v>
       </c>
       <c r="I101">
-        <v>110481</v>
+        <v>110482</v>
       </c>
       <c r="J101">
-        <v>66320</v>
+        <v>66720</v>
       </c>
     </row>
   </sheetData>
@@ -8795,7 +8795,7 @@
         <v>219</v>
       </c>
       <c r="J8">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="9" spans="1:10">
@@ -8859,7 +8859,7 @@
         <v>1135</v>
       </c>
       <c r="J10">
-        <v>643</v>
+        <v>649</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -8891,7 +8891,7 @@
         <v>1648</v>
       </c>
       <c r="J11">
-        <v>947</v>
+        <v>952</v>
       </c>
     </row>
   </sheetData>
@@ -8980,7 +8980,7 @@
         <v>327</v>
       </c>
       <c r="J2">
-        <v>168</v>
+        <v>169</v>
       </c>
     </row>
     <row r="3" spans="1:10">
@@ -9012,7 +9012,7 @@
         <v>439</v>
       </c>
       <c r="J3">
-        <v>250</v>
+        <v>253</v>
       </c>
     </row>
     <row r="4" spans="1:10">
@@ -9172,7 +9172,7 @@
         <v>1026</v>
       </c>
       <c r="J8">
-        <v>821</v>
+        <v>825</v>
       </c>
     </row>
     <row r="9" spans="1:10">
@@ -9236,7 +9236,7 @@
         <v>1271</v>
       </c>
       <c r="J10">
-        <v>745</v>
+        <v>750</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -9268,7 +9268,7 @@
         <v>3848</v>
       </c>
       <c r="J11">
-        <v>2422</v>
+        <v>2435</v>
       </c>
     </row>
   </sheetData>
@@ -9546,7 +9546,7 @@
         <v>336</v>
       </c>
       <c r="J8">
-        <v>179</v>
+        <v>180</v>
       </c>
     </row>
     <row r="9" spans="1:10">
@@ -9610,7 +9610,7 @@
         <v>2132</v>
       </c>
       <c r="J10">
-        <v>1228</v>
+        <v>1236</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -9642,7 +9642,7 @@
         <v>2923</v>
       </c>
       <c r="J11">
-        <v>1706</v>
+        <v>1715</v>
       </c>
     </row>
   </sheetData>
@@ -9914,7 +9914,7 @@
         <v>280</v>
       </c>
       <c r="J8">
-        <v>306</v>
+        <v>307</v>
       </c>
     </row>
     <row r="9" spans="1:10">
@@ -9946,7 +9946,7 @@
         <v>156</v>
       </c>
       <c r="J9">
-        <v>70</v>
+        <v>73</v>
       </c>
     </row>
     <row r="10" spans="1:10">
@@ -9978,7 +9978,7 @@
         <v>1034</v>
       </c>
       <c r="J10">
-        <v>491</v>
+        <v>495</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -10010,7 +10010,7 @@
         <v>1673</v>
       </c>
       <c r="J11">
-        <v>988</v>
+        <v>996</v>
       </c>
     </row>
   </sheetData>
@@ -10099,7 +10099,7 @@
         <v>235</v>
       </c>
       <c r="J2">
-        <v>139</v>
+        <v>141</v>
       </c>
     </row>
     <row r="3" spans="1:10">
@@ -10259,7 +10259,7 @@
         <v>29</v>
       </c>
       <c r="J7">
-        <v>16</v>
+        <v>17</v>
       </c>
     </row>
     <row r="8" spans="1:10">
@@ -10291,7 +10291,7 @@
         <v>516</v>
       </c>
       <c r="J8">
-        <v>399</v>
+        <v>400</v>
       </c>
     </row>
     <row r="9" spans="1:10">
@@ -10323,7 +10323,7 @@
         <v>295</v>
       </c>
       <c r="J9">
-        <v>157</v>
+        <v>158</v>
       </c>
     </row>
     <row r="10" spans="1:10">
@@ -10387,7 +10387,7 @@
         <v>2510</v>
       </c>
       <c r="J11">
-        <v>1555</v>
+        <v>1560</v>
       </c>
     </row>
   </sheetData>
@@ -10476,7 +10476,7 @@
         <v>142</v>
       </c>
       <c r="J2">
-        <v>83</v>
+        <v>84</v>
       </c>
     </row>
     <row r="3" spans="1:10">
@@ -10604,7 +10604,7 @@
         <v>17</v>
       </c>
       <c r="J6">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="7" spans="1:10">
@@ -10668,7 +10668,7 @@
         <v>392</v>
       </c>
       <c r="J8">
-        <v>303</v>
+        <v>304</v>
       </c>
     </row>
     <row r="9" spans="1:10">
@@ -10732,7 +10732,7 @@
         <v>433</v>
       </c>
       <c r="J10">
-        <v>283</v>
+        <v>284</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -10764,7 +10764,7 @@
         <v>1389</v>
       </c>
       <c r="J11">
-        <v>866</v>
+        <v>870</v>
       </c>
     </row>
   </sheetData>
@@ -10885,7 +10885,7 @@
         <v>74</v>
       </c>
       <c r="J3">
-        <v>37</v>
+        <v>39</v>
       </c>
     </row>
     <row r="4" spans="1:10">
@@ -10949,7 +10949,7 @@
         <v>39</v>
       </c>
       <c r="J5">
-        <v>24</v>
+        <v>25</v>
       </c>
     </row>
     <row r="6" spans="1:10">
@@ -11077,7 +11077,7 @@
         <v>55</v>
       </c>
       <c r="J9">
-        <v>44</v>
+        <v>45</v>
       </c>
     </row>
     <row r="10" spans="1:10">
@@ -11109,7 +11109,7 @@
         <v>271</v>
       </c>
       <c r="J10">
-        <v>146</v>
+        <v>149</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -11141,7 +11141,7 @@
         <v>729</v>
       </c>
       <c r="J11">
-        <v>487</v>
+        <v>494</v>
       </c>
     </row>
   </sheetData>
@@ -11422,7 +11422,7 @@
         <v>218</v>
       </c>
       <c r="J8">
-        <v>206</v>
+        <v>208</v>
       </c>
     </row>
     <row r="9" spans="1:10">
@@ -11486,7 +11486,7 @@
         <v>590</v>
       </c>
       <c r="J10">
-        <v>388</v>
+        <v>389</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -11518,7 +11518,7 @@
         <v>1491</v>
       </c>
       <c r="J11">
-        <v>1060</v>
+        <v>1063</v>
       </c>
     </row>
   </sheetData>
@@ -11735,7 +11735,7 @@
         <v>4</v>
       </c>
       <c r="J6">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="7" spans="1:10">
@@ -11799,7 +11799,7 @@
         <v>184</v>
       </c>
       <c r="J8">
-        <v>153</v>
+        <v>154</v>
       </c>
     </row>
     <row r="9" spans="1:10">
@@ -11831,7 +11831,7 @@
         <v>81</v>
       </c>
       <c r="J9">
-        <v>63</v>
+        <v>64</v>
       </c>
     </row>
     <row r="10" spans="1:10">
@@ -11895,7 +11895,7 @@
         <v>943</v>
       </c>
       <c r="J11">
-        <v>584</v>
+        <v>587</v>
       </c>
     </row>
   </sheetData>
@@ -11984,7 +11984,7 @@
         <v>108</v>
       </c>
       <c r="J2">
-        <v>72</v>
+        <v>74</v>
       </c>
     </row>
     <row r="3" spans="1:10">
@@ -12080,7 +12080,7 @@
         <v>69</v>
       </c>
       <c r="J5">
-        <v>39</v>
+        <v>40</v>
       </c>
     </row>
     <row r="6" spans="1:10">
@@ -12205,7 +12205,7 @@
         <v>243</v>
       </c>
       <c r="J9">
-        <v>144</v>
+        <v>145</v>
       </c>
     </row>
     <row r="10" spans="1:10">
@@ -12237,7 +12237,7 @@
         <v>2528</v>
       </c>
       <c r="J10">
-        <v>1452</v>
+        <v>1458</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -12269,7 +12269,7 @@
         <v>3506</v>
       </c>
       <c r="J11">
-        <v>2023</v>
+        <v>2033</v>
       </c>
     </row>
   </sheetData>
@@ -12454,7 +12454,7 @@
         <v>95</v>
       </c>
       <c r="J5">
-        <v>42</v>
+        <v>43</v>
       </c>
     </row>
     <row r="6" spans="1:10">
@@ -12550,7 +12550,7 @@
         <v>503</v>
       </c>
       <c r="J8">
-        <v>363</v>
+        <v>365</v>
       </c>
     </row>
     <row r="9" spans="1:10">
@@ -12582,7 +12582,7 @@
         <v>112</v>
       </c>
       <c r="J9">
-        <v>60</v>
+        <v>61</v>
       </c>
     </row>
     <row r="10" spans="1:10">
@@ -12614,7 +12614,7 @@
         <v>527</v>
       </c>
       <c r="J10">
-        <v>328</v>
+        <v>329</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -12646,7 +12646,7 @@
         <v>1491</v>
       </c>
       <c r="J11">
-        <v>945</v>
+        <v>950</v>
       </c>
     </row>
   </sheetData>
@@ -12735,7 +12735,7 @@
         <v>239</v>
       </c>
       <c r="J2">
-        <v>141</v>
+        <v>142</v>
       </c>
     </row>
     <row r="3" spans="1:10">
@@ -12831,7 +12831,7 @@
         <v>200</v>
       </c>
       <c r="J5">
-        <v>136</v>
+        <v>137</v>
       </c>
     </row>
     <row r="6" spans="1:10">
@@ -12927,7 +12927,7 @@
         <v>722</v>
       </c>
       <c r="J8">
-        <v>502</v>
+        <v>503</v>
       </c>
     </row>
     <row r="9" spans="1:10">
@@ -12959,7 +12959,7 @@
         <v>244</v>
       </c>
       <c r="J9">
-        <v>140</v>
+        <v>141</v>
       </c>
     </row>
     <row r="10" spans="1:10">
@@ -12991,7 +12991,7 @@
         <v>813</v>
       </c>
       <c r="J10">
-        <v>480</v>
+        <v>483</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -13023,7 +13023,7 @@
         <v>2547</v>
       </c>
       <c r="J11">
-        <v>1603</v>
+        <v>1610</v>
       </c>
     </row>
   </sheetData>
@@ -13112,7 +13112,7 @@
         <v>30</v>
       </c>
       <c r="J2">
-        <v>21</v>
+        <v>22</v>
       </c>
     </row>
     <row r="3" spans="1:10">
@@ -13283,7 +13283,7 @@
         <v>90</v>
       </c>
       <c r="J8">
-        <v>99</v>
+        <v>100</v>
       </c>
     </row>
     <row r="9" spans="1:10">
@@ -13347,7 +13347,7 @@
         <v>213</v>
       </c>
       <c r="J10">
-        <v>138</v>
+        <v>139</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -13379,7 +13379,7 @@
         <v>418</v>
       </c>
       <c r="J11">
-        <v>305</v>
+        <v>308</v>
       </c>
     </row>
   </sheetData>
@@ -13709,7 +13709,7 @@
         <v>448</v>
       </c>
       <c r="J10">
-        <v>229</v>
+        <v>230</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -13741,7 +13741,7 @@
         <v>706</v>
       </c>
       <c r="J11">
-        <v>391</v>
+        <v>392</v>
       </c>
     </row>
   </sheetData>
@@ -14022,7 +14022,7 @@
         <v>202</v>
       </c>
       <c r="J8">
-        <v>218</v>
+        <v>219</v>
       </c>
     </row>
     <row r="9" spans="1:10">
@@ -14054,7 +14054,7 @@
         <v>189</v>
       </c>
       <c r="J9">
-        <v>134</v>
+        <v>136</v>
       </c>
     </row>
     <row r="10" spans="1:10">
@@ -14086,7 +14086,7 @@
         <v>587</v>
       </c>
       <c r="J10">
-        <v>345</v>
+        <v>346</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -14118,7 +14118,7 @@
         <v>1515</v>
       </c>
       <c r="J11">
-        <v>1020</v>
+        <v>1024</v>
       </c>
     </row>
   </sheetData>
@@ -14424,7 +14424,7 @@
         <v>100</v>
       </c>
       <c r="J10">
-        <v>52</v>
+        <v>53</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -14456,7 +14456,7 @@
         <v>209</v>
       </c>
       <c r="J11">
-        <v>158</v>
+        <v>159</v>
       </c>
     </row>
   </sheetData>
@@ -14798,7 +14798,7 @@
         <v>379</v>
       </c>
       <c r="J10">
-        <v>197</v>
+        <v>198</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -14830,7 +14830,7 @@
         <v>768</v>
       </c>
       <c r="J11">
-        <v>480</v>
+        <v>481</v>
       </c>
     </row>
   </sheetData>
@@ -15009,7 +15009,7 @@
         <v>38</v>
       </c>
       <c r="J5">
-        <v>29</v>
+        <v>30</v>
       </c>
     </row>
     <row r="6" spans="1:10">
@@ -15192,7 +15192,7 @@
         <v>437</v>
       </c>
       <c r="J11">
-        <v>204</v>
+        <v>205</v>
       </c>
     </row>
   </sheetData>
@@ -15281,7 +15281,7 @@
         <v>190</v>
       </c>
       <c r="J2">
-        <v>100</v>
+        <v>101</v>
       </c>
     </row>
     <row r="3" spans="1:10">
@@ -15313,7 +15313,7 @@
         <v>205</v>
       </c>
       <c r="J3">
-        <v>123</v>
+        <v>125</v>
       </c>
     </row>
     <row r="4" spans="1:10">
@@ -15473,7 +15473,7 @@
         <v>484</v>
       </c>
       <c r="J8">
-        <v>287</v>
+        <v>293</v>
       </c>
     </row>
     <row r="9" spans="1:10">
@@ -15505,7 +15505,7 @@
         <v>123</v>
       </c>
       <c r="J9">
-        <v>92</v>
+        <v>93</v>
       </c>
     </row>
     <row r="10" spans="1:10">
@@ -15537,7 +15537,7 @@
         <v>612</v>
       </c>
       <c r="J10">
-        <v>336</v>
+        <v>340</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -15569,7 +15569,7 @@
         <v>1793</v>
       </c>
       <c r="J11">
-        <v>1019</v>
+        <v>1033</v>
       </c>
     </row>
   </sheetData>
@@ -15754,7 +15754,7 @@
         <v>90</v>
       </c>
       <c r="J5">
-        <v>45</v>
+        <v>46</v>
       </c>
     </row>
     <row r="6" spans="1:10">
@@ -15850,7 +15850,7 @@
         <v>224</v>
       </c>
       <c r="J8">
-        <v>175</v>
+        <v>176</v>
       </c>
     </row>
     <row r="9" spans="1:10">
@@ -15914,7 +15914,7 @@
         <v>610</v>
       </c>
       <c r="J10">
-        <v>298</v>
+        <v>300</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -15946,7 +15946,7 @@
         <v>1244</v>
       </c>
       <c r="J11">
-        <v>706</v>
+        <v>710</v>
       </c>
     </row>
   </sheetData>
@@ -16067,7 +16067,7 @@
         <v>42</v>
       </c>
       <c r="J3">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="4" spans="1:10">
@@ -16212,7 +16212,7 @@
         <v>294</v>
       </c>
       <c r="J8">
-        <v>220</v>
+        <v>221</v>
       </c>
     </row>
     <row r="9" spans="1:10">
@@ -16244,7 +16244,7 @@
         <v>147</v>
       </c>
       <c r="J9">
-        <v>72</v>
+        <v>74</v>
       </c>
     </row>
     <row r="10" spans="1:10">
@@ -16276,7 +16276,7 @@
         <v>2021</v>
       </c>
       <c r="J10">
-        <v>1003</v>
+        <v>1014</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -16308,7 +16308,7 @@
         <v>2663</v>
       </c>
       <c r="J11">
-        <v>1414</v>
+        <v>1429</v>
       </c>
     </row>
   </sheetData>
@@ -16397,7 +16397,7 @@
         <v>267</v>
       </c>
       <c r="J2">
-        <v>176</v>
+        <v>177</v>
       </c>
     </row>
     <row r="3" spans="1:10">
@@ -16429,7 +16429,7 @@
         <v>416</v>
       </c>
       <c r="J3">
-        <v>227</v>
+        <v>228</v>
       </c>
     </row>
     <row r="4" spans="1:10">
@@ -16589,7 +16589,7 @@
         <v>707</v>
       </c>
       <c r="J8">
-        <v>573</v>
+        <v>575</v>
       </c>
     </row>
     <row r="9" spans="1:10">
@@ -16621,7 +16621,7 @@
         <v>363</v>
       </c>
       <c r="J9">
-        <v>222</v>
+        <v>227</v>
       </c>
     </row>
     <row r="10" spans="1:10">
@@ -16653,7 +16653,7 @@
         <v>968</v>
       </c>
       <c r="J10">
-        <v>551</v>
+        <v>557</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -16685,7 +16685,7 @@
         <v>3011</v>
       </c>
       <c r="J11">
-        <v>1892</v>
+        <v>1907</v>
       </c>
     </row>
   </sheetData>
@@ -16774,7 +16774,7 @@
         <v>264</v>
       </c>
       <c r="J2">
-        <v>145</v>
+        <v>147</v>
       </c>
     </row>
     <row r="3" spans="1:10">
@@ -16870,7 +16870,7 @@
         <v>261</v>
       </c>
       <c r="J5">
-        <v>141</v>
+        <v>142</v>
       </c>
     </row>
     <row r="6" spans="1:10">
@@ -16966,7 +16966,7 @@
         <v>567</v>
       </c>
       <c r="J8">
-        <v>565</v>
+        <v>567</v>
       </c>
     </row>
     <row r="9" spans="1:10">
@@ -16998,7 +16998,7 @@
         <v>226</v>
       </c>
       <c r="J9">
-        <v>147</v>
+        <v>148</v>
       </c>
     </row>
     <row r="10" spans="1:10">
@@ -17030,7 +17030,7 @@
         <v>1023</v>
       </c>
       <c r="J10">
-        <v>512</v>
+        <v>513</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -17062,7 +17062,7 @@
         <v>2686</v>
       </c>
       <c r="J11">
-        <v>1671</v>
+        <v>1678</v>
       </c>
     </row>
   </sheetData>
@@ -17151,7 +17151,7 @@
         <v>457</v>
       </c>
       <c r="J2">
-        <v>282</v>
+        <v>284</v>
       </c>
     </row>
     <row r="3" spans="1:10">
@@ -17247,7 +17247,7 @@
         <v>251</v>
       </c>
       <c r="J5">
-        <v>121</v>
+        <v>122</v>
       </c>
     </row>
     <row r="6" spans="1:10">
@@ -17343,7 +17343,7 @@
         <v>1269</v>
       </c>
       <c r="J8">
-        <v>766</v>
+        <v>770</v>
       </c>
     </row>
     <row r="9" spans="1:10">
@@ -17375,7 +17375,7 @@
         <v>497</v>
       </c>
       <c r="J9">
-        <v>316</v>
+        <v>320</v>
       </c>
     </row>
     <row r="10" spans="1:10">
@@ -17407,7 +17407,7 @@
         <v>1652</v>
       </c>
       <c r="J10">
-        <v>915</v>
+        <v>922</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -17439,7 +17439,7 @@
         <v>4743</v>
       </c>
       <c r="J11">
-        <v>2812</v>
+        <v>2830</v>
       </c>
     </row>
   </sheetData>
@@ -17720,7 +17720,7 @@
         <v>441</v>
       </c>
       <c r="J8">
-        <v>338</v>
+        <v>339</v>
       </c>
     </row>
     <row r="9" spans="1:10">
@@ -17784,7 +17784,7 @@
         <v>455</v>
       </c>
       <c r="J10">
-        <v>302</v>
+        <v>303</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -17816,7 +17816,7 @@
         <v>1354</v>
       </c>
       <c r="J11">
-        <v>865</v>
+        <v>867</v>
       </c>
     </row>
   </sheetData>
@@ -18088,7 +18088,7 @@
         <v>250</v>
       </c>
       <c r="J8">
-        <v>181</v>
+        <v>185</v>
       </c>
     </row>
     <row r="9" spans="1:10">
@@ -18120,7 +18120,7 @@
         <v>61</v>
       </c>
       <c r="J9">
-        <v>43</v>
+        <v>44</v>
       </c>
     </row>
     <row r="10" spans="1:10">
@@ -18152,7 +18152,7 @@
         <v>417</v>
       </c>
       <c r="J10">
-        <v>241</v>
+        <v>243</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -18184,7 +18184,7 @@
         <v>903</v>
       </c>
       <c r="J11">
-        <v>559</v>
+        <v>566</v>
       </c>
     </row>
   </sheetData>
@@ -18273,7 +18273,7 @@
         <v>237</v>
       </c>
       <c r="J2">
-        <v>111</v>
+        <v>113</v>
       </c>
     </row>
     <row r="3" spans="1:10">
@@ -18305,7 +18305,7 @@
         <v>212</v>
       </c>
       <c r="J3">
-        <v>126</v>
+        <v>128</v>
       </c>
     </row>
     <row r="4" spans="1:10">
@@ -18369,7 +18369,7 @@
         <v>229</v>
       </c>
       <c r="J5">
-        <v>108</v>
+        <v>109</v>
       </c>
     </row>
     <row r="6" spans="1:10">
@@ -18401,7 +18401,7 @@
         <v>27</v>
       </c>
       <c r="J6">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="7" spans="1:10">
@@ -18465,7 +18465,7 @@
         <v>754</v>
       </c>
       <c r="J8">
-        <v>432</v>
+        <v>435</v>
       </c>
     </row>
     <row r="9" spans="1:10">
@@ -18497,7 +18497,7 @@
         <v>233</v>
       </c>
       <c r="J9">
-        <v>163</v>
+        <v>166</v>
       </c>
     </row>
     <row r="10" spans="1:10">
@@ -18529,7 +18529,7 @@
         <v>911</v>
       </c>
       <c r="J10">
-        <v>547</v>
+        <v>550</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -18561,7 +18561,7 @@
         <v>2636</v>
       </c>
       <c r="J11">
-        <v>1539</v>
+        <v>1554</v>
       </c>
     </row>
   </sheetData>
@@ -18650,7 +18650,7 @@
         <v>22</v>
       </c>
       <c r="J2">
-        <v>15</v>
+        <v>16</v>
       </c>
     </row>
     <row r="3" spans="1:10">
@@ -18911,7 +18911,7 @@
         <v>247</v>
       </c>
       <c r="J11">
-        <v>171</v>
+        <v>172</v>
       </c>
     </row>
   </sheetData>
@@ -19032,7 +19032,7 @@
         <v>177</v>
       </c>
       <c r="J3">
-        <v>101</v>
+        <v>103</v>
       </c>
     </row>
     <row r="4" spans="1:10">
@@ -19192,7 +19192,7 @@
         <v>363</v>
       </c>
       <c r="J8">
-        <v>282</v>
+        <v>284</v>
       </c>
     </row>
     <row r="9" spans="1:10">
@@ -19256,7 +19256,7 @@
         <v>828</v>
       </c>
       <c r="J10">
-        <v>437</v>
+        <v>438</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -19288,7 +19288,7 @@
         <v>2045</v>
       </c>
       <c r="J11">
-        <v>1111</v>
+        <v>1116</v>
       </c>
     </row>
   </sheetData>
@@ -19499,7 +19499,7 @@
         <v>23</v>
       </c>
       <c r="J6">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="7" spans="1:10">
@@ -19589,7 +19589,7 @@
         <v>45</v>
       </c>
       <c r="J9">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="10" spans="1:10">
@@ -19621,7 +19621,7 @@
         <v>630</v>
       </c>
       <c r="J10">
-        <v>311</v>
+        <v>313</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -19653,7 +19653,7 @@
         <v>960</v>
       </c>
       <c r="J11">
-        <v>561</v>
+        <v>565</v>
       </c>
     </row>
   </sheetData>
@@ -19832,7 +19832,7 @@
         <v>31</v>
       </c>
       <c r="J5">
-        <v>9</v>
+        <v>12</v>
       </c>
     </row>
     <row r="6" spans="1:10">
@@ -20015,7 +20015,7 @@
         <v>271</v>
       </c>
       <c r="J11">
-        <v>182</v>
+        <v>185</v>
       </c>
     </row>
   </sheetData>
@@ -20104,7 +20104,7 @@
         <v>87</v>
       </c>
       <c r="J2">
-        <v>54</v>
+        <v>55</v>
       </c>
     </row>
     <row r="3" spans="1:10">
@@ -20136,7 +20136,7 @@
         <v>98</v>
       </c>
       <c r="J3">
-        <v>73</v>
+        <v>74</v>
       </c>
     </row>
     <row r="4" spans="1:10">
@@ -20168,7 +20168,7 @@
         <v>3</v>
       </c>
       <c r="J4">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="5" spans="1:10">
@@ -20296,7 +20296,7 @@
         <v>308</v>
       </c>
       <c r="J8">
-        <v>228</v>
+        <v>231</v>
       </c>
     </row>
     <row r="9" spans="1:10">
@@ -20360,7 +20360,7 @@
         <v>320</v>
       </c>
       <c r="J10">
-        <v>187</v>
+        <v>190</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -20392,7 +20392,7 @@
         <v>970</v>
       </c>
       <c r="J11">
-        <v>623</v>
+        <v>632</v>
       </c>
     </row>
   </sheetData>
@@ -20667,7 +20667,7 @@
         <v>122</v>
       </c>
       <c r="J8">
-        <v>132</v>
+        <v>133</v>
       </c>
     </row>
     <row r="9" spans="1:10">
@@ -20763,7 +20763,7 @@
         <v>721</v>
       </c>
       <c r="J11">
-        <v>452</v>
+        <v>453</v>
       </c>
     </row>
   </sheetData>
@@ -21055,7 +21055,7 @@
         <v>18</v>
       </c>
       <c r="J9">
-        <v>20</v>
+        <v>21</v>
       </c>
     </row>
     <row r="10" spans="1:10">
@@ -21087,7 +21087,7 @@
         <v>280</v>
       </c>
       <c r="J10">
-        <v>143</v>
+        <v>144</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -21119,7 +21119,7 @@
         <v>436</v>
       </c>
       <c r="J11">
-        <v>278</v>
+        <v>280</v>
       </c>
     </row>
   </sheetData>
@@ -21765,7 +21765,7 @@
         <v>297</v>
       </c>
       <c r="J8">
-        <v>286</v>
+        <v>289</v>
       </c>
     </row>
     <row r="9" spans="1:10">
@@ -21797,7 +21797,7 @@
         <v>121</v>
       </c>
       <c r="J9">
-        <v>68</v>
+        <v>70</v>
       </c>
     </row>
     <row r="10" spans="1:10">
@@ -21829,7 +21829,7 @@
         <v>670</v>
       </c>
       <c r="J10">
-        <v>360</v>
+        <v>361</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -21861,7 +21861,7 @@
         <v>1337</v>
       </c>
       <c r="J11">
-        <v>886</v>
+        <v>892</v>
       </c>
     </row>
   </sheetData>
@@ -21950,7 +21950,7 @@
         <v>80</v>
       </c>
       <c r="J2">
-        <v>32</v>
+        <v>33</v>
       </c>
     </row>
     <row r="3" spans="1:10">
@@ -21982,7 +21982,7 @@
         <v>64</v>
       </c>
       <c r="J3">
-        <v>30</v>
+        <v>31</v>
       </c>
     </row>
     <row r="4" spans="1:10">
@@ -22142,7 +22142,7 @@
         <v>125</v>
       </c>
       <c r="J8">
-        <v>83</v>
+        <v>85</v>
       </c>
     </row>
     <row r="9" spans="1:10">
@@ -22206,7 +22206,7 @@
         <v>492</v>
       </c>
       <c r="J10">
-        <v>325</v>
+        <v>328</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -22238,7 +22238,7 @@
         <v>917</v>
       </c>
       <c r="J11">
-        <v>572</v>
+        <v>579</v>
       </c>
     </row>
   </sheetData>
@@ -22492,7 +22492,7 @@
         <v>89</v>
       </c>
       <c r="J8">
-        <v>63</v>
+        <v>65</v>
       </c>
     </row>
     <row r="9" spans="1:10">
@@ -22588,7 +22588,7 @@
         <v>412</v>
       </c>
       <c r="J11">
-        <v>233</v>
+        <v>235</v>
       </c>
     </row>
   </sheetData>
@@ -22677,7 +22677,7 @@
         <v>54</v>
       </c>
       <c r="J2">
-        <v>38</v>
+        <v>39</v>
       </c>
     </row>
     <row r="3" spans="1:10">
@@ -22962,7 +22962,7 @@
         <v>695</v>
       </c>
       <c r="J11">
-        <v>439</v>
+        <v>440</v>
       </c>
     </row>
   </sheetData>
@@ -23295,7 +23295,7 @@
         <v>277</v>
       </c>
       <c r="J10">
-        <v>180</v>
+        <v>182</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -23327,7 +23327,7 @@
         <v>500</v>
       </c>
       <c r="J11">
-        <v>352</v>
+        <v>354</v>
       </c>
     </row>
   </sheetData>
@@ -23416,7 +23416,7 @@
         <v>50</v>
       </c>
       <c r="J2">
-        <v>36</v>
+        <v>37</v>
       </c>
     </row>
     <row r="3" spans="1:10">
@@ -23669,7 +23669,7 @@
         <v>189</v>
       </c>
       <c r="J10">
-        <v>137</v>
+        <v>140</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -23701,7 +23701,7 @@
         <v>429</v>
       </c>
       <c r="J11">
-        <v>280</v>
+        <v>284</v>
       </c>
     </row>
   </sheetData>
@@ -23883,7 +23883,7 @@
         <v>77</v>
       </c>
       <c r="J5">
-        <v>36</v>
+        <v>37</v>
       </c>
     </row>
     <row r="6" spans="1:10">
@@ -23979,7 +23979,7 @@
         <v>178</v>
       </c>
       <c r="J8">
-        <v>193</v>
+        <v>194</v>
       </c>
     </row>
     <row r="9" spans="1:10">
@@ -24075,7 +24075,7 @@
         <v>793</v>
       </c>
       <c r="J11">
-        <v>572</v>
+        <v>574</v>
       </c>
     </row>
   </sheetData>
@@ -24344,7 +24344,7 @@
         <v>70</v>
       </c>
       <c r="J8">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="9" spans="1:10">
@@ -24440,7 +24440,7 @@
         <v>396</v>
       </c>
       <c r="J11">
-        <v>227</v>
+        <v>226</v>
       </c>
     </row>
   </sheetData>
@@ -24709,7 +24709,7 @@
         <v>167</v>
       </c>
       <c r="J8">
-        <v>123</v>
+        <v>122</v>
       </c>
     </row>
     <row r="9" spans="1:10">
@@ -24741,7 +24741,7 @@
         <v>88</v>
       </c>
       <c r="J9">
-        <v>32</v>
+        <v>33</v>
       </c>
     </row>
     <row r="10" spans="1:10">
@@ -24773,7 +24773,7 @@
         <v>784</v>
       </c>
       <c r="J10">
-        <v>498</v>
+        <v>499</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -24805,7 +24805,7 @@
         <v>1258</v>
       </c>
       <c r="J11">
-        <v>779</v>
+        <v>780</v>
       </c>
     </row>
   </sheetData>
@@ -24891,7 +24891,7 @@
         <v>61</v>
       </c>
       <c r="I2">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="J2">
         <v>43</v>
@@ -25086,7 +25086,7 @@
         <v>151</v>
       </c>
       <c r="J8">
-        <v>115</v>
+        <v>116</v>
       </c>
     </row>
     <row r="9" spans="1:10">
@@ -25150,7 +25150,7 @@
         <v>381</v>
       </c>
       <c r="J10">
-        <v>208</v>
+        <v>210</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -25179,10 +25179,10 @@
         <v>613</v>
       </c>
       <c r="I11">
-        <v>867</v>
+        <v>868</v>
       </c>
       <c r="J11">
-        <v>491</v>
+        <v>494</v>
       </c>
     </row>
   </sheetData>
@@ -25632,7 +25632,7 @@
         <v>53</v>
       </c>
       <c r="J3">
-        <v>40</v>
+        <v>41</v>
       </c>
     </row>
     <row r="4" spans="1:10">
@@ -25888,7 +25888,7 @@
         <v>462</v>
       </c>
       <c r="J11">
-        <v>308</v>
+        <v>309</v>
       </c>
     </row>
   </sheetData>
@@ -26119,7 +26119,7 @@
         <v>28</v>
       </c>
       <c r="J7">
-        <v>32</v>
+        <v>33</v>
       </c>
     </row>
     <row r="8" spans="1:10">
@@ -26183,7 +26183,7 @@
         <v>139</v>
       </c>
       <c r="J9">
-        <v>83</v>
+        <v>84</v>
       </c>
     </row>
     <row r="10" spans="1:10">
@@ -26215,7 +26215,7 @@
         <v>233</v>
       </c>
       <c r="J10">
-        <v>157</v>
+        <v>159</v>
       </c>
     </row>
   </sheetData>
@@ -26560,7 +26560,7 @@
         <v>1118</v>
       </c>
       <c r="J10">
-        <v>604</v>
+        <v>606</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -26592,7 +26592,7 @@
         <v>1797</v>
       </c>
       <c r="J11">
-        <v>1027</v>
+        <v>1029</v>
       </c>
     </row>
   </sheetData>
@@ -26806,7 +26806,7 @@
         <v>7</v>
       </c>
       <c r="J6">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="7" spans="1:10">
@@ -26864,7 +26864,7 @@
         <v>109</v>
       </c>
       <c r="J8">
-        <v>87</v>
+        <v>88</v>
       </c>
     </row>
     <row r="9" spans="1:10">
@@ -26896,7 +26896,7 @@
         <v>50</v>
       </c>
       <c r="J9">
-        <v>15</v>
+        <v>16</v>
       </c>
     </row>
     <row r="10" spans="1:10">
@@ -26928,7 +26928,7 @@
         <v>371</v>
       </c>
       <c r="J10">
-        <v>161</v>
+        <v>162</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -26960,7 +26960,7 @@
         <v>718</v>
       </c>
       <c r="J11">
-        <v>356</v>
+        <v>360</v>
       </c>
     </row>
   </sheetData>
@@ -27211,7 +27211,7 @@
         <v>99</v>
       </c>
       <c r="J8">
-        <v>81</v>
+        <v>82</v>
       </c>
     </row>
     <row r="9" spans="1:10">
@@ -27307,7 +27307,7 @@
         <v>715</v>
       </c>
       <c r="J11">
-        <v>438</v>
+        <v>439</v>
       </c>
     </row>
   </sheetData>
@@ -27508,6 +27508,9 @@
       <c r="I6">
         <v>3</v>
       </c>
+      <c r="J6">
+        <v>1</v>
+      </c>
     </row>
     <row r="7" spans="1:10">
       <c r="A7" s="1" t="s">
@@ -27619,7 +27622,7 @@
         <v>376</v>
       </c>
       <c r="J10">
-        <v>267</v>
+        <v>268</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -27651,7 +27654,7 @@
         <v>595</v>
       </c>
       <c r="J11">
-        <v>432</v>
+        <v>434</v>
       </c>
     </row>
   </sheetData>
@@ -27836,7 +27839,7 @@
         <v>48</v>
       </c>
       <c r="J5">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="6" spans="1:10">
@@ -27932,7 +27935,7 @@
         <v>141</v>
       </c>
       <c r="J8">
-        <v>111</v>
+        <v>113</v>
       </c>
     </row>
     <row r="9" spans="1:10">
@@ -27996,7 +27999,7 @@
         <v>193</v>
       </c>
       <c r="J10">
-        <v>91</v>
+        <v>93</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -28028,7 +28031,7 @@
         <v>519</v>
       </c>
       <c r="J11">
-        <v>311</v>
+        <v>316</v>
       </c>
     </row>
   </sheetData>
@@ -28688,7 +28691,7 @@
         <v>90</v>
       </c>
       <c r="J9">
-        <v>43</v>
+        <v>45</v>
       </c>
     </row>
     <row r="10" spans="1:10">
@@ -28720,7 +28723,7 @@
         <v>542</v>
       </c>
       <c r="J10">
-        <v>300</v>
+        <v>303</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -28752,7 +28755,7 @@
         <v>948</v>
       </c>
       <c r="J11">
-        <v>536</v>
+        <v>541</v>
       </c>
     </row>
   </sheetData>
@@ -29212,7 +29215,7 @@
         <v>77</v>
       </c>
       <c r="J2">
-        <v>65</v>
+        <v>68</v>
       </c>
     </row>
     <row r="3" spans="1:10">
@@ -29244,7 +29247,7 @@
         <v>71</v>
       </c>
       <c r="J3">
-        <v>49</v>
+        <v>50</v>
       </c>
     </row>
     <row r="4" spans="1:10">
@@ -29308,7 +29311,7 @@
         <v>131</v>
       </c>
       <c r="J5">
-        <v>80</v>
+        <v>81</v>
       </c>
     </row>
     <row r="6" spans="1:10">
@@ -29401,7 +29404,7 @@
         <v>216</v>
       </c>
       <c r="J8">
-        <v>197</v>
+        <v>198</v>
       </c>
     </row>
     <row r="9" spans="1:10">
@@ -29465,7 +29468,7 @@
         <v>1222</v>
       </c>
       <c r="J10">
-        <v>684</v>
+        <v>685</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -29497,7 +29500,7 @@
         <v>1879</v>
       </c>
       <c r="J11">
-        <v>1163</v>
+        <v>1170</v>
       </c>
     </row>
   </sheetData>
@@ -29839,7 +29842,7 @@
         <v>440</v>
       </c>
       <c r="J10">
-        <v>264</v>
+        <v>265</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -29871,7 +29874,7 @@
         <v>761</v>
       </c>
       <c r="J11">
-        <v>501</v>
+        <v>502</v>
       </c>
     </row>
   </sheetData>
@@ -29992,7 +29995,7 @@
         <v>158</v>
       </c>
       <c r="J3">
-        <v>84</v>
+        <v>85</v>
       </c>
     </row>
     <row r="4" spans="1:10">
@@ -30152,7 +30155,7 @@
         <v>383</v>
       </c>
       <c r="J8">
-        <v>303</v>
+        <v>305</v>
       </c>
     </row>
     <row r="9" spans="1:10">
@@ -30216,7 +30219,7 @@
         <v>527</v>
       </c>
       <c r="J10">
-        <v>325</v>
+        <v>326</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -30248,7 +30251,7 @@
         <v>1488</v>
       </c>
       <c r="J11">
-        <v>937</v>
+        <v>941</v>
       </c>
     </row>
   </sheetData>
@@ -30487,7 +30490,7 @@
         <v>27</v>
       </c>
       <c r="J8">
-        <v>44</v>
+        <v>45</v>
       </c>
     </row>
     <row r="9" spans="1:10">
@@ -30551,7 +30554,7 @@
         <v>152</v>
       </c>
       <c r="J10">
-        <v>80</v>
+        <v>81</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -30583,7 +30586,7 @@
         <v>248</v>
       </c>
       <c r="J11">
-        <v>171</v>
+        <v>173</v>
       </c>
     </row>
   </sheetData>
@@ -30828,7 +30831,7 @@
         <v>112</v>
       </c>
       <c r="J8">
-        <v>76</v>
+        <v>77</v>
       </c>
     </row>
     <row r="9" spans="1:10">
@@ -30892,7 +30895,7 @@
         <v>502</v>
       </c>
       <c r="J10">
-        <v>312</v>
+        <v>314</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -30924,7 +30927,7 @@
         <v>677</v>
       </c>
       <c r="J11">
-        <v>417</v>
+        <v>420</v>
       </c>
     </row>
   </sheetData>
@@ -31589,7 +31592,7 @@
         <v>124</v>
       </c>
       <c r="J10">
-        <v>76</v>
+        <v>77</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -31621,7 +31624,7 @@
         <v>335</v>
       </c>
       <c r="J11">
-        <v>259</v>
+        <v>260</v>
       </c>
     </row>
   </sheetData>
@@ -31934,7 +31937,7 @@
         <v>113</v>
       </c>
       <c r="J9">
-        <v>69</v>
+        <v>71</v>
       </c>
     </row>
     <row r="10" spans="1:10">
@@ -31966,7 +31969,7 @@
         <v>389</v>
       </c>
       <c r="J10">
-        <v>256</v>
+        <v>257</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -31998,7 +32001,7 @@
         <v>886</v>
       </c>
       <c r="J11">
-        <v>589</v>
+        <v>592</v>
       </c>
     </row>
   </sheetData>
@@ -32119,7 +32122,7 @@
         <v>89</v>
       </c>
       <c r="J3">
-        <v>46</v>
+        <v>47</v>
       </c>
     </row>
     <row r="4" spans="1:10">
@@ -32273,7 +32276,7 @@
         <v>405</v>
       </c>
       <c r="J8">
-        <v>353</v>
+        <v>354</v>
       </c>
     </row>
     <row r="9" spans="1:10">
@@ -32337,7 +32340,7 @@
         <v>670</v>
       </c>
       <c r="J10">
-        <v>321</v>
+        <v>323</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -32369,7 +32372,7 @@
         <v>1368</v>
       </c>
       <c r="J11">
-        <v>840</v>
+        <v>844</v>
       </c>
     </row>
   </sheetData>
@@ -32586,7 +32589,7 @@
         <v>42</v>
       </c>
       <c r="J6">
-        <v>28</v>
+        <v>29</v>
       </c>
     </row>
     <row r="7" spans="1:10">
@@ -32708,7 +32711,7 @@
         <v>1773</v>
       </c>
       <c r="J10">
-        <v>1033</v>
+        <v>1040</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -32740,7 +32743,7 @@
         <v>2622</v>
       </c>
       <c r="J11">
-        <v>1545</v>
+        <v>1553</v>
       </c>
     </row>
   </sheetData>
@@ -33006,7 +33009,7 @@
         <v>90</v>
       </c>
       <c r="J8">
-        <v>64</v>
+        <v>65</v>
       </c>
     </row>
     <row r="9" spans="1:10">
@@ -33102,7 +33105,7 @@
         <v>340</v>
       </c>
       <c r="J11">
-        <v>204</v>
+        <v>205</v>
       </c>
     </row>
   </sheetData>
@@ -33269,7 +33272,7 @@
         <v>11</v>
       </c>
       <c r="J5">
-        <v>12</v>
+        <v>13</v>
       </c>
     </row>
     <row r="6" spans="1:10">
@@ -33376,7 +33379,7 @@
         <v>87</v>
       </c>
       <c r="J9">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="10" spans="1:10">
@@ -33408,7 +33411,7 @@
         <v>174</v>
       </c>
       <c r="J10">
-        <v>78</v>
+        <v>79</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -33440,7 +33443,7 @@
         <v>337</v>
       </c>
       <c r="J11">
-        <v>155</v>
+        <v>158</v>
       </c>
     </row>
   </sheetData>
@@ -33712,7 +33715,7 @@
         <v>334</v>
       </c>
       <c r="J8">
-        <v>195</v>
+        <v>196</v>
       </c>
     </row>
     <row r="9" spans="1:10">
@@ -33808,7 +33811,7 @@
         <v>1187</v>
       </c>
       <c r="J11">
-        <v>640</v>
+        <v>641</v>
       </c>
     </row>
   </sheetData>
@@ -34083,7 +34086,7 @@
         <v>116</v>
       </c>
       <c r="J8">
-        <v>41</v>
+        <v>42</v>
       </c>
     </row>
     <row r="9" spans="1:10">
@@ -34115,7 +34118,7 @@
         <v>153</v>
       </c>
       <c r="J9">
-        <v>57</v>
+        <v>58</v>
       </c>
     </row>
   </sheetData>
@@ -34375,7 +34378,7 @@
         <v>50</v>
       </c>
       <c r="J8">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="9" spans="1:10">
@@ -34439,7 +34442,7 @@
         <v>313</v>
       </c>
       <c r="J10">
-        <v>153</v>
+        <v>157</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -34471,7 +34474,7 @@
         <v>494</v>
       </c>
       <c r="J11">
-        <v>255</v>
+        <v>260</v>
       </c>
     </row>
   </sheetData>
@@ -34745,7 +34748,7 @@
         <v>107</v>
       </c>
       <c r="J9">
-        <v>77</v>
+        <v>80</v>
       </c>
     </row>
     <row r="10" spans="1:10">
@@ -34777,7 +34780,7 @@
         <v>155</v>
       </c>
       <c r="J10">
-        <v>103</v>
+        <v>106</v>
       </c>
     </row>
   </sheetData>
@@ -35110,7 +35113,7 @@
         <v>211</v>
       </c>
       <c r="J10">
-        <v>146</v>
+        <v>147</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -35142,7 +35145,7 @@
         <v>406</v>
       </c>
       <c r="J11">
-        <v>289</v>
+        <v>290</v>
       </c>
     </row>
   </sheetData>
@@ -35761,7 +35764,7 @@
         <v>187</v>
       </c>
       <c r="J9">
-        <v>118</v>
+        <v>120</v>
       </c>
     </row>
     <row r="10" spans="1:10">
@@ -35793,7 +35796,7 @@
         <v>258</v>
       </c>
       <c r="J10">
-        <v>154</v>
+        <v>156</v>
       </c>
     </row>
   </sheetData>
@@ -36029,7 +36032,7 @@
         <v>12</v>
       </c>
       <c r="J8">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="9" spans="1:10">
@@ -36125,7 +36128,7 @@
         <v>99</v>
       </c>
       <c r="J11">
-        <v>36</v>
+        <v>37</v>
       </c>
     </row>
   </sheetData>
@@ -36310,7 +36313,7 @@
         <v>161</v>
       </c>
       <c r="J5">
-        <v>92</v>
+        <v>93</v>
       </c>
     </row>
     <row r="6" spans="1:10">
@@ -36406,7 +36409,7 @@
         <v>291</v>
       </c>
       <c r="J8">
-        <v>196</v>
+        <v>197</v>
       </c>
     </row>
     <row r="9" spans="1:10">
@@ -36470,7 +36473,7 @@
         <v>905</v>
       </c>
       <c r="J10">
-        <v>471</v>
+        <v>474</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -36502,7 +36505,7 @@
         <v>1669</v>
       </c>
       <c r="J11">
-        <v>943</v>
+        <v>948</v>
       </c>
     </row>
   </sheetData>
@@ -36777,7 +36780,7 @@
         <v>68</v>
       </c>
       <c r="J8">
-        <v>66</v>
+        <v>67</v>
       </c>
     </row>
     <row r="9" spans="1:10">
@@ -36841,7 +36844,7 @@
         <v>157</v>
       </c>
       <c r="J10">
-        <v>95</v>
+        <v>98</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -36873,7 +36876,7 @@
         <v>337</v>
       </c>
       <c r="J11">
-        <v>233</v>
+        <v>237</v>
       </c>
     </row>
   </sheetData>
@@ -37329,7 +37332,7 @@
         <v>22</v>
       </c>
       <c r="J3">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="4" spans="1:10">
@@ -37558,7 +37561,7 @@
         <v>236</v>
       </c>
       <c r="J11">
-        <v>158</v>
+        <v>159</v>
       </c>
     </row>
   </sheetData>
@@ -37809,7 +37812,7 @@
         <v>160</v>
       </c>
       <c r="J8">
-        <v>65</v>
+        <v>66</v>
       </c>
     </row>
     <row r="9" spans="1:10">
@@ -37841,7 +37844,7 @@
         <v>40</v>
       </c>
       <c r="J9">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="10" spans="1:10">
@@ -37873,7 +37876,7 @@
         <v>717</v>
       </c>
       <c r="J10">
-        <v>329</v>
+        <v>332</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -37905,7 +37908,7 @@
         <v>1066</v>
       </c>
       <c r="J11">
-        <v>494</v>
+        <v>499</v>
       </c>
     </row>
   </sheetData>
@@ -38214,7 +38217,7 @@
         <v>260</v>
       </c>
       <c r="J10">
-        <v>127</v>
+        <v>128</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -38246,7 +38249,7 @@
         <v>393</v>
       </c>
       <c r="J11">
-        <v>180</v>
+        <v>181</v>
       </c>
     </row>
   </sheetData>
@@ -38543,7 +38546,7 @@
         <v>135</v>
       </c>
       <c r="J10">
-        <v>70</v>
+        <v>71</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -38575,7 +38578,7 @@
         <v>219</v>
       </c>
       <c r="J11">
-        <v>127</v>
+        <v>128</v>
       </c>
     </row>
   </sheetData>
@@ -39512,7 +39515,7 @@
         <v>174</v>
       </c>
       <c r="J10">
-        <v>94</v>
+        <v>95</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -39544,7 +39547,7 @@
         <v>235</v>
       </c>
       <c r="J11">
-        <v>138</v>
+        <v>139</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add data for 2023-07-26
</commit_message>
<xml_diff>
--- a/output/index-crime-full-year.xlsx
+++ b/output/index-crime-full-year.xlsx
@@ -895,7 +895,7 @@
         <v>7278</v>
       </c>
       <c r="J2">
-        <v>4213</v>
+        <v>4239</v>
       </c>
     </row>
     <row r="3" spans="1:10">
@@ -927,7 +927,7 @@
         <v>7486</v>
       </c>
       <c r="J3">
-        <v>4434</v>
+        <v>4458</v>
       </c>
     </row>
     <row r="4" spans="1:10">
@@ -959,7 +959,7 @@
         <v>422</v>
       </c>
       <c r="J4">
-        <v>280</v>
+        <v>281</v>
       </c>
     </row>
     <row r="5" spans="1:10">
@@ -991,7 +991,7 @@
         <v>7592</v>
       </c>
       <c r="J5">
-        <v>4083</v>
+        <v>4102</v>
       </c>
     </row>
     <row r="6" spans="1:10">
@@ -1023,7 +1023,7 @@
         <v>1767</v>
       </c>
       <c r="J6">
-        <v>991</v>
+        <v>994</v>
       </c>
     </row>
     <row r="7" spans="1:10">
@@ -1055,7 +1055,7 @@
         <v>718</v>
       </c>
       <c r="J7">
-        <v>353</v>
+        <v>356</v>
       </c>
     </row>
     <row r="8" spans="1:10">
@@ -1087,7 +1087,7 @@
         <v>21446</v>
       </c>
       <c r="J8">
-        <v>16632</v>
+        <v>16727</v>
       </c>
     </row>
     <row r="9" spans="1:10">
@@ -1119,7 +1119,7 @@
         <v>8965</v>
       </c>
       <c r="J9">
-        <v>5292</v>
+        <v>5326</v>
       </c>
     </row>
     <row r="10" spans="1:10">
@@ -1151,7 +1151,7 @@
         <v>54808</v>
       </c>
       <c r="J10">
-        <v>30442</v>
+        <v>30624</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -1183,7 +1183,7 @@
         <v>110482</v>
       </c>
       <c r="J11">
-        <v>66720</v>
+        <v>67107</v>
       </c>
     </row>
   </sheetData>
@@ -1440,7 +1440,7 @@
         <v>227</v>
       </c>
       <c r="J8">
-        <v>221</v>
+        <v>223</v>
       </c>
     </row>
     <row r="9" spans="1:10">
@@ -1504,7 +1504,7 @@
         <v>648</v>
       </c>
       <c r="J10">
-        <v>412</v>
+        <v>413</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -1536,7 +1536,7 @@
         <v>1153</v>
       </c>
       <c r="J11">
-        <v>801</v>
+        <v>804</v>
       </c>
     </row>
   </sheetData>
@@ -1720,7 +1720,7 @@
         <v>7</v>
       </c>
       <c r="J6">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="7" spans="1:10">
@@ -1778,7 +1778,7 @@
         <v>38</v>
       </c>
       <c r="J8">
-        <v>24</v>
+        <v>25</v>
       </c>
     </row>
     <row r="9" spans="1:10">
@@ -1810,7 +1810,7 @@
         <v>57</v>
       </c>
       <c r="J9">
-        <v>35</v>
+        <v>37</v>
       </c>
     </row>
   </sheetData>
@@ -1963,7 +1963,7 @@
         <v>11</v>
       </c>
       <c r="J4">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="5" spans="1:10">
@@ -2091,7 +2091,7 @@
         <v>373</v>
       </c>
       <c r="J8">
-        <v>286</v>
+        <v>291</v>
       </c>
     </row>
     <row r="9" spans="1:10">
@@ -2155,7 +2155,7 @@
         <v>820</v>
       </c>
       <c r="J10">
-        <v>520</v>
+        <v>521</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -2187,7 +2187,7 @@
         <v>1712</v>
       </c>
       <c r="J11">
-        <v>1129</v>
+        <v>1136</v>
       </c>
     </row>
   </sheetData>
@@ -2462,7 +2462,7 @@
         <v>188</v>
       </c>
       <c r="J8">
-        <v>149</v>
+        <v>152</v>
       </c>
     </row>
     <row r="9" spans="1:10">
@@ -2526,7 +2526,7 @@
         <v>712</v>
       </c>
       <c r="J10">
-        <v>408</v>
+        <v>411</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -2558,7 +2558,7 @@
         <v>1228</v>
       </c>
       <c r="J11">
-        <v>737</v>
+        <v>743</v>
       </c>
     </row>
   </sheetData>
@@ -2775,7 +2775,7 @@
         <v>42</v>
       </c>
       <c r="J6">
-        <v>24</v>
+        <v>26</v>
       </c>
     </row>
     <row r="7" spans="1:10">
@@ -2839,7 +2839,7 @@
         <v>700</v>
       </c>
       <c r="J8">
-        <v>488</v>
+        <v>492</v>
       </c>
     </row>
     <row r="9" spans="1:10">
@@ -2903,7 +2903,7 @@
         <v>820</v>
       </c>
       <c r="J10">
-        <v>447</v>
+        <v>450</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -2935,7 +2935,7 @@
         <v>2472</v>
       </c>
       <c r="J11">
-        <v>1466</v>
+        <v>1475</v>
       </c>
     </row>
   </sheetData>
@@ -3213,7 +3213,7 @@
         <v>259</v>
       </c>
       <c r="J8">
-        <v>261</v>
+        <v>262</v>
       </c>
     </row>
     <row r="9" spans="1:10">
@@ -3277,7 +3277,7 @@
         <v>913</v>
       </c>
       <c r="J10">
-        <v>620</v>
+        <v>623</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -3309,7 +3309,7 @@
         <v>1600</v>
       </c>
       <c r="J11">
-        <v>1123</v>
+        <v>1127</v>
       </c>
     </row>
   </sheetData>
@@ -3584,7 +3584,7 @@
         <v>57</v>
       </c>
       <c r="J8">
-        <v>53</v>
+        <v>54</v>
       </c>
     </row>
     <row r="9" spans="1:10">
@@ -3680,7 +3680,7 @@
         <v>260</v>
       </c>
       <c r="J11">
-        <v>169</v>
+        <v>170</v>
       </c>
     </row>
   </sheetData>
@@ -3801,7 +3801,7 @@
         <v>71</v>
       </c>
       <c r="J3">
-        <v>35</v>
+        <v>36</v>
       </c>
     </row>
     <row r="4" spans="1:10">
@@ -3865,7 +3865,7 @@
         <v>139</v>
       </c>
       <c r="J5">
-        <v>70</v>
+        <v>71</v>
       </c>
     </row>
     <row r="6" spans="1:10">
@@ -4025,7 +4025,7 @@
         <v>681</v>
       </c>
       <c r="J10">
-        <v>494</v>
+        <v>497</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -4057,7 +4057,7 @@
         <v>1279</v>
       </c>
       <c r="J11">
-        <v>895</v>
+        <v>900</v>
       </c>
     </row>
   </sheetData>
@@ -4146,7 +4146,7 @@
         <v>459</v>
       </c>
       <c r="J2">
-        <v>269</v>
+        <v>271</v>
       </c>
     </row>
     <row r="3" spans="1:10">
@@ -4178,7 +4178,7 @@
         <v>530</v>
       </c>
       <c r="J3">
-        <v>299</v>
+        <v>301</v>
       </c>
     </row>
     <row r="4" spans="1:10">
@@ -4242,7 +4242,7 @@
         <v>268</v>
       </c>
       <c r="J5">
-        <v>160</v>
+        <v>161</v>
       </c>
     </row>
     <row r="6" spans="1:10">
@@ -4306,7 +4306,7 @@
         <v>49</v>
       </c>
       <c r="J7">
-        <v>36</v>
+        <v>37</v>
       </c>
     </row>
     <row r="8" spans="1:10">
@@ -4338,7 +4338,7 @@
         <v>794</v>
       </c>
       <c r="J8">
-        <v>608</v>
+        <v>617</v>
       </c>
     </row>
     <row r="9" spans="1:10">
@@ -4370,7 +4370,7 @@
         <v>433</v>
       </c>
       <c r="J9">
-        <v>213</v>
+        <v>214</v>
       </c>
     </row>
     <row r="10" spans="1:10">
@@ -4402,7 +4402,7 @@
         <v>1302</v>
       </c>
       <c r="J10">
-        <v>737</v>
+        <v>738</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -4434,7 +4434,7 @@
         <v>3950</v>
       </c>
       <c r="J11">
-        <v>2390</v>
+        <v>2407</v>
       </c>
     </row>
   </sheetData>
@@ -4555,7 +4555,7 @@
         <v>16</v>
       </c>
       <c r="J3">
-        <v>15</v>
+        <v>16</v>
       </c>
     </row>
     <row r="4" spans="1:10">
@@ -4697,7 +4697,7 @@
         <v>131</v>
       </c>
       <c r="J8">
-        <v>149</v>
+        <v>150</v>
       </c>
     </row>
     <row r="9" spans="1:10">
@@ -4761,7 +4761,7 @@
         <v>921</v>
       </c>
       <c r="J10">
-        <v>400</v>
+        <v>402</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -4793,7 +4793,7 @@
         <v>1318</v>
       </c>
       <c r="J11">
-        <v>691</v>
+        <v>695</v>
       </c>
     </row>
   </sheetData>
@@ -4882,7 +4882,7 @@
         <v>216</v>
       </c>
       <c r="J2">
-        <v>126</v>
+        <v>128</v>
       </c>
     </row>
     <row r="3" spans="1:10">
@@ -4914,7 +4914,7 @@
         <v>280</v>
       </c>
       <c r="J3">
-        <v>124</v>
+        <v>126</v>
       </c>
     </row>
     <row r="4" spans="1:10">
@@ -5074,7 +5074,7 @@
         <v>653</v>
       </c>
       <c r="J8">
-        <v>547</v>
+        <v>551</v>
       </c>
     </row>
     <row r="9" spans="1:10">
@@ -5106,7 +5106,7 @@
         <v>428</v>
       </c>
       <c r="J9">
-        <v>289</v>
+        <v>293</v>
       </c>
     </row>
     <row r="10" spans="1:10">
@@ -5138,7 +5138,7 @@
         <v>1089</v>
       </c>
       <c r="J10">
-        <v>689</v>
+        <v>690</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -5170,7 +5170,7 @@
         <v>2956</v>
       </c>
       <c r="J11">
-        <v>1937</v>
+        <v>1950</v>
       </c>
     </row>
   </sheetData>
@@ -5259,7 +5259,7 @@
         <v>917</v>
       </c>
       <c r="J2">
-        <v>579</v>
+        <v>584</v>
       </c>
     </row>
     <row r="3" spans="1:10">
@@ -5291,7 +5291,7 @@
         <v>155</v>
       </c>
       <c r="J3">
-        <v>106</v>
+        <v>107</v>
       </c>
     </row>
     <row r="4" spans="1:10">
@@ -5323,7 +5323,7 @@
         <v>436</v>
       </c>
       <c r="J4">
-        <v>255</v>
+        <v>258</v>
       </c>
     </row>
     <row r="5" spans="1:10">
@@ -5419,7 +5419,7 @@
         <v>2686</v>
       </c>
       <c r="J7">
-        <v>1678</v>
+        <v>1688</v>
       </c>
     </row>
     <row r="8" spans="1:10">
@@ -5451,7 +5451,7 @@
         <v>4743</v>
       </c>
       <c r="J8">
-        <v>2830</v>
+        <v>2851</v>
       </c>
     </row>
     <row r="9" spans="1:10">
@@ -5483,7 +5483,7 @@
         <v>519</v>
       </c>
       <c r="J9">
-        <v>316</v>
+        <v>318</v>
       </c>
     </row>
     <row r="10" spans="1:10">
@@ -5515,7 +5515,7 @@
         <v>948</v>
       </c>
       <c r="J10">
-        <v>541</v>
+        <v>543</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -5547,7 +5547,7 @@
         <v>1712</v>
       </c>
       <c r="J11">
-        <v>1129</v>
+        <v>1136</v>
       </c>
     </row>
     <row r="12" spans="1:10">
@@ -5579,7 +5579,7 @@
         <v>412</v>
       </c>
       <c r="J12">
-        <v>235</v>
+        <v>237</v>
       </c>
     </row>
     <row r="13" spans="1:10">
@@ -5611,7 +5611,7 @@
         <v>258</v>
       </c>
       <c r="J13">
-        <v>156</v>
+        <v>157</v>
       </c>
     </row>
     <row r="14" spans="1:10">
@@ -5643,7 +5643,7 @@
         <v>718</v>
       </c>
       <c r="J14">
-        <v>360</v>
+        <v>363</v>
       </c>
     </row>
     <row r="15" spans="1:10">
@@ -5675,7 +5675,7 @@
         <v>886</v>
       </c>
       <c r="J15">
-        <v>592</v>
+        <v>594</v>
       </c>
     </row>
     <row r="16" spans="1:10">
@@ -5707,7 +5707,7 @@
         <v>595</v>
       </c>
       <c r="J16">
-        <v>434</v>
+        <v>438</v>
       </c>
     </row>
     <row r="17" spans="1:10">
@@ -5771,7 +5771,7 @@
         <v>695</v>
       </c>
       <c r="J18">
-        <v>440</v>
+        <v>444</v>
       </c>
     </row>
     <row r="19" spans="1:10">
@@ -5803,7 +5803,7 @@
         <v>2636</v>
       </c>
       <c r="J19">
-        <v>1554</v>
+        <v>1561</v>
       </c>
     </row>
     <row r="20" spans="1:10">
@@ -5835,7 +5835,7 @@
         <v>2045</v>
       </c>
       <c r="J20">
-        <v>1116</v>
+        <v>1121</v>
       </c>
     </row>
     <row r="21" spans="1:10">
@@ -5867,7 +5867,7 @@
         <v>337</v>
       </c>
       <c r="J21">
-        <v>158</v>
+        <v>159</v>
       </c>
     </row>
     <row r="22" spans="1:10">
@@ -5899,7 +5899,7 @@
         <v>418</v>
       </c>
       <c r="J22">
-        <v>308</v>
+        <v>310</v>
       </c>
     </row>
     <row r="23" spans="1:10">
@@ -5931,7 +5931,7 @@
         <v>1368</v>
       </c>
       <c r="J23">
-        <v>844</v>
+        <v>850</v>
       </c>
     </row>
     <row r="24" spans="1:10">
@@ -5963,7 +5963,7 @@
         <v>500</v>
       </c>
       <c r="J24">
-        <v>354</v>
+        <v>357</v>
       </c>
     </row>
     <row r="25" spans="1:10">
@@ -5995,7 +5995,7 @@
         <v>429</v>
       </c>
       <c r="J25">
-        <v>284</v>
+        <v>288</v>
       </c>
     </row>
     <row r="26" spans="1:10">
@@ -6027,7 +6027,7 @@
         <v>248</v>
       </c>
       <c r="J26">
-        <v>173</v>
+        <v>174</v>
       </c>
     </row>
     <row r="27" spans="1:10">
@@ -6059,7 +6059,7 @@
         <v>1258</v>
       </c>
       <c r="J27">
-        <v>780</v>
+        <v>785</v>
       </c>
     </row>
     <row r="28" spans="1:10">
@@ -6123,7 +6123,7 @@
         <v>3950</v>
       </c>
       <c r="J29">
-        <v>2390</v>
+        <v>2407</v>
       </c>
     </row>
     <row r="30" spans="1:10">
@@ -6155,7 +6155,7 @@
         <v>260</v>
       </c>
       <c r="J30">
-        <v>169</v>
+        <v>170</v>
       </c>
     </row>
     <row r="31" spans="1:10">
@@ -6187,7 +6187,7 @@
         <v>868</v>
       </c>
       <c r="J31">
-        <v>494</v>
+        <v>496</v>
       </c>
     </row>
     <row r="32" spans="1:10">
@@ -6219,7 +6219,7 @@
         <v>209</v>
       </c>
       <c r="J32">
-        <v>159</v>
+        <v>160</v>
       </c>
     </row>
     <row r="33" spans="1:10">
@@ -6251,7 +6251,7 @@
         <v>3011</v>
       </c>
       <c r="J33">
-        <v>1907</v>
+        <v>1920</v>
       </c>
     </row>
     <row r="34" spans="1:10">
@@ -6283,7 +6283,7 @@
         <v>761</v>
       </c>
       <c r="J34">
-        <v>502</v>
+        <v>503</v>
       </c>
     </row>
     <row r="35" spans="1:10">
@@ -6315,7 +6315,7 @@
         <v>235</v>
       </c>
       <c r="J35">
-        <v>139</v>
+        <v>141</v>
       </c>
     </row>
     <row r="36" spans="1:10">
@@ -6347,7 +6347,7 @@
         <v>1491</v>
       </c>
       <c r="J36">
-        <v>950</v>
+        <v>953</v>
       </c>
     </row>
     <row r="37" spans="1:10">
@@ -6379,7 +6379,7 @@
         <v>2547</v>
       </c>
       <c r="J37">
-        <v>1610</v>
+        <v>1622</v>
       </c>
     </row>
     <row r="38" spans="1:10">
@@ -6411,7 +6411,7 @@
         <v>191</v>
       </c>
       <c r="J38">
-        <v>107</v>
+        <v>108</v>
       </c>
     </row>
     <row r="39" spans="1:10">
@@ -6443,7 +6443,7 @@
         <v>153</v>
       </c>
       <c r="J39">
-        <v>58</v>
+        <v>59</v>
       </c>
     </row>
     <row r="40" spans="1:10">
@@ -6475,7 +6475,7 @@
         <v>236</v>
       </c>
       <c r="J40">
-        <v>159</v>
+        <v>163</v>
       </c>
     </row>
     <row r="41" spans="1:10">
@@ -6507,7 +6507,7 @@
         <v>437</v>
       </c>
       <c r="J41">
-        <v>322</v>
+        <v>324</v>
       </c>
     </row>
     <row r="42" spans="1:10">
@@ -6539,7 +6539,7 @@
         <v>2956</v>
       </c>
       <c r="J42">
-        <v>1937</v>
+        <v>1950</v>
       </c>
     </row>
     <row r="43" spans="1:10">
@@ -6571,7 +6571,7 @@
         <v>1153</v>
       </c>
       <c r="J43">
-        <v>801</v>
+        <v>804</v>
       </c>
     </row>
     <row r="44" spans="1:10">
@@ -6603,7 +6603,7 @@
         <v>1228</v>
       </c>
       <c r="J44">
-        <v>737</v>
+        <v>743</v>
       </c>
     </row>
     <row r="45" spans="1:10">
@@ -6667,7 +6667,7 @@
         <v>436</v>
       </c>
       <c r="J46">
-        <v>280</v>
+        <v>281</v>
       </c>
     </row>
     <row r="47" spans="1:10">
@@ -6699,7 +6699,7 @@
         <v>903</v>
       </c>
       <c r="J47">
-        <v>566</v>
+        <v>570</v>
       </c>
     </row>
     <row r="48" spans="1:10">
@@ -6731,7 +6731,7 @@
         <v>2622</v>
       </c>
       <c r="J48">
-        <v>1553</v>
+        <v>1563</v>
       </c>
     </row>
     <row r="49" spans="1:10">
@@ -6763,7 +6763,7 @@
         <v>1648</v>
       </c>
       <c r="J49">
-        <v>952</v>
+        <v>957</v>
       </c>
     </row>
     <row r="50" spans="1:10">
@@ -6795,7 +6795,7 @@
         <v>960</v>
       </c>
       <c r="J50">
-        <v>565</v>
+        <v>566</v>
       </c>
     </row>
     <row r="51" spans="1:10">
@@ -6827,7 +6827,7 @@
         <v>1337</v>
       </c>
       <c r="J51">
-        <v>892</v>
+        <v>898</v>
       </c>
     </row>
     <row r="52" spans="1:10">
@@ -6859,7 +6859,7 @@
         <v>1491</v>
       </c>
       <c r="J52">
-        <v>1063</v>
+        <v>1068</v>
       </c>
     </row>
     <row r="53" spans="1:10">
@@ -6891,7 +6891,7 @@
         <v>1600</v>
       </c>
       <c r="J53">
-        <v>1123</v>
+        <v>1127</v>
       </c>
     </row>
     <row r="54" spans="1:10">
@@ -6923,7 +6923,7 @@
         <v>3506</v>
       </c>
       <c r="J54">
-        <v>2033</v>
+        <v>2038</v>
       </c>
     </row>
     <row r="55" spans="1:10">
@@ -6955,7 +6955,7 @@
         <v>1244</v>
       </c>
       <c r="J55">
-        <v>710</v>
+        <v>713</v>
       </c>
     </row>
     <row r="56" spans="1:10">
@@ -6987,7 +6987,7 @@
         <v>628</v>
       </c>
       <c r="J56">
-        <v>335</v>
+        <v>336</v>
       </c>
     </row>
     <row r="57" spans="1:10">
@@ -7019,7 +7019,7 @@
         <v>406</v>
       </c>
       <c r="J57">
-        <v>290</v>
+        <v>292</v>
       </c>
     </row>
     <row r="58" spans="1:10">
@@ -7083,7 +7083,7 @@
         <v>271</v>
       </c>
       <c r="J59">
-        <v>185</v>
+        <v>186</v>
       </c>
     </row>
     <row r="60" spans="1:10">
@@ -7115,7 +7115,7 @@
         <v>768</v>
       </c>
       <c r="J60">
-        <v>481</v>
+        <v>485</v>
       </c>
     </row>
     <row r="61" spans="1:10">
@@ -7179,7 +7179,7 @@
         <v>57</v>
       </c>
       <c r="J62">
-        <v>35</v>
+        <v>37</v>
       </c>
     </row>
     <row r="63" spans="1:10">
@@ -7211,7 +7211,7 @@
         <v>2481</v>
       </c>
       <c r="J63">
-        <v>744</v>
+        <v>756</v>
       </c>
     </row>
     <row r="64" spans="1:10">
@@ -7243,7 +7243,7 @@
         <v>1187</v>
       </c>
       <c r="J64">
-        <v>641</v>
+        <v>643</v>
       </c>
     </row>
     <row r="65" spans="1:10">
@@ -7275,7 +7275,7 @@
         <v>1515</v>
       </c>
       <c r="J65">
-        <v>1024</v>
+        <v>1027</v>
       </c>
     </row>
     <row r="66" spans="1:10">
@@ -7307,7 +7307,7 @@
         <v>715</v>
       </c>
       <c r="J66">
-        <v>439</v>
+        <v>440</v>
       </c>
     </row>
     <row r="67" spans="1:10">
@@ -7339,7 +7339,7 @@
         <v>2510</v>
       </c>
       <c r="J67">
-        <v>1560</v>
+        <v>1570</v>
       </c>
     </row>
     <row r="68" spans="1:10">
@@ -7371,7 +7371,7 @@
         <v>437</v>
       </c>
       <c r="J68">
-        <v>205</v>
+        <v>207</v>
       </c>
     </row>
     <row r="69" spans="1:10">
@@ -7403,7 +7403,7 @@
         <v>494</v>
       </c>
       <c r="J69">
-        <v>260</v>
+        <v>262</v>
       </c>
     </row>
     <row r="70" spans="1:10">
@@ -7435,7 +7435,7 @@
         <v>677</v>
       </c>
       <c r="J70">
-        <v>420</v>
+        <v>423</v>
       </c>
     </row>
     <row r="71" spans="1:10">
@@ -7467,7 +7467,7 @@
         <v>335</v>
       </c>
       <c r="J71">
-        <v>260</v>
+        <v>262</v>
       </c>
     </row>
     <row r="72" spans="1:10">
@@ -7499,7 +7499,7 @@
         <v>706</v>
       </c>
       <c r="J72">
-        <v>392</v>
+        <v>395</v>
       </c>
     </row>
     <row r="73" spans="1:10">
@@ -7531,7 +7531,7 @@
         <v>1279</v>
       </c>
       <c r="J73">
-        <v>895</v>
+        <v>900</v>
       </c>
     </row>
     <row r="74" spans="1:10">
@@ -7563,7 +7563,7 @@
         <v>307</v>
       </c>
       <c r="J74">
-        <v>158</v>
+        <v>159</v>
       </c>
     </row>
     <row r="75" spans="1:10">
@@ -7595,7 +7595,7 @@
         <v>340</v>
       </c>
       <c r="J75">
-        <v>205</v>
+        <v>207</v>
       </c>
     </row>
     <row r="76" spans="1:10">
@@ -7627,7 +7627,7 @@
         <v>2923</v>
       </c>
       <c r="J76">
-        <v>1715</v>
+        <v>1720</v>
       </c>
     </row>
     <row r="77" spans="1:10">
@@ -7659,7 +7659,7 @@
         <v>462</v>
       </c>
       <c r="J77">
-        <v>309</v>
+        <v>310</v>
       </c>
     </row>
     <row r="78" spans="1:10">
@@ -7691,7 +7691,7 @@
         <v>1797</v>
       </c>
       <c r="J78">
-        <v>1029</v>
+        <v>1032</v>
       </c>
     </row>
     <row r="79" spans="1:10">
@@ -7723,7 +7723,7 @@
         <v>2472</v>
       </c>
       <c r="J79">
-        <v>1466</v>
+        <v>1475</v>
       </c>
     </row>
     <row r="80" spans="1:10">
@@ -7755,7 +7755,7 @@
         <v>393</v>
       </c>
       <c r="J80">
-        <v>181</v>
+        <v>183</v>
       </c>
     </row>
     <row r="81" spans="1:10">
@@ -7787,7 +7787,7 @@
         <v>219</v>
       </c>
       <c r="J81">
-        <v>128</v>
+        <v>129</v>
       </c>
     </row>
     <row r="82" spans="1:10">
@@ -7851,7 +7851,7 @@
         <v>1793</v>
       </c>
       <c r="J83">
-        <v>1033</v>
+        <v>1041</v>
       </c>
     </row>
     <row r="84" spans="1:10">
@@ -7883,7 +7883,7 @@
         <v>729</v>
       </c>
       <c r="J84">
-        <v>494</v>
+        <v>497</v>
       </c>
     </row>
     <row r="85" spans="1:10">
@@ -7915,7 +7915,7 @@
         <v>3848</v>
       </c>
       <c r="J85">
-        <v>2435</v>
+        <v>2447</v>
       </c>
     </row>
     <row r="86" spans="1:10">
@@ -7947,7 +7947,7 @@
         <v>1066</v>
       </c>
       <c r="J86">
-        <v>499</v>
+        <v>502</v>
       </c>
     </row>
     <row r="87" spans="1:10">
@@ -7979,7 +7979,7 @@
         <v>396</v>
       </c>
       <c r="J87">
-        <v>226</v>
+        <v>227</v>
       </c>
     </row>
     <row r="88" spans="1:10">
@@ -8011,7 +8011,7 @@
         <v>943</v>
       </c>
       <c r="J88">
-        <v>587</v>
+        <v>591</v>
       </c>
     </row>
     <row r="89" spans="1:10">
@@ -8043,7 +8043,7 @@
         <v>1879</v>
       </c>
       <c r="J89">
-        <v>1170</v>
+        <v>1176</v>
       </c>
     </row>
     <row r="90" spans="1:10">
@@ -8075,7 +8075,7 @@
         <v>1354</v>
       </c>
       <c r="J90">
-        <v>867</v>
+        <v>872</v>
       </c>
     </row>
     <row r="91" spans="1:10">
@@ -8139,7 +8139,7 @@
         <v>337</v>
       </c>
       <c r="J92">
-        <v>237</v>
+        <v>238</v>
       </c>
     </row>
     <row r="93" spans="1:10">
@@ -8171,7 +8171,7 @@
         <v>721</v>
       </c>
       <c r="J93">
-        <v>453</v>
+        <v>457</v>
       </c>
     </row>
     <row r="94" spans="1:10">
@@ -8203,7 +8203,7 @@
         <v>2663</v>
       </c>
       <c r="J94">
-        <v>1429</v>
+        <v>1432</v>
       </c>
     </row>
     <row r="95" spans="1:10">
@@ -8235,7 +8235,7 @@
         <v>1389</v>
       </c>
       <c r="J95">
-        <v>870</v>
+        <v>873</v>
       </c>
     </row>
     <row r="96" spans="1:10">
@@ -8267,7 +8267,7 @@
         <v>1669</v>
       </c>
       <c r="J96">
-        <v>948</v>
+        <v>956</v>
       </c>
     </row>
     <row r="97" spans="1:10">
@@ -8299,7 +8299,7 @@
         <v>1673</v>
       </c>
       <c r="J97">
-        <v>996</v>
+        <v>1005</v>
       </c>
     </row>
     <row r="98" spans="1:10">
@@ -8331,7 +8331,7 @@
         <v>1318</v>
       </c>
       <c r="J98">
-        <v>691</v>
+        <v>695</v>
       </c>
     </row>
     <row r="99" spans="1:10">
@@ -8363,7 +8363,7 @@
         <v>1488</v>
       </c>
       <c r="J99">
-        <v>941</v>
+        <v>947</v>
       </c>
     </row>
     <row r="100" spans="1:10">
@@ -8395,7 +8395,7 @@
         <v>237</v>
       </c>
       <c r="J100">
-        <v>175</v>
+        <v>176</v>
       </c>
     </row>
     <row r="101" spans="1:10">
@@ -8427,7 +8427,7 @@
         <v>110482</v>
       </c>
       <c r="J101">
-        <v>66720</v>
+        <v>67107</v>
       </c>
     </row>
   </sheetData>
@@ -8795,7 +8795,7 @@
         <v>219</v>
       </c>
       <c r="J8">
-        <v>124</v>
+        <v>125</v>
       </c>
     </row>
     <row r="9" spans="1:10">
@@ -8859,7 +8859,7 @@
         <v>1135</v>
       </c>
       <c r="J10">
-        <v>649</v>
+        <v>653</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -8891,7 +8891,7 @@
         <v>1648</v>
       </c>
       <c r="J11">
-        <v>952</v>
+        <v>957</v>
       </c>
     </row>
   </sheetData>
@@ -8980,7 +8980,7 @@
         <v>327</v>
       </c>
       <c r="J2">
-        <v>169</v>
+        <v>171</v>
       </c>
     </row>
     <row r="3" spans="1:10">
@@ -9012,7 +9012,7 @@
         <v>439</v>
       </c>
       <c r="J3">
-        <v>253</v>
+        <v>254</v>
       </c>
     </row>
     <row r="4" spans="1:10">
@@ -9172,7 +9172,7 @@
         <v>1026</v>
       </c>
       <c r="J8">
-        <v>825</v>
+        <v>828</v>
       </c>
     </row>
     <row r="9" spans="1:10">
@@ -9236,7 +9236,7 @@
         <v>1271</v>
       </c>
       <c r="J10">
-        <v>750</v>
+        <v>756</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -9268,7 +9268,7 @@
         <v>3848</v>
       </c>
       <c r="J11">
-        <v>2435</v>
+        <v>2447</v>
       </c>
     </row>
   </sheetData>
@@ -9389,7 +9389,7 @@
         <v>80</v>
       </c>
       <c r="J3">
-        <v>45</v>
+        <v>46</v>
       </c>
     </row>
     <row r="4" spans="1:10">
@@ -9546,7 +9546,7 @@
         <v>336</v>
       </c>
       <c r="J8">
-        <v>180</v>
+        <v>181</v>
       </c>
     </row>
     <row r="9" spans="1:10">
@@ -9578,7 +9578,7 @@
         <v>179</v>
       </c>
       <c r="J9">
-        <v>125</v>
+        <v>126</v>
       </c>
     </row>
     <row r="10" spans="1:10">
@@ -9610,7 +9610,7 @@
         <v>2132</v>
       </c>
       <c r="J10">
-        <v>1236</v>
+        <v>1238</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -9642,7 +9642,7 @@
         <v>2923</v>
       </c>
       <c r="J11">
-        <v>1715</v>
+        <v>1720</v>
       </c>
     </row>
   </sheetData>
@@ -9821,7 +9821,7 @@
         <v>122</v>
       </c>
       <c r="J5">
-        <v>81</v>
+        <v>82</v>
       </c>
     </row>
     <row r="6" spans="1:10">
@@ -9914,7 +9914,7 @@
         <v>280</v>
       </c>
       <c r="J8">
-        <v>307</v>
+        <v>308</v>
       </c>
     </row>
     <row r="9" spans="1:10">
@@ -9978,7 +9978,7 @@
         <v>1034</v>
       </c>
       <c r="J10">
-        <v>495</v>
+        <v>502</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -10010,7 +10010,7 @@
         <v>1673</v>
       </c>
       <c r="J11">
-        <v>996</v>
+        <v>1005</v>
       </c>
     </row>
   </sheetData>
@@ -10099,7 +10099,7 @@
         <v>235</v>
       </c>
       <c r="J2">
-        <v>141</v>
+        <v>142</v>
       </c>
     </row>
     <row r="3" spans="1:10">
@@ -10291,7 +10291,7 @@
         <v>516</v>
       </c>
       <c r="J8">
-        <v>400</v>
+        <v>405</v>
       </c>
     </row>
     <row r="9" spans="1:10">
@@ -10323,7 +10323,7 @@
         <v>295</v>
       </c>
       <c r="J9">
-        <v>158</v>
+        <v>161</v>
       </c>
     </row>
     <row r="10" spans="1:10">
@@ -10355,7 +10355,7 @@
         <v>895</v>
       </c>
       <c r="J10">
-        <v>485</v>
+        <v>486</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -10387,7 +10387,7 @@
         <v>2510</v>
       </c>
       <c r="J11">
-        <v>1560</v>
+        <v>1570</v>
       </c>
     </row>
   </sheetData>
@@ -10476,7 +10476,7 @@
         <v>142</v>
       </c>
       <c r="J2">
-        <v>84</v>
+        <v>85</v>
       </c>
     </row>
     <row r="3" spans="1:10">
@@ -10508,7 +10508,7 @@
         <v>137</v>
       </c>
       <c r="J3">
-        <v>75</v>
+        <v>77</v>
       </c>
     </row>
     <row r="4" spans="1:10">
@@ -10764,7 +10764,7 @@
         <v>1389</v>
       </c>
       <c r="J11">
-        <v>870</v>
+        <v>873</v>
       </c>
     </row>
   </sheetData>
@@ -11045,7 +11045,7 @@
         <v>190</v>
       </c>
       <c r="J8">
-        <v>179</v>
+        <v>181</v>
       </c>
     </row>
     <row r="9" spans="1:10">
@@ -11109,7 +11109,7 @@
         <v>271</v>
       </c>
       <c r="J10">
-        <v>149</v>
+        <v>150</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -11141,7 +11141,7 @@
         <v>729</v>
       </c>
       <c r="J11">
-        <v>494</v>
+        <v>497</v>
       </c>
     </row>
   </sheetData>
@@ -11422,7 +11422,7 @@
         <v>218</v>
       </c>
       <c r="J8">
-        <v>208</v>
+        <v>211</v>
       </c>
     </row>
     <row r="9" spans="1:10">
@@ -11454,7 +11454,7 @@
         <v>196</v>
       </c>
       <c r="J9">
-        <v>177</v>
+        <v>178</v>
       </c>
     </row>
     <row r="10" spans="1:10">
@@ -11486,7 +11486,7 @@
         <v>590</v>
       </c>
       <c r="J10">
-        <v>389</v>
+        <v>390</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -11518,7 +11518,7 @@
         <v>1491</v>
       </c>
       <c r="J11">
-        <v>1063</v>
+        <v>1068</v>
       </c>
     </row>
   </sheetData>
@@ -11607,7 +11607,7 @@
         <v>67</v>
       </c>
       <c r="J2">
-        <v>37</v>
+        <v>38</v>
       </c>
     </row>
     <row r="3" spans="1:10">
@@ -11639,7 +11639,7 @@
         <v>78</v>
       </c>
       <c r="J3">
-        <v>54</v>
+        <v>55</v>
       </c>
     </row>
     <row r="4" spans="1:10">
@@ -11831,7 +11831,7 @@
         <v>81</v>
       </c>
       <c r="J9">
-        <v>64</v>
+        <v>66</v>
       </c>
     </row>
     <row r="10" spans="1:10">
@@ -11895,7 +11895,7 @@
         <v>943</v>
       </c>
       <c r="J11">
-        <v>587</v>
+        <v>591</v>
       </c>
     </row>
   </sheetData>
@@ -12205,7 +12205,7 @@
         <v>243</v>
       </c>
       <c r="J9">
-        <v>145</v>
+        <v>146</v>
       </c>
     </row>
     <row r="10" spans="1:10">
@@ -12237,7 +12237,7 @@
         <v>2528</v>
       </c>
       <c r="J10">
-        <v>1458</v>
+        <v>1462</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -12269,7 +12269,7 @@
         <v>3506</v>
       </c>
       <c r="J11">
-        <v>2033</v>
+        <v>2038</v>
       </c>
     </row>
   </sheetData>
@@ -12550,7 +12550,7 @@
         <v>503</v>
       </c>
       <c r="J8">
-        <v>365</v>
+        <v>367</v>
       </c>
     </row>
     <row r="9" spans="1:10">
@@ -12614,7 +12614,7 @@
         <v>527</v>
       </c>
       <c r="J10">
-        <v>329</v>
+        <v>330</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -12646,7 +12646,7 @@
         <v>1491</v>
       </c>
       <c r="J11">
-        <v>950</v>
+        <v>953</v>
       </c>
     </row>
   </sheetData>
@@ -12735,7 +12735,7 @@
         <v>239</v>
       </c>
       <c r="J2">
-        <v>142</v>
+        <v>143</v>
       </c>
     </row>
     <row r="3" spans="1:10">
@@ -12767,7 +12767,7 @@
         <v>261</v>
       </c>
       <c r="J3">
-        <v>169</v>
+        <v>172</v>
       </c>
     </row>
     <row r="4" spans="1:10">
@@ -12895,7 +12895,7 @@
         <v>23</v>
       </c>
       <c r="J7">
-        <v>18</v>
+        <v>19</v>
       </c>
     </row>
     <row r="8" spans="1:10">
@@ -12927,7 +12927,7 @@
         <v>722</v>
       </c>
       <c r="J8">
-        <v>503</v>
+        <v>505</v>
       </c>
     </row>
     <row r="9" spans="1:10">
@@ -12959,7 +12959,7 @@
         <v>244</v>
       </c>
       <c r="J9">
-        <v>141</v>
+        <v>142</v>
       </c>
     </row>
     <row r="10" spans="1:10">
@@ -12991,7 +12991,7 @@
         <v>813</v>
       </c>
       <c r="J10">
-        <v>483</v>
+        <v>487</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -13023,7 +13023,7 @@
         <v>2547</v>
       </c>
       <c r="J11">
-        <v>1610</v>
+        <v>1622</v>
       </c>
     </row>
   </sheetData>
@@ -13347,7 +13347,7 @@
         <v>213</v>
       </c>
       <c r="J10">
-        <v>139</v>
+        <v>141</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -13379,7 +13379,7 @@
         <v>418</v>
       </c>
       <c r="J11">
-        <v>308</v>
+        <v>310</v>
       </c>
     </row>
   </sheetData>
@@ -13468,7 +13468,7 @@
         <v>21</v>
       </c>
       <c r="J2">
-        <v>18</v>
+        <v>19</v>
       </c>
     </row>
     <row r="3" spans="1:10">
@@ -13645,7 +13645,7 @@
         <v>89</v>
       </c>
       <c r="J8">
-        <v>80</v>
+        <v>81</v>
       </c>
     </row>
     <row r="9" spans="1:10">
@@ -13709,7 +13709,7 @@
         <v>448</v>
       </c>
       <c r="J10">
-        <v>230</v>
+        <v>231</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -13741,7 +13741,7 @@
         <v>706</v>
       </c>
       <c r="J11">
-        <v>392</v>
+        <v>395</v>
       </c>
     </row>
   </sheetData>
@@ -13830,7 +13830,7 @@
         <v>194</v>
       </c>
       <c r="J2">
-        <v>113</v>
+        <v>114</v>
       </c>
     </row>
     <row r="3" spans="1:10">
@@ -14054,7 +14054,7 @@
         <v>189</v>
       </c>
       <c r="J9">
-        <v>136</v>
+        <v>137</v>
       </c>
     </row>
     <row r="10" spans="1:10">
@@ -14086,7 +14086,7 @@
         <v>587</v>
       </c>
       <c r="J10">
-        <v>346</v>
+        <v>347</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -14118,7 +14118,7 @@
         <v>1515</v>
       </c>
       <c r="J11">
-        <v>1024</v>
+        <v>1027</v>
       </c>
     </row>
   </sheetData>
@@ -14313,6 +14313,9 @@
       <c r="I6">
         <v>4</v>
       </c>
+      <c r="J6">
+        <v>1</v>
+      </c>
     </row>
     <row r="7" spans="1:10">
       <c r="A7" s="1" t="s">
@@ -14456,7 +14459,7 @@
         <v>209</v>
       </c>
       <c r="J11">
-        <v>159</v>
+        <v>160</v>
       </c>
     </row>
   </sheetData>
@@ -14734,7 +14737,7 @@
         <v>175</v>
       </c>
       <c r="J8">
-        <v>159</v>
+        <v>161</v>
       </c>
     </row>
     <row r="9" spans="1:10">
@@ -14766,7 +14769,7 @@
         <v>46</v>
       </c>
       <c r="J9">
-        <v>30</v>
+        <v>31</v>
       </c>
     </row>
     <row r="10" spans="1:10">
@@ -14798,7 +14801,7 @@
         <v>379</v>
       </c>
       <c r="J10">
-        <v>198</v>
+        <v>199</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -14830,7 +14833,7 @@
         <v>768</v>
       </c>
       <c r="J11">
-        <v>481</v>
+        <v>485</v>
       </c>
     </row>
   </sheetData>
@@ -15160,7 +15163,7 @@
         <v>255</v>
       </c>
       <c r="J10">
-        <v>113</v>
+        <v>115</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -15192,7 +15195,7 @@
         <v>437</v>
       </c>
       <c r="J11">
-        <v>205</v>
+        <v>207</v>
       </c>
     </row>
   </sheetData>
@@ -15281,7 +15284,7 @@
         <v>190</v>
       </c>
       <c r="J2">
-        <v>101</v>
+        <v>102</v>
       </c>
     </row>
     <row r="3" spans="1:10">
@@ -15377,7 +15380,7 @@
         <v>124</v>
       </c>
       <c r="J5">
-        <v>54</v>
+        <v>55</v>
       </c>
     </row>
     <row r="6" spans="1:10">
@@ -15441,7 +15444,7 @@
         <v>24</v>
       </c>
       <c r="J7">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="8" spans="1:10">
@@ -15473,7 +15476,7 @@
         <v>484</v>
       </c>
       <c r="J8">
-        <v>293</v>
+        <v>294</v>
       </c>
     </row>
     <row r="9" spans="1:10">
@@ -15505,7 +15508,7 @@
         <v>123</v>
       </c>
       <c r="J9">
-        <v>93</v>
+        <v>94</v>
       </c>
     </row>
     <row r="10" spans="1:10">
@@ -15537,7 +15540,7 @@
         <v>612</v>
       </c>
       <c r="J10">
-        <v>340</v>
+        <v>343</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -15569,7 +15572,7 @@
         <v>1793</v>
       </c>
       <c r="J11">
-        <v>1033</v>
+        <v>1041</v>
       </c>
     </row>
   </sheetData>
@@ -15658,7 +15661,7 @@
         <v>92</v>
       </c>
       <c r="J2">
-        <v>43</v>
+        <v>44</v>
       </c>
     </row>
     <row r="3" spans="1:10">
@@ -15882,7 +15885,7 @@
         <v>109</v>
       </c>
       <c r="J9">
-        <v>94</v>
+        <v>95</v>
       </c>
     </row>
     <row r="10" spans="1:10">
@@ -15914,7 +15917,7 @@
         <v>610</v>
       </c>
       <c r="J10">
-        <v>300</v>
+        <v>301</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -15946,7 +15949,7 @@
         <v>1244</v>
       </c>
       <c r="J11">
-        <v>710</v>
+        <v>713</v>
       </c>
     </row>
   </sheetData>
@@ -16212,7 +16215,7 @@
         <v>294</v>
       </c>
       <c r="J8">
-        <v>221</v>
+        <v>222</v>
       </c>
     </row>
     <row r="9" spans="1:10">
@@ -16276,7 +16279,7 @@
         <v>2021</v>
       </c>
       <c r="J10">
-        <v>1014</v>
+        <v>1016</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -16308,7 +16311,7 @@
         <v>2663</v>
       </c>
       <c r="J11">
-        <v>1429</v>
+        <v>1432</v>
       </c>
     </row>
   </sheetData>
@@ -16429,7 +16432,7 @@
         <v>416</v>
       </c>
       <c r="J3">
-        <v>228</v>
+        <v>229</v>
       </c>
     </row>
     <row r="4" spans="1:10">
@@ -16493,7 +16496,7 @@
         <v>170</v>
       </c>
       <c r="J5">
-        <v>69</v>
+        <v>72</v>
       </c>
     </row>
     <row r="6" spans="1:10">
@@ -16589,7 +16592,7 @@
         <v>707</v>
       </c>
       <c r="J8">
-        <v>575</v>
+        <v>579</v>
       </c>
     </row>
     <row r="9" spans="1:10">
@@ -16621,7 +16624,7 @@
         <v>363</v>
       </c>
       <c r="J9">
-        <v>227</v>
+        <v>230</v>
       </c>
     </row>
     <row r="10" spans="1:10">
@@ -16653,7 +16656,7 @@
         <v>968</v>
       </c>
       <c r="J10">
-        <v>557</v>
+        <v>559</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -16685,7 +16688,7 @@
         <v>3011</v>
       </c>
       <c r="J11">
-        <v>1907</v>
+        <v>1920</v>
       </c>
     </row>
   </sheetData>
@@ -16774,7 +16777,7 @@
         <v>264</v>
       </c>
       <c r="J2">
-        <v>147</v>
+        <v>148</v>
       </c>
     </row>
     <row r="3" spans="1:10">
@@ -16806,7 +16809,7 @@
         <v>248</v>
       </c>
       <c r="J3">
-        <v>131</v>
+        <v>132</v>
       </c>
     </row>
     <row r="4" spans="1:10">
@@ -16870,7 +16873,7 @@
         <v>261</v>
       </c>
       <c r="J5">
-        <v>142</v>
+        <v>143</v>
       </c>
     </row>
     <row r="6" spans="1:10">
@@ -16966,7 +16969,7 @@
         <v>567</v>
       </c>
       <c r="J8">
-        <v>567</v>
+        <v>571</v>
       </c>
     </row>
     <row r="9" spans="1:10">
@@ -16998,7 +17001,7 @@
         <v>226</v>
       </c>
       <c r="J9">
-        <v>148</v>
+        <v>149</v>
       </c>
     </row>
     <row r="10" spans="1:10">
@@ -17030,7 +17033,7 @@
         <v>1023</v>
       </c>
       <c r="J10">
-        <v>513</v>
+        <v>515</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -17062,7 +17065,7 @@
         <v>2686</v>
       </c>
       <c r="J11">
-        <v>1678</v>
+        <v>1688</v>
       </c>
     </row>
   </sheetData>
@@ -17151,7 +17154,7 @@
         <v>457</v>
       </c>
       <c r="J2">
-        <v>284</v>
+        <v>286</v>
       </c>
     </row>
     <row r="3" spans="1:10">
@@ -17183,7 +17186,7 @@
         <v>445</v>
       </c>
       <c r="J3">
-        <v>305</v>
+        <v>307</v>
       </c>
     </row>
     <row r="4" spans="1:10">
@@ -17215,7 +17218,7 @@
         <v>30</v>
       </c>
       <c r="J4">
-        <v>21</v>
+        <v>22</v>
       </c>
     </row>
     <row r="5" spans="1:10">
@@ -17343,7 +17346,7 @@
         <v>1269</v>
       </c>
       <c r="J8">
-        <v>770</v>
+        <v>774</v>
       </c>
     </row>
     <row r="9" spans="1:10">
@@ -17375,7 +17378,7 @@
         <v>497</v>
       </c>
       <c r="J9">
-        <v>320</v>
+        <v>322</v>
       </c>
     </row>
     <row r="10" spans="1:10">
@@ -17407,7 +17410,7 @@
         <v>1652</v>
       </c>
       <c r="J10">
-        <v>922</v>
+        <v>932</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -17439,7 +17442,7 @@
         <v>4743</v>
       </c>
       <c r="J11">
-        <v>2830</v>
+        <v>2851</v>
       </c>
     </row>
   </sheetData>
@@ -17528,7 +17531,7 @@
         <v>106</v>
       </c>
       <c r="J2">
-        <v>61</v>
+        <v>62</v>
       </c>
     </row>
     <row r="3" spans="1:10">
@@ -17624,7 +17627,7 @@
         <v>113</v>
       </c>
       <c r="J5">
-        <v>48</v>
+        <v>49</v>
       </c>
     </row>
     <row r="6" spans="1:10">
@@ -17720,7 +17723,7 @@
         <v>441</v>
       </c>
       <c r="J8">
-        <v>339</v>
+        <v>340</v>
       </c>
     </row>
     <row r="9" spans="1:10">
@@ -17784,7 +17787,7 @@
         <v>455</v>
       </c>
       <c r="J10">
-        <v>303</v>
+        <v>305</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -17816,7 +17819,7 @@
         <v>1354</v>
       </c>
       <c r="J11">
-        <v>867</v>
+        <v>872</v>
       </c>
     </row>
   </sheetData>
@@ -18088,7 +18091,7 @@
         <v>250</v>
       </c>
       <c r="J8">
-        <v>185</v>
+        <v>188</v>
       </c>
     </row>
     <row r="9" spans="1:10">
@@ -18152,7 +18155,7 @@
         <v>417</v>
       </c>
       <c r="J10">
-        <v>243</v>
+        <v>244</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -18184,7 +18187,7 @@
         <v>903</v>
       </c>
       <c r="J11">
-        <v>566</v>
+        <v>570</v>
       </c>
     </row>
   </sheetData>
@@ -18273,7 +18276,7 @@
         <v>237</v>
       </c>
       <c r="J2">
-        <v>113</v>
+        <v>114</v>
       </c>
     </row>
     <row r="3" spans="1:10">
@@ -18369,7 +18372,7 @@
         <v>229</v>
       </c>
       <c r="J5">
-        <v>109</v>
+        <v>110</v>
       </c>
     </row>
     <row r="6" spans="1:10">
@@ -18433,7 +18436,7 @@
         <v>23</v>
       </c>
       <c r="J7">
-        <v>19</v>
+        <v>20</v>
       </c>
     </row>
     <row r="8" spans="1:10">
@@ -18465,7 +18468,7 @@
         <v>754</v>
       </c>
       <c r="J8">
-        <v>435</v>
+        <v>437</v>
       </c>
     </row>
     <row r="9" spans="1:10">
@@ -18497,7 +18500,7 @@
         <v>233</v>
       </c>
       <c r="J9">
-        <v>166</v>
+        <v>167</v>
       </c>
     </row>
     <row r="10" spans="1:10">
@@ -18529,7 +18532,7 @@
         <v>911</v>
       </c>
       <c r="J10">
-        <v>550</v>
+        <v>551</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -18561,7 +18564,7 @@
         <v>2636</v>
       </c>
       <c r="J11">
-        <v>1554</v>
+        <v>1561</v>
       </c>
     </row>
   </sheetData>
@@ -19032,7 +19035,7 @@
         <v>177</v>
       </c>
       <c r="J3">
-        <v>103</v>
+        <v>105</v>
       </c>
     </row>
     <row r="4" spans="1:10">
@@ -19192,7 +19195,7 @@
         <v>363</v>
       </c>
       <c r="J8">
-        <v>284</v>
+        <v>285</v>
       </c>
     </row>
     <row r="9" spans="1:10">
@@ -19256,7 +19259,7 @@
         <v>828</v>
       </c>
       <c r="J10">
-        <v>438</v>
+        <v>440</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -19288,7 +19291,7 @@
         <v>2045</v>
       </c>
       <c r="J11">
-        <v>1116</v>
+        <v>1121</v>
       </c>
     </row>
   </sheetData>
@@ -19557,7 +19560,7 @@
         <v>98</v>
       </c>
       <c r="J8">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="9" spans="1:10">
@@ -19621,7 +19624,7 @@
         <v>630</v>
       </c>
       <c r="J10">
-        <v>313</v>
+        <v>315</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -19653,7 +19656,7 @@
         <v>960</v>
       </c>
       <c r="J11">
-        <v>565</v>
+        <v>566</v>
       </c>
     </row>
   </sheetData>
@@ -19983,7 +19986,7 @@
         <v>124</v>
       </c>
       <c r="J10">
-        <v>89</v>
+        <v>90</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -20015,7 +20018,7 @@
         <v>271</v>
       </c>
       <c r="J11">
-        <v>185</v>
+        <v>186</v>
       </c>
     </row>
   </sheetData>
@@ -20481,7 +20484,7 @@
         <v>41</v>
       </c>
       <c r="J2">
-        <v>15</v>
+        <v>16</v>
       </c>
     </row>
     <row r="3" spans="1:10">
@@ -20577,7 +20580,7 @@
         <v>64</v>
       </c>
       <c r="J5">
-        <v>50</v>
+        <v>51</v>
       </c>
     </row>
     <row r="6" spans="1:10">
@@ -20667,7 +20670,7 @@
         <v>122</v>
       </c>
       <c r="J8">
-        <v>133</v>
+        <v>135</v>
       </c>
     </row>
     <row r="9" spans="1:10">
@@ -20763,7 +20766,7 @@
         <v>721</v>
       </c>
       <c r="J11">
-        <v>453</v>
+        <v>457</v>
       </c>
     </row>
   </sheetData>
@@ -21087,7 +21090,7 @@
         <v>280</v>
       </c>
       <c r="J10">
-        <v>144</v>
+        <v>145</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -21119,7 +21122,7 @@
         <v>436</v>
       </c>
       <c r="J11">
-        <v>280</v>
+        <v>281</v>
       </c>
     </row>
   </sheetData>
@@ -21455,7 +21458,7 @@
         <v>216</v>
       </c>
       <c r="J10">
-        <v>120</v>
+        <v>123</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -21487,7 +21490,7 @@
         <v>436</v>
       </c>
       <c r="J11">
-        <v>255</v>
+        <v>258</v>
       </c>
     </row>
   </sheetData>
@@ -21765,7 +21768,7 @@
         <v>297</v>
       </c>
       <c r="J8">
-        <v>289</v>
+        <v>292</v>
       </c>
     </row>
     <row r="9" spans="1:10">
@@ -21829,7 +21832,7 @@
         <v>670</v>
       </c>
       <c r="J10">
-        <v>361</v>
+        <v>364</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -21861,7 +21864,7 @@
         <v>1337</v>
       </c>
       <c r="J11">
-        <v>892</v>
+        <v>898</v>
       </c>
     </row>
   </sheetData>
@@ -22142,7 +22145,7 @@
         <v>125</v>
       </c>
       <c r="J8">
-        <v>85</v>
+        <v>86</v>
       </c>
     </row>
     <row r="9" spans="1:10">
@@ -22206,7 +22209,7 @@
         <v>492</v>
       </c>
       <c r="J10">
-        <v>328</v>
+        <v>332</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -22238,7 +22241,7 @@
         <v>917</v>
       </c>
       <c r="J11">
-        <v>579</v>
+        <v>584</v>
       </c>
     </row>
   </sheetData>
@@ -22492,7 +22495,7 @@
         <v>89</v>
       </c>
       <c r="J8">
-        <v>65</v>
+        <v>66</v>
       </c>
     </row>
     <row r="9" spans="1:10">
@@ -22524,7 +22527,7 @@
         <v>36</v>
       </c>
       <c r="J9">
-        <v>21</v>
+        <v>22</v>
       </c>
     </row>
     <row r="10" spans="1:10">
@@ -22588,7 +22591,7 @@
         <v>412</v>
       </c>
       <c r="J11">
-        <v>235</v>
+        <v>237</v>
       </c>
     </row>
   </sheetData>
@@ -22866,7 +22869,7 @@
         <v>196</v>
       </c>
       <c r="J8">
-        <v>125</v>
+        <v>128</v>
       </c>
     </row>
     <row r="9" spans="1:10">
@@ -22930,7 +22933,7 @@
         <v>239</v>
       </c>
       <c r="J10">
-        <v>141</v>
+        <v>142</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -22962,7 +22965,7 @@
         <v>695</v>
       </c>
       <c r="J11">
-        <v>440</v>
+        <v>444</v>
       </c>
     </row>
   </sheetData>
@@ -23147,7 +23150,7 @@
         <v>59</v>
       </c>
       <c r="J5">
-        <v>27</v>
+        <v>28</v>
       </c>
     </row>
     <row r="6" spans="1:10">
@@ -23295,7 +23298,7 @@
         <v>277</v>
       </c>
       <c r="J10">
-        <v>182</v>
+        <v>184</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -23327,7 +23330,7 @@
         <v>500</v>
       </c>
       <c r="J11">
-        <v>354</v>
+        <v>357</v>
       </c>
     </row>
   </sheetData>
@@ -23448,7 +23451,7 @@
         <v>35</v>
       </c>
       <c r="J3">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="4" spans="1:10">
@@ -23669,7 +23672,7 @@
         <v>189</v>
       </c>
       <c r="J10">
-        <v>140</v>
+        <v>143</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -23701,7 +23704,7 @@
         <v>429</v>
       </c>
       <c r="J11">
-        <v>284</v>
+        <v>288</v>
       </c>
     </row>
   </sheetData>
@@ -24408,7 +24411,7 @@
         <v>216</v>
       </c>
       <c r="J10">
-        <v>112</v>
+        <v>113</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -24440,7 +24443,7 @@
         <v>396</v>
       </c>
       <c r="J11">
-        <v>226</v>
+        <v>227</v>
       </c>
     </row>
   </sheetData>
@@ -24619,7 +24622,7 @@
         <v>82</v>
       </c>
       <c r="J5">
-        <v>73</v>
+        <v>74</v>
       </c>
     </row>
     <row r="6" spans="1:10">
@@ -24709,7 +24712,7 @@
         <v>167</v>
       </c>
       <c r="J8">
-        <v>122</v>
+        <v>123</v>
       </c>
     </row>
     <row r="9" spans="1:10">
@@ -24773,7 +24776,7 @@
         <v>784</v>
       </c>
       <c r="J10">
-        <v>499</v>
+        <v>502</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -24805,7 +24808,7 @@
         <v>1258</v>
       </c>
       <c r="J11">
-        <v>780</v>
+        <v>785</v>
       </c>
     </row>
   </sheetData>
@@ -24894,7 +24897,7 @@
         <v>79</v>
       </c>
       <c r="J2">
-        <v>43</v>
+        <v>44</v>
       </c>
     </row>
     <row r="3" spans="1:10">
@@ -25150,7 +25153,7 @@
         <v>381</v>
       </c>
       <c r="J10">
-        <v>210</v>
+        <v>211</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -25182,7 +25185,7 @@
         <v>868</v>
       </c>
       <c r="J11">
-        <v>494</v>
+        <v>496</v>
       </c>
     </row>
   </sheetData>
@@ -25479,7 +25482,7 @@
         <v>576</v>
       </c>
       <c r="J10">
-        <v>310</v>
+        <v>311</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -25511,7 +25514,7 @@
         <v>628</v>
       </c>
       <c r="J11">
-        <v>335</v>
+        <v>336</v>
       </c>
     </row>
   </sheetData>
@@ -25856,7 +25859,7 @@
         <v>130</v>
       </c>
       <c r="J10">
-        <v>86</v>
+        <v>87</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -25888,7 +25891,7 @@
         <v>462</v>
       </c>
       <c r="J11">
-        <v>309</v>
+        <v>310</v>
       </c>
     </row>
   </sheetData>
@@ -26496,7 +26499,7 @@
         <v>198</v>
       </c>
       <c r="J8">
-        <v>159</v>
+        <v>160</v>
       </c>
     </row>
     <row r="9" spans="1:10">
@@ -26560,7 +26563,7 @@
         <v>1118</v>
       </c>
       <c r="J10">
-        <v>606</v>
+        <v>608</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -26592,7 +26595,7 @@
         <v>1797</v>
       </c>
       <c r="J11">
-        <v>1029</v>
+        <v>1032</v>
       </c>
     </row>
   </sheetData>
@@ -26928,7 +26931,7 @@
         <v>371</v>
       </c>
       <c r="J10">
-        <v>162</v>
+        <v>165</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -26960,7 +26963,7 @@
         <v>718</v>
       </c>
       <c r="J11">
-        <v>360</v>
+        <v>363</v>
       </c>
     </row>
   </sheetData>
@@ -27275,7 +27278,7 @@
         <v>462</v>
       </c>
       <c r="J10">
-        <v>251</v>
+        <v>252</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -27307,7 +27310,7 @@
         <v>715</v>
       </c>
       <c r="J11">
-        <v>439</v>
+        <v>440</v>
       </c>
     </row>
   </sheetData>
@@ -27590,7 +27593,7 @@
         <v>52</v>
       </c>
       <c r="J9">
-        <v>38</v>
+        <v>39</v>
       </c>
     </row>
     <row r="10" spans="1:10">
@@ -27622,7 +27625,7 @@
         <v>376</v>
       </c>
       <c r="J10">
-        <v>268</v>
+        <v>271</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -27654,7 +27657,7 @@
         <v>595</v>
       </c>
       <c r="J11">
-        <v>434</v>
+        <v>438</v>
       </c>
     </row>
   </sheetData>
@@ -27839,7 +27842,7 @@
         <v>48</v>
       </c>
       <c r="J5">
-        <v>26</v>
+        <v>27</v>
       </c>
     </row>
     <row r="6" spans="1:10">
@@ -27935,7 +27938,7 @@
         <v>141</v>
       </c>
       <c r="J8">
-        <v>113</v>
+        <v>114</v>
       </c>
     </row>
     <row r="9" spans="1:10">
@@ -28031,7 +28034,7 @@
         <v>519</v>
       </c>
       <c r="J11">
-        <v>316</v>
+        <v>318</v>
       </c>
     </row>
   </sheetData>
@@ -28659,7 +28662,7 @@
         <v>136</v>
       </c>
       <c r="J8">
-        <v>107</v>
+        <v>108</v>
       </c>
     </row>
     <row r="9" spans="1:10">
@@ -28723,7 +28726,7 @@
         <v>542</v>
       </c>
       <c r="J10">
-        <v>303</v>
+        <v>304</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -28755,7 +28758,7 @@
         <v>948</v>
       </c>
       <c r="J11">
-        <v>541</v>
+        <v>543</v>
       </c>
     </row>
   </sheetData>
@@ -28940,7 +28943,7 @@
         <v>27</v>
       </c>
       <c r="J5">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="6" spans="1:10">
@@ -29062,7 +29065,7 @@
         <v>35</v>
       </c>
       <c r="J9">
-        <v>48</v>
+        <v>49</v>
       </c>
     </row>
     <row r="10" spans="1:10">
@@ -29126,7 +29129,7 @@
         <v>437</v>
       </c>
       <c r="J11">
-        <v>322</v>
+        <v>324</v>
       </c>
     </row>
   </sheetData>
@@ -29311,7 +29314,7 @@
         <v>131</v>
       </c>
       <c r="J5">
-        <v>81</v>
+        <v>82</v>
       </c>
     </row>
     <row r="6" spans="1:10">
@@ -29404,7 +29407,7 @@
         <v>216</v>
       </c>
       <c r="J8">
-        <v>198</v>
+        <v>200</v>
       </c>
     </row>
     <row r="9" spans="1:10">
@@ -29436,7 +29439,7 @@
         <v>107</v>
       </c>
       <c r="J9">
-        <v>59</v>
+        <v>60</v>
       </c>
     </row>
     <row r="10" spans="1:10">
@@ -29468,7 +29471,7 @@
         <v>1222</v>
       </c>
       <c r="J10">
-        <v>685</v>
+        <v>687</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -29500,7 +29503,7 @@
         <v>1879</v>
       </c>
       <c r="J11">
-        <v>1170</v>
+        <v>1176</v>
       </c>
     </row>
   </sheetData>
@@ -29842,7 +29845,7 @@
         <v>440</v>
       </c>
       <c r="J10">
-        <v>265</v>
+        <v>266</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -29874,7 +29877,7 @@
         <v>761</v>
       </c>
       <c r="J11">
-        <v>502</v>
+        <v>503</v>
       </c>
     </row>
   </sheetData>
@@ -29963,7 +29966,7 @@
         <v>128</v>
       </c>
       <c r="J2">
-        <v>65</v>
+        <v>67</v>
       </c>
     </row>
     <row r="3" spans="1:10">
@@ -29995,7 +29998,7 @@
         <v>158</v>
       </c>
       <c r="J3">
-        <v>85</v>
+        <v>86</v>
       </c>
     </row>
     <row r="4" spans="1:10">
@@ -30059,7 +30062,7 @@
         <v>120</v>
       </c>
       <c r="J5">
-        <v>81</v>
+        <v>82</v>
       </c>
     </row>
     <row r="6" spans="1:10">
@@ -30187,7 +30190,7 @@
         <v>118</v>
       </c>
       <c r="J9">
-        <v>57</v>
+        <v>58</v>
       </c>
     </row>
     <row r="10" spans="1:10">
@@ -30219,7 +30222,7 @@
         <v>527</v>
       </c>
       <c r="J10">
-        <v>326</v>
+        <v>327</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -30251,7 +30254,7 @@
         <v>1488</v>
       </c>
       <c r="J11">
-        <v>941</v>
+        <v>947</v>
       </c>
     </row>
   </sheetData>
@@ -30554,7 +30557,7 @@
         <v>152</v>
       </c>
       <c r="J10">
-        <v>81</v>
+        <v>82</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -30586,7 +30589,7 @@
         <v>248</v>
       </c>
       <c r="J11">
-        <v>173</v>
+        <v>174</v>
       </c>
     </row>
   </sheetData>
@@ -30895,7 +30898,7 @@
         <v>502</v>
       </c>
       <c r="J10">
-        <v>314</v>
+        <v>317</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -30927,7 +30930,7 @@
         <v>677</v>
       </c>
       <c r="J11">
-        <v>420</v>
+        <v>423</v>
       </c>
     </row>
   </sheetData>
@@ -31166,7 +31169,7 @@
         <v>20</v>
       </c>
       <c r="J8">
-        <v>24</v>
+        <v>25</v>
       </c>
     </row>
     <row r="9" spans="1:10">
@@ -31262,7 +31265,7 @@
         <v>237</v>
       </c>
       <c r="J11">
-        <v>175</v>
+        <v>176</v>
       </c>
     </row>
   </sheetData>
@@ -31592,7 +31595,7 @@
         <v>124</v>
       </c>
       <c r="J10">
-        <v>77</v>
+        <v>79</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -31624,7 +31627,7 @@
         <v>335</v>
       </c>
       <c r="J11">
-        <v>260</v>
+        <v>262</v>
       </c>
     </row>
   </sheetData>
@@ -31969,7 +31972,7 @@
         <v>389</v>
       </c>
       <c r="J10">
-        <v>257</v>
+        <v>259</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -32001,7 +32004,7 @@
         <v>886</v>
       </c>
       <c r="J11">
-        <v>592</v>
+        <v>594</v>
       </c>
     </row>
   </sheetData>
@@ -32090,7 +32093,7 @@
         <v>70</v>
       </c>
       <c r="J2">
-        <v>43</v>
+        <v>44</v>
       </c>
     </row>
     <row r="3" spans="1:10">
@@ -32122,7 +32125,7 @@
         <v>89</v>
       </c>
       <c r="J3">
-        <v>47</v>
+        <v>48</v>
       </c>
     </row>
     <row r="4" spans="1:10">
@@ -32340,7 +32343,7 @@
         <v>670</v>
       </c>
       <c r="J10">
-        <v>323</v>
+        <v>327</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -32372,7 +32375,7 @@
         <v>1368</v>
       </c>
       <c r="J11">
-        <v>844</v>
+        <v>850</v>
       </c>
     </row>
   </sheetData>
@@ -32647,7 +32650,7 @@
         <v>338</v>
       </c>
       <c r="J8">
-        <v>262</v>
+        <v>265</v>
       </c>
     </row>
     <row r="9" spans="1:10">
@@ -32679,7 +32682,7 @@
         <v>169</v>
       </c>
       <c r="J9">
-        <v>84</v>
+        <v>86</v>
       </c>
     </row>
     <row r="10" spans="1:10">
@@ -32711,7 +32714,7 @@
         <v>1773</v>
       </c>
       <c r="J10">
-        <v>1040</v>
+        <v>1045</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -32743,7 +32746,7 @@
         <v>2622</v>
       </c>
       <c r="J11">
-        <v>1553</v>
+        <v>1563</v>
       </c>
     </row>
   </sheetData>
@@ -33009,7 +33012,7 @@
         <v>90</v>
       </c>
       <c r="J8">
-        <v>65</v>
+        <v>66</v>
       </c>
     </row>
     <row r="9" spans="1:10">
@@ -33073,7 +33076,7 @@
         <v>148</v>
       </c>
       <c r="J10">
-        <v>88</v>
+        <v>89</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -33105,7 +33108,7 @@
         <v>340</v>
       </c>
       <c r="J11">
-        <v>205</v>
+        <v>207</v>
       </c>
     </row>
   </sheetData>
@@ -33347,7 +33350,7 @@
         <v>36</v>
       </c>
       <c r="J8">
-        <v>28</v>
+        <v>29</v>
       </c>
     </row>
     <row r="9" spans="1:10">
@@ -33443,7 +33446,7 @@
         <v>337</v>
       </c>
       <c r="J11">
-        <v>158</v>
+        <v>159</v>
       </c>
     </row>
   </sheetData>
@@ -33779,7 +33782,7 @@
         <v>606</v>
       </c>
       <c r="J10">
-        <v>310</v>
+        <v>312</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -33811,7 +33814,7 @@
         <v>1187</v>
       </c>
       <c r="J11">
-        <v>641</v>
+        <v>643</v>
       </c>
     </row>
   </sheetData>
@@ -34022,7 +34025,7 @@
         <v>15</v>
       </c>
       <c r="J6">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="7" spans="1:10">
@@ -34118,7 +34121,7 @@
         <v>153</v>
       </c>
       <c r="J9">
-        <v>58</v>
+        <v>59</v>
       </c>
     </row>
   </sheetData>
@@ -34442,7 +34445,7 @@
         <v>313</v>
       </c>
       <c r="J10">
-        <v>157</v>
+        <v>159</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -34474,7 +34477,7 @@
         <v>494</v>
       </c>
       <c r="J11">
-        <v>260</v>
+        <v>262</v>
       </c>
     </row>
   </sheetData>
@@ -34748,7 +34751,7 @@
         <v>107</v>
       </c>
       <c r="J9">
-        <v>80</v>
+        <v>81</v>
       </c>
     </row>
     <row r="10" spans="1:10">
@@ -34780,7 +34783,7 @@
         <v>155</v>
       </c>
       <c r="J10">
-        <v>106</v>
+        <v>107</v>
       </c>
     </row>
   </sheetData>
@@ -35081,7 +35084,7 @@
         <v>28</v>
       </c>
       <c r="J9">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="10" spans="1:10">
@@ -35113,7 +35116,7 @@
         <v>211</v>
       </c>
       <c r="J10">
-        <v>147</v>
+        <v>148</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -35145,7 +35148,7 @@
         <v>406</v>
       </c>
       <c r="J11">
-        <v>290</v>
+        <v>292</v>
       </c>
     </row>
   </sheetData>
@@ -35764,7 +35767,7 @@
         <v>187</v>
       </c>
       <c r="J9">
-        <v>120</v>
+        <v>121</v>
       </c>
     </row>
     <row r="10" spans="1:10">
@@ -35796,7 +35799,7 @@
         <v>258</v>
       </c>
       <c r="J10">
-        <v>156</v>
+        <v>157</v>
       </c>
     </row>
   </sheetData>
@@ -36217,7 +36220,7 @@
         <v>89</v>
       </c>
       <c r="J2">
-        <v>53</v>
+        <v>54</v>
       </c>
     </row>
     <row r="3" spans="1:10">
@@ -36409,7 +36412,7 @@
         <v>291</v>
       </c>
       <c r="J8">
-        <v>197</v>
+        <v>199</v>
       </c>
     </row>
     <row r="9" spans="1:10">
@@ -36473,7 +36476,7 @@
         <v>905</v>
       </c>
       <c r="J10">
-        <v>474</v>
+        <v>479</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -36505,7 +36508,7 @@
         <v>1669</v>
       </c>
       <c r="J11">
-        <v>948</v>
+        <v>956</v>
       </c>
     </row>
   </sheetData>
@@ -36844,7 +36847,7 @@
         <v>157</v>
       </c>
       <c r="J10">
-        <v>98</v>
+        <v>99</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -36876,7 +36879,7 @@
         <v>337</v>
       </c>
       <c r="J11">
-        <v>237</v>
+        <v>238</v>
       </c>
     </row>
   </sheetData>
@@ -37497,7 +37500,7 @@
         <v>8</v>
       </c>
       <c r="J9">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="10" spans="1:10">
@@ -37529,7 +37532,7 @@
         <v>116</v>
       </c>
       <c r="J10">
-        <v>62</v>
+        <v>65</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -37561,7 +37564,7 @@
         <v>236</v>
       </c>
       <c r="J11">
-        <v>159</v>
+        <v>163</v>
       </c>
     </row>
   </sheetData>
@@ -37650,7 +37653,7 @@
         <v>31</v>
       </c>
       <c r="J2">
-        <v>12</v>
+        <v>13</v>
       </c>
     </row>
     <row r="3" spans="1:10">
@@ -37812,7 +37815,7 @@
         <v>160</v>
       </c>
       <c r="J8">
-        <v>66</v>
+        <v>67</v>
       </c>
     </row>
     <row r="9" spans="1:10">
@@ -37876,7 +37879,7 @@
         <v>717</v>
       </c>
       <c r="J10">
-        <v>332</v>
+        <v>333</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -37908,7 +37911,7 @@
         <v>1066</v>
       </c>
       <c r="J11">
-        <v>499</v>
+        <v>502</v>
       </c>
     </row>
   </sheetData>
@@ -38217,7 +38220,7 @@
         <v>260</v>
       </c>
       <c r="J10">
-        <v>128</v>
+        <v>130</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -38249,7 +38252,7 @@
         <v>393</v>
       </c>
       <c r="J11">
-        <v>181</v>
+        <v>183</v>
       </c>
     </row>
   </sheetData>
@@ -38546,7 +38549,7 @@
         <v>135</v>
       </c>
       <c r="J10">
-        <v>71</v>
+        <v>72</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -38578,7 +38581,7 @@
         <v>219</v>
       </c>
       <c r="J11">
-        <v>128</v>
+        <v>129</v>
       </c>
     </row>
   </sheetData>
@@ -38811,7 +38814,7 @@
         <v>32</v>
       </c>
       <c r="J8">
-        <v>21</v>
+        <v>22</v>
       </c>
     </row>
     <row r="9" spans="1:10">
@@ -38907,7 +38910,7 @@
         <v>307</v>
       </c>
       <c r="J11">
-        <v>158</v>
+        <v>159</v>
       </c>
     </row>
   </sheetData>
@@ -39515,7 +39518,7 @@
         <v>174</v>
       </c>
       <c r="J10">
-        <v>95</v>
+        <v>97</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -39547,7 +39550,7 @@
         <v>235</v>
       </c>
       <c r="J11">
-        <v>139</v>
+        <v>141</v>
       </c>
     </row>
   </sheetData>
@@ -39815,7 +39818,7 @@
         <v>155</v>
       </c>
       <c r="J9">
-        <v>94</v>
+        <v>95</v>
       </c>
     </row>
     <row r="10" spans="1:10">
@@ -39847,7 +39850,7 @@
         <v>191</v>
       </c>
       <c r="J10">
-        <v>107</v>
+        <v>108</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add data for 2023-07-27
</commit_message>
<xml_diff>
--- a/output/index-crime-full-year.xlsx
+++ b/output/index-crime-full-year.xlsx
@@ -895,7 +895,7 @@
         <v>7278</v>
       </c>
       <c r="J2">
-        <v>4239</v>
+        <v>4263</v>
       </c>
     </row>
     <row r="3" spans="1:10">
@@ -927,7 +927,7 @@
         <v>7486</v>
       </c>
       <c r="J3">
-        <v>4458</v>
+        <v>4472</v>
       </c>
     </row>
     <row r="4" spans="1:10">
@@ -959,7 +959,7 @@
         <v>422</v>
       </c>
       <c r="J4">
-        <v>281</v>
+        <v>282</v>
       </c>
     </row>
     <row r="5" spans="1:10">
@@ -991,7 +991,7 @@
         <v>7592</v>
       </c>
       <c r="J5">
-        <v>4102</v>
+        <v>4122</v>
       </c>
     </row>
     <row r="6" spans="1:10">
@@ -1023,7 +1023,7 @@
         <v>1767</v>
       </c>
       <c r="J6">
-        <v>994</v>
+        <v>999</v>
       </c>
     </row>
     <row r="7" spans="1:10">
@@ -1087,7 +1087,7 @@
         <v>21446</v>
       </c>
       <c r="J8">
-        <v>16727</v>
+        <v>16809</v>
       </c>
     </row>
     <row r="9" spans="1:10">
@@ -1119,7 +1119,7 @@
         <v>8965</v>
       </c>
       <c r="J9">
-        <v>5326</v>
+        <v>5345</v>
       </c>
     </row>
     <row r="10" spans="1:10">
@@ -1151,7 +1151,7 @@
         <v>54808</v>
       </c>
       <c r="J10">
-        <v>30624</v>
+        <v>30803</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -1183,7 +1183,7 @@
         <v>110482</v>
       </c>
       <c r="J11">
-        <v>67107</v>
+        <v>67451</v>
       </c>
     </row>
   </sheetData>
@@ -1440,7 +1440,7 @@
         <v>227</v>
       </c>
       <c r="J8">
-        <v>223</v>
+        <v>224</v>
       </c>
     </row>
     <row r="9" spans="1:10">
@@ -1504,7 +1504,7 @@
         <v>648</v>
       </c>
       <c r="J10">
-        <v>413</v>
+        <v>419</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -1536,7 +1536,7 @@
         <v>1153</v>
       </c>
       <c r="J11">
-        <v>804</v>
+        <v>811</v>
       </c>
     </row>
   </sheetData>
@@ -2091,7 +2091,7 @@
         <v>373</v>
       </c>
       <c r="J8">
-        <v>291</v>
+        <v>294</v>
       </c>
     </row>
     <row r="9" spans="1:10">
@@ -2155,7 +2155,7 @@
         <v>820</v>
       </c>
       <c r="J10">
-        <v>521</v>
+        <v>523</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -2187,7 +2187,7 @@
         <v>1712</v>
       </c>
       <c r="J11">
-        <v>1136</v>
+        <v>1141</v>
       </c>
     </row>
   </sheetData>
@@ -2462,7 +2462,7 @@
         <v>188</v>
       </c>
       <c r="J8">
-        <v>152</v>
+        <v>153</v>
       </c>
     </row>
     <row r="9" spans="1:10">
@@ -2558,7 +2558,7 @@
         <v>1228</v>
       </c>
       <c r="J11">
-        <v>743</v>
+        <v>744</v>
       </c>
     </row>
   </sheetData>
@@ -2647,7 +2647,7 @@
         <v>220</v>
       </c>
       <c r="J2">
-        <v>124</v>
+        <v>125</v>
       </c>
     </row>
     <row r="3" spans="1:10">
@@ -2743,7 +2743,7 @@
         <v>191</v>
       </c>
       <c r="J5">
-        <v>91</v>
+        <v>92</v>
       </c>
     </row>
     <row r="6" spans="1:10">
@@ -2775,7 +2775,7 @@
         <v>42</v>
       </c>
       <c r="J6">
-        <v>26</v>
+        <v>27</v>
       </c>
     </row>
     <row r="7" spans="1:10">
@@ -2839,7 +2839,7 @@
         <v>700</v>
       </c>
       <c r="J8">
-        <v>492</v>
+        <v>494</v>
       </c>
     </row>
     <row r="9" spans="1:10">
@@ -2903,7 +2903,7 @@
         <v>820</v>
       </c>
       <c r="J10">
-        <v>450</v>
+        <v>454</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -2935,7 +2935,7 @@
         <v>2472</v>
       </c>
       <c r="J11">
-        <v>1475</v>
+        <v>1484</v>
       </c>
     </row>
   </sheetData>
@@ -3056,7 +3056,7 @@
         <v>56</v>
       </c>
       <c r="J3">
-        <v>26</v>
+        <v>27</v>
       </c>
     </row>
     <row r="4" spans="1:10">
@@ -3117,7 +3117,7 @@
         <v>129</v>
       </c>
       <c r="J5">
-        <v>80</v>
+        <v>81</v>
       </c>
     </row>
     <row r="6" spans="1:10">
@@ -3277,7 +3277,7 @@
         <v>913</v>
       </c>
       <c r="J10">
-        <v>623</v>
+        <v>626</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -3309,7 +3309,7 @@
         <v>1600</v>
       </c>
       <c r="J11">
-        <v>1127</v>
+        <v>1132</v>
       </c>
     </row>
   </sheetData>
@@ -3584,7 +3584,7 @@
         <v>57</v>
       </c>
       <c r="J8">
-        <v>54</v>
+        <v>56</v>
       </c>
     </row>
     <row r="9" spans="1:10">
@@ -3680,7 +3680,7 @@
         <v>260</v>
       </c>
       <c r="J11">
-        <v>170</v>
+        <v>172</v>
       </c>
     </row>
   </sheetData>
@@ -4242,7 +4242,7 @@
         <v>268</v>
       </c>
       <c r="J5">
-        <v>161</v>
+        <v>162</v>
       </c>
     </row>
     <row r="6" spans="1:10">
@@ -4338,7 +4338,7 @@
         <v>794</v>
       </c>
       <c r="J8">
-        <v>617</v>
+        <v>622</v>
       </c>
     </row>
     <row r="9" spans="1:10">
@@ -4370,7 +4370,7 @@
         <v>433</v>
       </c>
       <c r="J9">
-        <v>214</v>
+        <v>215</v>
       </c>
     </row>
     <row r="10" spans="1:10">
@@ -4402,7 +4402,7 @@
         <v>1302</v>
       </c>
       <c r="J10">
-        <v>738</v>
+        <v>740</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -4434,7 +4434,7 @@
         <v>3950</v>
       </c>
       <c r="J11">
-        <v>2407</v>
+        <v>2416</v>
       </c>
     </row>
   </sheetData>
@@ -4697,7 +4697,7 @@
         <v>131</v>
       </c>
       <c r="J8">
-        <v>150</v>
+        <v>151</v>
       </c>
     </row>
     <row r="9" spans="1:10">
@@ -4761,7 +4761,7 @@
         <v>921</v>
       </c>
       <c r="J10">
-        <v>402</v>
+        <v>404</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -4793,7 +4793,7 @@
         <v>1318</v>
       </c>
       <c r="J11">
-        <v>695</v>
+        <v>698</v>
       </c>
     </row>
   </sheetData>
@@ -4914,7 +4914,7 @@
         <v>280</v>
       </c>
       <c r="J3">
-        <v>126</v>
+        <v>125</v>
       </c>
     </row>
     <row r="4" spans="1:10">
@@ -5010,7 +5010,7 @@
         <v>58</v>
       </c>
       <c r="J6">
-        <v>30</v>
+        <v>31</v>
       </c>
     </row>
     <row r="7" spans="1:10">
@@ -5074,7 +5074,7 @@
         <v>653</v>
       </c>
       <c r="J8">
-        <v>551</v>
+        <v>553</v>
       </c>
     </row>
     <row r="9" spans="1:10">
@@ -5106,7 +5106,7 @@
         <v>428</v>
       </c>
       <c r="J9">
-        <v>293</v>
+        <v>294</v>
       </c>
     </row>
     <row r="10" spans="1:10">
@@ -5138,7 +5138,7 @@
         <v>1089</v>
       </c>
       <c r="J10">
-        <v>690</v>
+        <v>692</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -5170,7 +5170,7 @@
         <v>2956</v>
       </c>
       <c r="J11">
-        <v>1950</v>
+        <v>1955</v>
       </c>
     </row>
   </sheetData>
@@ -5259,7 +5259,7 @@
         <v>917</v>
       </c>
       <c r="J2">
-        <v>584</v>
+        <v>587</v>
       </c>
     </row>
     <row r="3" spans="1:10">
@@ -5291,7 +5291,7 @@
         <v>155</v>
       </c>
       <c r="J3">
-        <v>107</v>
+        <v>108</v>
       </c>
     </row>
     <row r="4" spans="1:10">
@@ -5323,7 +5323,7 @@
         <v>436</v>
       </c>
       <c r="J4">
-        <v>258</v>
+        <v>261</v>
       </c>
     </row>
     <row r="5" spans="1:10">
@@ -5355,7 +5355,7 @@
         <v>247</v>
       </c>
       <c r="J5">
-        <v>172</v>
+        <v>174</v>
       </c>
     </row>
     <row r="6" spans="1:10">
@@ -5387,7 +5387,7 @@
         <v>793</v>
       </c>
       <c r="J6">
-        <v>574</v>
+        <v>576</v>
       </c>
     </row>
     <row r="7" spans="1:10">
@@ -5419,7 +5419,7 @@
         <v>2686</v>
       </c>
       <c r="J7">
-        <v>1688</v>
+        <v>1697</v>
       </c>
     </row>
     <row r="8" spans="1:10">
@@ -5451,7 +5451,7 @@
         <v>4743</v>
       </c>
       <c r="J8">
-        <v>2851</v>
+        <v>2857</v>
       </c>
     </row>
     <row r="9" spans="1:10">
@@ -5483,7 +5483,7 @@
         <v>519</v>
       </c>
       <c r="J9">
-        <v>318</v>
+        <v>319</v>
       </c>
     </row>
     <row r="10" spans="1:10">
@@ -5515,7 +5515,7 @@
         <v>948</v>
       </c>
       <c r="J10">
-        <v>543</v>
+        <v>545</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -5547,7 +5547,7 @@
         <v>1712</v>
       </c>
       <c r="J11">
-        <v>1136</v>
+        <v>1141</v>
       </c>
     </row>
     <row r="12" spans="1:10">
@@ -5643,7 +5643,7 @@
         <v>718</v>
       </c>
       <c r="J14">
-        <v>363</v>
+        <v>364</v>
       </c>
     </row>
     <row r="15" spans="1:10">
@@ -5675,7 +5675,7 @@
         <v>886</v>
       </c>
       <c r="J15">
-        <v>594</v>
+        <v>595</v>
       </c>
     </row>
     <row r="16" spans="1:10">
@@ -5707,7 +5707,7 @@
         <v>595</v>
       </c>
       <c r="J16">
-        <v>438</v>
+        <v>439</v>
       </c>
     </row>
     <row r="17" spans="1:10">
@@ -5739,7 +5739,7 @@
         <v>175</v>
       </c>
       <c r="J17">
-        <v>87</v>
+        <v>88</v>
       </c>
     </row>
     <row r="18" spans="1:10">
@@ -5771,7 +5771,7 @@
         <v>695</v>
       </c>
       <c r="J18">
-        <v>444</v>
+        <v>445</v>
       </c>
     </row>
     <row r="19" spans="1:10">
@@ -5803,7 +5803,7 @@
         <v>2636</v>
       </c>
       <c r="J19">
-        <v>1561</v>
+        <v>1568</v>
       </c>
     </row>
     <row r="20" spans="1:10">
@@ -5835,7 +5835,7 @@
         <v>2045</v>
       </c>
       <c r="J20">
-        <v>1121</v>
+        <v>1124</v>
       </c>
     </row>
     <row r="21" spans="1:10">
@@ -5867,7 +5867,7 @@
         <v>337</v>
       </c>
       <c r="J21">
-        <v>159</v>
+        <v>160</v>
       </c>
     </row>
     <row r="22" spans="1:10">
@@ -5899,7 +5899,7 @@
         <v>418</v>
       </c>
       <c r="J22">
-        <v>310</v>
+        <v>312</v>
       </c>
     </row>
     <row r="23" spans="1:10">
@@ -5931,7 +5931,7 @@
         <v>1368</v>
       </c>
       <c r="J23">
-        <v>850</v>
+        <v>854</v>
       </c>
     </row>
     <row r="24" spans="1:10">
@@ -5963,7 +5963,7 @@
         <v>500</v>
       </c>
       <c r="J24">
-        <v>357</v>
+        <v>360</v>
       </c>
     </row>
     <row r="25" spans="1:10">
@@ -5995,7 +5995,7 @@
         <v>429</v>
       </c>
       <c r="J25">
-        <v>288</v>
+        <v>290</v>
       </c>
     </row>
     <row r="26" spans="1:10">
@@ -6059,7 +6059,7 @@
         <v>1258</v>
       </c>
       <c r="J27">
-        <v>785</v>
+        <v>793</v>
       </c>
     </row>
     <row r="28" spans="1:10">
@@ -6091,7 +6091,7 @@
         <v>99</v>
       </c>
       <c r="J28">
-        <v>37</v>
+        <v>38</v>
       </c>
     </row>
     <row r="29" spans="1:10">
@@ -6123,7 +6123,7 @@
         <v>3950</v>
       </c>
       <c r="J29">
-        <v>2407</v>
+        <v>2416</v>
       </c>
     </row>
     <row r="30" spans="1:10">
@@ -6155,7 +6155,7 @@
         <v>260</v>
       </c>
       <c r="J30">
-        <v>170</v>
+        <v>172</v>
       </c>
     </row>
     <row r="31" spans="1:10">
@@ -6187,7 +6187,7 @@
         <v>868</v>
       </c>
       <c r="J31">
-        <v>496</v>
+        <v>499</v>
       </c>
     </row>
     <row r="32" spans="1:10">
@@ -6219,7 +6219,7 @@
         <v>209</v>
       </c>
       <c r="J32">
-        <v>160</v>
+        <v>161</v>
       </c>
     </row>
     <row r="33" spans="1:10">
@@ -6251,7 +6251,7 @@
         <v>3011</v>
       </c>
       <c r="J33">
-        <v>1920</v>
+        <v>1926</v>
       </c>
     </row>
     <row r="34" spans="1:10">
@@ -6283,7 +6283,7 @@
         <v>761</v>
       </c>
       <c r="J34">
-        <v>503</v>
+        <v>506</v>
       </c>
     </row>
     <row r="35" spans="1:10">
@@ -6347,7 +6347,7 @@
         <v>1491</v>
       </c>
       <c r="J36">
-        <v>953</v>
+        <v>958</v>
       </c>
     </row>
     <row r="37" spans="1:10">
@@ -6379,7 +6379,7 @@
         <v>2547</v>
       </c>
       <c r="J37">
-        <v>1622</v>
+        <v>1631</v>
       </c>
     </row>
     <row r="38" spans="1:10">
@@ -6411,7 +6411,7 @@
         <v>191</v>
       </c>
       <c r="J38">
-        <v>108</v>
+        <v>111</v>
       </c>
     </row>
     <row r="39" spans="1:10">
@@ -6539,7 +6539,7 @@
         <v>2956</v>
       </c>
       <c r="J42">
-        <v>1950</v>
+        <v>1955</v>
       </c>
     </row>
     <row r="43" spans="1:10">
@@ -6571,7 +6571,7 @@
         <v>1153</v>
       </c>
       <c r="J43">
-        <v>804</v>
+        <v>811</v>
       </c>
     </row>
     <row r="44" spans="1:10">
@@ -6603,7 +6603,7 @@
         <v>1228</v>
       </c>
       <c r="J44">
-        <v>743</v>
+        <v>744</v>
       </c>
     </row>
     <row r="45" spans="1:10">
@@ -6667,7 +6667,7 @@
         <v>436</v>
       </c>
       <c r="J46">
-        <v>281</v>
+        <v>282</v>
       </c>
     </row>
     <row r="47" spans="1:10">
@@ -6699,7 +6699,7 @@
         <v>903</v>
       </c>
       <c r="J47">
-        <v>570</v>
+        <v>575</v>
       </c>
     </row>
     <row r="48" spans="1:10">
@@ -6731,7 +6731,7 @@
         <v>2622</v>
       </c>
       <c r="J48">
-        <v>1563</v>
+        <v>1571</v>
       </c>
     </row>
     <row r="49" spans="1:10">
@@ -6763,7 +6763,7 @@
         <v>1648</v>
       </c>
       <c r="J49">
-        <v>957</v>
+        <v>967</v>
       </c>
     </row>
     <row r="50" spans="1:10">
@@ -6795,7 +6795,7 @@
         <v>960</v>
       </c>
       <c r="J50">
-        <v>566</v>
+        <v>571</v>
       </c>
     </row>
     <row r="51" spans="1:10">
@@ -6827,7 +6827,7 @@
         <v>1337</v>
       </c>
       <c r="J51">
-        <v>898</v>
+        <v>902</v>
       </c>
     </row>
     <row r="52" spans="1:10">
@@ -6859,7 +6859,7 @@
         <v>1491</v>
       </c>
       <c r="J52">
-        <v>1068</v>
+        <v>1075</v>
       </c>
     </row>
     <row r="53" spans="1:10">
@@ -6891,7 +6891,7 @@
         <v>1600</v>
       </c>
       <c r="J53">
-        <v>1127</v>
+        <v>1132</v>
       </c>
     </row>
     <row r="54" spans="1:10">
@@ -6923,7 +6923,7 @@
         <v>3506</v>
       </c>
       <c r="J54">
-        <v>2038</v>
+        <v>2048</v>
       </c>
     </row>
     <row r="55" spans="1:10">
@@ -6955,7 +6955,7 @@
         <v>1244</v>
       </c>
       <c r="J55">
-        <v>713</v>
+        <v>719</v>
       </c>
     </row>
     <row r="56" spans="1:10">
@@ -6987,7 +6987,7 @@
         <v>628</v>
       </c>
       <c r="J56">
-        <v>336</v>
+        <v>339</v>
       </c>
     </row>
     <row r="57" spans="1:10">
@@ -7019,7 +7019,7 @@
         <v>406</v>
       </c>
       <c r="J57">
-        <v>292</v>
+        <v>293</v>
       </c>
     </row>
     <row r="58" spans="1:10">
@@ -7083,7 +7083,7 @@
         <v>271</v>
       </c>
       <c r="J59">
-        <v>186</v>
+        <v>187</v>
       </c>
     </row>
     <row r="60" spans="1:10">
@@ -7115,7 +7115,7 @@
         <v>768</v>
       </c>
       <c r="J60">
-        <v>485</v>
+        <v>489</v>
       </c>
     </row>
     <row r="61" spans="1:10">
@@ -7211,7 +7211,7 @@
         <v>2481</v>
       </c>
       <c r="J63">
-        <v>756</v>
+        <v>797</v>
       </c>
     </row>
     <row r="64" spans="1:10">
@@ -7275,7 +7275,7 @@
         <v>1515</v>
       </c>
       <c r="J65">
-        <v>1027</v>
+        <v>1033</v>
       </c>
     </row>
     <row r="66" spans="1:10">
@@ -7307,7 +7307,7 @@
         <v>715</v>
       </c>
       <c r="J66">
-        <v>440</v>
+        <v>442</v>
       </c>
     </row>
     <row r="67" spans="1:10">
@@ -7339,7 +7339,7 @@
         <v>2510</v>
       </c>
       <c r="J67">
-        <v>1570</v>
+        <v>1576</v>
       </c>
     </row>
     <row r="68" spans="1:10">
@@ -7403,7 +7403,7 @@
         <v>494</v>
       </c>
       <c r="J69">
-        <v>262</v>
+        <v>266</v>
       </c>
     </row>
     <row r="70" spans="1:10">
@@ -7435,7 +7435,7 @@
         <v>677</v>
       </c>
       <c r="J70">
-        <v>423</v>
+        <v>424</v>
       </c>
     </row>
     <row r="71" spans="1:10">
@@ -7467,7 +7467,7 @@
         <v>335</v>
       </c>
       <c r="J71">
-        <v>262</v>
+        <v>263</v>
       </c>
     </row>
     <row r="72" spans="1:10">
@@ -7563,7 +7563,7 @@
         <v>307</v>
       </c>
       <c r="J74">
-        <v>159</v>
+        <v>160</v>
       </c>
     </row>
     <row r="75" spans="1:10">
@@ -7595,7 +7595,7 @@
         <v>340</v>
       </c>
       <c r="J75">
-        <v>207</v>
+        <v>208</v>
       </c>
     </row>
     <row r="76" spans="1:10">
@@ -7627,7 +7627,7 @@
         <v>2923</v>
       </c>
       <c r="J76">
-        <v>1720</v>
+        <v>1723</v>
       </c>
     </row>
     <row r="77" spans="1:10">
@@ -7691,7 +7691,7 @@
         <v>1797</v>
       </c>
       <c r="J78">
-        <v>1032</v>
+        <v>1034</v>
       </c>
     </row>
     <row r="79" spans="1:10">
@@ -7723,7 +7723,7 @@
         <v>2472</v>
       </c>
       <c r="J79">
-        <v>1475</v>
+        <v>1484</v>
       </c>
     </row>
     <row r="80" spans="1:10">
@@ -7787,7 +7787,7 @@
         <v>219</v>
       </c>
       <c r="J81">
-        <v>129</v>
+        <v>130</v>
       </c>
     </row>
     <row r="82" spans="1:10">
@@ -7819,7 +7819,7 @@
         <v>233</v>
       </c>
       <c r="J82">
-        <v>159</v>
+        <v>160</v>
       </c>
     </row>
     <row r="83" spans="1:10">
@@ -7851,7 +7851,7 @@
         <v>1793</v>
       </c>
       <c r="J83">
-        <v>1041</v>
+        <v>1045</v>
       </c>
     </row>
     <row r="84" spans="1:10">
@@ -7883,7 +7883,7 @@
         <v>729</v>
       </c>
       <c r="J84">
-        <v>497</v>
+        <v>499</v>
       </c>
     </row>
     <row r="85" spans="1:10">
@@ -7915,7 +7915,7 @@
         <v>3848</v>
       </c>
       <c r="J85">
-        <v>2447</v>
+        <v>2458</v>
       </c>
     </row>
     <row r="86" spans="1:10">
@@ -7947,7 +7947,7 @@
         <v>1066</v>
       </c>
       <c r="J86">
-        <v>502</v>
+        <v>507</v>
       </c>
     </row>
     <row r="87" spans="1:10">
@@ -8011,7 +8011,7 @@
         <v>943</v>
       </c>
       <c r="J88">
-        <v>591</v>
+        <v>592</v>
       </c>
     </row>
     <row r="89" spans="1:10">
@@ -8043,7 +8043,7 @@
         <v>1879</v>
       </c>
       <c r="J89">
-        <v>1176</v>
+        <v>1184</v>
       </c>
     </row>
     <row r="90" spans="1:10">
@@ -8075,7 +8075,7 @@
         <v>1354</v>
       </c>
       <c r="J90">
-        <v>872</v>
+        <v>875</v>
       </c>
     </row>
     <row r="91" spans="1:10">
@@ -8107,7 +8107,7 @@
         <v>970</v>
       </c>
       <c r="J91">
-        <v>632</v>
+        <v>635</v>
       </c>
     </row>
     <row r="92" spans="1:10">
@@ -8139,7 +8139,7 @@
         <v>337</v>
       </c>
       <c r="J92">
-        <v>238</v>
+        <v>241</v>
       </c>
     </row>
     <row r="93" spans="1:10">
@@ -8171,7 +8171,7 @@
         <v>721</v>
       </c>
       <c r="J93">
-        <v>457</v>
+        <v>459</v>
       </c>
     </row>
     <row r="94" spans="1:10">
@@ -8203,7 +8203,7 @@
         <v>2663</v>
       </c>
       <c r="J94">
-        <v>1432</v>
+        <v>1441</v>
       </c>
     </row>
     <row r="95" spans="1:10">
@@ -8235,7 +8235,7 @@
         <v>1389</v>
       </c>
       <c r="J95">
-        <v>873</v>
+        <v>877</v>
       </c>
     </row>
     <row r="96" spans="1:10">
@@ -8267,7 +8267,7 @@
         <v>1669</v>
       </c>
       <c r="J96">
-        <v>956</v>
+        <v>961</v>
       </c>
     </row>
     <row r="97" spans="1:10">
@@ -8299,7 +8299,7 @@
         <v>1673</v>
       </c>
       <c r="J97">
-        <v>1005</v>
+        <v>1011</v>
       </c>
     </row>
     <row r="98" spans="1:10">
@@ -8331,7 +8331,7 @@
         <v>1318</v>
       </c>
       <c r="J98">
-        <v>695</v>
+        <v>698</v>
       </c>
     </row>
     <row r="99" spans="1:10">
@@ -8363,7 +8363,7 @@
         <v>1488</v>
       </c>
       <c r="J99">
-        <v>947</v>
+        <v>949</v>
       </c>
     </row>
     <row r="100" spans="1:10">
@@ -8427,7 +8427,7 @@
         <v>110482</v>
       </c>
       <c r="J101">
-        <v>67107</v>
+        <v>67451</v>
       </c>
     </row>
   </sheetData>
@@ -8711,7 +8711,7 @@
         <v>121</v>
       </c>
       <c r="J5">
-        <v>71</v>
+        <v>72</v>
       </c>
     </row>
     <row r="6" spans="1:10">
@@ -8795,7 +8795,7 @@
         <v>219</v>
       </c>
       <c r="J8">
-        <v>125</v>
+        <v>126</v>
       </c>
     </row>
     <row r="9" spans="1:10">
@@ -8859,7 +8859,7 @@
         <v>1135</v>
       </c>
       <c r="J10">
-        <v>653</v>
+        <v>661</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -8891,7 +8891,7 @@
         <v>1648</v>
       </c>
       <c r="J11">
-        <v>957</v>
+        <v>967</v>
       </c>
     </row>
   </sheetData>
@@ -8980,7 +8980,7 @@
         <v>327</v>
       </c>
       <c r="J2">
-        <v>171</v>
+        <v>174</v>
       </c>
     </row>
     <row r="3" spans="1:10">
@@ -9012,7 +9012,7 @@
         <v>439</v>
       </c>
       <c r="J3">
-        <v>254</v>
+        <v>255</v>
       </c>
     </row>
     <row r="4" spans="1:10">
@@ -9076,7 +9076,7 @@
         <v>381</v>
       </c>
       <c r="J5">
-        <v>171</v>
+        <v>173</v>
       </c>
     </row>
     <row r="6" spans="1:10">
@@ -9172,7 +9172,7 @@
         <v>1026</v>
       </c>
       <c r="J8">
-        <v>828</v>
+        <v>830</v>
       </c>
     </row>
     <row r="9" spans="1:10">
@@ -9204,7 +9204,7 @@
         <v>303</v>
       </c>
       <c r="J9">
-        <v>190</v>
+        <v>191</v>
       </c>
     </row>
     <row r="10" spans="1:10">
@@ -9236,7 +9236,7 @@
         <v>1271</v>
       </c>
       <c r="J10">
-        <v>756</v>
+        <v>758</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -9268,7 +9268,7 @@
         <v>3848</v>
       </c>
       <c r="J11">
-        <v>2447</v>
+        <v>2458</v>
       </c>
     </row>
   </sheetData>
@@ -9610,7 +9610,7 @@
         <v>2132</v>
       </c>
       <c r="J10">
-        <v>1238</v>
+        <v>1241</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -9642,7 +9642,7 @@
         <v>2923</v>
       </c>
       <c r="J11">
-        <v>1720</v>
+        <v>1723</v>
       </c>
     </row>
   </sheetData>
@@ -9821,7 +9821,7 @@
         <v>122</v>
       </c>
       <c r="J5">
-        <v>82</v>
+        <v>83</v>
       </c>
     </row>
     <row r="6" spans="1:10">
@@ -9914,7 +9914,7 @@
         <v>280</v>
       </c>
       <c r="J8">
-        <v>308</v>
+        <v>309</v>
       </c>
     </row>
     <row r="9" spans="1:10">
@@ -9978,7 +9978,7 @@
         <v>1034</v>
       </c>
       <c r="J10">
-        <v>502</v>
+        <v>506</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -10010,7 +10010,7 @@
         <v>1673</v>
       </c>
       <c r="J11">
-        <v>1005</v>
+        <v>1011</v>
       </c>
     </row>
   </sheetData>
@@ -10291,7 +10291,7 @@
         <v>516</v>
       </c>
       <c r="J8">
-        <v>405</v>
+        <v>409</v>
       </c>
     </row>
     <row r="9" spans="1:10">
@@ -10355,7 +10355,7 @@
         <v>895</v>
       </c>
       <c r="J10">
-        <v>486</v>
+        <v>488</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -10387,7 +10387,7 @@
         <v>2510</v>
       </c>
       <c r="J11">
-        <v>1570</v>
+        <v>1576</v>
       </c>
     </row>
   </sheetData>
@@ -10508,7 +10508,7 @@
         <v>137</v>
       </c>
       <c r="J3">
-        <v>77</v>
+        <v>78</v>
       </c>
     </row>
     <row r="4" spans="1:10">
@@ -10700,7 +10700,7 @@
         <v>86</v>
       </c>
       <c r="J9">
-        <v>54</v>
+        <v>55</v>
       </c>
     </row>
     <row r="10" spans="1:10">
@@ -10732,7 +10732,7 @@
         <v>433</v>
       </c>
       <c r="J10">
-        <v>284</v>
+        <v>286</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -10764,7 +10764,7 @@
         <v>1389</v>
       </c>
       <c r="J11">
-        <v>873</v>
+        <v>877</v>
       </c>
     </row>
   </sheetData>
@@ -11045,7 +11045,7 @@
         <v>190</v>
       </c>
       <c r="J8">
-        <v>181</v>
+        <v>182</v>
       </c>
     </row>
     <row r="9" spans="1:10">
@@ -11109,7 +11109,7 @@
         <v>271</v>
       </c>
       <c r="J10">
-        <v>150</v>
+        <v>151</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -11141,7 +11141,7 @@
         <v>729</v>
       </c>
       <c r="J11">
-        <v>497</v>
+        <v>499</v>
       </c>
     </row>
   </sheetData>
@@ -11230,7 +11230,7 @@
         <v>146</v>
       </c>
       <c r="J2">
-        <v>96</v>
+        <v>98</v>
       </c>
     </row>
     <row r="3" spans="1:10">
@@ -11454,7 +11454,7 @@
         <v>196</v>
       </c>
       <c r="J9">
-        <v>178</v>
+        <v>179</v>
       </c>
     </row>
     <row r="10" spans="1:10">
@@ -11486,7 +11486,7 @@
         <v>590</v>
       </c>
       <c r="J10">
-        <v>390</v>
+        <v>394</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -11518,7 +11518,7 @@
         <v>1491</v>
       </c>
       <c r="J11">
-        <v>1068</v>
+        <v>1075</v>
       </c>
     </row>
   </sheetData>
@@ -11799,7 +11799,7 @@
         <v>184</v>
       </c>
       <c r="J8">
-        <v>154</v>
+        <v>155</v>
       </c>
     </row>
     <row r="9" spans="1:10">
@@ -11895,7 +11895,7 @@
         <v>943</v>
       </c>
       <c r="J11">
-        <v>591</v>
+        <v>592</v>
       </c>
     </row>
   </sheetData>
@@ -12173,7 +12173,7 @@
         <v>401</v>
       </c>
       <c r="J8">
-        <v>234</v>
+        <v>235</v>
       </c>
     </row>
     <row r="9" spans="1:10">
@@ -12237,7 +12237,7 @@
         <v>2528</v>
       </c>
       <c r="J10">
-        <v>1462</v>
+        <v>1471</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -12269,7 +12269,7 @@
         <v>3506</v>
       </c>
       <c r="J11">
-        <v>2038</v>
+        <v>2048</v>
       </c>
     </row>
   </sheetData>
@@ -12550,7 +12550,7 @@
         <v>503</v>
       </c>
       <c r="J8">
-        <v>367</v>
+        <v>370</v>
       </c>
     </row>
     <row r="9" spans="1:10">
@@ -12582,7 +12582,7 @@
         <v>112</v>
       </c>
       <c r="J9">
-        <v>61</v>
+        <v>62</v>
       </c>
     </row>
     <row r="10" spans="1:10">
@@ -12614,7 +12614,7 @@
         <v>527</v>
       </c>
       <c r="J10">
-        <v>330</v>
+        <v>331</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -12646,7 +12646,7 @@
         <v>1491</v>
       </c>
       <c r="J11">
-        <v>953</v>
+        <v>958</v>
       </c>
     </row>
   </sheetData>
@@ -12767,7 +12767,7 @@
         <v>261</v>
       </c>
       <c r="J3">
-        <v>172</v>
+        <v>173</v>
       </c>
     </row>
     <row r="4" spans="1:10">
@@ -12831,7 +12831,7 @@
         <v>200</v>
       </c>
       <c r="J5">
-        <v>137</v>
+        <v>138</v>
       </c>
     </row>
     <row r="6" spans="1:10">
@@ -12927,7 +12927,7 @@
         <v>722</v>
       </c>
       <c r="J8">
-        <v>505</v>
+        <v>509</v>
       </c>
     </row>
     <row r="9" spans="1:10">
@@ -12959,7 +12959,7 @@
         <v>244</v>
       </c>
       <c r="J9">
-        <v>142</v>
+        <v>143</v>
       </c>
     </row>
     <row r="10" spans="1:10">
@@ -12991,7 +12991,7 @@
         <v>813</v>
       </c>
       <c r="J10">
-        <v>487</v>
+        <v>489</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -13023,7 +13023,7 @@
         <v>2547</v>
       </c>
       <c r="J11">
-        <v>1622</v>
+        <v>1631</v>
       </c>
     </row>
   </sheetData>
@@ -13202,7 +13202,7 @@
         <v>46</v>
       </c>
       <c r="J5">
-        <v>28</v>
+        <v>29</v>
       </c>
     </row>
     <row r="6" spans="1:10">
@@ -13315,7 +13315,7 @@
         <v>19</v>
       </c>
       <c r="J9">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="10" spans="1:10">
@@ -13379,7 +13379,7 @@
         <v>418</v>
       </c>
       <c r="J11">
-        <v>310</v>
+        <v>312</v>
       </c>
     </row>
   </sheetData>
@@ -13830,7 +13830,7 @@
         <v>194</v>
       </c>
       <c r="J2">
-        <v>114</v>
+        <v>115</v>
       </c>
     </row>
     <row r="3" spans="1:10">
@@ -13926,7 +13926,7 @@
         <v>107</v>
       </c>
       <c r="J5">
-        <v>53</v>
+        <v>54</v>
       </c>
     </row>
     <row r="6" spans="1:10">
@@ -14022,7 +14022,7 @@
         <v>202</v>
       </c>
       <c r="J8">
-        <v>219</v>
+        <v>220</v>
       </c>
     </row>
     <row r="9" spans="1:10">
@@ -14086,7 +14086,7 @@
         <v>587</v>
       </c>
       <c r="J10">
-        <v>347</v>
+        <v>350</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -14118,7 +14118,7 @@
         <v>1515</v>
       </c>
       <c r="J11">
-        <v>1027</v>
+        <v>1033</v>
       </c>
     </row>
   </sheetData>
@@ -14427,7 +14427,7 @@
         <v>100</v>
       </c>
       <c r="J10">
-        <v>53</v>
+        <v>54</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -14459,7 +14459,7 @@
         <v>209</v>
       </c>
       <c r="J11">
-        <v>160</v>
+        <v>161</v>
       </c>
     </row>
   </sheetData>
@@ -14673,7 +14673,7 @@
         <v>4</v>
       </c>
       <c r="J6">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="7" spans="1:10">
@@ -14737,7 +14737,7 @@
         <v>175</v>
       </c>
       <c r="J8">
-        <v>161</v>
+        <v>164</v>
       </c>
     </row>
     <row r="9" spans="1:10">
@@ -14833,7 +14833,7 @@
         <v>768</v>
       </c>
       <c r="J11">
-        <v>485</v>
+        <v>489</v>
       </c>
     </row>
   </sheetData>
@@ -15284,7 +15284,7 @@
         <v>190</v>
       </c>
       <c r="J2">
-        <v>102</v>
+        <v>103</v>
       </c>
     </row>
     <row r="3" spans="1:10">
@@ -15380,7 +15380,7 @@
         <v>124</v>
       </c>
       <c r="J5">
-        <v>55</v>
+        <v>56</v>
       </c>
     </row>
     <row r="6" spans="1:10">
@@ -15476,7 +15476,7 @@
         <v>484</v>
       </c>
       <c r="J8">
-        <v>294</v>
+        <v>295</v>
       </c>
     </row>
     <row r="9" spans="1:10">
@@ -15540,7 +15540,7 @@
         <v>612</v>
       </c>
       <c r="J10">
-        <v>343</v>
+        <v>344</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -15572,7 +15572,7 @@
         <v>1793</v>
       </c>
       <c r="J11">
-        <v>1041</v>
+        <v>1045</v>
       </c>
     </row>
   </sheetData>
@@ -15661,7 +15661,7 @@
         <v>92</v>
       </c>
       <c r="J2">
-        <v>44</v>
+        <v>45</v>
       </c>
     </row>
     <row r="3" spans="1:10">
@@ -15693,7 +15693,7 @@
         <v>90</v>
       </c>
       <c r="J3">
-        <v>40</v>
+        <v>41</v>
       </c>
     </row>
     <row r="4" spans="1:10">
@@ -15853,7 +15853,7 @@
         <v>224</v>
       </c>
       <c r="J8">
-        <v>176</v>
+        <v>177</v>
       </c>
     </row>
     <row r="9" spans="1:10">
@@ -15885,7 +15885,7 @@
         <v>109</v>
       </c>
       <c r="J9">
-        <v>95</v>
+        <v>96</v>
       </c>
     </row>
     <row r="10" spans="1:10">
@@ -15917,7 +15917,7 @@
         <v>610</v>
       </c>
       <c r="J10">
-        <v>301</v>
+        <v>303</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -15949,7 +15949,7 @@
         <v>1244</v>
       </c>
       <c r="J11">
-        <v>713</v>
+        <v>719</v>
       </c>
     </row>
   </sheetData>
@@ -16122,7 +16122,7 @@
         <v>86</v>
       </c>
       <c r="J5">
-        <v>54</v>
+        <v>55</v>
       </c>
     </row>
     <row r="6" spans="1:10">
@@ -16154,7 +16154,7 @@
         <v>14</v>
       </c>
       <c r="J6">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="7" spans="1:10">
@@ -16247,7 +16247,7 @@
         <v>147</v>
       </c>
       <c r="J9">
-        <v>74</v>
+        <v>76</v>
       </c>
     </row>
     <row r="10" spans="1:10">
@@ -16279,7 +16279,7 @@
         <v>2021</v>
       </c>
       <c r="J10">
-        <v>1016</v>
+        <v>1021</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -16311,7 +16311,7 @@
         <v>2663</v>
       </c>
       <c r="J11">
-        <v>1432</v>
+        <v>1441</v>
       </c>
     </row>
   </sheetData>
@@ -16400,7 +16400,7 @@
         <v>267</v>
       </c>
       <c r="J2">
-        <v>177</v>
+        <v>178</v>
       </c>
     </row>
     <row r="3" spans="1:10">
@@ -16432,7 +16432,7 @@
         <v>416</v>
       </c>
       <c r="J3">
-        <v>229</v>
+        <v>230</v>
       </c>
     </row>
     <row r="4" spans="1:10">
@@ -16656,7 +16656,7 @@
         <v>968</v>
       </c>
       <c r="J10">
-        <v>559</v>
+        <v>563</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -16688,7 +16688,7 @@
         <v>3011</v>
       </c>
       <c r="J11">
-        <v>1920</v>
+        <v>1926</v>
       </c>
     </row>
   </sheetData>
@@ -16809,7 +16809,7 @@
         <v>248</v>
       </c>
       <c r="J3">
-        <v>132</v>
+        <v>134</v>
       </c>
     </row>
     <row r="4" spans="1:10">
@@ -16873,7 +16873,7 @@
         <v>261</v>
       </c>
       <c r="J5">
-        <v>143</v>
+        <v>144</v>
       </c>
     </row>
     <row r="6" spans="1:10">
@@ -16969,7 +16969,7 @@
         <v>567</v>
       </c>
       <c r="J8">
-        <v>571</v>
+        <v>576</v>
       </c>
     </row>
     <row r="9" spans="1:10">
@@ -17033,7 +17033,7 @@
         <v>1023</v>
       </c>
       <c r="J10">
-        <v>515</v>
+        <v>516</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -17065,7 +17065,7 @@
         <v>2686</v>
       </c>
       <c r="J11">
-        <v>1688</v>
+        <v>1697</v>
       </c>
     </row>
   </sheetData>
@@ -17154,7 +17154,7 @@
         <v>457</v>
       </c>
       <c r="J2">
-        <v>286</v>
+        <v>287</v>
       </c>
     </row>
     <row r="3" spans="1:10">
@@ -17186,7 +17186,7 @@
         <v>445</v>
       </c>
       <c r="J3">
-        <v>307</v>
+        <v>308</v>
       </c>
     </row>
     <row r="4" spans="1:10">
@@ -17218,7 +17218,7 @@
         <v>30</v>
       </c>
       <c r="J4">
-        <v>22</v>
+        <v>23</v>
       </c>
     </row>
     <row r="5" spans="1:10">
@@ -17346,7 +17346,7 @@
         <v>1269</v>
       </c>
       <c r="J8">
-        <v>774</v>
+        <v>775</v>
       </c>
     </row>
     <row r="9" spans="1:10">
@@ -17410,7 +17410,7 @@
         <v>1652</v>
       </c>
       <c r="J10">
-        <v>932</v>
+        <v>934</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -17442,7 +17442,7 @@
         <v>4743</v>
       </c>
       <c r="J11">
-        <v>2851</v>
+        <v>2857</v>
       </c>
     </row>
   </sheetData>
@@ -17531,7 +17531,7 @@
         <v>106</v>
       </c>
       <c r="J2">
-        <v>62</v>
+        <v>63</v>
       </c>
     </row>
     <row r="3" spans="1:10">
@@ -17723,7 +17723,7 @@
         <v>441</v>
       </c>
       <c r="J8">
-        <v>340</v>
+        <v>341</v>
       </c>
     </row>
     <row r="9" spans="1:10">
@@ -17755,7 +17755,7 @@
         <v>120</v>
       </c>
       <c r="J9">
-        <v>51</v>
+        <v>52</v>
       </c>
     </row>
     <row r="10" spans="1:10">
@@ -17819,7 +17819,7 @@
         <v>1354</v>
       </c>
       <c r="J11">
-        <v>872</v>
+        <v>875</v>
       </c>
     </row>
   </sheetData>
@@ -18091,7 +18091,7 @@
         <v>250</v>
       </c>
       <c r="J8">
-        <v>188</v>
+        <v>190</v>
       </c>
     </row>
     <row r="9" spans="1:10">
@@ -18155,7 +18155,7 @@
         <v>417</v>
       </c>
       <c r="J10">
-        <v>244</v>
+        <v>247</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -18187,7 +18187,7 @@
         <v>903</v>
       </c>
       <c r="J11">
-        <v>570</v>
+        <v>575</v>
       </c>
     </row>
   </sheetData>
@@ -18276,7 +18276,7 @@
         <v>237</v>
       </c>
       <c r="J2">
-        <v>114</v>
+        <v>117</v>
       </c>
     </row>
     <row r="3" spans="1:10">
@@ -18468,7 +18468,7 @@
         <v>754</v>
       </c>
       <c r="J8">
-        <v>437</v>
+        <v>440</v>
       </c>
     </row>
     <row r="9" spans="1:10">
@@ -18532,7 +18532,7 @@
         <v>911</v>
       </c>
       <c r="J10">
-        <v>551</v>
+        <v>552</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -18564,7 +18564,7 @@
         <v>2636</v>
       </c>
       <c r="J11">
-        <v>1561</v>
+        <v>1568</v>
       </c>
     </row>
   </sheetData>
@@ -18818,7 +18818,7 @@
         <v>49</v>
       </c>
       <c r="J8">
-        <v>55</v>
+        <v>56</v>
       </c>
     </row>
     <row r="9" spans="1:10">
@@ -18850,7 +18850,7 @@
         <v>31</v>
       </c>
       <c r="J9">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="10" spans="1:10">
@@ -18914,7 +18914,7 @@
         <v>247</v>
       </c>
       <c r="J11">
-        <v>172</v>
+        <v>174</v>
       </c>
     </row>
   </sheetData>
@@ -19003,7 +19003,7 @@
         <v>179</v>
       </c>
       <c r="J2">
-        <v>94</v>
+        <v>95</v>
       </c>
     </row>
     <row r="3" spans="1:10">
@@ -19195,7 +19195,7 @@
         <v>363</v>
       </c>
       <c r="J8">
-        <v>285</v>
+        <v>286</v>
       </c>
     </row>
     <row r="9" spans="1:10">
@@ -19259,7 +19259,7 @@
         <v>828</v>
       </c>
       <c r="J10">
-        <v>440</v>
+        <v>441</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -19291,7 +19291,7 @@
         <v>2045</v>
       </c>
       <c r="J11">
-        <v>1121</v>
+        <v>1124</v>
       </c>
     </row>
   </sheetData>
@@ -19380,7 +19380,7 @@
         <v>37</v>
       </c>
       <c r="J2">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="3" spans="1:10">
@@ -19624,7 +19624,7 @@
         <v>630</v>
       </c>
       <c r="J10">
-        <v>315</v>
+        <v>319</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -19656,7 +19656,7 @@
         <v>960</v>
       </c>
       <c r="J11">
-        <v>566</v>
+        <v>571</v>
       </c>
     </row>
   </sheetData>
@@ -19986,7 +19986,7 @@
         <v>124</v>
       </c>
       <c r="J10">
-        <v>90</v>
+        <v>91</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -20018,7 +20018,7 @@
         <v>271</v>
       </c>
       <c r="J11">
-        <v>186</v>
+        <v>187</v>
       </c>
     </row>
   </sheetData>
@@ -20299,7 +20299,7 @@
         <v>308</v>
       </c>
       <c r="J8">
-        <v>231</v>
+        <v>233</v>
       </c>
     </row>
     <row r="9" spans="1:10">
@@ -20363,7 +20363,7 @@
         <v>320</v>
       </c>
       <c r="J10">
-        <v>190</v>
+        <v>191</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -20395,7 +20395,7 @@
         <v>970</v>
       </c>
       <c r="J11">
-        <v>632</v>
+        <v>635</v>
       </c>
     </row>
   </sheetData>
@@ -20580,7 +20580,7 @@
         <v>64</v>
       </c>
       <c r="J5">
-        <v>51</v>
+        <v>52</v>
       </c>
     </row>
     <row r="6" spans="1:10">
@@ -20670,7 +20670,7 @@
         <v>122</v>
       </c>
       <c r="J8">
-        <v>135</v>
+        <v>136</v>
       </c>
     </row>
     <row r="9" spans="1:10">
@@ -20766,7 +20766,7 @@
         <v>721</v>
       </c>
       <c r="J11">
-        <v>457</v>
+        <v>459</v>
       </c>
     </row>
   </sheetData>
@@ -21026,7 +21026,7 @@
         <v>44</v>
       </c>
       <c r="J8">
-        <v>47</v>
+        <v>48</v>
       </c>
     </row>
     <row r="9" spans="1:10">
@@ -21122,7 +21122,7 @@
         <v>436</v>
       </c>
       <c r="J11">
-        <v>281</v>
+        <v>282</v>
       </c>
     </row>
   </sheetData>
@@ -21243,7 +21243,7 @@
         <v>28</v>
       </c>
       <c r="J3">
-        <v>15</v>
+        <v>16</v>
       </c>
     </row>
     <row r="4" spans="1:10">
@@ -21458,7 +21458,7 @@
         <v>216</v>
       </c>
       <c r="J10">
-        <v>123</v>
+        <v>125</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -21490,7 +21490,7 @@
         <v>436</v>
       </c>
       <c r="J11">
-        <v>258</v>
+        <v>261</v>
       </c>
     </row>
   </sheetData>
@@ -21672,7 +21672,7 @@
         <v>67</v>
       </c>
       <c r="J5">
-        <v>39</v>
+        <v>40</v>
       </c>
     </row>
     <row r="6" spans="1:10">
@@ -21768,7 +21768,7 @@
         <v>297</v>
       </c>
       <c r="J8">
-        <v>292</v>
+        <v>294</v>
       </c>
     </row>
     <row r="9" spans="1:10">
@@ -21832,7 +21832,7 @@
         <v>670</v>
       </c>
       <c r="J10">
-        <v>364</v>
+        <v>365</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -21864,7 +21864,7 @@
         <v>1337</v>
       </c>
       <c r="J11">
-        <v>898</v>
+        <v>902</v>
       </c>
     </row>
   </sheetData>
@@ -22049,7 +22049,7 @@
         <v>83</v>
       </c>
       <c r="J5">
-        <v>51</v>
+        <v>52</v>
       </c>
     </row>
     <row r="6" spans="1:10">
@@ -22145,7 +22145,7 @@
         <v>125</v>
       </c>
       <c r="J8">
-        <v>86</v>
+        <v>87</v>
       </c>
     </row>
     <row r="9" spans="1:10">
@@ -22209,7 +22209,7 @@
         <v>492</v>
       </c>
       <c r="J10">
-        <v>332</v>
+        <v>333</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -22241,7 +22241,7 @@
         <v>917</v>
       </c>
       <c r="J11">
-        <v>584</v>
+        <v>587</v>
       </c>
     </row>
   </sheetData>
@@ -22933,7 +22933,7 @@
         <v>239</v>
       </c>
       <c r="J10">
-        <v>142</v>
+        <v>143</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -22965,7 +22965,7 @@
         <v>695</v>
       </c>
       <c r="J11">
-        <v>444</v>
+        <v>445</v>
       </c>
     </row>
   </sheetData>
@@ -23298,7 +23298,7 @@
         <v>277</v>
       </c>
       <c r="J10">
-        <v>184</v>
+        <v>187</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -23330,7 +23330,7 @@
         <v>500</v>
       </c>
       <c r="J11">
-        <v>357</v>
+        <v>360</v>
       </c>
     </row>
   </sheetData>
@@ -23672,7 +23672,7 @@
         <v>189</v>
       </c>
       <c r="J10">
-        <v>143</v>
+        <v>145</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -23704,7 +23704,7 @@
         <v>429</v>
       </c>
       <c r="J11">
-        <v>288</v>
+        <v>290</v>
       </c>
     </row>
   </sheetData>
@@ -24014,7 +24014,7 @@
         <v>55</v>
       </c>
       <c r="J9">
-        <v>41</v>
+        <v>42</v>
       </c>
     </row>
     <row r="10" spans="1:10">
@@ -24046,7 +24046,7 @@
         <v>349</v>
       </c>
       <c r="J10">
-        <v>218</v>
+        <v>219</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -24078,7 +24078,7 @@
         <v>793</v>
       </c>
       <c r="J11">
-        <v>574</v>
+        <v>576</v>
       </c>
     </row>
   </sheetData>
@@ -24712,7 +24712,7 @@
         <v>167</v>
       </c>
       <c r="J8">
-        <v>123</v>
+        <v>125</v>
       </c>
     </row>
     <row r="9" spans="1:10">
@@ -24776,7 +24776,7 @@
         <v>784</v>
       </c>
       <c r="J10">
-        <v>502</v>
+        <v>508</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -24808,7 +24808,7 @@
         <v>1258</v>
       </c>
       <c r="J11">
-        <v>785</v>
+        <v>793</v>
       </c>
     </row>
   </sheetData>
@@ -24897,7 +24897,7 @@
         <v>79</v>
       </c>
       <c r="J2">
-        <v>44</v>
+        <v>45</v>
       </c>
     </row>
     <row r="3" spans="1:10">
@@ -25153,7 +25153,7 @@
         <v>381</v>
       </c>
       <c r="J10">
-        <v>211</v>
+        <v>213</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -25185,7 +25185,7 @@
         <v>868</v>
       </c>
       <c r="J11">
-        <v>496</v>
+        <v>499</v>
       </c>
     </row>
   </sheetData>
@@ -25482,7 +25482,7 @@
         <v>576</v>
       </c>
       <c r="J10">
-        <v>311</v>
+        <v>314</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -25514,7 +25514,7 @@
         <v>628</v>
       </c>
       <c r="J11">
-        <v>336</v>
+        <v>339</v>
       </c>
     </row>
   </sheetData>
@@ -26186,7 +26186,7 @@
         <v>139</v>
       </c>
       <c r="J9">
-        <v>84</v>
+        <v>85</v>
       </c>
     </row>
     <row r="10" spans="1:10">
@@ -26218,7 +26218,7 @@
         <v>233</v>
       </c>
       <c r="J10">
-        <v>159</v>
+        <v>160</v>
       </c>
     </row>
   </sheetData>
@@ -26339,7 +26339,7 @@
         <v>87</v>
       </c>
       <c r="J3">
-        <v>69</v>
+        <v>70</v>
       </c>
     </row>
     <row r="4" spans="1:10">
@@ -26499,7 +26499,7 @@
         <v>198</v>
       </c>
       <c r="J8">
-        <v>160</v>
+        <v>161</v>
       </c>
     </row>
     <row r="9" spans="1:10">
@@ -26595,7 +26595,7 @@
         <v>1797</v>
       </c>
       <c r="J11">
-        <v>1032</v>
+        <v>1034</v>
       </c>
     </row>
   </sheetData>
@@ -26931,7 +26931,7 @@
         <v>371</v>
       </c>
       <c r="J10">
-        <v>165</v>
+        <v>166</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -26963,7 +26963,7 @@
         <v>718</v>
       </c>
       <c r="J11">
-        <v>363</v>
+        <v>364</v>
       </c>
     </row>
   </sheetData>
@@ -27052,7 +27052,7 @@
         <v>21</v>
       </c>
       <c r="J2">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="3" spans="1:10">
@@ -27214,7 +27214,7 @@
         <v>99</v>
       </c>
       <c r="J8">
-        <v>82</v>
+        <v>83</v>
       </c>
     </row>
     <row r="9" spans="1:10">
@@ -27310,7 +27310,7 @@
         <v>715</v>
       </c>
       <c r="J11">
-        <v>440</v>
+        <v>442</v>
       </c>
     </row>
   </sheetData>
@@ -27561,7 +27561,7 @@
         <v>77</v>
       </c>
       <c r="J8">
-        <v>70</v>
+        <v>71</v>
       </c>
     </row>
     <row r="9" spans="1:10">
@@ -27657,7 +27657,7 @@
         <v>595</v>
       </c>
       <c r="J11">
-        <v>438</v>
+        <v>439</v>
       </c>
     </row>
   </sheetData>
@@ -27842,7 +27842,7 @@
         <v>48</v>
       </c>
       <c r="J5">
-        <v>27</v>
+        <v>28</v>
       </c>
     </row>
     <row r="6" spans="1:10">
@@ -28034,7 +28034,7 @@
         <v>519</v>
       </c>
       <c r="J11">
-        <v>318</v>
+        <v>319</v>
       </c>
     </row>
   </sheetData>
@@ -28288,7 +28288,7 @@
         <v>39</v>
       </c>
       <c r="J8">
-        <v>35</v>
+        <v>36</v>
       </c>
     </row>
     <row r="9" spans="1:10">
@@ -28384,7 +28384,7 @@
         <v>175</v>
       </c>
       <c r="J11">
-        <v>87</v>
+        <v>88</v>
       </c>
     </row>
   </sheetData>
@@ -28505,7 +28505,7 @@
         <v>37</v>
       </c>
       <c r="J3">
-        <v>18</v>
+        <v>19</v>
       </c>
     </row>
     <row r="4" spans="1:10">
@@ -28694,7 +28694,7 @@
         <v>90</v>
       </c>
       <c r="J9">
-        <v>45</v>
+        <v>46</v>
       </c>
     </row>
     <row r="10" spans="1:10">
@@ -28758,7 +28758,7 @@
         <v>948</v>
       </c>
       <c r="J11">
-        <v>543</v>
+        <v>545</v>
       </c>
     </row>
   </sheetData>
@@ -29250,7 +29250,7 @@
         <v>71</v>
       </c>
       <c r="J3">
-        <v>50</v>
+        <v>51</v>
       </c>
     </row>
     <row r="4" spans="1:10">
@@ -29314,7 +29314,7 @@
         <v>131</v>
       </c>
       <c r="J5">
-        <v>82</v>
+        <v>83</v>
       </c>
     </row>
     <row r="6" spans="1:10">
@@ -29407,7 +29407,7 @@
         <v>216</v>
       </c>
       <c r="J8">
-        <v>200</v>
+        <v>201</v>
       </c>
     </row>
     <row r="9" spans="1:10">
@@ -29471,7 +29471,7 @@
         <v>1222</v>
       </c>
       <c r="J10">
-        <v>687</v>
+        <v>692</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -29503,7 +29503,7 @@
         <v>1879</v>
       </c>
       <c r="J11">
-        <v>1176</v>
+        <v>1184</v>
       </c>
     </row>
   </sheetData>
@@ -29592,7 +29592,7 @@
         <v>46</v>
       </c>
       <c r="J2">
-        <v>21</v>
+        <v>22</v>
       </c>
     </row>
     <row r="3" spans="1:10">
@@ -29813,7 +29813,7 @@
         <v>24</v>
       </c>
       <c r="J9">
-        <v>24</v>
+        <v>25</v>
       </c>
     </row>
     <row r="10" spans="1:10">
@@ -29845,7 +29845,7 @@
         <v>440</v>
       </c>
       <c r="J10">
-        <v>266</v>
+        <v>267</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -29877,7 +29877,7 @@
         <v>761</v>
       </c>
       <c r="J11">
-        <v>503</v>
+        <v>506</v>
       </c>
     </row>
   </sheetData>
@@ -30062,7 +30062,7 @@
         <v>120</v>
       </c>
       <c r="J5">
-        <v>82</v>
+        <v>83</v>
       </c>
     </row>
     <row r="6" spans="1:10">
@@ -30158,7 +30158,7 @@
         <v>383</v>
       </c>
       <c r="J8">
-        <v>305</v>
+        <v>306</v>
       </c>
     </row>
     <row r="9" spans="1:10">
@@ -30254,7 +30254,7 @@
         <v>1488</v>
       </c>
       <c r="J11">
-        <v>947</v>
+        <v>949</v>
       </c>
     </row>
   </sheetData>
@@ -30898,7 +30898,7 @@
         <v>502</v>
       </c>
       <c r="J10">
-        <v>317</v>
+        <v>318</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -30930,7 +30930,7 @@
         <v>677</v>
       </c>
       <c r="J11">
-        <v>423</v>
+        <v>424</v>
       </c>
     </row>
   </sheetData>
@@ -31386,7 +31386,7 @@
         <v>27</v>
       </c>
       <c r="J3">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="4" spans="1:10">
@@ -31627,7 +31627,7 @@
         <v>335</v>
       </c>
       <c r="J11">
-        <v>262</v>
+        <v>263</v>
       </c>
     </row>
   </sheetData>
@@ -31716,7 +31716,7 @@
         <v>90</v>
       </c>
       <c r="J2">
-        <v>48</v>
+        <v>49</v>
       </c>
     </row>
     <row r="3" spans="1:10">
@@ -32004,7 +32004,7 @@
         <v>886</v>
       </c>
       <c r="J11">
-        <v>594</v>
+        <v>595</v>
       </c>
     </row>
   </sheetData>
@@ -32279,7 +32279,7 @@
         <v>405</v>
       </c>
       <c r="J8">
-        <v>354</v>
+        <v>356</v>
       </c>
     </row>
     <row r="9" spans="1:10">
@@ -32343,7 +32343,7 @@
         <v>670</v>
       </c>
       <c r="J10">
-        <v>327</v>
+        <v>329</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -32375,7 +32375,7 @@
         <v>1368</v>
       </c>
       <c r="J11">
-        <v>850</v>
+        <v>854</v>
       </c>
     </row>
   </sheetData>
@@ -32650,7 +32650,7 @@
         <v>338</v>
       </c>
       <c r="J8">
-        <v>265</v>
+        <v>268</v>
       </c>
     </row>
     <row r="9" spans="1:10">
@@ -32714,7 +32714,7 @@
         <v>1773</v>
       </c>
       <c r="J10">
-        <v>1045</v>
+        <v>1050</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -32746,7 +32746,7 @@
         <v>2622</v>
       </c>
       <c r="J11">
-        <v>1563</v>
+        <v>1571</v>
       </c>
     </row>
   </sheetData>
@@ -33044,7 +33044,7 @@
         <v>21</v>
       </c>
       <c r="J9">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="10" spans="1:10">
@@ -33108,7 +33108,7 @@
         <v>340</v>
       </c>
       <c r="J11">
-        <v>207</v>
+        <v>208</v>
       </c>
     </row>
   </sheetData>
@@ -33414,7 +33414,7 @@
         <v>174</v>
       </c>
       <c r="J10">
-        <v>79</v>
+        <v>80</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -33446,7 +33446,7 @@
         <v>337</v>
       </c>
       <c r="J11">
-        <v>159</v>
+        <v>160</v>
       </c>
     </row>
   </sheetData>
@@ -34210,7 +34210,7 @@
         <v>22</v>
       </c>
       <c r="J2">
-        <v>14</v>
+        <v>15</v>
       </c>
     </row>
     <row r="3" spans="1:10">
@@ -34445,7 +34445,7 @@
         <v>313</v>
       </c>
       <c r="J10">
-        <v>159</v>
+        <v>162</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -34477,7 +34477,7 @@
         <v>494</v>
       </c>
       <c r="J11">
-        <v>262</v>
+        <v>266</v>
       </c>
     </row>
   </sheetData>
@@ -34687,7 +34687,7 @@
         <v>19</v>
       </c>
       <c r="J7">
-        <v>17</v>
+        <v>18</v>
       </c>
     </row>
     <row r="8" spans="1:10">
@@ -34783,7 +34783,7 @@
         <v>155</v>
       </c>
       <c r="J10">
-        <v>107</v>
+        <v>108</v>
       </c>
     </row>
   </sheetData>
@@ -35116,7 +35116,7 @@
         <v>211</v>
       </c>
       <c r="J10">
-        <v>148</v>
+        <v>149</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -35148,7 +35148,7 @@
         <v>406</v>
       </c>
       <c r="J11">
-        <v>292</v>
+        <v>293</v>
       </c>
     </row>
   </sheetData>
@@ -36099,7 +36099,7 @@
         <v>47</v>
       </c>
       <c r="J10">
-        <v>17</v>
+        <v>18</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -36131,7 +36131,7 @@
         <v>99</v>
       </c>
       <c r="J11">
-        <v>37</v>
+        <v>38</v>
       </c>
     </row>
   </sheetData>
@@ -36316,7 +36316,7 @@
         <v>161</v>
       </c>
       <c r="J5">
-        <v>93</v>
+        <v>94</v>
       </c>
     </row>
     <row r="6" spans="1:10">
@@ -36476,7 +36476,7 @@
         <v>905</v>
       </c>
       <c r="J10">
-        <v>479</v>
+        <v>483</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -36508,7 +36508,7 @@
         <v>1669</v>
       </c>
       <c r="J11">
-        <v>956</v>
+        <v>961</v>
       </c>
     </row>
   </sheetData>
@@ -36783,7 +36783,7 @@
         <v>68</v>
       </c>
       <c r="J8">
-        <v>67</v>
+        <v>68</v>
       </c>
     </row>
     <row r="9" spans="1:10">
@@ -36815,7 +36815,7 @@
         <v>31</v>
       </c>
       <c r="J9">
-        <v>16</v>
+        <v>18</v>
       </c>
     </row>
     <row r="10" spans="1:10">
@@ -36879,7 +36879,7 @@
         <v>337</v>
       </c>
       <c r="J11">
-        <v>238</v>
+        <v>241</v>
       </c>
     </row>
   </sheetData>
@@ -37769,7 +37769,7 @@
         <v>80</v>
       </c>
       <c r="J6">
-        <v>48</v>
+        <v>49</v>
       </c>
     </row>
     <row r="7" spans="1:10">
@@ -37879,7 +37879,7 @@
         <v>717</v>
       </c>
       <c r="J10">
-        <v>333</v>
+        <v>337</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -37911,7 +37911,7 @@
         <v>1066</v>
       </c>
       <c r="J11">
-        <v>502</v>
+        <v>507</v>
       </c>
     </row>
   </sheetData>
@@ -38549,7 +38549,7 @@
         <v>135</v>
       </c>
       <c r="J10">
-        <v>72</v>
+        <v>73</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -38581,7 +38581,7 @@
         <v>219</v>
       </c>
       <c r="J11">
-        <v>129</v>
+        <v>130</v>
       </c>
     </row>
   </sheetData>
@@ -38878,7 +38878,7 @@
         <v>225</v>
       </c>
       <c r="J10">
-        <v>113</v>
+        <v>114</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -38910,7 +38910,7 @@
         <v>307</v>
       </c>
       <c r="J11">
-        <v>159</v>
+        <v>160</v>
       </c>
     </row>
   </sheetData>
@@ -39633,7 +39633,7 @@
         <v>4</v>
       </c>
       <c r="J2">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="3" spans="1:10">
@@ -39818,7 +39818,7 @@
         <v>155</v>
       </c>
       <c r="J9">
-        <v>95</v>
+        <v>97</v>
       </c>
     </row>
     <row r="10" spans="1:10">
@@ -39850,7 +39850,7 @@
         <v>191</v>
       </c>
       <c r="J10">
-        <v>108</v>
+        <v>111</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add data for 2024-02-25
</commit_message>
<xml_diff>
--- a/output/index-crime-full-year.xlsx
+++ b/output/index-crime-full-year.xlsx
@@ -902,7 +902,7 @@
         <v>7704</v>
       </c>
       <c r="K2">
-        <v>999</v>
+        <v>1008</v>
       </c>
     </row>
     <row r="3" spans="1:11">
@@ -937,7 +937,7 @@
         <v>8076</v>
       </c>
       <c r="K3">
-        <v>944</v>
+        <v>963</v>
       </c>
     </row>
     <row r="4" spans="1:11">
@@ -972,7 +972,7 @@
         <v>510</v>
       </c>
       <c r="K4">
-        <v>62</v>
+        <v>63</v>
       </c>
     </row>
     <row r="5" spans="1:11">
@@ -1007,7 +1007,7 @@
         <v>7462</v>
       </c>
       <c r="K5">
-        <v>956</v>
+        <v>972</v>
       </c>
     </row>
     <row r="6" spans="1:11">
@@ -1039,10 +1039,10 @@
         <v>1785</v>
       </c>
       <c r="J6">
-        <v>1798</v>
+        <v>1797</v>
       </c>
       <c r="K6">
-        <v>209</v>
+        <v>211</v>
       </c>
     </row>
     <row r="7" spans="1:11">
@@ -1112,7 +1112,7 @@
         <v>29205</v>
       </c>
       <c r="K8">
-        <v>3190</v>
+        <v>3260</v>
       </c>
     </row>
     <row r="9" spans="1:11">
@@ -1147,7 +1147,7 @@
         <v>11059</v>
       </c>
       <c r="K9">
-        <v>1299</v>
+        <v>1318</v>
       </c>
     </row>
     <row r="10" spans="1:11">
@@ -1179,10 +1179,10 @@
         <v>54863</v>
       </c>
       <c r="J10">
-        <v>57245</v>
+        <v>57248</v>
       </c>
       <c r="K10">
-        <v>7561</v>
+        <v>7701</v>
       </c>
     </row>
     <row r="11" spans="1:11">
@@ -1214,10 +1214,10 @@
         <v>110574</v>
       </c>
       <c r="J11">
-        <v>123684</v>
+        <v>123686</v>
       </c>
       <c r="K11">
-        <v>15276</v>
+        <v>15552</v>
       </c>
     </row>
   </sheetData>
@@ -1313,7 +1313,7 @@
         <v>177</v>
       </c>
       <c r="K2">
-        <v>21</v>
+        <v>22</v>
       </c>
     </row>
     <row r="3" spans="1:11">
@@ -1348,7 +1348,7 @@
         <v>209</v>
       </c>
       <c r="K3">
-        <v>14</v>
+        <v>15</v>
       </c>
     </row>
     <row r="4" spans="1:11">
@@ -1418,7 +1418,7 @@
         <v>81</v>
       </c>
       <c r="K5">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="6" spans="1:11">
@@ -1450,7 +1450,7 @@
         <v>40</v>
       </c>
       <c r="J6">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="K6">
         <v>4</v>
@@ -1523,7 +1523,7 @@
         <v>385</v>
       </c>
       <c r="K8">
-        <v>51</v>
+        <v>53</v>
       </c>
     </row>
     <row r="9" spans="1:11">
@@ -1593,7 +1593,7 @@
         <v>693</v>
       </c>
       <c r="K10">
-        <v>104</v>
+        <v>105</v>
       </c>
     </row>
     <row r="11" spans="1:11">
@@ -1625,10 +1625,10 @@
         <v>1499</v>
       </c>
       <c r="J11">
-        <v>1922</v>
+        <v>1923</v>
       </c>
       <c r="K11">
-        <v>244</v>
+        <v>250</v>
       </c>
     </row>
   </sheetData>
@@ -2066,7 +2066,7 @@
         <v>16</v>
       </c>
       <c r="K3">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="4" spans="1:11">
@@ -2284,7 +2284,7 @@
         <v>323</v>
       </c>
       <c r="K10">
-        <v>61</v>
+        <v>63</v>
       </c>
     </row>
     <row r="11" spans="1:11">
@@ -2319,7 +2319,7 @@
         <v>495</v>
       </c>
       <c r="K11">
-        <v>88</v>
+        <v>91</v>
       </c>
     </row>
   </sheetData>
@@ -2450,7 +2450,7 @@
         <v>56</v>
       </c>
       <c r="K3">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="4" spans="1:11">
@@ -2619,7 +2619,7 @@
         <v>472</v>
       </c>
       <c r="K8">
-        <v>63</v>
+        <v>64</v>
       </c>
     </row>
     <row r="9" spans="1:11">
@@ -2689,7 +2689,7 @@
         <v>1203</v>
       </c>
       <c r="K10">
-        <v>217</v>
+        <v>219</v>
       </c>
     </row>
     <row r="11" spans="1:11">
@@ -2724,7 +2724,7 @@
         <v>2251</v>
       </c>
       <c r="K11">
-        <v>332</v>
+        <v>336</v>
       </c>
     </row>
   </sheetData>
@@ -2820,7 +2820,7 @@
         <v>488</v>
       </c>
       <c r="K2">
-        <v>58</v>
+        <v>59</v>
       </c>
     </row>
     <row r="3" spans="1:11">
@@ -2855,7 +2855,7 @@
         <v>529</v>
       </c>
       <c r="K3">
-        <v>61</v>
+        <v>62</v>
       </c>
     </row>
     <row r="4" spans="1:11">
@@ -3030,7 +3030,7 @@
         <v>1245</v>
       </c>
       <c r="K8">
-        <v>145</v>
+        <v>148</v>
       </c>
     </row>
     <row r="9" spans="1:11">
@@ -3100,7 +3100,7 @@
         <v>1715</v>
       </c>
       <c r="K10">
-        <v>221</v>
+        <v>227</v>
       </c>
     </row>
     <row r="11" spans="1:11">
@@ -3135,7 +3135,7 @@
         <v>5075</v>
       </c>
       <c r="K11">
-        <v>606</v>
+        <v>617</v>
       </c>
     </row>
   </sheetData>
@@ -3854,7 +3854,7 @@
         <v>53</v>
       </c>
       <c r="K9">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="10" spans="1:11">
@@ -3889,7 +3889,7 @@
         <v>377</v>
       </c>
       <c r="K10">
-        <v>36</v>
+        <v>38</v>
       </c>
     </row>
     <row r="11" spans="1:11">
@@ -3924,7 +3924,7 @@
         <v>844</v>
       </c>
       <c r="K11">
-        <v>91</v>
+        <v>94</v>
       </c>
     </row>
   </sheetData>
@@ -4276,7 +4276,7 @@
         <v>149</v>
       </c>
       <c r="K10">
-        <v>21</v>
+        <v>22</v>
       </c>
     </row>
     <row r="11" spans="1:11">
@@ -4311,7 +4311,7 @@
         <v>449</v>
       </c>
       <c r="K11">
-        <v>63</v>
+        <v>64</v>
       </c>
     </row>
   </sheetData>
@@ -4617,7 +4617,7 @@
         <v>517</v>
       </c>
       <c r="K8">
-        <v>50</v>
+        <v>51</v>
       </c>
     </row>
     <row r="9" spans="1:11">
@@ -4687,7 +4687,7 @@
         <v>596</v>
       </c>
       <c r="K10">
-        <v>63</v>
+        <v>65</v>
       </c>
     </row>
     <row r="11" spans="1:11">
@@ -4722,7 +4722,7 @@
         <v>1811</v>
       </c>
       <c r="K11">
-        <v>188</v>
+        <v>191</v>
       </c>
     </row>
   </sheetData>
@@ -4818,7 +4818,7 @@
         <v>295</v>
       </c>
       <c r="K2">
-        <v>36</v>
+        <v>37</v>
       </c>
     </row>
     <row r="3" spans="1:11">
@@ -4853,7 +4853,7 @@
         <v>438</v>
       </c>
       <c r="K3">
-        <v>54</v>
+        <v>57</v>
       </c>
     </row>
     <row r="4" spans="1:11">
@@ -5025,10 +5025,10 @@
         <v>712</v>
       </c>
       <c r="J8">
-        <v>889</v>
+        <v>890</v>
       </c>
       <c r="K8">
-        <v>88</v>
+        <v>90</v>
       </c>
     </row>
     <row r="9" spans="1:11">
@@ -5063,7 +5063,7 @@
         <v>473</v>
       </c>
       <c r="K9">
-        <v>45</v>
+        <v>46</v>
       </c>
     </row>
     <row r="10" spans="1:11">
@@ -5098,7 +5098,7 @@
         <v>1032</v>
       </c>
       <c r="K10">
-        <v>125</v>
+        <v>126</v>
       </c>
     </row>
     <row r="11" spans="1:11">
@@ -5130,10 +5130,10 @@
         <v>3035</v>
       </c>
       <c r="J11">
-        <v>3404</v>
+        <v>3405</v>
       </c>
       <c r="K11">
-        <v>378</v>
+        <v>386</v>
       </c>
     </row>
   </sheetData>
@@ -5229,7 +5229,7 @@
         <v>234</v>
       </c>
       <c r="K2">
-        <v>37</v>
+        <v>38</v>
       </c>
     </row>
     <row r="3" spans="1:11">
@@ -5509,7 +5509,7 @@
         <v>827</v>
       </c>
       <c r="K10">
-        <v>99</v>
+        <v>101</v>
       </c>
     </row>
     <row r="11" spans="1:11">
@@ -5544,7 +5544,7 @@
         <v>2630</v>
       </c>
       <c r="K11">
-        <v>304</v>
+        <v>307</v>
       </c>
     </row>
   </sheetData>
@@ -5640,7 +5640,7 @@
         <v>1142</v>
       </c>
       <c r="K2">
-        <v>145</v>
+        <v>147</v>
       </c>
     </row>
     <row r="3" spans="1:11">
@@ -5675,7 +5675,7 @@
         <v>202</v>
       </c>
       <c r="K3">
-        <v>28</v>
+        <v>29</v>
       </c>
     </row>
     <row r="4" spans="1:11">
@@ -5710,7 +5710,7 @@
         <v>515</v>
       </c>
       <c r="K4">
-        <v>66</v>
+        <v>69</v>
       </c>
     </row>
     <row r="5" spans="1:11">
@@ -5780,7 +5780,7 @@
         <v>1102</v>
       </c>
       <c r="K6">
-        <v>147</v>
+        <v>148</v>
       </c>
     </row>
     <row r="7" spans="1:11">
@@ -5815,7 +5815,7 @@
         <v>2985</v>
       </c>
       <c r="K7">
-        <v>328</v>
+        <v>336</v>
       </c>
     </row>
     <row r="8" spans="1:11">
@@ -5850,7 +5850,7 @@
         <v>5075</v>
       </c>
       <c r="K8">
-        <v>606</v>
+        <v>617</v>
       </c>
     </row>
     <row r="9" spans="1:11">
@@ -5885,7 +5885,7 @@
         <v>541</v>
       </c>
       <c r="K9">
-        <v>50</v>
+        <v>51</v>
       </c>
     </row>
     <row r="10" spans="1:11">
@@ -5920,7 +5920,7 @@
         <v>1153</v>
       </c>
       <c r="K10">
-        <v>160</v>
+        <v>165</v>
       </c>
     </row>
     <row r="11" spans="1:11">
@@ -5952,10 +5952,10 @@
         <v>1720</v>
       </c>
       <c r="J11">
-        <v>2168</v>
+        <v>2169</v>
       </c>
       <c r="K11">
-        <v>305</v>
+        <v>307</v>
       </c>
     </row>
     <row r="12" spans="1:11">
@@ -6092,10 +6092,10 @@
         <v>888</v>
       </c>
       <c r="J15">
-        <v>1070</v>
+        <v>1071</v>
       </c>
       <c r="K15">
-        <v>137</v>
+        <v>142</v>
       </c>
     </row>
     <row r="16" spans="1:11">
@@ -6130,7 +6130,7 @@
         <v>828</v>
       </c>
       <c r="K16">
-        <v>107</v>
+        <v>108</v>
       </c>
     </row>
     <row r="17" spans="1:11">
@@ -6165,7 +6165,7 @@
         <v>145</v>
       </c>
       <c r="K17">
-        <v>14</v>
+        <v>15</v>
       </c>
     </row>
     <row r="18" spans="1:11">
@@ -6200,7 +6200,7 @@
         <v>859</v>
       </c>
       <c r="K18">
-        <v>117</v>
+        <v>121</v>
       </c>
     </row>
     <row r="19" spans="1:11">
@@ -6235,7 +6235,7 @@
         <v>2861</v>
       </c>
       <c r="K19">
-        <v>354</v>
+        <v>360</v>
       </c>
     </row>
     <row r="20" spans="1:11">
@@ -6270,7 +6270,7 @@
         <v>2178</v>
       </c>
       <c r="K20">
-        <v>246</v>
+        <v>251</v>
       </c>
     </row>
     <row r="21" spans="1:11">
@@ -6340,7 +6340,7 @@
         <v>538</v>
       </c>
       <c r="K22">
-        <v>48</v>
+        <v>49</v>
       </c>
     </row>
     <row r="23" spans="1:11">
@@ -6375,7 +6375,7 @@
         <v>1593</v>
       </c>
       <c r="K23">
-        <v>149</v>
+        <v>152</v>
       </c>
     </row>
     <row r="24" spans="1:11">
@@ -6585,7 +6585,7 @@
         <v>4178</v>
       </c>
       <c r="K29">
-        <v>454</v>
+        <v>461</v>
       </c>
     </row>
     <row r="30" spans="1:11">
@@ -6655,7 +6655,7 @@
         <v>1031</v>
       </c>
       <c r="K31">
-        <v>149</v>
+        <v>153</v>
       </c>
     </row>
     <row r="32" spans="1:11">
@@ -6690,7 +6690,7 @@
         <v>284</v>
       </c>
       <c r="K32">
-        <v>24</v>
+        <v>26</v>
       </c>
     </row>
     <row r="33" spans="1:11">
@@ -6722,10 +6722,10 @@
         <v>3035</v>
       </c>
       <c r="J33">
-        <v>3404</v>
+        <v>3405</v>
       </c>
       <c r="K33">
-        <v>378</v>
+        <v>386</v>
       </c>
     </row>
     <row r="34" spans="1:11">
@@ -6760,7 +6760,7 @@
         <v>950</v>
       </c>
       <c r="K34">
-        <v>155</v>
+        <v>157</v>
       </c>
     </row>
     <row r="35" spans="1:11">
@@ -6830,7 +6830,7 @@
         <v>1736</v>
       </c>
       <c r="K36">
-        <v>183</v>
+        <v>184</v>
       </c>
     </row>
     <row r="37" spans="1:11">
@@ -6865,7 +6865,7 @@
         <v>2972</v>
       </c>
       <c r="K37">
-        <v>354</v>
+        <v>357</v>
       </c>
     </row>
     <row r="38" spans="1:11">
@@ -6900,7 +6900,7 @@
         <v>261</v>
       </c>
       <c r="K38">
-        <v>15</v>
+        <v>16</v>
       </c>
     </row>
     <row r="39" spans="1:11">
@@ -6970,7 +6970,7 @@
         <v>299</v>
       </c>
       <c r="K40">
-        <v>53</v>
+        <v>54</v>
       </c>
     </row>
     <row r="41" spans="1:11">
@@ -7040,7 +7040,7 @@
         <v>3619</v>
       </c>
       <c r="K42">
-        <v>362</v>
+        <v>369</v>
       </c>
     </row>
     <row r="43" spans="1:11">
@@ -7072,10 +7072,10 @@
         <v>1161</v>
       </c>
       <c r="J43">
-        <v>1454</v>
+        <v>1453</v>
       </c>
       <c r="K43">
-        <v>169</v>
+        <v>172</v>
       </c>
     </row>
     <row r="44" spans="1:11">
@@ -7110,7 +7110,7 @@
         <v>1382</v>
       </c>
       <c r="K44">
-        <v>200</v>
+        <v>203</v>
       </c>
     </row>
     <row r="45" spans="1:11">
@@ -7145,7 +7145,7 @@
         <v>155</v>
       </c>
       <c r="K45">
-        <v>12</v>
+        <v>13</v>
       </c>
     </row>
     <row r="46" spans="1:11">
@@ -7215,7 +7215,7 @@
         <v>1025</v>
       </c>
       <c r="K47">
-        <v>156</v>
+        <v>158</v>
       </c>
     </row>
     <row r="48" spans="1:11">
@@ -7247,10 +7247,10 @@
         <v>2649</v>
       </c>
       <c r="J48">
-        <v>3090</v>
+        <v>3091</v>
       </c>
       <c r="K48">
-        <v>374</v>
+        <v>379</v>
       </c>
     </row>
     <row r="49" spans="1:11">
@@ -7285,7 +7285,7 @@
         <v>1840</v>
       </c>
       <c r="K49">
-        <v>246</v>
+        <v>251</v>
       </c>
     </row>
     <row r="50" spans="1:11">
@@ -7320,7 +7320,7 @@
         <v>1138</v>
       </c>
       <c r="K50">
-        <v>132</v>
+        <v>134</v>
       </c>
     </row>
     <row r="51" spans="1:11">
@@ -7355,7 +7355,7 @@
         <v>1653</v>
       </c>
       <c r="K51">
-        <v>221</v>
+        <v>225</v>
       </c>
     </row>
     <row r="52" spans="1:11">
@@ -7387,10 +7387,10 @@
         <v>1499</v>
       </c>
       <c r="J52">
-        <v>1922</v>
+        <v>1923</v>
       </c>
       <c r="K52">
-        <v>244</v>
+        <v>250</v>
       </c>
     </row>
     <row r="53" spans="1:11">
@@ -7425,7 +7425,7 @@
         <v>2251</v>
       </c>
       <c r="K53">
-        <v>332</v>
+        <v>336</v>
       </c>
     </row>
     <row r="54" spans="1:11">
@@ -7460,7 +7460,7 @@
         <v>3895</v>
       </c>
       <c r="K54">
-        <v>542</v>
+        <v>556</v>
       </c>
     </row>
     <row r="55" spans="1:11">
@@ -7495,7 +7495,7 @@
         <v>1477</v>
       </c>
       <c r="K55">
-        <v>174</v>
+        <v>179</v>
       </c>
     </row>
     <row r="56" spans="1:11">
@@ -7530,7 +7530,7 @@
         <v>670</v>
       </c>
       <c r="K56">
-        <v>93</v>
+        <v>94</v>
       </c>
     </row>
     <row r="57" spans="1:11">
@@ -7565,7 +7565,7 @@
         <v>552</v>
       </c>
       <c r="K57">
-        <v>68</v>
+        <v>69</v>
       </c>
     </row>
     <row r="58" spans="1:11">
@@ -7670,7 +7670,7 @@
         <v>844</v>
       </c>
       <c r="K60">
-        <v>91</v>
+        <v>94</v>
       </c>
     </row>
     <row r="61" spans="1:11">
@@ -7705,7 +7705,7 @@
         <v>166</v>
       </c>
       <c r="K61">
-        <v>20</v>
+        <v>21</v>
       </c>
     </row>
     <row r="62" spans="1:11">
@@ -7772,10 +7772,10 @@
         <v>1843</v>
       </c>
       <c r="J63">
-        <v>482</v>
+        <v>479</v>
       </c>
       <c r="K63">
-        <v>76</v>
+        <v>87</v>
       </c>
     </row>
     <row r="64" spans="1:11">
@@ -7810,7 +7810,7 @@
         <v>1202</v>
       </c>
       <c r="K64">
-        <v>140</v>
+        <v>144</v>
       </c>
     </row>
     <row r="65" spans="1:11">
@@ -7845,7 +7845,7 @@
         <v>1879</v>
       </c>
       <c r="K65">
-        <v>230</v>
+        <v>233</v>
       </c>
     </row>
     <row r="66" spans="1:11">
@@ -7915,7 +7915,7 @@
         <v>2745</v>
       </c>
       <c r="K67">
-        <v>310</v>
+        <v>315</v>
       </c>
     </row>
     <row r="68" spans="1:11">
@@ -7950,7 +7950,7 @@
         <v>420</v>
       </c>
       <c r="K68">
-        <v>54</v>
+        <v>55</v>
       </c>
     </row>
     <row r="69" spans="1:11">
@@ -7985,7 +7985,7 @@
         <v>495</v>
       </c>
       <c r="K69">
-        <v>88</v>
+        <v>91</v>
       </c>
     </row>
     <row r="70" spans="1:11">
@@ -8020,7 +8020,7 @@
         <v>738</v>
       </c>
       <c r="K70">
-        <v>95</v>
+        <v>97</v>
       </c>
     </row>
     <row r="71" spans="1:11">
@@ -8055,7 +8055,7 @@
         <v>449</v>
       </c>
       <c r="K71">
-        <v>63</v>
+        <v>64</v>
       </c>
     </row>
     <row r="72" spans="1:11">
@@ -8090,7 +8090,7 @@
         <v>766</v>
       </c>
       <c r="K72">
-        <v>103</v>
+        <v>105</v>
       </c>
     </row>
     <row r="73" spans="1:11">
@@ -8125,7 +8125,7 @@
         <v>1682</v>
       </c>
       <c r="K73">
-        <v>197</v>
+        <v>201</v>
       </c>
     </row>
     <row r="74" spans="1:11">
@@ -8160,7 +8160,7 @@
         <v>312</v>
       </c>
       <c r="K74">
-        <v>41</v>
+        <v>43</v>
       </c>
     </row>
     <row r="75" spans="1:11">
@@ -8230,7 +8230,7 @@
         <v>3193</v>
       </c>
       <c r="K76">
-        <v>387</v>
+        <v>392</v>
       </c>
     </row>
     <row r="77" spans="1:11">
@@ -8262,10 +8262,10 @@
         <v>466</v>
       </c>
       <c r="J77">
-        <v>522</v>
+        <v>523</v>
       </c>
       <c r="K77">
-        <v>61</v>
+        <v>62</v>
       </c>
     </row>
     <row r="78" spans="1:11">
@@ -8300,7 +8300,7 @@
         <v>2011</v>
       </c>
       <c r="K78">
-        <v>327</v>
+        <v>332</v>
       </c>
     </row>
     <row r="79" spans="1:11">
@@ -8335,7 +8335,7 @@
         <v>2630</v>
       </c>
       <c r="K79">
-        <v>304</v>
+        <v>307</v>
       </c>
     </row>
     <row r="80" spans="1:11">
@@ -8370,7 +8370,7 @@
         <v>355</v>
       </c>
       <c r="K80">
-        <v>51</v>
+        <v>53</v>
       </c>
     </row>
     <row r="81" spans="1:11">
@@ -8405,7 +8405,7 @@
         <v>256</v>
       </c>
       <c r="K81">
-        <v>26</v>
+        <v>27</v>
       </c>
     </row>
     <row r="82" spans="1:11">
@@ -8440,7 +8440,7 @@
         <v>283</v>
       </c>
       <c r="K82">
-        <v>41</v>
+        <v>42</v>
       </c>
     </row>
     <row r="83" spans="1:11">
@@ -8475,7 +8475,7 @@
         <v>1811</v>
       </c>
       <c r="K83">
-        <v>188</v>
+        <v>191</v>
       </c>
     </row>
     <row r="84" spans="1:11">
@@ -8510,7 +8510,7 @@
         <v>976</v>
       </c>
       <c r="K84">
-        <v>117</v>
+        <v>118</v>
       </c>
     </row>
     <row r="85" spans="1:11">
@@ -8545,7 +8545,7 @@
         <v>4213</v>
       </c>
       <c r="K85">
-        <v>514</v>
+        <v>518</v>
       </c>
     </row>
     <row r="86" spans="1:11">
@@ -8580,7 +8580,7 @@
         <v>1001</v>
       </c>
       <c r="K86">
-        <v>122</v>
+        <v>126</v>
       </c>
     </row>
     <row r="87" spans="1:11">
@@ -8615,7 +8615,7 @@
         <v>418</v>
       </c>
       <c r="K87">
-        <v>35</v>
+        <v>36</v>
       </c>
     </row>
     <row r="88" spans="1:11">
@@ -8650,7 +8650,7 @@
         <v>1060</v>
       </c>
       <c r="K88">
-        <v>132</v>
+        <v>138</v>
       </c>
     </row>
     <row r="89" spans="1:11">
@@ -8685,7 +8685,7 @@
         <v>2258</v>
       </c>
       <c r="K89">
-        <v>268</v>
+        <v>272</v>
       </c>
     </row>
     <row r="90" spans="1:11">
@@ -8755,7 +8755,7 @@
         <v>1144</v>
       </c>
       <c r="K91">
-        <v>122</v>
+        <v>127</v>
       </c>
     </row>
     <row r="92" spans="1:11">
@@ -8790,7 +8790,7 @@
         <v>457</v>
       </c>
       <c r="K92">
-        <v>49</v>
+        <v>50</v>
       </c>
     </row>
     <row r="93" spans="1:11">
@@ -8825,7 +8825,7 @@
         <v>849</v>
       </c>
       <c r="K93">
-        <v>115</v>
+        <v>117</v>
       </c>
     </row>
     <row r="94" spans="1:11">
@@ -8860,7 +8860,7 @@
         <v>2778</v>
       </c>
       <c r="K94">
-        <v>385</v>
+        <v>394</v>
       </c>
     </row>
     <row r="95" spans="1:11">
@@ -8895,7 +8895,7 @@
         <v>1485</v>
       </c>
       <c r="K95">
-        <v>197</v>
+        <v>199</v>
       </c>
     </row>
     <row r="96" spans="1:11">
@@ -8930,7 +8930,7 @@
         <v>1808</v>
       </c>
       <c r="K96">
-        <v>264</v>
+        <v>267</v>
       </c>
     </row>
     <row r="97" spans="1:11">
@@ -8965,7 +8965,7 @@
         <v>1902</v>
       </c>
       <c r="K97">
-        <v>253</v>
+        <v>256</v>
       </c>
     </row>
     <row r="98" spans="1:11">
@@ -9000,7 +9000,7 @@
         <v>1351</v>
       </c>
       <c r="K98">
-        <v>214</v>
+        <v>218</v>
       </c>
     </row>
     <row r="99" spans="1:11">
@@ -9035,7 +9035,7 @@
         <v>1727</v>
       </c>
       <c r="K99">
-        <v>198</v>
+        <v>207</v>
       </c>
     </row>
     <row r="100" spans="1:11">
@@ -9070,7 +9070,7 @@
         <v>318</v>
       </c>
       <c r="K100">
-        <v>37</v>
+        <v>40</v>
       </c>
     </row>
     <row r="101" spans="1:11">
@@ -9102,10 +9102,10 @@
         <v>110574</v>
       </c>
       <c r="J101">
-        <v>123684</v>
+        <v>123686</v>
       </c>
       <c r="K101">
-        <v>15276</v>
+        <v>15552</v>
       </c>
     </row>
   </sheetData>
@@ -9876,7 +9876,7 @@
         <v>98</v>
       </c>
       <c r="K8">
-        <v>19</v>
+        <v>20</v>
       </c>
     </row>
     <row r="9" spans="1:11">
@@ -9978,7 +9978,7 @@
         <v>299</v>
       </c>
       <c r="K11">
-        <v>53</v>
+        <v>54</v>
       </c>
     </row>
   </sheetData>
@@ -10173,7 +10173,7 @@
         <v>66</v>
       </c>
       <c r="K5">
-        <v>6</v>
+        <v>8</v>
       </c>
     </row>
     <row r="6" spans="1:11">
@@ -10275,7 +10275,7 @@
         <v>365</v>
       </c>
       <c r="K8">
-        <v>32</v>
+        <v>33</v>
       </c>
     </row>
     <row r="9" spans="1:11">
@@ -10345,7 +10345,7 @@
         <v>579</v>
       </c>
       <c r="K10">
-        <v>80</v>
+        <v>81</v>
       </c>
     </row>
     <row r="11" spans="1:11">
@@ -10380,7 +10380,7 @@
         <v>1202</v>
       </c>
       <c r="K11">
-        <v>140</v>
+        <v>144</v>
       </c>
     </row>
   </sheetData>
@@ -10581,7 +10581,7 @@
         <v>78</v>
       </c>
       <c r="K5">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="6" spans="1:11">
@@ -10756,7 +10756,7 @@
         <v>491</v>
       </c>
       <c r="K10">
-        <v>88</v>
+        <v>89</v>
       </c>
     </row>
     <row r="11" spans="1:11">
@@ -10791,7 +10791,7 @@
         <v>1485</v>
       </c>
       <c r="K11">
-        <v>197</v>
+        <v>199</v>
       </c>
     </row>
   </sheetData>
@@ -10887,7 +10887,7 @@
         <v>273</v>
       </c>
       <c r="K2">
-        <v>22</v>
+        <v>23</v>
       </c>
     </row>
     <row r="3" spans="1:11">
@@ -11097,7 +11097,7 @@
         <v>891</v>
       </c>
       <c r="K8">
-        <v>87</v>
+        <v>88</v>
       </c>
     </row>
     <row r="9" spans="1:11">
@@ -11167,7 +11167,7 @@
         <v>936</v>
       </c>
       <c r="K10">
-        <v>125</v>
+        <v>126</v>
       </c>
     </row>
     <row r="11" spans="1:11">
@@ -11202,7 +11202,7 @@
         <v>2972</v>
       </c>
       <c r="K11">
-        <v>354</v>
+        <v>357</v>
       </c>
     </row>
   </sheetData>
@@ -11298,7 +11298,7 @@
         <v>211</v>
       </c>
       <c r="K2">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="3" spans="1:11">
@@ -11575,7 +11575,7 @@
         <v>643</v>
       </c>
       <c r="K10">
-        <v>68</v>
+        <v>70</v>
       </c>
     </row>
     <row r="11" spans="1:11">
@@ -11610,7 +11610,7 @@
         <v>1879</v>
       </c>
       <c r="K11">
-        <v>230</v>
+        <v>233</v>
       </c>
     </row>
   </sheetData>
@@ -12315,7 +12315,7 @@
         <v>493</v>
       </c>
       <c r="K8">
-        <v>40</v>
+        <v>43</v>
       </c>
     </row>
     <row r="9" spans="1:11">
@@ -12385,7 +12385,7 @@
         <v>629</v>
       </c>
       <c r="K10">
-        <v>81</v>
+        <v>87</v>
       </c>
     </row>
     <row r="11" spans="1:11">
@@ -12420,7 +12420,7 @@
         <v>1727</v>
       </c>
       <c r="K11">
-        <v>198</v>
+        <v>207</v>
       </c>
     </row>
   </sheetData>
@@ -13180,7 +13180,7 @@
         <v>404</v>
       </c>
       <c r="K10">
-        <v>64</v>
+        <v>68</v>
       </c>
     </row>
     <row r="11" spans="1:11">
@@ -13215,7 +13215,7 @@
         <v>1031</v>
       </c>
       <c r="K11">
-        <v>149</v>
+        <v>153</v>
       </c>
     </row>
   </sheetData>
@@ -13917,7 +13917,7 @@
         <v>664</v>
       </c>
       <c r="K8">
-        <v>66</v>
+        <v>69</v>
       </c>
     </row>
     <row r="9" spans="1:11">
@@ -13987,7 +13987,7 @@
         <v>884</v>
       </c>
       <c r="K10">
-        <v>81</v>
+        <v>83</v>
       </c>
     </row>
     <row r="11" spans="1:11">
@@ -14022,7 +14022,7 @@
         <v>2745</v>
       </c>
       <c r="K11">
-        <v>310</v>
+        <v>315</v>
       </c>
     </row>
   </sheetData>
@@ -14392,7 +14392,7 @@
         <v>338</v>
       </c>
       <c r="K10">
-        <v>57</v>
+        <v>58</v>
       </c>
     </row>
     <row r="11" spans="1:11">
@@ -14427,7 +14427,7 @@
         <v>976</v>
       </c>
       <c r="K11">
-        <v>117</v>
+        <v>118</v>
       </c>
     </row>
   </sheetData>
@@ -14712,7 +14712,7 @@
         <v>422</v>
       </c>
       <c r="K8">
-        <v>45</v>
+        <v>47</v>
       </c>
     </row>
     <row r="9" spans="1:11">
@@ -14782,7 +14782,7 @@
         <v>1911</v>
       </c>
       <c r="K10">
-        <v>285</v>
+        <v>292</v>
       </c>
     </row>
     <row r="11" spans="1:11">
@@ -14817,7 +14817,7 @@
         <v>2778</v>
       </c>
       <c r="K11">
-        <v>385</v>
+        <v>394</v>
       </c>
     </row>
   </sheetData>
@@ -15114,7 +15114,7 @@
         <v>331</v>
       </c>
       <c r="K8">
-        <v>46</v>
+        <v>47</v>
       </c>
     </row>
     <row r="9" spans="1:11">
@@ -15184,7 +15184,7 @@
         <v>2311</v>
       </c>
       <c r="K10">
-        <v>269</v>
+        <v>273</v>
       </c>
     </row>
     <row r="11" spans="1:11">
@@ -15219,7 +15219,7 @@
         <v>3193</v>
       </c>
       <c r="K11">
-        <v>387</v>
+        <v>392</v>
       </c>
     </row>
   </sheetData>
@@ -15501,7 +15501,7 @@
         <v>88</v>
       </c>
       <c r="K8">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="9" spans="1:11">
@@ -15603,7 +15603,7 @@
         <v>418</v>
       </c>
       <c r="K11">
-        <v>35</v>
+        <v>36</v>
       </c>
     </row>
   </sheetData>
@@ -16304,7 +16304,7 @@
         <v>23</v>
       </c>
       <c r="K9">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="10" spans="1:11">
@@ -16339,7 +16339,7 @@
         <v>210</v>
       </c>
       <c r="K10">
-        <v>25</v>
+        <v>27</v>
       </c>
     </row>
     <row r="11" spans="1:11">
@@ -16374,7 +16374,7 @@
         <v>318</v>
       </c>
       <c r="K11">
-        <v>37</v>
+        <v>40</v>
       </c>
     </row>
   </sheetData>
@@ -16638,7 +16638,7 @@
         <v>119</v>
       </c>
       <c r="K8">
-        <v>15</v>
+        <v>16</v>
       </c>
     </row>
     <row r="9" spans="1:11">
@@ -16743,7 +16743,7 @@
         <v>828</v>
       </c>
       <c r="K11">
-        <v>107</v>
+        <v>108</v>
       </c>
     </row>
   </sheetData>
@@ -17031,7 +17031,7 @@
         <v>239</v>
       </c>
       <c r="K8">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="9" spans="1:11">
@@ -17066,7 +17066,7 @@
         <v>100</v>
       </c>
       <c r="K9">
-        <v>15</v>
+        <v>16</v>
       </c>
     </row>
     <row r="10" spans="1:11">
@@ -17101,7 +17101,7 @@
         <v>1268</v>
       </c>
       <c r="K10">
-        <v>185</v>
+        <v>188</v>
       </c>
     </row>
     <row r="11" spans="1:11">
@@ -17136,7 +17136,7 @@
         <v>1840</v>
       </c>
       <c r="K11">
-        <v>246</v>
+        <v>251</v>
       </c>
     </row>
   </sheetData>
@@ -17433,7 +17433,7 @@
         <v>496</v>
       </c>
       <c r="K8">
-        <v>63</v>
+        <v>64</v>
       </c>
     </row>
     <row r="9" spans="1:11">
@@ -17503,7 +17503,7 @@
         <v>1012</v>
       </c>
       <c r="K10">
-        <v>135</v>
+        <v>137</v>
       </c>
     </row>
     <row r="11" spans="1:11">
@@ -17538,7 +17538,7 @@
         <v>1902</v>
       </c>
       <c r="K11">
-        <v>253</v>
+        <v>256</v>
       </c>
     </row>
   </sheetData>
@@ -17669,7 +17669,7 @@
         <v>83</v>
       </c>
       <c r="K3">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="4" spans="1:11">
@@ -17739,7 +17739,7 @@
         <v>168</v>
       </c>
       <c r="K5">
-        <v>20</v>
+        <v>21</v>
       </c>
     </row>
     <row r="6" spans="1:11">
@@ -17876,7 +17876,7 @@
         <v>128</v>
       </c>
       <c r="K9">
-        <v>29</v>
+        <v>30</v>
       </c>
     </row>
     <row r="10" spans="1:11">
@@ -17946,7 +17946,7 @@
         <v>1808</v>
       </c>
       <c r="K11">
-        <v>264</v>
+        <v>267</v>
       </c>
     </row>
   </sheetData>
@@ -18316,7 +18316,7 @@
         <v>619</v>
       </c>
       <c r="K10">
-        <v>86</v>
+        <v>91</v>
       </c>
     </row>
     <row r="11" spans="1:11">
@@ -18351,7 +18351,7 @@
         <v>1477</v>
       </c>
       <c r="K11">
-        <v>174</v>
+        <v>179</v>
       </c>
     </row>
   </sheetData>
@@ -18552,7 +18552,7 @@
         <v>92</v>
       </c>
       <c r="K5">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="6" spans="1:11">
@@ -18654,7 +18654,7 @@
         <v>419</v>
       </c>
       <c r="K8">
-        <v>68</v>
+        <v>71</v>
       </c>
     </row>
     <row r="9" spans="1:11">
@@ -18689,7 +18689,7 @@
         <v>264</v>
       </c>
       <c r="K9">
-        <v>25</v>
+        <v>27</v>
       </c>
     </row>
     <row r="10" spans="1:11">
@@ -18724,7 +18724,7 @@
         <v>2806</v>
       </c>
       <c r="K10">
-        <v>395</v>
+        <v>403</v>
       </c>
     </row>
     <row r="11" spans="1:11">
@@ -18759,7 +18759,7 @@
         <v>3895</v>
       </c>
       <c r="K11">
-        <v>542</v>
+        <v>556</v>
       </c>
     </row>
   </sheetData>
@@ -19062,7 +19062,7 @@
         <v>384</v>
       </c>
       <c r="K8">
-        <v>51</v>
+        <v>52</v>
       </c>
     </row>
     <row r="9" spans="1:11">
@@ -19097,7 +19097,7 @@
         <v>105</v>
       </c>
       <c r="K9">
-        <v>16</v>
+        <v>17</v>
       </c>
     </row>
     <row r="10" spans="1:11">
@@ -19132,7 +19132,7 @@
         <v>884</v>
       </c>
       <c r="K10">
-        <v>94</v>
+        <v>96</v>
       </c>
     </row>
     <row r="11" spans="1:11">
@@ -19167,7 +19167,7 @@
         <v>1682</v>
       </c>
       <c r="K11">
-        <v>197</v>
+        <v>201</v>
       </c>
     </row>
   </sheetData>
@@ -19368,7 +19368,7 @@
         <v>250</v>
       </c>
       <c r="K5">
-        <v>26</v>
+        <v>27</v>
       </c>
     </row>
     <row r="6" spans="1:11">
@@ -19403,7 +19403,7 @@
         <v>83</v>
       </c>
       <c r="K6">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="7" spans="1:11">
@@ -19473,7 +19473,7 @@
         <v>1031</v>
       </c>
       <c r="K8">
-        <v>117</v>
+        <v>121</v>
       </c>
     </row>
     <row r="9" spans="1:11">
@@ -19508,7 +19508,7 @@
         <v>399</v>
       </c>
       <c r="K9">
-        <v>68</v>
+        <v>69</v>
       </c>
     </row>
     <row r="10" spans="1:11">
@@ -19543,7 +19543,7 @@
         <v>1304</v>
       </c>
       <c r="K10">
-        <v>142</v>
+        <v>144</v>
       </c>
     </row>
     <row r="11" spans="1:11">
@@ -19578,7 +19578,7 @@
         <v>4178</v>
       </c>
       <c r="K11">
-        <v>454</v>
+        <v>461</v>
       </c>
     </row>
   </sheetData>
@@ -19773,7 +19773,7 @@
         <v>181</v>
       </c>
       <c r="J5">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="K5">
         <v>24</v>
@@ -19872,7 +19872,7 @@
         <v>462</v>
       </c>
       <c r="K8">
-        <v>41</v>
+        <v>42</v>
       </c>
     </row>
     <row r="9" spans="1:11">
@@ -19942,7 +19942,7 @@
         <v>2120</v>
       </c>
       <c r="K10">
-        <v>276</v>
+        <v>280</v>
       </c>
     </row>
     <row r="11" spans="1:11">
@@ -19974,10 +19974,10 @@
         <v>2649</v>
       </c>
       <c r="J11">
-        <v>3090</v>
+        <v>3091</v>
       </c>
       <c r="K11">
-        <v>374</v>
+        <v>379</v>
       </c>
     </row>
   </sheetData>
@@ -20073,7 +20073,7 @@
         <v>212</v>
       </c>
       <c r="K2">
-        <v>30</v>
+        <v>31</v>
       </c>
     </row>
     <row r="3" spans="1:11">
@@ -20178,7 +20178,7 @@
         <v>197</v>
       </c>
       <c r="K5">
-        <v>26</v>
+        <v>27</v>
       </c>
     </row>
     <row r="6" spans="1:11">
@@ -20283,7 +20283,7 @@
         <v>774</v>
       </c>
       <c r="K8">
-        <v>89</v>
+        <v>91</v>
       </c>
     </row>
     <row r="9" spans="1:11">
@@ -20353,7 +20353,7 @@
         <v>1014</v>
       </c>
       <c r="K10">
-        <v>141</v>
+        <v>143</v>
       </c>
     </row>
     <row r="11" spans="1:11">
@@ -20388,7 +20388,7 @@
         <v>2861</v>
       </c>
       <c r="K11">
-        <v>354</v>
+        <v>360</v>
       </c>
     </row>
   </sheetData>
@@ -20894,7 +20894,7 @@
         <v>51</v>
       </c>
       <c r="K3">
-        <v>8</v>
+        <v>10</v>
       </c>
     </row>
     <row r="4" spans="1:11">
@@ -21133,7 +21133,7 @@
         <v>722</v>
       </c>
       <c r="K10">
-        <v>104</v>
+        <v>105</v>
       </c>
     </row>
     <row r="11" spans="1:11">
@@ -21168,7 +21168,7 @@
         <v>1382</v>
       </c>
       <c r="K11">
-        <v>200</v>
+        <v>203</v>
       </c>
     </row>
   </sheetData>
@@ -21369,7 +21369,7 @@
         <v>180</v>
       </c>
       <c r="K5">
-        <v>22</v>
+        <v>23</v>
       </c>
     </row>
     <row r="6" spans="1:11">
@@ -21471,7 +21471,7 @@
         <v>910</v>
       </c>
       <c r="K8">
-        <v>101</v>
+        <v>104</v>
       </c>
     </row>
     <row r="9" spans="1:11">
@@ -21506,7 +21506,7 @@
         <v>653</v>
       </c>
       <c r="K9">
-        <v>46</v>
+        <v>48</v>
       </c>
     </row>
     <row r="10" spans="1:11">
@@ -21541,7 +21541,7 @@
         <v>1268</v>
       </c>
       <c r="K10">
-        <v>122</v>
+        <v>123</v>
       </c>
     </row>
     <row r="11" spans="1:11">
@@ -21576,7 +21576,7 @@
         <v>3619</v>
       </c>
       <c r="K11">
-        <v>362</v>
+        <v>369</v>
       </c>
     </row>
   </sheetData>
@@ -21934,7 +21934,7 @@
         <v>256</v>
       </c>
       <c r="K10">
-        <v>17</v>
+        <v>18</v>
       </c>
     </row>
     <row r="11" spans="1:11">
@@ -21969,7 +21969,7 @@
         <v>538</v>
       </c>
       <c r="K11">
-        <v>48</v>
+        <v>49</v>
       </c>
     </row>
   </sheetData>
@@ -22100,7 +22100,7 @@
         <v>253</v>
       </c>
       <c r="K3">
-        <v>25</v>
+        <v>27</v>
       </c>
     </row>
     <row r="4" spans="1:11">
@@ -22272,7 +22272,7 @@
         <v>943</v>
       </c>
       <c r="K8">
-        <v>90</v>
+        <v>93</v>
       </c>
     </row>
     <row r="9" spans="1:11">
@@ -22342,7 +22342,7 @@
         <v>979</v>
       </c>
       <c r="K10">
-        <v>118</v>
+        <v>121</v>
       </c>
     </row>
     <row r="11" spans="1:11">
@@ -22377,7 +22377,7 @@
         <v>2985</v>
       </c>
       <c r="K11">
-        <v>328</v>
+        <v>336</v>
       </c>
     </row>
   </sheetData>
@@ -22741,7 +22741,7 @@
         <v>411</v>
       </c>
       <c r="K10">
-        <v>72</v>
+        <v>73</v>
       </c>
     </row>
     <row r="11" spans="1:11">
@@ -22776,7 +22776,7 @@
         <v>1102</v>
       </c>
       <c r="K11">
-        <v>147</v>
+        <v>148</v>
       </c>
     </row>
   </sheetData>
@@ -23545,7 +23545,7 @@
         <v>631</v>
       </c>
       <c r="K10">
-        <v>69</v>
+        <v>70</v>
       </c>
     </row>
     <row r="11" spans="1:11">
@@ -23580,7 +23580,7 @@
         <v>1736</v>
       </c>
       <c r="K11">
-        <v>183</v>
+        <v>184</v>
       </c>
     </row>
   </sheetData>
@@ -24127,7 +24127,7 @@
         <v>65</v>
       </c>
       <c r="K5">
-        <v>15</v>
+        <v>16</v>
       </c>
     </row>
     <row r="6" spans="1:11">
@@ -24226,7 +24226,7 @@
         <v>228</v>
       </c>
       <c r="K8">
-        <v>22</v>
+        <v>24</v>
       </c>
     </row>
     <row r="9" spans="1:11">
@@ -24296,7 +24296,7 @@
         <v>650</v>
       </c>
       <c r="K10">
-        <v>99</v>
+        <v>101</v>
       </c>
     </row>
     <row r="11" spans="1:11">
@@ -24331,7 +24331,7 @@
         <v>1153</v>
       </c>
       <c r="K11">
-        <v>160</v>
+        <v>165</v>
       </c>
     </row>
   </sheetData>
@@ -24517,7 +24517,7 @@
         <v>20</v>
       </c>
       <c r="K5">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="6" spans="1:11">
@@ -24671,7 +24671,7 @@
         <v>693</v>
       </c>
       <c r="K10">
-        <v>84</v>
+        <v>87</v>
       </c>
     </row>
     <row r="11" spans="1:11">
@@ -24706,7 +24706,7 @@
         <v>1001</v>
       </c>
       <c r="K11">
-        <v>122</v>
+        <v>126</v>
       </c>
     </row>
   </sheetData>
@@ -25009,7 +25009,7 @@
         <v>430</v>
       </c>
       <c r="K8">
-        <v>69</v>
+        <v>71</v>
       </c>
     </row>
     <row r="9" spans="1:11">
@@ -25044,7 +25044,7 @@
         <v>106</v>
       </c>
       <c r="K9">
-        <v>18</v>
+        <v>19</v>
       </c>
     </row>
     <row r="10" spans="1:11">
@@ -25079,7 +25079,7 @@
         <v>1134</v>
       </c>
       <c r="K10">
-        <v>185</v>
+        <v>187</v>
       </c>
     </row>
     <row r="11" spans="1:11">
@@ -25114,7 +25114,7 @@
         <v>2011</v>
       </c>
       <c r="K11">
-        <v>327</v>
+        <v>332</v>
       </c>
     </row>
   </sheetData>
@@ -25469,7 +25469,7 @@
         <v>227</v>
       </c>
       <c r="K10">
-        <v>32</v>
+        <v>33</v>
       </c>
     </row>
     <row r="11" spans="1:11">
@@ -25504,7 +25504,7 @@
         <v>420</v>
       </c>
       <c r="K11">
-        <v>54</v>
+        <v>55</v>
       </c>
     </row>
   </sheetData>
@@ -26024,6 +26024,9 @@
       <c r="J3">
         <v>74</v>
       </c>
+      <c r="K3">
+        <v>1</v>
+      </c>
     </row>
     <row r="4" spans="1:11">
       <c r="A4" s="1" t="s">
@@ -26261,10 +26264,10 @@
         <v>390</v>
       </c>
       <c r="J10">
-        <v>423</v>
+        <v>424</v>
       </c>
       <c r="K10">
-        <v>71</v>
+        <v>75</v>
       </c>
     </row>
     <row r="11" spans="1:11">
@@ -26296,10 +26299,10 @@
         <v>888</v>
       </c>
       <c r="J11">
-        <v>1070</v>
+        <v>1071</v>
       </c>
       <c r="K11">
-        <v>137</v>
+        <v>142</v>
       </c>
     </row>
   </sheetData>
@@ -26631,7 +26634,7 @@
         <v>111</v>
       </c>
       <c r="J9">
-        <v>259</v>
+        <v>260</v>
       </c>
       <c r="K9">
         <v>35</v>
@@ -26669,7 +26672,7 @@
         <v>962</v>
       </c>
       <c r="K10">
-        <v>147</v>
+        <v>149</v>
       </c>
     </row>
     <row r="11" spans="1:11">
@@ -26701,10 +26704,10 @@
         <v>1720</v>
       </c>
       <c r="J11">
-        <v>2168</v>
+        <v>2169</v>
       </c>
       <c r="K11">
-        <v>305</v>
+        <v>307</v>
       </c>
     </row>
   </sheetData>
@@ -26998,7 +27001,7 @@
         <v>592</v>
       </c>
       <c r="K8">
-        <v>38</v>
+        <v>39</v>
       </c>
     </row>
     <row r="9" spans="1:11">
@@ -27068,7 +27071,7 @@
         <v>677</v>
       </c>
       <c r="K10">
-        <v>76</v>
+        <v>78</v>
       </c>
     </row>
     <row r="11" spans="1:11">
@@ -27103,7 +27106,7 @@
         <v>1593</v>
       </c>
       <c r="K11">
-        <v>149</v>
+        <v>152</v>
       </c>
     </row>
   </sheetData>
@@ -27335,6 +27338,9 @@
       <c r="J6">
         <v>16</v>
       </c>
+      <c r="K6">
+        <v>1</v>
+      </c>
     </row>
     <row r="7" spans="1:11">
       <c r="A7" s="1" t="s">
@@ -27403,7 +27409,7 @@
         <v>402</v>
       </c>
       <c r="K8">
-        <v>31</v>
+        <v>32</v>
       </c>
     </row>
     <row r="9" spans="1:11">
@@ -27473,7 +27479,7 @@
         <v>341</v>
       </c>
       <c r="K10">
-        <v>42</v>
+        <v>45</v>
       </c>
     </row>
     <row r="11" spans="1:11">
@@ -27508,7 +27514,7 @@
         <v>1144</v>
       </c>
       <c r="K11">
-        <v>122</v>
+        <v>127</v>
       </c>
     </row>
   </sheetData>
@@ -27808,7 +27814,7 @@
         <v>467</v>
       </c>
       <c r="K8">
-        <v>49</v>
+        <v>51</v>
       </c>
     </row>
     <row r="9" spans="1:11">
@@ -27878,7 +27884,7 @@
         <v>749</v>
       </c>
       <c r="K10">
-        <v>113</v>
+        <v>115</v>
       </c>
     </row>
     <row r="11" spans="1:11">
@@ -27913,7 +27919,7 @@
         <v>1653</v>
       </c>
       <c r="K11">
-        <v>221</v>
+        <v>225</v>
       </c>
     </row>
   </sheetData>
@@ -28044,7 +28050,7 @@
         <v>208</v>
       </c>
       <c r="K3">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="4" spans="1:11">
@@ -28079,7 +28085,7 @@
         <v>13</v>
       </c>
       <c r="K4">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="5" spans="1:11">
@@ -28216,7 +28222,7 @@
         <v>564</v>
       </c>
       <c r="K8">
-        <v>69</v>
+        <v>71</v>
       </c>
     </row>
     <row r="9" spans="1:11">
@@ -28251,7 +28257,7 @@
         <v>183</v>
       </c>
       <c r="K9">
-        <v>37</v>
+        <v>38</v>
       </c>
     </row>
     <row r="10" spans="1:11">
@@ -28321,7 +28327,7 @@
         <v>2178</v>
       </c>
       <c r="K11">
-        <v>246</v>
+        <v>251</v>
       </c>
     </row>
   </sheetData>
@@ -28876,7 +28882,7 @@
         <v>50</v>
       </c>
       <c r="K5">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="6" spans="1:11">
@@ -29013,7 +29019,7 @@
         <v>96</v>
       </c>
       <c r="K9">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="10" spans="1:11">
@@ -29083,7 +29089,7 @@
         <v>1025</v>
       </c>
       <c r="K11">
-        <v>156</v>
+        <v>158</v>
       </c>
     </row>
   </sheetData>
@@ -29779,7 +29785,7 @@
         <v>185</v>
       </c>
       <c r="K8">
-        <v>18</v>
+        <v>19</v>
       </c>
     </row>
     <row r="9" spans="1:11">
@@ -29849,7 +29855,7 @@
         <v>637</v>
       </c>
       <c r="K10">
-        <v>72</v>
+        <v>73</v>
       </c>
     </row>
     <row r="11" spans="1:11">
@@ -29884,7 +29890,7 @@
         <v>1138</v>
       </c>
       <c r="K11">
-        <v>132</v>
+        <v>134</v>
       </c>
     </row>
   </sheetData>
@@ -30175,7 +30181,7 @@
         <v>268</v>
       </c>
       <c r="K8">
-        <v>43</v>
+        <v>45</v>
       </c>
     </row>
     <row r="9" spans="1:11">
@@ -30280,7 +30286,7 @@
         <v>849</v>
       </c>
       <c r="K11">
-        <v>115</v>
+        <v>117</v>
       </c>
     </row>
   </sheetData>
@@ -30580,7 +30586,7 @@
         <v>254</v>
       </c>
       <c r="K8">
-        <v>33</v>
+        <v>35</v>
       </c>
     </row>
     <row r="9" spans="1:11">
@@ -30650,7 +30656,7 @@
         <v>311</v>
       </c>
       <c r="K10">
-        <v>49</v>
+        <v>51</v>
       </c>
     </row>
     <row r="11" spans="1:11">
@@ -30685,7 +30691,7 @@
         <v>859</v>
       </c>
       <c r="K11">
-        <v>117</v>
+        <v>121</v>
       </c>
     </row>
   </sheetData>
@@ -30903,7 +30909,7 @@
         <v>5</v>
       </c>
       <c r="K6">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="7" spans="1:11">
@@ -30949,7 +30955,7 @@
         <v>132</v>
       </c>
       <c r="K8">
-        <v>26</v>
+        <v>27</v>
       </c>
     </row>
     <row r="9" spans="1:11">
@@ -31054,7 +31060,7 @@
         <v>738</v>
       </c>
       <c r="K11">
-        <v>95</v>
+        <v>97</v>
       </c>
     </row>
   </sheetData>
@@ -31284,7 +31290,7 @@
         <v>7</v>
       </c>
       <c r="J6">
-        <v>18</v>
+        <v>19</v>
       </c>
     </row>
     <row r="7" spans="1:11">
@@ -31421,7 +31427,7 @@
         <v>150</v>
       </c>
       <c r="K10">
-        <v>22</v>
+        <v>23</v>
       </c>
     </row>
     <row r="11" spans="1:11">
@@ -31453,10 +31459,10 @@
         <v>466</v>
       </c>
       <c r="J11">
-        <v>522</v>
+        <v>523</v>
       </c>
       <c r="K11">
-        <v>61</v>
+        <v>62</v>
       </c>
     </row>
   </sheetData>
@@ -31775,7 +31781,7 @@
         <v>612</v>
       </c>
       <c r="K10">
-        <v>85</v>
+        <v>86</v>
       </c>
     </row>
     <row r="11" spans="1:11">
@@ -31810,7 +31816,7 @@
         <v>670</v>
       </c>
       <c r="K11">
-        <v>93</v>
+        <v>94</v>
       </c>
     </row>
   </sheetData>
@@ -32561,7 +32567,7 @@
         <v>624</v>
       </c>
       <c r="K10">
-        <v>83</v>
+        <v>85</v>
       </c>
     </row>
     <row r="11" spans="1:11">
@@ -32596,7 +32602,7 @@
         <v>1142</v>
       </c>
       <c r="K11">
-        <v>145</v>
+        <v>147</v>
       </c>
     </row>
   </sheetData>
@@ -32884,7 +32890,7 @@
         <v>127</v>
       </c>
       <c r="K8">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="9" spans="1:11">
@@ -32919,7 +32925,7 @@
         <v>41</v>
       </c>
       <c r="K9">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="10" spans="1:11">
@@ -32989,7 +32995,7 @@
         <v>766</v>
       </c>
       <c r="K11">
-        <v>103</v>
+        <v>105</v>
       </c>
     </row>
   </sheetData>
@@ -33204,7 +33210,7 @@
         <v>14</v>
       </c>
       <c r="J6">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="K6">
         <v>2</v>
@@ -33335,7 +33341,7 @@
         <v>752</v>
       </c>
       <c r="K10">
-        <v>93</v>
+        <v>96</v>
       </c>
     </row>
     <row r="11" spans="1:11">
@@ -33367,10 +33373,10 @@
         <v>1161</v>
       </c>
       <c r="J11">
-        <v>1454</v>
+        <v>1453</v>
       </c>
       <c r="K11">
-        <v>169</v>
+        <v>172</v>
       </c>
     </row>
   </sheetData>
@@ -33643,7 +33649,7 @@
         <v>50</v>
       </c>
       <c r="K8">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="9" spans="1:11">
@@ -33748,7 +33754,7 @@
         <v>145</v>
       </c>
       <c r="K11">
-        <v>14</v>
+        <v>15</v>
       </c>
     </row>
   </sheetData>
@@ -34039,7 +34045,7 @@
         <v>104</v>
       </c>
       <c r="K8">
-        <v>19</v>
+        <v>21</v>
       </c>
     </row>
     <row r="9" spans="1:11">
@@ -34109,7 +34115,7 @@
         <v>244</v>
       </c>
       <c r="K10">
-        <v>31</v>
+        <v>32</v>
       </c>
     </row>
     <row r="11" spans="1:11">
@@ -34144,7 +34150,7 @@
         <v>515</v>
       </c>
       <c r="K11">
-        <v>66</v>
+        <v>69</v>
       </c>
     </row>
   </sheetData>
@@ -34443,7 +34449,7 @@
         <v>29</v>
       </c>
       <c r="K9">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="10" spans="1:11">
@@ -34478,7 +34484,7 @@
         <v>255</v>
       </c>
       <c r="K10">
-        <v>33</v>
+        <v>34</v>
       </c>
     </row>
     <row r="11" spans="1:11">
@@ -34513,7 +34519,7 @@
         <v>355</v>
       </c>
       <c r="K11">
-        <v>51</v>
+        <v>53</v>
       </c>
     </row>
   </sheetData>
@@ -34813,7 +34819,7 @@
         <v>240</v>
       </c>
       <c r="K8">
-        <v>52</v>
+        <v>54</v>
       </c>
     </row>
     <row r="9" spans="1:11">
@@ -34918,7 +34924,7 @@
         <v>950</v>
       </c>
       <c r="K11">
-        <v>155</v>
+        <v>157</v>
       </c>
     </row>
   </sheetData>
@@ -35119,7 +35125,7 @@
         <v>159</v>
       </c>
       <c r="K5">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="6" spans="1:11">
@@ -35253,7 +35259,7 @@
         <v>114</v>
       </c>
       <c r="K9">
-        <v>18</v>
+        <v>19</v>
       </c>
     </row>
     <row r="10" spans="1:11">
@@ -35288,7 +35294,7 @@
         <v>1368</v>
       </c>
       <c r="K10">
-        <v>157</v>
+        <v>159</v>
       </c>
     </row>
     <row r="11" spans="1:11">
@@ -35323,7 +35329,7 @@
         <v>2258</v>
       </c>
       <c r="K11">
-        <v>268</v>
+        <v>272</v>
       </c>
     </row>
   </sheetData>
@@ -35801,6 +35807,9 @@
       <c r="J3">
         <v>10</v>
       </c>
+      <c r="K3">
+        <v>1</v>
+      </c>
     </row>
     <row r="4" spans="1:11">
       <c r="A4" s="1" t="s">
@@ -36017,7 +36026,7 @@
         <v>155</v>
       </c>
       <c r="K10">
-        <v>12</v>
+        <v>13</v>
       </c>
     </row>
   </sheetData>
@@ -36148,7 +36157,7 @@
         <v>12</v>
       </c>
       <c r="K3">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="4" spans="1:11">
@@ -36278,7 +36287,7 @@
         <v>105</v>
       </c>
       <c r="K8">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="9" spans="1:11">
@@ -36383,7 +36392,7 @@
         <v>284</v>
       </c>
       <c r="K11">
-        <v>24</v>
+        <v>26</v>
       </c>
     </row>
   </sheetData>
@@ -36989,7 +36998,7 @@
         <v>235</v>
       </c>
       <c r="K8">
-        <v>17</v>
+        <v>20</v>
       </c>
     </row>
     <row r="9" spans="1:11">
@@ -37059,7 +37068,7 @@
         <v>797</v>
       </c>
       <c r="K10">
-        <v>158</v>
+        <v>159</v>
       </c>
     </row>
     <row r="11" spans="1:11">
@@ -37094,7 +37103,7 @@
         <v>1351</v>
       </c>
       <c r="K11">
-        <v>214</v>
+        <v>218</v>
       </c>
     </row>
   </sheetData>
@@ -37649,7 +37658,7 @@
         <v>51</v>
       </c>
       <c r="K5">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="6" spans="1:11">
@@ -37850,7 +37859,7 @@
         <v>457</v>
       </c>
       <c r="K11">
-        <v>49</v>
+        <v>50</v>
       </c>
     </row>
   </sheetData>
@@ -37946,7 +37955,7 @@
         <v>17</v>
       </c>
       <c r="K2">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="3" spans="1:11">
@@ -38210,7 +38219,7 @@
         <v>166</v>
       </c>
       <c r="K11">
-        <v>20</v>
+        <v>21</v>
       </c>
     </row>
   </sheetData>
@@ -38524,7 +38533,7 @@
         <v>170</v>
       </c>
       <c r="K9">
-        <v>26</v>
+        <v>27</v>
       </c>
     </row>
     <row r="10" spans="1:11">
@@ -38559,7 +38568,7 @@
         <v>283</v>
       </c>
       <c r="K10">
-        <v>41</v>
+        <v>42</v>
       </c>
     </row>
   </sheetData>
@@ -38690,7 +38699,7 @@
         <v>48</v>
       </c>
       <c r="K3">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="4" spans="1:11">
@@ -38964,7 +38973,7 @@
         <v>541</v>
       </c>
       <c r="K11">
-        <v>50</v>
+        <v>51</v>
       </c>
     </row>
   </sheetData>
@@ -39270,7 +39279,7 @@
         <v>1311</v>
       </c>
       <c r="K8">
-        <v>84</v>
+        <v>85</v>
       </c>
     </row>
     <row r="9" spans="1:11">
@@ -39340,7 +39349,7 @@
         <v>1373</v>
       </c>
       <c r="K10">
-        <v>189</v>
+        <v>192</v>
       </c>
     </row>
     <row r="11" spans="1:11">
@@ -39375,7 +39384,7 @@
         <v>4213</v>
       </c>
       <c r="K11">
-        <v>514</v>
+        <v>518</v>
       </c>
     </row>
   </sheetData>
@@ -40420,7 +40429,7 @@
         <v>62</v>
       </c>
       <c r="K9">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="10" spans="1:11">
@@ -40490,7 +40499,7 @@
         <v>552</v>
       </c>
       <c r="K11">
-        <v>68</v>
+        <v>69</v>
       </c>
     </row>
   </sheetData>
@@ -40621,7 +40630,7 @@
         <v>68</v>
       </c>
       <c r="K3">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="4" spans="1:11">
@@ -40796,7 +40805,7 @@
         <v>253</v>
       </c>
       <c r="K8">
-        <v>19</v>
+        <v>22</v>
       </c>
     </row>
     <row r="9" spans="1:11">
@@ -40831,7 +40840,7 @@
         <v>165</v>
       </c>
       <c r="K9">
-        <v>26</v>
+        <v>27</v>
       </c>
     </row>
     <row r="10" spans="1:11">
@@ -40866,7 +40875,7 @@
         <v>427</v>
       </c>
       <c r="K10">
-        <v>50</v>
+        <v>51</v>
       </c>
     </row>
     <row r="11" spans="1:11">
@@ -40901,7 +40910,7 @@
         <v>1060</v>
       </c>
       <c r="K11">
-        <v>132</v>
+        <v>138</v>
       </c>
     </row>
   </sheetData>
@@ -41217,7 +41226,7 @@
         <v>227</v>
       </c>
       <c r="K10">
-        <v>31</v>
+        <v>33</v>
       </c>
     </row>
     <row r="11" spans="1:11">
@@ -41252,7 +41261,7 @@
         <v>312</v>
       </c>
       <c r="K11">
-        <v>41</v>
+        <v>43</v>
       </c>
     </row>
   </sheetData>
@@ -41542,7 +41551,7 @@
         <v>135</v>
       </c>
       <c r="K9">
-        <v>17</v>
+        <v>18</v>
       </c>
     </row>
     <row r="10" spans="1:11">
@@ -41577,7 +41586,7 @@
         <v>202</v>
       </c>
       <c r="K10">
-        <v>28</v>
+        <v>29</v>
       </c>
     </row>
   </sheetData>
@@ -41823,7 +41832,7 @@
         <v>37</v>
       </c>
       <c r="K8">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="9" spans="1:11">
@@ -41928,7 +41937,7 @@
         <v>256</v>
       </c>
       <c r="K11">
-        <v>26</v>
+        <v>27</v>
       </c>
     </row>
   </sheetData>
@@ -42218,7 +42227,7 @@
         <v>229</v>
       </c>
       <c r="K9">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="10" spans="1:11">
@@ -42253,7 +42262,7 @@
         <v>261</v>
       </c>
       <c r="K10">
-        <v>15</v>
+        <v>16</v>
       </c>
     </row>
   </sheetData>
@@ -42445,7 +42454,7 @@
         <v>53</v>
       </c>
       <c r="K5">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="6" spans="1:11">
@@ -42593,7 +42602,7 @@
         <v>207</v>
       </c>
       <c r="K10">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="11" spans="1:11">

</xml_diff>

<commit_message>
Add data for 2024-02-26
</commit_message>
<xml_diff>
--- a/output/index-crime-full-year.xlsx
+++ b/output/index-crime-full-year.xlsx
@@ -31,8 +31,8 @@
     <sheet name="Near South Side" sheetId="22" r:id="rId22"/>
     <sheet name="West Pullman" sheetId="23" r:id="rId23"/>
     <sheet name="Grand Crossing" sheetId="24" r:id="rId24"/>
-    <sheet name="Edgewater" sheetId="25" r:id="rId25"/>
-    <sheet name="New City" sheetId="26" r:id="rId26"/>
+    <sheet name="New City" sheetId="25" r:id="rId25"/>
+    <sheet name="Edgewater" sheetId="26" r:id="rId26"/>
     <sheet name="Woodlawn" sheetId="27" r:id="rId27"/>
     <sheet name="Fuller Park" sheetId="28" r:id="rId28"/>
     <sheet name="Gage Park" sheetId="29" r:id="rId29"/>
@@ -902,7 +902,7 @@
         <v>7704</v>
       </c>
       <c r="K2">
-        <v>1008</v>
+        <v>1034</v>
       </c>
     </row>
     <row r="3" spans="1:11">
@@ -937,7 +937,7 @@
         <v>8076</v>
       </c>
       <c r="K3">
-        <v>963</v>
+        <v>983</v>
       </c>
     </row>
     <row r="4" spans="1:11">
@@ -972,7 +972,7 @@
         <v>510</v>
       </c>
       <c r="K4">
-        <v>63</v>
+        <v>66</v>
       </c>
     </row>
     <row r="5" spans="1:11">
@@ -1007,7 +1007,7 @@
         <v>7462</v>
       </c>
       <c r="K5">
-        <v>972</v>
+        <v>987</v>
       </c>
     </row>
     <row r="6" spans="1:11">
@@ -1024,13 +1024,13 @@
         <v>1965</v>
       </c>
       <c r="E6">
-        <v>2021</v>
+        <v>2022</v>
       </c>
       <c r="F6">
         <v>1907</v>
       </c>
       <c r="G6">
-        <v>1479</v>
+        <v>1480</v>
       </c>
       <c r="H6">
         <v>1720</v>
@@ -1039,10 +1039,10 @@
         <v>1785</v>
       </c>
       <c r="J6">
-        <v>1797</v>
+        <v>1798</v>
       </c>
       <c r="K6">
-        <v>211</v>
+        <v>214</v>
       </c>
     </row>
     <row r="7" spans="1:11">
@@ -1077,7 +1077,7 @@
         <v>625</v>
       </c>
       <c r="K7">
-        <v>56</v>
+        <v>60</v>
       </c>
     </row>
     <row r="8" spans="1:11">
@@ -1109,10 +1109,10 @@
         <v>21457</v>
       </c>
       <c r="J8">
-        <v>29205</v>
+        <v>29206</v>
       </c>
       <c r="K8">
-        <v>3260</v>
+        <v>3335</v>
       </c>
     </row>
     <row r="9" spans="1:11">
@@ -1147,7 +1147,7 @@
         <v>11059</v>
       </c>
       <c r="K9">
-        <v>1318</v>
+        <v>1334</v>
       </c>
     </row>
     <row r="10" spans="1:11">
@@ -1179,10 +1179,10 @@
         <v>54863</v>
       </c>
       <c r="J10">
-        <v>57248</v>
+        <v>57253</v>
       </c>
       <c r="K10">
-        <v>7701</v>
+        <v>7826</v>
       </c>
     </row>
     <row r="11" spans="1:11">
@@ -1199,13 +1199,13 @@
         <v>117366</v>
       </c>
       <c r="E11">
-        <v>113419</v>
+        <v>113420</v>
       </c>
       <c r="F11">
         <v>105585</v>
       </c>
       <c r="G11">
-        <v>85337</v>
+        <v>85338</v>
       </c>
       <c r="H11">
         <v>84633</v>
@@ -1214,10 +1214,10 @@
         <v>110574</v>
       </c>
       <c r="J11">
-        <v>123686</v>
+        <v>123693</v>
       </c>
       <c r="K11">
-        <v>15552</v>
+        <v>15839</v>
       </c>
     </row>
   </sheetData>
@@ -1348,7 +1348,7 @@
         <v>209</v>
       </c>
       <c r="K3">
-        <v>15</v>
+        <v>16</v>
       </c>
     </row>
     <row r="4" spans="1:11">
@@ -1383,7 +1383,7 @@
         <v>21</v>
       </c>
       <c r="K4">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="5" spans="1:11">
@@ -1523,7 +1523,7 @@
         <v>385</v>
       </c>
       <c r="K8">
-        <v>53</v>
+        <v>56</v>
       </c>
     </row>
     <row r="9" spans="1:11">
@@ -1593,7 +1593,7 @@
         <v>693</v>
       </c>
       <c r="K10">
-        <v>105</v>
+        <v>108</v>
       </c>
     </row>
     <row r="11" spans="1:11">
@@ -1628,7 +1628,7 @@
         <v>1923</v>
       </c>
       <c r="K11">
-        <v>250</v>
+        <v>258</v>
       </c>
     </row>
   </sheetData>
@@ -2066,7 +2066,7 @@
         <v>16</v>
       </c>
       <c r="K3">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="4" spans="1:11">
@@ -2284,7 +2284,7 @@
         <v>323</v>
       </c>
       <c r="K10">
-        <v>63</v>
+        <v>65</v>
       </c>
     </row>
     <row r="11" spans="1:11">
@@ -2319,7 +2319,7 @@
         <v>495</v>
       </c>
       <c r="K11">
-        <v>91</v>
+        <v>94</v>
       </c>
     </row>
   </sheetData>
@@ -2415,7 +2415,7 @@
         <v>79</v>
       </c>
       <c r="K2">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="3" spans="1:11">
@@ -2619,7 +2619,7 @@
         <v>472</v>
       </c>
       <c r="K8">
-        <v>64</v>
+        <v>65</v>
       </c>
     </row>
     <row r="9" spans="1:11">
@@ -2654,7 +2654,7 @@
         <v>284</v>
       </c>
       <c r="K9">
-        <v>19</v>
+        <v>20</v>
       </c>
     </row>
     <row r="10" spans="1:11">
@@ -2689,7 +2689,7 @@
         <v>1203</v>
       </c>
       <c r="K10">
-        <v>219</v>
+        <v>221</v>
       </c>
     </row>
     <row r="11" spans="1:11">
@@ -2724,7 +2724,7 @@
         <v>2251</v>
       </c>
       <c r="K11">
-        <v>336</v>
+        <v>341</v>
       </c>
     </row>
   </sheetData>
@@ -2820,7 +2820,7 @@
         <v>488</v>
       </c>
       <c r="K2">
-        <v>59</v>
+        <v>61</v>
       </c>
     </row>
     <row r="3" spans="1:11">
@@ -2890,7 +2890,7 @@
         <v>39</v>
       </c>
       <c r="K4">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="5" spans="1:11">
@@ -2925,7 +2925,7 @@
         <v>224</v>
       </c>
       <c r="K5">
-        <v>29</v>
+        <v>30</v>
       </c>
     </row>
     <row r="6" spans="1:11">
@@ -3030,7 +3030,7 @@
         <v>1245</v>
       </c>
       <c r="K8">
-        <v>148</v>
+        <v>154</v>
       </c>
     </row>
     <row r="9" spans="1:11">
@@ -3065,7 +3065,7 @@
         <v>690</v>
       </c>
       <c r="K9">
-        <v>69</v>
+        <v>72</v>
       </c>
     </row>
     <row r="10" spans="1:11">
@@ -3097,10 +3097,10 @@
         <v>1664</v>
       </c>
       <c r="J10">
-        <v>1715</v>
+        <v>1716</v>
       </c>
       <c r="K10">
-        <v>227</v>
+        <v>230</v>
       </c>
     </row>
     <row r="11" spans="1:11">
@@ -3132,10 +3132,10 @@
         <v>4761</v>
       </c>
       <c r="J11">
-        <v>5075</v>
+        <v>5076</v>
       </c>
       <c r="K11">
-        <v>617</v>
+        <v>633</v>
       </c>
     </row>
   </sheetData>
@@ -3449,7 +3449,7 @@
         <v>39</v>
       </c>
       <c r="K9">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="10" spans="1:11">
@@ -3519,7 +3519,7 @@
         <v>539</v>
       </c>
       <c r="K11">
-        <v>56</v>
+        <v>57</v>
       </c>
     </row>
   </sheetData>
@@ -4442,7 +4442,7 @@
         <v>214</v>
       </c>
       <c r="K3">
-        <v>19</v>
+        <v>20</v>
       </c>
     </row>
     <row r="4" spans="1:11">
@@ -4617,7 +4617,7 @@
         <v>517</v>
       </c>
       <c r="K8">
-        <v>51</v>
+        <v>54</v>
       </c>
     </row>
     <row r="9" spans="1:11">
@@ -4687,7 +4687,7 @@
         <v>596</v>
       </c>
       <c r="K10">
-        <v>65</v>
+        <v>66</v>
       </c>
     </row>
     <row r="11" spans="1:11">
@@ -4722,7 +4722,7 @@
         <v>1811</v>
       </c>
       <c r="K11">
-        <v>191</v>
+        <v>196</v>
       </c>
     </row>
   </sheetData>
@@ -4818,7 +4818,7 @@
         <v>295</v>
       </c>
       <c r="K2">
-        <v>37</v>
+        <v>39</v>
       </c>
     </row>
     <row r="3" spans="1:11">
@@ -5028,7 +5028,7 @@
         <v>890</v>
       </c>
       <c r="K8">
-        <v>90</v>
+        <v>91</v>
       </c>
     </row>
     <row r="9" spans="1:11">
@@ -5063,7 +5063,7 @@
         <v>473</v>
       </c>
       <c r="K9">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="10" spans="1:11">
@@ -5098,7 +5098,7 @@
         <v>1032</v>
       </c>
       <c r="K10">
-        <v>126</v>
+        <v>127</v>
       </c>
     </row>
     <row r="11" spans="1:11">
@@ -5133,7 +5133,7 @@
         <v>3405</v>
       </c>
       <c r="K11">
-        <v>386</v>
+        <v>389</v>
       </c>
     </row>
   </sheetData>
@@ -5369,7 +5369,7 @@
         <v>43</v>
       </c>
       <c r="K6">
-        <v>6</v>
+        <v>8</v>
       </c>
     </row>
     <row r="7" spans="1:11">
@@ -5439,7 +5439,7 @@
         <v>813</v>
       </c>
       <c r="K8">
-        <v>80</v>
+        <v>83</v>
       </c>
     </row>
     <row r="9" spans="1:11">
@@ -5509,7 +5509,7 @@
         <v>827</v>
       </c>
       <c r="K10">
-        <v>101</v>
+        <v>103</v>
       </c>
     </row>
     <row r="11" spans="1:11">
@@ -5544,7 +5544,7 @@
         <v>2630</v>
       </c>
       <c r="K11">
-        <v>307</v>
+        <v>314</v>
       </c>
     </row>
   </sheetData>
@@ -5640,7 +5640,7 @@
         <v>1142</v>
       </c>
       <c r="K2">
-        <v>147</v>
+        <v>149</v>
       </c>
     </row>
     <row r="3" spans="1:11">
@@ -5710,7 +5710,7 @@
         <v>515</v>
       </c>
       <c r="K4">
-        <v>69</v>
+        <v>70</v>
       </c>
     </row>
     <row r="5" spans="1:11">
@@ -5780,7 +5780,7 @@
         <v>1102</v>
       </c>
       <c r="K6">
-        <v>148</v>
+        <v>149</v>
       </c>
     </row>
     <row r="7" spans="1:11">
@@ -5815,7 +5815,7 @@
         <v>2985</v>
       </c>
       <c r="K7">
-        <v>336</v>
+        <v>343</v>
       </c>
     </row>
     <row r="8" spans="1:11">
@@ -5847,10 +5847,10 @@
         <v>4761</v>
       </c>
       <c r="J8">
-        <v>5075</v>
+        <v>5076</v>
       </c>
       <c r="K8">
-        <v>617</v>
+        <v>633</v>
       </c>
     </row>
     <row r="9" spans="1:11">
@@ -5885,7 +5885,7 @@
         <v>541</v>
       </c>
       <c r="K9">
-        <v>51</v>
+        <v>53</v>
       </c>
     </row>
     <row r="10" spans="1:11">
@@ -5920,7 +5920,7 @@
         <v>1153</v>
       </c>
       <c r="K10">
-        <v>165</v>
+        <v>166</v>
       </c>
     </row>
     <row r="11" spans="1:11">
@@ -5952,10 +5952,10 @@
         <v>1720</v>
       </c>
       <c r="J11">
-        <v>2169</v>
+        <v>2170</v>
       </c>
       <c r="K11">
-        <v>307</v>
+        <v>314</v>
       </c>
     </row>
     <row r="12" spans="1:11">
@@ -5990,7 +5990,7 @@
         <v>437</v>
       </c>
       <c r="K12">
-        <v>53</v>
+        <v>55</v>
       </c>
     </row>
     <row r="13" spans="1:11">
@@ -6060,7 +6060,7 @@
         <v>740</v>
       </c>
       <c r="K14">
-        <v>92</v>
+        <v>93</v>
       </c>
     </row>
     <row r="15" spans="1:11">
@@ -6095,7 +6095,7 @@
         <v>1071</v>
       </c>
       <c r="K15">
-        <v>142</v>
+        <v>147</v>
       </c>
     </row>
     <row r="16" spans="1:11">
@@ -6130,7 +6130,7 @@
         <v>828</v>
       </c>
       <c r="K16">
-        <v>108</v>
+        <v>111</v>
       </c>
     </row>
     <row r="17" spans="1:11">
@@ -6200,7 +6200,7 @@
         <v>859</v>
       </c>
       <c r="K18">
-        <v>121</v>
+        <v>123</v>
       </c>
     </row>
     <row r="19" spans="1:11">
@@ -6235,7 +6235,7 @@
         <v>2861</v>
       </c>
       <c r="K19">
-        <v>360</v>
+        <v>371</v>
       </c>
     </row>
     <row r="20" spans="1:11">
@@ -6270,7 +6270,7 @@
         <v>2178</v>
       </c>
       <c r="K20">
-        <v>251</v>
+        <v>262</v>
       </c>
     </row>
     <row r="21" spans="1:11">
@@ -6410,7 +6410,7 @@
         <v>735</v>
       </c>
       <c r="K24">
-        <v>93</v>
+        <v>95</v>
       </c>
     </row>
     <row r="25" spans="1:11">
@@ -6445,7 +6445,7 @@
         <v>596</v>
       </c>
       <c r="K25">
-        <v>53</v>
+        <v>54</v>
       </c>
     </row>
     <row r="26" spans="1:11">
@@ -6515,7 +6515,7 @@
         <v>1511</v>
       </c>
       <c r="K27">
-        <v>229</v>
+        <v>231</v>
       </c>
     </row>
     <row r="28" spans="1:11">
@@ -6550,7 +6550,7 @@
         <v>71</v>
       </c>
       <c r="K28">
-        <v>21</v>
+        <v>22</v>
       </c>
     </row>
     <row r="29" spans="1:11">
@@ -6585,7 +6585,7 @@
         <v>4178</v>
       </c>
       <c r="K29">
-        <v>461</v>
+        <v>466</v>
       </c>
     </row>
     <row r="30" spans="1:11">
@@ -6655,7 +6655,7 @@
         <v>1031</v>
       </c>
       <c r="K31">
-        <v>153</v>
+        <v>154</v>
       </c>
     </row>
     <row r="32" spans="1:11">
@@ -6690,7 +6690,7 @@
         <v>284</v>
       </c>
       <c r="K32">
-        <v>26</v>
+        <v>27</v>
       </c>
     </row>
     <row r="33" spans="1:11">
@@ -6725,7 +6725,7 @@
         <v>3405</v>
       </c>
       <c r="K33">
-        <v>386</v>
+        <v>389</v>
       </c>
     </row>
     <row r="34" spans="1:11">
@@ -6760,7 +6760,7 @@
         <v>950</v>
       </c>
       <c r="K34">
-        <v>157</v>
+        <v>159</v>
       </c>
     </row>
     <row r="35" spans="1:11">
@@ -6795,7 +6795,7 @@
         <v>268</v>
       </c>
       <c r="K35">
-        <v>42</v>
+        <v>44</v>
       </c>
     </row>
     <row r="36" spans="1:11">
@@ -6830,7 +6830,7 @@
         <v>1736</v>
       </c>
       <c r="K36">
-        <v>184</v>
+        <v>188</v>
       </c>
     </row>
     <row r="37" spans="1:11">
@@ -6862,10 +6862,10 @@
         <v>2566</v>
       </c>
       <c r="J37">
-        <v>2972</v>
+        <v>2973</v>
       </c>
       <c r="K37">
-        <v>357</v>
+        <v>361</v>
       </c>
     </row>
     <row r="38" spans="1:11">
@@ -6935,7 +6935,7 @@
         <v>129</v>
       </c>
       <c r="K39">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="40" spans="1:11">
@@ -7040,7 +7040,7 @@
         <v>3619</v>
       </c>
       <c r="K42">
-        <v>369</v>
+        <v>375</v>
       </c>
     </row>
     <row r="43" spans="1:11">
@@ -7075,7 +7075,7 @@
         <v>1453</v>
       </c>
       <c r="K43">
-        <v>172</v>
+        <v>174</v>
       </c>
     </row>
     <row r="44" spans="1:11">
@@ -7110,7 +7110,7 @@
         <v>1382</v>
       </c>
       <c r="K44">
-        <v>203</v>
+        <v>207</v>
       </c>
     </row>
     <row r="45" spans="1:11">
@@ -7145,7 +7145,7 @@
         <v>155</v>
       </c>
       <c r="K45">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="46" spans="1:11">
@@ -7180,7 +7180,7 @@
         <v>539</v>
       </c>
       <c r="K46">
-        <v>56</v>
+        <v>57</v>
       </c>
     </row>
     <row r="47" spans="1:11">
@@ -7215,7 +7215,7 @@
         <v>1025</v>
       </c>
       <c r="K47">
-        <v>158</v>
+        <v>159</v>
       </c>
     </row>
     <row r="48" spans="1:11">
@@ -7250,7 +7250,7 @@
         <v>3091</v>
       </c>
       <c r="K48">
-        <v>379</v>
+        <v>383</v>
       </c>
     </row>
     <row r="49" spans="1:11">
@@ -7285,7 +7285,7 @@
         <v>1840</v>
       </c>
       <c r="K49">
-        <v>251</v>
+        <v>252</v>
       </c>
     </row>
     <row r="50" spans="1:11">
@@ -7320,7 +7320,7 @@
         <v>1138</v>
       </c>
       <c r="K50">
-        <v>134</v>
+        <v>138</v>
       </c>
     </row>
     <row r="51" spans="1:11">
@@ -7355,7 +7355,7 @@
         <v>1653</v>
       </c>
       <c r="K51">
-        <v>225</v>
+        <v>227</v>
       </c>
     </row>
     <row r="52" spans="1:11">
@@ -7390,7 +7390,7 @@
         <v>1923</v>
       </c>
       <c r="K52">
-        <v>250</v>
+        <v>258</v>
       </c>
     </row>
     <row r="53" spans="1:11">
@@ -7425,7 +7425,7 @@
         <v>2251</v>
       </c>
       <c r="K53">
-        <v>336</v>
+        <v>341</v>
       </c>
     </row>
     <row r="54" spans="1:11">
@@ -7460,7 +7460,7 @@
         <v>3895</v>
       </c>
       <c r="K54">
-        <v>556</v>
+        <v>565</v>
       </c>
     </row>
     <row r="55" spans="1:11">
@@ -7495,7 +7495,7 @@
         <v>1477</v>
       </c>
       <c r="K55">
-        <v>179</v>
+        <v>182</v>
       </c>
     </row>
     <row r="56" spans="1:11">
@@ -7530,7 +7530,7 @@
         <v>670</v>
       </c>
       <c r="K56">
-        <v>94</v>
+        <v>96</v>
       </c>
     </row>
     <row r="57" spans="1:11">
@@ -7635,7 +7635,7 @@
         <v>346</v>
       </c>
       <c r="K59">
-        <v>45</v>
+        <v>46</v>
       </c>
     </row>
     <row r="60" spans="1:11">
@@ -7772,10 +7772,10 @@
         <v>1843</v>
       </c>
       <c r="J63">
-        <v>479</v>
+        <v>483</v>
       </c>
       <c r="K63">
-        <v>87</v>
+        <v>108</v>
       </c>
     </row>
     <row r="64" spans="1:11">
@@ -7810,7 +7810,7 @@
         <v>1202</v>
       </c>
       <c r="K64">
-        <v>144</v>
+        <v>149</v>
       </c>
     </row>
     <row r="65" spans="1:11">
@@ -7845,7 +7845,7 @@
         <v>1879</v>
       </c>
       <c r="K65">
-        <v>233</v>
+        <v>235</v>
       </c>
     </row>
     <row r="66" spans="1:11">
@@ -7880,7 +7880,7 @@
         <v>812</v>
       </c>
       <c r="K66">
-        <v>78</v>
+        <v>80</v>
       </c>
     </row>
     <row r="67" spans="1:11">
@@ -7915,7 +7915,7 @@
         <v>2745</v>
       </c>
       <c r="K67">
-        <v>315</v>
+        <v>319</v>
       </c>
     </row>
     <row r="68" spans="1:11">
@@ -7950,7 +7950,7 @@
         <v>420</v>
       </c>
       <c r="K68">
-        <v>55</v>
+        <v>57</v>
       </c>
     </row>
     <row r="69" spans="1:11">
@@ -7985,7 +7985,7 @@
         <v>495</v>
       </c>
       <c r="K69">
-        <v>91</v>
+        <v>94</v>
       </c>
     </row>
     <row r="70" spans="1:11">
@@ -8020,7 +8020,7 @@
         <v>738</v>
       </c>
       <c r="K70">
-        <v>97</v>
+        <v>100</v>
       </c>
     </row>
     <row r="71" spans="1:11">
@@ -8125,7 +8125,7 @@
         <v>1682</v>
       </c>
       <c r="K73">
-        <v>201</v>
+        <v>203</v>
       </c>
     </row>
     <row r="74" spans="1:11">
@@ -8160,7 +8160,7 @@
         <v>312</v>
       </c>
       <c r="K74">
-        <v>43</v>
+        <v>44</v>
       </c>
     </row>
     <row r="75" spans="1:11">
@@ -8195,7 +8195,7 @@
         <v>420</v>
       </c>
       <c r="K75">
-        <v>65</v>
+        <v>67</v>
       </c>
     </row>
     <row r="76" spans="1:11">
@@ -8230,7 +8230,7 @@
         <v>3193</v>
       </c>
       <c r="K76">
-        <v>392</v>
+        <v>401</v>
       </c>
     </row>
     <row r="77" spans="1:11">
@@ -8300,7 +8300,7 @@
         <v>2011</v>
       </c>
       <c r="K78">
-        <v>332</v>
+        <v>337</v>
       </c>
     </row>
     <row r="79" spans="1:11">
@@ -8335,7 +8335,7 @@
         <v>2630</v>
       </c>
       <c r="K79">
-        <v>307</v>
+        <v>314</v>
       </c>
     </row>
     <row r="80" spans="1:11">
@@ -8405,7 +8405,7 @@
         <v>256</v>
       </c>
       <c r="K81">
-        <v>27</v>
+        <v>28</v>
       </c>
     </row>
     <row r="82" spans="1:11">
@@ -8440,7 +8440,7 @@
         <v>283</v>
       </c>
       <c r="K82">
-        <v>42</v>
+        <v>43</v>
       </c>
     </row>
     <row r="83" spans="1:11">
@@ -8475,7 +8475,7 @@
         <v>1811</v>
       </c>
       <c r="K83">
-        <v>191</v>
+        <v>196</v>
       </c>
     </row>
     <row r="84" spans="1:11">
@@ -8545,7 +8545,7 @@
         <v>4213</v>
       </c>
       <c r="K85">
-        <v>518</v>
+        <v>530</v>
       </c>
     </row>
     <row r="86" spans="1:11">
@@ -8580,7 +8580,7 @@
         <v>1001</v>
       </c>
       <c r="K86">
-        <v>126</v>
+        <v>130</v>
       </c>
     </row>
     <row r="87" spans="1:11">
@@ -8615,7 +8615,7 @@
         <v>418</v>
       </c>
       <c r="K87">
-        <v>36</v>
+        <v>37</v>
       </c>
     </row>
     <row r="88" spans="1:11">
@@ -8650,7 +8650,7 @@
         <v>1060</v>
       </c>
       <c r="K88">
-        <v>138</v>
+        <v>143</v>
       </c>
     </row>
     <row r="89" spans="1:11">
@@ -8673,7 +8673,7 @@
         <v>1374</v>
       </c>
       <c r="G89">
-        <v>1277</v>
+        <v>1278</v>
       </c>
       <c r="H89">
         <v>1294</v>
@@ -8685,7 +8685,7 @@
         <v>2258</v>
       </c>
       <c r="K89">
-        <v>272</v>
+        <v>279</v>
       </c>
     </row>
     <row r="90" spans="1:11">
@@ -8702,7 +8702,7 @@
         <v>1280</v>
       </c>
       <c r="E90">
-        <v>1210</v>
+        <v>1211</v>
       </c>
       <c r="F90">
         <v>1190</v>
@@ -8720,7 +8720,7 @@
         <v>1435</v>
       </c>
       <c r="K90">
-        <v>159</v>
+        <v>163</v>
       </c>
     </row>
     <row r="91" spans="1:11">
@@ -8755,7 +8755,7 @@
         <v>1144</v>
       </c>
       <c r="K91">
-        <v>127</v>
+        <v>128</v>
       </c>
     </row>
     <row r="92" spans="1:11">
@@ -8790,7 +8790,7 @@
         <v>457</v>
       </c>
       <c r="K92">
-        <v>50</v>
+        <v>53</v>
       </c>
     </row>
     <row r="93" spans="1:11">
@@ -8825,7 +8825,7 @@
         <v>849</v>
       </c>
       <c r="K93">
-        <v>117</v>
+        <v>118</v>
       </c>
     </row>
     <row r="94" spans="1:11">
@@ -8860,7 +8860,7 @@
         <v>2778</v>
       </c>
       <c r="K94">
-        <v>394</v>
+        <v>402</v>
       </c>
     </row>
     <row r="95" spans="1:11">
@@ -8895,7 +8895,7 @@
         <v>1485</v>
       </c>
       <c r="K95">
-        <v>199</v>
+        <v>200</v>
       </c>
     </row>
     <row r="96" spans="1:11">
@@ -8930,7 +8930,7 @@
         <v>1808</v>
       </c>
       <c r="K96">
-        <v>267</v>
+        <v>268</v>
       </c>
     </row>
     <row r="97" spans="1:11">
@@ -8965,7 +8965,7 @@
         <v>1902</v>
       </c>
       <c r="K97">
-        <v>256</v>
+        <v>258</v>
       </c>
     </row>
     <row r="98" spans="1:11">
@@ -9000,7 +9000,7 @@
         <v>1351</v>
       </c>
       <c r="K98">
-        <v>218</v>
+        <v>220</v>
       </c>
     </row>
     <row r="99" spans="1:11">
@@ -9035,7 +9035,7 @@
         <v>1727</v>
       </c>
       <c r="K99">
-        <v>207</v>
+        <v>213</v>
       </c>
     </row>
     <row r="100" spans="1:11">
@@ -9070,7 +9070,7 @@
         <v>318</v>
       </c>
       <c r="K100">
-        <v>40</v>
+        <v>41</v>
       </c>
     </row>
     <row r="101" spans="1:11">
@@ -9087,13 +9087,13 @@
         <v>117366</v>
       </c>
       <c r="E101">
-        <v>113419</v>
+        <v>113420</v>
       </c>
       <c r="F101">
         <v>105585</v>
       </c>
       <c r="G101">
-        <v>85337</v>
+        <v>85338</v>
       </c>
       <c r="H101">
         <v>84633</v>
@@ -9102,10 +9102,10 @@
         <v>110574</v>
       </c>
       <c r="J101">
-        <v>123686</v>
+        <v>123693</v>
       </c>
       <c r="K101">
-        <v>15552</v>
+        <v>15839</v>
       </c>
     </row>
   </sheetData>
@@ -9303,7 +9303,7 @@
         <v>35</v>
       </c>
       <c r="K2">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="3" spans="1:11">
@@ -9501,7 +9501,7 @@
         <v>124</v>
       </c>
       <c r="K8">
-        <v>14</v>
+        <v>15</v>
       </c>
     </row>
     <row r="9" spans="1:11">
@@ -9606,7 +9606,7 @@
         <v>420</v>
       </c>
       <c r="K11">
-        <v>65</v>
+        <v>67</v>
       </c>
     </row>
   </sheetData>
@@ -10109,7 +10109,7 @@
         <v>46</v>
       </c>
       <c r="K3">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="4" spans="1:11">
@@ -10275,7 +10275,7 @@
         <v>365</v>
       </c>
       <c r="K8">
-        <v>33</v>
+        <v>35</v>
       </c>
     </row>
     <row r="9" spans="1:11">
@@ -10345,7 +10345,7 @@
         <v>579</v>
       </c>
       <c r="K10">
-        <v>81</v>
+        <v>83</v>
       </c>
     </row>
     <row r="11" spans="1:11">
@@ -10380,7 +10380,7 @@
         <v>1202</v>
       </c>
       <c r="K11">
-        <v>144</v>
+        <v>149</v>
       </c>
     </row>
   </sheetData>
@@ -10511,7 +10511,7 @@
         <v>151</v>
       </c>
       <c r="K3">
-        <v>15</v>
+        <v>16</v>
       </c>
     </row>
     <row r="4" spans="1:11">
@@ -10791,7 +10791,7 @@
         <v>1485</v>
       </c>
       <c r="K11">
-        <v>199</v>
+        <v>200</v>
       </c>
     </row>
   </sheetData>
@@ -10887,7 +10887,7 @@
         <v>273</v>
       </c>
       <c r="K2">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="3" spans="1:11">
@@ -10992,7 +10992,7 @@
         <v>226</v>
       </c>
       <c r="K5">
-        <v>26</v>
+        <v>29</v>
       </c>
     </row>
     <row r="6" spans="1:11">
@@ -11164,7 +11164,7 @@
         <v>821</v>
       </c>
       <c r="J10">
-        <v>936</v>
+        <v>937</v>
       </c>
       <c r="K10">
         <v>126</v>
@@ -11199,10 +11199,10 @@
         <v>2566</v>
       </c>
       <c r="J11">
-        <v>2972</v>
+        <v>2973</v>
       </c>
       <c r="K11">
-        <v>357</v>
+        <v>361</v>
       </c>
     </row>
   </sheetData>
@@ -11271,34 +11271,34 @@
         <v>1</v>
       </c>
       <c r="B2">
-        <v>26</v>
+        <v>102</v>
       </c>
       <c r="C2">
-        <v>23</v>
+        <v>166</v>
       </c>
       <c r="D2">
-        <v>32</v>
+        <v>152</v>
       </c>
       <c r="E2">
-        <v>48</v>
+        <v>178</v>
       </c>
       <c r="F2">
-        <v>40</v>
+        <v>125</v>
       </c>
       <c r="G2">
-        <v>41</v>
+        <v>169</v>
       </c>
       <c r="H2">
-        <v>40</v>
+        <v>188</v>
       </c>
       <c r="I2">
-        <v>61</v>
+        <v>194</v>
       </c>
       <c r="J2">
-        <v>48</v>
+        <v>211</v>
       </c>
       <c r="K2">
-        <v>14</v>
+        <v>24</v>
       </c>
     </row>
     <row r="3" spans="1:11">
@@ -11306,34 +11306,34 @@
         <v>2</v>
       </c>
       <c r="B3">
-        <v>25</v>
+        <v>183</v>
       </c>
       <c r="C3">
-        <v>30</v>
+        <v>245</v>
       </c>
       <c r="D3">
-        <v>38</v>
+        <v>213</v>
       </c>
       <c r="E3">
-        <v>27</v>
+        <v>167</v>
       </c>
       <c r="F3">
-        <v>26</v>
+        <v>171</v>
       </c>
       <c r="G3">
-        <v>40</v>
+        <v>175</v>
       </c>
       <c r="H3">
-        <v>42</v>
+        <v>204</v>
       </c>
       <c r="I3">
-        <v>42</v>
+        <v>182</v>
       </c>
       <c r="J3">
-        <v>42</v>
+        <v>193</v>
       </c>
       <c r="K3">
-        <v>5</v>
+        <v>22</v>
       </c>
     </row>
     <row r="4" spans="1:11">
@@ -11341,28 +11341,34 @@
         <v>3</v>
       </c>
       <c r="B4">
-        <v>1</v>
+        <v>9</v>
+      </c>
+      <c r="C4">
+        <v>17</v>
       </c>
       <c r="D4">
-        <v>2</v>
+        <v>22</v>
       </c>
       <c r="E4">
-        <v>1</v>
+        <v>22</v>
+      </c>
+      <c r="F4">
+        <v>10</v>
       </c>
       <c r="G4">
-        <v>2</v>
+        <v>16</v>
       </c>
       <c r="H4">
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="I4">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="J4">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="K4">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="5" spans="1:11">
@@ -11370,34 +11376,34 @@
         <v>4</v>
       </c>
       <c r="B5">
-        <v>101</v>
+        <v>253</v>
       </c>
       <c r="C5">
-        <v>108</v>
+        <v>300</v>
       </c>
       <c r="D5">
-        <v>79</v>
+        <v>180</v>
       </c>
       <c r="E5">
-        <v>119</v>
+        <v>177</v>
       </c>
       <c r="F5">
-        <v>82</v>
+        <v>156</v>
       </c>
       <c r="G5">
-        <v>79</v>
+        <v>107</v>
       </c>
       <c r="H5">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="I5">
-        <v>83</v>
+        <v>107</v>
       </c>
       <c r="J5">
-        <v>131</v>
+        <v>106</v>
       </c>
       <c r="K5">
-        <v>10</v>
+        <v>17</v>
       </c>
     </row>
     <row r="6" spans="1:11">
@@ -11405,34 +11411,31 @@
         <v>5</v>
       </c>
       <c r="B6">
-        <v>14</v>
+        <v>21</v>
       </c>
       <c r="C6">
-        <v>24</v>
+        <v>39</v>
       </c>
       <c r="D6">
-        <v>16</v>
+        <v>29</v>
       </c>
       <c r="E6">
-        <v>24</v>
+        <v>36</v>
       </c>
       <c r="F6">
-        <v>24</v>
+        <v>34</v>
       </c>
       <c r="G6">
-        <v>17</v>
+        <v>30</v>
       </c>
       <c r="H6">
         <v>23</v>
       </c>
       <c r="I6">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="J6">
-        <v>21</v>
-      </c>
-      <c r="K6">
-        <v>5</v>
+        <v>29</v>
       </c>
     </row>
     <row r="7" spans="1:11">
@@ -11440,28 +11443,34 @@
         <v>6</v>
       </c>
       <c r="B7">
-        <v>1</v>
+        <v>17</v>
       </c>
       <c r="C7">
-        <v>1</v>
+        <v>41</v>
       </c>
       <c r="D7">
-        <v>2</v>
+        <v>19</v>
+      </c>
+      <c r="E7">
+        <v>23</v>
+      </c>
+      <c r="F7">
+        <v>6</v>
       </c>
       <c r="G7">
-        <v>1</v>
+        <v>15</v>
       </c>
       <c r="H7">
-        <v>1</v>
+        <v>15</v>
       </c>
       <c r="I7">
-        <v>3</v>
+        <v>20</v>
       </c>
       <c r="J7">
-        <v>3</v>
+        <v>20</v>
       </c>
       <c r="K7">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="8" spans="1:11">
@@ -11469,34 +11478,34 @@
         <v>7</v>
       </c>
       <c r="B8">
-        <v>82</v>
+        <v>157</v>
       </c>
       <c r="C8">
-        <v>81</v>
+        <v>186</v>
       </c>
       <c r="D8">
-        <v>77</v>
+        <v>196</v>
       </c>
       <c r="E8">
-        <v>82</v>
+        <v>138</v>
       </c>
       <c r="F8">
-        <v>48</v>
+        <v>136</v>
       </c>
       <c r="G8">
-        <v>48</v>
+        <v>149</v>
       </c>
       <c r="H8">
-        <v>76</v>
+        <v>146</v>
       </c>
       <c r="I8">
-        <v>167</v>
+        <v>203</v>
       </c>
       <c r="J8">
-        <v>254</v>
+        <v>392</v>
       </c>
       <c r="K8">
-        <v>37</v>
+        <v>45</v>
       </c>
     </row>
     <row r="9" spans="1:11">
@@ -11504,34 +11513,34 @@
         <v>8</v>
       </c>
       <c r="B9">
-        <v>44</v>
+        <v>174</v>
       </c>
       <c r="C9">
-        <v>84</v>
+        <v>251</v>
       </c>
       <c r="D9">
-        <v>78</v>
+        <v>201</v>
       </c>
       <c r="E9">
-        <v>65</v>
+        <v>158</v>
       </c>
       <c r="F9">
-        <v>60</v>
+        <v>120</v>
       </c>
       <c r="G9">
-        <v>58</v>
+        <v>114</v>
       </c>
       <c r="H9">
-        <v>69</v>
+        <v>113</v>
       </c>
       <c r="I9">
-        <v>88</v>
+        <v>189</v>
       </c>
       <c r="J9">
-        <v>65</v>
+        <v>274</v>
       </c>
       <c r="K9">
-        <v>20</v>
+        <v>52</v>
       </c>
     </row>
     <row r="10" spans="1:11">
@@ -11539,34 +11548,34 @@
         <v>9</v>
       </c>
       <c r="B10">
-        <v>585</v>
+        <v>817</v>
       </c>
       <c r="C10">
-        <v>614</v>
+        <v>721</v>
       </c>
       <c r="D10">
-        <v>758</v>
+        <v>783</v>
       </c>
       <c r="E10">
-        <v>697</v>
+        <v>748</v>
       </c>
       <c r="F10">
-        <v>692</v>
+        <v>717</v>
       </c>
       <c r="G10">
-        <v>586</v>
+        <v>480</v>
       </c>
       <c r="H10">
-        <v>622</v>
+        <v>417</v>
       </c>
       <c r="I10">
-        <v>793</v>
+        <v>591</v>
       </c>
       <c r="J10">
-        <v>946</v>
+        <v>643</v>
       </c>
       <c r="K10">
-        <v>136</v>
+        <v>70</v>
       </c>
     </row>
     <row r="11" spans="1:11">
@@ -11574,34 +11583,34 @@
         <v>10</v>
       </c>
       <c r="B11">
-        <v>879</v>
+        <v>1733</v>
       </c>
       <c r="C11">
-        <v>965</v>
+        <v>1966</v>
       </c>
       <c r="D11">
-        <v>1082</v>
+        <v>1795</v>
       </c>
       <c r="E11">
-        <v>1063</v>
+        <v>1647</v>
       </c>
       <c r="F11">
-        <v>972</v>
+        <v>1475</v>
       </c>
       <c r="G11">
-        <v>872</v>
+        <v>1255</v>
       </c>
       <c r="H11">
-        <v>969</v>
+        <v>1206</v>
       </c>
       <c r="I11">
-        <v>1269</v>
+        <v>1522</v>
       </c>
       <c r="J11">
-        <v>1511</v>
+        <v>1879</v>
       </c>
       <c r="K11">
-        <v>229</v>
+        <v>235</v>
       </c>
     </row>
   </sheetData>
@@ -11670,34 +11679,34 @@
         <v>1</v>
       </c>
       <c r="B2">
-        <v>102</v>
+        <v>26</v>
       </c>
       <c r="C2">
-        <v>166</v>
+        <v>23</v>
       </c>
       <c r="D2">
-        <v>152</v>
+        <v>32</v>
       </c>
       <c r="E2">
-        <v>178</v>
+        <v>48</v>
       </c>
       <c r="F2">
-        <v>125</v>
+        <v>40</v>
       </c>
       <c r="G2">
-        <v>169</v>
+        <v>41</v>
       </c>
       <c r="H2">
-        <v>188</v>
+        <v>40</v>
       </c>
       <c r="I2">
-        <v>194</v>
+        <v>61</v>
       </c>
       <c r="J2">
-        <v>211</v>
+        <v>48</v>
       </c>
       <c r="K2">
-        <v>24</v>
+        <v>14</v>
       </c>
     </row>
     <row r="3" spans="1:11">
@@ -11705,34 +11714,34 @@
         <v>2</v>
       </c>
       <c r="B3">
-        <v>183</v>
+        <v>25</v>
       </c>
       <c r="C3">
-        <v>245</v>
+        <v>30</v>
       </c>
       <c r="D3">
-        <v>213</v>
+        <v>38</v>
       </c>
       <c r="E3">
-        <v>167</v>
+        <v>27</v>
       </c>
       <c r="F3">
-        <v>171</v>
+        <v>26</v>
       </c>
       <c r="G3">
-        <v>175</v>
+        <v>40</v>
       </c>
       <c r="H3">
-        <v>204</v>
+        <v>42</v>
       </c>
       <c r="I3">
-        <v>182</v>
+        <v>42</v>
       </c>
       <c r="J3">
-        <v>193</v>
+        <v>42</v>
       </c>
       <c r="K3">
-        <v>21</v>
+        <v>5</v>
       </c>
     </row>
     <row r="4" spans="1:11">
@@ -11740,34 +11749,28 @@
         <v>3</v>
       </c>
       <c r="B4">
-        <v>9</v>
-      </c>
-      <c r="C4">
-        <v>17</v>
+        <v>1</v>
       </c>
       <c r="D4">
-        <v>22</v>
+        <v>2</v>
       </c>
       <c r="E4">
-        <v>22</v>
-      </c>
-      <c r="F4">
-        <v>10</v>
+        <v>1</v>
       </c>
       <c r="G4">
-        <v>16</v>
+        <v>2</v>
       </c>
       <c r="H4">
-        <v>8</v>
+        <v>1</v>
       </c>
       <c r="I4">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="J4">
-        <v>11</v>
+        <v>1</v>
       </c>
       <c r="K4">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="5" spans="1:11">
@@ -11775,34 +11778,34 @@
         <v>4</v>
       </c>
       <c r="B5">
-        <v>253</v>
+        <v>101</v>
       </c>
       <c r="C5">
-        <v>300</v>
+        <v>108</v>
       </c>
       <c r="D5">
-        <v>180</v>
+        <v>79</v>
       </c>
       <c r="E5">
-        <v>177</v>
+        <v>119</v>
       </c>
       <c r="F5">
-        <v>156</v>
+        <v>82</v>
       </c>
       <c r="G5">
-        <v>107</v>
+        <v>79</v>
       </c>
       <c r="H5">
-        <v>92</v>
+        <v>95</v>
       </c>
       <c r="I5">
-        <v>107</v>
+        <v>83</v>
       </c>
       <c r="J5">
-        <v>106</v>
+        <v>131</v>
       </c>
       <c r="K5">
-        <v>17</v>
+        <v>10</v>
       </c>
     </row>
     <row r="6" spans="1:11">
@@ -11810,31 +11813,34 @@
         <v>5</v>
       </c>
       <c r="B6">
-        <v>21</v>
+        <v>14</v>
       </c>
       <c r="C6">
-        <v>39</v>
+        <v>24</v>
       </c>
       <c r="D6">
-        <v>29</v>
+        <v>16</v>
       </c>
       <c r="E6">
-        <v>36</v>
+        <v>24</v>
       </c>
       <c r="F6">
-        <v>34</v>
+        <v>24</v>
       </c>
       <c r="G6">
-        <v>30</v>
+        <v>17</v>
       </c>
       <c r="H6">
         <v>23</v>
       </c>
       <c r="I6">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="J6">
-        <v>29</v>
+        <v>21</v>
+      </c>
+      <c r="K6">
+        <v>5</v>
       </c>
     </row>
     <row r="7" spans="1:11">
@@ -11842,34 +11848,28 @@
         <v>6</v>
       </c>
       <c r="B7">
-        <v>17</v>
+        <v>1</v>
       </c>
       <c r="C7">
-        <v>41</v>
+        <v>1</v>
       </c>
       <c r="D7">
-        <v>19</v>
-      </c>
-      <c r="E7">
-        <v>23</v>
-      </c>
-      <c r="F7">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="G7">
-        <v>15</v>
+        <v>1</v>
       </c>
       <c r="H7">
-        <v>15</v>
+        <v>1</v>
       </c>
       <c r="I7">
-        <v>20</v>
+        <v>3</v>
       </c>
       <c r="J7">
-        <v>20</v>
+        <v>3</v>
       </c>
       <c r="K7">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="8" spans="1:11">
@@ -11877,34 +11877,34 @@
         <v>7</v>
       </c>
       <c r="B8">
-        <v>157</v>
+        <v>82</v>
       </c>
       <c r="C8">
-        <v>186</v>
+        <v>81</v>
       </c>
       <c r="D8">
-        <v>196</v>
+        <v>77</v>
       </c>
       <c r="E8">
-        <v>138</v>
+        <v>82</v>
       </c>
       <c r="F8">
-        <v>136</v>
+        <v>48</v>
       </c>
       <c r="G8">
-        <v>149</v>
+        <v>48</v>
       </c>
       <c r="H8">
-        <v>146</v>
+        <v>76</v>
       </c>
       <c r="I8">
-        <v>203</v>
+        <v>167</v>
       </c>
       <c r="J8">
-        <v>392</v>
+        <v>254</v>
       </c>
       <c r="K8">
-        <v>45</v>
+        <v>37</v>
       </c>
     </row>
     <row r="9" spans="1:11">
@@ -11912,34 +11912,34 @@
         <v>8</v>
       </c>
       <c r="B9">
-        <v>174</v>
+        <v>44</v>
       </c>
       <c r="C9">
-        <v>251</v>
+        <v>84</v>
       </c>
       <c r="D9">
-        <v>201</v>
+        <v>78</v>
       </c>
       <c r="E9">
-        <v>158</v>
+        <v>65</v>
       </c>
       <c r="F9">
-        <v>120</v>
+        <v>60</v>
       </c>
       <c r="G9">
-        <v>114</v>
+        <v>58</v>
       </c>
       <c r="H9">
-        <v>113</v>
+        <v>69</v>
       </c>
       <c r="I9">
-        <v>189</v>
+        <v>88</v>
       </c>
       <c r="J9">
-        <v>274</v>
+        <v>65</v>
       </c>
       <c r="K9">
-        <v>52</v>
+        <v>20</v>
       </c>
     </row>
     <row r="10" spans="1:11">
@@ -11947,34 +11947,34 @@
         <v>9</v>
       </c>
       <c r="B10">
-        <v>817</v>
+        <v>585</v>
       </c>
       <c r="C10">
-        <v>721</v>
+        <v>614</v>
       </c>
       <c r="D10">
-        <v>783</v>
+        <v>758</v>
       </c>
       <c r="E10">
-        <v>748</v>
+        <v>697</v>
       </c>
       <c r="F10">
-        <v>717</v>
+        <v>692</v>
       </c>
       <c r="G10">
-        <v>480</v>
+        <v>586</v>
       </c>
       <c r="H10">
-        <v>417</v>
+        <v>622</v>
       </c>
       <c r="I10">
-        <v>591</v>
+        <v>793</v>
       </c>
       <c r="J10">
-        <v>643</v>
+        <v>946</v>
       </c>
       <c r="K10">
-        <v>70</v>
+        <v>138</v>
       </c>
     </row>
     <row r="11" spans="1:11">
@@ -11982,34 +11982,34 @@
         <v>10</v>
       </c>
       <c r="B11">
-        <v>1733</v>
+        <v>879</v>
       </c>
       <c r="C11">
-        <v>1966</v>
+        <v>965</v>
       </c>
       <c r="D11">
-        <v>1795</v>
+        <v>1082</v>
       </c>
       <c r="E11">
-        <v>1647</v>
+        <v>1063</v>
       </c>
       <c r="F11">
-        <v>1475</v>
+        <v>972</v>
       </c>
       <c r="G11">
-        <v>1255</v>
+        <v>872</v>
       </c>
       <c r="H11">
-        <v>1206</v>
+        <v>969</v>
       </c>
       <c r="I11">
-        <v>1522</v>
+        <v>1269</v>
       </c>
       <c r="J11">
-        <v>1879</v>
+        <v>1511</v>
       </c>
       <c r="K11">
-        <v>233</v>
+        <v>231</v>
       </c>
     </row>
   </sheetData>
@@ -12140,7 +12140,7 @@
         <v>174</v>
       </c>
       <c r="K3">
-        <v>19</v>
+        <v>20</v>
       </c>
     </row>
     <row r="4" spans="1:11">
@@ -12315,7 +12315,7 @@
         <v>493</v>
       </c>
       <c r="K8">
-        <v>43</v>
+        <v>46</v>
       </c>
     </row>
     <row r="9" spans="1:11">
@@ -12350,7 +12350,7 @@
         <v>119</v>
       </c>
       <c r="K9">
-        <v>18</v>
+        <v>19</v>
       </c>
     </row>
     <row r="10" spans="1:11">
@@ -12385,7 +12385,7 @@
         <v>629</v>
       </c>
       <c r="K10">
-        <v>87</v>
+        <v>88</v>
       </c>
     </row>
     <row r="11" spans="1:11">
@@ -12420,7 +12420,7 @@
         <v>1727</v>
       </c>
       <c r="K11">
-        <v>207</v>
+        <v>213</v>
       </c>
     </row>
   </sheetData>
@@ -13145,7 +13145,7 @@
         <v>111</v>
       </c>
       <c r="K9">
-        <v>14</v>
+        <v>15</v>
       </c>
     </row>
     <row r="10" spans="1:11">
@@ -13215,7 +13215,7 @@
         <v>1031</v>
       </c>
       <c r="K11">
-        <v>153</v>
+        <v>154</v>
       </c>
     </row>
   </sheetData>
@@ -13576,7 +13576,7 @@
         <v>321</v>
       </c>
       <c r="K10">
-        <v>49</v>
+        <v>50</v>
       </c>
     </row>
     <row r="11" spans="1:11">
@@ -13611,7 +13611,7 @@
         <v>740</v>
       </c>
       <c r="K11">
-        <v>92</v>
+        <v>93</v>
       </c>
     </row>
   </sheetData>
@@ -13707,7 +13707,7 @@
         <v>272</v>
       </c>
       <c r="K2">
-        <v>43</v>
+        <v>44</v>
       </c>
     </row>
     <row r="3" spans="1:11">
@@ -13742,7 +13742,7 @@
         <v>395</v>
       </c>
       <c r="K3">
-        <v>42</v>
+        <v>44</v>
       </c>
     </row>
     <row r="4" spans="1:11">
@@ -13847,7 +13847,7 @@
         <v>73</v>
       </c>
       <c r="K6">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="7" spans="1:11">
@@ -13952,7 +13952,7 @@
         <v>293</v>
       </c>
       <c r="K9">
-        <v>49</v>
+        <v>50</v>
       </c>
     </row>
     <row r="10" spans="1:11">
@@ -13987,7 +13987,7 @@
         <v>884</v>
       </c>
       <c r="K10">
-        <v>83</v>
+        <v>84</v>
       </c>
     </row>
     <row r="11" spans="1:11">
@@ -14022,7 +14022,7 @@
         <v>2745</v>
       </c>
       <c r="K11">
-        <v>315</v>
+        <v>319</v>
       </c>
     </row>
   </sheetData>
@@ -14613,7 +14613,7 @@
         <v>112</v>
       </c>
       <c r="K5">
-        <v>14</v>
+        <v>16</v>
       </c>
     </row>
     <row r="6" spans="1:11">
@@ -14712,7 +14712,7 @@
         <v>422</v>
       </c>
       <c r="K8">
-        <v>47</v>
+        <v>49</v>
       </c>
     </row>
     <row r="9" spans="1:11">
@@ -14782,7 +14782,7 @@
         <v>1911</v>
       </c>
       <c r="K10">
-        <v>292</v>
+        <v>296</v>
       </c>
     </row>
     <row r="11" spans="1:11">
@@ -14817,7 +14817,7 @@
         <v>2778</v>
       </c>
       <c r="K11">
-        <v>394</v>
+        <v>402</v>
       </c>
     </row>
   </sheetData>
@@ -14948,7 +14948,7 @@
         <v>90</v>
       </c>
       <c r="K3">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="4" spans="1:11">
@@ -15114,7 +15114,7 @@
         <v>331</v>
       </c>
       <c r="K8">
-        <v>47</v>
+        <v>48</v>
       </c>
     </row>
     <row r="9" spans="1:11">
@@ -15149,7 +15149,7 @@
         <v>214</v>
       </c>
       <c r="K9">
-        <v>27</v>
+        <v>28</v>
       </c>
     </row>
     <row r="10" spans="1:11">
@@ -15184,7 +15184,7 @@
         <v>2311</v>
       </c>
       <c r="K10">
-        <v>273</v>
+        <v>279</v>
       </c>
     </row>
     <row r="11" spans="1:11">
@@ -15219,7 +15219,7 @@
         <v>3193</v>
       </c>
       <c r="K11">
-        <v>392</v>
+        <v>401</v>
       </c>
     </row>
   </sheetData>
@@ -15501,7 +15501,7 @@
         <v>88</v>
       </c>
       <c r="K8">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="9" spans="1:11">
@@ -15603,7 +15603,7 @@
         <v>418</v>
       </c>
       <c r="K11">
-        <v>36</v>
+        <v>37</v>
       </c>
     </row>
   </sheetData>
@@ -15909,7 +15909,7 @@
         <v>138</v>
       </c>
       <c r="K8">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="9" spans="1:11">
@@ -16014,7 +16014,7 @@
         <v>596</v>
       </c>
       <c r="K11">
-        <v>53</v>
+        <v>54</v>
       </c>
     </row>
   </sheetData>
@@ -16339,7 +16339,7 @@
         <v>210</v>
       </c>
       <c r="K10">
-        <v>27</v>
+        <v>28</v>
       </c>
     </row>
     <row r="11" spans="1:11">
@@ -16374,7 +16374,7 @@
         <v>318</v>
       </c>
       <c r="K11">
-        <v>40</v>
+        <v>41</v>
       </c>
     </row>
   </sheetData>
@@ -16708,7 +16708,7 @@
         <v>528</v>
       </c>
       <c r="K10">
-        <v>75</v>
+        <v>78</v>
       </c>
     </row>
     <row r="11" spans="1:11">
@@ -16743,7 +16743,7 @@
         <v>828</v>
       </c>
       <c r="K11">
-        <v>108</v>
+        <v>111</v>
       </c>
     </row>
   </sheetData>
@@ -17101,7 +17101,7 @@
         <v>1268</v>
       </c>
       <c r="K10">
-        <v>188</v>
+        <v>189</v>
       </c>
     </row>
     <row r="11" spans="1:11">
@@ -17136,7 +17136,7 @@
         <v>1840</v>
       </c>
       <c r="K11">
-        <v>251</v>
+        <v>252</v>
       </c>
     </row>
   </sheetData>
@@ -17232,7 +17232,7 @@
         <v>45</v>
       </c>
       <c r="K2">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="3" spans="1:11">
@@ -17503,7 +17503,7 @@
         <v>1012</v>
       </c>
       <c r="K10">
-        <v>137</v>
+        <v>138</v>
       </c>
     </row>
     <row r="11" spans="1:11">
@@ -17538,7 +17538,7 @@
         <v>1902</v>
       </c>
       <c r="K11">
-        <v>256</v>
+        <v>258</v>
       </c>
     </row>
   </sheetData>
@@ -17634,7 +17634,7 @@
         <v>93</v>
       </c>
       <c r="K2">
-        <v>19</v>
+        <v>20</v>
       </c>
     </row>
     <row r="3" spans="1:11">
@@ -17946,7 +17946,7 @@
         <v>1808</v>
       </c>
       <c r="K11">
-        <v>267</v>
+        <v>268</v>
       </c>
     </row>
   </sheetData>
@@ -18246,7 +18246,7 @@
         <v>326</v>
       </c>
       <c r="K8">
-        <v>46</v>
+        <v>48</v>
       </c>
     </row>
     <row r="9" spans="1:11">
@@ -18316,7 +18316,7 @@
         <v>619</v>
       </c>
       <c r="K10">
-        <v>91</v>
+        <v>92</v>
       </c>
     </row>
     <row r="11" spans="1:11">
@@ -18351,7 +18351,7 @@
         <v>1477</v>
       </c>
       <c r="K11">
-        <v>179</v>
+        <v>182</v>
       </c>
     </row>
   </sheetData>
@@ -18552,7 +18552,7 @@
         <v>92</v>
       </c>
       <c r="K5">
-        <v>14</v>
+        <v>16</v>
       </c>
     </row>
     <row r="6" spans="1:11">
@@ -18654,7 +18654,7 @@
         <v>419</v>
       </c>
       <c r="K8">
-        <v>71</v>
+        <v>73</v>
       </c>
     </row>
     <row r="9" spans="1:11">
@@ -18724,7 +18724,7 @@
         <v>2806</v>
       </c>
       <c r="K10">
-        <v>403</v>
+        <v>408</v>
       </c>
     </row>
     <row r="11" spans="1:11">
@@ -18759,7 +18759,7 @@
         <v>3895</v>
       </c>
       <c r="K11">
-        <v>556</v>
+        <v>565</v>
       </c>
     </row>
   </sheetData>
@@ -18960,7 +18960,7 @@
         <v>117</v>
       </c>
       <c r="K5">
-        <v>12</v>
+        <v>13</v>
       </c>
     </row>
     <row r="6" spans="1:11">
@@ -19132,7 +19132,7 @@
         <v>884</v>
       </c>
       <c r="K10">
-        <v>96</v>
+        <v>97</v>
       </c>
     </row>
     <row r="11" spans="1:11">
@@ -19167,7 +19167,7 @@
         <v>1682</v>
       </c>
       <c r="K11">
-        <v>201</v>
+        <v>203</v>
       </c>
     </row>
   </sheetData>
@@ -19263,7 +19263,7 @@
         <v>471</v>
       </c>
       <c r="K2">
-        <v>41</v>
+        <v>42</v>
       </c>
     </row>
     <row r="3" spans="1:11">
@@ -19298,7 +19298,7 @@
         <v>548</v>
       </c>
       <c r="K3">
-        <v>46</v>
+        <v>47</v>
       </c>
     </row>
     <row r="4" spans="1:11">
@@ -19368,7 +19368,7 @@
         <v>250</v>
       </c>
       <c r="K5">
-        <v>27</v>
+        <v>28</v>
       </c>
     </row>
     <row r="6" spans="1:11">
@@ -19473,7 +19473,7 @@
         <v>1031</v>
       </c>
       <c r="K8">
-        <v>121</v>
+        <v>122</v>
       </c>
     </row>
     <row r="9" spans="1:11">
@@ -19543,7 +19543,7 @@
         <v>1304</v>
       </c>
       <c r="K10">
-        <v>144</v>
+        <v>145</v>
       </c>
     </row>
     <row r="11" spans="1:11">
@@ -19578,7 +19578,7 @@
         <v>4178</v>
       </c>
       <c r="K11">
-        <v>461</v>
+        <v>466</v>
       </c>
     </row>
   </sheetData>
@@ -19872,7 +19872,7 @@
         <v>462</v>
       </c>
       <c r="K8">
-        <v>42</v>
+        <v>43</v>
       </c>
     </row>
     <row r="9" spans="1:11">
@@ -19907,7 +19907,7 @@
         <v>154</v>
       </c>
       <c r="K9">
-        <v>15</v>
+        <v>16</v>
       </c>
     </row>
     <row r="10" spans="1:11">
@@ -19942,7 +19942,7 @@
         <v>2120</v>
       </c>
       <c r="K10">
-        <v>280</v>
+        <v>282</v>
       </c>
     </row>
     <row r="11" spans="1:11">
@@ -19977,7 +19977,7 @@
         <v>3091</v>
       </c>
       <c r="K11">
-        <v>379</v>
+        <v>383</v>
       </c>
     </row>
   </sheetData>
@@ -20248,7 +20248,7 @@
         <v>31</v>
       </c>
       <c r="K7">
-        <v>4</v>
+        <v>7</v>
       </c>
     </row>
     <row r="8" spans="1:11">
@@ -20283,7 +20283,7 @@
         <v>774</v>
       </c>
       <c r="K8">
-        <v>91</v>
+        <v>95</v>
       </c>
     </row>
     <row r="9" spans="1:11">
@@ -20353,7 +20353,7 @@
         <v>1014</v>
       </c>
       <c r="K10">
-        <v>143</v>
+        <v>147</v>
       </c>
     </row>
     <row r="11" spans="1:11">
@@ -20388,7 +20388,7 @@
         <v>2861</v>
       </c>
       <c r="K11">
-        <v>360</v>
+        <v>371</v>
       </c>
     </row>
   </sheetData>
@@ -20658,7 +20658,7 @@
         <v>146</v>
       </c>
       <c r="K8">
-        <v>12</v>
+        <v>13</v>
       </c>
     </row>
     <row r="9" spans="1:11">
@@ -20728,7 +20728,7 @@
         <v>469</v>
       </c>
       <c r="K10">
-        <v>40</v>
+        <v>41</v>
       </c>
     </row>
     <row r="11" spans="1:11">
@@ -20763,7 +20763,7 @@
         <v>812</v>
       </c>
       <c r="K11">
-        <v>78</v>
+        <v>80</v>
       </c>
     </row>
   </sheetData>
@@ -20894,7 +20894,7 @@
         <v>51</v>
       </c>
       <c r="K3">
-        <v>10</v>
+        <v>12</v>
       </c>
     </row>
     <row r="4" spans="1:11">
@@ -21063,7 +21063,7 @@
         <v>314</v>
       </c>
       <c r="K8">
-        <v>44</v>
+        <v>45</v>
       </c>
     </row>
     <row r="9" spans="1:11">
@@ -21133,7 +21133,7 @@
         <v>722</v>
       </c>
       <c r="K10">
-        <v>105</v>
+        <v>106</v>
       </c>
     </row>
     <row r="11" spans="1:11">
@@ -21168,7 +21168,7 @@
         <v>1382</v>
       </c>
       <c r="K11">
-        <v>203</v>
+        <v>207</v>
       </c>
     </row>
   </sheetData>
@@ -21264,7 +21264,7 @@
         <v>257</v>
       </c>
       <c r="K2">
-        <v>25</v>
+        <v>27</v>
       </c>
     </row>
     <row r="3" spans="1:11">
@@ -21404,7 +21404,7 @@
         <v>57</v>
       </c>
       <c r="K6">
-        <v>5</v>
+        <v>7</v>
       </c>
     </row>
     <row r="7" spans="1:11">
@@ -21541,7 +21541,7 @@
         <v>1268</v>
       </c>
       <c r="K10">
-        <v>123</v>
+        <v>125</v>
       </c>
     </row>
     <row r="11" spans="1:11">
@@ -21576,7 +21576,7 @@
         <v>3619</v>
       </c>
       <c r="K11">
-        <v>369</v>
+        <v>375</v>
       </c>
     </row>
   </sheetData>
@@ -22100,7 +22100,7 @@
         <v>253</v>
       </c>
       <c r="K3">
-        <v>27</v>
+        <v>28</v>
       </c>
     </row>
     <row r="4" spans="1:11">
@@ -22167,7 +22167,7 @@
         <v>225</v>
       </c>
       <c r="K5">
-        <v>18</v>
+        <v>19</v>
       </c>
     </row>
     <row r="6" spans="1:11">
@@ -22272,7 +22272,7 @@
         <v>943</v>
       </c>
       <c r="K8">
-        <v>93</v>
+        <v>95</v>
       </c>
     </row>
     <row r="9" spans="1:11">
@@ -22307,7 +22307,7 @@
         <v>257</v>
       </c>
       <c r="K9">
-        <v>27</v>
+        <v>29</v>
       </c>
     </row>
     <row r="10" spans="1:11">
@@ -22342,7 +22342,7 @@
         <v>979</v>
       </c>
       <c r="K10">
-        <v>121</v>
+        <v>122</v>
       </c>
     </row>
     <row r="11" spans="1:11">
@@ -22377,7 +22377,7 @@
         <v>2985</v>
       </c>
       <c r="K11">
-        <v>336</v>
+        <v>343</v>
       </c>
     </row>
   </sheetData>
@@ -22671,7 +22671,7 @@
         <v>385</v>
       </c>
       <c r="K8">
-        <v>39</v>
+        <v>40</v>
       </c>
     </row>
     <row r="9" spans="1:11">
@@ -22776,7 +22776,7 @@
         <v>1102</v>
       </c>
       <c r="K11">
-        <v>148</v>
+        <v>149</v>
       </c>
     </row>
   </sheetData>
@@ -23475,7 +23475,7 @@
         <v>620</v>
       </c>
       <c r="K8">
-        <v>57</v>
+        <v>60</v>
       </c>
     </row>
     <row r="9" spans="1:11">
@@ -23545,7 +23545,7 @@
         <v>631</v>
       </c>
       <c r="K10">
-        <v>70</v>
+        <v>71</v>
       </c>
     </row>
     <row r="11" spans="1:11">
@@ -23580,7 +23580,7 @@
         <v>1736</v>
       </c>
       <c r="K11">
-        <v>184</v>
+        <v>188</v>
       </c>
     </row>
   </sheetData>
@@ -24296,7 +24296,7 @@
         <v>650</v>
       </c>
       <c r="K10">
-        <v>101</v>
+        <v>102</v>
       </c>
     </row>
     <row r="11" spans="1:11">
@@ -24331,7 +24331,7 @@
         <v>1153</v>
       </c>
       <c r="K11">
-        <v>165</v>
+        <v>166</v>
       </c>
     </row>
   </sheetData>
@@ -24462,7 +24462,7 @@
         <v>29</v>
       </c>
       <c r="K3">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="4" spans="1:11">
@@ -24552,7 +24552,7 @@
         <v>95</v>
       </c>
       <c r="K6">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="7" spans="1:11">
@@ -24601,7 +24601,7 @@
         <v>112</v>
       </c>
       <c r="K8">
-        <v>12</v>
+        <v>13</v>
       </c>
     </row>
     <row r="9" spans="1:11">
@@ -24671,7 +24671,7 @@
         <v>693</v>
       </c>
       <c r="K10">
-        <v>87</v>
+        <v>88</v>
       </c>
     </row>
     <row r="11" spans="1:11">
@@ -24706,7 +24706,7 @@
         <v>1001</v>
       </c>
       <c r="K11">
-        <v>126</v>
+        <v>130</v>
       </c>
     </row>
   </sheetData>
@@ -24837,7 +24837,7 @@
         <v>104</v>
       </c>
       <c r="K3">
-        <v>14</v>
+        <v>15</v>
       </c>
     </row>
     <row r="4" spans="1:11">
@@ -24976,6 +24976,9 @@
       <c r="J7">
         <v>5</v>
       </c>
+      <c r="K7">
+        <v>1</v>
+      </c>
     </row>
     <row r="8" spans="1:11">
       <c r="A8" s="1" t="s">
@@ -25009,7 +25012,7 @@
         <v>430</v>
       </c>
       <c r="K8">
-        <v>71</v>
+        <v>72</v>
       </c>
     </row>
     <row r="9" spans="1:11">
@@ -25079,7 +25082,7 @@
         <v>1134</v>
       </c>
       <c r="K10">
-        <v>187</v>
+        <v>189</v>
       </c>
     </row>
     <row r="11" spans="1:11">
@@ -25114,7 +25117,7 @@
         <v>2011</v>
       </c>
       <c r="K11">
-        <v>332</v>
+        <v>337</v>
       </c>
     </row>
   </sheetData>
@@ -25399,7 +25402,7 @@
         <v>86</v>
       </c>
       <c r="K8">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="9" spans="1:11">
@@ -25469,7 +25472,7 @@
         <v>227</v>
       </c>
       <c r="K10">
-        <v>33</v>
+        <v>34</v>
       </c>
     </row>
     <row r="11" spans="1:11">
@@ -25504,7 +25507,7 @@
         <v>420</v>
       </c>
       <c r="K11">
-        <v>55</v>
+        <v>57</v>
       </c>
     </row>
   </sheetData>
@@ -25859,7 +25862,7 @@
         <v>381</v>
       </c>
       <c r="K10">
-        <v>50</v>
+        <v>52</v>
       </c>
     </row>
     <row r="11" spans="1:11">
@@ -25894,7 +25897,7 @@
         <v>735</v>
       </c>
       <c r="K11">
-        <v>93</v>
+        <v>95</v>
       </c>
     </row>
   </sheetData>
@@ -25990,7 +25993,7 @@
         <v>98</v>
       </c>
       <c r="K2">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="3" spans="1:11">
@@ -26025,7 +26028,7 @@
         <v>74</v>
       </c>
       <c r="K3">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="4" spans="1:11">
@@ -26232,7 +26235,7 @@
         <v>166</v>
       </c>
       <c r="K9">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="10" spans="1:11">
@@ -26267,7 +26270,7 @@
         <v>424</v>
       </c>
       <c r="K10">
-        <v>75</v>
+        <v>77</v>
       </c>
     </row>
     <row r="11" spans="1:11">
@@ -26302,7 +26305,7 @@
         <v>1071</v>
       </c>
       <c r="K11">
-        <v>142</v>
+        <v>147</v>
       </c>
     </row>
   </sheetData>
@@ -26433,7 +26436,7 @@
         <v>92</v>
       </c>
       <c r="K3">
-        <v>14</v>
+        <v>15</v>
       </c>
     </row>
     <row r="4" spans="1:11">
@@ -26567,7 +26570,7 @@
         <v>9</v>
       </c>
       <c r="J7">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="8" spans="1:11">
@@ -26602,7 +26605,7 @@
         <v>524</v>
       </c>
       <c r="K8">
-        <v>64</v>
+        <v>65</v>
       </c>
     </row>
     <row r="9" spans="1:11">
@@ -26637,7 +26640,7 @@
         <v>260</v>
       </c>
       <c r="K9">
-        <v>35</v>
+        <v>37</v>
       </c>
     </row>
     <row r="10" spans="1:11">
@@ -26672,7 +26675,7 @@
         <v>962</v>
       </c>
       <c r="K10">
-        <v>149</v>
+        <v>152</v>
       </c>
     </row>
     <row r="11" spans="1:11">
@@ -26704,10 +26707,10 @@
         <v>1720</v>
       </c>
       <c r="J11">
-        <v>2169</v>
+        <v>2170</v>
       </c>
       <c r="K11">
-        <v>307</v>
+        <v>314</v>
       </c>
     </row>
   </sheetData>
@@ -27409,7 +27412,7 @@
         <v>402</v>
       </c>
       <c r="K8">
-        <v>32</v>
+        <v>33</v>
       </c>
     </row>
     <row r="9" spans="1:11">
@@ -27514,7 +27517,7 @@
         <v>1144</v>
       </c>
       <c r="K11">
-        <v>127</v>
+        <v>128</v>
       </c>
     </row>
   </sheetData>
@@ -27884,7 +27887,7 @@
         <v>749</v>
       </c>
       <c r="K10">
-        <v>115</v>
+        <v>117</v>
       </c>
     </row>
     <row r="11" spans="1:11">
@@ -27919,7 +27922,7 @@
         <v>1653</v>
       </c>
       <c r="K11">
-        <v>225</v>
+        <v>227</v>
       </c>
     </row>
   </sheetData>
@@ -28015,7 +28018,7 @@
         <v>173</v>
       </c>
       <c r="K2">
-        <v>19</v>
+        <v>23</v>
       </c>
     </row>
     <row r="3" spans="1:11">
@@ -28222,7 +28225,7 @@
         <v>564</v>
       </c>
       <c r="K8">
-        <v>71</v>
+        <v>75</v>
       </c>
     </row>
     <row r="9" spans="1:11">
@@ -28292,7 +28295,7 @@
         <v>818</v>
       </c>
       <c r="K10">
-        <v>78</v>
+        <v>81</v>
       </c>
     </row>
     <row r="11" spans="1:11">
@@ -28327,7 +28330,7 @@
         <v>2178</v>
       </c>
       <c r="K11">
-        <v>251</v>
+        <v>262</v>
       </c>
     </row>
   </sheetData>
@@ -29054,7 +29057,7 @@
         <v>444</v>
       </c>
       <c r="K10">
-        <v>81</v>
+        <v>82</v>
       </c>
     </row>
     <row r="11" spans="1:11">
@@ -29089,7 +29092,7 @@
         <v>1025</v>
       </c>
       <c r="K11">
-        <v>158</v>
+        <v>159</v>
       </c>
     </row>
   </sheetData>
@@ -29185,7 +29188,7 @@
         <v>110</v>
       </c>
       <c r="K2">
-        <v>10</v>
+        <v>12</v>
       </c>
     </row>
     <row r="3" spans="1:11">
@@ -29304,7 +29307,7 @@
         <v>20</v>
       </c>
       <c r="E6">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="F6">
         <v>17</v>
@@ -29322,7 +29325,7 @@
         <v>11</v>
       </c>
       <c r="K6">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="7" spans="1:11">
@@ -29462,7 +29465,7 @@
         <v>519</v>
       </c>
       <c r="K10">
-        <v>67</v>
+        <v>70</v>
       </c>
     </row>
     <row r="11" spans="1:11">
@@ -29479,7 +29482,7 @@
         <v>1280</v>
       </c>
       <c r="E11">
-        <v>1210</v>
+        <v>1211</v>
       </c>
       <c r="F11">
         <v>1190</v>
@@ -29497,7 +29500,7 @@
         <v>1435</v>
       </c>
       <c r="K11">
-        <v>159</v>
+        <v>163</v>
       </c>
     </row>
   </sheetData>
@@ -29785,7 +29788,7 @@
         <v>185</v>
       </c>
       <c r="K8">
-        <v>19</v>
+        <v>20</v>
       </c>
     </row>
     <row r="9" spans="1:11">
@@ -29855,7 +29858,7 @@
         <v>637</v>
       </c>
       <c r="K10">
-        <v>73</v>
+        <v>76</v>
       </c>
     </row>
     <row r="11" spans="1:11">
@@ -29890,7 +29893,7 @@
         <v>1138</v>
       </c>
       <c r="K11">
-        <v>134</v>
+        <v>138</v>
       </c>
     </row>
   </sheetData>
@@ -29986,7 +29989,7 @@
         <v>36</v>
       </c>
       <c r="K2">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="3" spans="1:11">
@@ -30286,7 +30289,7 @@
         <v>849</v>
       </c>
       <c r="K11">
-        <v>117</v>
+        <v>118</v>
       </c>
     </row>
   </sheetData>
@@ -30586,7 +30589,7 @@
         <v>254</v>
       </c>
       <c r="K8">
-        <v>35</v>
+        <v>36</v>
       </c>
     </row>
     <row r="9" spans="1:11">
@@ -30656,7 +30659,7 @@
         <v>311</v>
       </c>
       <c r="K10">
-        <v>51</v>
+        <v>52</v>
       </c>
     </row>
     <row r="11" spans="1:11">
@@ -30691,7 +30694,7 @@
         <v>859</v>
       </c>
       <c r="K11">
-        <v>121</v>
+        <v>123</v>
       </c>
     </row>
   </sheetData>
@@ -31025,7 +31028,7 @@
         <v>552</v>
       </c>
       <c r="K10">
-        <v>59</v>
+        <v>62</v>
       </c>
     </row>
     <row r="11" spans="1:11">
@@ -31060,7 +31063,7 @@
         <v>738</v>
       </c>
       <c r="K11">
-        <v>97</v>
+        <v>100</v>
       </c>
     </row>
   </sheetData>
@@ -31781,7 +31784,7 @@
         <v>612</v>
       </c>
       <c r="K10">
-        <v>86</v>
+        <v>88</v>
       </c>
     </row>
     <row r="11" spans="1:11">
@@ -31816,7 +31819,7 @@
         <v>670</v>
       </c>
       <c r="K11">
-        <v>94</v>
+        <v>96</v>
       </c>
     </row>
   </sheetData>
@@ -32293,7 +32296,7 @@
         <v>67</v>
       </c>
       <c r="K2">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="3" spans="1:11">
@@ -32567,7 +32570,7 @@
         <v>624</v>
       </c>
       <c r="K10">
-        <v>85</v>
+        <v>86</v>
       </c>
     </row>
     <row r="11" spans="1:11">
@@ -32602,7 +32605,7 @@
         <v>1142</v>
       </c>
       <c r="K11">
-        <v>147</v>
+        <v>149</v>
       </c>
     </row>
   </sheetData>
@@ -33271,7 +33274,7 @@
         <v>375</v>
       </c>
       <c r="K8">
-        <v>26</v>
+        <v>27</v>
       </c>
     </row>
     <row r="9" spans="1:11">
@@ -33341,7 +33344,7 @@
         <v>752</v>
       </c>
       <c r="K10">
-        <v>96</v>
+        <v>97</v>
       </c>
     </row>
     <row r="11" spans="1:11">
@@ -33376,7 +33379,7 @@
         <v>1453</v>
       </c>
       <c r="K11">
-        <v>172</v>
+        <v>174</v>
       </c>
     </row>
   </sheetData>
@@ -33850,7 +33853,7 @@
         <v>41</v>
       </c>
       <c r="K2">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="3" spans="1:11">
@@ -34150,7 +34153,7 @@
         <v>515</v>
       </c>
       <c r="K11">
-        <v>69</v>
+        <v>70</v>
       </c>
     </row>
   </sheetData>
@@ -34615,7 +34618,7 @@
         <v>36</v>
       </c>
       <c r="K2">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="3" spans="1:11">
@@ -34819,7 +34822,7 @@
         <v>240</v>
       </c>
       <c r="K8">
-        <v>54</v>
+        <v>55</v>
       </c>
     </row>
     <row r="9" spans="1:11">
@@ -34924,7 +34927,7 @@
         <v>950</v>
       </c>
       <c r="K11">
-        <v>157</v>
+        <v>159</v>
       </c>
     </row>
   </sheetData>
@@ -35148,7 +35151,7 @@
         <v>36</v>
       </c>
       <c r="G6">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="H6">
         <v>36</v>
@@ -35224,7 +35227,7 @@
         <v>364</v>
       </c>
       <c r="K8">
-        <v>32</v>
+        <v>34</v>
       </c>
     </row>
     <row r="9" spans="1:11">
@@ -35294,7 +35297,7 @@
         <v>1368</v>
       </c>
       <c r="K10">
-        <v>159</v>
+        <v>164</v>
       </c>
     </row>
     <row r="11" spans="1:11">
@@ -35317,7 +35320,7 @@
         <v>1374</v>
       </c>
       <c r="G11">
-        <v>1277</v>
+        <v>1278</v>
       </c>
       <c r="H11">
         <v>1294</v>
@@ -35329,7 +35332,7 @@
         <v>2258</v>
       </c>
       <c r="K11">
-        <v>272</v>
+        <v>279</v>
       </c>
     </row>
   </sheetData>
@@ -35456,6 +35459,9 @@
       <c r="J3">
         <v>5</v>
       </c>
+      <c r="K3">
+        <v>1</v>
+      </c>
     </row>
     <row r="4" spans="1:11">
       <c r="A4" s="1" t="s">
@@ -35642,7 +35648,7 @@
         <v>199</v>
       </c>
       <c r="K10">
-        <v>33</v>
+        <v>34</v>
       </c>
     </row>
     <row r="11" spans="1:11">
@@ -35677,7 +35683,7 @@
         <v>268</v>
       </c>
       <c r="K11">
-        <v>42</v>
+        <v>44</v>
       </c>
     </row>
   </sheetData>
@@ -35807,9 +35813,6 @@
       <c r="J3">
         <v>10</v>
       </c>
-      <c r="K3">
-        <v>1</v>
-      </c>
     </row>
     <row r="4" spans="1:11">
       <c r="A4" s="1" t="s">
@@ -36026,7 +36029,7 @@
         <v>155</v>
       </c>
       <c r="K10">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
   </sheetData>
@@ -36287,7 +36290,7 @@
         <v>105</v>
       </c>
       <c r="K8">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="9" spans="1:11">
@@ -36392,7 +36395,7 @@
         <v>284</v>
       </c>
       <c r="K11">
-        <v>26</v>
+        <v>27</v>
       </c>
     </row>
   </sheetData>
@@ -36998,7 +37001,7 @@
         <v>235</v>
       </c>
       <c r="K8">
-        <v>20</v>
+        <v>21</v>
       </c>
     </row>
     <row r="9" spans="1:11">
@@ -37068,7 +37071,7 @@
         <v>797</v>
       </c>
       <c r="K10">
-        <v>159</v>
+        <v>160</v>
       </c>
     </row>
     <row r="11" spans="1:11">
@@ -37103,7 +37106,7 @@
         <v>1351</v>
       </c>
       <c r="K11">
-        <v>218</v>
+        <v>220</v>
       </c>
     </row>
   </sheetData>
@@ -37754,7 +37757,7 @@
         <v>130</v>
       </c>
       <c r="K8">
-        <v>14</v>
+        <v>15</v>
       </c>
     </row>
     <row r="9" spans="1:11">
@@ -37789,7 +37792,7 @@
         <v>34</v>
       </c>
       <c r="K9">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="10" spans="1:11">
@@ -37824,7 +37827,7 @@
         <v>178</v>
       </c>
       <c r="K10">
-        <v>19</v>
+        <v>20</v>
       </c>
     </row>
     <row r="11" spans="1:11">
@@ -37859,7 +37862,7 @@
         <v>457</v>
       </c>
       <c r="K11">
-        <v>50</v>
+        <v>53</v>
       </c>
     </row>
   </sheetData>
@@ -38533,7 +38536,7 @@
         <v>170</v>
       </c>
       <c r="K9">
-        <v>27</v>
+        <v>28</v>
       </c>
     </row>
     <row r="10" spans="1:11">
@@ -38568,7 +38571,7 @@
         <v>283</v>
       </c>
       <c r="K10">
-        <v>42</v>
+        <v>43</v>
       </c>
     </row>
   </sheetData>
@@ -38868,7 +38871,7 @@
         <v>185</v>
       </c>
       <c r="K8">
-        <v>10</v>
+        <v>12</v>
       </c>
     </row>
     <row r="9" spans="1:11">
@@ -38973,7 +38976,7 @@
         <v>541</v>
       </c>
       <c r="K11">
-        <v>51</v>
+        <v>53</v>
       </c>
     </row>
   </sheetData>
@@ -39069,7 +39072,7 @@
         <v>319</v>
       </c>
       <c r="K2">
-        <v>68</v>
+        <v>69</v>
       </c>
     </row>
     <row r="3" spans="1:11">
@@ -39104,7 +39107,7 @@
         <v>432</v>
       </c>
       <c r="K3">
-        <v>55</v>
+        <v>57</v>
       </c>
     </row>
     <row r="4" spans="1:11">
@@ -39174,7 +39177,7 @@
         <v>317</v>
       </c>
       <c r="K5">
-        <v>62</v>
+        <v>64</v>
       </c>
     </row>
     <row r="6" spans="1:11">
@@ -39279,7 +39282,7 @@
         <v>1311</v>
       </c>
       <c r="K8">
-        <v>85</v>
+        <v>88</v>
       </c>
     </row>
     <row r="9" spans="1:11">
@@ -39314,7 +39317,7 @@
         <v>341</v>
       </c>
       <c r="K9">
-        <v>38</v>
+        <v>39</v>
       </c>
     </row>
     <row r="10" spans="1:11">
@@ -39349,7 +39352,7 @@
         <v>1373</v>
       </c>
       <c r="K10">
-        <v>192</v>
+        <v>195</v>
       </c>
     </row>
     <row r="11" spans="1:11">
@@ -39384,7 +39387,7 @@
         <v>4213</v>
       </c>
       <c r="K11">
-        <v>518</v>
+        <v>530</v>
       </c>
     </row>
   </sheetData>
@@ -39669,7 +39672,7 @@
         <v>121</v>
       </c>
       <c r="K8">
-        <v>12</v>
+        <v>13</v>
       </c>
     </row>
     <row r="9" spans="1:11">
@@ -39774,7 +39777,7 @@
         <v>346</v>
       </c>
       <c r="K11">
-        <v>45</v>
+        <v>46</v>
       </c>
     </row>
   </sheetData>
@@ -40068,7 +40071,7 @@
         <v>79</v>
       </c>
       <c r="K8">
-        <v>15</v>
+        <v>16</v>
       </c>
     </row>
     <row r="9" spans="1:11">
@@ -40103,7 +40106,7 @@
         <v>129</v>
       </c>
       <c r="K9">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
   </sheetData>
@@ -40805,7 +40808,7 @@
         <v>253</v>
       </c>
       <c r="K8">
-        <v>22</v>
+        <v>23</v>
       </c>
     </row>
     <row r="9" spans="1:11">
@@ -40875,7 +40878,7 @@
         <v>427</v>
       </c>
       <c r="K10">
-        <v>51</v>
+        <v>55</v>
       </c>
     </row>
     <row r="11" spans="1:11">
@@ -40910,7 +40913,7 @@
         <v>1060</v>
       </c>
       <c r="K11">
-        <v>138</v>
+        <v>143</v>
       </c>
     </row>
   </sheetData>
@@ -41226,7 +41229,7 @@
         <v>227</v>
       </c>
       <c r="K10">
-        <v>33</v>
+        <v>34</v>
       </c>
     </row>
     <row r="11" spans="1:11">
@@ -41261,7 +41264,7 @@
         <v>312</v>
       </c>
       <c r="K11">
-        <v>43</v>
+        <v>44</v>
       </c>
     </row>
   </sheetData>
@@ -41832,7 +41835,7 @@
         <v>37</v>
       </c>
       <c r="K8">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="9" spans="1:11">
@@ -41937,7 +41940,7 @@
         <v>256</v>
       </c>
       <c r="K11">
-        <v>27</v>
+        <v>28</v>
       </c>
     </row>
   </sheetData>
@@ -42454,7 +42457,7 @@
         <v>53</v>
       </c>
       <c r="K5">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="6" spans="1:11">
@@ -42602,7 +42605,7 @@
         <v>207</v>
       </c>
       <c r="K10">
-        <v>33</v>
+        <v>34</v>
       </c>
     </row>
     <row r="11" spans="1:11">
@@ -42637,7 +42640,7 @@
         <v>437</v>
       </c>
       <c r="K11">
-        <v>53</v>
+        <v>55</v>
       </c>
     </row>
   </sheetData>
@@ -42733,7 +42736,7 @@
         <v>2</v>
       </c>
       <c r="K2">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="3" spans="1:11">
@@ -42985,7 +42988,7 @@
         <v>71</v>
       </c>
       <c r="K11">
-        <v>21</v>
+        <v>22</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add data for 2024-04-13
</commit_message>
<xml_diff>
--- a/output/index-crime-full-year.xlsx
+++ b/output/index-crime-full-year.xlsx
@@ -902,7 +902,7 @@
         <v>7707</v>
       </c>
       <c r="K2">
-        <v>1976</v>
+        <v>1996</v>
       </c>
     </row>
     <row r="3" spans="1:11">
@@ -937,7 +937,7 @@
         <v>8080</v>
       </c>
       <c r="K3">
-        <v>1902</v>
+        <v>1928</v>
       </c>
     </row>
     <row r="4" spans="1:11">
@@ -972,7 +972,7 @@
         <v>512</v>
       </c>
       <c r="K4">
-        <v>121</v>
+        <v>122</v>
       </c>
     </row>
     <row r="5" spans="1:11">
@@ -1007,7 +1007,7 @@
         <v>7473</v>
       </c>
       <c r="K5">
-        <v>1875</v>
+        <v>1898</v>
       </c>
     </row>
     <row r="6" spans="1:11">
@@ -1039,10 +1039,10 @@
         <v>1784</v>
       </c>
       <c r="J6">
-        <v>1803</v>
+        <v>1802</v>
       </c>
       <c r="K6">
-        <v>403</v>
+        <v>407</v>
       </c>
     </row>
     <row r="7" spans="1:11">
@@ -1077,7 +1077,7 @@
         <v>625</v>
       </c>
       <c r="K7">
-        <v>125</v>
+        <v>126</v>
       </c>
     </row>
     <row r="8" spans="1:11">
@@ -1109,10 +1109,10 @@
         <v>21456</v>
       </c>
       <c r="J8">
-        <v>29229</v>
+        <v>29230</v>
       </c>
       <c r="K8">
-        <v>6039</v>
+        <v>6119</v>
       </c>
     </row>
     <row r="9" spans="1:11">
@@ -1147,7 +1147,7 @@
         <v>11059</v>
       </c>
       <c r="K9">
-        <v>2428</v>
+        <v>2453</v>
       </c>
     </row>
     <row r="10" spans="1:11">
@@ -1179,10 +1179,10 @@
         <v>54874</v>
       </c>
       <c r="J10">
-        <v>57343</v>
+        <v>57344</v>
       </c>
       <c r="K10">
-        <v>14494</v>
+        <v>14651</v>
       </c>
     </row>
     <row r="11" spans="1:11">
@@ -1214,10 +1214,10 @@
         <v>110581</v>
       </c>
       <c r="J11">
-        <v>123831</v>
+        <v>123832</v>
       </c>
       <c r="K11">
-        <v>29363</v>
+        <v>29700</v>
       </c>
     </row>
   </sheetData>
@@ -1313,7 +1313,7 @@
         <v>177</v>
       </c>
       <c r="K2">
-        <v>47</v>
+        <v>48</v>
       </c>
     </row>
     <row r="3" spans="1:11">
@@ -1348,7 +1348,7 @@
         <v>209</v>
       </c>
       <c r="K3">
-        <v>40</v>
+        <v>41</v>
       </c>
     </row>
     <row r="4" spans="1:11">
@@ -1593,7 +1593,7 @@
         <v>697</v>
       </c>
       <c r="K10">
-        <v>202</v>
+        <v>203</v>
       </c>
     </row>
     <row r="11" spans="1:11">
@@ -1628,7 +1628,7 @@
         <v>1929</v>
       </c>
       <c r="K11">
-        <v>494</v>
+        <v>497</v>
       </c>
     </row>
   </sheetData>
@@ -2284,7 +2284,7 @@
         <v>323</v>
       </c>
       <c r="K10">
-        <v>108</v>
+        <v>113</v>
       </c>
     </row>
     <row r="11" spans="1:11">
@@ -2319,7 +2319,7 @@
         <v>496</v>
       </c>
       <c r="K11">
-        <v>160</v>
+        <v>165</v>
       </c>
     </row>
   </sheetData>
@@ -2692,7 +2692,7 @@
         <v>1203</v>
       </c>
       <c r="K10">
-        <v>371</v>
+        <v>372</v>
       </c>
     </row>
     <row r="11" spans="1:11">
@@ -2727,7 +2727,7 @@
         <v>2251</v>
       </c>
       <c r="K11">
-        <v>603</v>
+        <v>604</v>
       </c>
     </row>
   </sheetData>
@@ -2823,7 +2823,7 @@
         <v>488</v>
       </c>
       <c r="K2">
-        <v>131</v>
+        <v>133</v>
       </c>
     </row>
     <row r="3" spans="1:11">
@@ -2858,7 +2858,7 @@
         <v>530</v>
       </c>
       <c r="K3">
-        <v>132</v>
+        <v>133</v>
       </c>
     </row>
     <row r="4" spans="1:11">
@@ -2928,7 +2928,7 @@
         <v>224</v>
       </c>
       <c r="K5">
-        <v>57</v>
+        <v>58</v>
       </c>
     </row>
     <row r="6" spans="1:11">
@@ -3033,7 +3033,7 @@
         <v>1245</v>
       </c>
       <c r="K8">
-        <v>273</v>
+        <v>281</v>
       </c>
     </row>
     <row r="9" spans="1:11">
@@ -3068,7 +3068,7 @@
         <v>690</v>
       </c>
       <c r="K9">
-        <v>161</v>
+        <v>162</v>
       </c>
     </row>
     <row r="10" spans="1:11">
@@ -3103,7 +3103,7 @@
         <v>1719</v>
       </c>
       <c r="K10">
-        <v>389</v>
+        <v>396</v>
       </c>
     </row>
     <row r="11" spans="1:11">
@@ -3138,7 +3138,7 @@
         <v>5079</v>
       </c>
       <c r="K11">
-        <v>1185</v>
+        <v>1205</v>
       </c>
     </row>
   </sheetData>
@@ -3417,7 +3417,7 @@
         <v>85</v>
       </c>
       <c r="K8">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="9" spans="1:11">
@@ -3487,7 +3487,7 @@
         <v>308</v>
       </c>
       <c r="K10">
-        <v>77</v>
+        <v>79</v>
       </c>
     </row>
     <row r="11" spans="1:11">
@@ -3522,7 +3522,7 @@
         <v>539</v>
       </c>
       <c r="K11">
-        <v>124</v>
+        <v>127</v>
       </c>
     </row>
   </sheetData>
@@ -3618,7 +3618,7 @@
         <v>59</v>
       </c>
       <c r="K2">
-        <v>12</v>
+        <v>13</v>
       </c>
     </row>
     <row r="3" spans="1:11">
@@ -3822,7 +3822,7 @@
         <v>243</v>
       </c>
       <c r="K8">
-        <v>49</v>
+        <v>52</v>
       </c>
     </row>
     <row r="9" spans="1:11">
@@ -3892,7 +3892,7 @@
         <v>378</v>
       </c>
       <c r="K10">
-        <v>78</v>
+        <v>80</v>
       </c>
     </row>
     <row r="11" spans="1:11">
@@ -3927,7 +3927,7 @@
         <v>845</v>
       </c>
       <c r="K11">
-        <v>185</v>
+        <v>191</v>
       </c>
     </row>
   </sheetData>
@@ -4058,7 +4058,7 @@
         <v>26</v>
       </c>
       <c r="K3">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="4" spans="1:11">
@@ -4209,7 +4209,7 @@
         <v>197</v>
       </c>
       <c r="K8">
-        <v>42</v>
+        <v>43</v>
       </c>
     </row>
     <row r="9" spans="1:11">
@@ -4279,7 +4279,7 @@
         <v>150</v>
       </c>
       <c r="K10">
-        <v>40</v>
+        <v>41</v>
       </c>
     </row>
     <row r="11" spans="1:11">
@@ -4314,7 +4314,7 @@
         <v>449</v>
       </c>
       <c r="K11">
-        <v>102</v>
+        <v>105</v>
       </c>
     </row>
   </sheetData>
@@ -4410,7 +4410,7 @@
         <v>176</v>
       </c>
       <c r="K2">
-        <v>59</v>
+        <v>60</v>
       </c>
     </row>
     <row r="3" spans="1:11">
@@ -4515,7 +4515,7 @@
         <v>94</v>
       </c>
       <c r="K5">
-        <v>20</v>
+        <v>21</v>
       </c>
     </row>
     <row r="6" spans="1:11">
@@ -4547,7 +4547,7 @@
         <v>27</v>
       </c>
       <c r="J6">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="K6">
         <v>9</v>
@@ -4655,7 +4655,7 @@
         <v>162</v>
       </c>
       <c r="K9">
-        <v>31</v>
+        <v>32</v>
       </c>
     </row>
     <row r="10" spans="1:11">
@@ -4690,7 +4690,7 @@
         <v>598</v>
       </c>
       <c r="K10">
-        <v>137</v>
+        <v>141</v>
       </c>
     </row>
     <row r="11" spans="1:11">
@@ -4722,10 +4722,10 @@
         <v>1808</v>
       </c>
       <c r="J11">
-        <v>1814</v>
+        <v>1815</v>
       </c>
       <c r="K11">
-        <v>402</v>
+        <v>409</v>
       </c>
     </row>
   </sheetData>
@@ -4821,7 +4821,7 @@
         <v>295</v>
       </c>
       <c r="K2">
-        <v>76</v>
+        <v>77</v>
       </c>
     </row>
     <row r="3" spans="1:11">
@@ -4856,7 +4856,7 @@
         <v>437</v>
       </c>
       <c r="K3">
-        <v>107</v>
+        <v>108</v>
       </c>
     </row>
     <row r="4" spans="1:11">
@@ -4926,7 +4926,7 @@
         <v>144</v>
       </c>
       <c r="K5">
-        <v>45</v>
+        <v>46</v>
       </c>
     </row>
     <row r="6" spans="1:11">
@@ -5066,7 +5066,7 @@
         <v>473</v>
       </c>
       <c r="K9">
-        <v>71</v>
+        <v>73</v>
       </c>
     </row>
     <row r="10" spans="1:11">
@@ -5101,7 +5101,7 @@
         <v>1034</v>
       </c>
       <c r="K10">
-        <v>242</v>
+        <v>246</v>
       </c>
     </row>
     <row r="11" spans="1:11">
@@ -5136,7 +5136,7 @@
         <v>3405</v>
       </c>
       <c r="K11">
-        <v>715</v>
+        <v>724</v>
       </c>
     </row>
   </sheetData>
@@ -5232,7 +5232,7 @@
         <v>234</v>
       </c>
       <c r="K2">
-        <v>60</v>
+        <v>61</v>
       </c>
     </row>
     <row r="3" spans="1:11">
@@ -5337,7 +5337,7 @@
         <v>174</v>
       </c>
       <c r="K5">
-        <v>41</v>
+        <v>43</v>
       </c>
     </row>
     <row r="6" spans="1:11">
@@ -5442,7 +5442,7 @@
         <v>814</v>
       </c>
       <c r="K8">
-        <v>134</v>
+        <v>137</v>
       </c>
     </row>
     <row r="9" spans="1:11">
@@ -5512,7 +5512,7 @@
         <v>828</v>
       </c>
       <c r="K10">
-        <v>237</v>
+        <v>241</v>
       </c>
     </row>
     <row r="11" spans="1:11">
@@ -5547,7 +5547,7 @@
         <v>2633</v>
       </c>
       <c r="K11">
-        <v>594</v>
+        <v>604</v>
       </c>
     </row>
   </sheetData>
@@ -5643,7 +5643,7 @@
         <v>1144</v>
       </c>
       <c r="K2">
-        <v>286</v>
+        <v>290</v>
       </c>
     </row>
     <row r="3" spans="1:11">
@@ -5678,7 +5678,7 @@
         <v>202</v>
       </c>
       <c r="K3">
-        <v>64</v>
+        <v>66</v>
       </c>
     </row>
     <row r="4" spans="1:11">
@@ -5783,7 +5783,7 @@
         <v>1104</v>
       </c>
       <c r="K6">
-        <v>277</v>
+        <v>280</v>
       </c>
     </row>
     <row r="7" spans="1:11">
@@ -5818,7 +5818,7 @@
         <v>2991</v>
       </c>
       <c r="K7">
-        <v>646</v>
+        <v>656</v>
       </c>
     </row>
     <row r="8" spans="1:11">
@@ -5853,7 +5853,7 @@
         <v>5079</v>
       </c>
       <c r="K8">
-        <v>1185</v>
+        <v>1205</v>
       </c>
     </row>
     <row r="9" spans="1:11">
@@ -5888,7 +5888,7 @@
         <v>541</v>
       </c>
       <c r="K9">
-        <v>111</v>
+        <v>112</v>
       </c>
     </row>
     <row r="10" spans="1:11">
@@ -5920,10 +5920,10 @@
         <v>953</v>
       </c>
       <c r="J10">
-        <v>1155</v>
+        <v>1157</v>
       </c>
       <c r="K10">
-        <v>324</v>
+        <v>329</v>
       </c>
     </row>
     <row r="11" spans="1:11">
@@ -5958,7 +5958,7 @@
         <v>2170</v>
       </c>
       <c r="K11">
-        <v>578</v>
+        <v>582</v>
       </c>
     </row>
     <row r="12" spans="1:11">
@@ -6063,7 +6063,7 @@
         <v>741</v>
       </c>
       <c r="K14">
-        <v>167</v>
+        <v>168</v>
       </c>
     </row>
     <row r="15" spans="1:11">
@@ -6098,7 +6098,7 @@
         <v>1072</v>
       </c>
       <c r="K15">
-        <v>267</v>
+        <v>272</v>
       </c>
     </row>
     <row r="16" spans="1:11">
@@ -6133,7 +6133,7 @@
         <v>830</v>
       </c>
       <c r="K16">
-        <v>186</v>
+        <v>187</v>
       </c>
     </row>
     <row r="17" spans="1:11">
@@ -6203,7 +6203,7 @@
         <v>862</v>
       </c>
       <c r="K18">
-        <v>202</v>
+        <v>208</v>
       </c>
     </row>
     <row r="19" spans="1:11">
@@ -6238,7 +6238,7 @@
         <v>2867</v>
       </c>
       <c r="K19">
-        <v>689</v>
+        <v>696</v>
       </c>
     </row>
     <row r="20" spans="1:11">
@@ -6273,7 +6273,7 @@
         <v>2182</v>
       </c>
       <c r="K20">
-        <v>500</v>
+        <v>501</v>
       </c>
     </row>
     <row r="21" spans="1:11">
@@ -6308,7 +6308,7 @@
         <v>335</v>
       </c>
       <c r="K21">
-        <v>73</v>
+        <v>75</v>
       </c>
     </row>
     <row r="22" spans="1:11">
@@ -6378,7 +6378,7 @@
         <v>1593</v>
       </c>
       <c r="K23">
-        <v>301</v>
+        <v>303</v>
       </c>
     </row>
     <row r="24" spans="1:11">
@@ -6413,7 +6413,7 @@
         <v>736</v>
       </c>
       <c r="K24">
-        <v>162</v>
+        <v>164</v>
       </c>
     </row>
     <row r="25" spans="1:11">
@@ -6448,7 +6448,7 @@
         <v>596</v>
       </c>
       <c r="K25">
-        <v>104</v>
+        <v>106</v>
       </c>
     </row>
     <row r="26" spans="1:11">
@@ -6518,7 +6518,7 @@
         <v>1513</v>
       </c>
       <c r="K27">
-        <v>430</v>
+        <v>432</v>
       </c>
     </row>
     <row r="28" spans="1:11">
@@ -6585,10 +6585,10 @@
         <v>3981</v>
       </c>
       <c r="J29">
-        <v>4184</v>
+        <v>4183</v>
       </c>
       <c r="K29">
-        <v>911</v>
+        <v>921</v>
       </c>
     </row>
     <row r="30" spans="1:11">
@@ -6658,7 +6658,7 @@
         <v>1031</v>
       </c>
       <c r="K31">
-        <v>287</v>
+        <v>290</v>
       </c>
     </row>
     <row r="32" spans="1:11">
@@ -6693,7 +6693,7 @@
         <v>285</v>
       </c>
       <c r="K32">
-        <v>54</v>
+        <v>56</v>
       </c>
     </row>
     <row r="33" spans="1:11">
@@ -6728,7 +6728,7 @@
         <v>3405</v>
       </c>
       <c r="K33">
-        <v>715</v>
+        <v>724</v>
       </c>
     </row>
     <row r="34" spans="1:11">
@@ -6760,10 +6760,10 @@
         <v>766</v>
       </c>
       <c r="J34">
-        <v>951</v>
+        <v>952</v>
       </c>
       <c r="K34">
-        <v>298</v>
+        <v>300</v>
       </c>
     </row>
     <row r="35" spans="1:11">
@@ -6798,7 +6798,7 @@
         <v>268</v>
       </c>
       <c r="K35">
-        <v>73</v>
+        <v>74</v>
       </c>
     </row>
     <row r="36" spans="1:11">
@@ -6833,7 +6833,7 @@
         <v>1737</v>
       </c>
       <c r="K36">
-        <v>387</v>
+        <v>391</v>
       </c>
     </row>
     <row r="37" spans="1:11">
@@ -6868,7 +6868,7 @@
         <v>2977</v>
       </c>
       <c r="K37">
-        <v>723</v>
+        <v>733</v>
       </c>
     </row>
     <row r="38" spans="1:11">
@@ -6973,7 +6973,7 @@
         <v>299</v>
       </c>
       <c r="K40">
-        <v>87</v>
+        <v>90</v>
       </c>
     </row>
     <row r="41" spans="1:11">
@@ -7008,7 +7008,7 @@
         <v>647</v>
       </c>
       <c r="K41">
-        <v>136</v>
+        <v>137</v>
       </c>
     </row>
     <row r="42" spans="1:11">
@@ -7043,7 +7043,7 @@
         <v>3622</v>
       </c>
       <c r="K42">
-        <v>757</v>
+        <v>767</v>
       </c>
     </row>
     <row r="43" spans="1:11">
@@ -7078,7 +7078,7 @@
         <v>1454</v>
       </c>
       <c r="K43">
-        <v>326</v>
+        <v>330</v>
       </c>
     </row>
     <row r="44" spans="1:11">
@@ -7113,7 +7113,7 @@
         <v>1385</v>
       </c>
       <c r="K44">
-        <v>364</v>
+        <v>367</v>
       </c>
     </row>
     <row r="45" spans="1:11">
@@ -7148,7 +7148,7 @@
         <v>156</v>
       </c>
       <c r="K45">
-        <v>31</v>
+        <v>32</v>
       </c>
     </row>
     <row r="46" spans="1:11">
@@ -7183,7 +7183,7 @@
         <v>539</v>
       </c>
       <c r="K46">
-        <v>124</v>
+        <v>127</v>
       </c>
     </row>
     <row r="47" spans="1:11">
@@ -7218,7 +7218,7 @@
         <v>1025</v>
       </c>
       <c r="K47">
-        <v>248</v>
+        <v>251</v>
       </c>
     </row>
     <row r="48" spans="1:11">
@@ -7253,7 +7253,7 @@
         <v>3095</v>
       </c>
       <c r="K48">
-        <v>761</v>
+        <v>775</v>
       </c>
     </row>
     <row r="49" spans="1:11">
@@ -7288,7 +7288,7 @@
         <v>1841</v>
       </c>
       <c r="K49">
-        <v>481</v>
+        <v>487</v>
       </c>
     </row>
     <row r="50" spans="1:11">
@@ -7323,7 +7323,7 @@
         <v>1137</v>
       </c>
       <c r="K50">
-        <v>263</v>
+        <v>267</v>
       </c>
     </row>
     <row r="51" spans="1:11">
@@ -7358,7 +7358,7 @@
         <v>1652</v>
       </c>
       <c r="K51">
-        <v>357</v>
+        <v>359</v>
       </c>
     </row>
     <row r="52" spans="1:11">
@@ -7393,7 +7393,7 @@
         <v>1929</v>
       </c>
       <c r="K52">
-        <v>494</v>
+        <v>497</v>
       </c>
     </row>
     <row r="53" spans="1:11">
@@ -7428,7 +7428,7 @@
         <v>2251</v>
       </c>
       <c r="K53">
-        <v>603</v>
+        <v>604</v>
       </c>
     </row>
     <row r="54" spans="1:11">
@@ -7463,7 +7463,7 @@
         <v>3898</v>
       </c>
       <c r="K54">
-        <v>1030</v>
+        <v>1046</v>
       </c>
     </row>
     <row r="55" spans="1:11">
@@ -7498,7 +7498,7 @@
         <v>1477</v>
       </c>
       <c r="K55">
-        <v>325</v>
+        <v>330</v>
       </c>
     </row>
     <row r="56" spans="1:11">
@@ -7533,7 +7533,7 @@
         <v>670</v>
       </c>
       <c r="K56">
-        <v>193</v>
+        <v>200</v>
       </c>
     </row>
     <row r="57" spans="1:11">
@@ -7568,7 +7568,7 @@
         <v>553</v>
       </c>
       <c r="K57">
-        <v>134</v>
+        <v>135</v>
       </c>
     </row>
     <row r="58" spans="1:11">
@@ -7673,7 +7673,7 @@
         <v>845</v>
       </c>
       <c r="K60">
-        <v>185</v>
+        <v>191</v>
       </c>
     </row>
     <row r="61" spans="1:11">
@@ -7775,10 +7775,10 @@
         <v>1856</v>
       </c>
       <c r="J63">
-        <v>496</v>
+        <v>493</v>
       </c>
       <c r="K63">
-        <v>168</v>
+        <v>126</v>
       </c>
     </row>
     <row r="64" spans="1:11">
@@ -7813,7 +7813,7 @@
         <v>1207</v>
       </c>
       <c r="K64">
-        <v>256</v>
+        <v>259</v>
       </c>
     </row>
     <row r="65" spans="1:11">
@@ -7848,7 +7848,7 @@
         <v>1883</v>
       </c>
       <c r="K65">
-        <v>407</v>
+        <v>412</v>
       </c>
     </row>
     <row r="66" spans="1:11">
@@ -7883,7 +7883,7 @@
         <v>811</v>
       </c>
       <c r="K66">
-        <v>160</v>
+        <v>162</v>
       </c>
     </row>
     <row r="67" spans="1:11">
@@ -7918,7 +7918,7 @@
         <v>2748</v>
       </c>
       <c r="K67">
-        <v>569</v>
+        <v>573</v>
       </c>
     </row>
     <row r="68" spans="1:11">
@@ -7953,7 +7953,7 @@
         <v>421</v>
       </c>
       <c r="K68">
-        <v>104</v>
+        <v>108</v>
       </c>
     </row>
     <row r="69" spans="1:11">
@@ -7988,7 +7988,7 @@
         <v>496</v>
       </c>
       <c r="K69">
-        <v>160</v>
+        <v>165</v>
       </c>
     </row>
     <row r="70" spans="1:11">
@@ -8023,7 +8023,7 @@
         <v>739</v>
       </c>
       <c r="K70">
-        <v>189</v>
+        <v>192</v>
       </c>
     </row>
     <row r="71" spans="1:11">
@@ -8058,7 +8058,7 @@
         <v>449</v>
       </c>
       <c r="K71">
-        <v>102</v>
+        <v>105</v>
       </c>
     </row>
     <row r="72" spans="1:11">
@@ -8093,7 +8093,7 @@
         <v>766</v>
       </c>
       <c r="K72">
-        <v>181</v>
+        <v>186</v>
       </c>
     </row>
     <row r="73" spans="1:11">
@@ -8128,7 +8128,7 @@
         <v>1682</v>
       </c>
       <c r="K73">
-        <v>390</v>
+        <v>397</v>
       </c>
     </row>
     <row r="74" spans="1:11">
@@ -8163,7 +8163,7 @@
         <v>313</v>
       </c>
       <c r="K74">
-        <v>85</v>
+        <v>86</v>
       </c>
     </row>
     <row r="75" spans="1:11">
@@ -8198,7 +8198,7 @@
         <v>420</v>
       </c>
       <c r="K75">
-        <v>120</v>
+        <v>121</v>
       </c>
     </row>
     <row r="76" spans="1:11">
@@ -8233,7 +8233,7 @@
         <v>3197</v>
       </c>
       <c r="K76">
-        <v>724</v>
+        <v>732</v>
       </c>
     </row>
     <row r="77" spans="1:11">
@@ -8268,7 +8268,7 @@
         <v>524</v>
       </c>
       <c r="K77">
-        <v>115</v>
+        <v>117</v>
       </c>
     </row>
     <row r="78" spans="1:11">
@@ -8303,7 +8303,7 @@
         <v>2013</v>
       </c>
       <c r="K78">
-        <v>598</v>
+        <v>613</v>
       </c>
     </row>
     <row r="79" spans="1:11">
@@ -8338,7 +8338,7 @@
         <v>2633</v>
       </c>
       <c r="K79">
-        <v>594</v>
+        <v>604</v>
       </c>
     </row>
     <row r="80" spans="1:11">
@@ -8373,7 +8373,7 @@
         <v>356</v>
       </c>
       <c r="K80">
-        <v>100</v>
+        <v>102</v>
       </c>
     </row>
     <row r="81" spans="1:11">
@@ -8408,7 +8408,7 @@
         <v>256</v>
       </c>
       <c r="K81">
-        <v>56</v>
+        <v>58</v>
       </c>
     </row>
     <row r="82" spans="1:11">
@@ -8443,7 +8443,7 @@
         <v>283</v>
       </c>
       <c r="K82">
-        <v>81</v>
+        <v>82</v>
       </c>
     </row>
     <row r="83" spans="1:11">
@@ -8475,10 +8475,10 @@
         <v>1808</v>
       </c>
       <c r="J83">
-        <v>1814</v>
+        <v>1815</v>
       </c>
       <c r="K83">
-        <v>402</v>
+        <v>409</v>
       </c>
     </row>
     <row r="84" spans="1:11">
@@ -8513,7 +8513,7 @@
         <v>976</v>
       </c>
       <c r="K84">
-        <v>206</v>
+        <v>210</v>
       </c>
     </row>
     <row r="85" spans="1:11">
@@ -8545,10 +8545,10 @@
         <v>3862</v>
       </c>
       <c r="J85">
-        <v>4216</v>
+        <v>4217</v>
       </c>
       <c r="K85">
-        <v>1019</v>
+        <v>1026</v>
       </c>
     </row>
     <row r="86" spans="1:11">
@@ -8583,7 +8583,7 @@
         <v>1000</v>
       </c>
       <c r="K86">
-        <v>230</v>
+        <v>236</v>
       </c>
     </row>
     <row r="87" spans="1:11">
@@ -8653,7 +8653,7 @@
         <v>1063</v>
       </c>
       <c r="K88">
-        <v>262</v>
+        <v>267</v>
       </c>
     </row>
     <row r="89" spans="1:11">
@@ -8688,7 +8688,7 @@
         <v>2262</v>
       </c>
       <c r="K89">
-        <v>511</v>
+        <v>518</v>
       </c>
     </row>
     <row r="90" spans="1:11">
@@ -8723,7 +8723,7 @@
         <v>1437</v>
       </c>
       <c r="K90">
-        <v>297</v>
+        <v>298</v>
       </c>
     </row>
     <row r="91" spans="1:11">
@@ -8758,7 +8758,7 @@
         <v>1145</v>
       </c>
       <c r="K91">
-        <v>249</v>
+        <v>251</v>
       </c>
     </row>
     <row r="92" spans="1:11">
@@ -8793,7 +8793,7 @@
         <v>457</v>
       </c>
       <c r="K92">
-        <v>90</v>
+        <v>91</v>
       </c>
     </row>
     <row r="93" spans="1:11">
@@ -8828,7 +8828,7 @@
         <v>850</v>
       </c>
       <c r="K93">
-        <v>211</v>
+        <v>215</v>
       </c>
     </row>
     <row r="94" spans="1:11">
@@ -8863,7 +8863,7 @@
         <v>2779</v>
       </c>
       <c r="K94">
-        <v>721</v>
+        <v>733</v>
       </c>
     </row>
     <row r="95" spans="1:11">
@@ -8898,7 +8898,7 @@
         <v>1484</v>
       </c>
       <c r="K95">
-        <v>346</v>
+        <v>349</v>
       </c>
     </row>
     <row r="96" spans="1:11">
@@ -8933,7 +8933,7 @@
         <v>1810</v>
       </c>
       <c r="K96">
-        <v>483</v>
+        <v>493</v>
       </c>
     </row>
     <row r="97" spans="1:11">
@@ -8968,7 +8968,7 @@
         <v>1904</v>
       </c>
       <c r="K97">
-        <v>489</v>
+        <v>494</v>
       </c>
     </row>
     <row r="98" spans="1:11">
@@ -9003,7 +9003,7 @@
         <v>1353</v>
       </c>
       <c r="K98">
-        <v>366</v>
+        <v>370</v>
       </c>
     </row>
     <row r="99" spans="1:11">
@@ -9038,7 +9038,7 @@
         <v>1727</v>
       </c>
       <c r="K99">
-        <v>401</v>
+        <v>405</v>
       </c>
     </row>
     <row r="100" spans="1:11">
@@ -9105,10 +9105,10 @@
         <v>110581</v>
       </c>
       <c r="J101">
-        <v>123831</v>
+        <v>123832</v>
       </c>
       <c r="K101">
-        <v>29363</v>
+        <v>29700</v>
       </c>
     </row>
   </sheetData>
@@ -9571,7 +9571,7 @@
         <v>197</v>
       </c>
       <c r="K10">
-        <v>65</v>
+        <v>66</v>
       </c>
     </row>
     <row r="11" spans="1:11">
@@ -9606,7 +9606,7 @@
         <v>420</v>
       </c>
       <c r="K11">
-        <v>120</v>
+        <v>121</v>
       </c>
     </row>
   </sheetData>
@@ -9737,7 +9737,7 @@
         <v>25</v>
       </c>
       <c r="K3">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="4" spans="1:11">
@@ -9876,7 +9876,7 @@
         <v>98</v>
       </c>
       <c r="K8">
-        <v>28</v>
+        <v>29</v>
       </c>
     </row>
     <row r="9" spans="1:11">
@@ -9946,7 +9946,7 @@
         <v>116</v>
       </c>
       <c r="K10">
-        <v>42</v>
+        <v>43</v>
       </c>
     </row>
     <row r="11" spans="1:11">
@@ -9981,7 +9981,7 @@
         <v>299</v>
       </c>
       <c r="K11">
-        <v>87</v>
+        <v>90</v>
       </c>
     </row>
   </sheetData>
@@ -10176,7 +10176,7 @@
         <v>65</v>
       </c>
       <c r="K5">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="6" spans="1:11">
@@ -10348,7 +10348,7 @@
         <v>584</v>
       </c>
       <c r="K10">
-        <v>133</v>
+        <v>135</v>
       </c>
     </row>
     <row r="11" spans="1:11">
@@ -10383,7 +10383,7 @@
         <v>1207</v>
       </c>
       <c r="K11">
-        <v>256</v>
+        <v>259</v>
       </c>
     </row>
   </sheetData>
@@ -10584,7 +10584,7 @@
         <v>78</v>
       </c>
       <c r="K5">
-        <v>26</v>
+        <v>27</v>
       </c>
     </row>
     <row r="6" spans="1:11">
@@ -10759,7 +10759,7 @@
         <v>491</v>
       </c>
       <c r="K10">
-        <v>143</v>
+        <v>145</v>
       </c>
     </row>
     <row r="11" spans="1:11">
@@ -10794,7 +10794,7 @@
         <v>1484</v>
       </c>
       <c r="K11">
-        <v>346</v>
+        <v>349</v>
       </c>
     </row>
   </sheetData>
@@ -10925,7 +10925,7 @@
         <v>303</v>
       </c>
       <c r="K3">
-        <v>75</v>
+        <v>76</v>
       </c>
     </row>
     <row r="4" spans="1:11">
@@ -10960,7 +10960,7 @@
         <v>18</v>
       </c>
       <c r="K4">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="5" spans="1:11">
@@ -11100,7 +11100,7 @@
         <v>892</v>
       </c>
       <c r="K8">
-        <v>171</v>
+        <v>175</v>
       </c>
     </row>
     <row r="9" spans="1:11">
@@ -11170,7 +11170,7 @@
         <v>939</v>
       </c>
       <c r="K10">
-        <v>261</v>
+        <v>265</v>
       </c>
     </row>
     <row r="11" spans="1:11">
@@ -11205,7 +11205,7 @@
         <v>2977</v>
       </c>
       <c r="K11">
-        <v>723</v>
+        <v>733</v>
       </c>
     </row>
   </sheetData>
@@ -11336,7 +11336,7 @@
         <v>42</v>
       </c>
       <c r="K3">
-        <v>14</v>
+        <v>15</v>
       </c>
     </row>
     <row r="4" spans="1:11">
@@ -11534,7 +11534,7 @@
         <v>65</v>
       </c>
       <c r="K9">
-        <v>30</v>
+        <v>31</v>
       </c>
     </row>
     <row r="10" spans="1:11">
@@ -11604,7 +11604,7 @@
         <v>1513</v>
       </c>
       <c r="K11">
-        <v>430</v>
+        <v>432</v>
       </c>
     </row>
   </sheetData>
@@ -11700,7 +11700,7 @@
         <v>211</v>
       </c>
       <c r="K2">
-        <v>45</v>
+        <v>47</v>
       </c>
     </row>
     <row r="3" spans="1:11">
@@ -11805,7 +11805,7 @@
         <v>106</v>
       </c>
       <c r="K5">
-        <v>26</v>
+        <v>28</v>
       </c>
     </row>
     <row r="6" spans="1:11">
@@ -11945,7 +11945,7 @@
         <v>274</v>
       </c>
       <c r="K9">
-        <v>71</v>
+        <v>72</v>
       </c>
     </row>
     <row r="10" spans="1:11">
@@ -12015,7 +12015,7 @@
         <v>1883</v>
       </c>
       <c r="K11">
-        <v>407</v>
+        <v>412</v>
       </c>
     </row>
   </sheetData>
@@ -12146,7 +12146,7 @@
         <v>174</v>
       </c>
       <c r="K3">
-        <v>40</v>
+        <v>41</v>
       </c>
     </row>
     <row r="4" spans="1:11">
@@ -12391,7 +12391,7 @@
         <v>630</v>
       </c>
       <c r="K10">
-        <v>155</v>
+        <v>158</v>
       </c>
     </row>
     <row r="11" spans="1:11">
@@ -12426,7 +12426,7 @@
         <v>1727</v>
       </c>
       <c r="K11">
-        <v>401</v>
+        <v>405</v>
       </c>
     </row>
   </sheetData>
@@ -13020,7 +13020,7 @@
         <v>75</v>
       </c>
       <c r="K5">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="6" spans="1:11">
@@ -13195,7 +13195,7 @@
         <v>404</v>
       </c>
       <c r="K10">
-        <v>130</v>
+        <v>132</v>
       </c>
     </row>
     <row r="11" spans="1:11">
@@ -13230,7 +13230,7 @@
         <v>1031</v>
       </c>
       <c r="K11">
-        <v>287</v>
+        <v>290</v>
       </c>
     </row>
   </sheetData>
@@ -13521,7 +13521,7 @@
         <v>171</v>
       </c>
       <c r="K8">
-        <v>18</v>
+        <v>19</v>
       </c>
     </row>
     <row r="9" spans="1:11">
@@ -13626,7 +13626,7 @@
         <v>741</v>
       </c>
       <c r="K11">
-        <v>167</v>
+        <v>168</v>
       </c>
     </row>
   </sheetData>
@@ -13932,7 +13932,7 @@
         <v>664</v>
       </c>
       <c r="K8">
-        <v>110</v>
+        <v>111</v>
       </c>
     </row>
     <row r="9" spans="1:11">
@@ -13967,7 +13967,7 @@
         <v>293</v>
       </c>
       <c r="K9">
-        <v>88</v>
+        <v>90</v>
       </c>
     </row>
     <row r="10" spans="1:11">
@@ -14002,7 +14002,7 @@
         <v>886</v>
       </c>
       <c r="K10">
-        <v>160</v>
+        <v>161</v>
       </c>
     </row>
     <row r="11" spans="1:11">
@@ -14037,7 +14037,7 @@
         <v>2748</v>
       </c>
       <c r="K11">
-        <v>569</v>
+        <v>573</v>
       </c>
     </row>
   </sheetData>
@@ -14168,7 +14168,7 @@
         <v>76</v>
       </c>
       <c r="K3">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="4" spans="1:11">
@@ -14337,7 +14337,7 @@
         <v>344</v>
       </c>
       <c r="K8">
-        <v>54</v>
+        <v>57</v>
       </c>
     </row>
     <row r="9" spans="1:11">
@@ -14442,7 +14442,7 @@
         <v>976</v>
       </c>
       <c r="K11">
-        <v>206</v>
+        <v>210</v>
       </c>
     </row>
   </sheetData>
@@ -14730,7 +14730,7 @@
         <v>423</v>
       </c>
       <c r="K8">
-        <v>99</v>
+        <v>101</v>
       </c>
     </row>
     <row r="9" spans="1:11">
@@ -14800,7 +14800,7 @@
         <v>1911</v>
       </c>
       <c r="K10">
-        <v>516</v>
+        <v>526</v>
       </c>
     </row>
     <row r="11" spans="1:11">
@@ -14835,7 +14835,7 @@
         <v>2779</v>
       </c>
       <c r="K11">
-        <v>721</v>
+        <v>733</v>
       </c>
     </row>
   </sheetData>
@@ -15132,7 +15132,7 @@
         <v>331</v>
       </c>
       <c r="K8">
-        <v>86</v>
+        <v>87</v>
       </c>
     </row>
     <row r="9" spans="1:11">
@@ -15167,7 +15167,7 @@
         <v>214</v>
       </c>
       <c r="K9">
-        <v>55</v>
+        <v>58</v>
       </c>
     </row>
     <row r="10" spans="1:11">
@@ -15202,7 +15202,7 @@
         <v>2314</v>
       </c>
       <c r="K10">
-        <v>504</v>
+        <v>508</v>
       </c>
     </row>
     <row r="11" spans="1:11">
@@ -15237,7 +15237,7 @@
         <v>3197</v>
       </c>
       <c r="K11">
-        <v>724</v>
+        <v>732</v>
       </c>
     </row>
   </sheetData>
@@ -15930,7 +15930,7 @@
         <v>138</v>
       </c>
       <c r="K8">
-        <v>32</v>
+        <v>34</v>
       </c>
     </row>
     <row r="9" spans="1:11">
@@ -16035,7 +16035,7 @@
         <v>596</v>
       </c>
       <c r="K11">
-        <v>104</v>
+        <v>106</v>
       </c>
     </row>
   </sheetData>
@@ -16735,7 +16735,7 @@
         <v>528</v>
       </c>
       <c r="K10">
-        <v>127</v>
+        <v>128</v>
       </c>
     </row>
     <row r="11" spans="1:11">
@@ -16770,7 +16770,7 @@
         <v>830</v>
       </c>
       <c r="K11">
-        <v>186</v>
+        <v>187</v>
       </c>
     </row>
   </sheetData>
@@ -16968,7 +16968,7 @@
         <v>152</v>
       </c>
       <c r="K5">
-        <v>38</v>
+        <v>39</v>
       </c>
     </row>
     <row r="6" spans="1:11">
@@ -17058,7 +17058,7 @@
         <v>240</v>
       </c>
       <c r="K8">
-        <v>52</v>
+        <v>53</v>
       </c>
     </row>
     <row r="9" spans="1:11">
@@ -17093,7 +17093,7 @@
         <v>100</v>
       </c>
       <c r="K9">
-        <v>26</v>
+        <v>27</v>
       </c>
     </row>
     <row r="10" spans="1:11">
@@ -17128,7 +17128,7 @@
         <v>1268</v>
       </c>
       <c r="K10">
-        <v>351</v>
+        <v>354</v>
       </c>
     </row>
     <row r="11" spans="1:11">
@@ -17163,7 +17163,7 @@
         <v>1841</v>
       </c>
       <c r="K11">
-        <v>481</v>
+        <v>487</v>
       </c>
     </row>
   </sheetData>
@@ -17259,7 +17259,7 @@
         <v>46</v>
       </c>
       <c r="K2">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="3" spans="1:11">
@@ -17361,7 +17361,7 @@
         <v>134</v>
       </c>
       <c r="K5">
-        <v>46</v>
+        <v>47</v>
       </c>
     </row>
     <row r="6" spans="1:11">
@@ -17463,7 +17463,7 @@
         <v>496</v>
       </c>
       <c r="K8">
-        <v>118</v>
+        <v>119</v>
       </c>
     </row>
     <row r="9" spans="1:11">
@@ -17533,7 +17533,7 @@
         <v>1013</v>
       </c>
       <c r="K10">
-        <v>262</v>
+        <v>264</v>
       </c>
     </row>
     <row r="11" spans="1:11">
@@ -17568,7 +17568,7 @@
         <v>1904</v>
       </c>
       <c r="K11">
-        <v>489</v>
+        <v>494</v>
       </c>
     </row>
   </sheetData>
@@ -17699,7 +17699,7 @@
         <v>83</v>
       </c>
       <c r="K3">
-        <v>14</v>
+        <v>16</v>
       </c>
     </row>
     <row r="4" spans="1:11">
@@ -17769,7 +17769,7 @@
         <v>168</v>
       </c>
       <c r="K5">
-        <v>38</v>
+        <v>39</v>
       </c>
     </row>
     <row r="6" spans="1:11">
@@ -17909,7 +17909,7 @@
         <v>128</v>
       </c>
       <c r="K9">
-        <v>45</v>
+        <v>46</v>
       </c>
     </row>
     <row r="10" spans="1:11">
@@ -17944,7 +17944,7 @@
         <v>864</v>
       </c>
       <c r="K10">
-        <v>198</v>
+        <v>204</v>
       </c>
     </row>
     <row r="11" spans="1:11">
@@ -17979,7 +17979,7 @@
         <v>1810</v>
       </c>
       <c r="K11">
-        <v>483</v>
+        <v>493</v>
       </c>
     </row>
   </sheetData>
@@ -18110,7 +18110,7 @@
         <v>90</v>
       </c>
       <c r="K3">
-        <v>14</v>
+        <v>15</v>
       </c>
     </row>
     <row r="4" spans="1:11">
@@ -18282,7 +18282,7 @@
         <v>326</v>
       </c>
       <c r="K8">
-        <v>80</v>
+        <v>81</v>
       </c>
     </row>
     <row r="9" spans="1:11">
@@ -18317,7 +18317,7 @@
         <v>257</v>
       </c>
       <c r="K9">
-        <v>24</v>
+        <v>25</v>
       </c>
     </row>
     <row r="10" spans="1:11">
@@ -18352,7 +18352,7 @@
         <v>620</v>
       </c>
       <c r="K10">
-        <v>157</v>
+        <v>159</v>
       </c>
     </row>
     <row r="11" spans="1:11">
@@ -18387,7 +18387,7 @@
         <v>1477</v>
       </c>
       <c r="K11">
-        <v>325</v>
+        <v>330</v>
       </c>
     </row>
   </sheetData>
@@ -18623,7 +18623,7 @@
         <v>49</v>
       </c>
       <c r="K6">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="7" spans="1:11">
@@ -18690,7 +18690,7 @@
         <v>420</v>
       </c>
       <c r="K8">
-        <v>138</v>
+        <v>140</v>
       </c>
     </row>
     <row r="9" spans="1:11">
@@ -18725,7 +18725,7 @@
         <v>263</v>
       </c>
       <c r="K9">
-        <v>49</v>
+        <v>50</v>
       </c>
     </row>
     <row r="10" spans="1:11">
@@ -18760,7 +18760,7 @@
         <v>2808</v>
       </c>
       <c r="K10">
-        <v>744</v>
+        <v>756</v>
       </c>
     </row>
     <row r="11" spans="1:11">
@@ -18795,7 +18795,7 @@
         <v>3898</v>
       </c>
       <c r="K11">
-        <v>1030</v>
+        <v>1046</v>
       </c>
     </row>
   </sheetData>
@@ -18891,7 +18891,7 @@
         <v>88</v>
       </c>
       <c r="K2">
-        <v>19</v>
+        <v>20</v>
       </c>
     </row>
     <row r="3" spans="1:11">
@@ -18926,7 +18926,7 @@
         <v>75</v>
       </c>
       <c r="K3">
-        <v>16</v>
+        <v>17</v>
       </c>
     </row>
     <row r="4" spans="1:11">
@@ -18996,7 +18996,7 @@
         <v>117</v>
       </c>
       <c r="K5">
-        <v>28</v>
+        <v>29</v>
       </c>
     </row>
     <row r="6" spans="1:11">
@@ -19098,7 +19098,7 @@
         <v>384</v>
       </c>
       <c r="K8">
-        <v>88</v>
+        <v>90</v>
       </c>
     </row>
     <row r="9" spans="1:11">
@@ -19133,7 +19133,7 @@
         <v>105</v>
       </c>
       <c r="K9">
-        <v>27</v>
+        <v>28</v>
       </c>
     </row>
     <row r="10" spans="1:11">
@@ -19168,7 +19168,7 @@
         <v>884</v>
       </c>
       <c r="K10">
-        <v>208</v>
+        <v>209</v>
       </c>
     </row>
     <row r="11" spans="1:11">
@@ -19203,7 +19203,7 @@
         <v>1682</v>
       </c>
       <c r="K11">
-        <v>390</v>
+        <v>397</v>
       </c>
     </row>
   </sheetData>
@@ -19299,7 +19299,7 @@
         <v>471</v>
       </c>
       <c r="K2">
-        <v>86</v>
+        <v>88</v>
       </c>
     </row>
     <row r="3" spans="1:11">
@@ -19334,7 +19334,7 @@
         <v>547</v>
       </c>
       <c r="K3">
-        <v>110</v>
+        <v>112</v>
       </c>
     </row>
     <row r="4" spans="1:11">
@@ -19436,10 +19436,10 @@
         <v>87</v>
       </c>
       <c r="J6">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="K6">
-        <v>16</v>
+        <v>17</v>
       </c>
     </row>
     <row r="7" spans="1:11">
@@ -19509,7 +19509,7 @@
         <v>1033</v>
       </c>
       <c r="K8">
-        <v>222</v>
+        <v>223</v>
       </c>
     </row>
     <row r="9" spans="1:11">
@@ -19579,7 +19579,7 @@
         <v>1305</v>
       </c>
       <c r="K10">
-        <v>303</v>
+        <v>307</v>
       </c>
     </row>
     <row r="11" spans="1:11">
@@ -19611,10 +19611,10 @@
         <v>3981</v>
       </c>
       <c r="J11">
-        <v>4184</v>
+        <v>4183</v>
       </c>
       <c r="K11">
-        <v>911</v>
+        <v>921</v>
       </c>
     </row>
   </sheetData>
@@ -19812,7 +19812,7 @@
         <v>183</v>
       </c>
       <c r="K5">
-        <v>71</v>
+        <v>72</v>
       </c>
     </row>
     <row r="6" spans="1:11">
@@ -19908,7 +19908,7 @@
         <v>462</v>
       </c>
       <c r="K8">
-        <v>94</v>
+        <v>96</v>
       </c>
     </row>
     <row r="9" spans="1:11">
@@ -19943,7 +19943,7 @@
         <v>154</v>
       </c>
       <c r="K9">
-        <v>39</v>
+        <v>40</v>
       </c>
     </row>
     <row r="10" spans="1:11">
@@ -19978,7 +19978,7 @@
         <v>2124</v>
       </c>
       <c r="K10">
-        <v>515</v>
+        <v>525</v>
       </c>
     </row>
     <row r="11" spans="1:11">
@@ -20013,7 +20013,7 @@
         <v>3095</v>
       </c>
       <c r="K11">
-        <v>761</v>
+        <v>775</v>
       </c>
     </row>
   </sheetData>
@@ -20109,7 +20109,7 @@
         <v>212</v>
       </c>
       <c r="K2">
-        <v>58</v>
+        <v>60</v>
       </c>
     </row>
     <row r="3" spans="1:11">
@@ -20214,7 +20214,7 @@
         <v>197</v>
       </c>
       <c r="K5">
-        <v>54</v>
+        <v>55</v>
       </c>
     </row>
     <row r="6" spans="1:11">
@@ -20249,7 +20249,7 @@
         <v>44</v>
       </c>
       <c r="K6">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="7" spans="1:11">
@@ -20319,7 +20319,7 @@
         <v>776</v>
       </c>
       <c r="K8">
-        <v>177</v>
+        <v>179</v>
       </c>
     </row>
     <row r="9" spans="1:11">
@@ -20389,7 +20389,7 @@
         <v>1018</v>
       </c>
       <c r="K10">
-        <v>265</v>
+        <v>266</v>
       </c>
     </row>
     <row r="11" spans="1:11">
@@ -20424,7 +20424,7 @@
         <v>2867</v>
       </c>
       <c r="K11">
-        <v>689</v>
+        <v>696</v>
       </c>
     </row>
   </sheetData>
@@ -20613,7 +20613,7 @@
         <v>106</v>
       </c>
       <c r="K5">
-        <v>19</v>
+        <v>20</v>
       </c>
     </row>
     <row r="6" spans="1:11">
@@ -20694,7 +20694,7 @@
         <v>146</v>
       </c>
       <c r="K8">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="9" spans="1:11">
@@ -20799,7 +20799,7 @@
         <v>811</v>
       </c>
       <c r="K11">
-        <v>160</v>
+        <v>162</v>
       </c>
     </row>
   </sheetData>
@@ -20930,7 +20930,7 @@
         <v>51</v>
       </c>
       <c r="K3">
-        <v>19</v>
+        <v>20</v>
       </c>
     </row>
     <row r="4" spans="1:11">
@@ -21169,7 +21169,7 @@
         <v>724</v>
       </c>
       <c r="K10">
-        <v>182</v>
+        <v>184</v>
       </c>
     </row>
     <row r="11" spans="1:11">
@@ -21204,7 +21204,7 @@
         <v>1385</v>
       </c>
       <c r="K11">
-        <v>364</v>
+        <v>367</v>
       </c>
     </row>
   </sheetData>
@@ -21335,7 +21335,7 @@
         <v>250</v>
       </c>
       <c r="K3">
-        <v>67</v>
+        <v>69</v>
       </c>
     </row>
     <row r="4" spans="1:11">
@@ -21405,7 +21405,7 @@
         <v>181</v>
       </c>
       <c r="K5">
-        <v>46</v>
+        <v>47</v>
       </c>
     </row>
     <row r="6" spans="1:11">
@@ -21510,7 +21510,7 @@
         <v>910</v>
       </c>
       <c r="K8">
-        <v>182</v>
+        <v>186</v>
       </c>
     </row>
     <row r="9" spans="1:11">
@@ -21580,7 +21580,7 @@
         <v>1271</v>
       </c>
       <c r="K10">
-        <v>285</v>
+        <v>288</v>
       </c>
     </row>
     <row r="11" spans="1:11">
@@ -21615,7 +21615,7 @@
         <v>3622</v>
       </c>
       <c r="K11">
-        <v>757</v>
+        <v>767</v>
       </c>
     </row>
   </sheetData>
@@ -22104,7 +22104,7 @@
         <v>258</v>
       </c>
       <c r="K2">
-        <v>69</v>
+        <v>70</v>
       </c>
     </row>
     <row r="3" spans="1:11">
@@ -22311,7 +22311,7 @@
         <v>945</v>
       </c>
       <c r="K8">
-        <v>164</v>
+        <v>170</v>
       </c>
     </row>
     <row r="9" spans="1:11">
@@ -22346,7 +22346,7 @@
         <v>257</v>
       </c>
       <c r="K9">
-        <v>53</v>
+        <v>54</v>
       </c>
     </row>
     <row r="10" spans="1:11">
@@ -22381,7 +22381,7 @@
         <v>982</v>
       </c>
       <c r="K10">
-        <v>232</v>
+        <v>234</v>
       </c>
     </row>
     <row r="11" spans="1:11">
@@ -22416,7 +22416,7 @@
         <v>2991</v>
       </c>
       <c r="K11">
-        <v>646</v>
+        <v>656</v>
       </c>
     </row>
   </sheetData>
@@ -22547,7 +22547,7 @@
         <v>55</v>
       </c>
       <c r="K3">
-        <v>15</v>
+        <v>16</v>
       </c>
     </row>
     <row r="4" spans="1:11">
@@ -22716,7 +22716,7 @@
         <v>385</v>
       </c>
       <c r="K8">
-        <v>84</v>
+        <v>86</v>
       </c>
     </row>
     <row r="9" spans="1:11">
@@ -22821,7 +22821,7 @@
         <v>1104</v>
       </c>
       <c r="K11">
-        <v>277</v>
+        <v>280</v>
       </c>
     </row>
   </sheetData>
@@ -22952,7 +22952,7 @@
         <v>36</v>
       </c>
       <c r="K3">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="4" spans="1:11">
@@ -23226,7 +23226,7 @@
         <v>647</v>
       </c>
       <c r="K11">
-        <v>136</v>
+        <v>137</v>
       </c>
     </row>
   </sheetData>
@@ -23357,7 +23357,7 @@
         <v>132</v>
       </c>
       <c r="K3">
-        <v>29</v>
+        <v>30</v>
       </c>
     </row>
     <row r="4" spans="1:11">
@@ -23529,7 +23529,7 @@
         <v>620</v>
       </c>
       <c r="K8">
-        <v>118</v>
+        <v>120</v>
       </c>
     </row>
     <row r="9" spans="1:11">
@@ -23599,7 +23599,7 @@
         <v>632</v>
       </c>
       <c r="K10">
-        <v>154</v>
+        <v>155</v>
       </c>
     </row>
     <row r="11" spans="1:11">
@@ -23634,7 +23634,7 @@
         <v>1737</v>
       </c>
       <c r="K11">
-        <v>387</v>
+        <v>391</v>
       </c>
     </row>
   </sheetData>
@@ -24184,7 +24184,7 @@
         <v>79</v>
       </c>
       <c r="J5">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="K5">
         <v>22</v>
@@ -24356,10 +24356,10 @@
         <v>544</v>
       </c>
       <c r="J10">
-        <v>651</v>
+        <v>652</v>
       </c>
       <c r="K10">
-        <v>212</v>
+        <v>217</v>
       </c>
     </row>
     <row r="11" spans="1:11">
@@ -24391,10 +24391,10 @@
         <v>953</v>
       </c>
       <c r="J11">
-        <v>1155</v>
+        <v>1157</v>
       </c>
       <c r="K11">
-        <v>324</v>
+        <v>329</v>
       </c>
     </row>
   </sheetData>
@@ -24615,7 +24615,7 @@
         <v>94</v>
       </c>
       <c r="K6">
-        <v>20</v>
+        <v>21</v>
       </c>
     </row>
     <row r="7" spans="1:11">
@@ -24664,7 +24664,7 @@
         <v>112</v>
       </c>
       <c r="K8">
-        <v>26</v>
+        <v>27</v>
       </c>
     </row>
     <row r="9" spans="1:11">
@@ -24734,7 +24734,7 @@
         <v>693</v>
       </c>
       <c r="K10">
-        <v>153</v>
+        <v>157</v>
       </c>
     </row>
     <row r="11" spans="1:11">
@@ -24769,7 +24769,7 @@
         <v>1000</v>
       </c>
       <c r="K11">
-        <v>230</v>
+        <v>236</v>
       </c>
     </row>
   </sheetData>
@@ -24900,7 +24900,7 @@
         <v>104</v>
       </c>
       <c r="K3">
-        <v>20</v>
+        <v>21</v>
       </c>
     </row>
     <row r="4" spans="1:11">
@@ -24970,7 +24970,7 @@
         <v>105</v>
       </c>
       <c r="K5">
-        <v>36</v>
+        <v>37</v>
       </c>
     </row>
     <row r="6" spans="1:11">
@@ -25075,7 +25075,7 @@
         <v>430</v>
       </c>
       <c r="K8">
-        <v>130</v>
+        <v>136</v>
       </c>
     </row>
     <row r="9" spans="1:11">
@@ -25110,7 +25110,7 @@
         <v>106</v>
       </c>
       <c r="K9">
-        <v>31</v>
+        <v>32</v>
       </c>
     </row>
     <row r="10" spans="1:11">
@@ -25145,7 +25145,7 @@
         <v>1136</v>
       </c>
       <c r="K10">
-        <v>344</v>
+        <v>350</v>
       </c>
     </row>
     <row r="11" spans="1:11">
@@ -25180,7 +25180,7 @@
         <v>2013</v>
       </c>
       <c r="K11">
-        <v>598</v>
+        <v>613</v>
       </c>
     </row>
   </sheetData>
@@ -25311,7 +25311,7 @@
         <v>17</v>
       </c>
       <c r="K3">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="4" spans="1:11">
@@ -25372,7 +25372,7 @@
         <v>43</v>
       </c>
       <c r="K5">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="6" spans="1:11">
@@ -25535,7 +25535,7 @@
         <v>228</v>
       </c>
       <c r="K10">
-        <v>62</v>
+        <v>64</v>
       </c>
     </row>
     <row r="11" spans="1:11">
@@ -25570,7 +25570,7 @@
         <v>421</v>
       </c>
       <c r="K11">
-        <v>104</v>
+        <v>108</v>
       </c>
     </row>
   </sheetData>
@@ -25666,7 +25666,7 @@
         <v>32</v>
       </c>
       <c r="K2">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="3" spans="1:11">
@@ -25858,7 +25858,7 @@
         <v>188</v>
       </c>
       <c r="K8">
-        <v>34</v>
+        <v>35</v>
       </c>
     </row>
     <row r="9" spans="1:11">
@@ -25963,7 +25963,7 @@
         <v>736</v>
       </c>
       <c r="K11">
-        <v>162</v>
+        <v>164</v>
       </c>
     </row>
   </sheetData>
@@ -26059,7 +26059,7 @@
         <v>98</v>
       </c>
       <c r="K2">
-        <v>19</v>
+        <v>20</v>
       </c>
     </row>
     <row r="3" spans="1:11">
@@ -26269,7 +26269,7 @@
         <v>221</v>
       </c>
       <c r="K8">
-        <v>57</v>
+        <v>59</v>
       </c>
     </row>
     <row r="9" spans="1:11">
@@ -26339,7 +26339,7 @@
         <v>425</v>
       </c>
       <c r="K10">
-        <v>129</v>
+        <v>131</v>
       </c>
     </row>
     <row r="11" spans="1:11">
@@ -26374,7 +26374,7 @@
         <v>1072</v>
       </c>
       <c r="K11">
-        <v>267</v>
+        <v>272</v>
       </c>
     </row>
   </sheetData>
@@ -26677,7 +26677,7 @@
         <v>524</v>
       </c>
       <c r="K8">
-        <v>118</v>
+        <v>120</v>
       </c>
     </row>
     <row r="9" spans="1:11">
@@ -26747,7 +26747,7 @@
         <v>963</v>
       </c>
       <c r="K10">
-        <v>287</v>
+        <v>289</v>
       </c>
     </row>
     <row r="11" spans="1:11">
@@ -26782,7 +26782,7 @@
         <v>2170</v>
       </c>
       <c r="K11">
-        <v>578</v>
+        <v>582</v>
       </c>
     </row>
   </sheetData>
@@ -27076,7 +27076,7 @@
         <v>592</v>
       </c>
       <c r="K8">
-        <v>76</v>
+        <v>77</v>
       </c>
     </row>
     <row r="9" spans="1:11">
@@ -27146,7 +27146,7 @@
         <v>677</v>
       </c>
       <c r="K10">
-        <v>150</v>
+        <v>151</v>
       </c>
     </row>
     <row r="11" spans="1:11">
@@ -27181,7 +27181,7 @@
         <v>1593</v>
       </c>
       <c r="K11">
-        <v>301</v>
+        <v>303</v>
       </c>
     </row>
   </sheetData>
@@ -27452,7 +27452,7 @@
         <v>10</v>
       </c>
       <c r="K7">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="8" spans="1:11">
@@ -27557,7 +27557,7 @@
         <v>341</v>
       </c>
       <c r="K10">
-        <v>91</v>
+        <v>92</v>
       </c>
     </row>
     <row r="11" spans="1:11">
@@ -27592,7 +27592,7 @@
         <v>1145</v>
       </c>
       <c r="K11">
-        <v>249</v>
+        <v>251</v>
       </c>
     </row>
   </sheetData>
@@ -27965,7 +27965,7 @@
         <v>749</v>
       </c>
       <c r="K10">
-        <v>187</v>
+        <v>189</v>
       </c>
     </row>
     <row r="11" spans="1:11">
@@ -28000,7 +28000,7 @@
         <v>1652</v>
       </c>
       <c r="K11">
-        <v>357</v>
+        <v>359</v>
       </c>
     </row>
   </sheetData>
@@ -28096,7 +28096,7 @@
         <v>173</v>
       </c>
       <c r="K2">
-        <v>47</v>
+        <v>48</v>
       </c>
     </row>
     <row r="3" spans="1:11">
@@ -28411,7 +28411,7 @@
         <v>2182</v>
       </c>
       <c r="K11">
-        <v>500</v>
+        <v>501</v>
       </c>
     </row>
   </sheetData>
@@ -28739,7 +28739,7 @@
         <v>187</v>
       </c>
       <c r="K10">
-        <v>37</v>
+        <v>39</v>
       </c>
     </row>
     <row r="11" spans="1:11">
@@ -28774,7 +28774,7 @@
         <v>335</v>
       </c>
       <c r="K11">
-        <v>73</v>
+        <v>75</v>
       </c>
     </row>
   </sheetData>
@@ -29068,7 +29068,7 @@
         <v>319</v>
       </c>
       <c r="K8">
-        <v>72</v>
+        <v>74</v>
       </c>
     </row>
     <row r="9" spans="1:11">
@@ -29138,7 +29138,7 @@
         <v>444</v>
       </c>
       <c r="K10">
-        <v>125</v>
+        <v>126</v>
       </c>
     </row>
     <row r="11" spans="1:11">
@@ -29173,7 +29173,7 @@
         <v>1025</v>
       </c>
       <c r="K11">
-        <v>248</v>
+        <v>251</v>
       </c>
     </row>
   </sheetData>
@@ -29546,7 +29546,7 @@
         <v>520</v>
       </c>
       <c r="K10">
-        <v>138</v>
+        <v>139</v>
       </c>
     </row>
     <row r="11" spans="1:11">
@@ -29581,7 +29581,7 @@
         <v>1437</v>
       </c>
       <c r="K11">
-        <v>297</v>
+        <v>298</v>
       </c>
     </row>
   </sheetData>
@@ -29773,7 +29773,7 @@
         <v>130</v>
       </c>
       <c r="K5">
-        <v>31</v>
+        <v>32</v>
       </c>
     </row>
     <row r="6" spans="1:11">
@@ -29907,7 +29907,7 @@
         <v>62</v>
       </c>
       <c r="K9">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="10" spans="1:11">
@@ -29942,7 +29942,7 @@
         <v>637</v>
       </c>
       <c r="K10">
-        <v>147</v>
+        <v>149</v>
       </c>
     </row>
     <row r="11" spans="1:11">
@@ -29977,7 +29977,7 @@
         <v>1137</v>
       </c>
       <c r="K11">
-        <v>263</v>
+        <v>267</v>
       </c>
     </row>
   </sheetData>
@@ -30268,7 +30268,7 @@
         <v>269</v>
       </c>
       <c r="K8">
-        <v>74</v>
+        <v>75</v>
       </c>
     </row>
     <row r="9" spans="1:11">
@@ -30338,7 +30338,7 @@
         <v>362</v>
       </c>
       <c r="K10">
-        <v>92</v>
+        <v>95</v>
       </c>
     </row>
     <row r="11" spans="1:11">
@@ -30373,7 +30373,7 @@
         <v>850</v>
       </c>
       <c r="K11">
-        <v>211</v>
+        <v>215</v>
       </c>
     </row>
   </sheetData>
@@ -30679,7 +30679,7 @@
         <v>254</v>
       </c>
       <c r="K8">
-        <v>60</v>
+        <v>63</v>
       </c>
     </row>
     <row r="9" spans="1:11">
@@ -30749,7 +30749,7 @@
         <v>314</v>
       </c>
       <c r="K10">
-        <v>80</v>
+        <v>83</v>
       </c>
     </row>
     <row r="11" spans="1:11">
@@ -30784,7 +30784,7 @@
         <v>862</v>
       </c>
       <c r="K11">
-        <v>202</v>
+        <v>208</v>
       </c>
     </row>
   </sheetData>
@@ -31048,7 +31048,7 @@
         <v>132</v>
       </c>
       <c r="K8">
-        <v>42</v>
+        <v>44</v>
       </c>
     </row>
     <row r="9" spans="1:11">
@@ -31118,7 +31118,7 @@
         <v>553</v>
       </c>
       <c r="K10">
-        <v>130</v>
+        <v>131</v>
       </c>
     </row>
     <row r="11" spans="1:11">
@@ -31153,7 +31153,7 @@
         <v>739</v>
       </c>
       <c r="K11">
-        <v>189</v>
+        <v>192</v>
       </c>
     </row>
   </sheetData>
@@ -31284,7 +31284,7 @@
         <v>67</v>
       </c>
       <c r="K3">
-        <v>14</v>
+        <v>15</v>
       </c>
     </row>
     <row r="4" spans="1:11">
@@ -31389,7 +31389,7 @@
         <v>18</v>
       </c>
       <c r="K6">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="7" spans="1:11">
@@ -31561,7 +31561,7 @@
         <v>524</v>
       </c>
       <c r="K11">
-        <v>115</v>
+        <v>117</v>
       </c>
     </row>
   </sheetData>
@@ -31886,7 +31886,7 @@
         <v>612</v>
       </c>
       <c r="K10">
-        <v>176</v>
+        <v>183</v>
       </c>
     </row>
     <row r="11" spans="1:11">
@@ -31921,7 +31921,7 @@
         <v>670</v>
       </c>
       <c r="K11">
-        <v>193</v>
+        <v>200</v>
       </c>
     </row>
   </sheetData>
@@ -32672,7 +32672,7 @@
         <v>626</v>
       </c>
       <c r="K10">
-        <v>153</v>
+        <v>157</v>
       </c>
     </row>
     <row r="11" spans="1:11">
@@ -32707,7 +32707,7 @@
         <v>1144</v>
       </c>
       <c r="K11">
-        <v>286</v>
+        <v>290</v>
       </c>
     </row>
   </sheetData>
@@ -32838,7 +32838,7 @@
         <v>31</v>
       </c>
       <c r="K3">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="4" spans="1:11">
@@ -33030,7 +33030,7 @@
         <v>41</v>
       </c>
       <c r="K9">
-        <v>16</v>
+        <v>17</v>
       </c>
     </row>
     <row r="10" spans="1:11">
@@ -33065,7 +33065,7 @@
         <v>481</v>
       </c>
       <c r="K10">
-        <v>123</v>
+        <v>126</v>
       </c>
     </row>
     <row r="11" spans="1:11">
@@ -33100,7 +33100,7 @@
         <v>766</v>
       </c>
       <c r="K11">
-        <v>181</v>
+        <v>186</v>
       </c>
     </row>
   </sheetData>
@@ -33446,7 +33446,7 @@
         <v>752</v>
       </c>
       <c r="K10">
-        <v>172</v>
+        <v>176</v>
       </c>
     </row>
     <row r="11" spans="1:11">
@@ -33481,7 +33481,7 @@
         <v>1454</v>
       </c>
       <c r="K11">
-        <v>326</v>
+        <v>330</v>
       </c>
     </row>
   </sheetData>
@@ -34592,7 +34592,7 @@
         <v>256</v>
       </c>
       <c r="K10">
-        <v>64</v>
+        <v>66</v>
       </c>
     </row>
     <row r="11" spans="1:11">
@@ -34627,7 +34627,7 @@
         <v>356</v>
       </c>
       <c r="K11">
-        <v>100</v>
+        <v>102</v>
       </c>
     </row>
   </sheetData>
@@ -34924,7 +34924,7 @@
         <v>140</v>
       </c>
       <c r="J8">
-        <v>241</v>
+        <v>242</v>
       </c>
       <c r="K8">
         <v>122</v>
@@ -34962,7 +34962,7 @@
         <v>52</v>
       </c>
       <c r="K9">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="10" spans="1:11">
@@ -34997,7 +34997,7 @@
         <v>505</v>
       </c>
       <c r="K10">
-        <v>114</v>
+        <v>115</v>
       </c>
     </row>
     <row r="11" spans="1:11">
@@ -35029,10 +35029,10 @@
         <v>766</v>
       </c>
       <c r="J11">
-        <v>951</v>
+        <v>952</v>
       </c>
       <c r="K11">
-        <v>298</v>
+        <v>300</v>
       </c>
     </row>
   </sheetData>
@@ -35332,7 +35332,7 @@
         <v>364</v>
       </c>
       <c r="K8">
-        <v>66</v>
+        <v>68</v>
       </c>
     </row>
     <row r="9" spans="1:11">
@@ -35402,7 +35402,7 @@
         <v>1368</v>
       </c>
       <c r="K10">
-        <v>318</v>
+        <v>323</v>
       </c>
     </row>
     <row r="11" spans="1:11">
@@ -35437,7 +35437,7 @@
         <v>2262</v>
       </c>
       <c r="K11">
-        <v>511</v>
+        <v>518</v>
       </c>
     </row>
   </sheetData>
@@ -35756,7 +35756,7 @@
         <v>199</v>
       </c>
       <c r="K10">
-        <v>59</v>
+        <v>60</v>
       </c>
     </row>
     <row r="11" spans="1:11">
@@ -35791,7 +35791,7 @@
         <v>268</v>
       </c>
       <c r="K11">
-        <v>73</v>
+        <v>74</v>
       </c>
     </row>
   </sheetData>
@@ -36111,7 +36111,7 @@
         <v>70</v>
       </c>
       <c r="K9">
-        <v>16</v>
+        <v>17</v>
       </c>
     </row>
     <row r="10" spans="1:11">
@@ -36146,7 +36146,7 @@
         <v>156</v>
       </c>
       <c r="K10">
-        <v>31</v>
+        <v>32</v>
       </c>
     </row>
   </sheetData>
@@ -36326,7 +36326,7 @@
         <v>24</v>
       </c>
       <c r="K5">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="6" spans="1:11">
@@ -36477,7 +36477,7 @@
         <v>108</v>
       </c>
       <c r="K10">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="11" spans="1:11">
@@ -36512,7 +36512,7 @@
         <v>285</v>
       </c>
       <c r="K11">
-        <v>54</v>
+        <v>56</v>
       </c>
     </row>
   </sheetData>
@@ -37121,7 +37121,7 @@
         <v>235</v>
       </c>
       <c r="K8">
-        <v>42</v>
+        <v>44</v>
       </c>
     </row>
     <row r="9" spans="1:11">
@@ -37191,7 +37191,7 @@
         <v>799</v>
       </c>
       <c r="K10">
-        <v>248</v>
+        <v>250</v>
       </c>
     </row>
     <row r="11" spans="1:11">
@@ -37226,7 +37226,7 @@
         <v>1353</v>
       </c>
       <c r="K11">
-        <v>366</v>
+        <v>370</v>
       </c>
     </row>
   </sheetData>
@@ -37682,7 +37682,7 @@
         <v>29</v>
       </c>
       <c r="K2">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="3" spans="1:11">
@@ -37982,7 +37982,7 @@
         <v>457</v>
       </c>
       <c r="K11">
-        <v>90</v>
+        <v>91</v>
       </c>
     </row>
   </sheetData>
@@ -38659,7 +38659,7 @@
         <v>170</v>
       </c>
       <c r="K9">
-        <v>52</v>
+        <v>53</v>
       </c>
     </row>
     <row r="10" spans="1:11">
@@ -38694,7 +38694,7 @@
         <v>283</v>
       </c>
       <c r="K10">
-        <v>81</v>
+        <v>82</v>
       </c>
     </row>
   </sheetData>
@@ -39032,7 +39032,7 @@
         <v>47</v>
       </c>
       <c r="K9">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="10" spans="1:11">
@@ -39102,7 +39102,7 @@
         <v>541</v>
       </c>
       <c r="K11">
-        <v>111</v>
+        <v>112</v>
       </c>
     </row>
   </sheetData>
@@ -39230,7 +39230,7 @@
         <v>439</v>
       </c>
       <c r="J3">
-        <v>432</v>
+        <v>433</v>
       </c>
       <c r="K3">
         <v>116</v>
@@ -39303,7 +39303,7 @@
         <v>317</v>
       </c>
       <c r="K5">
-        <v>112</v>
+        <v>113</v>
       </c>
     </row>
     <row r="6" spans="1:11">
@@ -39408,7 +39408,7 @@
         <v>1312</v>
       </c>
       <c r="K8">
-        <v>181</v>
+        <v>183</v>
       </c>
     </row>
     <row r="9" spans="1:11">
@@ -39443,7 +39443,7 @@
         <v>341</v>
       </c>
       <c r="K9">
-        <v>82</v>
+        <v>83</v>
       </c>
     </row>
     <row r="10" spans="1:11">
@@ -39478,7 +39478,7 @@
         <v>1374</v>
       </c>
       <c r="K10">
-        <v>377</v>
+        <v>380</v>
       </c>
     </row>
     <row r="11" spans="1:11">
@@ -39510,10 +39510,10 @@
         <v>3862</v>
       </c>
       <c r="J11">
-        <v>4216</v>
+        <v>4217</v>
       </c>
       <c r="K11">
-        <v>1019</v>
+        <v>1026</v>
       </c>
     </row>
   </sheetData>
@@ -40596,7 +40596,7 @@
         <v>258</v>
       </c>
       <c r="K10">
-        <v>71</v>
+        <v>72</v>
       </c>
     </row>
     <row r="11" spans="1:11">
@@ -40631,7 +40631,7 @@
         <v>553</v>
       </c>
       <c r="K11">
-        <v>134</v>
+        <v>135</v>
       </c>
     </row>
   </sheetData>
@@ -40832,7 +40832,7 @@
         <v>59</v>
       </c>
       <c r="K5">
-        <v>20</v>
+        <v>21</v>
       </c>
     </row>
     <row r="6" spans="1:11">
@@ -40937,7 +40937,7 @@
         <v>253</v>
       </c>
       <c r="K8">
-        <v>40</v>
+        <v>41</v>
       </c>
     </row>
     <row r="9" spans="1:11">
@@ -40972,7 +40972,7 @@
         <v>166</v>
       </c>
       <c r="K9">
-        <v>49</v>
+        <v>50</v>
       </c>
     </row>
     <row r="10" spans="1:11">
@@ -41007,7 +41007,7 @@
         <v>429</v>
       </c>
       <c r="K10">
-        <v>110</v>
+        <v>112</v>
       </c>
     </row>
     <row r="11" spans="1:11">
@@ -41042,7 +41042,7 @@
         <v>1063</v>
       </c>
       <c r="K11">
-        <v>262</v>
+        <v>267</v>
       </c>
     </row>
   </sheetData>
@@ -41361,7 +41361,7 @@
         <v>228</v>
       </c>
       <c r="K10">
-        <v>72</v>
+        <v>73</v>
       </c>
     </row>
     <row r="11" spans="1:11">
@@ -41396,7 +41396,7 @@
         <v>313</v>
       </c>
       <c r="K11">
-        <v>85</v>
+        <v>86</v>
       </c>
     </row>
   </sheetData>
@@ -41561,7 +41561,7 @@
         <v>19</v>
       </c>
       <c r="K5">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="6" spans="1:11">
@@ -41689,7 +41689,7 @@
         <v>135</v>
       </c>
       <c r="K9">
-        <v>44</v>
+        <v>45</v>
       </c>
     </row>
     <row r="10" spans="1:11">
@@ -41724,7 +41724,7 @@
         <v>202</v>
       </c>
       <c r="K10">
-        <v>64</v>
+        <v>66</v>
       </c>
     </row>
   </sheetData>
@@ -41901,7 +41901,7 @@
         <v>39</v>
       </c>
       <c r="K5">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="6" spans="1:11">
@@ -42040,7 +42040,7 @@
         <v>151</v>
       </c>
       <c r="K10">
-        <v>32</v>
+        <v>33</v>
       </c>
     </row>
     <row r="11" spans="1:11">
@@ -42075,7 +42075,7 @@
         <v>256</v>
       </c>
       <c r="K11">
-        <v>56</v>
+        <v>58</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add data for 2025-03-17
</commit_message>
<xml_diff>
--- a/output/index-crime-full-year.xlsx
+++ b/output/index-crime-full-year.xlsx
@@ -909,7 +909,7 @@
         <v>7900</v>
       </c>
       <c r="L2">
-        <v>1146</v>
+        <v>1158</v>
       </c>
     </row>
     <row r="3" spans="1:12">
@@ -947,7 +947,7 @@
         <v>8184</v>
       </c>
       <c r="L3">
-        <v>1151</v>
+        <v>1166</v>
       </c>
     </row>
     <row r="4" spans="1:12">
@@ -1023,7 +1023,7 @@
         <v>7640</v>
       </c>
       <c r="L5">
-        <v>1159</v>
+        <v>1175</v>
       </c>
     </row>
     <row r="6" spans="1:12">
@@ -1061,7 +1061,7 @@
         <v>1746</v>
       </c>
       <c r="L6">
-        <v>320</v>
+        <v>324</v>
       </c>
     </row>
     <row r="7" spans="1:12">
@@ -1099,7 +1099,7 @@
         <v>586</v>
       </c>
       <c r="L7">
-        <v>75</v>
+        <v>76</v>
       </c>
     </row>
     <row r="8" spans="1:12">
@@ -1137,7 +1137,7 @@
         <v>21675</v>
       </c>
       <c r="L8">
-        <v>3077</v>
+        <v>3129</v>
       </c>
     </row>
     <row r="9" spans="1:12">
@@ -1175,7 +1175,7 @@
         <v>9122</v>
       </c>
       <c r="L9">
-        <v>1170</v>
+        <v>1183</v>
       </c>
     </row>
     <row r="10" spans="1:12">
@@ -1210,10 +1210,10 @@
         <v>57476</v>
       </c>
       <c r="K10">
-        <v>61138</v>
+        <v>61137</v>
       </c>
       <c r="L10">
-        <v>10268</v>
+        <v>10411</v>
       </c>
     </row>
     <row r="11" spans="1:12">
@@ -1248,10 +1248,10 @@
         <v>124053</v>
       </c>
       <c r="K11">
-        <v>118473</v>
+        <v>118472</v>
       </c>
       <c r="L11">
-        <v>18437</v>
+        <v>18693</v>
       </c>
     </row>
   </sheetData>
@@ -1354,7 +1354,7 @@
         <v>191</v>
       </c>
       <c r="L2">
-        <v>24</v>
+        <v>25</v>
       </c>
     </row>
     <row r="3" spans="1:12">
@@ -1392,7 +1392,7 @@
         <v>195</v>
       </c>
       <c r="L3">
-        <v>20</v>
+        <v>21</v>
       </c>
     </row>
     <row r="4" spans="1:12">
@@ -1620,7 +1620,7 @@
         <v>251</v>
       </c>
       <c r="L9">
-        <v>19</v>
+        <v>20</v>
       </c>
     </row>
     <row r="10" spans="1:12">
@@ -1696,7 +1696,7 @@
         <v>1853</v>
       </c>
       <c r="L11">
-        <v>237</v>
+        <v>240</v>
       </c>
     </row>
   </sheetData>
@@ -2236,7 +2236,7 @@
         <v>59</v>
       </c>
       <c r="L5">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="6" spans="1:12">
@@ -2332,7 +2332,7 @@
         <v>68</v>
       </c>
       <c r="L8">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="9" spans="1:12">
@@ -2446,7 +2446,7 @@
         <v>540</v>
       </c>
       <c r="L11">
-        <v>94</v>
+        <v>96</v>
       </c>
     </row>
   </sheetData>
@@ -2774,7 +2774,7 @@
         <v>386</v>
       </c>
       <c r="L8">
-        <v>50</v>
+        <v>51</v>
       </c>
     </row>
     <row r="9" spans="1:12">
@@ -2850,7 +2850,7 @@
         <v>1475</v>
       </c>
       <c r="L10">
-        <v>210</v>
+        <v>213</v>
       </c>
     </row>
     <row r="11" spans="1:12">
@@ -2888,7 +2888,7 @@
         <v>2349</v>
       </c>
       <c r="L11">
-        <v>325</v>
+        <v>329</v>
       </c>
     </row>
   </sheetData>
@@ -3029,7 +3029,7 @@
         <v>546</v>
       </c>
       <c r="L3">
-        <v>71</v>
+        <v>72</v>
       </c>
     </row>
     <row r="4" spans="1:12">
@@ -3219,7 +3219,7 @@
         <v>932</v>
       </c>
       <c r="L8">
-        <v>161</v>
+        <v>162</v>
       </c>
     </row>
     <row r="9" spans="1:12">
@@ -3333,7 +3333,7 @@
         <v>4988</v>
       </c>
       <c r="L11">
-        <v>882</v>
+        <v>884</v>
       </c>
     </row>
   </sheetData>
@@ -4143,7 +4143,7 @@
         <v>386</v>
       </c>
       <c r="L10">
-        <v>77</v>
+        <v>79</v>
       </c>
     </row>
     <row r="11" spans="1:12">
@@ -4181,7 +4181,7 @@
         <v>785</v>
       </c>
       <c r="L11">
-        <v>122</v>
+        <v>124</v>
       </c>
     </row>
   </sheetData>
@@ -4382,6 +4382,9 @@
       <c r="K5">
         <v>13</v>
       </c>
+      <c r="L5">
+        <v>1</v>
+      </c>
     </row>
     <row r="6" spans="1:12">
       <c r="A6" s="1" t="s">
@@ -4558,7 +4561,7 @@
         <v>163</v>
       </c>
       <c r="L10">
-        <v>30</v>
+        <v>31</v>
       </c>
     </row>
     <row r="11" spans="1:12">
@@ -4596,7 +4599,7 @@
         <v>378</v>
       </c>
       <c r="L11">
-        <v>61</v>
+        <v>63</v>
       </c>
     </row>
   </sheetData>
@@ -4737,7 +4740,7 @@
         <v>203</v>
       </c>
       <c r="L3">
-        <v>39</v>
+        <v>40</v>
       </c>
     </row>
     <row r="4" spans="1:12">
@@ -4927,7 +4930,7 @@
         <v>330</v>
       </c>
       <c r="L8">
-        <v>69</v>
+        <v>70</v>
       </c>
     </row>
     <row r="9" spans="1:12">
@@ -4965,7 +4968,7 @@
         <v>139</v>
       </c>
       <c r="L9">
-        <v>19</v>
+        <v>20</v>
       </c>
     </row>
     <row r="10" spans="1:12">
@@ -5003,7 +5006,7 @@
         <v>579</v>
       </c>
       <c r="L10">
-        <v>82</v>
+        <v>83</v>
       </c>
     </row>
     <row r="11" spans="1:12">
@@ -5041,7 +5044,7 @@
         <v>1630</v>
       </c>
       <c r="L11">
-        <v>269</v>
+        <v>273</v>
       </c>
     </row>
   </sheetData>
@@ -5182,7 +5185,7 @@
         <v>409</v>
       </c>
       <c r="L3">
-        <v>61</v>
+        <v>62</v>
       </c>
     </row>
     <row r="4" spans="1:12">
@@ -5369,7 +5372,7 @@
         <v>542</v>
       </c>
       <c r="L8">
-        <v>91</v>
+        <v>93</v>
       </c>
     </row>
     <row r="9" spans="1:12">
@@ -5407,7 +5410,7 @@
         <v>364</v>
       </c>
       <c r="L9">
-        <v>59</v>
+        <v>60</v>
       </c>
     </row>
     <row r="10" spans="1:12">
@@ -5445,7 +5448,7 @@
         <v>933</v>
       </c>
       <c r="L10">
-        <v>137</v>
+        <v>138</v>
       </c>
     </row>
     <row r="11" spans="1:12">
@@ -5483,7 +5486,7 @@
         <v>2799</v>
       </c>
       <c r="L11">
-        <v>411</v>
+        <v>416</v>
       </c>
     </row>
   </sheetData>
@@ -5586,7 +5589,7 @@
         <v>219</v>
       </c>
       <c r="L2">
-        <v>34</v>
+        <v>36</v>
       </c>
     </row>
     <row r="3" spans="1:12">
@@ -5700,7 +5703,7 @@
         <v>156</v>
       </c>
       <c r="L5">
-        <v>24</v>
+        <v>25</v>
       </c>
     </row>
     <row r="6" spans="1:12">
@@ -5814,7 +5817,7 @@
         <v>553</v>
       </c>
       <c r="L8">
-        <v>102</v>
+        <v>105</v>
       </c>
     </row>
     <row r="9" spans="1:12">
@@ -5928,7 +5931,7 @@
         <v>2269</v>
       </c>
       <c r="L11">
-        <v>404</v>
+        <v>410</v>
       </c>
     </row>
   </sheetData>
@@ -6031,7 +6034,7 @@
         <v>1107</v>
       </c>
       <c r="L2">
-        <v>179</v>
+        <v>186</v>
       </c>
     </row>
     <row r="3" spans="1:12">
@@ -6107,7 +6110,7 @@
         <v>616</v>
       </c>
       <c r="L4">
-        <v>132</v>
+        <v>134</v>
       </c>
     </row>
     <row r="5" spans="1:12">
@@ -6221,7 +6224,7 @@
         <v>2521</v>
       </c>
       <c r="L7">
-        <v>442</v>
+        <v>450</v>
       </c>
     </row>
     <row r="8" spans="1:12">
@@ -6259,7 +6262,7 @@
         <v>4988</v>
       </c>
       <c r="L8">
-        <v>882</v>
+        <v>884</v>
       </c>
     </row>
     <row r="9" spans="1:12">
@@ -6297,7 +6300,7 @@
         <v>485</v>
       </c>
       <c r="L9">
-        <v>72</v>
+        <v>75</v>
       </c>
     </row>
     <row r="10" spans="1:12">
@@ -6335,7 +6338,7 @@
         <v>1287</v>
       </c>
       <c r="L10">
-        <v>196</v>
+        <v>199</v>
       </c>
     </row>
     <row r="11" spans="1:12">
@@ -6373,7 +6376,7 @@
         <v>2123</v>
       </c>
       <c r="L11">
-        <v>323</v>
+        <v>328</v>
       </c>
     </row>
     <row r="12" spans="1:12">
@@ -6411,7 +6414,7 @@
         <v>559</v>
       </c>
       <c r="L12">
-        <v>69</v>
+        <v>71</v>
       </c>
     </row>
     <row r="13" spans="1:12">
@@ -6487,7 +6490,7 @@
         <v>723</v>
       </c>
       <c r="L14">
-        <v>126</v>
+        <v>128</v>
       </c>
     </row>
     <row r="15" spans="1:12">
@@ -6601,7 +6604,7 @@
         <v>140</v>
       </c>
       <c r="L17">
-        <v>17</v>
+        <v>18</v>
       </c>
     </row>
     <row r="18" spans="1:12">
@@ -6639,7 +6642,7 @@
         <v>751</v>
       </c>
       <c r="L18">
-        <v>125</v>
+        <v>126</v>
       </c>
     </row>
     <row r="19" spans="1:12">
@@ -6677,7 +6680,7 @@
         <v>2529</v>
       </c>
       <c r="L19">
-        <v>479</v>
+        <v>483</v>
       </c>
     </row>
     <row r="20" spans="1:12">
@@ -6715,7 +6718,7 @@
         <v>1977</v>
       </c>
       <c r="L20">
-        <v>347</v>
+        <v>355</v>
       </c>
     </row>
     <row r="21" spans="1:12">
@@ -6829,7 +6832,7 @@
         <v>1331</v>
       </c>
       <c r="L23">
-        <v>206</v>
+        <v>208</v>
       </c>
     </row>
     <row r="24" spans="1:12">
@@ -6867,7 +6870,7 @@
         <v>675</v>
       </c>
       <c r="L24">
-        <v>94</v>
+        <v>96</v>
       </c>
     </row>
     <row r="25" spans="1:12">
@@ -6905,7 +6908,7 @@
         <v>556</v>
       </c>
       <c r="L25">
-        <v>110</v>
+        <v>111</v>
       </c>
     </row>
     <row r="26" spans="1:12">
@@ -6943,7 +6946,7 @@
         <v>281</v>
       </c>
       <c r="L26">
-        <v>44</v>
+        <v>47</v>
       </c>
     </row>
     <row r="27" spans="1:12">
@@ -6981,7 +6984,7 @@
         <v>1555</v>
       </c>
       <c r="L27">
-        <v>276</v>
+        <v>279</v>
       </c>
     </row>
     <row r="28" spans="1:12">
@@ -7054,10 +7057,10 @@
         <v>4175</v>
       </c>
       <c r="K29">
-        <v>3878</v>
+        <v>3879</v>
       </c>
       <c r="L29">
-        <v>549</v>
+        <v>557</v>
       </c>
     </row>
     <row r="30" spans="1:12">
@@ -7130,10 +7133,10 @@
         <v>1028</v>
       </c>
       <c r="K31">
-        <v>1043</v>
+        <v>1044</v>
       </c>
       <c r="L31">
-        <v>184</v>
+        <v>189</v>
       </c>
     </row>
     <row r="32" spans="1:12">
@@ -7209,7 +7212,7 @@
         <v>2799</v>
       </c>
       <c r="L33">
-        <v>411</v>
+        <v>416</v>
       </c>
     </row>
     <row r="34" spans="1:12">
@@ -7247,7 +7250,7 @@
         <v>977</v>
       </c>
       <c r="L34">
-        <v>118</v>
+        <v>119</v>
       </c>
     </row>
     <row r="35" spans="1:12">
@@ -7323,7 +7326,7 @@
         <v>1715</v>
       </c>
       <c r="L36">
-        <v>254</v>
+        <v>256</v>
       </c>
     </row>
     <row r="37" spans="1:12">
@@ -7361,7 +7364,7 @@
         <v>2724</v>
       </c>
       <c r="L37">
-        <v>370</v>
+        <v>379</v>
       </c>
     </row>
     <row r="38" spans="1:12">
@@ -7551,7 +7554,7 @@
         <v>3262</v>
       </c>
       <c r="L42">
-        <v>428</v>
+        <v>432</v>
       </c>
     </row>
     <row r="43" spans="1:12">
@@ -7589,7 +7592,7 @@
         <v>1331</v>
       </c>
       <c r="L43">
-        <v>280</v>
+        <v>281</v>
       </c>
     </row>
     <row r="44" spans="1:12">
@@ -7627,7 +7630,7 @@
         <v>1296</v>
       </c>
       <c r="L44">
-        <v>181</v>
+        <v>184</v>
       </c>
     </row>
     <row r="45" spans="1:12">
@@ -7741,7 +7744,7 @@
         <v>1049</v>
       </c>
       <c r="L47">
-        <v>144</v>
+        <v>145</v>
       </c>
     </row>
     <row r="48" spans="1:12">
@@ -7779,7 +7782,7 @@
         <v>3221</v>
       </c>
       <c r="L48">
-        <v>489</v>
+        <v>493</v>
       </c>
     </row>
     <row r="49" spans="1:12">
@@ -7817,7 +7820,7 @@
         <v>2193</v>
       </c>
       <c r="L49">
-        <v>305</v>
+        <v>307</v>
       </c>
     </row>
     <row r="50" spans="1:12">
@@ -7855,7 +7858,7 @@
         <v>1042</v>
       </c>
       <c r="L50">
-        <v>179</v>
+        <v>181</v>
       </c>
     </row>
     <row r="51" spans="1:12">
@@ -7893,7 +7896,7 @@
         <v>1494</v>
       </c>
       <c r="L51">
-        <v>249</v>
+        <v>254</v>
       </c>
     </row>
     <row r="52" spans="1:12">
@@ -7931,7 +7934,7 @@
         <v>1853</v>
       </c>
       <c r="L52">
-        <v>237</v>
+        <v>240</v>
       </c>
     </row>
     <row r="53" spans="1:12">
@@ -7969,7 +7972,7 @@
         <v>2349</v>
       </c>
       <c r="L53">
-        <v>325</v>
+        <v>329</v>
       </c>
     </row>
     <row r="54" spans="1:12">
@@ -8007,7 +8010,7 @@
         <v>4187</v>
       </c>
       <c r="L54">
-        <v>654</v>
+        <v>668</v>
       </c>
     </row>
     <row r="55" spans="1:12">
@@ -8045,7 +8048,7 @@
         <v>1293</v>
       </c>
       <c r="L55">
-        <v>175</v>
+        <v>177</v>
       </c>
     </row>
     <row r="56" spans="1:12">
@@ -8083,7 +8086,7 @@
         <v>718</v>
       </c>
       <c r="L56">
-        <v>87</v>
+        <v>90</v>
       </c>
     </row>
     <row r="57" spans="1:12">
@@ -8121,7 +8124,7 @@
         <v>575</v>
       </c>
       <c r="L57">
-        <v>98</v>
+        <v>100</v>
       </c>
     </row>
     <row r="58" spans="1:12">
@@ -8235,7 +8238,7 @@
         <v>785</v>
       </c>
       <c r="L60">
-        <v>122</v>
+        <v>124</v>
       </c>
     </row>
     <row r="61" spans="1:12">
@@ -8346,10 +8349,10 @@
         <v>970</v>
       </c>
       <c r="K63">
-        <v>440</v>
+        <v>435</v>
       </c>
       <c r="L63">
-        <v>103</v>
+        <v>124</v>
       </c>
     </row>
     <row r="64" spans="1:12">
@@ -8387,7 +8390,7 @@
         <v>1134</v>
       </c>
       <c r="L64">
-        <v>177</v>
+        <v>178</v>
       </c>
     </row>
     <row r="65" spans="1:12">
@@ -8425,7 +8428,7 @@
         <v>1690</v>
       </c>
       <c r="L65">
-        <v>251</v>
+        <v>254</v>
       </c>
     </row>
     <row r="66" spans="1:12">
@@ -8463,7 +8466,7 @@
         <v>723</v>
       </c>
       <c r="L66">
-        <v>90</v>
+        <v>91</v>
       </c>
     </row>
     <row r="67" spans="1:12">
@@ -8501,7 +8504,7 @@
         <v>2439</v>
       </c>
       <c r="L67">
-        <v>350</v>
+        <v>352</v>
       </c>
     </row>
     <row r="68" spans="1:12">
@@ -8539,7 +8542,7 @@
         <v>498</v>
       </c>
       <c r="L68">
-        <v>107</v>
+        <v>108</v>
       </c>
     </row>
     <row r="69" spans="1:12">
@@ -8577,7 +8580,7 @@
         <v>540</v>
       </c>
       <c r="L69">
-        <v>94</v>
+        <v>96</v>
       </c>
     </row>
     <row r="70" spans="1:12">
@@ -8615,7 +8618,7 @@
         <v>682</v>
       </c>
       <c r="L70">
-        <v>128</v>
+        <v>132</v>
       </c>
     </row>
     <row r="71" spans="1:12">
@@ -8653,7 +8656,7 @@
         <v>378</v>
       </c>
       <c r="L71">
-        <v>61</v>
+        <v>63</v>
       </c>
     </row>
     <row r="72" spans="1:12">
@@ -8691,7 +8694,7 @@
         <v>756</v>
       </c>
       <c r="L72">
-        <v>125</v>
+        <v>127</v>
       </c>
     </row>
     <row r="73" spans="1:12">
@@ -8729,7 +8732,7 @@
         <v>1506</v>
       </c>
       <c r="L73">
-        <v>233</v>
+        <v>235</v>
       </c>
     </row>
     <row r="74" spans="1:12">
@@ -8840,10 +8843,10 @@
         <v>3184</v>
       </c>
       <c r="K76">
-        <v>3063</v>
+        <v>3064</v>
       </c>
       <c r="L76">
-        <v>473</v>
+        <v>481</v>
       </c>
     </row>
     <row r="77" spans="1:12">
@@ -8881,7 +8884,7 @@
         <v>447</v>
       </c>
       <c r="L77">
-        <v>85</v>
+        <v>86</v>
       </c>
     </row>
     <row r="78" spans="1:12">
@@ -8919,7 +8922,7 @@
         <v>1948</v>
       </c>
       <c r="L78">
-        <v>318</v>
+        <v>321</v>
       </c>
     </row>
     <row r="79" spans="1:12">
@@ -8957,7 +8960,7 @@
         <v>2269</v>
       </c>
       <c r="L79">
-        <v>404</v>
+        <v>410</v>
       </c>
     </row>
     <row r="80" spans="1:12">
@@ -9071,7 +9074,7 @@
         <v>285</v>
       </c>
       <c r="L82">
-        <v>50</v>
+        <v>51</v>
       </c>
     </row>
     <row r="83" spans="1:12">
@@ -9109,7 +9112,7 @@
         <v>1630</v>
       </c>
       <c r="L83">
-        <v>269</v>
+        <v>273</v>
       </c>
     </row>
     <row r="84" spans="1:12">
@@ -9147,7 +9150,7 @@
         <v>879</v>
       </c>
       <c r="L84">
-        <v>149</v>
+        <v>150</v>
       </c>
     </row>
     <row r="85" spans="1:12">
@@ -9185,7 +9188,7 @@
         <v>3845</v>
       </c>
       <c r="L85">
-        <v>602</v>
+        <v>609</v>
       </c>
     </row>
     <row r="86" spans="1:12">
@@ -9223,7 +9226,7 @@
         <v>1011</v>
       </c>
       <c r="L86">
-        <v>140</v>
+        <v>143</v>
       </c>
     </row>
     <row r="87" spans="1:12">
@@ -9261,7 +9264,7 @@
         <v>492</v>
       </c>
       <c r="L87">
-        <v>72</v>
+        <v>73</v>
       </c>
     </row>
     <row r="88" spans="1:12">
@@ -9299,7 +9302,7 @@
         <v>1020</v>
       </c>
       <c r="L88">
-        <v>154</v>
+        <v>156</v>
       </c>
     </row>
     <row r="89" spans="1:12">
@@ -9337,7 +9340,7 @@
         <v>2321</v>
       </c>
       <c r="L89">
-        <v>331</v>
+        <v>333</v>
       </c>
     </row>
     <row r="90" spans="1:12">
@@ -9375,7 +9378,7 @@
         <v>1148</v>
       </c>
       <c r="L90">
-        <v>157</v>
+        <v>164</v>
       </c>
     </row>
     <row r="91" spans="1:12">
@@ -9413,7 +9416,7 @@
         <v>1048</v>
       </c>
       <c r="L91">
-        <v>154</v>
+        <v>158</v>
       </c>
     </row>
     <row r="92" spans="1:12">
@@ -9489,7 +9492,7 @@
         <v>934</v>
       </c>
       <c r="L93">
-        <v>163</v>
+        <v>168</v>
       </c>
     </row>
     <row r="94" spans="1:12">
@@ -9527,7 +9530,7 @@
         <v>3008</v>
       </c>
       <c r="L94">
-        <v>401</v>
+        <v>404</v>
       </c>
     </row>
     <row r="95" spans="1:12">
@@ -9562,10 +9565,10 @@
         <v>1484</v>
       </c>
       <c r="K95">
-        <v>1447</v>
+        <v>1448</v>
       </c>
       <c r="L95">
-        <v>216</v>
+        <v>222</v>
       </c>
     </row>
     <row r="96" spans="1:12">
@@ -9603,7 +9606,7 @@
         <v>1638</v>
       </c>
       <c r="L96">
-        <v>239</v>
+        <v>241</v>
       </c>
     </row>
     <row r="97" spans="1:12">
@@ -9641,7 +9644,7 @@
         <v>1819</v>
       </c>
       <c r="L97">
-        <v>323</v>
+        <v>325</v>
       </c>
     </row>
     <row r="98" spans="1:12">
@@ -9679,7 +9682,7 @@
         <v>1500</v>
       </c>
       <c r="L98">
-        <v>230</v>
+        <v>235</v>
       </c>
     </row>
     <row r="99" spans="1:12">
@@ -9755,7 +9758,7 @@
         <v>347</v>
       </c>
       <c r="L100">
-        <v>49</v>
+        <v>50</v>
       </c>
     </row>
     <row r="101" spans="1:12">
@@ -9790,10 +9793,10 @@
         <v>124053</v>
       </c>
       <c r="K101">
-        <v>118473</v>
+        <v>118472</v>
       </c>
       <c r="L101">
-        <v>18437</v>
+        <v>18693</v>
       </c>
     </row>
   </sheetData>
@@ -11041,7 +11044,7 @@
         <v>253</v>
       </c>
       <c r="L8">
-        <v>39</v>
+        <v>40</v>
       </c>
     </row>
     <row r="9" spans="1:12">
@@ -11155,7 +11158,7 @@
         <v>1134</v>
       </c>
       <c r="L11">
-        <v>177</v>
+        <v>178</v>
       </c>
     </row>
   </sheetData>
@@ -11372,7 +11375,7 @@
         <v>107</v>
       </c>
       <c r="L5">
-        <v>15</v>
+        <v>16</v>
       </c>
     </row>
     <row r="6" spans="1:12">
@@ -11486,7 +11489,7 @@
         <v>320</v>
       </c>
       <c r="L8">
-        <v>48</v>
+        <v>50</v>
       </c>
     </row>
     <row r="9" spans="1:12">
@@ -11524,7 +11527,7 @@
         <v>109</v>
       </c>
       <c r="L9">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="10" spans="1:12">
@@ -11559,10 +11562,10 @@
         <v>491</v>
       </c>
       <c r="K10">
-        <v>545</v>
+        <v>546</v>
       </c>
       <c r="L10">
-        <v>93</v>
+        <v>95</v>
       </c>
     </row>
     <row r="11" spans="1:12">
@@ -11597,10 +11600,10 @@
         <v>1484</v>
       </c>
       <c r="K11">
-        <v>1447</v>
+        <v>1448</v>
       </c>
       <c r="L11">
-        <v>216</v>
+        <v>222</v>
       </c>
     </row>
   </sheetData>
@@ -11703,7 +11706,7 @@
         <v>259</v>
       </c>
       <c r="L2">
-        <v>40</v>
+        <v>41</v>
       </c>
     </row>
     <row r="3" spans="1:12">
@@ -11741,7 +11744,7 @@
         <v>304</v>
       </c>
       <c r="L3">
-        <v>34</v>
+        <v>35</v>
       </c>
     </row>
     <row r="4" spans="1:12">
@@ -11931,7 +11934,7 @@
         <v>579</v>
       </c>
       <c r="L8">
-        <v>87</v>
+        <v>90</v>
       </c>
     </row>
     <row r="9" spans="1:12">
@@ -11969,7 +11972,7 @@
         <v>273</v>
       </c>
       <c r="L9">
-        <v>37</v>
+        <v>38</v>
       </c>
     </row>
     <row r="10" spans="1:12">
@@ -12007,7 +12010,7 @@
         <v>978</v>
       </c>
       <c r="L10">
-        <v>131</v>
+        <v>134</v>
       </c>
     </row>
     <row r="11" spans="1:12">
@@ -12045,7 +12048,7 @@
         <v>2724</v>
       </c>
       <c r="L11">
-        <v>370</v>
+        <v>379</v>
       </c>
     </row>
   </sheetData>
@@ -12376,7 +12379,7 @@
         <v>272</v>
       </c>
       <c r="L8">
-        <v>40</v>
+        <v>41</v>
       </c>
     </row>
     <row r="9" spans="1:12">
@@ -12414,7 +12417,7 @@
         <v>236</v>
       </c>
       <c r="L9">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="10" spans="1:12">
@@ -12452,7 +12455,7 @@
         <v>639</v>
       </c>
       <c r="L10">
-        <v>113</v>
+        <v>114</v>
       </c>
     </row>
     <row r="11" spans="1:12">
@@ -12490,7 +12493,7 @@
         <v>1690</v>
       </c>
       <c r="L11">
-        <v>251</v>
+        <v>254</v>
       </c>
     </row>
   </sheetData>
@@ -12882,7 +12885,7 @@
         <v>961</v>
       </c>
       <c r="L10">
-        <v>182</v>
+        <v>185</v>
       </c>
     </row>
     <row r="11" spans="1:12">
@@ -12920,7 +12923,7 @@
         <v>1555</v>
       </c>
       <c r="L11">
-        <v>276</v>
+        <v>279</v>
       </c>
     </row>
   </sheetData>
@@ -14044,7 +14047,7 @@
         <v>16</v>
       </c>
       <c r="K6">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="L6">
         <v>3</v>
@@ -14123,7 +14126,7 @@
         <v>214</v>
       </c>
       <c r="L8">
-        <v>43</v>
+        <v>45</v>
       </c>
     </row>
     <row r="9" spans="1:12">
@@ -14199,7 +14202,7 @@
         <v>442</v>
       </c>
       <c r="L10">
-        <v>87</v>
+        <v>90</v>
       </c>
     </row>
     <row r="11" spans="1:12">
@@ -14234,10 +14237,10 @@
         <v>1028</v>
       </c>
       <c r="K11">
-        <v>1043</v>
+        <v>1044</v>
       </c>
       <c r="L11">
-        <v>184</v>
+        <v>189</v>
       </c>
     </row>
   </sheetData>
@@ -14629,7 +14632,7 @@
         <v>370</v>
       </c>
       <c r="L10">
-        <v>73</v>
+        <v>75</v>
       </c>
     </row>
     <row r="11" spans="1:12">
@@ -14667,7 +14670,7 @@
         <v>723</v>
       </c>
       <c r="L11">
-        <v>126</v>
+        <v>128</v>
       </c>
     </row>
   </sheetData>
@@ -15074,7 +15077,7 @@
         <v>821</v>
       </c>
       <c r="L10">
-        <v>130</v>
+        <v>132</v>
       </c>
     </row>
     <row r="11" spans="1:12">
@@ -15112,7 +15115,7 @@
         <v>2439</v>
       </c>
       <c r="L11">
-        <v>350</v>
+        <v>352</v>
       </c>
     </row>
   </sheetData>
@@ -15478,7 +15481,7 @@
         <v>48</v>
       </c>
       <c r="L9">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="10" spans="1:12">
@@ -15554,7 +15557,7 @@
         <v>879</v>
       </c>
       <c r="L11">
-        <v>149</v>
+        <v>150</v>
       </c>
     </row>
   </sheetData>
@@ -15794,7 +15797,7 @@
         <v>30</v>
       </c>
       <c r="L6">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="7" spans="1:12">
@@ -15943,7 +15946,7 @@
         <v>2127</v>
       </c>
       <c r="L10">
-        <v>272</v>
+        <v>274</v>
       </c>
     </row>
     <row r="11" spans="1:12">
@@ -15981,7 +15984,7 @@
         <v>3008</v>
       </c>
       <c r="L11">
-        <v>401</v>
+        <v>404</v>
       </c>
     </row>
   </sheetData>
@@ -16382,10 +16385,10 @@
         <v>2307</v>
       </c>
       <c r="K10">
-        <v>2257</v>
+        <v>2258</v>
       </c>
       <c r="L10">
-        <v>392</v>
+        <v>400</v>
       </c>
     </row>
     <row r="11" spans="1:12">
@@ -16420,10 +16423,10 @@
         <v>3184</v>
       </c>
       <c r="K11">
-        <v>3063</v>
+        <v>3064</v>
       </c>
       <c r="L11">
-        <v>473</v>
+        <v>481</v>
       </c>
     </row>
   </sheetData>
@@ -16806,7 +16809,7 @@
         <v>309</v>
       </c>
       <c r="L10">
-        <v>43</v>
+        <v>44</v>
       </c>
     </row>
     <row r="11" spans="1:12">
@@ -16844,7 +16847,7 @@
         <v>492</v>
       </c>
       <c r="L11">
-        <v>72</v>
+        <v>73</v>
       </c>
     </row>
   </sheetData>
@@ -17242,7 +17245,7 @@
         <v>192</v>
       </c>
       <c r="L10">
-        <v>51</v>
+        <v>52</v>
       </c>
     </row>
     <row r="11" spans="1:12">
@@ -17280,7 +17283,7 @@
         <v>556</v>
       </c>
       <c r="L11">
-        <v>110</v>
+        <v>111</v>
       </c>
     </row>
   </sheetData>
@@ -17627,7 +17630,7 @@
         <v>230</v>
       </c>
       <c r="L10">
-        <v>37</v>
+        <v>38</v>
       </c>
     </row>
     <row r="11" spans="1:12">
@@ -17665,7 +17668,7 @@
         <v>347</v>
       </c>
       <c r="L11">
-        <v>49</v>
+        <v>50</v>
       </c>
     </row>
   </sheetData>
@@ -18378,7 +18381,7 @@
         <v>226</v>
       </c>
       <c r="L8">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="9" spans="1:12">
@@ -18454,7 +18457,7 @@
         <v>1654</v>
       </c>
       <c r="L10">
-        <v>227</v>
+        <v>228</v>
       </c>
     </row>
     <row r="11" spans="1:12">
@@ -18492,7 +18495,7 @@
         <v>2193</v>
       </c>
       <c r="L11">
-        <v>305</v>
+        <v>307</v>
       </c>
     </row>
   </sheetData>
@@ -18890,7 +18893,7 @@
         <v>996</v>
       </c>
       <c r="L10">
-        <v>199</v>
+        <v>201</v>
       </c>
     </row>
     <row r="11" spans="1:12">
@@ -18928,7 +18931,7 @@
         <v>1819</v>
       </c>
       <c r="L11">
-        <v>323</v>
+        <v>325</v>
       </c>
     </row>
   </sheetData>
@@ -19291,7 +19294,7 @@
         <v>119</v>
       </c>
       <c r="L9">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="10" spans="1:12">
@@ -19329,7 +19332,7 @@
         <v>831</v>
       </c>
       <c r="L10">
-        <v>135</v>
+        <v>136</v>
       </c>
     </row>
     <row r="11" spans="1:12">
@@ -19367,7 +19370,7 @@
         <v>1638</v>
       </c>
       <c r="L11">
-        <v>239</v>
+        <v>241</v>
       </c>
     </row>
   </sheetData>
@@ -19470,7 +19473,7 @@
         <v>87</v>
       </c>
       <c r="L2">
-        <v>17</v>
+        <v>18</v>
       </c>
     </row>
     <row r="3" spans="1:12">
@@ -19774,7 +19777,7 @@
         <v>647</v>
       </c>
       <c r="L10">
-        <v>94</v>
+        <v>95</v>
       </c>
     </row>
     <row r="11" spans="1:12">
@@ -19812,7 +19815,7 @@
         <v>1293</v>
       </c>
       <c r="L11">
-        <v>175</v>
+        <v>177</v>
       </c>
     </row>
   </sheetData>
@@ -20067,7 +20070,7 @@
         <v>40</v>
       </c>
       <c r="L6">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="7" spans="1:12">
@@ -20137,7 +20140,7 @@
         <v>456</v>
       </c>
       <c r="L8">
-        <v>55</v>
+        <v>56</v>
       </c>
     </row>
     <row r="9" spans="1:12">
@@ -20175,7 +20178,7 @@
         <v>282</v>
       </c>
       <c r="L9">
-        <v>41</v>
+        <v>42</v>
       </c>
     </row>
     <row r="10" spans="1:12">
@@ -20213,7 +20216,7 @@
         <v>3093</v>
       </c>
       <c r="L10">
-        <v>495</v>
+        <v>506</v>
       </c>
     </row>
     <row r="11" spans="1:12">
@@ -20251,7 +20254,7 @@
         <v>4187</v>
       </c>
       <c r="L11">
-        <v>654</v>
+        <v>668</v>
       </c>
     </row>
   </sheetData>
@@ -20579,7 +20582,7 @@
         <v>257</v>
       </c>
       <c r="L8">
-        <v>45</v>
+        <v>46</v>
       </c>
     </row>
     <row r="9" spans="1:12">
@@ -20655,7 +20658,7 @@
         <v>885</v>
       </c>
       <c r="L10">
-        <v>147</v>
+        <v>148</v>
       </c>
     </row>
     <row r="11" spans="1:12">
@@ -20693,7 +20696,7 @@
         <v>1506</v>
       </c>
       <c r="L11">
-        <v>233</v>
+        <v>235</v>
       </c>
     </row>
   </sheetData>
@@ -20834,7 +20837,7 @@
         <v>534</v>
       </c>
       <c r="L3">
-        <v>60</v>
+        <v>63</v>
       </c>
     </row>
     <row r="4" spans="1:12">
@@ -21024,7 +21027,7 @@
         <v>832</v>
       </c>
       <c r="L8">
-        <v>124</v>
+        <v>126</v>
       </c>
     </row>
     <row r="9" spans="1:12">
@@ -21059,10 +21062,10 @@
         <v>399</v>
       </c>
       <c r="K9">
-        <v>448</v>
+        <v>449</v>
       </c>
       <c r="L9">
-        <v>49</v>
+        <v>50</v>
       </c>
     </row>
     <row r="10" spans="1:12">
@@ -21100,7 +21103,7 @@
         <v>1294</v>
       </c>
       <c r="L10">
-        <v>201</v>
+        <v>203</v>
       </c>
     </row>
     <row r="11" spans="1:12">
@@ -21135,10 +21138,10 @@
         <v>4175</v>
       </c>
       <c r="K11">
-        <v>3878</v>
+        <v>3879</v>
       </c>
       <c r="L11">
-        <v>549</v>
+        <v>557</v>
       </c>
     </row>
   </sheetData>
@@ -21279,7 +21282,7 @@
         <v>83</v>
       </c>
       <c r="L3">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="4" spans="1:12">
@@ -21530,7 +21533,7 @@
         <v>2261</v>
       </c>
       <c r="L10">
-        <v>340</v>
+        <v>343</v>
       </c>
     </row>
     <row r="11" spans="1:12">
@@ -21568,7 +21571,7 @@
         <v>3221</v>
       </c>
       <c r="L11">
-        <v>489</v>
+        <v>493</v>
       </c>
     </row>
   </sheetData>
@@ -21899,7 +21902,7 @@
         <v>509</v>
       </c>
       <c r="L8">
-        <v>66</v>
+        <v>67</v>
       </c>
     </row>
     <row r="9" spans="1:12">
@@ -21975,7 +21978,7 @@
         <v>1010</v>
       </c>
       <c r="L10">
-        <v>250</v>
+        <v>253</v>
       </c>
     </row>
     <row r="11" spans="1:12">
@@ -22013,7 +22016,7 @@
         <v>2529</v>
       </c>
       <c r="L11">
-        <v>479</v>
+        <v>483</v>
       </c>
     </row>
   </sheetData>
@@ -22381,7 +22384,7 @@
         <v>421</v>
       </c>
       <c r="L10">
-        <v>60</v>
+        <v>61</v>
       </c>
     </row>
     <row r="11" spans="1:12">
@@ -22419,7 +22422,7 @@
         <v>723</v>
       </c>
       <c r="L11">
-        <v>90</v>
+        <v>91</v>
       </c>
     </row>
   </sheetData>
@@ -22817,7 +22820,7 @@
         <v>713</v>
       </c>
       <c r="L10">
-        <v>111</v>
+        <v>114</v>
       </c>
     </row>
     <row r="11" spans="1:12">
@@ -22855,7 +22858,7 @@
         <v>1296</v>
       </c>
       <c r="L11">
-        <v>181</v>
+        <v>184</v>
       </c>
     </row>
   </sheetData>
@@ -22958,7 +22961,7 @@
         <v>270</v>
       </c>
       <c r="L2">
-        <v>31</v>
+        <v>32</v>
       </c>
     </row>
     <row r="3" spans="1:12">
@@ -22996,7 +22999,7 @@
         <v>299</v>
       </c>
       <c r="L3">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="4" spans="1:12">
@@ -23183,7 +23186,7 @@
         <v>719</v>
       </c>
       <c r="L8">
-        <v>75</v>
+        <v>76</v>
       </c>
     </row>
     <row r="9" spans="1:12">
@@ -23259,7 +23262,7 @@
         <v>1251</v>
       </c>
       <c r="L10">
-        <v>210</v>
+        <v>211</v>
       </c>
     </row>
     <row r="11" spans="1:12">
@@ -23297,7 +23300,7 @@
         <v>3262</v>
       </c>
       <c r="L11">
-        <v>428</v>
+        <v>432</v>
       </c>
     </row>
   </sheetData>
@@ -23821,7 +23824,7 @@
         <v>267</v>
       </c>
       <c r="L2">
-        <v>28</v>
+        <v>29</v>
       </c>
     </row>
     <row r="3" spans="1:12">
@@ -23859,7 +23862,7 @@
         <v>259</v>
       </c>
       <c r="L3">
-        <v>42</v>
+        <v>43</v>
       </c>
     </row>
     <row r="4" spans="1:12">
@@ -23935,7 +23938,7 @@
         <v>207</v>
       </c>
       <c r="L5">
-        <v>36</v>
+        <v>39</v>
       </c>
     </row>
     <row r="6" spans="1:12">
@@ -24125,7 +24128,7 @@
         <v>899</v>
       </c>
       <c r="L10">
-        <v>176</v>
+        <v>179</v>
       </c>
     </row>
     <row r="11" spans="1:12">
@@ -24163,7 +24166,7 @@
         <v>2521</v>
       </c>
       <c r="L11">
-        <v>442</v>
+        <v>450</v>
       </c>
     </row>
   </sheetData>
@@ -25354,7 +25357,7 @@
         <v>455</v>
       </c>
       <c r="L8">
-        <v>77</v>
+        <v>78</v>
       </c>
     </row>
     <row r="9" spans="1:12">
@@ -25430,7 +25433,7 @@
         <v>795</v>
       </c>
       <c r="L10">
-        <v>97</v>
+        <v>98</v>
       </c>
     </row>
     <row r="11" spans="1:12">
@@ -25468,7 +25471,7 @@
         <v>1715</v>
       </c>
       <c r="L11">
-        <v>254</v>
+        <v>256</v>
       </c>
     </row>
   </sheetData>
@@ -26249,7 +26252,7 @@
         <v>875</v>
       </c>
       <c r="L10">
-        <v>136</v>
+        <v>139</v>
       </c>
     </row>
     <row r="11" spans="1:12">
@@ -26287,7 +26290,7 @@
         <v>1287</v>
       </c>
       <c r="L11">
-        <v>196</v>
+        <v>199</v>
       </c>
     </row>
   </sheetData>
@@ -26579,7 +26582,7 @@
         <v>98</v>
       </c>
       <c r="L8">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="9" spans="1:12">
@@ -26655,7 +26658,7 @@
         <v>725</v>
       </c>
       <c r="L10">
-        <v>97</v>
+        <v>99</v>
       </c>
     </row>
     <row r="11" spans="1:12">
@@ -26693,7 +26696,7 @@
         <v>1011</v>
       </c>
       <c r="L11">
-        <v>140</v>
+        <v>143</v>
       </c>
     </row>
   </sheetData>
@@ -27024,7 +27027,7 @@
         <v>353</v>
       </c>
       <c r="L8">
-        <v>51</v>
+        <v>52</v>
       </c>
     </row>
     <row r="9" spans="1:12">
@@ -27100,7 +27103,7 @@
         <v>1145</v>
       </c>
       <c r="L10">
-        <v>181</v>
+        <v>183</v>
       </c>
     </row>
     <row r="11" spans="1:12">
@@ -27138,7 +27141,7 @@
         <v>1948</v>
       </c>
       <c r="L11">
-        <v>318</v>
+        <v>321</v>
       </c>
     </row>
   </sheetData>
@@ -27442,7 +27445,7 @@
         <v>73</v>
       </c>
       <c r="L8">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="9" spans="1:12">
@@ -27556,7 +27559,7 @@
         <v>498</v>
       </c>
       <c r="L11">
-        <v>107</v>
+        <v>108</v>
       </c>
     </row>
   </sheetData>
@@ -27948,7 +27951,7 @@
         <v>377</v>
       </c>
       <c r="L10">
-        <v>57</v>
+        <v>59</v>
       </c>
     </row>
     <row r="11" spans="1:12">
@@ -27986,7 +27989,7 @@
         <v>675</v>
       </c>
       <c r="L11">
-        <v>94</v>
+        <v>96</v>
       </c>
     </row>
   </sheetData>
@@ -28753,7 +28756,7 @@
         <v>367</v>
       </c>
       <c r="L8">
-        <v>42</v>
+        <v>44</v>
       </c>
     </row>
     <row r="9" spans="1:12">
@@ -28791,7 +28794,7 @@
         <v>164</v>
       </c>
       <c r="L9">
-        <v>18</v>
+        <v>19</v>
       </c>
     </row>
     <row r="10" spans="1:12">
@@ -28829,7 +28832,7 @@
         <v>1156</v>
       </c>
       <c r="L10">
-        <v>204</v>
+        <v>206</v>
       </c>
     </row>
     <row r="11" spans="1:12">
@@ -28867,7 +28870,7 @@
         <v>2123</v>
       </c>
       <c r="L11">
-        <v>323</v>
+        <v>328</v>
       </c>
     </row>
   </sheetData>
@@ -28970,7 +28973,7 @@
         <v>73</v>
       </c>
       <c r="L2">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="3" spans="1:12">
@@ -29265,7 +29268,7 @@
         <v>725</v>
       </c>
       <c r="L10">
-        <v>114</v>
+        <v>115</v>
       </c>
     </row>
     <row r="11" spans="1:12">
@@ -29303,7 +29306,7 @@
         <v>1331</v>
       </c>
       <c r="L11">
-        <v>206</v>
+        <v>208</v>
       </c>
     </row>
   </sheetData>
@@ -29710,7 +29713,7 @@
         <v>387</v>
       </c>
       <c r="L10">
-        <v>50</v>
+        <v>54</v>
       </c>
     </row>
     <row r="11" spans="1:12">
@@ -29748,7 +29751,7 @@
         <v>1048</v>
       </c>
       <c r="L11">
-        <v>154</v>
+        <v>158</v>
       </c>
     </row>
   </sheetData>
@@ -30070,7 +30073,7 @@
         <v>307</v>
       </c>
       <c r="L8">
-        <v>56</v>
+        <v>57</v>
       </c>
     </row>
     <row r="9" spans="1:12">
@@ -30146,7 +30149,7 @@
         <v>764</v>
       </c>
       <c r="L10">
-        <v>136</v>
+        <v>140</v>
       </c>
     </row>
     <row r="11" spans="1:12">
@@ -30184,7 +30187,7 @@
         <v>1494</v>
       </c>
       <c r="L11">
-        <v>249</v>
+        <v>254</v>
       </c>
     </row>
   </sheetData>
@@ -30287,7 +30290,7 @@
         <v>227</v>
       </c>
       <c r="L2">
-        <v>34</v>
+        <v>37</v>
       </c>
     </row>
     <row r="3" spans="1:12">
@@ -30401,7 +30404,7 @@
         <v>119</v>
       </c>
       <c r="L5">
-        <v>26</v>
+        <v>27</v>
       </c>
     </row>
     <row r="6" spans="1:12">
@@ -30515,7 +30518,7 @@
         <v>396</v>
       </c>
       <c r="L8">
-        <v>49</v>
+        <v>51</v>
       </c>
     </row>
     <row r="9" spans="1:12">
@@ -30591,7 +30594,7 @@
         <v>768</v>
       </c>
       <c r="L10">
-        <v>168</v>
+        <v>170</v>
       </c>
     </row>
     <row r="11" spans="1:12">
@@ -30629,7 +30632,7 @@
         <v>1977</v>
       </c>
       <c r="L11">
-        <v>347</v>
+        <v>355</v>
       </c>
     </row>
   </sheetData>
@@ -31415,7 +31418,7 @@
         <v>523</v>
       </c>
       <c r="L10">
-        <v>85</v>
+        <v>86</v>
       </c>
     </row>
     <row r="11" spans="1:12">
@@ -31453,7 +31456,7 @@
         <v>1049</v>
       </c>
       <c r="L11">
-        <v>144</v>
+        <v>145</v>
       </c>
     </row>
   </sheetData>
@@ -31667,7 +31670,7 @@
         <v>83</v>
       </c>
       <c r="L5">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="6" spans="1:12">
@@ -31781,7 +31784,7 @@
         <v>304</v>
       </c>
       <c r="L8">
-        <v>38</v>
+        <v>40</v>
       </c>
     </row>
     <row r="9" spans="1:12">
@@ -31819,7 +31822,7 @@
         <v>70</v>
       </c>
       <c r="L9">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="10" spans="1:12">
@@ -31857,7 +31860,7 @@
         <v>495</v>
       </c>
       <c r="L10">
-        <v>75</v>
+        <v>78</v>
       </c>
     </row>
     <row r="11" spans="1:12">
@@ -31895,7 +31898,7 @@
         <v>1148</v>
       </c>
       <c r="L11">
-        <v>157</v>
+        <v>164</v>
       </c>
     </row>
   </sheetData>
@@ -32036,7 +32039,7 @@
         <v>22</v>
       </c>
       <c r="L3">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="4" spans="1:12">
@@ -32284,7 +32287,7 @@
         <v>639</v>
       </c>
       <c r="L10">
-        <v>122</v>
+        <v>123</v>
       </c>
     </row>
     <row r="11" spans="1:12">
@@ -32322,7 +32325,7 @@
         <v>1042</v>
       </c>
       <c r="L11">
-        <v>179</v>
+        <v>181</v>
       </c>
     </row>
   </sheetData>
@@ -32536,7 +32539,7 @@
         <v>66</v>
       </c>
       <c r="L5">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="6" spans="1:12">
@@ -32641,7 +32644,7 @@
         <v>271</v>
       </c>
       <c r="L8">
-        <v>37</v>
+        <v>39</v>
       </c>
     </row>
     <row r="9" spans="1:12">
@@ -32717,7 +32720,7 @@
         <v>480</v>
       </c>
       <c r="L10">
-        <v>95</v>
+        <v>97</v>
       </c>
     </row>
     <row r="11" spans="1:12">
@@ -32755,7 +32758,7 @@
         <v>934</v>
       </c>
       <c r="L11">
-        <v>163</v>
+        <v>168</v>
       </c>
     </row>
   </sheetData>
@@ -33156,7 +33159,7 @@
         <v>291</v>
       </c>
       <c r="L10">
-        <v>42</v>
+        <v>43</v>
       </c>
     </row>
     <row r="11" spans="1:12">
@@ -33194,7 +33197,7 @@
         <v>751</v>
       </c>
       <c r="L11">
-        <v>125</v>
+        <v>126</v>
       </c>
     </row>
   </sheetData>
@@ -33474,7 +33477,7 @@
         <v>120</v>
       </c>
       <c r="L8">
-        <v>15</v>
+        <v>16</v>
       </c>
     </row>
     <row r="9" spans="1:12">
@@ -33550,7 +33553,7 @@
         <v>500</v>
       </c>
       <c r="L10">
-        <v>96</v>
+        <v>99</v>
       </c>
     </row>
     <row r="11" spans="1:12">
@@ -33588,7 +33591,7 @@
         <v>682</v>
       </c>
       <c r="L11">
-        <v>128</v>
+        <v>132</v>
       </c>
     </row>
   </sheetData>
@@ -33992,7 +33995,7 @@
         <v>148</v>
       </c>
       <c r="L10">
-        <v>37</v>
+        <v>38</v>
       </c>
     </row>
     <row r="11" spans="1:12">
@@ -34030,7 +34033,7 @@
         <v>447</v>
       </c>
       <c r="L11">
-        <v>85</v>
+        <v>86</v>
       </c>
     </row>
   </sheetData>
@@ -34374,7 +34377,7 @@
         <v>669</v>
       </c>
       <c r="L10">
-        <v>84</v>
+        <v>87</v>
       </c>
     </row>
     <row r="11" spans="1:12">
@@ -34412,7 +34415,7 @@
         <v>718</v>
       </c>
       <c r="L11">
-        <v>87</v>
+        <v>90</v>
       </c>
     </row>
   </sheetData>
@@ -34965,7 +34968,7 @@
         <v>71</v>
       </c>
       <c r="L3">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="4" spans="1:12">
@@ -35038,7 +35041,7 @@
         <v>91</v>
       </c>
       <c r="L5">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="6" spans="1:12">
@@ -35146,7 +35149,7 @@
         <v>154</v>
       </c>
       <c r="L8">
-        <v>29</v>
+        <v>30</v>
       </c>
     </row>
     <row r="9" spans="1:12">
@@ -35222,7 +35225,7 @@
         <v>617</v>
       </c>
       <c r="L10">
-        <v>113</v>
+        <v>117</v>
       </c>
     </row>
     <row r="11" spans="1:12">
@@ -35260,7 +35263,7 @@
         <v>1107</v>
       </c>
       <c r="L11">
-        <v>179</v>
+        <v>186</v>
       </c>
     </row>
   </sheetData>
@@ -35531,6 +35534,9 @@
       <c r="I7">
         <v>2</v>
       </c>
+      <c r="L7">
+        <v>1</v>
+      </c>
     </row>
     <row r="8" spans="1:12">
       <c r="A8" s="1" t="s">
@@ -35643,7 +35649,7 @@
         <v>487</v>
       </c>
       <c r="L10">
-        <v>88</v>
+        <v>89</v>
       </c>
     </row>
     <row r="11" spans="1:12">
@@ -35681,7 +35687,7 @@
         <v>756</v>
       </c>
       <c r="L11">
-        <v>125</v>
+        <v>127</v>
       </c>
     </row>
   </sheetData>
@@ -36058,7 +36064,7 @@
         <v>808</v>
       </c>
       <c r="L10">
-        <v>204</v>
+        <v>205</v>
       </c>
     </row>
     <row r="11" spans="1:12">
@@ -36096,7 +36102,7 @@
         <v>1331</v>
       </c>
       <c r="L11">
-        <v>280</v>
+        <v>281</v>
       </c>
     </row>
   </sheetData>
@@ -36394,7 +36400,7 @@
         <v>33</v>
       </c>
       <c r="L8">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="9" spans="1:12">
@@ -36508,7 +36514,7 @@
         <v>140</v>
       </c>
       <c r="L11">
-        <v>17</v>
+        <v>18</v>
       </c>
     </row>
   </sheetData>
@@ -36894,7 +36900,7 @@
         <v>353</v>
       </c>
       <c r="L10">
-        <v>91</v>
+        <v>93</v>
       </c>
     </row>
     <row r="11" spans="1:12">
@@ -36932,7 +36938,7 @@
         <v>616</v>
       </c>
       <c r="L11">
-        <v>132</v>
+        <v>134</v>
       </c>
     </row>
   </sheetData>
@@ -37727,7 +37733,7 @@
         <v>411</v>
       </c>
       <c r="L10">
-        <v>55</v>
+        <v>56</v>
       </c>
     </row>
     <row r="11" spans="1:12">
@@ -37765,7 +37771,7 @@
         <v>977</v>
       </c>
       <c r="L11">
-        <v>118</v>
+        <v>119</v>
       </c>
     </row>
   </sheetData>
@@ -38128,7 +38134,7 @@
         <v>121</v>
       </c>
       <c r="L9">
-        <v>12</v>
+        <v>13</v>
       </c>
     </row>
     <row r="10" spans="1:12">
@@ -38166,7 +38172,7 @@
         <v>1481</v>
       </c>
       <c r="L10">
-        <v>224</v>
+        <v>225</v>
       </c>
     </row>
     <row r="11" spans="1:12">
@@ -38204,7 +38210,7 @@
         <v>2321</v>
       </c>
       <c r="L11">
-        <v>331</v>
+        <v>333</v>
       </c>
     </row>
   </sheetData>
@@ -39917,7 +39923,7 @@
         <v>122</v>
       </c>
       <c r="L5">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="6" spans="1:12">
@@ -39955,7 +39961,7 @@
         <v>9</v>
       </c>
       <c r="L6">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="7" spans="1:12">
@@ -40095,7 +40101,7 @@
         <v>963</v>
       </c>
       <c r="L10">
-        <v>154</v>
+        <v>157</v>
       </c>
     </row>
     <row r="11" spans="1:12">
@@ -40133,7 +40139,7 @@
         <v>1500</v>
       </c>
       <c r="L11">
-        <v>230</v>
+        <v>235</v>
       </c>
     </row>
   </sheetData>
@@ -40398,7 +40404,7 @@
         <v>76</v>
       </c>
       <c r="L8">
-        <v>7</v>
+        <v>10</v>
       </c>
     </row>
     <row r="9" spans="1:12">
@@ -40512,7 +40518,7 @@
         <v>281</v>
       </c>
       <c r="L11">
-        <v>44</v>
+        <v>47</v>
       </c>
     </row>
   </sheetData>
@@ -41678,7 +41684,7 @@
         <v>165</v>
       </c>
       <c r="L9">
-        <v>26</v>
+        <v>27</v>
       </c>
     </row>
     <row r="10" spans="1:12">
@@ -41716,7 +41722,7 @@
         <v>285</v>
       </c>
       <c r="L10">
-        <v>50</v>
+        <v>51</v>
       </c>
     </row>
   </sheetData>
@@ -42044,7 +42050,7 @@
         <v>120</v>
       </c>
       <c r="L8">
-        <v>15</v>
+        <v>18</v>
       </c>
     </row>
     <row r="9" spans="1:12">
@@ -42158,7 +42164,7 @@
         <v>485</v>
       </c>
       <c r="L11">
-        <v>72</v>
+        <v>75</v>
       </c>
     </row>
   </sheetData>
@@ -42261,7 +42267,7 @@
         <v>424</v>
       </c>
       <c r="L2">
-        <v>50</v>
+        <v>52</v>
       </c>
     </row>
     <row r="3" spans="1:12">
@@ -42375,7 +42381,7 @@
         <v>429</v>
       </c>
       <c r="L5">
-        <v>55</v>
+        <v>56</v>
       </c>
     </row>
     <row r="6" spans="1:12">
@@ -42489,7 +42495,7 @@
         <v>636</v>
       </c>
       <c r="L8">
-        <v>77</v>
+        <v>78</v>
       </c>
     </row>
     <row r="9" spans="1:12">
@@ -42565,7 +42571,7 @@
         <v>1484</v>
       </c>
       <c r="L10">
-        <v>266</v>
+        <v>269</v>
       </c>
     </row>
     <row r="11" spans="1:12">
@@ -42603,7 +42609,7 @@
         <v>3845</v>
       </c>
       <c r="L11">
-        <v>602</v>
+        <v>609</v>
       </c>
     </row>
   </sheetData>
@@ -43764,7 +43770,7 @@
         <v>337</v>
       </c>
       <c r="L10">
-        <v>64</v>
+        <v>66</v>
       </c>
     </row>
     <row r="11" spans="1:12">
@@ -43802,7 +43808,7 @@
         <v>575</v>
       </c>
       <c r="L11">
-        <v>98</v>
+        <v>100</v>
       </c>
     </row>
   </sheetData>
@@ -44016,7 +44022,7 @@
         <v>70</v>
       </c>
       <c r="L5">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="6" spans="1:12">
@@ -44206,7 +44212,7 @@
         <v>476</v>
       </c>
       <c r="L10">
-        <v>67</v>
+        <v>68</v>
       </c>
     </row>
     <row r="11" spans="1:12">
@@ -44244,7 +44250,7 @@
         <v>1020</v>
       </c>
       <c r="L11">
-        <v>154</v>
+        <v>156</v>
       </c>
     </row>
   </sheetData>
@@ -45866,7 +45872,7 @@
         <v>13</v>
       </c>
       <c r="L3">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="4" spans="1:12">
@@ -46099,7 +46105,7 @@
         <v>404</v>
       </c>
       <c r="L10">
-        <v>33</v>
+        <v>34</v>
       </c>
     </row>
     <row r="11" spans="1:12">
@@ -46137,7 +46143,7 @@
         <v>559</v>
       </c>
       <c r="L11">
-        <v>69</v>
+        <v>71</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add data for 2025-07-14
</commit_message>
<xml_diff>
--- a/output/index-crime-full-year.xlsx
+++ b/output/index-crime-full-year.xlsx
@@ -891,7 +891,7 @@
         <v>6002</v>
       </c>
       <c r="F2">
-        <v>5841</v>
+        <v>5842</v>
       </c>
       <c r="G2">
         <v>6265</v>
@@ -909,7 +909,7 @@
         <v>7903</v>
       </c>
       <c r="L2">
-        <v>3509</v>
+        <v>3522</v>
       </c>
     </row>
     <row r="3" spans="1:12">
@@ -947,7 +947,7 @@
         <v>8184</v>
       </c>
       <c r="L3">
-        <v>3669</v>
+        <v>3696</v>
       </c>
     </row>
     <row r="4" spans="1:12">
@@ -985,7 +985,7 @@
         <v>483</v>
       </c>
       <c r="L4">
-        <v>208</v>
+        <v>210</v>
       </c>
     </row>
     <row r="5" spans="1:12">
@@ -1023,7 +1023,7 @@
         <v>7651</v>
       </c>
       <c r="L5">
-        <v>3160</v>
+        <v>3175</v>
       </c>
     </row>
     <row r="6" spans="1:12">
@@ -1058,10 +1058,10 @@
         <v>1869</v>
       </c>
       <c r="K6">
-        <v>1770</v>
+        <v>1769</v>
       </c>
       <c r="L6">
-        <v>912</v>
+        <v>916</v>
       </c>
     </row>
     <row r="7" spans="1:12">
@@ -1099,7 +1099,7 @@
         <v>587</v>
       </c>
       <c r="L7">
-        <v>220</v>
+        <v>221</v>
       </c>
     </row>
     <row r="8" spans="1:12">
@@ -1137,7 +1137,7 @@
         <v>21702</v>
       </c>
       <c r="L8">
-        <v>8573</v>
+        <v>8632</v>
       </c>
     </row>
     <row r="9" spans="1:12">
@@ -1175,7 +1175,7 @@
         <v>9119</v>
       </c>
       <c r="L9">
-        <v>3209</v>
+        <v>3235</v>
       </c>
     </row>
     <row r="10" spans="1:12">
@@ -1213,7 +1213,7 @@
         <v>61250</v>
       </c>
       <c r="L10">
-        <v>29877</v>
+        <v>30033</v>
       </c>
     </row>
     <row r="11" spans="1:12">
@@ -1233,7 +1233,7 @@
         <v>113451</v>
       </c>
       <c r="F11">
-        <v>105613</v>
+        <v>105614</v>
       </c>
       <c r="G11">
         <v>85387</v>
@@ -1248,10 +1248,10 @@
         <v>124084</v>
       </c>
       <c r="K11">
-        <v>118649</v>
+        <v>118648</v>
       </c>
       <c r="L11">
-        <v>53337</v>
+        <v>53640</v>
       </c>
     </row>
   </sheetData>
@@ -1392,7 +1392,7 @@
         <v>194</v>
       </c>
       <c r="L3">
-        <v>72</v>
+        <v>73</v>
       </c>
     </row>
     <row r="4" spans="1:12">
@@ -1430,7 +1430,7 @@
         <v>14</v>
       </c>
       <c r="L4">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="5" spans="1:12">
@@ -1506,7 +1506,7 @@
         <v>41</v>
       </c>
       <c r="L6">
-        <v>17</v>
+        <v>18</v>
       </c>
     </row>
     <row r="7" spans="1:12">
@@ -1620,7 +1620,7 @@
         <v>248</v>
       </c>
       <c r="L9">
-        <v>62</v>
+        <v>63</v>
       </c>
     </row>
     <row r="10" spans="1:12">
@@ -1658,7 +1658,7 @@
         <v>849</v>
       </c>
       <c r="L10">
-        <v>340</v>
+        <v>342</v>
       </c>
     </row>
     <row r="11" spans="1:12">
@@ -1696,7 +1696,7 @@
         <v>1847</v>
       </c>
       <c r="L11">
-        <v>710</v>
+        <v>716</v>
       </c>
     </row>
   </sheetData>
@@ -2338,7 +2338,7 @@
         <v>69</v>
       </c>
       <c r="L8">
-        <v>26</v>
+        <v>27</v>
       </c>
     </row>
     <row r="9" spans="1:12">
@@ -2414,7 +2414,7 @@
         <v>349</v>
       </c>
       <c r="L10">
-        <v>180</v>
+        <v>183</v>
       </c>
     </row>
     <row r="11" spans="1:12">
@@ -2452,7 +2452,7 @@
         <v>539</v>
       </c>
       <c r="L11">
-        <v>255</v>
+        <v>259</v>
       </c>
     </row>
   </sheetData>
@@ -2859,7 +2859,7 @@
         <v>1473</v>
       </c>
       <c r="L10">
-        <v>602</v>
+        <v>603</v>
       </c>
     </row>
     <row r="11" spans="1:12">
@@ -2897,7 +2897,7 @@
         <v>2352</v>
       </c>
       <c r="L11">
-        <v>911</v>
+        <v>912</v>
       </c>
     </row>
   </sheetData>
@@ -3038,7 +3038,7 @@
         <v>543</v>
       </c>
       <c r="L3">
-        <v>248</v>
+        <v>249</v>
       </c>
     </row>
     <row r="4" spans="1:12">
@@ -3228,7 +3228,7 @@
         <v>931</v>
       </c>
       <c r="L8">
-        <v>377</v>
+        <v>380</v>
       </c>
     </row>
     <row r="9" spans="1:12">
@@ -3266,7 +3266,7 @@
         <v>610</v>
       </c>
       <c r="L9">
-        <v>207</v>
+        <v>208</v>
       </c>
     </row>
     <row r="10" spans="1:12">
@@ -3304,7 +3304,7 @@
         <v>1964</v>
       </c>
       <c r="L10">
-        <v>1146</v>
+        <v>1152</v>
       </c>
     </row>
     <row r="11" spans="1:12">
@@ -3342,7 +3342,7 @@
         <v>4976</v>
       </c>
       <c r="L11">
-        <v>2414</v>
+        <v>2425</v>
       </c>
     </row>
   </sheetData>
@@ -4079,7 +4079,7 @@
         <v>190</v>
       </c>
       <c r="L8">
-        <v>59</v>
+        <v>60</v>
       </c>
     </row>
     <row r="9" spans="1:12">
@@ -4155,7 +4155,7 @@
         <v>386</v>
       </c>
       <c r="L10">
-        <v>213</v>
+        <v>214</v>
       </c>
     </row>
     <row r="11" spans="1:12">
@@ -4193,7 +4193,7 @@
         <v>784</v>
       </c>
       <c r="L11">
-        <v>355</v>
+        <v>357</v>
       </c>
     </row>
   </sheetData>
@@ -4573,7 +4573,7 @@
         <v>163</v>
       </c>
       <c r="L10">
-        <v>85</v>
+        <v>86</v>
       </c>
     </row>
     <row r="11" spans="1:12">
@@ -4611,7 +4611,7 @@
         <v>378</v>
       </c>
       <c r="L11">
-        <v>182</v>
+        <v>183</v>
       </c>
     </row>
   </sheetData>
@@ -4942,7 +4942,7 @@
         <v>331</v>
       </c>
       <c r="L8">
-        <v>216</v>
+        <v>217</v>
       </c>
     </row>
     <row r="9" spans="1:12">
@@ -5018,7 +5018,7 @@
         <v>576</v>
       </c>
       <c r="L10">
-        <v>231</v>
+        <v>234</v>
       </c>
     </row>
     <row r="11" spans="1:12">
@@ -5056,7 +5056,7 @@
         <v>1627</v>
       </c>
       <c r="L11">
-        <v>792</v>
+        <v>796</v>
       </c>
     </row>
   </sheetData>
@@ -5197,7 +5197,7 @@
         <v>406</v>
       </c>
       <c r="L3">
-        <v>173</v>
+        <v>174</v>
       </c>
     </row>
     <row r="4" spans="1:12">
@@ -5387,7 +5387,7 @@
         <v>539</v>
       </c>
       <c r="L8">
-        <v>240</v>
+        <v>241</v>
       </c>
     </row>
     <row r="9" spans="1:12">
@@ -5425,7 +5425,7 @@
         <v>363</v>
       </c>
       <c r="L9">
-        <v>180</v>
+        <v>181</v>
       </c>
     </row>
     <row r="10" spans="1:12">
@@ -5463,7 +5463,7 @@
         <v>929</v>
       </c>
       <c r="L10">
-        <v>414</v>
+        <v>417</v>
       </c>
     </row>
     <row r="11" spans="1:12">
@@ -5501,7 +5501,7 @@
         <v>2788</v>
       </c>
       <c r="L11">
-        <v>1270</v>
+        <v>1276</v>
       </c>
     </row>
   </sheetData>
@@ -5604,7 +5604,7 @@
         <v>218</v>
       </c>
       <c r="L2">
-        <v>102</v>
+        <v>103</v>
       </c>
     </row>
     <row r="3" spans="1:12">
@@ -5870,7 +5870,7 @@
         <v>176</v>
       </c>
       <c r="L9">
-        <v>57</v>
+        <v>58</v>
       </c>
     </row>
     <row r="10" spans="1:12">
@@ -5908,7 +5908,7 @@
         <v>874</v>
       </c>
       <c r="L10">
-        <v>448</v>
+        <v>449</v>
       </c>
     </row>
     <row r="11" spans="1:12">
@@ -5946,7 +5946,7 @@
         <v>2264</v>
       </c>
       <c r="L11">
-        <v>1067</v>
+        <v>1070</v>
       </c>
     </row>
   </sheetData>
@@ -6049,7 +6049,7 @@
         <v>1104</v>
       </c>
       <c r="L2">
-        <v>481</v>
+        <v>482</v>
       </c>
     </row>
     <row r="3" spans="1:12">
@@ -6087,7 +6087,7 @@
         <v>263</v>
       </c>
       <c r="L3">
-        <v>143</v>
+        <v>144</v>
       </c>
     </row>
     <row r="4" spans="1:12">
@@ -6125,7 +6125,7 @@
         <v>616</v>
       </c>
       <c r="L4">
-        <v>302</v>
+        <v>306</v>
       </c>
     </row>
     <row r="5" spans="1:12">
@@ -6163,7 +6163,7 @@
         <v>251</v>
       </c>
       <c r="L5">
-        <v>144</v>
+        <v>145</v>
       </c>
     </row>
     <row r="6" spans="1:12">
@@ -6239,7 +6239,7 @@
         <v>2524</v>
       </c>
       <c r="L7">
-        <v>1282</v>
+        <v>1292</v>
       </c>
     </row>
     <row r="8" spans="1:12">
@@ -6277,7 +6277,7 @@
         <v>4976</v>
       </c>
       <c r="L8">
-        <v>2414</v>
+        <v>2425</v>
       </c>
     </row>
     <row r="9" spans="1:12">
@@ -6315,7 +6315,7 @@
         <v>484</v>
       </c>
       <c r="L9">
-        <v>222</v>
+        <v>223</v>
       </c>
     </row>
     <row r="10" spans="1:12">
@@ -6353,7 +6353,7 @@
         <v>1286</v>
       </c>
       <c r="L10">
-        <v>604</v>
+        <v>607</v>
       </c>
     </row>
     <row r="11" spans="1:12">
@@ -6391,7 +6391,7 @@
         <v>2119</v>
       </c>
       <c r="L11">
-        <v>882</v>
+        <v>885</v>
       </c>
     </row>
     <row r="12" spans="1:12">
@@ -6429,7 +6429,7 @@
         <v>559</v>
       </c>
       <c r="L12">
-        <v>214</v>
+        <v>217</v>
       </c>
     </row>
     <row r="13" spans="1:12">
@@ -6505,7 +6505,7 @@
         <v>720</v>
       </c>
       <c r="L14">
-        <v>352</v>
+        <v>355</v>
       </c>
     </row>
     <row r="15" spans="1:12">
@@ -6581,7 +6581,7 @@
         <v>938</v>
       </c>
       <c r="L16">
-        <v>392</v>
+        <v>393</v>
       </c>
     </row>
     <row r="17" spans="1:12">
@@ -6619,7 +6619,7 @@
         <v>140</v>
       </c>
       <c r="L17">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="18" spans="1:12">
@@ -6657,7 +6657,7 @@
         <v>751</v>
       </c>
       <c r="L18">
-        <v>338</v>
+        <v>341</v>
       </c>
     </row>
     <row r="19" spans="1:12">
@@ -6695,7 +6695,7 @@
         <v>2526</v>
       </c>
       <c r="L19">
-        <v>1301</v>
+        <v>1307</v>
       </c>
     </row>
     <row r="20" spans="1:12">
@@ -6733,7 +6733,7 @@
         <v>1973</v>
       </c>
       <c r="L20">
-        <v>942</v>
+        <v>944</v>
       </c>
     </row>
     <row r="21" spans="1:12">
@@ -6771,7 +6771,7 @@
         <v>321</v>
       </c>
       <c r="L21">
-        <v>127</v>
+        <v>128</v>
       </c>
     </row>
     <row r="22" spans="1:12">
@@ -6809,7 +6809,7 @@
         <v>441</v>
       </c>
       <c r="L22">
-        <v>198</v>
+        <v>201</v>
       </c>
     </row>
     <row r="23" spans="1:12">
@@ -6847,7 +6847,7 @@
         <v>1330</v>
       </c>
       <c r="L23">
-        <v>640</v>
+        <v>642</v>
       </c>
     </row>
     <row r="24" spans="1:12">
@@ -6885,7 +6885,7 @@
         <v>675</v>
       </c>
       <c r="L24">
-        <v>249</v>
+        <v>251</v>
       </c>
     </row>
     <row r="25" spans="1:12">
@@ -6923,7 +6923,7 @@
         <v>555</v>
       </c>
       <c r="L25">
-        <v>310</v>
+        <v>313</v>
       </c>
     </row>
     <row r="26" spans="1:12">
@@ -7037,7 +7037,7 @@
         <v>97</v>
       </c>
       <c r="L28">
-        <v>51</v>
+        <v>52</v>
       </c>
     </row>
     <row r="29" spans="1:12">
@@ -7075,7 +7075,7 @@
         <v>3877</v>
       </c>
       <c r="L29">
-        <v>1724</v>
+        <v>1734</v>
       </c>
     </row>
     <row r="30" spans="1:12">
@@ -7151,7 +7151,7 @@
         <v>1039</v>
       </c>
       <c r="L31">
-        <v>480</v>
+        <v>483</v>
       </c>
     </row>
     <row r="32" spans="1:12">
@@ -7227,7 +7227,7 @@
         <v>2788</v>
       </c>
       <c r="L33">
-        <v>1270</v>
+        <v>1276</v>
       </c>
     </row>
     <row r="34" spans="1:12">
@@ -7265,7 +7265,7 @@
         <v>973</v>
       </c>
       <c r="L34">
-        <v>368</v>
+        <v>369</v>
       </c>
     </row>
     <row r="35" spans="1:12">
@@ -7303,7 +7303,7 @@
         <v>337</v>
       </c>
       <c r="L35">
-        <v>183</v>
+        <v>184</v>
       </c>
     </row>
     <row r="36" spans="1:12">
@@ -7341,7 +7341,7 @@
         <v>1711</v>
       </c>
       <c r="L36">
-        <v>710</v>
+        <v>715</v>
       </c>
     </row>
     <row r="37" spans="1:12">
@@ -7379,7 +7379,7 @@
         <v>2715</v>
       </c>
       <c r="L37">
-        <v>1164</v>
+        <v>1170</v>
       </c>
     </row>
     <row r="38" spans="1:12">
@@ -7417,7 +7417,7 @@
         <v>151</v>
       </c>
       <c r="L38">
-        <v>58</v>
+        <v>59</v>
       </c>
     </row>
     <row r="39" spans="1:12">
@@ -7455,7 +7455,7 @@
         <v>194</v>
       </c>
       <c r="L39">
-        <v>80</v>
+        <v>81</v>
       </c>
     </row>
     <row r="40" spans="1:12">
@@ -7493,7 +7493,7 @@
         <v>352</v>
       </c>
       <c r="L40">
-        <v>197</v>
+        <v>198</v>
       </c>
     </row>
     <row r="41" spans="1:12">
@@ -7569,7 +7569,7 @@
         <v>3265</v>
       </c>
       <c r="L42">
-        <v>1244</v>
+        <v>1255</v>
       </c>
     </row>
     <row r="43" spans="1:12">
@@ -7607,7 +7607,7 @@
         <v>1329</v>
       </c>
       <c r="L43">
-        <v>803</v>
+        <v>807</v>
       </c>
     </row>
     <row r="44" spans="1:12">
@@ -7645,7 +7645,7 @@
         <v>1296</v>
       </c>
       <c r="L44">
-        <v>507</v>
+        <v>508</v>
       </c>
     </row>
     <row r="45" spans="1:12">
@@ -7683,7 +7683,7 @@
         <v>170</v>
       </c>
       <c r="L45">
-        <v>63</v>
+        <v>66</v>
       </c>
     </row>
     <row r="46" spans="1:12">
@@ -7759,7 +7759,7 @@
         <v>1046</v>
       </c>
       <c r="L47">
-        <v>463</v>
+        <v>466</v>
       </c>
     </row>
     <row r="48" spans="1:12">
@@ -7797,7 +7797,7 @@
         <v>3217</v>
       </c>
       <c r="L48">
-        <v>1448</v>
+        <v>1457</v>
       </c>
     </row>
     <row r="49" spans="1:12">
@@ -7835,7 +7835,7 @@
         <v>2189</v>
       </c>
       <c r="L49">
-        <v>901</v>
+        <v>905</v>
       </c>
     </row>
     <row r="50" spans="1:12">
@@ -7873,7 +7873,7 @@
         <v>1038</v>
       </c>
       <c r="L50">
-        <v>524</v>
+        <v>528</v>
       </c>
     </row>
     <row r="51" spans="1:12">
@@ -7911,7 +7911,7 @@
         <v>1492</v>
       </c>
       <c r="L51">
-        <v>763</v>
+        <v>768</v>
       </c>
     </row>
     <row r="52" spans="1:12">
@@ -7949,7 +7949,7 @@
         <v>1847</v>
       </c>
       <c r="L52">
-        <v>710</v>
+        <v>716</v>
       </c>
     </row>
     <row r="53" spans="1:12">
@@ -7987,7 +7987,7 @@
         <v>2352</v>
       </c>
       <c r="L53">
-        <v>911</v>
+        <v>912</v>
       </c>
     </row>
     <row r="54" spans="1:12">
@@ -8025,7 +8025,7 @@
         <v>4179</v>
       </c>
       <c r="L54">
-        <v>1986</v>
+        <v>1994</v>
       </c>
     </row>
     <row r="55" spans="1:12">
@@ -8063,7 +8063,7 @@
         <v>1291</v>
       </c>
       <c r="L55">
-        <v>535</v>
+        <v>537</v>
       </c>
     </row>
     <row r="56" spans="1:12">
@@ -8101,7 +8101,7 @@
         <v>718</v>
       </c>
       <c r="L56">
-        <v>289</v>
+        <v>292</v>
       </c>
     </row>
     <row r="57" spans="1:12">
@@ -8177,7 +8177,7 @@
         <v>202</v>
       </c>
       <c r="L58">
-        <v>50</v>
+        <v>51</v>
       </c>
     </row>
     <row r="59" spans="1:12">
@@ -8215,7 +8215,7 @@
         <v>248</v>
       </c>
       <c r="L59">
-        <v>132</v>
+        <v>133</v>
       </c>
     </row>
     <row r="60" spans="1:12">
@@ -8253,7 +8253,7 @@
         <v>784</v>
       </c>
       <c r="L60">
-        <v>355</v>
+        <v>357</v>
       </c>
     </row>
     <row r="61" spans="1:12">
@@ -8291,7 +8291,7 @@
         <v>167</v>
       </c>
       <c r="L61">
-        <v>66</v>
+        <v>67</v>
       </c>
     </row>
     <row r="62" spans="1:12">
@@ -8349,7 +8349,7 @@
         <v>2106</v>
       </c>
       <c r="F63">
-        <v>1376</v>
+        <v>1377</v>
       </c>
       <c r="G63">
         <v>1907</v>
@@ -8364,10 +8364,10 @@
         <v>1001</v>
       </c>
       <c r="K63">
-        <v>795</v>
+        <v>794</v>
       </c>
       <c r="L63">
-        <v>248</v>
+        <v>269</v>
       </c>
     </row>
     <row r="64" spans="1:12">
@@ -8405,7 +8405,7 @@
         <v>1133</v>
       </c>
       <c r="L64">
-        <v>469</v>
+        <v>471</v>
       </c>
     </row>
     <row r="65" spans="1:12">
@@ -8443,7 +8443,7 @@
         <v>1683</v>
       </c>
       <c r="L65">
-        <v>733</v>
+        <v>735</v>
       </c>
     </row>
     <row r="66" spans="1:12">
@@ -8481,7 +8481,7 @@
         <v>722</v>
       </c>
       <c r="L66">
-        <v>278</v>
+        <v>279</v>
       </c>
     </row>
     <row r="67" spans="1:12">
@@ -8519,7 +8519,7 @@
         <v>2435</v>
       </c>
       <c r="L67">
-        <v>1002</v>
+        <v>1005</v>
       </c>
     </row>
     <row r="68" spans="1:12">
@@ -8557,7 +8557,7 @@
         <v>497</v>
       </c>
       <c r="L68">
-        <v>269</v>
+        <v>272</v>
       </c>
     </row>
     <row r="69" spans="1:12">
@@ -8595,7 +8595,7 @@
         <v>539</v>
       </c>
       <c r="L69">
-        <v>255</v>
+        <v>259</v>
       </c>
     </row>
     <row r="70" spans="1:12">
@@ -8633,7 +8633,7 @@
         <v>686</v>
       </c>
       <c r="L70">
-        <v>361</v>
+        <v>362</v>
       </c>
     </row>
     <row r="71" spans="1:12">
@@ -8671,7 +8671,7 @@
         <v>378</v>
       </c>
       <c r="L71">
-        <v>182</v>
+        <v>183</v>
       </c>
     </row>
     <row r="72" spans="1:12">
@@ -8747,7 +8747,7 @@
         <v>1505</v>
       </c>
       <c r="L73">
-        <v>664</v>
+        <v>668</v>
       </c>
     </row>
     <row r="74" spans="1:12">
@@ -8785,7 +8785,7 @@
         <v>360</v>
       </c>
       <c r="L74">
-        <v>176</v>
+        <v>177</v>
       </c>
     </row>
     <row r="75" spans="1:12">
@@ -8823,7 +8823,7 @@
         <v>490</v>
       </c>
       <c r="L75">
-        <v>239</v>
+        <v>240</v>
       </c>
     </row>
     <row r="76" spans="1:12">
@@ -8861,7 +8861,7 @@
         <v>3058</v>
       </c>
       <c r="L76">
-        <v>1567</v>
+        <v>1579</v>
       </c>
     </row>
     <row r="77" spans="1:12">
@@ -8937,7 +8937,7 @@
         <v>1940</v>
       </c>
       <c r="L78">
-        <v>827</v>
+        <v>830</v>
       </c>
     </row>
     <row r="79" spans="1:12">
@@ -8975,7 +8975,7 @@
         <v>2264</v>
       </c>
       <c r="L79">
-        <v>1067</v>
+        <v>1070</v>
       </c>
     </row>
     <row r="80" spans="1:12">
@@ -9013,7 +9013,7 @@
         <v>478</v>
       </c>
       <c r="L80">
-        <v>248</v>
+        <v>250</v>
       </c>
     </row>
     <row r="81" spans="1:12">
@@ -9127,7 +9127,7 @@
         <v>1627</v>
       </c>
       <c r="L83">
-        <v>792</v>
+        <v>796</v>
       </c>
     </row>
     <row r="84" spans="1:12">
@@ -9165,7 +9165,7 @@
         <v>876</v>
       </c>
       <c r="L84">
-        <v>423</v>
+        <v>424</v>
       </c>
     </row>
     <row r="85" spans="1:12">
@@ -9203,7 +9203,7 @@
         <v>3838</v>
       </c>
       <c r="L85">
-        <v>1779</v>
+        <v>1794</v>
       </c>
     </row>
     <row r="86" spans="1:12">
@@ -9241,7 +9241,7 @@
         <v>1009</v>
       </c>
       <c r="L86">
-        <v>456</v>
+        <v>458</v>
       </c>
     </row>
     <row r="87" spans="1:12">
@@ -9317,7 +9317,7 @@
         <v>1020</v>
       </c>
       <c r="L88">
-        <v>442</v>
+        <v>445</v>
       </c>
     </row>
     <row r="89" spans="1:12">
@@ -9355,7 +9355,7 @@
         <v>2322</v>
       </c>
       <c r="L89">
-        <v>1065</v>
+        <v>1075</v>
       </c>
     </row>
     <row r="90" spans="1:12">
@@ -9393,7 +9393,7 @@
         <v>1145</v>
       </c>
       <c r="L90">
-        <v>539</v>
+        <v>541</v>
       </c>
     </row>
     <row r="91" spans="1:12">
@@ -9431,7 +9431,7 @@
         <v>1048</v>
       </c>
       <c r="L91">
-        <v>510</v>
+        <v>518</v>
       </c>
     </row>
     <row r="92" spans="1:12">
@@ -9469,7 +9469,7 @@
         <v>402</v>
       </c>
       <c r="L92">
-        <v>177</v>
+        <v>178</v>
       </c>
     </row>
     <row r="93" spans="1:12">
@@ -9545,7 +9545,7 @@
         <v>3002</v>
       </c>
       <c r="L94">
-        <v>1328</v>
+        <v>1335</v>
       </c>
     </row>
     <row r="95" spans="1:12">
@@ -9583,7 +9583,7 @@
         <v>1445</v>
       </c>
       <c r="L95">
-        <v>622</v>
+        <v>625</v>
       </c>
     </row>
     <row r="96" spans="1:12">
@@ -9621,7 +9621,7 @@
         <v>1635</v>
       </c>
       <c r="L96">
-        <v>621</v>
+        <v>625</v>
       </c>
     </row>
     <row r="97" spans="1:12">
@@ -9659,7 +9659,7 @@
         <v>1818</v>
       </c>
       <c r="L97">
-        <v>917</v>
+        <v>919</v>
       </c>
     </row>
     <row r="98" spans="1:12">
@@ -9697,7 +9697,7 @@
         <v>1500</v>
       </c>
       <c r="L98">
-        <v>591</v>
+        <v>595</v>
       </c>
     </row>
     <row r="99" spans="1:12">
@@ -9735,7 +9735,7 @@
         <v>1588</v>
       </c>
       <c r="L99">
-        <v>715</v>
+        <v>719</v>
       </c>
     </row>
     <row r="100" spans="1:12">
@@ -9773,7 +9773,7 @@
         <v>347</v>
       </c>
       <c r="L100">
-        <v>148</v>
+        <v>149</v>
       </c>
     </row>
     <row r="101" spans="1:12">
@@ -9793,7 +9793,7 @@
         <v>113451</v>
       </c>
       <c r="F101">
-        <v>105613</v>
+        <v>105614</v>
       </c>
       <c r="G101">
         <v>85387</v>
@@ -9808,10 +9808,10 @@
         <v>124084</v>
       </c>
       <c r="K101">
-        <v>118649</v>
+        <v>118648</v>
       </c>
       <c r="L101">
-        <v>53337</v>
+        <v>53640</v>
       </c>
     </row>
   </sheetData>
@@ -10016,7 +10016,7 @@
         <v>35</v>
       </c>
       <c r="L2">
-        <v>19</v>
+        <v>20</v>
       </c>
     </row>
     <row r="3" spans="1:12">
@@ -10337,7 +10337,7 @@
         <v>490</v>
       </c>
       <c r="L11">
-        <v>239</v>
+        <v>240</v>
       </c>
     </row>
   </sheetData>
@@ -10670,7 +10670,7 @@
         <v>11</v>
       </c>
       <c r="L9">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="10" spans="1:12">
@@ -10746,7 +10746,7 @@
         <v>352</v>
       </c>
       <c r="L11">
-        <v>197</v>
+        <v>198</v>
       </c>
     </row>
   </sheetData>
@@ -11141,7 +11141,7 @@
         <v>653</v>
       </c>
       <c r="L10">
-        <v>257</v>
+        <v>259</v>
       </c>
     </row>
     <row r="11" spans="1:12">
@@ -11179,7 +11179,7 @@
         <v>1133</v>
       </c>
       <c r="L11">
-        <v>469</v>
+        <v>471</v>
       </c>
     </row>
   </sheetData>
@@ -11320,7 +11320,7 @@
         <v>154</v>
       </c>
       <c r="L3">
-        <v>51</v>
+        <v>52</v>
       </c>
     </row>
     <row r="4" spans="1:12">
@@ -11510,7 +11510,7 @@
         <v>320</v>
       </c>
       <c r="L8">
-        <v>140</v>
+        <v>141</v>
       </c>
     </row>
     <row r="9" spans="1:12">
@@ -11586,7 +11586,7 @@
         <v>545</v>
       </c>
       <c r="L10">
-        <v>243</v>
+        <v>244</v>
       </c>
     </row>
     <row r="11" spans="1:12">
@@ -11624,7 +11624,7 @@
         <v>1445</v>
       </c>
       <c r="L11">
-        <v>622</v>
+        <v>625</v>
       </c>
     </row>
   </sheetData>
@@ -11765,7 +11765,7 @@
         <v>304</v>
       </c>
       <c r="L3">
-        <v>129</v>
+        <v>131</v>
       </c>
     </row>
     <row r="4" spans="1:12">
@@ -11841,7 +11841,7 @@
         <v>230</v>
       </c>
       <c r="L5">
-        <v>74</v>
+        <v>75</v>
       </c>
     </row>
     <row r="6" spans="1:12">
@@ -11955,7 +11955,7 @@
         <v>578</v>
       </c>
       <c r="L8">
-        <v>225</v>
+        <v>227</v>
       </c>
     </row>
     <row r="9" spans="1:12">
@@ -12031,7 +12031,7 @@
         <v>976</v>
       </c>
       <c r="L10">
-        <v>443</v>
+        <v>444</v>
       </c>
     </row>
     <row r="11" spans="1:12">
@@ -12069,7 +12069,7 @@
         <v>2715</v>
       </c>
       <c r="L11">
-        <v>1164</v>
+        <v>1170</v>
       </c>
     </row>
   </sheetData>
@@ -12438,7 +12438,7 @@
         <v>236</v>
       </c>
       <c r="L9">
-        <v>64</v>
+        <v>65</v>
       </c>
     </row>
     <row r="10" spans="1:12">
@@ -12476,7 +12476,7 @@
         <v>637</v>
       </c>
       <c r="L10">
-        <v>327</v>
+        <v>328</v>
       </c>
     </row>
     <row r="11" spans="1:12">
@@ -12514,7 +12514,7 @@
         <v>1683</v>
       </c>
       <c r="L11">
-        <v>733</v>
+        <v>735</v>
       </c>
     </row>
   </sheetData>
@@ -13088,7 +13088,7 @@
         <v>194</v>
       </c>
       <c r="L3">
-        <v>77</v>
+        <v>78</v>
       </c>
     </row>
     <row r="4" spans="1:12">
@@ -13278,7 +13278,7 @@
         <v>311</v>
       </c>
       <c r="L8">
-        <v>128</v>
+        <v>130</v>
       </c>
     </row>
     <row r="9" spans="1:12">
@@ -13354,7 +13354,7 @@
         <v>687</v>
       </c>
       <c r="L10">
-        <v>342</v>
+        <v>343</v>
       </c>
     </row>
     <row r="11" spans="1:12">
@@ -13392,7 +13392,7 @@
         <v>1588</v>
       </c>
       <c r="L11">
-        <v>715</v>
+        <v>719</v>
       </c>
     </row>
   </sheetData>
@@ -14232,7 +14232,7 @@
         <v>439</v>
       </c>
       <c r="L10">
-        <v>258</v>
+        <v>261</v>
       </c>
     </row>
     <row r="11" spans="1:12">
@@ -14270,7 +14270,7 @@
         <v>1039</v>
       </c>
       <c r="L11">
-        <v>480</v>
+        <v>483</v>
       </c>
     </row>
   </sheetData>
@@ -14484,7 +14484,7 @@
         <v>77</v>
       </c>
       <c r="L5">
-        <v>31</v>
+        <v>32</v>
       </c>
     </row>
     <row r="6" spans="1:12">
@@ -14668,7 +14668,7 @@
         <v>369</v>
       </c>
       <c r="L10">
-        <v>204</v>
+        <v>206</v>
       </c>
     </row>
     <row r="11" spans="1:12">
@@ -14706,7 +14706,7 @@
         <v>720</v>
       </c>
       <c r="L11">
-        <v>352</v>
+        <v>355</v>
       </c>
     </row>
   </sheetData>
@@ -14847,7 +14847,7 @@
         <v>380</v>
       </c>
       <c r="L3">
-        <v>155</v>
+        <v>156</v>
       </c>
     </row>
     <row r="4" spans="1:12">
@@ -15037,7 +15037,7 @@
         <v>409</v>
       </c>
       <c r="L8">
-        <v>161</v>
+        <v>162</v>
       </c>
     </row>
     <row r="9" spans="1:12">
@@ -15075,7 +15075,7 @@
         <v>305</v>
       </c>
       <c r="L9">
-        <v>95</v>
+        <v>96</v>
       </c>
     </row>
     <row r="10" spans="1:12">
@@ -15151,7 +15151,7 @@
         <v>2435</v>
       </c>
       <c r="L11">
-        <v>1002</v>
+        <v>1005</v>
       </c>
     </row>
   </sheetData>
@@ -15558,7 +15558,7 @@
         <v>412</v>
       </c>
       <c r="L10">
-        <v>199</v>
+        <v>200</v>
       </c>
     </row>
     <row r="11" spans="1:12">
@@ -15596,7 +15596,7 @@
         <v>876</v>
       </c>
       <c r="L11">
-        <v>423</v>
+        <v>424</v>
       </c>
     </row>
   </sheetData>
@@ -15912,7 +15912,7 @@
         <v>380</v>
       </c>
       <c r="L8">
-        <v>153</v>
+        <v>156</v>
       </c>
     </row>
     <row r="9" spans="1:12">
@@ -15988,7 +15988,7 @@
         <v>2124</v>
       </c>
       <c r="L10">
-        <v>977</v>
+        <v>981</v>
       </c>
     </row>
     <row r="11" spans="1:12">
@@ -16026,7 +16026,7 @@
         <v>3002</v>
       </c>
       <c r="L11">
-        <v>1328</v>
+        <v>1335</v>
       </c>
     </row>
   </sheetData>
@@ -16129,7 +16129,7 @@
         <v>82</v>
       </c>
       <c r="L2">
-        <v>31</v>
+        <v>32</v>
       </c>
     </row>
     <row r="3" spans="1:12">
@@ -16240,7 +16240,7 @@
         <v>121</v>
       </c>
       <c r="L5">
-        <v>33</v>
+        <v>34</v>
       </c>
     </row>
     <row r="6" spans="1:12">
@@ -16316,7 +16316,7 @@
         <v>3</v>
       </c>
       <c r="L7">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="8" spans="1:12">
@@ -16392,7 +16392,7 @@
         <v>188</v>
       </c>
       <c r="L9">
-        <v>77</v>
+        <v>79</v>
       </c>
     </row>
     <row r="10" spans="1:12">
@@ -16430,7 +16430,7 @@
         <v>2251</v>
       </c>
       <c r="L10">
-        <v>1268</v>
+        <v>1275</v>
       </c>
     </row>
     <row r="11" spans="1:12">
@@ -16468,7 +16468,7 @@
         <v>3058</v>
       </c>
       <c r="L11">
-        <v>1567</v>
+        <v>1579</v>
       </c>
     </row>
   </sheetData>
@@ -16992,7 +16992,7 @@
         <v>50</v>
       </c>
       <c r="L2">
-        <v>18</v>
+        <v>20</v>
       </c>
     </row>
     <row r="3" spans="1:12">
@@ -17293,7 +17293,7 @@
         <v>193</v>
       </c>
       <c r="L10">
-        <v>112</v>
+        <v>113</v>
       </c>
     </row>
     <row r="11" spans="1:12">
@@ -17331,7 +17331,7 @@
         <v>555</v>
       </c>
       <c r="L11">
-        <v>310</v>
+        <v>313</v>
       </c>
     </row>
   </sheetData>
@@ -17684,7 +17684,7 @@
         <v>230</v>
       </c>
       <c r="L10">
-        <v>111</v>
+        <v>112</v>
       </c>
     </row>
     <row r="11" spans="1:12">
@@ -17722,7 +17722,7 @@
         <v>347</v>
       </c>
       <c r="L11">
-        <v>148</v>
+        <v>149</v>
       </c>
     </row>
   </sheetData>
@@ -18093,7 +18093,7 @@
         <v>655</v>
       </c>
       <c r="L10">
-        <v>307</v>
+        <v>308</v>
       </c>
     </row>
     <row r="11" spans="1:12">
@@ -18131,7 +18131,7 @@
         <v>938</v>
       </c>
       <c r="L11">
-        <v>392</v>
+        <v>393</v>
       </c>
     </row>
   </sheetData>
@@ -18520,7 +18520,7 @@
         <v>1650</v>
       </c>
       <c r="L10">
-        <v>700</v>
+        <v>704</v>
       </c>
     </row>
     <row r="11" spans="1:12">
@@ -18558,7 +18558,7 @@
         <v>2189</v>
       </c>
       <c r="L11">
-        <v>901</v>
+        <v>905</v>
       </c>
     </row>
   </sheetData>
@@ -18959,7 +18959,7 @@
         <v>994</v>
       </c>
       <c r="L10">
-        <v>607</v>
+        <v>609</v>
       </c>
     </row>
     <row r="11" spans="1:12">
@@ -18997,7 +18997,7 @@
         <v>1818</v>
       </c>
       <c r="L11">
-        <v>917</v>
+        <v>919</v>
       </c>
     </row>
   </sheetData>
@@ -19138,7 +19138,7 @@
         <v>64</v>
       </c>
       <c r="L3">
-        <v>30</v>
+        <v>31</v>
       </c>
     </row>
     <row r="4" spans="1:12">
@@ -19211,7 +19211,7 @@
         <v>110</v>
       </c>
       <c r="L5">
-        <v>43</v>
+        <v>44</v>
       </c>
     </row>
     <row r="6" spans="1:12">
@@ -19363,7 +19363,7 @@
         <v>119</v>
       </c>
       <c r="L9">
-        <v>27</v>
+        <v>28</v>
       </c>
     </row>
     <row r="10" spans="1:12">
@@ -19401,7 +19401,7 @@
         <v>830</v>
       </c>
       <c r="L10">
-        <v>348</v>
+        <v>349</v>
       </c>
     </row>
     <row r="11" spans="1:12">
@@ -19439,7 +19439,7 @@
         <v>1635</v>
       </c>
       <c r="L11">
-        <v>621</v>
+        <v>625</v>
       </c>
     </row>
   </sheetData>
@@ -19770,7 +19770,7 @@
         <v>259</v>
       </c>
       <c r="L8">
-        <v>91</v>
+        <v>93</v>
       </c>
     </row>
     <row r="9" spans="1:12">
@@ -19884,7 +19884,7 @@
         <v>1291</v>
       </c>
       <c r="L11">
-        <v>535</v>
+        <v>537</v>
       </c>
     </row>
   </sheetData>
@@ -20250,7 +20250,7 @@
         <v>278</v>
       </c>
       <c r="L9">
-        <v>114</v>
+        <v>115</v>
       </c>
     </row>
     <row r="10" spans="1:12">
@@ -20288,7 +20288,7 @@
         <v>3090</v>
       </c>
       <c r="L10">
-        <v>1529</v>
+        <v>1536</v>
       </c>
     </row>
     <row r="11" spans="1:12">
@@ -20326,7 +20326,7 @@
         <v>4179</v>
       </c>
       <c r="L11">
-        <v>1986</v>
+        <v>1994</v>
       </c>
     </row>
   </sheetData>
@@ -20467,7 +20467,7 @@
         <v>61</v>
       </c>
       <c r="L3">
-        <v>25</v>
+        <v>27</v>
       </c>
     </row>
     <row r="4" spans="1:12">
@@ -20733,7 +20733,7 @@
         <v>884</v>
       </c>
       <c r="L10">
-        <v>435</v>
+        <v>437</v>
       </c>
     </row>
     <row r="11" spans="1:12">
@@ -20771,7 +20771,7 @@
         <v>1505</v>
       </c>
       <c r="L11">
-        <v>664</v>
+        <v>668</v>
       </c>
     </row>
   </sheetData>
@@ -20874,7 +20874,7 @@
         <v>428</v>
       </c>
       <c r="L2">
-        <v>181</v>
+        <v>183</v>
       </c>
     </row>
     <row r="3" spans="1:12">
@@ -20988,7 +20988,7 @@
         <v>193</v>
       </c>
       <c r="L5">
-        <v>116</v>
+        <v>118</v>
       </c>
     </row>
     <row r="6" spans="1:12">
@@ -21102,7 +21102,7 @@
         <v>832</v>
       </c>
       <c r="L8">
-        <v>338</v>
+        <v>342</v>
       </c>
     </row>
     <row r="9" spans="1:12">
@@ -21178,7 +21178,7 @@
         <v>1294</v>
       </c>
       <c r="L10">
-        <v>641</v>
+        <v>643</v>
       </c>
     </row>
     <row r="11" spans="1:12">
@@ -21216,7 +21216,7 @@
         <v>3877</v>
       </c>
       <c r="L11">
-        <v>1724</v>
+        <v>1734</v>
       </c>
     </row>
   </sheetData>
@@ -21427,7 +21427,7 @@
         <v>233</v>
       </c>
       <c r="L5">
-        <v>121</v>
+        <v>122</v>
       </c>
     </row>
     <row r="6" spans="1:12">
@@ -21532,7 +21532,7 @@
         <v>377</v>
       </c>
       <c r="L8">
-        <v>137</v>
+        <v>138</v>
       </c>
     </row>
     <row r="9" spans="1:12">
@@ -21570,7 +21570,7 @@
         <v>158</v>
       </c>
       <c r="L9">
-        <v>70</v>
+        <v>73</v>
       </c>
     </row>
     <row r="10" spans="1:12">
@@ -21608,7 +21608,7 @@
         <v>2258</v>
       </c>
       <c r="L10">
-        <v>1029</v>
+        <v>1033</v>
       </c>
     </row>
     <row r="11" spans="1:12">
@@ -21646,7 +21646,7 @@
         <v>3217</v>
       </c>
       <c r="L11">
-        <v>1448</v>
+        <v>1457</v>
       </c>
     </row>
   </sheetData>
@@ -21977,7 +21977,7 @@
         <v>510</v>
       </c>
       <c r="L8">
-        <v>220</v>
+        <v>222</v>
       </c>
     </row>
     <row r="9" spans="1:12">
@@ -22053,7 +22053,7 @@
         <v>1013</v>
       </c>
       <c r="L10">
-        <v>652</v>
+        <v>656</v>
       </c>
     </row>
     <row r="11" spans="1:12">
@@ -22091,7 +22091,7 @@
         <v>2526</v>
       </c>
       <c r="L11">
-        <v>1301</v>
+        <v>1307</v>
       </c>
     </row>
   </sheetData>
@@ -22465,7 +22465,7 @@
         <v>420</v>
       </c>
       <c r="L10">
-        <v>179</v>
+        <v>180</v>
       </c>
     </row>
     <row r="11" spans="1:12">
@@ -22503,7 +22503,7 @@
         <v>722</v>
       </c>
       <c r="L11">
-        <v>278</v>
+        <v>279</v>
       </c>
     </row>
   </sheetData>
@@ -22828,7 +22828,7 @@
         <v>238</v>
       </c>
       <c r="L8">
-        <v>84</v>
+        <v>85</v>
       </c>
     </row>
     <row r="9" spans="1:12">
@@ -22942,7 +22942,7 @@
         <v>1296</v>
       </c>
       <c r="L11">
-        <v>507</v>
+        <v>508</v>
       </c>
     </row>
   </sheetData>
@@ -23045,7 +23045,7 @@
         <v>270</v>
       </c>
       <c r="L2">
-        <v>108</v>
+        <v>113</v>
       </c>
     </row>
     <row r="3" spans="1:12">
@@ -23311,7 +23311,7 @@
         <v>396</v>
       </c>
       <c r="L9">
-        <v>104</v>
+        <v>105</v>
       </c>
     </row>
     <row r="10" spans="1:12">
@@ -23349,7 +23349,7 @@
         <v>1252</v>
       </c>
       <c r="L10">
-        <v>602</v>
+        <v>607</v>
       </c>
     </row>
     <row r="11" spans="1:12">
@@ -23387,7 +23387,7 @@
         <v>3265</v>
       </c>
       <c r="L11">
-        <v>1244</v>
+        <v>1255</v>
       </c>
     </row>
   </sheetData>
@@ -23773,7 +23773,7 @@
         <v>182</v>
       </c>
       <c r="L10">
-        <v>100</v>
+        <v>103</v>
       </c>
     </row>
     <row r="11" spans="1:12">
@@ -23811,7 +23811,7 @@
         <v>441</v>
       </c>
       <c r="L11">
-        <v>198</v>
+        <v>201</v>
       </c>
     </row>
   </sheetData>
@@ -23952,7 +23952,7 @@
         <v>259</v>
       </c>
       <c r="L3">
-        <v>117</v>
+        <v>122</v>
       </c>
     </row>
     <row r="4" spans="1:12">
@@ -24028,7 +24028,7 @@
         <v>205</v>
       </c>
       <c r="L5">
-        <v>87</v>
+        <v>88</v>
       </c>
     </row>
     <row r="6" spans="1:12">
@@ -24218,7 +24218,7 @@
         <v>903</v>
       </c>
       <c r="L10">
-        <v>487</v>
+        <v>491</v>
       </c>
     </row>
     <row r="11" spans="1:12">
@@ -24256,7 +24256,7 @@
         <v>2524</v>
       </c>
       <c r="L11">
-        <v>1282</v>
+        <v>1292</v>
       </c>
     </row>
   </sheetData>
@@ -24581,7 +24581,7 @@
         <v>393</v>
       </c>
       <c r="L8">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="9" spans="1:12">
@@ -24619,7 +24619,7 @@
         <v>49</v>
       </c>
       <c r="L9">
-        <v>18</v>
+        <v>19</v>
       </c>
     </row>
     <row r="10" spans="1:12">
@@ -25462,7 +25462,7 @@
         <v>454</v>
       </c>
       <c r="L8">
-        <v>211</v>
+        <v>215</v>
       </c>
     </row>
     <row r="9" spans="1:12">
@@ -25538,7 +25538,7 @@
         <v>795</v>
       </c>
       <c r="L10">
-        <v>306</v>
+        <v>307</v>
       </c>
     </row>
     <row r="11" spans="1:12">
@@ -25576,7 +25576,7 @@
         <v>1711</v>
       </c>
       <c r="L11">
-        <v>710</v>
+        <v>715</v>
       </c>
     </row>
   </sheetData>
@@ -26363,7 +26363,7 @@
         <v>872</v>
       </c>
       <c r="L10">
-        <v>438</v>
+        <v>441</v>
       </c>
     </row>
     <row r="11" spans="1:12">
@@ -26401,7 +26401,7 @@
         <v>1286</v>
       </c>
       <c r="L11">
-        <v>604</v>
+        <v>607</v>
       </c>
     </row>
   </sheetData>
@@ -26772,7 +26772,7 @@
         <v>723</v>
       </c>
       <c r="L10">
-        <v>314</v>
+        <v>316</v>
       </c>
     </row>
     <row r="11" spans="1:12">
@@ -26810,7 +26810,7 @@
         <v>1009</v>
       </c>
       <c r="L11">
-        <v>456</v>
+        <v>458</v>
       </c>
     </row>
   </sheetData>
@@ -27027,7 +27027,7 @@
         <v>110</v>
       </c>
       <c r="L5">
-        <v>49</v>
+        <v>50</v>
       </c>
     </row>
     <row r="6" spans="1:12">
@@ -27179,7 +27179,7 @@
         <v>108</v>
       </c>
       <c r="L9">
-        <v>44</v>
+        <v>45</v>
       </c>
     </row>
     <row r="10" spans="1:12">
@@ -27217,7 +27217,7 @@
         <v>1139</v>
       </c>
       <c r="L10">
-        <v>508</v>
+        <v>509</v>
       </c>
     </row>
     <row r="11" spans="1:12">
@@ -27255,7 +27255,7 @@
         <v>1940</v>
       </c>
       <c r="L11">
-        <v>827</v>
+        <v>830</v>
       </c>
     </row>
   </sheetData>
@@ -27396,7 +27396,7 @@
         <v>16</v>
       </c>
       <c r="L3">
-        <v>12</v>
+        <v>13</v>
       </c>
     </row>
     <row r="4" spans="1:12">
@@ -27559,7 +27559,7 @@
         <v>73</v>
       </c>
       <c r="L8">
-        <v>28</v>
+        <v>29</v>
       </c>
     </row>
     <row r="9" spans="1:12">
@@ -27635,7 +27635,7 @@
         <v>316</v>
       </c>
       <c r="L10">
-        <v>180</v>
+        <v>181</v>
       </c>
     </row>
     <row r="11" spans="1:12">
@@ -27673,7 +27673,7 @@
         <v>497</v>
       </c>
       <c r="L11">
-        <v>269</v>
+        <v>272</v>
       </c>
     </row>
   </sheetData>
@@ -27989,7 +27989,7 @@
         <v>148</v>
       </c>
       <c r="L8">
-        <v>47</v>
+        <v>48</v>
       </c>
     </row>
     <row r="9" spans="1:12">
@@ -28065,7 +28065,7 @@
         <v>377</v>
       </c>
       <c r="L10">
-        <v>150</v>
+        <v>151</v>
       </c>
     </row>
     <row r="11" spans="1:12">
@@ -28103,7 +28103,7 @@
         <v>675</v>
       </c>
       <c r="L11">
-        <v>249</v>
+        <v>251</v>
       </c>
     </row>
   </sheetData>
@@ -28765,7 +28765,7 @@
         <v>112</v>
       </c>
       <c r="L5">
-        <v>46</v>
+        <v>47</v>
       </c>
     </row>
     <row r="6" spans="1:12">
@@ -28879,7 +28879,7 @@
         <v>365</v>
       </c>
       <c r="L8">
-        <v>113</v>
+        <v>114</v>
       </c>
     </row>
     <row r="9" spans="1:12">
@@ -28955,7 +28955,7 @@
         <v>1153</v>
       </c>
       <c r="L10">
-        <v>529</v>
+        <v>530</v>
       </c>
     </row>
     <row r="11" spans="1:12">
@@ -28993,7 +28993,7 @@
         <v>2119</v>
       </c>
       <c r="L11">
-        <v>882</v>
+        <v>885</v>
       </c>
     </row>
   </sheetData>
@@ -29318,7 +29318,7 @@
         <v>280</v>
       </c>
       <c r="L8">
-        <v>154</v>
+        <v>155</v>
       </c>
     </row>
     <row r="9" spans="1:12">
@@ -29394,7 +29394,7 @@
         <v>725</v>
       </c>
       <c r="L10">
-        <v>341</v>
+        <v>342</v>
       </c>
     </row>
     <row r="11" spans="1:12">
@@ -29432,7 +29432,7 @@
         <v>1330</v>
       </c>
       <c r="L11">
-        <v>640</v>
+        <v>642</v>
       </c>
     </row>
   </sheetData>
@@ -29763,7 +29763,7 @@
         <v>284</v>
       </c>
       <c r="L8">
-        <v>138</v>
+        <v>144</v>
       </c>
     </row>
     <row r="9" spans="1:12">
@@ -29839,7 +29839,7 @@
         <v>388</v>
       </c>
       <c r="L10">
-        <v>188</v>
+        <v>190</v>
       </c>
     </row>
     <row r="11" spans="1:12">
@@ -29877,7 +29877,7 @@
         <v>1048</v>
       </c>
       <c r="L11">
-        <v>510</v>
+        <v>518</v>
       </c>
     </row>
   </sheetData>
@@ -30205,7 +30205,7 @@
         <v>308</v>
       </c>
       <c r="L8">
-        <v>157</v>
+        <v>160</v>
       </c>
     </row>
     <row r="9" spans="1:12">
@@ -30281,7 +30281,7 @@
         <v>763</v>
       </c>
       <c r="L10">
-        <v>431</v>
+        <v>433</v>
       </c>
     </row>
     <row r="11" spans="1:12">
@@ -30319,7 +30319,7 @@
         <v>1492</v>
       </c>
       <c r="L11">
-        <v>763</v>
+        <v>768</v>
       </c>
     </row>
   </sheetData>
@@ -30460,7 +30460,7 @@
         <v>209</v>
       </c>
       <c r="L3">
-        <v>92</v>
+        <v>93</v>
       </c>
     </row>
     <row r="4" spans="1:12">
@@ -30688,7 +30688,7 @@
         <v>193</v>
       </c>
       <c r="L9">
-        <v>78</v>
+        <v>79</v>
       </c>
     </row>
     <row r="10" spans="1:12">
@@ -30764,7 +30764,7 @@
         <v>1973</v>
       </c>
       <c r="L11">
-        <v>942</v>
+        <v>944</v>
       </c>
     </row>
   </sheetData>
@@ -31123,7 +31123,7 @@
         <v>165</v>
       </c>
       <c r="L10">
-        <v>76</v>
+        <v>77</v>
       </c>
     </row>
     <row r="11" spans="1:12">
@@ -31161,7 +31161,7 @@
         <v>321</v>
       </c>
       <c r="L11">
-        <v>127</v>
+        <v>128</v>
       </c>
     </row>
   </sheetData>
@@ -31302,7 +31302,7 @@
         <v>59</v>
       </c>
       <c r="L3">
-        <v>29</v>
+        <v>30</v>
       </c>
     </row>
     <row r="4" spans="1:12">
@@ -31410,7 +31410,7 @@
         <v>18</v>
       </c>
       <c r="L6">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="7" spans="1:12">
@@ -31480,7 +31480,7 @@
         <v>280</v>
       </c>
       <c r="L8">
-        <v>95</v>
+        <v>96</v>
       </c>
     </row>
     <row r="9" spans="1:12">
@@ -31594,7 +31594,7 @@
         <v>1046</v>
       </c>
       <c r="L11">
-        <v>463</v>
+        <v>466</v>
       </c>
     </row>
   </sheetData>
@@ -31735,7 +31735,7 @@
         <v>69</v>
       </c>
       <c r="L3">
-        <v>32</v>
+        <v>33</v>
       </c>
     </row>
     <row r="4" spans="1:12">
@@ -31922,7 +31922,7 @@
         <v>305</v>
       </c>
       <c r="L8">
-        <v>139</v>
+        <v>140</v>
       </c>
     </row>
     <row r="9" spans="1:12">
@@ -32036,7 +32036,7 @@
         <v>1145</v>
       </c>
       <c r="L11">
-        <v>539</v>
+        <v>541</v>
       </c>
     </row>
   </sheetData>
@@ -32393,7 +32393,7 @@
         <v>54</v>
       </c>
       <c r="L9">
-        <v>12</v>
+        <v>13</v>
       </c>
     </row>
     <row r="10" spans="1:12">
@@ -32431,7 +32431,7 @@
         <v>636</v>
       </c>
       <c r="L10">
-        <v>385</v>
+        <v>388</v>
       </c>
     </row>
     <row r="11" spans="1:12">
@@ -32469,7 +32469,7 @@
         <v>1038</v>
       </c>
       <c r="L11">
-        <v>524</v>
+        <v>528</v>
       </c>
     </row>
   </sheetData>
@@ -33312,7 +33312,7 @@
         <v>291</v>
       </c>
       <c r="L10">
-        <v>132</v>
+        <v>135</v>
       </c>
     </row>
     <row r="11" spans="1:12">
@@ -33350,7 +33350,7 @@
         <v>751</v>
       </c>
       <c r="L11">
-        <v>338</v>
+        <v>341</v>
       </c>
     </row>
   </sheetData>
@@ -33709,7 +33709,7 @@
         <v>502</v>
       </c>
       <c r="L10">
-        <v>288</v>
+        <v>289</v>
       </c>
     </row>
     <row r="11" spans="1:12">
@@ -33747,7 +33747,7 @@
         <v>686</v>
       </c>
       <c r="L11">
-        <v>361</v>
+        <v>362</v>
       </c>
     </row>
   </sheetData>
@@ -34542,7 +34542,7 @@
         <v>669</v>
       </c>
       <c r="L10">
-        <v>276</v>
+        <v>279</v>
       </c>
     </row>
     <row r="11" spans="1:12">
@@ -34580,7 +34580,7 @@
         <v>718</v>
       </c>
       <c r="L11">
-        <v>289</v>
+        <v>292</v>
       </c>
     </row>
   </sheetData>
@@ -34960,7 +34960,7 @@
         <v>118</v>
       </c>
       <c r="L10">
-        <v>64</v>
+        <v>65</v>
       </c>
     </row>
     <row r="11" spans="1:12">
@@ -34998,7 +34998,7 @@
         <v>251</v>
       </c>
       <c r="L11">
-        <v>144</v>
+        <v>145</v>
       </c>
     </row>
   </sheetData>
@@ -35139,7 +35139,7 @@
         <v>71</v>
       </c>
       <c r="L3">
-        <v>29</v>
+        <v>30</v>
       </c>
     </row>
     <row r="4" spans="1:12">
@@ -35443,7 +35443,7 @@
         <v>1104</v>
       </c>
       <c r="L11">
-        <v>481</v>
+        <v>482</v>
       </c>
     </row>
   </sheetData>
@@ -36168,7 +36168,7 @@
         <v>215</v>
       </c>
       <c r="L8">
-        <v>89</v>
+        <v>90</v>
       </c>
     </row>
     <row r="9" spans="1:12">
@@ -36244,7 +36244,7 @@
         <v>807</v>
       </c>
       <c r="L10">
-        <v>590</v>
+        <v>593</v>
       </c>
     </row>
     <row r="11" spans="1:12">
@@ -36282,7 +36282,7 @@
         <v>1329</v>
       </c>
       <c r="L11">
-        <v>803</v>
+        <v>807</v>
       </c>
     </row>
   </sheetData>
@@ -36662,7 +36662,7 @@
         <v>37</v>
       </c>
       <c r="L10">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="11" spans="1:12">
@@ -36700,7 +36700,7 @@
         <v>140</v>
       </c>
       <c r="L11">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
   </sheetData>
@@ -37013,7 +37013,7 @@
         <v>113</v>
       </c>
       <c r="L8">
-        <v>35</v>
+        <v>37</v>
       </c>
     </row>
     <row r="9" spans="1:12">
@@ -37089,7 +37089,7 @@
         <v>354</v>
       </c>
       <c r="L10">
-        <v>201</v>
+        <v>203</v>
       </c>
     </row>
     <row r="11" spans="1:12">
@@ -37127,7 +37127,7 @@
         <v>616</v>
       </c>
       <c r="L11">
-        <v>302</v>
+        <v>306</v>
       </c>
     </row>
   </sheetData>
@@ -37448,7 +37448,7 @@
         <v>52</v>
       </c>
       <c r="L9">
-        <v>17</v>
+        <v>19</v>
       </c>
     </row>
     <row r="10" spans="1:12">
@@ -37524,7 +37524,7 @@
         <v>478</v>
       </c>
       <c r="L11">
-        <v>248</v>
+        <v>250</v>
       </c>
     </row>
   </sheetData>
@@ -37887,7 +37887,7 @@
         <v>44</v>
       </c>
       <c r="L9">
-        <v>26</v>
+        <v>27</v>
       </c>
     </row>
     <row r="10" spans="1:12">
@@ -37963,7 +37963,7 @@
         <v>973</v>
       </c>
       <c r="L11">
-        <v>368</v>
+        <v>369</v>
       </c>
     </row>
   </sheetData>
@@ -38142,7 +38142,7 @@
         <v>2</v>
       </c>
       <c r="L4">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="5" spans="1:12">
@@ -38218,7 +38218,7 @@
         <v>49</v>
       </c>
       <c r="L6">
-        <v>28</v>
+        <v>29</v>
       </c>
     </row>
     <row r="7" spans="1:12">
@@ -38288,7 +38288,7 @@
         <v>259</v>
       </c>
       <c r="L8">
-        <v>87</v>
+        <v>90</v>
       </c>
     </row>
     <row r="9" spans="1:12">
@@ -38364,7 +38364,7 @@
         <v>1482</v>
       </c>
       <c r="L10">
-        <v>741</v>
+        <v>746</v>
       </c>
     </row>
     <row r="11" spans="1:12">
@@ -38402,7 +38402,7 @@
         <v>2322</v>
       </c>
       <c r="L11">
-        <v>1065</v>
+        <v>1075</v>
       </c>
     </row>
   </sheetData>
@@ -38752,7 +38752,7 @@
         <v>256</v>
       </c>
       <c r="L10">
-        <v>147</v>
+        <v>148</v>
       </c>
     </row>
     <row r="11" spans="1:12">
@@ -38790,7 +38790,7 @@
         <v>337</v>
       </c>
       <c r="L11">
-        <v>183</v>
+        <v>184</v>
       </c>
     </row>
   </sheetData>
@@ -39062,7 +39062,7 @@
         <v>25</v>
       </c>
       <c r="L7">
-        <v>7</v>
+        <v>10</v>
       </c>
     </row>
     <row r="8" spans="1:12">
@@ -39176,7 +39176,7 @@
         <v>170</v>
       </c>
       <c r="L10">
-        <v>63</v>
+        <v>66</v>
       </c>
     </row>
   </sheetData>
@@ -39896,7 +39896,7 @@
         <v>167</v>
       </c>
       <c r="L10">
-        <v>44</v>
+        <v>45</v>
       </c>
     </row>
     <row r="11" spans="1:12">
@@ -39934,7 +39934,7 @@
         <v>202</v>
       </c>
       <c r="L11">
-        <v>50</v>
+        <v>51</v>
       </c>
     </row>
   </sheetData>
@@ -40244,7 +40244,7 @@
         <v>265</v>
       </c>
       <c r="L8">
-        <v>77</v>
+        <v>78</v>
       </c>
     </row>
     <row r="9" spans="1:12">
@@ -40320,7 +40320,7 @@
         <v>962</v>
       </c>
       <c r="L10">
-        <v>410</v>
+        <v>413</v>
       </c>
     </row>
     <row r="11" spans="1:12">
@@ -40358,7 +40358,7 @@
         <v>1500</v>
       </c>
       <c r="L11">
-        <v>591</v>
+        <v>595</v>
       </c>
     </row>
   </sheetData>
@@ -41141,7 +41141,7 @@
         <v>159</v>
       </c>
       <c r="L10">
-        <v>88</v>
+        <v>89</v>
       </c>
     </row>
     <row r="11" spans="1:12">
@@ -41179,7 +41179,7 @@
         <v>402</v>
       </c>
       <c r="L11">
-        <v>177</v>
+        <v>178</v>
       </c>
     </row>
   </sheetData>
@@ -41532,7 +41532,7 @@
         <v>112</v>
       </c>
       <c r="L10">
-        <v>37</v>
+        <v>38</v>
       </c>
     </row>
     <row r="11" spans="1:12">
@@ -41570,7 +41570,7 @@
         <v>167</v>
       </c>
       <c r="L11">
-        <v>66</v>
+        <v>67</v>
       </c>
     </row>
   </sheetData>
@@ -42371,7 +42371,7 @@
         <v>192</v>
       </c>
       <c r="L10">
-        <v>77</v>
+        <v>78</v>
       </c>
     </row>
     <row r="11" spans="1:12">
@@ -42409,7 +42409,7 @@
         <v>484</v>
       </c>
       <c r="L11">
-        <v>222</v>
+        <v>223</v>
       </c>
     </row>
   </sheetData>
@@ -42550,7 +42550,7 @@
         <v>438</v>
       </c>
       <c r="L3">
-        <v>240</v>
+        <v>245</v>
       </c>
     </row>
     <row r="4" spans="1:12">
@@ -42626,7 +42626,7 @@
         <v>426</v>
       </c>
       <c r="L5">
-        <v>158</v>
+        <v>160</v>
       </c>
     </row>
     <row r="6" spans="1:12">
@@ -42740,7 +42740,7 @@
         <v>635</v>
       </c>
       <c r="L8">
-        <v>322</v>
+        <v>326</v>
       </c>
     </row>
     <row r="9" spans="1:12">
@@ -42778,7 +42778,7 @@
         <v>315</v>
       </c>
       <c r="L9">
-        <v>123</v>
+        <v>124</v>
       </c>
     </row>
     <row r="10" spans="1:12">
@@ -42816,7 +42816,7 @@
         <v>1486</v>
       </c>
       <c r="L10">
-        <v>708</v>
+        <v>711</v>
       </c>
     </row>
     <row r="11" spans="1:12">
@@ -42854,7 +42854,7 @@
         <v>3838</v>
       </c>
       <c r="L11">
-        <v>1779</v>
+        <v>1794</v>
       </c>
     </row>
   </sheetData>
@@ -43234,7 +43234,7 @@
         <v>127</v>
       </c>
       <c r="L10">
-        <v>81</v>
+        <v>82</v>
       </c>
     </row>
     <row r="11" spans="1:12">
@@ -43272,7 +43272,7 @@
         <v>248</v>
       </c>
       <c r="L11">
-        <v>132</v>
+        <v>133</v>
       </c>
     </row>
   </sheetData>
@@ -43594,7 +43594,7 @@
         <v>125</v>
       </c>
       <c r="L8">
-        <v>65</v>
+        <v>66</v>
       </c>
     </row>
     <row r="9" spans="1:12">
@@ -43632,7 +43632,7 @@
         <v>194</v>
       </c>
       <c r="L9">
-        <v>80</v>
+        <v>81</v>
       </c>
     </row>
   </sheetData>
@@ -44390,7 +44390,7 @@
         <v>181</v>
       </c>
       <c r="L8">
-        <v>70</v>
+        <v>71</v>
       </c>
     </row>
     <row r="9" spans="1:12">
@@ -44466,7 +44466,7 @@
         <v>476</v>
       </c>
       <c r="L10">
-        <v>219</v>
+        <v>221</v>
       </c>
     </row>
     <row r="11" spans="1:12">
@@ -44504,7 +44504,7 @@
         <v>1020</v>
       </c>
       <c r="L11">
-        <v>442</v>
+        <v>445</v>
       </c>
     </row>
   </sheetData>
@@ -44854,7 +44854,7 @@
         <v>295</v>
       </c>
       <c r="L10">
-        <v>156</v>
+        <v>157</v>
       </c>
     </row>
     <row r="11" spans="1:12">
@@ -44892,7 +44892,7 @@
         <v>360</v>
       </c>
       <c r="L11">
-        <v>176</v>
+        <v>177</v>
       </c>
     </row>
   </sheetData>
@@ -45076,7 +45076,7 @@
         <v>26</v>
       </c>
       <c r="L5">
-        <v>14</v>
+        <v>15</v>
       </c>
     </row>
     <row r="6" spans="1:12">
@@ -45262,7 +45262,7 @@
         <v>263</v>
       </c>
       <c r="L11">
-        <v>143</v>
+        <v>144</v>
       </c>
     </row>
   </sheetData>
@@ -45825,7 +45825,7 @@
         <v>1</v>
       </c>
       <c r="L5">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="6" spans="1:12">
@@ -46009,7 +46009,7 @@
         <v>151</v>
       </c>
       <c r="L10">
-        <v>58</v>
+        <v>59</v>
       </c>
     </row>
   </sheetData>
@@ -46383,7 +46383,7 @@
         <v>405</v>
       </c>
       <c r="L10">
-        <v>135</v>
+        <v>138</v>
       </c>
     </row>
     <row r="11" spans="1:12">
@@ -46421,7 +46421,7 @@
         <v>559</v>
       </c>
       <c r="L11">
-        <v>214</v>
+        <v>217</v>
       </c>
     </row>
   </sheetData>
@@ -46762,7 +46762,7 @@
         <v>67</v>
       </c>
       <c r="L10">
-        <v>33</v>
+        <v>34</v>
       </c>
     </row>
     <row r="11" spans="1:12">
@@ -46800,7 +46800,7 @@
         <v>97</v>
       </c>
       <c r="L11">
-        <v>51</v>
+        <v>52</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add data for 2025-07-21
</commit_message>
<xml_diff>
--- a/output/index-crime-full-year.xlsx
+++ b/output/index-crime-full-year.xlsx
@@ -909,7 +909,7 @@
         <v>7903</v>
       </c>
       <c r="L2">
-        <v>3656</v>
+        <v>3689</v>
       </c>
     </row>
     <row r="3" spans="1:12">
@@ -947,7 +947,7 @@
         <v>8184</v>
       </c>
       <c r="L3">
-        <v>3825</v>
+        <v>3844</v>
       </c>
     </row>
     <row r="4" spans="1:12">
@@ -1023,7 +1023,7 @@
         <v>7651</v>
       </c>
       <c r="L5">
-        <v>3295</v>
+        <v>3314</v>
       </c>
     </row>
     <row r="6" spans="1:12">
@@ -1061,7 +1061,7 @@
         <v>1769</v>
       </c>
       <c r="L6">
-        <v>951</v>
+        <v>954</v>
       </c>
     </row>
     <row r="7" spans="1:12">
@@ -1099,7 +1099,7 @@
         <v>588</v>
       </c>
       <c r="L7">
-        <v>230</v>
+        <v>231</v>
       </c>
     </row>
     <row r="8" spans="1:12">
@@ -1137,7 +1137,7 @@
         <v>21704</v>
       </c>
       <c r="L8">
-        <v>8979</v>
+        <v>9041</v>
       </c>
     </row>
     <row r="9" spans="1:12">
@@ -1175,7 +1175,7 @@
         <v>9119</v>
       </c>
       <c r="L9">
-        <v>3333</v>
+        <v>3364</v>
       </c>
     </row>
     <row r="10" spans="1:12">
@@ -1213,7 +1213,7 @@
         <v>61254</v>
       </c>
       <c r="L10">
-        <v>31204</v>
+        <v>31391</v>
       </c>
     </row>
     <row r="11" spans="1:12">
@@ -1251,7 +1251,7 @@
         <v>118655</v>
       </c>
       <c r="L11">
-        <v>55687</v>
+        <v>56042</v>
       </c>
     </row>
   </sheetData>
@@ -1354,7 +1354,7 @@
         <v>191</v>
       </c>
       <c r="L2">
-        <v>83</v>
+        <v>84</v>
       </c>
     </row>
     <row r="3" spans="1:12">
@@ -1392,7 +1392,7 @@
         <v>194</v>
       </c>
       <c r="L3">
-        <v>74</v>
+        <v>76</v>
       </c>
     </row>
     <row r="4" spans="1:12">
@@ -1620,7 +1620,7 @@
         <v>248</v>
       </c>
       <c r="L9">
-        <v>63</v>
+        <v>64</v>
       </c>
     </row>
     <row r="10" spans="1:12">
@@ -1658,7 +1658,7 @@
         <v>849</v>
       </c>
       <c r="L10">
-        <v>357</v>
+        <v>360</v>
       </c>
     </row>
     <row r="11" spans="1:12">
@@ -1696,7 +1696,7 @@
         <v>1847</v>
       </c>
       <c r="L11">
-        <v>734</v>
+        <v>741</v>
       </c>
     </row>
   </sheetData>
@@ -1993,7 +1993,7 @@
         <v>54</v>
       </c>
       <c r="L9">
-        <v>21</v>
+        <v>22</v>
       </c>
     </row>
     <row r="10" spans="1:12">
@@ -2031,7 +2031,7 @@
         <v>76</v>
       </c>
       <c r="L10">
-        <v>31</v>
+        <v>32</v>
       </c>
     </row>
   </sheetData>
@@ -2134,7 +2134,7 @@
         <v>19</v>
       </c>
       <c r="L2">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="3" spans="1:12">
@@ -2242,7 +2242,7 @@
         <v>59</v>
       </c>
       <c r="L5">
-        <v>17</v>
+        <v>18</v>
       </c>
     </row>
     <row r="6" spans="1:12">
@@ -2452,7 +2452,7 @@
         <v>539</v>
       </c>
       <c r="L11">
-        <v>264</v>
+        <v>266</v>
       </c>
     </row>
   </sheetData>
@@ -2783,7 +2783,7 @@
         <v>388</v>
       </c>
       <c r="L8">
-        <v>130</v>
+        <v>131</v>
       </c>
     </row>
     <row r="9" spans="1:12">
@@ -2821,7 +2821,7 @@
         <v>144</v>
       </c>
       <c r="L9">
-        <v>46</v>
+        <v>47</v>
       </c>
     </row>
     <row r="10" spans="1:12">
@@ -2859,7 +2859,7 @@
         <v>1473</v>
       </c>
       <c r="L10">
-        <v>622</v>
+        <v>626</v>
       </c>
     </row>
     <row r="11" spans="1:12">
@@ -2897,7 +2897,7 @@
         <v>2353</v>
       </c>
       <c r="L11">
-        <v>946</v>
+        <v>952</v>
       </c>
     </row>
   </sheetData>
@@ -3000,7 +3000,7 @@
         <v>492</v>
       </c>
       <c r="L2">
-        <v>224</v>
+        <v>228</v>
       </c>
     </row>
     <row r="3" spans="1:12">
@@ -3038,7 +3038,7 @@
         <v>543</v>
       </c>
       <c r="L3">
-        <v>258</v>
+        <v>260</v>
       </c>
     </row>
     <row r="4" spans="1:12">
@@ -3228,7 +3228,7 @@
         <v>931</v>
       </c>
       <c r="L8">
-        <v>389</v>
+        <v>392</v>
       </c>
     </row>
     <row r="9" spans="1:12">
@@ -3266,7 +3266,7 @@
         <v>610</v>
       </c>
       <c r="L9">
-        <v>211</v>
+        <v>214</v>
       </c>
     </row>
     <row r="10" spans="1:12">
@@ -3304,7 +3304,7 @@
         <v>1965</v>
       </c>
       <c r="L10">
-        <v>1181</v>
+        <v>1183</v>
       </c>
     </row>
     <row r="11" spans="1:12">
@@ -3342,7 +3342,7 @@
         <v>4977</v>
       </c>
       <c r="L11">
-        <v>2494</v>
+        <v>2508</v>
       </c>
     </row>
   </sheetData>
@@ -3860,7 +3860,7 @@
         <v>56</v>
       </c>
       <c r="L2">
-        <v>21</v>
+        <v>23</v>
       </c>
     </row>
     <row r="3" spans="1:12">
@@ -4082,7 +4082,7 @@
         <v>190</v>
       </c>
       <c r="L8">
-        <v>63</v>
+        <v>64</v>
       </c>
     </row>
     <row r="9" spans="1:12">
@@ -4196,7 +4196,7 @@
         <v>784</v>
       </c>
       <c r="L11">
-        <v>374</v>
+        <v>377</v>
       </c>
     </row>
   </sheetData>
@@ -4299,7 +4299,7 @@
         <v>27</v>
       </c>
       <c r="L2">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="3" spans="1:12">
@@ -4614,7 +4614,7 @@
         <v>378</v>
       </c>
       <c r="L11">
-        <v>190</v>
+        <v>191</v>
       </c>
     </row>
   </sheetData>
@@ -4945,7 +4945,7 @@
         <v>331</v>
       </c>
       <c r="L8">
-        <v>224</v>
+        <v>228</v>
       </c>
     </row>
     <row r="9" spans="1:12">
@@ -5021,7 +5021,7 @@
         <v>576</v>
       </c>
       <c r="L10">
-        <v>243</v>
+        <v>244</v>
       </c>
     </row>
     <row r="11" spans="1:12">
@@ -5059,7 +5059,7 @@
         <v>1627</v>
       </c>
       <c r="L11">
-        <v>822</v>
+        <v>827</v>
       </c>
     </row>
   </sheetData>
@@ -5200,7 +5200,7 @@
         <v>406</v>
       </c>
       <c r="L3">
-        <v>182</v>
+        <v>183</v>
       </c>
     </row>
     <row r="4" spans="1:12">
@@ -5466,7 +5466,7 @@
         <v>929</v>
       </c>
       <c r="L10">
-        <v>437</v>
+        <v>438</v>
       </c>
     </row>
     <row r="11" spans="1:12">
@@ -5504,7 +5504,7 @@
         <v>2788</v>
       </c>
       <c r="L11">
-        <v>1320</v>
+        <v>1322</v>
       </c>
     </row>
   </sheetData>
@@ -5607,7 +5607,7 @@
         <v>218</v>
       </c>
       <c r="L2">
-        <v>108</v>
+        <v>110</v>
       </c>
     </row>
     <row r="3" spans="1:12">
@@ -5721,7 +5721,7 @@
         <v>156</v>
       </c>
       <c r="L5">
-        <v>70</v>
+        <v>71</v>
       </c>
     </row>
     <row r="6" spans="1:12">
@@ -5759,7 +5759,7 @@
         <v>43</v>
       </c>
       <c r="L6">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="7" spans="1:12">
@@ -5835,7 +5835,7 @@
         <v>551</v>
       </c>
       <c r="L8">
-        <v>251</v>
+        <v>252</v>
       </c>
     </row>
     <row r="9" spans="1:12">
@@ -5949,7 +5949,7 @@
         <v>2264</v>
       </c>
       <c r="L11">
-        <v>1113</v>
+        <v>1116</v>
       </c>
     </row>
   </sheetData>
@@ -6052,7 +6052,7 @@
         <v>1104</v>
       </c>
       <c r="L2">
-        <v>502</v>
+        <v>507</v>
       </c>
     </row>
     <row r="3" spans="1:12">
@@ -6090,7 +6090,7 @@
         <v>263</v>
       </c>
       <c r="L3">
-        <v>150</v>
+        <v>151</v>
       </c>
     </row>
     <row r="4" spans="1:12">
@@ -6128,7 +6128,7 @@
         <v>616</v>
       </c>
       <c r="L4">
-        <v>321</v>
+        <v>323</v>
       </c>
     </row>
     <row r="5" spans="1:12">
@@ -6204,7 +6204,7 @@
         <v>1111</v>
       </c>
       <c r="L6">
-        <v>406</v>
+        <v>413</v>
       </c>
     </row>
     <row r="7" spans="1:12">
@@ -6242,7 +6242,7 @@
         <v>2524</v>
       </c>
       <c r="L7">
-        <v>1343</v>
+        <v>1355</v>
       </c>
     </row>
     <row r="8" spans="1:12">
@@ -6280,7 +6280,7 @@
         <v>4977</v>
       </c>
       <c r="L8">
-        <v>2494</v>
+        <v>2508</v>
       </c>
     </row>
     <row r="9" spans="1:12">
@@ -6318,7 +6318,7 @@
         <v>484</v>
       </c>
       <c r="L9">
-        <v>230</v>
+        <v>231</v>
       </c>
     </row>
     <row r="10" spans="1:12">
@@ -6356,7 +6356,7 @@
         <v>1286</v>
       </c>
       <c r="L10">
-        <v>623</v>
+        <v>626</v>
       </c>
     </row>
     <row r="11" spans="1:12">
@@ -6394,7 +6394,7 @@
         <v>2119</v>
       </c>
       <c r="L11">
-        <v>929</v>
+        <v>933</v>
       </c>
     </row>
     <row r="12" spans="1:12">
@@ -6470,7 +6470,7 @@
         <v>296</v>
       </c>
       <c r="L13">
-        <v>136</v>
+        <v>138</v>
       </c>
     </row>
     <row r="14" spans="1:12">
@@ -6508,7 +6508,7 @@
         <v>720</v>
       </c>
       <c r="L14">
-        <v>366</v>
+        <v>368</v>
       </c>
     </row>
     <row r="15" spans="1:12">
@@ -6546,7 +6546,7 @@
         <v>986</v>
       </c>
       <c r="L15">
-        <v>414</v>
+        <v>415</v>
       </c>
     </row>
     <row r="16" spans="1:12">
@@ -6584,7 +6584,7 @@
         <v>938</v>
       </c>
       <c r="L16">
-        <v>402</v>
+        <v>403</v>
       </c>
     </row>
     <row r="17" spans="1:12">
@@ -6660,7 +6660,7 @@
         <v>751</v>
       </c>
       <c r="L18">
-        <v>354</v>
+        <v>358</v>
       </c>
     </row>
     <row r="19" spans="1:12">
@@ -6698,7 +6698,7 @@
         <v>2526</v>
       </c>
       <c r="L19">
-        <v>1342</v>
+        <v>1350</v>
       </c>
     </row>
     <row r="20" spans="1:12">
@@ -6736,7 +6736,7 @@
         <v>1973</v>
       </c>
       <c r="L20">
-        <v>972</v>
+        <v>979</v>
       </c>
     </row>
     <row r="21" spans="1:12">
@@ -6774,7 +6774,7 @@
         <v>321</v>
       </c>
       <c r="L21">
-        <v>131</v>
+        <v>132</v>
       </c>
     </row>
     <row r="22" spans="1:12">
@@ -6812,7 +6812,7 @@
         <v>441</v>
       </c>
       <c r="L22">
-        <v>208</v>
+        <v>209</v>
       </c>
     </row>
     <row r="23" spans="1:12">
@@ -6850,7 +6850,7 @@
         <v>1330</v>
       </c>
       <c r="L23">
-        <v>670</v>
+        <v>672</v>
       </c>
     </row>
     <row r="24" spans="1:12">
@@ -6888,7 +6888,7 @@
         <v>675</v>
       </c>
       <c r="L24">
-        <v>257</v>
+        <v>258</v>
       </c>
     </row>
     <row r="25" spans="1:12">
@@ -6926,7 +6926,7 @@
         <v>555</v>
       </c>
       <c r="L25">
-        <v>320</v>
+        <v>321</v>
       </c>
     </row>
     <row r="26" spans="1:12">
@@ -6964,7 +6964,7 @@
         <v>281</v>
       </c>
       <c r="L26">
-        <v>117</v>
+        <v>119</v>
       </c>
     </row>
     <row r="27" spans="1:12">
@@ -7002,7 +7002,7 @@
         <v>1554</v>
       </c>
       <c r="L27">
-        <v>720</v>
+        <v>725</v>
       </c>
     </row>
     <row r="28" spans="1:12">
@@ -7078,7 +7078,7 @@
         <v>3877</v>
       </c>
       <c r="L29">
-        <v>1815</v>
+        <v>1828</v>
       </c>
     </row>
     <row r="30" spans="1:12">
@@ -7116,7 +7116,7 @@
         <v>269</v>
       </c>
       <c r="L30">
-        <v>158</v>
+        <v>160</v>
       </c>
     </row>
     <row r="31" spans="1:12">
@@ -7154,7 +7154,7 @@
         <v>1039</v>
       </c>
       <c r="L31">
-        <v>508</v>
+        <v>513</v>
       </c>
     </row>
     <row r="32" spans="1:12">
@@ -7230,7 +7230,7 @@
         <v>2788</v>
       </c>
       <c r="L33">
-        <v>1320</v>
+        <v>1322</v>
       </c>
     </row>
     <row r="34" spans="1:12">
@@ -7268,7 +7268,7 @@
         <v>973</v>
       </c>
       <c r="L34">
-        <v>383</v>
+        <v>386</v>
       </c>
     </row>
     <row r="35" spans="1:12">
@@ -7306,7 +7306,7 @@
         <v>337</v>
       </c>
       <c r="L35">
-        <v>190</v>
+        <v>193</v>
       </c>
     </row>
     <row r="36" spans="1:12">
@@ -7344,7 +7344,7 @@
         <v>1711</v>
       </c>
       <c r="L36">
-        <v>746</v>
+        <v>749</v>
       </c>
     </row>
     <row r="37" spans="1:12">
@@ -7382,7 +7382,7 @@
         <v>2714</v>
       </c>
       <c r="L37">
-        <v>1222</v>
+        <v>1226</v>
       </c>
     </row>
     <row r="38" spans="1:12">
@@ -7496,7 +7496,7 @@
         <v>352</v>
       </c>
       <c r="L40">
-        <v>204</v>
+        <v>205</v>
       </c>
     </row>
     <row r="41" spans="1:12">
@@ -7534,7 +7534,7 @@
         <v>495</v>
       </c>
       <c r="L41">
-        <v>179</v>
+        <v>180</v>
       </c>
     </row>
     <row r="42" spans="1:12">
@@ -7572,7 +7572,7 @@
         <v>3265</v>
       </c>
       <c r="L42">
-        <v>1300</v>
+        <v>1307</v>
       </c>
     </row>
     <row r="43" spans="1:12">
@@ -7610,7 +7610,7 @@
         <v>1329</v>
       </c>
       <c r="L43">
-        <v>832</v>
+        <v>836</v>
       </c>
     </row>
     <row r="44" spans="1:12">
@@ -7648,7 +7648,7 @@
         <v>1296</v>
       </c>
       <c r="L44">
-        <v>532</v>
+        <v>536</v>
       </c>
     </row>
     <row r="45" spans="1:12">
@@ -7762,7 +7762,7 @@
         <v>1046</v>
       </c>
       <c r="L47">
-        <v>493</v>
+        <v>499</v>
       </c>
     </row>
     <row r="48" spans="1:12">
@@ -7800,7 +7800,7 @@
         <v>3217</v>
       </c>
       <c r="L48">
-        <v>1517</v>
+        <v>1525</v>
       </c>
     </row>
     <row r="49" spans="1:12">
@@ -7838,7 +7838,7 @@
         <v>2190</v>
       </c>
       <c r="L49">
-        <v>934</v>
+        <v>939</v>
       </c>
     </row>
     <row r="50" spans="1:12">
@@ -7876,7 +7876,7 @@
         <v>1038</v>
       </c>
       <c r="L50">
-        <v>548</v>
+        <v>552</v>
       </c>
     </row>
     <row r="51" spans="1:12">
@@ -7914,7 +7914,7 @@
         <v>1492</v>
       </c>
       <c r="L51">
-        <v>790</v>
+        <v>797</v>
       </c>
     </row>
     <row r="52" spans="1:12">
@@ -7952,7 +7952,7 @@
         <v>1847</v>
       </c>
       <c r="L52">
-        <v>734</v>
+        <v>741</v>
       </c>
     </row>
     <row r="53" spans="1:12">
@@ -7990,7 +7990,7 @@
         <v>2353</v>
       </c>
       <c r="L53">
-        <v>946</v>
+        <v>952</v>
       </c>
     </row>
     <row r="54" spans="1:12">
@@ -8028,7 +8028,7 @@
         <v>4179</v>
       </c>
       <c r="L54">
-        <v>2061</v>
+        <v>2076</v>
       </c>
     </row>
     <row r="55" spans="1:12">
@@ -8066,7 +8066,7 @@
         <v>1291</v>
       </c>
       <c r="L55">
-        <v>562</v>
+        <v>565</v>
       </c>
     </row>
     <row r="56" spans="1:12">
@@ -8104,7 +8104,7 @@
         <v>718</v>
       </c>
       <c r="L56">
-        <v>309</v>
+        <v>310</v>
       </c>
     </row>
     <row r="57" spans="1:12">
@@ -8180,7 +8180,7 @@
         <v>202</v>
       </c>
       <c r="L58">
-        <v>55</v>
+        <v>56</v>
       </c>
     </row>
     <row r="59" spans="1:12">
@@ -8218,7 +8218,7 @@
         <v>248</v>
       </c>
       <c r="L59">
-        <v>143</v>
+        <v>145</v>
       </c>
     </row>
     <row r="60" spans="1:12">
@@ -8256,7 +8256,7 @@
         <v>784</v>
       </c>
       <c r="L60">
-        <v>374</v>
+        <v>377</v>
       </c>
     </row>
     <row r="61" spans="1:12">
@@ -8294,7 +8294,7 @@
         <v>167</v>
       </c>
       <c r="L61">
-        <v>70</v>
+        <v>71</v>
       </c>
     </row>
     <row r="62" spans="1:12">
@@ -8332,7 +8332,7 @@
         <v>76</v>
       </c>
       <c r="L62">
-        <v>31</v>
+        <v>32</v>
       </c>
     </row>
     <row r="63" spans="1:12">
@@ -8367,10 +8367,10 @@
         <v>1002</v>
       </c>
       <c r="K63">
-        <v>795</v>
+        <v>794</v>
       </c>
       <c r="L63">
-        <v>256</v>
+        <v>274</v>
       </c>
     </row>
     <row r="64" spans="1:12">
@@ -8408,7 +8408,7 @@
         <v>1133</v>
       </c>
       <c r="L64">
-        <v>498</v>
+        <v>501</v>
       </c>
     </row>
     <row r="65" spans="1:12">
@@ -8446,7 +8446,7 @@
         <v>1683</v>
       </c>
       <c r="L65">
-        <v>758</v>
+        <v>761</v>
       </c>
     </row>
     <row r="66" spans="1:12">
@@ -8484,7 +8484,7 @@
         <v>722</v>
       </c>
       <c r="L66">
-        <v>293</v>
+        <v>295</v>
       </c>
     </row>
     <row r="67" spans="1:12">
@@ -8522,7 +8522,7 @@
         <v>2435</v>
       </c>
       <c r="L67">
-        <v>1036</v>
+        <v>1040</v>
       </c>
     </row>
     <row r="68" spans="1:12">
@@ -8560,7 +8560,7 @@
         <v>497</v>
       </c>
       <c r="L68">
-        <v>280</v>
+        <v>281</v>
       </c>
     </row>
     <row r="69" spans="1:12">
@@ -8598,7 +8598,7 @@
         <v>539</v>
       </c>
       <c r="L69">
-        <v>264</v>
+        <v>266</v>
       </c>
     </row>
     <row r="70" spans="1:12">
@@ -8674,7 +8674,7 @@
         <v>378</v>
       </c>
       <c r="L71">
-        <v>190</v>
+        <v>191</v>
       </c>
     </row>
     <row r="72" spans="1:12">
@@ -8750,7 +8750,7 @@
         <v>1505</v>
       </c>
       <c r="L73">
-        <v>699</v>
+        <v>704</v>
       </c>
     </row>
     <row r="74" spans="1:12">
@@ -8788,7 +8788,7 @@
         <v>360</v>
       </c>
       <c r="L74">
-        <v>183</v>
+        <v>184</v>
       </c>
     </row>
     <row r="75" spans="1:12">
@@ -8826,7 +8826,7 @@
         <v>490</v>
       </c>
       <c r="L75">
-        <v>246</v>
+        <v>247</v>
       </c>
     </row>
     <row r="76" spans="1:12">
@@ -8864,7 +8864,7 @@
         <v>3058</v>
       </c>
       <c r="L76">
-        <v>1636</v>
+        <v>1649</v>
       </c>
     </row>
     <row r="77" spans="1:12">
@@ -8902,7 +8902,7 @@
         <v>447</v>
       </c>
       <c r="L77">
-        <v>242</v>
+        <v>243</v>
       </c>
     </row>
     <row r="78" spans="1:12">
@@ -8940,7 +8940,7 @@
         <v>1940</v>
       </c>
       <c r="L78">
-        <v>856</v>
+        <v>859</v>
       </c>
     </row>
     <row r="79" spans="1:12">
@@ -8978,7 +8978,7 @@
         <v>2264</v>
       </c>
       <c r="L79">
-        <v>1113</v>
+        <v>1116</v>
       </c>
     </row>
     <row r="80" spans="1:12">
@@ -9130,7 +9130,7 @@
         <v>1627</v>
       </c>
       <c r="L83">
-        <v>822</v>
+        <v>827</v>
       </c>
     </row>
     <row r="84" spans="1:12">
@@ -9168,7 +9168,7 @@
         <v>876</v>
       </c>
       <c r="L84">
-        <v>441</v>
+        <v>442</v>
       </c>
     </row>
     <row r="85" spans="1:12">
@@ -9206,7 +9206,7 @@
         <v>3838</v>
       </c>
       <c r="L85">
-        <v>1882</v>
+        <v>1898</v>
       </c>
     </row>
     <row r="86" spans="1:12">
@@ -9241,10 +9241,10 @@
         <v>997</v>
       </c>
       <c r="K86">
-        <v>1009</v>
+        <v>1010</v>
       </c>
       <c r="L86">
-        <v>479</v>
+        <v>480</v>
       </c>
     </row>
     <row r="87" spans="1:12">
@@ -9320,7 +9320,7 @@
         <v>1021</v>
       </c>
       <c r="L88">
-        <v>456</v>
+        <v>462</v>
       </c>
     </row>
     <row r="89" spans="1:12">
@@ -9358,7 +9358,7 @@
         <v>2322</v>
       </c>
       <c r="L89">
-        <v>1109</v>
+        <v>1117</v>
       </c>
     </row>
     <row r="90" spans="1:12">
@@ -9396,7 +9396,7 @@
         <v>1145</v>
       </c>
       <c r="L90">
-        <v>561</v>
+        <v>564</v>
       </c>
     </row>
     <row r="91" spans="1:12">
@@ -9434,7 +9434,7 @@
         <v>1048</v>
       </c>
       <c r="L91">
-        <v>537</v>
+        <v>543</v>
       </c>
     </row>
     <row r="92" spans="1:12">
@@ -9472,7 +9472,7 @@
         <v>402</v>
       </c>
       <c r="L92">
-        <v>184</v>
+        <v>185</v>
       </c>
     </row>
     <row r="93" spans="1:12">
@@ -9510,7 +9510,7 @@
         <v>935</v>
       </c>
       <c r="L93">
-        <v>430</v>
+        <v>437</v>
       </c>
     </row>
     <row r="94" spans="1:12">
@@ -9548,7 +9548,7 @@
         <v>3002</v>
       </c>
       <c r="L94">
-        <v>1398</v>
+        <v>1409</v>
       </c>
     </row>
     <row r="95" spans="1:12">
@@ -9586,7 +9586,7 @@
         <v>1445</v>
       </c>
       <c r="L95">
-        <v>653</v>
+        <v>657</v>
       </c>
     </row>
     <row r="96" spans="1:12">
@@ -9624,7 +9624,7 @@
         <v>1635</v>
       </c>
       <c r="L96">
-        <v>658</v>
+        <v>660</v>
       </c>
     </row>
     <row r="97" spans="1:12">
@@ -9662,7 +9662,7 @@
         <v>1818</v>
       </c>
       <c r="L97">
-        <v>964</v>
+        <v>965</v>
       </c>
     </row>
     <row r="98" spans="1:12">
@@ -9700,7 +9700,7 @@
         <v>1502</v>
       </c>
       <c r="L98">
-        <v>613</v>
+        <v>618</v>
       </c>
     </row>
     <row r="99" spans="1:12">
@@ -9738,7 +9738,7 @@
         <v>1588</v>
       </c>
       <c r="L99">
-        <v>755</v>
+        <v>761</v>
       </c>
     </row>
     <row r="100" spans="1:12">
@@ -9776,7 +9776,7 @@
         <v>347</v>
       </c>
       <c r="L100">
-        <v>152</v>
+        <v>154</v>
       </c>
     </row>
     <row r="101" spans="1:12">
@@ -9814,7 +9814,7 @@
         <v>118655</v>
       </c>
       <c r="L101">
-        <v>55687</v>
+        <v>56042</v>
       </c>
     </row>
   </sheetData>
@@ -10302,7 +10302,7 @@
         <v>275</v>
       </c>
       <c r="L10">
-        <v>157</v>
+        <v>158</v>
       </c>
     </row>
     <row r="11" spans="1:12">
@@ -10340,7 +10340,7 @@
         <v>490</v>
       </c>
       <c r="L11">
-        <v>246</v>
+        <v>247</v>
       </c>
     </row>
   </sheetData>
@@ -10711,7 +10711,7 @@
         <v>171</v>
       </c>
       <c r="L10">
-        <v>102</v>
+        <v>103</v>
       </c>
     </row>
     <row r="11" spans="1:12">
@@ -10749,7 +10749,7 @@
         <v>352</v>
       </c>
       <c r="L11">
-        <v>204</v>
+        <v>205</v>
       </c>
     </row>
   </sheetData>
@@ -10890,7 +10890,7 @@
         <v>45</v>
       </c>
       <c r="L3">
-        <v>20</v>
+        <v>21</v>
       </c>
     </row>
     <row r="4" spans="1:12">
@@ -11068,7 +11068,7 @@
         <v>253</v>
       </c>
       <c r="L8">
-        <v>124</v>
+        <v>125</v>
       </c>
     </row>
     <row r="9" spans="1:12">
@@ -11144,7 +11144,7 @@
         <v>653</v>
       </c>
       <c r="L10">
-        <v>273</v>
+        <v>274</v>
       </c>
     </row>
     <row r="11" spans="1:12">
@@ -11182,7 +11182,7 @@
         <v>1133</v>
       </c>
       <c r="L11">
-        <v>498</v>
+        <v>501</v>
       </c>
     </row>
   </sheetData>
@@ -11399,7 +11399,7 @@
         <v>107</v>
       </c>
       <c r="L5">
-        <v>72</v>
+        <v>73</v>
       </c>
     </row>
     <row r="6" spans="1:12">
@@ -11551,7 +11551,7 @@
         <v>107</v>
       </c>
       <c r="L9">
-        <v>35</v>
+        <v>36</v>
       </c>
     </row>
     <row r="10" spans="1:12">
@@ -11589,7 +11589,7 @@
         <v>545</v>
       </c>
       <c r="L10">
-        <v>252</v>
+        <v>254</v>
       </c>
     </row>
     <row r="11" spans="1:12">
@@ -11627,7 +11627,7 @@
         <v>1445</v>
       </c>
       <c r="L11">
-        <v>653</v>
+        <v>657</v>
       </c>
     </row>
   </sheetData>
@@ -11730,7 +11730,7 @@
         <v>258</v>
       </c>
       <c r="L2">
-        <v>131</v>
+        <v>133</v>
       </c>
     </row>
     <row r="3" spans="1:12">
@@ -11844,7 +11844,7 @@
         <v>230</v>
       </c>
       <c r="L5">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="6" spans="1:12">
@@ -11996,7 +11996,7 @@
         <v>272</v>
       </c>
       <c r="L9">
-        <v>121</v>
+        <v>122</v>
       </c>
     </row>
     <row r="10" spans="1:12">
@@ -12034,7 +12034,7 @@
         <v>975</v>
       </c>
       <c r="L10">
-        <v>460</v>
+        <v>462</v>
       </c>
     </row>
     <row r="11" spans="1:12">
@@ -12072,7 +12072,7 @@
         <v>2714</v>
       </c>
       <c r="L11">
-        <v>1222</v>
+        <v>1226</v>
       </c>
     </row>
   </sheetData>
@@ -12403,7 +12403,7 @@
         <v>270</v>
       </c>
       <c r="L8">
-        <v>141</v>
+        <v>142</v>
       </c>
     </row>
     <row r="9" spans="1:12">
@@ -12479,7 +12479,7 @@
         <v>637</v>
       </c>
       <c r="L10">
-        <v>338</v>
+        <v>340</v>
       </c>
     </row>
     <row r="11" spans="1:12">
@@ -12517,7 +12517,7 @@
         <v>1683</v>
       </c>
       <c r="L11">
-        <v>758</v>
+        <v>761</v>
       </c>
     </row>
   </sheetData>
@@ -12728,7 +12728,7 @@
         <v>108</v>
       </c>
       <c r="L5">
-        <v>69</v>
+        <v>71</v>
       </c>
     </row>
     <row r="6" spans="1:12">
@@ -12874,7 +12874,7 @@
         <v>93</v>
       </c>
       <c r="L9">
-        <v>32</v>
+        <v>33</v>
       </c>
     </row>
     <row r="10" spans="1:12">
@@ -12912,7 +12912,7 @@
         <v>958</v>
       </c>
       <c r="L10">
-        <v>464</v>
+        <v>466</v>
       </c>
     </row>
     <row r="11" spans="1:12">
@@ -12950,7 +12950,7 @@
         <v>1554</v>
       </c>
       <c r="L11">
-        <v>720</v>
+        <v>725</v>
       </c>
     </row>
   </sheetData>
@@ -13091,7 +13091,7 @@
         <v>194</v>
       </c>
       <c r="L3">
-        <v>83</v>
+        <v>84</v>
       </c>
     </row>
     <row r="4" spans="1:12">
@@ -13205,7 +13205,7 @@
         <v>20</v>
       </c>
       <c r="L6">
-        <v>16</v>
+        <v>17</v>
       </c>
     </row>
     <row r="7" spans="1:12">
@@ -13281,7 +13281,7 @@
         <v>311</v>
       </c>
       <c r="L8">
-        <v>133</v>
+        <v>135</v>
       </c>
     </row>
     <row r="9" spans="1:12">
@@ -13357,7 +13357,7 @@
         <v>687</v>
       </c>
       <c r="L10">
-        <v>370</v>
+        <v>372</v>
       </c>
     </row>
     <row r="11" spans="1:12">
@@ -13395,7 +13395,7 @@
         <v>1588</v>
       </c>
       <c r="L11">
-        <v>755</v>
+        <v>761</v>
       </c>
     </row>
   </sheetData>
@@ -13714,7 +13714,7 @@
         <v>43</v>
       </c>
       <c r="L8">
-        <v>30</v>
+        <v>32</v>
       </c>
     </row>
     <row r="9" spans="1:12">
@@ -13828,7 +13828,7 @@
         <v>269</v>
       </c>
       <c r="L11">
-        <v>158</v>
+        <v>160</v>
       </c>
     </row>
   </sheetData>
@@ -13931,7 +13931,7 @@
         <v>93</v>
       </c>
       <c r="L2">
-        <v>40</v>
+        <v>42</v>
       </c>
     </row>
     <row r="3" spans="1:12">
@@ -14045,7 +14045,7 @@
         <v>55</v>
       </c>
       <c r="L5">
-        <v>28</v>
+        <v>29</v>
       </c>
     </row>
     <row r="6" spans="1:12">
@@ -14159,7 +14159,7 @@
         <v>211</v>
       </c>
       <c r="L8">
-        <v>90</v>
+        <v>91</v>
       </c>
     </row>
     <row r="9" spans="1:12">
@@ -14197,7 +14197,7 @@
         <v>129</v>
       </c>
       <c r="L9">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="10" spans="1:12">
@@ -14235,7 +14235,7 @@
         <v>439</v>
       </c>
       <c r="L10">
-        <v>271</v>
+        <v>273</v>
       </c>
     </row>
     <row r="11" spans="1:12">
@@ -14273,7 +14273,7 @@
         <v>1039</v>
       </c>
       <c r="L11">
-        <v>508</v>
+        <v>513</v>
       </c>
     </row>
   </sheetData>
@@ -14595,7 +14595,7 @@
         <v>143</v>
       </c>
       <c r="L8">
-        <v>62</v>
+        <v>63</v>
       </c>
     </row>
     <row r="9" spans="1:12">
@@ -14671,7 +14671,7 @@
         <v>369</v>
       </c>
       <c r="L10">
-        <v>211</v>
+        <v>212</v>
       </c>
     </row>
     <row r="11" spans="1:12">
@@ -14709,7 +14709,7 @@
         <v>720</v>
       </c>
       <c r="L11">
-        <v>366</v>
+        <v>368</v>
       </c>
     </row>
   </sheetData>
@@ -14812,7 +14812,7 @@
         <v>299</v>
       </c>
       <c r="L2">
-        <v>122</v>
+        <v>123</v>
       </c>
     </row>
     <row r="3" spans="1:12">
@@ -14850,7 +14850,7 @@
         <v>380</v>
       </c>
       <c r="L3">
-        <v>163</v>
+        <v>165</v>
       </c>
     </row>
     <row r="4" spans="1:12">
@@ -15040,7 +15040,7 @@
         <v>409</v>
       </c>
       <c r="L8">
-        <v>166</v>
+        <v>167</v>
       </c>
     </row>
     <row r="9" spans="1:12">
@@ -15154,7 +15154,7 @@
         <v>2435</v>
       </c>
       <c r="L11">
-        <v>1036</v>
+        <v>1040</v>
       </c>
     </row>
   </sheetData>
@@ -15485,7 +15485,7 @@
         <v>199</v>
       </c>
       <c r="L8">
-        <v>92</v>
+        <v>93</v>
       </c>
     </row>
     <row r="9" spans="1:12">
@@ -15599,7 +15599,7 @@
         <v>876</v>
       </c>
       <c r="L11">
-        <v>441</v>
+        <v>442</v>
       </c>
     </row>
   </sheetData>
@@ -15702,7 +15702,7 @@
         <v>86</v>
       </c>
       <c r="L2">
-        <v>35</v>
+        <v>36</v>
       </c>
     </row>
     <row r="3" spans="1:12">
@@ -15804,7 +15804,7 @@
         <v>127</v>
       </c>
       <c r="L5">
-        <v>56</v>
+        <v>57</v>
       </c>
     </row>
     <row r="6" spans="1:12">
@@ -15915,7 +15915,7 @@
         <v>380</v>
       </c>
       <c r="L8">
-        <v>163</v>
+        <v>164</v>
       </c>
     </row>
     <row r="9" spans="1:12">
@@ -15953,7 +15953,7 @@
         <v>173</v>
       </c>
       <c r="L9">
-        <v>54</v>
+        <v>57</v>
       </c>
     </row>
     <row r="10" spans="1:12">
@@ -15991,7 +15991,7 @@
         <v>2124</v>
       </c>
       <c r="L10">
-        <v>1027</v>
+        <v>1032</v>
       </c>
     </row>
     <row r="11" spans="1:12">
@@ -16029,7 +16029,7 @@
         <v>3002</v>
       </c>
       <c r="L11">
-        <v>1398</v>
+        <v>1409</v>
       </c>
     </row>
   </sheetData>
@@ -16243,7 +16243,7 @@
         <v>121</v>
       </c>
       <c r="L5">
-        <v>39</v>
+        <v>40</v>
       </c>
     </row>
     <row r="6" spans="1:12">
@@ -16281,7 +16281,7 @@
         <v>32</v>
       </c>
       <c r="L6">
-        <v>22</v>
+        <v>23</v>
       </c>
     </row>
     <row r="7" spans="1:12">
@@ -16395,7 +16395,7 @@
         <v>188</v>
       </c>
       <c r="L9">
-        <v>81</v>
+        <v>82</v>
       </c>
     </row>
     <row r="10" spans="1:12">
@@ -16433,7 +16433,7 @@
         <v>2251</v>
       </c>
       <c r="L10">
-        <v>1318</v>
+        <v>1328</v>
       </c>
     </row>
     <row r="11" spans="1:12">
@@ -16471,7 +16471,7 @@
         <v>3058</v>
       </c>
       <c r="L11">
-        <v>1636</v>
+        <v>1649</v>
       </c>
     </row>
   </sheetData>
@@ -17109,7 +17109,7 @@
         <v>51</v>
       </c>
       <c r="L5">
-        <v>16</v>
+        <v>17</v>
       </c>
     </row>
     <row r="6" spans="1:12">
@@ -17334,7 +17334,7 @@
         <v>555</v>
       </c>
       <c r="L11">
-        <v>320</v>
+        <v>321</v>
       </c>
     </row>
   </sheetData>
@@ -17527,7 +17527,7 @@
         <v>26</v>
       </c>
       <c r="L5">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="6" spans="1:12">
@@ -17687,7 +17687,7 @@
         <v>230</v>
       </c>
       <c r="L10">
-        <v>114</v>
+        <v>115</v>
       </c>
     </row>
     <row r="11" spans="1:12">
@@ -17725,7 +17725,7 @@
         <v>347</v>
       </c>
       <c r="L11">
-        <v>152</v>
+        <v>154</v>
       </c>
     </row>
   </sheetData>
@@ -18096,7 +18096,7 @@
         <v>655</v>
       </c>
       <c r="L10">
-        <v>315</v>
+        <v>316</v>
       </c>
     </row>
     <row r="11" spans="1:12">
@@ -18134,7 +18134,7 @@
         <v>938</v>
       </c>
       <c r="L11">
-        <v>402</v>
+        <v>403</v>
       </c>
     </row>
   </sheetData>
@@ -18523,7 +18523,7 @@
         <v>1651</v>
       </c>
       <c r="L10">
-        <v>722</v>
+        <v>727</v>
       </c>
     </row>
     <row r="11" spans="1:12">
@@ -18561,7 +18561,7 @@
         <v>2190</v>
       </c>
       <c r="L11">
-        <v>934</v>
+        <v>939</v>
       </c>
     </row>
   </sheetData>
@@ -18886,7 +18886,7 @@
         <v>424</v>
       </c>
       <c r="L8">
-        <v>153</v>
+        <v>154</v>
       </c>
     </row>
     <row r="9" spans="1:12">
@@ -19000,7 +19000,7 @@
         <v>1818</v>
       </c>
       <c r="L11">
-        <v>964</v>
+        <v>965</v>
       </c>
     </row>
   </sheetData>
@@ -19214,7 +19214,7 @@
         <v>110</v>
       </c>
       <c r="L5">
-        <v>48</v>
+        <v>49</v>
       </c>
     </row>
     <row r="6" spans="1:12">
@@ -19328,7 +19328,7 @@
         <v>388</v>
       </c>
       <c r="L8">
-        <v>125</v>
+        <v>126</v>
       </c>
     </row>
     <row r="9" spans="1:12">
@@ -19442,7 +19442,7 @@
         <v>1635</v>
       </c>
       <c r="L11">
-        <v>658</v>
+        <v>660</v>
       </c>
     </row>
   </sheetData>
@@ -19773,7 +19773,7 @@
         <v>259</v>
       </c>
       <c r="L8">
-        <v>101</v>
+        <v>102</v>
       </c>
     </row>
     <row r="9" spans="1:12">
@@ -19849,7 +19849,7 @@
         <v>645</v>
       </c>
       <c r="L10">
-        <v>305</v>
+        <v>307</v>
       </c>
     </row>
     <row r="11" spans="1:12">
@@ -19887,7 +19887,7 @@
         <v>1291</v>
       </c>
       <c r="L11">
-        <v>562</v>
+        <v>565</v>
       </c>
     </row>
   </sheetData>
@@ -20028,7 +20028,7 @@
         <v>123</v>
       </c>
       <c r="L3">
-        <v>58</v>
+        <v>59</v>
       </c>
     </row>
     <row r="4" spans="1:12">
@@ -20253,7 +20253,7 @@
         <v>278</v>
       </c>
       <c r="L9">
-        <v>117</v>
+        <v>118</v>
       </c>
     </row>
     <row r="10" spans="1:12">
@@ -20291,7 +20291,7 @@
         <v>3090</v>
       </c>
       <c r="L10">
-        <v>1593</v>
+        <v>1606</v>
       </c>
     </row>
     <row r="11" spans="1:12">
@@ -20329,7 +20329,7 @@
         <v>4179</v>
       </c>
       <c r="L11">
-        <v>2061</v>
+        <v>2076</v>
       </c>
     </row>
   </sheetData>
@@ -20546,7 +20546,7 @@
         <v>116</v>
       </c>
       <c r="L5">
-        <v>40</v>
+        <v>41</v>
       </c>
     </row>
     <row r="6" spans="1:12">
@@ -20660,7 +20660,7 @@
         <v>255</v>
       </c>
       <c r="L8">
-        <v>96</v>
+        <v>97</v>
       </c>
     </row>
     <row r="9" spans="1:12">
@@ -20736,7 +20736,7 @@
         <v>884</v>
       </c>
       <c r="L10">
-        <v>458</v>
+        <v>461</v>
       </c>
     </row>
     <row r="11" spans="1:12">
@@ -20774,7 +20774,7 @@
         <v>1505</v>
       </c>
       <c r="L11">
-        <v>699</v>
+        <v>704</v>
       </c>
     </row>
   </sheetData>
@@ -20877,7 +20877,7 @@
         <v>428</v>
       </c>
       <c r="L2">
-        <v>200</v>
+        <v>201</v>
       </c>
     </row>
     <row r="3" spans="1:12">
@@ -20915,7 +20915,7 @@
         <v>533</v>
       </c>
       <c r="L3">
-        <v>247</v>
+        <v>249</v>
       </c>
     </row>
     <row r="4" spans="1:12">
@@ -21105,7 +21105,7 @@
         <v>832</v>
       </c>
       <c r="L8">
-        <v>353</v>
+        <v>357</v>
       </c>
     </row>
     <row r="9" spans="1:12">
@@ -21143,7 +21143,7 @@
         <v>447</v>
       </c>
       <c r="L9">
-        <v>165</v>
+        <v>167</v>
       </c>
     </row>
     <row r="10" spans="1:12">
@@ -21181,7 +21181,7 @@
         <v>1294</v>
       </c>
       <c r="L10">
-        <v>676</v>
+        <v>680</v>
       </c>
     </row>
     <row r="11" spans="1:12">
@@ -21219,7 +21219,7 @@
         <v>3877</v>
       </c>
       <c r="L11">
-        <v>1815</v>
+        <v>1828</v>
       </c>
     </row>
   </sheetData>
@@ -21535,7 +21535,7 @@
         <v>377</v>
       </c>
       <c r="L8">
-        <v>139</v>
+        <v>140</v>
       </c>
     </row>
     <row r="9" spans="1:12">
@@ -21611,7 +21611,7 @@
         <v>2258</v>
       </c>
       <c r="L10">
-        <v>1088</v>
+        <v>1095</v>
       </c>
     </row>
     <row r="11" spans="1:12">
@@ -21649,7 +21649,7 @@
         <v>3217</v>
       </c>
       <c r="L11">
-        <v>1517</v>
+        <v>1525</v>
       </c>
     </row>
   </sheetData>
@@ -21942,7 +21942,7 @@
         <v>25</v>
       </c>
       <c r="L7">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="8" spans="1:12">
@@ -22018,7 +22018,7 @@
         <v>266</v>
       </c>
       <c r="L9">
-        <v>99</v>
+        <v>101</v>
       </c>
     </row>
     <row r="10" spans="1:12">
@@ -22056,7 +22056,7 @@
         <v>1013</v>
       </c>
       <c r="L10">
-        <v>668</v>
+        <v>673</v>
       </c>
     </row>
     <row r="11" spans="1:12">
@@ -22094,7 +22094,7 @@
         <v>2526</v>
       </c>
       <c r="L11">
-        <v>1342</v>
+        <v>1350</v>
       </c>
     </row>
   </sheetData>
@@ -22468,7 +22468,7 @@
         <v>420</v>
       </c>
       <c r="L10">
-        <v>187</v>
+        <v>189</v>
       </c>
     </row>
     <row r="11" spans="1:12">
@@ -22506,7 +22506,7 @@
         <v>722</v>
       </c>
       <c r="L11">
-        <v>293</v>
+        <v>295</v>
       </c>
     </row>
   </sheetData>
@@ -22831,7 +22831,7 @@
         <v>238</v>
       </c>
       <c r="L8">
-        <v>88</v>
+        <v>89</v>
       </c>
     </row>
     <row r="9" spans="1:12">
@@ -22907,7 +22907,7 @@
         <v>713</v>
       </c>
       <c r="L10">
-        <v>320</v>
+        <v>323</v>
       </c>
     </row>
     <row r="11" spans="1:12">
@@ -22945,7 +22945,7 @@
         <v>1296</v>
       </c>
       <c r="L11">
-        <v>532</v>
+        <v>536</v>
       </c>
     </row>
   </sheetData>
@@ -23162,7 +23162,7 @@
         <v>243</v>
       </c>
       <c r="L5">
-        <v>65</v>
+        <v>67</v>
       </c>
     </row>
     <row r="6" spans="1:12">
@@ -23276,7 +23276,7 @@
         <v>719</v>
       </c>
       <c r="L8">
-        <v>217</v>
+        <v>218</v>
       </c>
     </row>
     <row r="9" spans="1:12">
@@ -23314,7 +23314,7 @@
         <v>396</v>
       </c>
       <c r="L9">
-        <v>108</v>
+        <v>110</v>
       </c>
     </row>
     <row r="10" spans="1:12">
@@ -23352,7 +23352,7 @@
         <v>1252</v>
       </c>
       <c r="L10">
-        <v>633</v>
+        <v>635</v>
       </c>
     </row>
     <row r="11" spans="1:12">
@@ -23390,7 +23390,7 @@
         <v>3265</v>
       </c>
       <c r="L11">
-        <v>1300</v>
+        <v>1307</v>
       </c>
     </row>
   </sheetData>
@@ -23700,7 +23700,7 @@
         <v>129</v>
       </c>
       <c r="L8">
-        <v>48</v>
+        <v>49</v>
       </c>
     </row>
     <row r="9" spans="1:12">
@@ -23814,7 +23814,7 @@
         <v>441</v>
       </c>
       <c r="L11">
-        <v>208</v>
+        <v>209</v>
       </c>
     </row>
   </sheetData>
@@ -24145,7 +24145,7 @@
         <v>588</v>
       </c>
       <c r="L8">
-        <v>324</v>
+        <v>329</v>
       </c>
     </row>
     <row r="9" spans="1:12">
@@ -24221,7 +24221,7 @@
         <v>903</v>
       </c>
       <c r="L10">
-        <v>515</v>
+        <v>522</v>
       </c>
     </row>
     <row r="11" spans="1:12">
@@ -24259,7 +24259,7 @@
         <v>2524</v>
       </c>
       <c r="L11">
-        <v>1343</v>
+        <v>1355</v>
       </c>
     </row>
   </sheetData>
@@ -24362,7 +24362,7 @@
         <v>78</v>
       </c>
       <c r="L2">
-        <v>39</v>
+        <v>41</v>
       </c>
     </row>
     <row r="3" spans="1:12">
@@ -24584,7 +24584,7 @@
         <v>393</v>
       </c>
       <c r="L8">
-        <v>118</v>
+        <v>119</v>
       </c>
     </row>
     <row r="9" spans="1:12">
@@ -24622,7 +24622,7 @@
         <v>49</v>
       </c>
       <c r="L9">
-        <v>20</v>
+        <v>21</v>
       </c>
     </row>
     <row r="10" spans="1:12">
@@ -24660,7 +24660,7 @@
         <v>428</v>
       </c>
       <c r="L10">
-        <v>151</v>
+        <v>154</v>
       </c>
     </row>
     <row r="11" spans="1:12">
@@ -24698,7 +24698,7 @@
         <v>1111</v>
       </c>
       <c r="L11">
-        <v>406</v>
+        <v>413</v>
       </c>
     </row>
   </sheetData>
@@ -25096,7 +25096,7 @@
         <v>170</v>
       </c>
       <c r="L10">
-        <v>78</v>
+        <v>79</v>
       </c>
     </row>
     <row r="11" spans="1:12">
@@ -25134,7 +25134,7 @@
         <v>495</v>
       </c>
       <c r="L11">
-        <v>179</v>
+        <v>180</v>
       </c>
     </row>
   </sheetData>
@@ -25237,7 +25237,7 @@
         <v>133</v>
       </c>
       <c r="L2">
-        <v>60</v>
+        <v>62</v>
       </c>
     </row>
     <row r="3" spans="1:12">
@@ -25541,7 +25541,7 @@
         <v>795</v>
       </c>
       <c r="L10">
-        <v>322</v>
+        <v>323</v>
       </c>
     </row>
     <row r="11" spans="1:12">
@@ -25579,7 +25579,7 @@
         <v>1711</v>
       </c>
       <c r="L11">
-        <v>746</v>
+        <v>749</v>
       </c>
     </row>
   </sheetData>
@@ -25924,7 +25924,7 @@
         <v>231</v>
       </c>
       <c r="L9">
-        <v>101</v>
+        <v>103</v>
       </c>
     </row>
     <row r="10" spans="1:12">
@@ -25962,7 +25962,7 @@
         <v>296</v>
       </c>
       <c r="L10">
-        <v>136</v>
+        <v>138</v>
       </c>
     </row>
   </sheetData>
@@ -26290,7 +26290,7 @@
         <v>172</v>
       </c>
       <c r="L8">
-        <v>63</v>
+        <v>64</v>
       </c>
     </row>
     <row r="9" spans="1:12">
@@ -26366,7 +26366,7 @@
         <v>872</v>
       </c>
       <c r="L10">
-        <v>451</v>
+        <v>453</v>
       </c>
     </row>
     <row r="11" spans="1:12">
@@ -26404,7 +26404,7 @@
         <v>1286</v>
       </c>
       <c r="L11">
-        <v>623</v>
+        <v>626</v>
       </c>
     </row>
   </sheetData>
@@ -26772,10 +26772,10 @@
         <v>690</v>
       </c>
       <c r="K10">
-        <v>723</v>
+        <v>724</v>
       </c>
       <c r="L10">
-        <v>333</v>
+        <v>334</v>
       </c>
     </row>
     <row r="11" spans="1:12">
@@ -26810,10 +26810,10 @@
         <v>997</v>
       </c>
       <c r="K11">
-        <v>1009</v>
+        <v>1010</v>
       </c>
       <c r="L11">
-        <v>479</v>
+        <v>480</v>
       </c>
     </row>
   </sheetData>
@@ -26954,7 +26954,7 @@
         <v>84</v>
       </c>
       <c r="L3">
-        <v>43</v>
+        <v>44</v>
       </c>
     </row>
     <row r="4" spans="1:12">
@@ -27030,7 +27030,7 @@
         <v>110</v>
       </c>
       <c r="L5">
-        <v>50</v>
+        <v>51</v>
       </c>
     </row>
     <row r="6" spans="1:12">
@@ -27220,7 +27220,7 @@
         <v>1139</v>
       </c>
       <c r="L10">
-        <v>526</v>
+        <v>527</v>
       </c>
     </row>
     <row r="11" spans="1:12">
@@ -27258,7 +27258,7 @@
         <v>1940</v>
       </c>
       <c r="L11">
-        <v>856</v>
+        <v>859</v>
       </c>
     </row>
   </sheetData>
@@ -27399,7 +27399,7 @@
         <v>16</v>
       </c>
       <c r="L3">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="4" spans="1:12">
@@ -27676,7 +27676,7 @@
         <v>497</v>
       </c>
       <c r="L11">
-        <v>280</v>
+        <v>281</v>
       </c>
     </row>
   </sheetData>
@@ -28068,7 +28068,7 @@
         <v>377</v>
       </c>
       <c r="L10">
-        <v>154</v>
+        <v>155</v>
       </c>
     </row>
     <row r="11" spans="1:12">
@@ -28106,7 +28106,7 @@
         <v>675</v>
       </c>
       <c r="L11">
-        <v>257</v>
+        <v>258</v>
       </c>
     </row>
   </sheetData>
@@ -28513,7 +28513,7 @@
         <v>449</v>
       </c>
       <c r="L10">
-        <v>234</v>
+        <v>235</v>
       </c>
     </row>
     <row r="11" spans="1:12">
@@ -28551,7 +28551,7 @@
         <v>986</v>
       </c>
       <c r="L11">
-        <v>414</v>
+        <v>415</v>
       </c>
     </row>
   </sheetData>
@@ -28654,7 +28654,7 @@
         <v>166</v>
       </c>
       <c r="L2">
-        <v>76</v>
+        <v>77</v>
       </c>
     </row>
     <row r="3" spans="1:12">
@@ -28920,7 +28920,7 @@
         <v>165</v>
       </c>
       <c r="L9">
-        <v>49</v>
+        <v>50</v>
       </c>
     </row>
     <row r="10" spans="1:12">
@@ -28958,7 +28958,7 @@
         <v>1153</v>
       </c>
       <c r="L10">
-        <v>551</v>
+        <v>553</v>
       </c>
     </row>
     <row r="11" spans="1:12">
@@ -28996,7 +28996,7 @@
         <v>2119</v>
       </c>
       <c r="L11">
-        <v>929</v>
+        <v>933</v>
       </c>
     </row>
   </sheetData>
@@ -29321,7 +29321,7 @@
         <v>280</v>
       </c>
       <c r="L8">
-        <v>160</v>
+        <v>161</v>
       </c>
     </row>
     <row r="9" spans="1:12">
@@ -29397,7 +29397,7 @@
         <v>725</v>
       </c>
       <c r="L10">
-        <v>360</v>
+        <v>361</v>
       </c>
     </row>
     <row r="11" spans="1:12">
@@ -29435,7 +29435,7 @@
         <v>1330</v>
       </c>
       <c r="L11">
-        <v>670</v>
+        <v>672</v>
       </c>
     </row>
   </sheetData>
@@ -29538,7 +29538,7 @@
         <v>88</v>
       </c>
       <c r="L2">
-        <v>60</v>
+        <v>62</v>
       </c>
     </row>
     <row r="3" spans="1:12">
@@ -29576,7 +29576,7 @@
         <v>151</v>
       </c>
       <c r="L3">
-        <v>73</v>
+        <v>74</v>
       </c>
     </row>
     <row r="4" spans="1:12">
@@ -29766,7 +29766,7 @@
         <v>284</v>
       </c>
       <c r="L8">
-        <v>151</v>
+        <v>152</v>
       </c>
     </row>
     <row r="9" spans="1:12">
@@ -29804,7 +29804,7 @@
         <v>61</v>
       </c>
       <c r="L9">
-        <v>22</v>
+        <v>23</v>
       </c>
     </row>
     <row r="10" spans="1:12">
@@ -29842,7 +29842,7 @@
         <v>388</v>
       </c>
       <c r="L10">
-        <v>195</v>
+        <v>196</v>
       </c>
     </row>
     <row r="11" spans="1:12">
@@ -29880,7 +29880,7 @@
         <v>1048</v>
       </c>
       <c r="L11">
-        <v>537</v>
+        <v>543</v>
       </c>
     </row>
   </sheetData>
@@ -29983,7 +29983,7 @@
         <v>96</v>
       </c>
       <c r="L2">
-        <v>45</v>
+        <v>46</v>
       </c>
     </row>
     <row r="3" spans="1:12">
@@ -30208,7 +30208,7 @@
         <v>308</v>
       </c>
       <c r="L8">
-        <v>164</v>
+        <v>167</v>
       </c>
     </row>
     <row r="9" spans="1:12">
@@ -30284,7 +30284,7 @@
         <v>763</v>
       </c>
       <c r="L10">
-        <v>448</v>
+        <v>451</v>
       </c>
     </row>
     <row r="11" spans="1:12">
@@ -30322,7 +30322,7 @@
         <v>1492</v>
       </c>
       <c r="L11">
-        <v>790</v>
+        <v>797</v>
       </c>
     </row>
   </sheetData>
@@ -30463,7 +30463,7 @@
         <v>209</v>
       </c>
       <c r="L3">
-        <v>95</v>
+        <v>96</v>
       </c>
     </row>
     <row r="4" spans="1:12">
@@ -30653,7 +30653,7 @@
         <v>396</v>
       </c>
       <c r="L8">
-        <v>147</v>
+        <v>149</v>
       </c>
     </row>
     <row r="9" spans="1:12">
@@ -30729,7 +30729,7 @@
         <v>768</v>
       </c>
       <c r="L10">
-        <v>441</v>
+        <v>445</v>
       </c>
     </row>
     <row r="11" spans="1:12">
@@ -30767,7 +30767,7 @@
         <v>1973</v>
       </c>
       <c r="L11">
-        <v>972</v>
+        <v>979</v>
       </c>
     </row>
   </sheetData>
@@ -31126,7 +31126,7 @@
         <v>165</v>
       </c>
       <c r="L10">
-        <v>80</v>
+        <v>81</v>
       </c>
     </row>
     <row r="11" spans="1:12">
@@ -31164,7 +31164,7 @@
         <v>321</v>
       </c>
       <c r="L11">
-        <v>131</v>
+        <v>132</v>
       </c>
     </row>
   </sheetData>
@@ -31267,7 +31267,7 @@
         <v>53</v>
       </c>
       <c r="L2">
-        <v>30</v>
+        <v>31</v>
       </c>
     </row>
     <row r="3" spans="1:12">
@@ -31305,7 +31305,7 @@
         <v>59</v>
       </c>
       <c r="L3">
-        <v>30</v>
+        <v>31</v>
       </c>
     </row>
     <row r="4" spans="1:12">
@@ -31375,7 +31375,7 @@
         <v>49</v>
       </c>
       <c r="L5">
-        <v>19</v>
+        <v>20</v>
       </c>
     </row>
     <row r="6" spans="1:12">
@@ -31483,7 +31483,7 @@
         <v>280</v>
       </c>
       <c r="L8">
-        <v>101</v>
+        <v>102</v>
       </c>
     </row>
     <row r="9" spans="1:12">
@@ -31559,7 +31559,7 @@
         <v>523</v>
       </c>
       <c r="L10">
-        <v>286</v>
+        <v>288</v>
       </c>
     </row>
     <row r="11" spans="1:12">
@@ -31597,7 +31597,7 @@
         <v>1046</v>
       </c>
       <c r="L11">
-        <v>493</v>
+        <v>499</v>
       </c>
     </row>
   </sheetData>
@@ -31925,7 +31925,7 @@
         <v>305</v>
       </c>
       <c r="L8">
-        <v>147</v>
+        <v>148</v>
       </c>
     </row>
     <row r="9" spans="1:12">
@@ -31963,7 +31963,7 @@
         <v>69</v>
       </c>
       <c r="L9">
-        <v>30</v>
+        <v>31</v>
       </c>
     </row>
     <row r="10" spans="1:12">
@@ -32001,7 +32001,7 @@
         <v>496</v>
       </c>
       <c r="L10">
-        <v>258</v>
+        <v>259</v>
       </c>
     </row>
     <row r="11" spans="1:12">
@@ -32039,7 +32039,7 @@
         <v>1145</v>
       </c>
       <c r="L11">
-        <v>561</v>
+        <v>564</v>
       </c>
     </row>
   </sheetData>
@@ -32250,7 +32250,7 @@
         <v>108</v>
       </c>
       <c r="L5">
-        <v>33</v>
+        <v>34</v>
       </c>
     </row>
     <row r="6" spans="1:12">
@@ -32434,7 +32434,7 @@
         <v>636</v>
       </c>
       <c r="L10">
-        <v>403</v>
+        <v>406</v>
       </c>
     </row>
     <row r="11" spans="1:12">
@@ -32472,7 +32472,7 @@
         <v>1038</v>
       </c>
       <c r="L11">
-        <v>548</v>
+        <v>552</v>
       </c>
     </row>
   </sheetData>
@@ -32689,7 +32689,7 @@
         <v>66</v>
       </c>
       <c r="L5">
-        <v>30</v>
+        <v>31</v>
       </c>
     </row>
     <row r="6" spans="1:12">
@@ -32794,7 +32794,7 @@
         <v>271</v>
       </c>
       <c r="L8">
-        <v>80</v>
+        <v>84</v>
       </c>
     </row>
     <row r="9" spans="1:12">
@@ -32870,7 +32870,7 @@
         <v>479</v>
       </c>
       <c r="L10">
-        <v>255</v>
+        <v>257</v>
       </c>
     </row>
     <row r="11" spans="1:12">
@@ -32908,7 +32908,7 @@
         <v>935</v>
       </c>
       <c r="L11">
-        <v>430</v>
+        <v>437</v>
       </c>
     </row>
   </sheetData>
@@ -33239,7 +33239,7 @@
         <v>203</v>
       </c>
       <c r="L8">
-        <v>100</v>
+        <v>102</v>
       </c>
     </row>
     <row r="9" spans="1:12">
@@ -33315,7 +33315,7 @@
         <v>291</v>
       </c>
       <c r="L10">
-        <v>140</v>
+        <v>142</v>
       </c>
     </row>
     <row r="11" spans="1:12">
@@ -33353,7 +33353,7 @@
         <v>751</v>
       </c>
       <c r="L11">
-        <v>354</v>
+        <v>358</v>
       </c>
     </row>
   </sheetData>
@@ -34154,7 +34154,7 @@
         <v>148</v>
       </c>
       <c r="L10">
-        <v>96</v>
+        <v>97</v>
       </c>
     </row>
     <row r="11" spans="1:12">
@@ -34192,7 +34192,7 @@
         <v>447</v>
       </c>
       <c r="L11">
-        <v>242</v>
+        <v>243</v>
       </c>
     </row>
   </sheetData>
@@ -34545,7 +34545,7 @@
         <v>669</v>
       </c>
       <c r="L10">
-        <v>293</v>
+        <v>294</v>
       </c>
     </row>
     <row r="11" spans="1:12">
@@ -34583,7 +34583,7 @@
         <v>718</v>
       </c>
       <c r="L11">
-        <v>309</v>
+        <v>310</v>
       </c>
     </row>
   </sheetData>
@@ -35370,7 +35370,7 @@
         <v>72</v>
       </c>
       <c r="L9">
-        <v>25</v>
+        <v>27</v>
       </c>
     </row>
     <row r="10" spans="1:12">
@@ -35408,7 +35408,7 @@
         <v>615</v>
       </c>
       <c r="L10">
-        <v>292</v>
+        <v>295</v>
       </c>
     </row>
     <row r="11" spans="1:12">
@@ -35446,7 +35446,7 @@
         <v>1104</v>
       </c>
       <c r="L11">
-        <v>502</v>
+        <v>507</v>
       </c>
     </row>
   </sheetData>
@@ -36209,7 +36209,7 @@
         <v>82</v>
       </c>
       <c r="L9">
-        <v>28</v>
+        <v>29</v>
       </c>
     </row>
     <row r="10" spans="1:12">
@@ -36247,7 +36247,7 @@
         <v>807</v>
       </c>
       <c r="L10">
-        <v>613</v>
+        <v>616</v>
       </c>
     </row>
     <row r="11" spans="1:12">
@@ -36285,7 +36285,7 @@
         <v>1329</v>
       </c>
       <c r="L11">
-        <v>832</v>
+        <v>836</v>
       </c>
     </row>
   </sheetData>
@@ -37016,7 +37016,7 @@
         <v>113</v>
       </c>
       <c r="L8">
-        <v>38</v>
+        <v>39</v>
       </c>
     </row>
     <row r="9" spans="1:12">
@@ -37092,7 +37092,7 @@
         <v>354</v>
       </c>
       <c r="L10">
-        <v>214</v>
+        <v>215</v>
       </c>
     </row>
     <row r="11" spans="1:12">
@@ -37130,7 +37130,7 @@
         <v>616</v>
       </c>
       <c r="L11">
-        <v>321</v>
+        <v>323</v>
       </c>
     </row>
   </sheetData>
@@ -37630,7 +37630,7 @@
         <v>61</v>
       </c>
       <c r="L2">
-        <v>20</v>
+        <v>21</v>
       </c>
     </row>
     <row r="3" spans="1:12">
@@ -37928,7 +37928,7 @@
         <v>411</v>
       </c>
       <c r="L10">
-        <v>209</v>
+        <v>211</v>
       </c>
     </row>
     <row r="11" spans="1:12">
@@ -37966,7 +37966,7 @@
         <v>973</v>
       </c>
       <c r="L11">
-        <v>383</v>
+        <v>386</v>
       </c>
     </row>
   </sheetData>
@@ -38069,7 +38069,7 @@
         <v>112</v>
       </c>
       <c r="L2">
-        <v>48</v>
+        <v>49</v>
       </c>
     </row>
     <row r="3" spans="1:12">
@@ -38329,7 +38329,7 @@
         <v>120</v>
       </c>
       <c r="L9">
-        <v>42</v>
+        <v>44</v>
       </c>
     </row>
     <row r="10" spans="1:12">
@@ -38367,7 +38367,7 @@
         <v>1482</v>
       </c>
       <c r="L10">
-        <v>767</v>
+        <v>772</v>
       </c>
     </row>
     <row r="11" spans="1:12">
@@ -38405,7 +38405,7 @@
         <v>2322</v>
       </c>
       <c r="L11">
-        <v>1109</v>
+        <v>1117</v>
       </c>
     </row>
   </sheetData>
@@ -38717,7 +38717,7 @@
         <v>23</v>
       </c>
       <c r="L9">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="10" spans="1:12">
@@ -38755,7 +38755,7 @@
         <v>256</v>
       </c>
       <c r="L10">
-        <v>154</v>
+        <v>156</v>
       </c>
     </row>
     <row r="11" spans="1:12">
@@ -38793,7 +38793,7 @@
         <v>337</v>
       </c>
       <c r="L11">
-        <v>190</v>
+        <v>193</v>
       </c>
     </row>
   </sheetData>
@@ -39899,7 +39899,7 @@
         <v>167</v>
       </c>
       <c r="L10">
-        <v>49</v>
+        <v>50</v>
       </c>
     </row>
     <row r="11" spans="1:12">
@@ -39937,7 +39937,7 @@
         <v>202</v>
       </c>
       <c r="L11">
-        <v>55</v>
+        <v>56</v>
       </c>
     </row>
   </sheetData>
@@ -40142,7 +40142,7 @@
         <v>122</v>
       </c>
       <c r="L5">
-        <v>36</v>
+        <v>38</v>
       </c>
     </row>
     <row r="6" spans="1:12">
@@ -40323,7 +40323,7 @@
         <v>964</v>
       </c>
       <c r="L10">
-        <v>426</v>
+        <v>429</v>
       </c>
     </row>
     <row r="11" spans="1:12">
@@ -40361,7 +40361,7 @@
         <v>1502</v>
       </c>
       <c r="L11">
-        <v>613</v>
+        <v>618</v>
       </c>
     </row>
   </sheetData>
@@ -40632,7 +40632,7 @@
         <v>76</v>
       </c>
       <c r="L8">
-        <v>18</v>
+        <v>19</v>
       </c>
     </row>
     <row r="9" spans="1:12">
@@ -40670,7 +40670,7 @@
         <v>25</v>
       </c>
       <c r="L9">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="10" spans="1:12">
@@ -40746,7 +40746,7 @@
         <v>281</v>
       </c>
       <c r="L11">
-        <v>117</v>
+        <v>119</v>
       </c>
     </row>
   </sheetData>
@@ -41144,7 +41144,7 @@
         <v>159</v>
       </c>
       <c r="L10">
-        <v>92</v>
+        <v>93</v>
       </c>
     </row>
     <row r="11" spans="1:12">
@@ -41182,7 +41182,7 @@
         <v>402</v>
       </c>
       <c r="L11">
-        <v>184</v>
+        <v>185</v>
       </c>
     </row>
   </sheetData>
@@ -41535,7 +41535,7 @@
         <v>112</v>
       </c>
       <c r="L10">
-        <v>41</v>
+        <v>42</v>
       </c>
     </row>
     <row r="11" spans="1:12">
@@ -41573,7 +41573,7 @@
         <v>167</v>
       </c>
       <c r="L11">
-        <v>70</v>
+        <v>71</v>
       </c>
     </row>
   </sheetData>
@@ -42184,7 +42184,7 @@
         <v>41</v>
       </c>
       <c r="L5">
-        <v>17</v>
+        <v>18</v>
       </c>
     </row>
     <row r="6" spans="1:12">
@@ -42412,7 +42412,7 @@
         <v>484</v>
       </c>
       <c r="L11">
-        <v>230</v>
+        <v>231</v>
       </c>
     </row>
   </sheetData>
@@ -42515,7 +42515,7 @@
         <v>422</v>
       </c>
       <c r="L2">
-        <v>180</v>
+        <v>184</v>
       </c>
     </row>
     <row r="3" spans="1:12">
@@ -42553,7 +42553,7 @@
         <v>438</v>
       </c>
       <c r="L3">
-        <v>257</v>
+        <v>258</v>
       </c>
     </row>
     <row r="4" spans="1:12">
@@ -42743,7 +42743,7 @@
         <v>635</v>
       </c>
       <c r="L8">
-        <v>338</v>
+        <v>340</v>
       </c>
     </row>
     <row r="9" spans="1:12">
@@ -42781,7 +42781,7 @@
         <v>315</v>
       </c>
       <c r="L9">
-        <v>131</v>
+        <v>132</v>
       </c>
     </row>
     <row r="10" spans="1:12">
@@ -42819,7 +42819,7 @@
         <v>1486</v>
       </c>
       <c r="L10">
-        <v>750</v>
+        <v>758</v>
       </c>
     </row>
     <row r="11" spans="1:12">
@@ -42857,7 +42857,7 @@
         <v>3838</v>
       </c>
       <c r="L11">
-        <v>1882</v>
+        <v>1898</v>
       </c>
     </row>
   </sheetData>
@@ -43102,6 +43102,9 @@
       <c r="K6">
         <v>4</v>
       </c>
+      <c r="L6">
+        <v>1</v>
+      </c>
     </row>
     <row r="7" spans="1:12">
       <c r="A7" s="1" t="s">
@@ -43237,7 +43240,7 @@
         <v>127</v>
       </c>
       <c r="L10">
-        <v>87</v>
+        <v>88</v>
       </c>
     </row>
     <row r="11" spans="1:12">
@@ -43275,7 +43278,7 @@
         <v>248</v>
       </c>
       <c r="L11">
-        <v>143</v>
+        <v>145</v>
       </c>
     </row>
   </sheetData>
@@ -44393,7 +44396,7 @@
         <v>181</v>
       </c>
       <c r="L8">
-        <v>73</v>
+        <v>75</v>
       </c>
     </row>
     <row r="9" spans="1:12">
@@ -44431,7 +44434,7 @@
         <v>111</v>
       </c>
       <c r="L9">
-        <v>41</v>
+        <v>42</v>
       </c>
     </row>
     <row r="10" spans="1:12">
@@ -44469,7 +44472,7 @@
         <v>476</v>
       </c>
       <c r="L10">
-        <v>226</v>
+        <v>229</v>
       </c>
     </row>
     <row r="11" spans="1:12">
@@ -44507,7 +44510,7 @@
         <v>1021</v>
       </c>
       <c r="L11">
-        <v>456</v>
+        <v>462</v>
       </c>
     </row>
   </sheetData>
@@ -44857,7 +44860,7 @@
         <v>295</v>
       </c>
       <c r="L10">
-        <v>160</v>
+        <v>161</v>
       </c>
     </row>
     <row r="11" spans="1:12">
@@ -44895,7 +44898,7 @@
         <v>360</v>
       </c>
       <c r="L11">
-        <v>183</v>
+        <v>184</v>
       </c>
     </row>
   </sheetData>
@@ -45030,7 +45033,7 @@
         <v>1</v>
       </c>
       <c r="L3">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="4" spans="1:12">
@@ -45265,7 +45268,7 @@
         <v>263</v>
       </c>
       <c r="L11">
-        <v>150</v>
+        <v>151</v>
       </c>
     </row>
   </sheetData>

</xml_diff>